<commit_message>
Agrego casos de uso referentes a la responsividad de la web
</commit_message>
<xml_diff>
--- a/Testing 2024/template_caso_prueba-ISPC2024-sprint-1.xlsx
+++ b/Testing 2024/template_caso_prueba-ISPC2024-sprint-1.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ancal\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ancal\Desktop\ISPC_2024\practicaProfesionalizante-ISPC\Testing 2024\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="63">
   <si>
     <t>Id</t>
   </si>
@@ -172,6 +172,48 @@
   </si>
   <si>
     <t>TC-020</t>
+  </si>
+  <si>
+    <t>Usabilidad</t>
+  </si>
+  <si>
+    <t>Probar que el sitio sea responsive para Desktop</t>
+  </si>
+  <si>
+    <t>El usuario puede utilizar la pagina web desde una computadora</t>
+  </si>
+  <si>
+    <t>Sitio responsive. El usuario ingresa desde una computadora</t>
+  </si>
+  <si>
+    <t>1.</t>
+  </si>
+  <si>
+    <t>Ingresar a la url localhost:3000</t>
+  </si>
+  <si>
+    <t>Se visualiza la home page con toda su información de forma correcta y adaptada al tamaño del dispositivo</t>
+  </si>
+  <si>
+    <t>Andrea Caligiuri</t>
+  </si>
+  <si>
+    <t>Probar que el sitio sea responsive para Tablet</t>
+  </si>
+  <si>
+    <t>El usuario puede utilizar la pagina web desde una tablet</t>
+  </si>
+  <si>
+    <t>Sitio responsive. El usuario ingresa desde una tablet</t>
+  </si>
+  <si>
+    <t>Probar que el sitio sea responsive para Mobile</t>
+  </si>
+  <si>
+    <t>El usuario puede utilizar la pagina web desde un celular</t>
+  </si>
+  <si>
+    <t>Sitio responsive. El usuario ingresa desde un celular</t>
   </si>
 </sst>
 </file>
@@ -683,15 +725,6 @@
     <xf numFmtId="0" fontId="12" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -701,13 +734,19 @@
     <xf numFmtId="0" fontId="1" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -715,24 +754,6 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -748,25 +769,62 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="10" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="10" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="10" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="32">
+  <dxfs count="12">
     <dxf>
       <fill>
         <patternFill patternType="solid">
           <fgColor rgb="FFFCE5CD"/>
           <bgColor rgb="FFFCE5CD"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFCE5CD"/>
+          <bgColor rgb="FFFCE5CD"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF93C47D"/>
+          <bgColor rgb="FF93C47D"/>
         </patternFill>
       </fill>
     </dxf>
@@ -789,22 +847,6 @@
     <dxf>
       <fill>
         <patternFill patternType="solid">
-          <fgColor rgb="FFFCE5CD"/>
-          <bgColor rgb="FFFCE5CD"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FF93C47D"/>
-          <bgColor rgb="FF93C47D"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
           <fgColor rgb="FFFFF2CC"/>
           <bgColor rgb="FFFFF2CC"/>
         </patternFill>
@@ -815,166 +857,6 @@
         <patternFill patternType="solid">
           <fgColor rgb="FFA2C4C9"/>
           <bgColor rgb="FFA2C4C9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFA2C4C9"/>
-          <bgColor rgb="FFA2C4C9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFCE5CD"/>
-          <bgColor rgb="FFFCE5CD"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FF93C47D"/>
-          <bgColor rgb="FF93C47D"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFF2CC"/>
-          <bgColor rgb="FFFFF2CC"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFCE5CD"/>
-          <bgColor rgb="FFFCE5CD"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FF93C47D"/>
-          <bgColor rgb="FF93C47D"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFF2CC"/>
-          <bgColor rgb="FFFFF2CC"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFA2C4C9"/>
-          <bgColor rgb="FFA2C4C9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFA2C4C9"/>
-          <bgColor rgb="FFA2C4C9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFCE5CD"/>
-          <bgColor rgb="FFFCE5CD"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FF93C47D"/>
-          <bgColor rgb="FF93C47D"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFF2CC"/>
-          <bgColor rgb="FFFFF2CC"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFCE5CD"/>
-          <bgColor rgb="FFFCE5CD"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FF93C47D"/>
-          <bgColor rgb="FF93C47D"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFF2CC"/>
-          <bgColor rgb="FFFFF2CC"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFA2C4C9"/>
-          <bgColor rgb="FFA2C4C9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFA2C4C9"/>
-          <bgColor rgb="FFA2C4C9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFCE5CD"/>
-          <bgColor rgb="FFFCE5CD"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FF93C47D"/>
-          <bgColor rgb="FF93C47D"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFF2CC"/>
-          <bgColor rgb="FFFFF2CC"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1368,7 +1250,7 @@
   <dimension ref="A1:AA935"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="60" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8:B11"/>
+      <selection activeCell="G21" sqref="G21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5703125" defaultRowHeight="12.75"/>
@@ -1417,33 +1299,33 @@
       <c r="AA1" s="2"/>
     </row>
     <row r="2" spans="1:27" s="31" customFormat="1" ht="15.75" customHeight="1">
-      <c r="A2" s="59" t="s">
+      <c r="A2" s="61" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="57" t="s">
+      <c r="B2" s="51" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="59" t="s">
+      <c r="C2" s="61" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="57" t="s">
+      <c r="D2" s="51" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="57" t="s">
+      <c r="E2" s="51" t="s">
         <v>4</v>
       </c>
-      <c r="F2" s="63" t="s">
+      <c r="F2" s="56" t="s">
         <v>5</v>
       </c>
-      <c r="G2" s="64"/>
-      <c r="H2" s="65"/>
-      <c r="I2" s="66" t="s">
+      <c r="G2" s="57"/>
+      <c r="H2" s="58"/>
+      <c r="I2" s="59" t="s">
         <v>6</v>
       </c>
-      <c r="J2" s="57" t="s">
+      <c r="J2" s="51" t="s">
         <v>7</v>
       </c>
-      <c r="K2" s="57" t="s">
+      <c r="K2" s="51" t="s">
         <v>27</v>
       </c>
       <c r="L2" s="32"/>
@@ -1464,11 +1346,11 @@
       <c r="AA2" s="33"/>
     </row>
     <row r="3" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A3" s="60"/>
-      <c r="B3" s="58"/>
-      <c r="C3" s="60"/>
-      <c r="D3" s="58"/>
-      <c r="E3" s="58"/>
+      <c r="A3" s="62"/>
+      <c r="B3" s="52"/>
+      <c r="C3" s="62"/>
+      <c r="D3" s="52"/>
+      <c r="E3" s="52"/>
       <c r="F3" s="34" t="s">
         <v>8</v>
       </c>
@@ -1478,9 +1360,9 @@
       <c r="H3" s="42" t="s">
         <v>10</v>
       </c>
-      <c r="I3" s="67"/>
-      <c r="J3" s="58"/>
-      <c r="K3" s="58"/>
+      <c r="I3" s="60"/>
+      <c r="J3" s="52"/>
+      <c r="K3" s="52"/>
       <c r="L3" s="3"/>
       <c r="M3" s="2"/>
       <c r="N3" s="2"/>
@@ -1499,21 +1381,37 @@
       <c r="AA3" s="2"/>
     </row>
     <row r="4" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A4" s="68" t="s">
+      <c r="A4" s="48" t="s">
         <v>29</v>
       </c>
-      <c r="B4" s="48"/>
-      <c r="C4" s="48"/>
-      <c r="D4" s="48"/>
-      <c r="E4" s="48"/>
-      <c r="F4" s="48"/>
-      <c r="G4" s="48"/>
-      <c r="H4" s="61"/>
-      <c r="I4" s="54" t="s">
+      <c r="B4" s="45" t="s">
+        <v>49</v>
+      </c>
+      <c r="C4" s="45" t="s">
+        <v>50</v>
+      </c>
+      <c r="D4" s="45" t="s">
+        <v>51</v>
+      </c>
+      <c r="E4" s="45" t="s">
+        <v>52</v>
+      </c>
+      <c r="F4" s="45" t="s">
+        <v>53</v>
+      </c>
+      <c r="G4" s="45" t="s">
+        <v>54</v>
+      </c>
+      <c r="H4" s="63" t="s">
+        <v>55</v>
+      </c>
+      <c r="I4" s="53" t="s">
         <v>26</v>
       </c>
-      <c r="J4" s="45"/>
-      <c r="K4" s="54" t="s">
+      <c r="J4" s="65" t="s">
+        <v>56</v>
+      </c>
+      <c r="K4" s="53" t="s">
         <v>28</v>
       </c>
       <c r="L4" s="3"/>
@@ -1534,17 +1432,17 @@
       <c r="AA4" s="2"/>
     </row>
     <row r="5" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A5" s="69"/>
-      <c r="B5" s="49"/>
-      <c r="C5" s="49"/>
-      <c r="D5" s="49"/>
-      <c r="E5" s="49"/>
-      <c r="F5" s="50"/>
-      <c r="G5" s="50"/>
-      <c r="H5" s="62"/>
-      <c r="I5" s="55"/>
-      <c r="J5" s="46"/>
-      <c r="K5" s="55"/>
+      <c r="A5" s="49"/>
+      <c r="B5" s="46"/>
+      <c r="C5" s="46"/>
+      <c r="D5" s="46"/>
+      <c r="E5" s="46"/>
+      <c r="F5" s="47"/>
+      <c r="G5" s="47"/>
+      <c r="H5" s="64"/>
+      <c r="I5" s="54"/>
+      <c r="J5" s="66"/>
+      <c r="K5" s="54"/>
       <c r="L5" s="3"/>
       <c r="M5" s="2"/>
       <c r="N5" s="2"/>
@@ -1563,17 +1461,17 @@
       <c r="AA5" s="2"/>
     </row>
     <row r="6" spans="1:27" s="29" customFormat="1" ht="15.75" customHeight="1">
-      <c r="A6" s="69"/>
-      <c r="B6" s="49"/>
-      <c r="C6" s="49"/>
-      <c r="D6" s="49"/>
-      <c r="E6" s="49"/>
+      <c r="A6" s="49"/>
+      <c r="B6" s="46"/>
+      <c r="C6" s="46"/>
+      <c r="D6" s="46"/>
+      <c r="E6" s="46"/>
       <c r="F6" s="30"/>
       <c r="G6" s="35"/>
       <c r="H6" s="35"/>
-      <c r="I6" s="55"/>
-      <c r="J6" s="46"/>
-      <c r="K6" s="55"/>
+      <c r="I6" s="54"/>
+      <c r="J6" s="66"/>
+      <c r="K6" s="54"/>
       <c r="L6" s="27"/>
       <c r="M6" s="28"/>
       <c r="N6" s="28"/>
@@ -1592,17 +1490,17 @@
       <c r="AA6" s="28"/>
     </row>
     <row r="7" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A7" s="70"/>
-      <c r="B7" s="50"/>
-      <c r="C7" s="50"/>
-      <c r="D7" s="50"/>
-      <c r="E7" s="50"/>
+      <c r="A7" s="50"/>
+      <c r="B7" s="47"/>
+      <c r="C7" s="47"/>
+      <c r="D7" s="47"/>
+      <c r="E7" s="47"/>
       <c r="F7" s="30"/>
       <c r="G7" s="35"/>
       <c r="H7" s="35"/>
-      <c r="I7" s="56"/>
-      <c r="J7" s="47"/>
-      <c r="K7" s="56"/>
+      <c r="I7" s="55"/>
+      <c r="J7" s="67"/>
+      <c r="K7" s="55"/>
       <c r="L7" s="3"/>
       <c r="M7" s="2"/>
       <c r="N7" s="2"/>
@@ -1621,21 +1519,37 @@
       <c r="AA7" s="2"/>
     </row>
     <row r="8" spans="1:27">
-      <c r="A8" s="68" t="s">
+      <c r="A8" s="48" t="s">
         <v>30</v>
       </c>
-      <c r="B8" s="48"/>
-      <c r="C8" s="48"/>
-      <c r="D8" s="48"/>
-      <c r="E8" s="48"/>
-      <c r="F8" s="48"/>
-      <c r="G8" s="48"/>
-      <c r="H8" s="61"/>
-      <c r="I8" s="54" t="s">
+      <c r="B8" s="45" t="s">
+        <v>49</v>
+      </c>
+      <c r="C8" s="45" t="s">
+        <v>57</v>
+      </c>
+      <c r="D8" s="45" t="s">
+        <v>58</v>
+      </c>
+      <c r="E8" s="45" t="s">
+        <v>59</v>
+      </c>
+      <c r="F8" s="45" t="s">
+        <v>53</v>
+      </c>
+      <c r="G8" s="45" t="s">
+        <v>54</v>
+      </c>
+      <c r="H8" s="63" t="s">
+        <v>55</v>
+      </c>
+      <c r="I8" s="53" t="s">
         <v>26</v>
       </c>
-      <c r="J8" s="45"/>
-      <c r="K8" s="54" t="s">
+      <c r="J8" s="65" t="s">
+        <v>56</v>
+      </c>
+      <c r="K8" s="53" t="s">
         <v>28</v>
       </c>
       <c r="L8" s="3"/>
@@ -1656,17 +1570,17 @@
       <c r="AA8" s="2"/>
     </row>
     <row r="9" spans="1:27">
-      <c r="A9" s="69"/>
-      <c r="B9" s="49"/>
-      <c r="C9" s="49"/>
-      <c r="D9" s="49"/>
-      <c r="E9" s="49"/>
-      <c r="F9" s="50"/>
-      <c r="G9" s="50"/>
-      <c r="H9" s="62"/>
-      <c r="I9" s="55"/>
-      <c r="J9" s="46"/>
-      <c r="K9" s="55"/>
+      <c r="A9" s="49"/>
+      <c r="B9" s="46"/>
+      <c r="C9" s="46"/>
+      <c r="D9" s="46"/>
+      <c r="E9" s="46"/>
+      <c r="F9" s="47"/>
+      <c r="G9" s="47"/>
+      <c r="H9" s="64"/>
+      <c r="I9" s="54"/>
+      <c r="J9" s="66"/>
+      <c r="K9" s="54"/>
       <c r="L9" s="3"/>
       <c r="M9" s="2"/>
       <c r="N9" s="2"/>
@@ -1685,17 +1599,17 @@
       <c r="AA9" s="2"/>
     </row>
     <row r="10" spans="1:27" s="29" customFormat="1" ht="15.75" customHeight="1">
-      <c r="A10" s="69"/>
-      <c r="B10" s="49"/>
-      <c r="C10" s="49"/>
-      <c r="D10" s="49"/>
-      <c r="E10" s="49"/>
+      <c r="A10" s="49"/>
+      <c r="B10" s="46"/>
+      <c r="C10" s="46"/>
+      <c r="D10" s="46"/>
+      <c r="E10" s="46"/>
       <c r="F10" s="30"/>
       <c r="G10" s="35"/>
       <c r="H10" s="35"/>
-      <c r="I10" s="55"/>
-      <c r="J10" s="46"/>
-      <c r="K10" s="55"/>
+      <c r="I10" s="54"/>
+      <c r="J10" s="66"/>
+      <c r="K10" s="54"/>
       <c r="L10" s="27"/>
       <c r="M10" s="28"/>
       <c r="N10" s="28"/>
@@ -1714,17 +1628,17 @@
       <c r="AA10" s="28"/>
     </row>
     <row r="11" spans="1:27">
-      <c r="A11" s="70"/>
-      <c r="B11" s="50"/>
-      <c r="C11" s="50"/>
-      <c r="D11" s="50"/>
-      <c r="E11" s="50"/>
+      <c r="A11" s="50"/>
+      <c r="B11" s="47"/>
+      <c r="C11" s="47"/>
+      <c r="D11" s="47"/>
+      <c r="E11" s="47"/>
       <c r="F11" s="30"/>
       <c r="G11" s="35"/>
       <c r="H11" s="35"/>
-      <c r="I11" s="56"/>
-      <c r="J11" s="47"/>
-      <c r="K11" s="56"/>
+      <c r="I11" s="55"/>
+      <c r="J11" s="67"/>
+      <c r="K11" s="55"/>
       <c r="L11" s="3"/>
       <c r="M11" s="2"/>
       <c r="N11" s="2"/>
@@ -1743,21 +1657,37 @@
       <c r="AA11" s="2"/>
     </row>
     <row r="12" spans="1:27">
-      <c r="A12" s="68" t="s">
+      <c r="A12" s="48" t="s">
         <v>31</v>
       </c>
-      <c r="B12" s="48"/>
-      <c r="C12" s="48"/>
-      <c r="D12" s="48"/>
-      <c r="E12" s="48"/>
-      <c r="F12" s="48"/>
-      <c r="G12" s="48"/>
-      <c r="H12" s="61"/>
-      <c r="I12" s="54" t="s">
+      <c r="B12" s="45" t="s">
+        <v>49</v>
+      </c>
+      <c r="C12" s="45" t="s">
+        <v>60</v>
+      </c>
+      <c r="D12" s="45" t="s">
+        <v>61</v>
+      </c>
+      <c r="E12" s="45" t="s">
+        <v>62</v>
+      </c>
+      <c r="F12" s="45" t="s">
+        <v>53</v>
+      </c>
+      <c r="G12" s="45" t="s">
+        <v>54</v>
+      </c>
+      <c r="H12" s="63" t="s">
+        <v>55</v>
+      </c>
+      <c r="I12" s="53" t="s">
         <v>26</v>
       </c>
-      <c r="J12" s="45"/>
-      <c r="K12" s="54" t="s">
+      <c r="J12" s="65" t="s">
+        <v>56</v>
+      </c>
+      <c r="K12" s="53" t="s">
         <v>28</v>
       </c>
       <c r="L12" s="2"/>
@@ -1778,17 +1708,17 @@
       <c r="AA12" s="2"/>
     </row>
     <row r="13" spans="1:27">
-      <c r="A13" s="69"/>
-      <c r="B13" s="49"/>
-      <c r="C13" s="49"/>
-      <c r="D13" s="49"/>
-      <c r="E13" s="49"/>
-      <c r="F13" s="50"/>
-      <c r="G13" s="50"/>
-      <c r="H13" s="62"/>
-      <c r="I13" s="55"/>
-      <c r="J13" s="46"/>
-      <c r="K13" s="55"/>
+      <c r="A13" s="49"/>
+      <c r="B13" s="46"/>
+      <c r="C13" s="46"/>
+      <c r="D13" s="46"/>
+      <c r="E13" s="46"/>
+      <c r="F13" s="47"/>
+      <c r="G13" s="47"/>
+      <c r="H13" s="64"/>
+      <c r="I13" s="54"/>
+      <c r="J13" s="66"/>
+      <c r="K13" s="54"/>
       <c r="L13" s="2"/>
       <c r="M13" s="2"/>
       <c r="N13" s="2"/>
@@ -1807,17 +1737,17 @@
       <c r="AA13" s="2"/>
     </row>
     <row r="14" spans="1:27" s="29" customFormat="1">
-      <c r="A14" s="69"/>
-      <c r="B14" s="49"/>
-      <c r="C14" s="49"/>
-      <c r="D14" s="49"/>
-      <c r="E14" s="49"/>
+      <c r="A14" s="49"/>
+      <c r="B14" s="46"/>
+      <c r="C14" s="46"/>
+      <c r="D14" s="46"/>
+      <c r="E14" s="46"/>
       <c r="F14" s="30"/>
       <c r="G14" s="35"/>
       <c r="H14" s="35"/>
-      <c r="I14" s="55"/>
-      <c r="J14" s="46"/>
-      <c r="K14" s="55"/>
+      <c r="I14" s="54"/>
+      <c r="J14" s="66"/>
+      <c r="K14" s="54"/>
       <c r="L14" s="28"/>
       <c r="M14" s="28"/>
       <c r="N14" s="28"/>
@@ -1836,17 +1766,17 @@
       <c r="AA14" s="28"/>
     </row>
     <row r="15" spans="1:27">
-      <c r="A15" s="70"/>
-      <c r="B15" s="50"/>
-      <c r="C15" s="50"/>
-      <c r="D15" s="50"/>
-      <c r="E15" s="50"/>
+      <c r="A15" s="50"/>
+      <c r="B15" s="47"/>
+      <c r="C15" s="47"/>
+      <c r="D15" s="47"/>
+      <c r="E15" s="47"/>
       <c r="F15" s="30"/>
       <c r="G15" s="35"/>
       <c r="H15" s="35"/>
-      <c r="I15" s="56"/>
-      <c r="J15" s="47"/>
-      <c r="K15" s="56"/>
+      <c r="I15" s="55"/>
+      <c r="J15" s="67"/>
+      <c r="K15" s="55"/>
       <c r="L15" s="2"/>
       <c r="M15" s="2"/>
       <c r="N15" s="2"/>
@@ -1865,21 +1795,21 @@
       <c r="AA15" s="2"/>
     </row>
     <row r="16" spans="1:27">
-      <c r="A16" s="68" t="s">
+      <c r="A16" s="48" t="s">
         <v>32</v>
       </c>
-      <c r="B16" s="48"/>
-      <c r="C16" s="48"/>
-      <c r="D16" s="48"/>
-      <c r="E16" s="48"/>
+      <c r="B16" s="45"/>
+      <c r="C16" s="45"/>
+      <c r="D16" s="45"/>
+      <c r="E16" s="45"/>
       <c r="F16" s="30"/>
       <c r="G16" s="44"/>
       <c r="H16" s="44"/>
-      <c r="I16" s="54" t="s">
+      <c r="I16" s="53" t="s">
         <v>26</v>
       </c>
-      <c r="J16" s="45"/>
-      <c r="K16" s="54" t="s">
+      <c r="J16" s="65"/>
+      <c r="K16" s="53" t="s">
         <v>28</v>
       </c>
       <c r="L16" s="2"/>
@@ -1900,17 +1830,17 @@
       <c r="AA16" s="2"/>
     </row>
     <row r="17" spans="1:27" ht="16.5" customHeight="1">
-      <c r="A17" s="69"/>
-      <c r="B17" s="49"/>
-      <c r="C17" s="49"/>
-      <c r="D17" s="49"/>
-      <c r="E17" s="49"/>
+      <c r="A17" s="49"/>
+      <c r="B17" s="46"/>
+      <c r="C17" s="46"/>
+      <c r="D17" s="46"/>
+      <c r="E17" s="46"/>
       <c r="F17" s="30"/>
       <c r="G17" s="44"/>
       <c r="H17" s="44"/>
-      <c r="I17" s="55"/>
-      <c r="J17" s="46"/>
-      <c r="K17" s="55"/>
+      <c r="I17" s="54"/>
+      <c r="J17" s="66"/>
+      <c r="K17" s="54"/>
       <c r="L17" s="2"/>
       <c r="M17" s="2"/>
       <c r="N17" s="2"/>
@@ -1929,17 +1859,17 @@
       <c r="AA17" s="2"/>
     </row>
     <row r="18" spans="1:27" s="29" customFormat="1">
-      <c r="A18" s="69"/>
-      <c r="B18" s="49"/>
-      <c r="C18" s="49"/>
-      <c r="D18" s="49"/>
-      <c r="E18" s="49"/>
+      <c r="A18" s="49"/>
+      <c r="B18" s="46"/>
+      <c r="C18" s="46"/>
+      <c r="D18" s="46"/>
+      <c r="E18" s="46"/>
       <c r="F18" s="30"/>
       <c r="G18" s="44"/>
       <c r="H18" s="44"/>
-      <c r="I18" s="55"/>
-      <c r="J18" s="46"/>
-      <c r="K18" s="55"/>
+      <c r="I18" s="54"/>
+      <c r="J18" s="66"/>
+      <c r="K18" s="54"/>
       <c r="L18" s="28"/>
       <c r="M18" s="28"/>
       <c r="N18" s="28"/>
@@ -1958,17 +1888,17 @@
       <c r="AA18" s="28"/>
     </row>
     <row r="19" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A19" s="70"/>
-      <c r="B19" s="50"/>
-      <c r="C19" s="50"/>
-      <c r="D19" s="50"/>
-      <c r="E19" s="50"/>
+      <c r="A19" s="50"/>
+      <c r="B19" s="47"/>
+      <c r="C19" s="47"/>
+      <c r="D19" s="47"/>
+      <c r="E19" s="47"/>
       <c r="F19" s="30"/>
       <c r="G19" s="44"/>
       <c r="H19" s="44"/>
-      <c r="I19" s="56"/>
-      <c r="J19" s="47"/>
-      <c r="K19" s="56"/>
+      <c r="I19" s="55"/>
+      <c r="J19" s="67"/>
+      <c r="K19" s="55"/>
       <c r="L19" s="2"/>
       <c r="M19" s="2"/>
       <c r="N19" s="2"/>
@@ -1987,21 +1917,21 @@
       <c r="AA19" s="2"/>
     </row>
     <row r="20" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A20" s="68" t="s">
+      <c r="A20" s="48" t="s">
         <v>33</v>
       </c>
-      <c r="B20" s="48"/>
-      <c r="C20" s="48"/>
-      <c r="D20" s="48"/>
-      <c r="E20" s="48"/>
+      <c r="B20" s="45"/>
+      <c r="C20" s="45"/>
+      <c r="D20" s="45"/>
+      <c r="E20" s="45"/>
       <c r="F20" s="30"/>
       <c r="G20" s="44"/>
       <c r="H20" s="44"/>
-      <c r="I20" s="54" t="s">
+      <c r="I20" s="53" t="s">
         <v>26</v>
       </c>
-      <c r="J20" s="45"/>
-      <c r="K20" s="54" t="s">
+      <c r="J20" s="65"/>
+      <c r="K20" s="53" t="s">
         <v>28</v>
       </c>
       <c r="L20" s="2"/>
@@ -2022,17 +1952,17 @@
       <c r="AA20" s="2"/>
     </row>
     <row r="21" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A21" s="69"/>
-      <c r="B21" s="49"/>
-      <c r="C21" s="49"/>
-      <c r="D21" s="49"/>
-      <c r="E21" s="49"/>
+      <c r="A21" s="49"/>
+      <c r="B21" s="46"/>
+      <c r="C21" s="46"/>
+      <c r="D21" s="46"/>
+      <c r="E21" s="46"/>
       <c r="F21" s="30"/>
       <c r="G21" s="44"/>
       <c r="H21" s="44"/>
-      <c r="I21" s="55"/>
-      <c r="J21" s="46"/>
-      <c r="K21" s="55"/>
+      <c r="I21" s="54"/>
+      <c r="J21" s="66"/>
+      <c r="K21" s="54"/>
       <c r="L21" s="2"/>
       <c r="M21" s="2"/>
       <c r="N21" s="2"/>
@@ -2051,17 +1981,17 @@
       <c r="AA21" s="2"/>
     </row>
     <row r="22" spans="1:27" s="29" customFormat="1" ht="15.75" customHeight="1">
-      <c r="A22" s="69"/>
-      <c r="B22" s="49"/>
-      <c r="C22" s="49"/>
-      <c r="D22" s="49"/>
-      <c r="E22" s="49"/>
+      <c r="A22" s="49"/>
+      <c r="B22" s="46"/>
+      <c r="C22" s="46"/>
+      <c r="D22" s="46"/>
+      <c r="E22" s="46"/>
       <c r="F22" s="30"/>
       <c r="G22" s="44"/>
       <c r="H22" s="44"/>
-      <c r="I22" s="55"/>
-      <c r="J22" s="46"/>
-      <c r="K22" s="55"/>
+      <c r="I22" s="54"/>
+      <c r="J22" s="66"/>
+      <c r="K22" s="54"/>
       <c r="L22" s="28"/>
       <c r="M22" s="28"/>
       <c r="N22" s="28"/>
@@ -2080,17 +2010,17 @@
       <c r="AA22" s="28"/>
     </row>
     <row r="23" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A23" s="70"/>
-      <c r="B23" s="50"/>
-      <c r="C23" s="50"/>
-      <c r="D23" s="50"/>
-      <c r="E23" s="50"/>
+      <c r="A23" s="50"/>
+      <c r="B23" s="47"/>
+      <c r="C23" s="47"/>
+      <c r="D23" s="47"/>
+      <c r="E23" s="47"/>
       <c r="F23" s="30"/>
       <c r="G23" s="44"/>
       <c r="H23" s="44"/>
-      <c r="I23" s="56"/>
-      <c r="J23" s="47"/>
-      <c r="K23" s="56"/>
+      <c r="I23" s="55"/>
+      <c r="J23" s="67"/>
+      <c r="K23" s="55"/>
       <c r="L23" s="2"/>
       <c r="M23" s="2"/>
       <c r="N23" s="2"/>
@@ -2109,21 +2039,21 @@
       <c r="AA23" s="2"/>
     </row>
     <row r="24" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A24" s="68" t="s">
+      <c r="A24" s="48" t="s">
         <v>34</v>
       </c>
-      <c r="B24" s="48"/>
-      <c r="C24" s="48"/>
-      <c r="D24" s="48"/>
-      <c r="E24" s="48"/>
+      <c r="B24" s="45"/>
+      <c r="C24" s="45"/>
+      <c r="D24" s="45"/>
+      <c r="E24" s="45"/>
       <c r="F24" s="30"/>
       <c r="G24" s="44"/>
       <c r="H24" s="44"/>
-      <c r="I24" s="54" t="s">
+      <c r="I24" s="53" t="s">
         <v>26</v>
       </c>
-      <c r="J24" s="45"/>
-      <c r="K24" s="54" t="s">
+      <c r="J24" s="65"/>
+      <c r="K24" s="53" t="s">
         <v>28</v>
       </c>
       <c r="L24" s="2"/>
@@ -2144,17 +2074,17 @@
       <c r="AA24" s="2"/>
     </row>
     <row r="25" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A25" s="69"/>
-      <c r="B25" s="49"/>
-      <c r="C25" s="49"/>
-      <c r="D25" s="49"/>
-      <c r="E25" s="49"/>
+      <c r="A25" s="49"/>
+      <c r="B25" s="46"/>
+      <c r="C25" s="46"/>
+      <c r="D25" s="46"/>
+      <c r="E25" s="46"/>
       <c r="F25" s="30"/>
       <c r="G25" s="44"/>
       <c r="H25" s="44"/>
-      <c r="I25" s="55"/>
-      <c r="J25" s="46"/>
-      <c r="K25" s="55"/>
+      <c r="I25" s="54"/>
+      <c r="J25" s="66"/>
+      <c r="K25" s="54"/>
       <c r="L25" s="2"/>
       <c r="M25" s="2"/>
       <c r="N25" s="2"/>
@@ -2173,17 +2103,17 @@
       <c r="AA25" s="2"/>
     </row>
     <row r="26" spans="1:27" s="29" customFormat="1" ht="15.75" customHeight="1">
-      <c r="A26" s="69"/>
-      <c r="B26" s="49"/>
-      <c r="C26" s="49"/>
-      <c r="D26" s="49"/>
-      <c r="E26" s="49"/>
+      <c r="A26" s="49"/>
+      <c r="B26" s="46"/>
+      <c r="C26" s="46"/>
+      <c r="D26" s="46"/>
+      <c r="E26" s="46"/>
       <c r="F26" s="30"/>
       <c r="G26" s="44"/>
       <c r="H26" s="44"/>
-      <c r="I26" s="55"/>
-      <c r="J26" s="46"/>
-      <c r="K26" s="55"/>
+      <c r="I26" s="54"/>
+      <c r="J26" s="66"/>
+      <c r="K26" s="54"/>
       <c r="L26" s="28"/>
       <c r="M26" s="28"/>
       <c r="N26" s="28"/>
@@ -2202,17 +2132,17 @@
       <c r="AA26" s="28"/>
     </row>
     <row r="27" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A27" s="70"/>
-      <c r="B27" s="50"/>
-      <c r="C27" s="50"/>
-      <c r="D27" s="50"/>
-      <c r="E27" s="50"/>
+      <c r="A27" s="50"/>
+      <c r="B27" s="47"/>
+      <c r="C27" s="47"/>
+      <c r="D27" s="47"/>
+      <c r="E27" s="47"/>
       <c r="F27" s="30"/>
       <c r="G27" s="44"/>
       <c r="H27" s="44"/>
-      <c r="I27" s="56"/>
-      <c r="J27" s="47"/>
-      <c r="K27" s="56"/>
+      <c r="I27" s="55"/>
+      <c r="J27" s="67"/>
+      <c r="K27" s="55"/>
       <c r="L27" s="2"/>
       <c r="M27" s="2"/>
       <c r="N27" s="2"/>
@@ -2231,21 +2161,21 @@
       <c r="AA27" s="2"/>
     </row>
     <row r="28" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A28" s="68" t="s">
+      <c r="A28" s="48" t="s">
         <v>35</v>
       </c>
-      <c r="B28" s="48"/>
-      <c r="C28" s="48"/>
-      <c r="D28" s="48"/>
-      <c r="E28" s="48"/>
+      <c r="B28" s="45"/>
+      <c r="C28" s="45"/>
+      <c r="D28" s="45"/>
+      <c r="E28" s="45"/>
       <c r="F28" s="30"/>
       <c r="G28" s="44"/>
       <c r="H28" s="44"/>
-      <c r="I28" s="54" t="s">
+      <c r="I28" s="53" t="s">
         <v>26</v>
       </c>
-      <c r="J28" s="45"/>
-      <c r="K28" s="54" t="s">
+      <c r="J28" s="65"/>
+      <c r="K28" s="53" t="s">
         <v>28</v>
       </c>
       <c r="L28" s="2"/>
@@ -2266,17 +2196,17 @@
       <c r="AA28" s="2"/>
     </row>
     <row r="29" spans="1:27">
-      <c r="A29" s="69"/>
-      <c r="B29" s="49"/>
-      <c r="C29" s="49"/>
-      <c r="D29" s="49"/>
-      <c r="E29" s="49"/>
+      <c r="A29" s="49"/>
+      <c r="B29" s="46"/>
+      <c r="C29" s="46"/>
+      <c r="D29" s="46"/>
+      <c r="E29" s="46"/>
       <c r="F29" s="30"/>
       <c r="G29" s="44"/>
       <c r="H29" s="44"/>
-      <c r="I29" s="55"/>
-      <c r="J29" s="46"/>
-      <c r="K29" s="55"/>
+      <c r="I29" s="54"/>
+      <c r="J29" s="66"/>
+      <c r="K29" s="54"/>
       <c r="L29" s="2"/>
       <c r="M29" s="2"/>
       <c r="N29" s="2"/>
@@ -2295,17 +2225,17 @@
       <c r="AA29" s="2"/>
     </row>
     <row r="30" spans="1:27" s="29" customFormat="1" ht="15.75" customHeight="1">
-      <c r="A30" s="69"/>
-      <c r="B30" s="49"/>
-      <c r="C30" s="49"/>
-      <c r="D30" s="49"/>
-      <c r="E30" s="49"/>
+      <c r="A30" s="49"/>
+      <c r="B30" s="46"/>
+      <c r="C30" s="46"/>
+      <c r="D30" s="46"/>
+      <c r="E30" s="46"/>
       <c r="F30" s="30"/>
       <c r="G30" s="44"/>
       <c r="H30" s="44"/>
-      <c r="I30" s="55"/>
-      <c r="J30" s="46"/>
-      <c r="K30" s="55"/>
+      <c r="I30" s="54"/>
+      <c r="J30" s="66"/>
+      <c r="K30" s="54"/>
       <c r="L30" s="28"/>
       <c r="M30" s="28"/>
       <c r="N30" s="28"/>
@@ -2324,17 +2254,17 @@
       <c r="AA30" s="28"/>
     </row>
     <row r="31" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A31" s="70"/>
-      <c r="B31" s="50"/>
-      <c r="C31" s="50"/>
-      <c r="D31" s="50"/>
-      <c r="E31" s="50"/>
+      <c r="A31" s="50"/>
+      <c r="B31" s="47"/>
+      <c r="C31" s="47"/>
+      <c r="D31" s="47"/>
+      <c r="E31" s="47"/>
       <c r="F31" s="30"/>
       <c r="G31" s="44"/>
       <c r="H31" s="44"/>
-      <c r="I31" s="56"/>
-      <c r="J31" s="47"/>
-      <c r="K31" s="56"/>
+      <c r="I31" s="55"/>
+      <c r="J31" s="67"/>
+      <c r="K31" s="55"/>
       <c r="L31" s="2"/>
       <c r="M31" s="2"/>
       <c r="N31" s="2"/>
@@ -2353,21 +2283,21 @@
       <c r="AA31" s="2"/>
     </row>
     <row r="32" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A32" s="68" t="s">
+      <c r="A32" s="48" t="s">
         <v>36</v>
       </c>
-      <c r="B32" s="48"/>
-      <c r="C32" s="48"/>
-      <c r="D32" s="48"/>
-      <c r="E32" s="48"/>
+      <c r="B32" s="45"/>
+      <c r="C32" s="45"/>
+      <c r="D32" s="45"/>
+      <c r="E32" s="45"/>
       <c r="F32" s="30"/>
       <c r="G32" s="35"/>
       <c r="H32" s="35"/>
-      <c r="I32" s="54" t="s">
+      <c r="I32" s="53" t="s">
         <v>26</v>
       </c>
-      <c r="J32" s="45"/>
-      <c r="K32" s="54" t="s">
+      <c r="J32" s="65"/>
+      <c r="K32" s="53" t="s">
         <v>28</v>
       </c>
       <c r="L32" s="2"/>
@@ -2388,17 +2318,17 @@
       <c r="AA32" s="2"/>
     </row>
     <row r="33" spans="1:27">
-      <c r="A33" s="69"/>
-      <c r="B33" s="49"/>
-      <c r="C33" s="49"/>
-      <c r="D33" s="49"/>
-      <c r="E33" s="49"/>
+      <c r="A33" s="49"/>
+      <c r="B33" s="46"/>
+      <c r="C33" s="46"/>
+      <c r="D33" s="46"/>
+      <c r="E33" s="46"/>
       <c r="F33" s="30"/>
       <c r="G33" s="35"/>
       <c r="H33" s="35"/>
-      <c r="I33" s="55"/>
-      <c r="J33" s="46"/>
-      <c r="K33" s="55"/>
+      <c r="I33" s="54"/>
+      <c r="J33" s="66"/>
+      <c r="K33" s="54"/>
       <c r="L33" s="2"/>
       <c r="M33" s="2"/>
       <c r="N33" s="2"/>
@@ -2417,17 +2347,17 @@
       <c r="AA33" s="2"/>
     </row>
     <row r="34" spans="1:27">
-      <c r="A34" s="69"/>
-      <c r="B34" s="49"/>
-      <c r="C34" s="49"/>
-      <c r="D34" s="49"/>
-      <c r="E34" s="49"/>
+      <c r="A34" s="49"/>
+      <c r="B34" s="46"/>
+      <c r="C34" s="46"/>
+      <c r="D34" s="46"/>
+      <c r="E34" s="46"/>
       <c r="F34" s="30"/>
       <c r="G34" s="35"/>
       <c r="H34" s="35"/>
-      <c r="I34" s="55"/>
-      <c r="J34" s="46"/>
-      <c r="K34" s="55"/>
+      <c r="I34" s="54"/>
+      <c r="J34" s="66"/>
+      <c r="K34" s="54"/>
       <c r="L34" s="2"/>
       <c r="M34" s="2"/>
       <c r="N34" s="2"/>
@@ -2446,17 +2376,17 @@
       <c r="AA34" s="2"/>
     </row>
     <row r="35" spans="1:27">
-      <c r="A35" s="70"/>
-      <c r="B35" s="50"/>
-      <c r="C35" s="50"/>
-      <c r="D35" s="50"/>
-      <c r="E35" s="50"/>
+      <c r="A35" s="50"/>
+      <c r="B35" s="47"/>
+      <c r="C35" s="47"/>
+      <c r="D35" s="47"/>
+      <c r="E35" s="47"/>
       <c r="F35" s="30"/>
       <c r="G35" s="35"/>
       <c r="H35" s="35"/>
-      <c r="I35" s="56"/>
-      <c r="J35" s="47"/>
-      <c r="K35" s="56"/>
+      <c r="I35" s="55"/>
+      <c r="J35" s="67"/>
+      <c r="K35" s="55"/>
       <c r="L35" s="2"/>
       <c r="M35" s="2"/>
       <c r="N35" s="2"/>
@@ -2475,21 +2405,21 @@
       <c r="AA35" s="2"/>
     </row>
     <row r="36" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A36" s="68" t="s">
+      <c r="A36" s="48" t="s">
         <v>37</v>
       </c>
-      <c r="B36" s="48"/>
-      <c r="C36" s="51"/>
-      <c r="D36" s="48"/>
-      <c r="E36" s="48"/>
+      <c r="B36" s="45"/>
+      <c r="C36" s="68"/>
+      <c r="D36" s="45"/>
+      <c r="E36" s="45"/>
       <c r="F36" s="30"/>
       <c r="G36" s="35"/>
       <c r="H36" s="35"/>
-      <c r="I36" s="54" t="s">
+      <c r="I36" s="53" t="s">
         <v>26</v>
       </c>
-      <c r="J36" s="45"/>
-      <c r="K36" s="54" t="s">
+      <c r="J36" s="65"/>
+      <c r="K36" s="53" t="s">
         <v>28</v>
       </c>
       <c r="L36" s="2"/>
@@ -2510,17 +2440,17 @@
       <c r="AA36" s="2"/>
     </row>
     <row r="37" spans="1:27">
-      <c r="A37" s="69"/>
-      <c r="B37" s="49"/>
-      <c r="C37" s="52"/>
-      <c r="D37" s="49"/>
-      <c r="E37" s="49"/>
+      <c r="A37" s="49"/>
+      <c r="B37" s="46"/>
+      <c r="C37" s="69"/>
+      <c r="D37" s="46"/>
+      <c r="E37" s="46"/>
       <c r="F37" s="30"/>
       <c r="G37" s="35"/>
       <c r="H37" s="35"/>
-      <c r="I37" s="55"/>
-      <c r="J37" s="46"/>
-      <c r="K37" s="55"/>
+      <c r="I37" s="54"/>
+      <c r="J37" s="66"/>
+      <c r="K37" s="54"/>
       <c r="L37" s="2"/>
       <c r="M37" s="2"/>
       <c r="N37" s="2"/>
@@ -2539,17 +2469,17 @@
       <c r="AA37" s="2"/>
     </row>
     <row r="38" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A38" s="69"/>
-      <c r="B38" s="49"/>
-      <c r="C38" s="52"/>
-      <c r="D38" s="49"/>
-      <c r="E38" s="49"/>
+      <c r="A38" s="49"/>
+      <c r="B38" s="46"/>
+      <c r="C38" s="69"/>
+      <c r="D38" s="46"/>
+      <c r="E38" s="46"/>
       <c r="F38" s="30"/>
       <c r="G38" s="35"/>
       <c r="H38" s="35"/>
-      <c r="I38" s="55"/>
-      <c r="J38" s="46"/>
-      <c r="K38" s="55"/>
+      <c r="I38" s="54"/>
+      <c r="J38" s="66"/>
+      <c r="K38" s="54"/>
       <c r="L38" s="2"/>
       <c r="M38" s="2"/>
       <c r="N38" s="2"/>
@@ -2568,17 +2498,17 @@
       <c r="AA38" s="2"/>
     </row>
     <row r="39" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A39" s="70"/>
-      <c r="B39" s="50"/>
-      <c r="C39" s="53"/>
-      <c r="D39" s="50"/>
-      <c r="E39" s="50"/>
+      <c r="A39" s="50"/>
+      <c r="B39" s="47"/>
+      <c r="C39" s="70"/>
+      <c r="D39" s="47"/>
+      <c r="E39" s="47"/>
       <c r="F39" s="30"/>
       <c r="G39" s="35"/>
       <c r="H39" s="35"/>
-      <c r="I39" s="56"/>
-      <c r="J39" s="47"/>
-      <c r="K39" s="56"/>
+      <c r="I39" s="55"/>
+      <c r="J39" s="67"/>
+      <c r="K39" s="55"/>
       <c r="L39" s="2"/>
       <c r="M39" s="2"/>
       <c r="N39" s="2"/>
@@ -2597,21 +2527,21 @@
       <c r="AA39" s="2"/>
     </row>
     <row r="40" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A40" s="68" t="s">
+      <c r="A40" s="48" t="s">
         <v>38</v>
       </c>
-      <c r="B40" s="48"/>
-      <c r="C40" s="51"/>
-      <c r="D40" s="48"/>
-      <c r="E40" s="48"/>
+      <c r="B40" s="45"/>
+      <c r="C40" s="68"/>
+      <c r="D40" s="45"/>
+      <c r="E40" s="45"/>
       <c r="F40" s="30"/>
       <c r="G40" s="35"/>
       <c r="H40" s="35"/>
-      <c r="I40" s="54" t="s">
+      <c r="I40" s="53" t="s">
         <v>26</v>
       </c>
-      <c r="J40" s="45"/>
-      <c r="K40" s="54" t="s">
+      <c r="J40" s="65"/>
+      <c r="K40" s="53" t="s">
         <v>28</v>
       </c>
       <c r="L40" s="2"/>
@@ -2632,17 +2562,17 @@
       <c r="AA40" s="2"/>
     </row>
     <row r="41" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A41" s="69"/>
-      <c r="B41" s="49"/>
-      <c r="C41" s="52"/>
-      <c r="D41" s="49"/>
-      <c r="E41" s="49"/>
+      <c r="A41" s="49"/>
+      <c r="B41" s="46"/>
+      <c r="C41" s="69"/>
+      <c r="D41" s="46"/>
+      <c r="E41" s="46"/>
       <c r="F41" s="30"/>
       <c r="G41" s="35"/>
       <c r="H41" s="35"/>
-      <c r="I41" s="55"/>
-      <c r="J41" s="46"/>
-      <c r="K41" s="55"/>
+      <c r="I41" s="54"/>
+      <c r="J41" s="66"/>
+      <c r="K41" s="54"/>
       <c r="L41" s="2"/>
       <c r="M41" s="2"/>
       <c r="N41" s="2"/>
@@ -2661,17 +2591,17 @@
       <c r="AA41" s="2"/>
     </row>
     <row r="42" spans="1:27">
-      <c r="A42" s="69"/>
-      <c r="B42" s="49"/>
-      <c r="C42" s="52"/>
-      <c r="D42" s="49"/>
-      <c r="E42" s="49"/>
+      <c r="A42" s="49"/>
+      <c r="B42" s="46"/>
+      <c r="C42" s="69"/>
+      <c r="D42" s="46"/>
+      <c r="E42" s="46"/>
       <c r="F42" s="30"/>
       <c r="G42" s="35"/>
       <c r="H42" s="35"/>
-      <c r="I42" s="55"/>
-      <c r="J42" s="46"/>
-      <c r="K42" s="55"/>
+      <c r="I42" s="54"/>
+      <c r="J42" s="66"/>
+      <c r="K42" s="54"/>
       <c r="L42" s="2"/>
       <c r="M42" s="2"/>
       <c r="N42" s="2"/>
@@ -2690,17 +2620,17 @@
       <c r="AA42" s="2"/>
     </row>
     <row r="43" spans="1:27" ht="18.75" customHeight="1">
-      <c r="A43" s="70"/>
-      <c r="B43" s="50"/>
-      <c r="C43" s="53"/>
-      <c r="D43" s="50"/>
-      <c r="E43" s="50"/>
+      <c r="A43" s="50"/>
+      <c r="B43" s="47"/>
+      <c r="C43" s="70"/>
+      <c r="D43" s="47"/>
+      <c r="E43" s="47"/>
       <c r="F43" s="30"/>
       <c r="G43" s="35"/>
       <c r="H43" s="35"/>
-      <c r="I43" s="56"/>
-      <c r="J43" s="47"/>
-      <c r="K43" s="56"/>
+      <c r="I43" s="55"/>
+      <c r="J43" s="67"/>
+      <c r="K43" s="55"/>
       <c r="L43" s="2"/>
       <c r="M43" s="2"/>
       <c r="N43" s="2"/>
@@ -2719,21 +2649,21 @@
       <c r="AA43" s="2"/>
     </row>
     <row r="44" spans="1:27">
-      <c r="A44" s="68" t="s">
+      <c r="A44" s="48" t="s">
         <v>39</v>
       </c>
-      <c r="B44" s="48"/>
-      <c r="C44" s="48"/>
-      <c r="D44" s="48"/>
-      <c r="E44" s="48"/>
+      <c r="B44" s="45"/>
+      <c r="C44" s="45"/>
+      <c r="D44" s="45"/>
+      <c r="E44" s="45"/>
       <c r="F44" s="30"/>
       <c r="G44" s="35"/>
       <c r="H44" s="35"/>
-      <c r="I44" s="54" t="s">
+      <c r="I44" s="53" t="s">
         <v>26</v>
       </c>
-      <c r="J44" s="45"/>
-      <c r="K44" s="54" t="s">
+      <c r="J44" s="65"/>
+      <c r="K44" s="53" t="s">
         <v>28</v>
       </c>
       <c r="L44" s="2"/>
@@ -2754,17 +2684,17 @@
       <c r="AA44" s="2"/>
     </row>
     <row r="45" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A45" s="69"/>
-      <c r="B45" s="49"/>
-      <c r="C45" s="49"/>
-      <c r="D45" s="49"/>
-      <c r="E45" s="49"/>
+      <c r="A45" s="49"/>
+      <c r="B45" s="46"/>
+      <c r="C45" s="46"/>
+      <c r="D45" s="46"/>
+      <c r="E45" s="46"/>
       <c r="F45" s="30"/>
       <c r="G45" s="35"/>
       <c r="H45" s="35"/>
-      <c r="I45" s="55"/>
-      <c r="J45" s="46"/>
-      <c r="K45" s="55"/>
+      <c r="I45" s="54"/>
+      <c r="J45" s="66"/>
+      <c r="K45" s="54"/>
       <c r="L45" s="2"/>
       <c r="M45" s="2"/>
       <c r="N45" s="2"/>
@@ -2783,17 +2713,17 @@
       <c r="AA45" s="2"/>
     </row>
     <row r="46" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A46" s="69"/>
-      <c r="B46" s="49"/>
-      <c r="C46" s="49"/>
-      <c r="D46" s="49"/>
-      <c r="E46" s="49"/>
+      <c r="A46" s="49"/>
+      <c r="B46" s="46"/>
+      <c r="C46" s="46"/>
+      <c r="D46" s="46"/>
+      <c r="E46" s="46"/>
       <c r="F46" s="30"/>
       <c r="G46" s="35"/>
       <c r="H46" s="35"/>
-      <c r="I46" s="55"/>
-      <c r="J46" s="46"/>
-      <c r="K46" s="55"/>
+      <c r="I46" s="54"/>
+      <c r="J46" s="66"/>
+      <c r="K46" s="54"/>
       <c r="L46" s="2"/>
       <c r="M46" s="2"/>
       <c r="N46" s="2"/>
@@ -2812,17 +2742,17 @@
       <c r="AA46" s="2"/>
     </row>
     <row r="47" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A47" s="70"/>
-      <c r="B47" s="50"/>
-      <c r="C47" s="50"/>
-      <c r="D47" s="50"/>
-      <c r="E47" s="50"/>
+      <c r="A47" s="50"/>
+      <c r="B47" s="47"/>
+      <c r="C47" s="47"/>
+      <c r="D47" s="47"/>
+      <c r="E47" s="47"/>
       <c r="F47" s="30"/>
       <c r="G47" s="35"/>
       <c r="H47" s="35"/>
-      <c r="I47" s="56"/>
-      <c r="J47" s="47"/>
-      <c r="K47" s="56"/>
+      <c r="I47" s="55"/>
+      <c r="J47" s="67"/>
+      <c r="K47" s="55"/>
       <c r="L47" s="2"/>
       <c r="M47" s="2"/>
       <c r="N47" s="2"/>
@@ -2841,21 +2771,21 @@
       <c r="AA47" s="2"/>
     </row>
     <row r="48" spans="1:27">
-      <c r="A48" s="68" t="s">
+      <c r="A48" s="48" t="s">
         <v>40</v>
       </c>
-      <c r="B48" s="48"/>
-      <c r="C48" s="48"/>
-      <c r="D48" s="48"/>
-      <c r="E48" s="48"/>
+      <c r="B48" s="45"/>
+      <c r="C48" s="45"/>
+      <c r="D48" s="45"/>
+      <c r="E48" s="45"/>
       <c r="F48" s="30"/>
       <c r="G48" s="35"/>
       <c r="H48" s="35"/>
-      <c r="I48" s="54" t="s">
+      <c r="I48" s="53" t="s">
         <v>26</v>
       </c>
-      <c r="J48" s="45"/>
-      <c r="K48" s="54" t="s">
+      <c r="J48" s="65"/>
+      <c r="K48" s="53" t="s">
         <v>28</v>
       </c>
       <c r="L48" s="2"/>
@@ -2876,17 +2806,17 @@
       <c r="AA48" s="2"/>
     </row>
     <row r="49" spans="1:27">
-      <c r="A49" s="69"/>
-      <c r="B49" s="49"/>
-      <c r="C49" s="49"/>
-      <c r="D49" s="49"/>
-      <c r="E49" s="49"/>
+      <c r="A49" s="49"/>
+      <c r="B49" s="46"/>
+      <c r="C49" s="46"/>
+      <c r="D49" s="46"/>
+      <c r="E49" s="46"/>
       <c r="F49" s="30"/>
       <c r="G49" s="43"/>
       <c r="H49" s="43"/>
-      <c r="I49" s="55"/>
-      <c r="J49" s="46"/>
-      <c r="K49" s="55"/>
+      <c r="I49" s="54"/>
+      <c r="J49" s="66"/>
+      <c r="K49" s="54"/>
       <c r="L49" s="2"/>
       <c r="M49" s="2"/>
       <c r="N49" s="2"/>
@@ -2905,17 +2835,17 @@
       <c r="AA49" s="2"/>
     </row>
     <row r="50" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A50" s="69"/>
-      <c r="B50" s="49"/>
-      <c r="C50" s="49"/>
-      <c r="D50" s="49"/>
-      <c r="E50" s="49"/>
+      <c r="A50" s="49"/>
+      <c r="B50" s="46"/>
+      <c r="C50" s="46"/>
+      <c r="D50" s="46"/>
+      <c r="E50" s="46"/>
       <c r="F50" s="30"/>
       <c r="G50" s="43"/>
       <c r="H50" s="43"/>
-      <c r="I50" s="55"/>
-      <c r="J50" s="46"/>
-      <c r="K50" s="55"/>
+      <c r="I50" s="54"/>
+      <c r="J50" s="66"/>
+      <c r="K50" s="54"/>
       <c r="L50" s="2"/>
       <c r="M50" s="2"/>
       <c r="N50" s="2"/>
@@ -2934,17 +2864,17 @@
       <c r="AA50" s="2"/>
     </row>
     <row r="51" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A51" s="70"/>
-      <c r="B51" s="50"/>
-      <c r="C51" s="50"/>
-      <c r="D51" s="50"/>
-      <c r="E51" s="50"/>
+      <c r="A51" s="50"/>
+      <c r="B51" s="47"/>
+      <c r="C51" s="47"/>
+      <c r="D51" s="47"/>
+      <c r="E51" s="47"/>
       <c r="F51" s="30"/>
       <c r="G51" s="35"/>
       <c r="H51" s="35"/>
-      <c r="I51" s="56"/>
-      <c r="J51" s="47"/>
-      <c r="K51" s="56"/>
+      <c r="I51" s="55"/>
+      <c r="J51" s="67"/>
+      <c r="K51" s="55"/>
       <c r="L51" s="2"/>
       <c r="M51" s="2"/>
       <c r="N51" s="2"/>
@@ -2963,21 +2893,21 @@
       <c r="AA51" s="2"/>
     </row>
     <row r="52" spans="1:27">
-      <c r="A52" s="68" t="s">
+      <c r="A52" s="48" t="s">
         <v>41</v>
       </c>
-      <c r="B52" s="48"/>
-      <c r="C52" s="48"/>
-      <c r="D52" s="48"/>
-      <c r="E52" s="48"/>
+      <c r="B52" s="45"/>
+      <c r="C52" s="45"/>
+      <c r="D52" s="45"/>
+      <c r="E52" s="45"/>
       <c r="F52" s="30"/>
       <c r="G52" s="35"/>
       <c r="H52" s="35"/>
-      <c r="I52" s="54" t="s">
+      <c r="I52" s="53" t="s">
         <v>26</v>
       </c>
-      <c r="J52" s="45"/>
-      <c r="K52" s="54" t="s">
+      <c r="J52" s="65"/>
+      <c r="K52" s="53" t="s">
         <v>28</v>
       </c>
       <c r="L52" s="2"/>
@@ -2998,17 +2928,17 @@
       <c r="AA52" s="2"/>
     </row>
     <row r="53" spans="1:27">
-      <c r="A53" s="69"/>
-      <c r="B53" s="49"/>
-      <c r="C53" s="49"/>
-      <c r="D53" s="49"/>
-      <c r="E53" s="49"/>
+      <c r="A53" s="49"/>
+      <c r="B53" s="46"/>
+      <c r="C53" s="46"/>
+      <c r="D53" s="46"/>
+      <c r="E53" s="46"/>
       <c r="F53" s="30"/>
       <c r="G53" s="35"/>
       <c r="H53" s="35"/>
-      <c r="I53" s="55"/>
-      <c r="J53" s="46"/>
-      <c r="K53" s="55"/>
+      <c r="I53" s="54"/>
+      <c r="J53" s="66"/>
+      <c r="K53" s="54"/>
       <c r="L53" s="2"/>
       <c r="M53" s="2"/>
       <c r="N53" s="2"/>
@@ -3027,17 +2957,17 @@
       <c r="AA53" s="2"/>
     </row>
     <row r="54" spans="1:27">
-      <c r="A54" s="69"/>
-      <c r="B54" s="49"/>
-      <c r="C54" s="49"/>
-      <c r="D54" s="49"/>
-      <c r="E54" s="49"/>
+      <c r="A54" s="49"/>
+      <c r="B54" s="46"/>
+      <c r="C54" s="46"/>
+      <c r="D54" s="46"/>
+      <c r="E54" s="46"/>
       <c r="F54" s="30"/>
       <c r="G54" s="35"/>
       <c r="H54" s="35"/>
-      <c r="I54" s="55"/>
-      <c r="J54" s="46"/>
-      <c r="K54" s="55"/>
+      <c r="I54" s="54"/>
+      <c r="J54" s="66"/>
+      <c r="K54" s="54"/>
       <c r="L54" s="2"/>
       <c r="M54" s="2"/>
       <c r="N54" s="2"/>
@@ -3056,17 +2986,17 @@
       <c r="AA54" s="2"/>
     </row>
     <row r="55" spans="1:27">
-      <c r="A55" s="70"/>
-      <c r="B55" s="50"/>
-      <c r="C55" s="50"/>
-      <c r="D55" s="50"/>
-      <c r="E55" s="50"/>
+      <c r="A55" s="50"/>
+      <c r="B55" s="47"/>
+      <c r="C55" s="47"/>
+      <c r="D55" s="47"/>
+      <c r="E55" s="47"/>
       <c r="F55" s="30"/>
       <c r="G55" s="35"/>
       <c r="H55" s="35"/>
-      <c r="I55" s="56"/>
-      <c r="J55" s="47"/>
-      <c r="K55" s="56"/>
+      <c r="I55" s="55"/>
+      <c r="J55" s="67"/>
+      <c r="K55" s="55"/>
       <c r="L55" s="2"/>
       <c r="M55" s="2"/>
       <c r="N55" s="2"/>
@@ -3085,21 +3015,21 @@
       <c r="AA55" s="2"/>
     </row>
     <row r="56" spans="1:27">
-      <c r="A56" s="68" t="s">
+      <c r="A56" s="48" t="s">
         <v>42</v>
       </c>
-      <c r="B56" s="48"/>
-      <c r="C56" s="48"/>
-      <c r="D56" s="48"/>
-      <c r="E56" s="48"/>
+      <c r="B56" s="45"/>
+      <c r="C56" s="45"/>
+      <c r="D56" s="45"/>
+      <c r="E56" s="45"/>
       <c r="F56" s="30"/>
       <c r="G56" s="35"/>
       <c r="H56" s="35"/>
-      <c r="I56" s="54" t="s">
+      <c r="I56" s="53" t="s">
         <v>26</v>
       </c>
-      <c r="J56" s="45"/>
-      <c r="K56" s="54" t="s">
+      <c r="J56" s="65"/>
+      <c r="K56" s="53" t="s">
         <v>28</v>
       </c>
       <c r="L56" s="2"/>
@@ -3120,17 +3050,17 @@
       <c r="AA56" s="2"/>
     </row>
     <row r="57" spans="1:27">
-      <c r="A57" s="69"/>
-      <c r="B57" s="49"/>
-      <c r="C57" s="49"/>
-      <c r="D57" s="49"/>
-      <c r="E57" s="49"/>
+      <c r="A57" s="49"/>
+      <c r="B57" s="46"/>
+      <c r="C57" s="46"/>
+      <c r="D57" s="46"/>
+      <c r="E57" s="46"/>
       <c r="F57" s="30"/>
       <c r="G57" s="35"/>
       <c r="H57" s="35"/>
-      <c r="I57" s="55"/>
-      <c r="J57" s="46"/>
-      <c r="K57" s="55"/>
+      <c r="I57" s="54"/>
+      <c r="J57" s="66"/>
+      <c r="K57" s="54"/>
       <c r="L57" s="2"/>
       <c r="M57" s="2"/>
       <c r="N57" s="2"/>
@@ -3149,17 +3079,17 @@
       <c r="AA57" s="2"/>
     </row>
     <row r="58" spans="1:27">
-      <c r="A58" s="69"/>
-      <c r="B58" s="49"/>
-      <c r="C58" s="49"/>
-      <c r="D58" s="49"/>
-      <c r="E58" s="49"/>
+      <c r="A58" s="49"/>
+      <c r="B58" s="46"/>
+      <c r="C58" s="46"/>
+      <c r="D58" s="46"/>
+      <c r="E58" s="46"/>
       <c r="F58" s="30"/>
       <c r="G58" s="35"/>
       <c r="H58" s="35"/>
-      <c r="I58" s="55"/>
-      <c r="J58" s="46"/>
-      <c r="K58" s="55"/>
+      <c r="I58" s="54"/>
+      <c r="J58" s="66"/>
+      <c r="K58" s="54"/>
       <c r="L58" s="2"/>
       <c r="M58" s="2"/>
       <c r="N58" s="2"/>
@@ -3178,17 +3108,17 @@
       <c r="AA58" s="2"/>
     </row>
     <row r="59" spans="1:27">
-      <c r="A59" s="70"/>
-      <c r="B59" s="50"/>
-      <c r="C59" s="50"/>
-      <c r="D59" s="50"/>
-      <c r="E59" s="50"/>
+      <c r="A59" s="50"/>
+      <c r="B59" s="47"/>
+      <c r="C59" s="47"/>
+      <c r="D59" s="47"/>
+      <c r="E59" s="47"/>
       <c r="F59" s="30"/>
       <c r="G59" s="35"/>
       <c r="H59" s="35"/>
-      <c r="I59" s="56"/>
-      <c r="J59" s="47"/>
-      <c r="K59" s="56"/>
+      <c r="I59" s="55"/>
+      <c r="J59" s="67"/>
+      <c r="K59" s="55"/>
       <c r="L59" s="2"/>
       <c r="M59" s="2"/>
       <c r="N59" s="2"/>
@@ -3207,21 +3137,21 @@
       <c r="AA59" s="2"/>
     </row>
     <row r="60" spans="1:27">
-      <c r="A60" s="68" t="s">
+      <c r="A60" s="48" t="s">
         <v>43</v>
       </c>
-      <c r="B60" s="48"/>
-      <c r="C60" s="48"/>
-      <c r="D60" s="48"/>
-      <c r="E60" s="48"/>
+      <c r="B60" s="45"/>
+      <c r="C60" s="45"/>
+      <c r="D60" s="45"/>
+      <c r="E60" s="45"/>
       <c r="F60" s="30"/>
       <c r="G60" s="35"/>
       <c r="H60" s="35"/>
-      <c r="I60" s="54" t="s">
+      <c r="I60" s="53" t="s">
         <v>26</v>
       </c>
-      <c r="J60" s="45"/>
-      <c r="K60" s="54" t="s">
+      <c r="J60" s="65"/>
+      <c r="K60" s="53" t="s">
         <v>28</v>
       </c>
       <c r="L60" s="2"/>
@@ -3242,17 +3172,17 @@
       <c r="AA60" s="2"/>
     </row>
     <row r="61" spans="1:27">
-      <c r="A61" s="69"/>
-      <c r="B61" s="49"/>
-      <c r="C61" s="49"/>
-      <c r="D61" s="49"/>
-      <c r="E61" s="49"/>
+      <c r="A61" s="49"/>
+      <c r="B61" s="46"/>
+      <c r="C61" s="46"/>
+      <c r="D61" s="46"/>
+      <c r="E61" s="46"/>
       <c r="F61" s="30"/>
       <c r="G61" s="35"/>
       <c r="H61" s="35"/>
-      <c r="I61" s="55"/>
-      <c r="J61" s="46"/>
-      <c r="K61" s="55"/>
+      <c r="I61" s="54"/>
+      <c r="J61" s="66"/>
+      <c r="K61" s="54"/>
       <c r="L61" s="2"/>
       <c r="M61" s="2"/>
       <c r="N61" s="2"/>
@@ -3271,17 +3201,17 @@
       <c r="AA61" s="2"/>
     </row>
     <row r="62" spans="1:27">
-      <c r="A62" s="69"/>
-      <c r="B62" s="49"/>
-      <c r="C62" s="49"/>
-      <c r="D62" s="49"/>
-      <c r="E62" s="49"/>
+      <c r="A62" s="49"/>
+      <c r="B62" s="46"/>
+      <c r="C62" s="46"/>
+      <c r="D62" s="46"/>
+      <c r="E62" s="46"/>
       <c r="F62" s="30"/>
       <c r="G62" s="35"/>
       <c r="H62" s="35"/>
-      <c r="I62" s="55"/>
-      <c r="J62" s="46"/>
-      <c r="K62" s="55"/>
+      <c r="I62" s="54"/>
+      <c r="J62" s="66"/>
+      <c r="K62" s="54"/>
       <c r="L62" s="2"/>
       <c r="M62" s="2"/>
       <c r="N62" s="2"/>
@@ -3300,17 +3230,17 @@
       <c r="AA62" s="2"/>
     </row>
     <row r="63" spans="1:27">
-      <c r="A63" s="70"/>
-      <c r="B63" s="50"/>
-      <c r="C63" s="50"/>
-      <c r="D63" s="50"/>
-      <c r="E63" s="50"/>
+      <c r="A63" s="50"/>
+      <c r="B63" s="47"/>
+      <c r="C63" s="47"/>
+      <c r="D63" s="47"/>
+      <c r="E63" s="47"/>
       <c r="F63" s="30"/>
       <c r="G63" s="35"/>
       <c r="H63" s="36"/>
-      <c r="I63" s="56"/>
-      <c r="J63" s="47"/>
-      <c r="K63" s="56"/>
+      <c r="I63" s="55"/>
+      <c r="J63" s="67"/>
+      <c r="K63" s="55"/>
       <c r="L63" s="2"/>
       <c r="M63" s="2"/>
       <c r="N63" s="2"/>
@@ -3329,21 +3259,21 @@
       <c r="AA63" s="2"/>
     </row>
     <row r="64" spans="1:27">
-      <c r="A64" s="68" t="s">
+      <c r="A64" s="48" t="s">
         <v>44</v>
       </c>
-      <c r="B64" s="48"/>
-      <c r="C64" s="48"/>
-      <c r="D64" s="48"/>
-      <c r="E64" s="48"/>
+      <c r="B64" s="45"/>
+      <c r="C64" s="45"/>
+      <c r="D64" s="45"/>
+      <c r="E64" s="45"/>
       <c r="F64" s="30"/>
       <c r="G64" s="35"/>
       <c r="H64" s="35"/>
-      <c r="I64" s="54" t="s">
+      <c r="I64" s="53" t="s">
         <v>26</v>
       </c>
-      <c r="J64" s="45"/>
-      <c r="K64" s="54" t="s">
+      <c r="J64" s="65"/>
+      <c r="K64" s="53" t="s">
         <v>28</v>
       </c>
       <c r="L64" s="2"/>
@@ -3364,17 +3294,17 @@
       <c r="AA64" s="2"/>
     </row>
     <row r="65" spans="1:27">
-      <c r="A65" s="69"/>
-      <c r="B65" s="49"/>
-      <c r="C65" s="49"/>
-      <c r="D65" s="49"/>
-      <c r="E65" s="49"/>
+      <c r="A65" s="49"/>
+      <c r="B65" s="46"/>
+      <c r="C65" s="46"/>
+      <c r="D65" s="46"/>
+      <c r="E65" s="46"/>
       <c r="F65" s="30"/>
       <c r="G65" s="35"/>
       <c r="H65" s="35"/>
-      <c r="I65" s="55"/>
-      <c r="J65" s="46"/>
-      <c r="K65" s="55"/>
+      <c r="I65" s="54"/>
+      <c r="J65" s="66"/>
+      <c r="K65" s="54"/>
       <c r="L65" s="2"/>
       <c r="M65" s="2"/>
       <c r="N65" s="2"/>
@@ -3393,17 +3323,17 @@
       <c r="AA65" s="2"/>
     </row>
     <row r="66" spans="1:27">
-      <c r="A66" s="69"/>
-      <c r="B66" s="49"/>
-      <c r="C66" s="49"/>
-      <c r="D66" s="49"/>
-      <c r="E66" s="49"/>
+      <c r="A66" s="49"/>
+      <c r="B66" s="46"/>
+      <c r="C66" s="46"/>
+      <c r="D66" s="46"/>
+      <c r="E66" s="46"/>
       <c r="F66" s="30"/>
       <c r="G66" s="35"/>
       <c r="H66" s="35"/>
-      <c r="I66" s="55"/>
-      <c r="J66" s="46"/>
-      <c r="K66" s="55"/>
+      <c r="I66" s="54"/>
+      <c r="J66" s="66"/>
+      <c r="K66" s="54"/>
       <c r="L66" s="2"/>
       <c r="M66" s="2"/>
       <c r="N66" s="2"/>
@@ -3422,17 +3352,17 @@
       <c r="AA66" s="2"/>
     </row>
     <row r="67" spans="1:27">
-      <c r="A67" s="70"/>
-      <c r="B67" s="50"/>
-      <c r="C67" s="50"/>
-      <c r="D67" s="50"/>
-      <c r="E67" s="50"/>
+      <c r="A67" s="50"/>
+      <c r="B67" s="47"/>
+      <c r="C67" s="47"/>
+      <c r="D67" s="47"/>
+      <c r="E67" s="47"/>
       <c r="F67" s="30"/>
       <c r="G67" s="35"/>
       <c r="H67" s="36"/>
-      <c r="I67" s="56"/>
-      <c r="J67" s="47"/>
-      <c r="K67" s="56"/>
+      <c r="I67" s="55"/>
+      <c r="J67" s="67"/>
+      <c r="K67" s="55"/>
       <c r="L67" s="2"/>
       <c r="M67" s="2"/>
       <c r="N67" s="2"/>
@@ -3451,21 +3381,21 @@
       <c r="AA67" s="2"/>
     </row>
     <row r="68" spans="1:27">
-      <c r="A68" s="68" t="s">
+      <c r="A68" s="48" t="s">
         <v>45</v>
       </c>
-      <c r="B68" s="48"/>
-      <c r="C68" s="48"/>
-      <c r="D68" s="48"/>
-      <c r="E68" s="48"/>
+      <c r="B68" s="45"/>
+      <c r="C68" s="45"/>
+      <c r="D68" s="45"/>
+      <c r="E68" s="45"/>
       <c r="F68" s="30"/>
       <c r="G68" s="35"/>
       <c r="H68" s="35"/>
-      <c r="I68" s="54" t="s">
+      <c r="I68" s="53" t="s">
         <v>26</v>
       </c>
-      <c r="J68" s="45"/>
-      <c r="K68" s="54" t="s">
+      <c r="J68" s="65"/>
+      <c r="K68" s="53" t="s">
         <v>28</v>
       </c>
       <c r="L68" s="2"/>
@@ -3486,17 +3416,17 @@
       <c r="AA68" s="2"/>
     </row>
     <row r="69" spans="1:27">
-      <c r="A69" s="69"/>
-      <c r="B69" s="49"/>
-      <c r="C69" s="49"/>
-      <c r="D69" s="49"/>
-      <c r="E69" s="49"/>
+      <c r="A69" s="49"/>
+      <c r="B69" s="46"/>
+      <c r="C69" s="46"/>
+      <c r="D69" s="46"/>
+      <c r="E69" s="46"/>
       <c r="F69" s="30"/>
       <c r="G69" s="36"/>
       <c r="H69" s="36"/>
-      <c r="I69" s="55"/>
-      <c r="J69" s="46"/>
-      <c r="K69" s="55"/>
+      <c r="I69" s="54"/>
+      <c r="J69" s="66"/>
+      <c r="K69" s="54"/>
       <c r="L69" s="2"/>
       <c r="M69" s="2"/>
       <c r="N69" s="2"/>
@@ -3515,17 +3445,17 @@
       <c r="AA69" s="2"/>
     </row>
     <row r="70" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A70" s="69"/>
-      <c r="B70" s="49"/>
-      <c r="C70" s="49"/>
-      <c r="D70" s="49"/>
-      <c r="E70" s="49"/>
+      <c r="A70" s="49"/>
+      <c r="B70" s="46"/>
+      <c r="C70" s="46"/>
+      <c r="D70" s="46"/>
+      <c r="E70" s="46"/>
       <c r="F70" s="30"/>
       <c r="G70" s="43"/>
       <c r="H70" s="43"/>
-      <c r="I70" s="55"/>
-      <c r="J70" s="46"/>
-      <c r="K70" s="55"/>
+      <c r="I70" s="54"/>
+      <c r="J70" s="66"/>
+      <c r="K70" s="54"/>
       <c r="L70" s="2"/>
       <c r="M70" s="2"/>
       <c r="N70" s="2"/>
@@ -3544,17 +3474,17 @@
       <c r="AA70" s="2"/>
     </row>
     <row r="71" spans="1:27">
-      <c r="A71" s="70"/>
-      <c r="B71" s="50"/>
-      <c r="C71" s="50"/>
-      <c r="D71" s="50"/>
-      <c r="E71" s="50"/>
+      <c r="A71" s="50"/>
+      <c r="B71" s="47"/>
+      <c r="C71" s="47"/>
+      <c r="D71" s="47"/>
+      <c r="E71" s="47"/>
       <c r="F71" s="30"/>
       <c r="G71" s="43"/>
       <c r="H71" s="43"/>
-      <c r="I71" s="56"/>
-      <c r="J71" s="47"/>
-      <c r="K71" s="56"/>
+      <c r="I71" s="55"/>
+      <c r="J71" s="67"/>
+      <c r="K71" s="55"/>
       <c r="L71" s="2"/>
       <c r="M71" s="2"/>
       <c r="N71" s="2"/>
@@ -3573,21 +3503,21 @@
       <c r="AA71" s="2"/>
     </row>
     <row r="72" spans="1:27">
-      <c r="A72" s="68" t="s">
+      <c r="A72" s="48" t="s">
         <v>46</v>
       </c>
-      <c r="B72" s="48"/>
-      <c r="C72" s="48"/>
-      <c r="D72" s="48"/>
-      <c r="E72" s="48"/>
+      <c r="B72" s="45"/>
+      <c r="C72" s="45"/>
+      <c r="D72" s="45"/>
+      <c r="E72" s="45"/>
       <c r="F72" s="30"/>
       <c r="G72" s="35"/>
       <c r="H72" s="35"/>
-      <c r="I72" s="54" t="s">
+      <c r="I72" s="53" t="s">
         <v>26</v>
       </c>
-      <c r="J72" s="45"/>
-      <c r="K72" s="54" t="s">
+      <c r="J72" s="65"/>
+      <c r="K72" s="53" t="s">
         <v>28</v>
       </c>
       <c r="L72" s="2"/>
@@ -3608,17 +3538,17 @@
       <c r="AA72" s="2"/>
     </row>
     <row r="73" spans="1:27">
-      <c r="A73" s="69"/>
-      <c r="B73" s="49"/>
-      <c r="C73" s="49"/>
-      <c r="D73" s="49"/>
-      <c r="E73" s="49"/>
+      <c r="A73" s="49"/>
+      <c r="B73" s="46"/>
+      <c r="C73" s="46"/>
+      <c r="D73" s="46"/>
+      <c r="E73" s="46"/>
       <c r="F73" s="30"/>
       <c r="G73" s="36"/>
       <c r="H73" s="36"/>
-      <c r="I73" s="55"/>
-      <c r="J73" s="46"/>
-      <c r="K73" s="55"/>
+      <c r="I73" s="54"/>
+      <c r="J73" s="66"/>
+      <c r="K73" s="54"/>
       <c r="L73" s="2"/>
       <c r="M73" s="2"/>
       <c r="N73" s="2"/>
@@ -3637,17 +3567,17 @@
       <c r="AA73" s="2"/>
     </row>
     <row r="74" spans="1:27">
-      <c r="A74" s="69"/>
-      <c r="B74" s="49"/>
-      <c r="C74" s="49"/>
-      <c r="D74" s="49"/>
-      <c r="E74" s="49"/>
+      <c r="A74" s="49"/>
+      <c r="B74" s="46"/>
+      <c r="C74" s="46"/>
+      <c r="D74" s="46"/>
+      <c r="E74" s="46"/>
       <c r="F74" s="30"/>
       <c r="G74" s="36"/>
       <c r="H74" s="36"/>
-      <c r="I74" s="55"/>
-      <c r="J74" s="46"/>
-      <c r="K74" s="55"/>
+      <c r="I74" s="54"/>
+      <c r="J74" s="66"/>
+      <c r="K74" s="54"/>
       <c r="L74" s="2"/>
       <c r="M74" s="2"/>
       <c r="N74" s="2"/>
@@ -3666,17 +3596,17 @@
       <c r="AA74" s="2"/>
     </row>
     <row r="75" spans="1:27">
-      <c r="A75" s="70"/>
-      <c r="B75" s="50"/>
-      <c r="C75" s="50"/>
-      <c r="D75" s="50"/>
-      <c r="E75" s="50"/>
+      <c r="A75" s="50"/>
+      <c r="B75" s="47"/>
+      <c r="C75" s="47"/>
+      <c r="D75" s="47"/>
+      <c r="E75" s="47"/>
       <c r="F75" s="30"/>
       <c r="G75" s="35"/>
       <c r="H75" s="36"/>
-      <c r="I75" s="56"/>
-      <c r="J75" s="47"/>
-      <c r="K75" s="56"/>
+      <c r="I75" s="55"/>
+      <c r="J75" s="67"/>
+      <c r="K75" s="55"/>
       <c r="L75" s="2"/>
       <c r="M75" s="2"/>
       <c r="N75" s="2"/>
@@ -3695,21 +3625,21 @@
       <c r="AA75" s="2"/>
     </row>
     <row r="76" spans="1:27">
-      <c r="A76" s="68" t="s">
+      <c r="A76" s="48" t="s">
         <v>47</v>
       </c>
-      <c r="B76" s="48"/>
-      <c r="C76" s="48"/>
-      <c r="D76" s="48"/>
-      <c r="E76" s="48"/>
+      <c r="B76" s="45"/>
+      <c r="C76" s="45"/>
+      <c r="D76" s="45"/>
+      <c r="E76" s="45"/>
       <c r="F76" s="30"/>
       <c r="G76" s="35"/>
       <c r="H76" s="35"/>
-      <c r="I76" s="54" t="s">
+      <c r="I76" s="53" t="s">
         <v>26</v>
       </c>
-      <c r="J76" s="45"/>
-      <c r="K76" s="54" t="s">
+      <c r="J76" s="65"/>
+      <c r="K76" s="53" t="s">
         <v>28</v>
       </c>
       <c r="L76" s="2"/>
@@ -3730,17 +3660,17 @@
       <c r="AA76" s="2"/>
     </row>
     <row r="77" spans="1:27">
-      <c r="A77" s="69"/>
-      <c r="B77" s="49"/>
-      <c r="C77" s="49"/>
-      <c r="D77" s="49"/>
-      <c r="E77" s="49"/>
+      <c r="A77" s="49"/>
+      <c r="B77" s="46"/>
+      <c r="C77" s="46"/>
+      <c r="D77" s="46"/>
+      <c r="E77" s="46"/>
       <c r="F77" s="30"/>
       <c r="G77" s="35"/>
       <c r="H77" s="36"/>
-      <c r="I77" s="55"/>
-      <c r="J77" s="46"/>
-      <c r="K77" s="55"/>
+      <c r="I77" s="54"/>
+      <c r="J77" s="66"/>
+      <c r="K77" s="54"/>
       <c r="L77" s="2"/>
       <c r="M77" s="2"/>
       <c r="N77" s="2"/>
@@ -3759,17 +3689,17 @@
       <c r="AA77" s="2"/>
     </row>
     <row r="78" spans="1:27">
-      <c r="A78" s="69"/>
-      <c r="B78" s="49"/>
-      <c r="C78" s="49"/>
-      <c r="D78" s="49"/>
-      <c r="E78" s="49"/>
+      <c r="A78" s="49"/>
+      <c r="B78" s="46"/>
+      <c r="C78" s="46"/>
+      <c r="D78" s="46"/>
+      <c r="E78" s="46"/>
       <c r="F78" s="30"/>
       <c r="G78" s="36"/>
       <c r="H78" s="36"/>
-      <c r="I78" s="55"/>
-      <c r="J78" s="46"/>
-      <c r="K78" s="55"/>
+      <c r="I78" s="54"/>
+      <c r="J78" s="66"/>
+      <c r="K78" s="54"/>
       <c r="L78" s="2"/>
       <c r="M78" s="2"/>
       <c r="N78" s="2"/>
@@ -3788,17 +3718,17 @@
       <c r="AA78" s="2"/>
     </row>
     <row r="79" spans="1:27">
-      <c r="A79" s="70"/>
-      <c r="B79" s="50"/>
-      <c r="C79" s="50"/>
-      <c r="D79" s="50"/>
-      <c r="E79" s="50"/>
+      <c r="A79" s="50"/>
+      <c r="B79" s="47"/>
+      <c r="C79" s="47"/>
+      <c r="D79" s="47"/>
+      <c r="E79" s="47"/>
       <c r="F79" s="30"/>
       <c r="G79" s="35"/>
       <c r="H79" s="35"/>
-      <c r="I79" s="56"/>
-      <c r="J79" s="47"/>
-      <c r="K79" s="56"/>
+      <c r="I79" s="55"/>
+      <c r="J79" s="67"/>
+      <c r="K79" s="55"/>
       <c r="L79" s="2"/>
       <c r="M79" s="2"/>
       <c r="N79" s="2"/>
@@ -3817,21 +3747,21 @@
       <c r="AA79" s="2"/>
     </row>
     <row r="80" spans="1:27">
-      <c r="A80" s="68" t="s">
+      <c r="A80" s="48" t="s">
         <v>48</v>
       </c>
-      <c r="B80" s="48"/>
-      <c r="C80" s="51"/>
-      <c r="D80" s="48"/>
-      <c r="E80" s="48"/>
+      <c r="B80" s="45"/>
+      <c r="C80" s="68"/>
+      <c r="D80" s="45"/>
+      <c r="E80" s="45"/>
       <c r="F80" s="30"/>
       <c r="G80" s="35"/>
       <c r="H80" s="35"/>
-      <c r="I80" s="54" t="s">
+      <c r="I80" s="53" t="s">
         <v>26</v>
       </c>
-      <c r="J80" s="45"/>
-      <c r="K80" s="54" t="s">
+      <c r="J80" s="65"/>
+      <c r="K80" s="53" t="s">
         <v>28</v>
       </c>
       <c r="L80" s="2"/>
@@ -3852,17 +3782,17 @@
       <c r="AA80" s="2"/>
     </row>
     <row r="81" spans="1:27">
-      <c r="A81" s="69"/>
-      <c r="B81" s="49"/>
-      <c r="C81" s="52"/>
-      <c r="D81" s="49"/>
-      <c r="E81" s="49"/>
+      <c r="A81" s="49"/>
+      <c r="B81" s="46"/>
+      <c r="C81" s="69"/>
+      <c r="D81" s="46"/>
+      <c r="E81" s="46"/>
       <c r="F81" s="30"/>
       <c r="G81" s="35"/>
       <c r="H81" s="35"/>
-      <c r="I81" s="55"/>
-      <c r="J81" s="46"/>
-      <c r="K81" s="55"/>
+      <c r="I81" s="54"/>
+      <c r="J81" s="66"/>
+      <c r="K81" s="54"/>
       <c r="L81" s="2"/>
       <c r="M81" s="2"/>
       <c r="N81" s="2"/>
@@ -3881,17 +3811,17 @@
       <c r="AA81" s="2"/>
     </row>
     <row r="82" spans="1:27">
-      <c r="A82" s="69"/>
-      <c r="B82" s="49"/>
-      <c r="C82" s="52"/>
-      <c r="D82" s="49"/>
-      <c r="E82" s="49"/>
+      <c r="A82" s="49"/>
+      <c r="B82" s="46"/>
+      <c r="C82" s="69"/>
+      <c r="D82" s="46"/>
+      <c r="E82" s="46"/>
       <c r="F82" s="30"/>
       <c r="G82" s="35"/>
       <c r="H82" s="35"/>
-      <c r="I82" s="55"/>
-      <c r="J82" s="46"/>
-      <c r="K82" s="55"/>
+      <c r="I82" s="54"/>
+      <c r="J82" s="66"/>
+      <c r="K82" s="54"/>
       <c r="L82" s="2"/>
       <c r="M82" s="2"/>
       <c r="N82" s="2"/>
@@ -3910,17 +3840,17 @@
       <c r="AA82" s="2"/>
     </row>
     <row r="83" spans="1:27">
-      <c r="A83" s="70"/>
-      <c r="B83" s="50"/>
-      <c r="C83" s="53"/>
-      <c r="D83" s="50"/>
-      <c r="E83" s="50"/>
+      <c r="A83" s="50"/>
+      <c r="B83" s="47"/>
+      <c r="C83" s="70"/>
+      <c r="D83" s="47"/>
+      <c r="E83" s="47"/>
       <c r="F83" s="30"/>
       <c r="G83" s="35"/>
       <c r="H83" s="35"/>
-      <c r="I83" s="56"/>
-      <c r="J83" s="47"/>
-      <c r="K83" s="56"/>
+      <c r="I83" s="55"/>
+      <c r="J83" s="67"/>
+      <c r="K83" s="55"/>
       <c r="L83" s="2"/>
       <c r="M83" s="2"/>
       <c r="N83" s="2"/>
@@ -28648,28 +28578,138 @@
     </row>
   </sheetData>
   <mergeCells count="178">
-    <mergeCell ref="C32:C35"/>
-    <mergeCell ref="B32:B35"/>
-    <mergeCell ref="B28:B31"/>
-    <mergeCell ref="C4:C7"/>
-    <mergeCell ref="C8:C11"/>
-    <mergeCell ref="C12:C15"/>
-    <mergeCell ref="C16:C19"/>
-    <mergeCell ref="C20:C23"/>
-    <mergeCell ref="C24:C27"/>
-    <mergeCell ref="C28:C31"/>
-    <mergeCell ref="A4:A7"/>
-    <mergeCell ref="A8:A11"/>
-    <mergeCell ref="A12:A15"/>
-    <mergeCell ref="A16:A19"/>
-    <mergeCell ref="A20:A23"/>
-    <mergeCell ref="A24:A27"/>
-    <mergeCell ref="B24:B27"/>
-    <mergeCell ref="B20:B23"/>
-    <mergeCell ref="B16:B19"/>
-    <mergeCell ref="B12:B15"/>
-    <mergeCell ref="B8:B11"/>
-    <mergeCell ref="B4:B7"/>
+    <mergeCell ref="B36:B39"/>
+    <mergeCell ref="C36:C39"/>
+    <mergeCell ref="D36:D39"/>
+    <mergeCell ref="E36:E39"/>
+    <mergeCell ref="J44:J47"/>
+    <mergeCell ref="K44:K47"/>
+    <mergeCell ref="I48:I51"/>
+    <mergeCell ref="J48:J51"/>
+    <mergeCell ref="K48:K51"/>
+    <mergeCell ref="B48:B51"/>
+    <mergeCell ref="C48:C51"/>
+    <mergeCell ref="D48:D51"/>
+    <mergeCell ref="E48:E51"/>
+    <mergeCell ref="K40:K43"/>
+    <mergeCell ref="I40:I43"/>
+    <mergeCell ref="B40:B43"/>
+    <mergeCell ref="J36:J39"/>
+    <mergeCell ref="C40:C43"/>
+    <mergeCell ref="D40:D43"/>
+    <mergeCell ref="E40:E43"/>
+    <mergeCell ref="A76:A79"/>
+    <mergeCell ref="B76:B79"/>
+    <mergeCell ref="C76:C79"/>
+    <mergeCell ref="D76:D79"/>
+    <mergeCell ref="E76:E79"/>
+    <mergeCell ref="I76:I79"/>
+    <mergeCell ref="J76:J79"/>
+    <mergeCell ref="K76:K79"/>
+    <mergeCell ref="J80:J83"/>
+    <mergeCell ref="K80:K83"/>
+    <mergeCell ref="A80:A83"/>
+    <mergeCell ref="B80:B83"/>
+    <mergeCell ref="C80:C83"/>
+    <mergeCell ref="D80:D83"/>
+    <mergeCell ref="E80:E83"/>
+    <mergeCell ref="I80:I83"/>
+    <mergeCell ref="A60:A63"/>
+    <mergeCell ref="J56:J59"/>
+    <mergeCell ref="K56:K59"/>
+    <mergeCell ref="J60:J63"/>
+    <mergeCell ref="K60:K63"/>
+    <mergeCell ref="I68:I71"/>
+    <mergeCell ref="J68:J71"/>
+    <mergeCell ref="K68:K71"/>
+    <mergeCell ref="A72:A75"/>
+    <mergeCell ref="B72:B75"/>
+    <mergeCell ref="C72:C75"/>
+    <mergeCell ref="D72:D75"/>
+    <mergeCell ref="E72:E75"/>
+    <mergeCell ref="I72:I75"/>
+    <mergeCell ref="J72:J75"/>
+    <mergeCell ref="K72:K75"/>
+    <mergeCell ref="A68:A71"/>
+    <mergeCell ref="B68:B71"/>
+    <mergeCell ref="C68:C71"/>
+    <mergeCell ref="D68:D71"/>
+    <mergeCell ref="E68:E71"/>
+    <mergeCell ref="A64:A67"/>
+    <mergeCell ref="J64:J67"/>
+    <mergeCell ref="K64:K67"/>
+    <mergeCell ref="D2:D3"/>
+    <mergeCell ref="J52:J55"/>
+    <mergeCell ref="K52:K55"/>
+    <mergeCell ref="E52:E55"/>
+    <mergeCell ref="B44:B47"/>
+    <mergeCell ref="C44:C47"/>
+    <mergeCell ref="D44:D47"/>
+    <mergeCell ref="E44:E47"/>
+    <mergeCell ref="B64:B67"/>
+    <mergeCell ref="C64:C67"/>
+    <mergeCell ref="D64:D67"/>
+    <mergeCell ref="E64:E67"/>
+    <mergeCell ref="I64:I67"/>
+    <mergeCell ref="B60:B63"/>
+    <mergeCell ref="C60:C63"/>
+    <mergeCell ref="D60:D63"/>
+    <mergeCell ref="E60:E63"/>
+    <mergeCell ref="I60:I63"/>
+    <mergeCell ref="E56:E59"/>
+    <mergeCell ref="I52:I55"/>
+    <mergeCell ref="B56:B59"/>
+    <mergeCell ref="I56:I59"/>
+    <mergeCell ref="I44:I47"/>
+    <mergeCell ref="J40:J43"/>
+    <mergeCell ref="J32:J35"/>
+    <mergeCell ref="B2:B3"/>
+    <mergeCell ref="A2:A3"/>
+    <mergeCell ref="A52:A55"/>
+    <mergeCell ref="B52:B55"/>
+    <mergeCell ref="C56:C59"/>
+    <mergeCell ref="D56:D59"/>
+    <mergeCell ref="C52:C55"/>
+    <mergeCell ref="D52:D55"/>
+    <mergeCell ref="A44:A47"/>
+    <mergeCell ref="A48:A51"/>
+    <mergeCell ref="D24:D27"/>
+    <mergeCell ref="D20:D23"/>
+    <mergeCell ref="D16:D19"/>
+    <mergeCell ref="D12:D15"/>
+    <mergeCell ref="D8:D11"/>
+    <mergeCell ref="D4:D7"/>
+    <mergeCell ref="A28:A31"/>
+    <mergeCell ref="A32:A35"/>
+    <mergeCell ref="A36:A39"/>
+    <mergeCell ref="A40:A43"/>
+    <mergeCell ref="D32:D35"/>
+    <mergeCell ref="D28:D31"/>
+    <mergeCell ref="A56:A59"/>
+    <mergeCell ref="E32:E35"/>
+    <mergeCell ref="C2:C3"/>
+    <mergeCell ref="H4:H5"/>
+    <mergeCell ref="G4:G5"/>
+    <mergeCell ref="H8:H9"/>
+    <mergeCell ref="H12:H13"/>
+    <mergeCell ref="K32:K35"/>
+    <mergeCell ref="K36:K39"/>
+    <mergeCell ref="J4:J7"/>
+    <mergeCell ref="J8:J11"/>
+    <mergeCell ref="J12:J15"/>
+    <mergeCell ref="J16:J19"/>
+    <mergeCell ref="J20:J23"/>
+    <mergeCell ref="J24:J27"/>
+    <mergeCell ref="J28:J31"/>
+    <mergeCell ref="I32:I35"/>
+    <mergeCell ref="I36:I39"/>
+    <mergeCell ref="K4:K7"/>
+    <mergeCell ref="K8:K11"/>
+    <mergeCell ref="K12:K15"/>
+    <mergeCell ref="K16:K19"/>
+    <mergeCell ref="K20:K23"/>
+    <mergeCell ref="K24:K27"/>
+    <mergeCell ref="J2:J3"/>
     <mergeCell ref="K2:K3"/>
     <mergeCell ref="I4:I7"/>
     <mergeCell ref="I8:I11"/>
@@ -28694,164 +28734,74 @@
     <mergeCell ref="E4:E7"/>
     <mergeCell ref="E8:E11"/>
     <mergeCell ref="E12:E15"/>
-    <mergeCell ref="E32:E35"/>
-    <mergeCell ref="C2:C3"/>
-    <mergeCell ref="H4:H5"/>
-    <mergeCell ref="G4:G5"/>
-    <mergeCell ref="H8:H9"/>
-    <mergeCell ref="H12:H13"/>
-    <mergeCell ref="K32:K35"/>
-    <mergeCell ref="K36:K39"/>
-    <mergeCell ref="J4:J7"/>
-    <mergeCell ref="J8:J11"/>
-    <mergeCell ref="J12:J15"/>
-    <mergeCell ref="J16:J19"/>
-    <mergeCell ref="J20:J23"/>
-    <mergeCell ref="J24:J27"/>
-    <mergeCell ref="J28:J31"/>
-    <mergeCell ref="I32:I35"/>
-    <mergeCell ref="I36:I39"/>
-    <mergeCell ref="K4:K7"/>
-    <mergeCell ref="K8:K11"/>
-    <mergeCell ref="K12:K15"/>
-    <mergeCell ref="K16:K19"/>
-    <mergeCell ref="K20:K23"/>
-    <mergeCell ref="K24:K27"/>
-    <mergeCell ref="J2:J3"/>
-    <mergeCell ref="J32:J35"/>
-    <mergeCell ref="B2:B3"/>
-    <mergeCell ref="A2:A3"/>
-    <mergeCell ref="A52:A55"/>
-    <mergeCell ref="B52:B55"/>
-    <mergeCell ref="C56:C59"/>
-    <mergeCell ref="D56:D59"/>
-    <mergeCell ref="C52:C55"/>
-    <mergeCell ref="D52:D55"/>
-    <mergeCell ref="A44:A47"/>
-    <mergeCell ref="A48:A51"/>
-    <mergeCell ref="D24:D27"/>
-    <mergeCell ref="D20:D23"/>
-    <mergeCell ref="D16:D19"/>
-    <mergeCell ref="D12:D15"/>
-    <mergeCell ref="D8:D11"/>
-    <mergeCell ref="D4:D7"/>
-    <mergeCell ref="A28:A31"/>
-    <mergeCell ref="A32:A35"/>
-    <mergeCell ref="A36:A39"/>
-    <mergeCell ref="A40:A43"/>
-    <mergeCell ref="D32:D35"/>
-    <mergeCell ref="D28:D31"/>
-    <mergeCell ref="A56:A59"/>
-    <mergeCell ref="D2:D3"/>
-    <mergeCell ref="J52:J55"/>
-    <mergeCell ref="K52:K55"/>
-    <mergeCell ref="E52:E55"/>
-    <mergeCell ref="B44:B47"/>
-    <mergeCell ref="C44:C47"/>
-    <mergeCell ref="D44:D47"/>
-    <mergeCell ref="E44:E47"/>
-    <mergeCell ref="B64:B67"/>
-    <mergeCell ref="C64:C67"/>
-    <mergeCell ref="D64:D67"/>
-    <mergeCell ref="E64:E67"/>
-    <mergeCell ref="I64:I67"/>
-    <mergeCell ref="B60:B63"/>
-    <mergeCell ref="C60:C63"/>
-    <mergeCell ref="D60:D63"/>
-    <mergeCell ref="E60:E63"/>
-    <mergeCell ref="I60:I63"/>
-    <mergeCell ref="E56:E59"/>
-    <mergeCell ref="I52:I55"/>
-    <mergeCell ref="B56:B59"/>
-    <mergeCell ref="I56:I59"/>
-    <mergeCell ref="I44:I47"/>
-    <mergeCell ref="A60:A63"/>
-    <mergeCell ref="J56:J59"/>
-    <mergeCell ref="K56:K59"/>
-    <mergeCell ref="J60:J63"/>
-    <mergeCell ref="K60:K63"/>
-    <mergeCell ref="I68:I71"/>
-    <mergeCell ref="J68:J71"/>
-    <mergeCell ref="K68:K71"/>
-    <mergeCell ref="A72:A75"/>
-    <mergeCell ref="B72:B75"/>
-    <mergeCell ref="C72:C75"/>
-    <mergeCell ref="D72:D75"/>
-    <mergeCell ref="E72:E75"/>
-    <mergeCell ref="I72:I75"/>
-    <mergeCell ref="J72:J75"/>
-    <mergeCell ref="K72:K75"/>
-    <mergeCell ref="A68:A71"/>
-    <mergeCell ref="B68:B71"/>
-    <mergeCell ref="C68:C71"/>
-    <mergeCell ref="D68:D71"/>
-    <mergeCell ref="E68:E71"/>
-    <mergeCell ref="A64:A67"/>
-    <mergeCell ref="J64:J67"/>
-    <mergeCell ref="K64:K67"/>
-    <mergeCell ref="A76:A79"/>
-    <mergeCell ref="B76:B79"/>
-    <mergeCell ref="C76:C79"/>
-    <mergeCell ref="D76:D79"/>
-    <mergeCell ref="E76:E79"/>
-    <mergeCell ref="I76:I79"/>
-    <mergeCell ref="J76:J79"/>
-    <mergeCell ref="K76:K79"/>
-    <mergeCell ref="J80:J83"/>
-    <mergeCell ref="K80:K83"/>
-    <mergeCell ref="A80:A83"/>
-    <mergeCell ref="B80:B83"/>
-    <mergeCell ref="C80:C83"/>
-    <mergeCell ref="D80:D83"/>
-    <mergeCell ref="E80:E83"/>
-    <mergeCell ref="I80:I83"/>
-    <mergeCell ref="J40:J43"/>
-    <mergeCell ref="B36:B39"/>
-    <mergeCell ref="C36:C39"/>
-    <mergeCell ref="D36:D39"/>
-    <mergeCell ref="E36:E39"/>
-    <mergeCell ref="J44:J47"/>
-    <mergeCell ref="K44:K47"/>
-    <mergeCell ref="I48:I51"/>
-    <mergeCell ref="J48:J51"/>
-    <mergeCell ref="K48:K51"/>
-    <mergeCell ref="B48:B51"/>
-    <mergeCell ref="C48:C51"/>
-    <mergeCell ref="D48:D51"/>
-    <mergeCell ref="E48:E51"/>
-    <mergeCell ref="K40:K43"/>
-    <mergeCell ref="I40:I43"/>
-    <mergeCell ref="B40:B43"/>
-    <mergeCell ref="J36:J39"/>
-    <mergeCell ref="C40:C43"/>
-    <mergeCell ref="D40:D43"/>
-    <mergeCell ref="E40:E43"/>
+    <mergeCell ref="A4:A7"/>
+    <mergeCell ref="A8:A11"/>
+    <mergeCell ref="A12:A15"/>
+    <mergeCell ref="A16:A19"/>
+    <mergeCell ref="A20:A23"/>
+    <mergeCell ref="A24:A27"/>
+    <mergeCell ref="B24:B27"/>
+    <mergeCell ref="B20:B23"/>
+    <mergeCell ref="B16:B19"/>
+    <mergeCell ref="B12:B15"/>
+    <mergeCell ref="B8:B11"/>
+    <mergeCell ref="B4:B7"/>
+    <mergeCell ref="C32:C35"/>
+    <mergeCell ref="B32:B35"/>
+    <mergeCell ref="B28:B31"/>
+    <mergeCell ref="C4:C7"/>
+    <mergeCell ref="C8:C11"/>
+    <mergeCell ref="C12:C15"/>
+    <mergeCell ref="C16:C19"/>
+    <mergeCell ref="C20:C23"/>
+    <mergeCell ref="C24:C27"/>
+    <mergeCell ref="C28:C31"/>
   </mergeCells>
-  <conditionalFormatting sqref="I4 I8 I12 I20 I16 I24 I28 I32 I36 I40 I44 I48 I52 I56 I60 I64 I68 I72 I76 I80">
-    <cfRule type="cellIs" dxfId="31" priority="101" operator="equal">
+  <conditionalFormatting sqref="I20 I16 I24 I28 I32 I36 I40 I44 I48 I52 I56 I60 I64 I68 I72 I76 I80">
+    <cfRule type="cellIs" dxfId="11" priority="105" operator="equal">
       <formula>"TO DO"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I4 I8 I12 I20 I16 I24 I28 I32 I36 I40 I44 I48 I52 I56 I60 I64 I68 I72 I76 I80">
-    <cfRule type="cellIs" dxfId="30" priority="102" operator="equal">
+  <conditionalFormatting sqref="I20 I16 I24 I28 I32 I36 I40 I44 I48 I52 I56 I60 I64 I68 I72 I76 I80">
+    <cfRule type="cellIs" dxfId="10" priority="106" operator="equal">
       <formula>"IN PROGRESS"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I4 I8 I12 I20 I16 I24 I28 I32 I36 I40 I44 I48 I52 I56 I60 I64 I68 I72 I76 I80">
-    <cfRule type="cellIs" dxfId="29" priority="103" operator="equal">
+  <conditionalFormatting sqref="I20 I16 I24 I28 I32 I36 I40 I44 I48 I52 I56 I60 I64 I68 I72 I76 I80">
+    <cfRule type="cellIs" dxfId="9" priority="107" operator="equal">
       <formula>"REVIEWED"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I4 I8 I12 I20 I16 I24 I28 I32 I36 I40 I44 I48 I52 I56 I60 I64 I68 I72 I76 I80">
-    <cfRule type="cellIs" dxfId="28" priority="104" operator="equal">
+  <conditionalFormatting sqref="I20 I16 I24 I28 I32 I36 I40 I44 I48 I52 I56 I60 I64 I68 I72 I76 I80">
+    <cfRule type="cellIs" dxfId="8" priority="108" operator="equal">
+      <formula>"IN REVIEW"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I4 I8 I12">
+    <cfRule type="cellIs" dxfId="7" priority="1" operator="equal">
+      <formula>"TO DO"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I4 I8 I12">
+    <cfRule type="cellIs" dxfId="5" priority="2" operator="equal">
+      <formula>"IN PROGRESS"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I4 I8 I12">
+    <cfRule type="cellIs" dxfId="3" priority="3" operator="equal">
+      <formula>"REVIEWED"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I4 I8 I12">
+    <cfRule type="cellIs" dxfId="1" priority="4" operator="equal">
       <formula>"IN REVIEW"</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" sqref="I4 I8 I28 I40 I32 I20 I16 I24 I36 I48 I52 I44 I56 I60 I12 I64 I68 I72 I76 I80">
+    <dataValidation type="list" allowBlank="1" sqref="I72 I76 I28 I40 I32 I20 I16 I24 I36 I48 I52 I44 I56 I60 I80 I64 I68 I4 I8 I12">
       <formula1>"TO DO,In Progress,In Review,Reviewed"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" sqref="K4 K36 K40 K32 K12 K16 K20 K24 K48 K44 K52 K60 K56 K64 K68 K72 K80 K76 K8 K28">
+    <dataValidation type="list" allowBlank="1" sqref="K76 K36 K40 K32 K28 K16 K20 K24 K48 K44 K52 K60 K56 K64 K68 K72 K80 K4 K12 K8">
       <formula1>"Smoke,Regresión"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
Agrego casos de uso referentes al listado y busqueda de productos en la web
</commit_message>
<xml_diff>
--- a/Testing 2024/template_caso_prueba-ISPC2024-sprint-1.xlsx
+++ b/Testing 2024/template_caso_prueba-ISPC2024-sprint-1.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="84">
   <si>
     <t>Id</t>
   </si>
@@ -215,6 +215,69 @@
   <si>
     <t>Sitio responsive. El usuario ingresa desde un celular</t>
   </si>
+  <si>
+    <t>Listado y Búsqueda de Productos</t>
+  </si>
+  <si>
+    <t>Filtrar por categoria</t>
+  </si>
+  <si>
+    <t>Cualquier usuario que acceda a la home page puede listar todos los libros que correspondan a la categoría seleccionada</t>
+  </si>
+  <si>
+    <t>Se visualiza la home page</t>
+  </si>
+  <si>
+    <t>2.</t>
+  </si>
+  <si>
+    <t>Seleccionar la opción "Catálogo" en la navbar</t>
+  </si>
+  <si>
+    <t>Se visualiza una sección con 7 categorías</t>
+  </si>
+  <si>
+    <t>3.</t>
+  </si>
+  <si>
+    <t>Seleccionar la categoria deseada</t>
+  </si>
+  <si>
+    <t>Se visualiza opciones que coincidan con la categoria seleccionada</t>
+  </si>
+  <si>
+    <t>Búsqueda un libro mediante la barra de búsqueda</t>
+  </si>
+  <si>
+    <t>El usuario realizara la búsqueda de un libro escribiendo el nombre del libro en la barra de búsqueda</t>
+  </si>
+  <si>
+    <t>Tener un buscador con filtros</t>
+  </si>
+  <si>
+    <t>Se visualiza la barra de úsqueda en la home page</t>
+  </si>
+  <si>
+    <t>Escribir el nombre de un libro en la barra de búsqueda</t>
+  </si>
+  <si>
+    <t>Presionar la tecla "enter"</t>
+  </si>
+  <si>
+    <t>Se visualizan los resultados que coincidan con la búsqueda</t>
+  </si>
+  <si>
+    <t>Búsqueda un libro no existente mediante la barra de búsqueda</t>
+  </si>
+  <si>
+    <t>El usuario realizara la búsqueda de un libro escribiendo el nombre del libro en la barra de búsqueda pero este no existe en el catálogo</t>
+  </si>
+  <si>
+    <t>Se visualizan el mensaje "Lo sentimos, no encontramos el libro que estas buscando"</t>
+  </si>
+  <si>
+    <t>El usuario debe estar situado en la home page</t>
+  </si>
 </sst>
 </file>
 
@@ -295,7 +358,7 @@
       <name val="ArialMT"/>
     </font>
   </fonts>
-  <fills count="11">
+  <fills count="12">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -353,6 +416,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor rgb="FFFFFFCC"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
         <bgColor rgb="FFFFFFCC"/>
       </patternFill>
     </fill>
@@ -627,7 +696,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="71">
+  <cellXfs count="74">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -734,6 +803,29 @@
     <xf numFmtId="0" fontId="1" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="11" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="10" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -749,11 +841,18 @@
     <xf numFmtId="0" fontId="7" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -769,41 +868,20 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="11" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="11" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="1" fillId="11" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="12">
+  <dxfs count="16">
     <dxf>
       <fill>
         <patternFill patternType="solid">
@@ -857,6 +935,38 @@
         <patternFill patternType="solid">
           <fgColor rgb="FFA2C4C9"/>
           <bgColor rgb="FFA2C4C9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFA2C4C9"/>
+          <bgColor rgb="FFA2C4C9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFCE5CD"/>
+          <bgColor rgb="FFFCE5CD"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF93C47D"/>
+          <bgColor rgb="FF93C47D"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFF2CC"/>
+          <bgColor rgb="FFFFF2CC"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1249,8 +1359,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AA935"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="60" workbookViewId="0">
-      <selection activeCell="G21" sqref="G21"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="60" workbookViewId="0">
+      <selection activeCell="G30" sqref="G30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5703125" defaultRowHeight="12.75"/>
@@ -1299,33 +1409,33 @@
       <c r="AA1" s="2"/>
     </row>
     <row r="2" spans="1:27" s="31" customFormat="1" ht="15.75" customHeight="1">
-      <c r="A2" s="61" t="s">
+      <c r="A2" s="62" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="51" t="s">
+      <c r="B2" s="60" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="61" t="s">
+      <c r="C2" s="62" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="51" t="s">
+      <c r="D2" s="60" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="51" t="s">
+      <c r="E2" s="60" t="s">
         <v>4</v>
       </c>
-      <c r="F2" s="56" t="s">
+      <c r="F2" s="66" t="s">
         <v>5</v>
       </c>
-      <c r="G2" s="57"/>
-      <c r="H2" s="58"/>
-      <c r="I2" s="59" t="s">
+      <c r="G2" s="67"/>
+      <c r="H2" s="68"/>
+      <c r="I2" s="69" t="s">
         <v>6</v>
       </c>
-      <c r="J2" s="51" t="s">
+      <c r="J2" s="60" t="s">
         <v>7</v>
       </c>
-      <c r="K2" s="51" t="s">
+      <c r="K2" s="60" t="s">
         <v>27</v>
       </c>
       <c r="L2" s="32"/>
@@ -1346,11 +1456,11 @@
       <c r="AA2" s="33"/>
     </row>
     <row r="3" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A3" s="62"/>
-      <c r="B3" s="52"/>
-      <c r="C3" s="62"/>
-      <c r="D3" s="52"/>
-      <c r="E3" s="52"/>
+      <c r="A3" s="63"/>
+      <c r="B3" s="61"/>
+      <c r="C3" s="63"/>
+      <c r="D3" s="61"/>
+      <c r="E3" s="61"/>
       <c r="F3" s="34" t="s">
         <v>8</v>
       </c>
@@ -1360,9 +1470,9 @@
       <c r="H3" s="42" t="s">
         <v>10</v>
       </c>
-      <c r="I3" s="60"/>
-      <c r="J3" s="52"/>
-      <c r="K3" s="52"/>
+      <c r="I3" s="70"/>
+      <c r="J3" s="61"/>
+      <c r="K3" s="61"/>
       <c r="L3" s="3"/>
       <c r="M3" s="2"/>
       <c r="N3" s="2"/>
@@ -1381,7 +1491,7 @@
       <c r="AA3" s="2"/>
     </row>
     <row r="4" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A4" s="48" t="s">
+      <c r="A4" s="57" t="s">
         <v>29</v>
       </c>
       <c r="B4" s="45" t="s">
@@ -1402,16 +1512,16 @@
       <c r="G4" s="45" t="s">
         <v>54</v>
       </c>
-      <c r="H4" s="63" t="s">
+      <c r="H4" s="64" t="s">
         <v>55</v>
       </c>
-      <c r="I4" s="53" t="s">
+      <c r="I4" s="54" t="s">
         <v>26</v>
       </c>
-      <c r="J4" s="65" t="s">
+      <c r="J4" s="51" t="s">
         <v>56</v>
       </c>
-      <c r="K4" s="53" t="s">
+      <c r="K4" s="54" t="s">
         <v>28</v>
       </c>
       <c r="L4" s="3"/>
@@ -1432,17 +1542,17 @@
       <c r="AA4" s="2"/>
     </row>
     <row r="5" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A5" s="49"/>
+      <c r="A5" s="58"/>
       <c r="B5" s="46"/>
       <c r="C5" s="46"/>
       <c r="D5" s="46"/>
       <c r="E5" s="46"/>
       <c r="F5" s="47"/>
       <c r="G5" s="47"/>
-      <c r="H5" s="64"/>
-      <c r="I5" s="54"/>
-      <c r="J5" s="66"/>
-      <c r="K5" s="54"/>
+      <c r="H5" s="65"/>
+      <c r="I5" s="55"/>
+      <c r="J5" s="52"/>
+      <c r="K5" s="55"/>
       <c r="L5" s="3"/>
       <c r="M5" s="2"/>
       <c r="N5" s="2"/>
@@ -1461,7 +1571,7 @@
       <c r="AA5" s="2"/>
     </row>
     <row r="6" spans="1:27" s="29" customFormat="1" ht="15.75" customHeight="1">
-      <c r="A6" s="49"/>
+      <c r="A6" s="58"/>
       <c r="B6" s="46"/>
       <c r="C6" s="46"/>
       <c r="D6" s="46"/>
@@ -1469,9 +1579,9 @@
       <c r="F6" s="30"/>
       <c r="G6" s="35"/>
       <c r="H6" s="35"/>
-      <c r="I6" s="54"/>
-      <c r="J6" s="66"/>
-      <c r="K6" s="54"/>
+      <c r="I6" s="55"/>
+      <c r="J6" s="52"/>
+      <c r="K6" s="55"/>
       <c r="L6" s="27"/>
       <c r="M6" s="28"/>
       <c r="N6" s="28"/>
@@ -1490,7 +1600,7 @@
       <c r="AA6" s="28"/>
     </row>
     <row r="7" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A7" s="50"/>
+      <c r="A7" s="59"/>
       <c r="B7" s="47"/>
       <c r="C7" s="47"/>
       <c r="D7" s="47"/>
@@ -1498,9 +1608,9 @@
       <c r="F7" s="30"/>
       <c r="G7" s="35"/>
       <c r="H7" s="35"/>
-      <c r="I7" s="55"/>
-      <c r="J7" s="67"/>
-      <c r="K7" s="55"/>
+      <c r="I7" s="56"/>
+      <c r="J7" s="53"/>
+      <c r="K7" s="56"/>
       <c r="L7" s="3"/>
       <c r="M7" s="2"/>
       <c r="N7" s="2"/>
@@ -1519,7 +1629,7 @@
       <c r="AA7" s="2"/>
     </row>
     <row r="8" spans="1:27">
-      <c r="A8" s="48" t="s">
+      <c r="A8" s="57" t="s">
         <v>30</v>
       </c>
       <c r="B8" s="45" t="s">
@@ -1540,16 +1650,16 @@
       <c r="G8" s="45" t="s">
         <v>54</v>
       </c>
-      <c r="H8" s="63" t="s">
+      <c r="H8" s="64" t="s">
         <v>55</v>
       </c>
-      <c r="I8" s="53" t="s">
+      <c r="I8" s="54" t="s">
         <v>26</v>
       </c>
-      <c r="J8" s="65" t="s">
+      <c r="J8" s="51" t="s">
         <v>56</v>
       </c>
-      <c r="K8" s="53" t="s">
+      <c r="K8" s="54" t="s">
         <v>28</v>
       </c>
       <c r="L8" s="3"/>
@@ -1570,17 +1680,17 @@
       <c r="AA8" s="2"/>
     </row>
     <row r="9" spans="1:27">
-      <c r="A9" s="49"/>
+      <c r="A9" s="58"/>
       <c r="B9" s="46"/>
       <c r="C9" s="46"/>
       <c r="D9" s="46"/>
       <c r="E9" s="46"/>
       <c r="F9" s="47"/>
       <c r="G9" s="47"/>
-      <c r="H9" s="64"/>
-      <c r="I9" s="54"/>
-      <c r="J9" s="66"/>
-      <c r="K9" s="54"/>
+      <c r="H9" s="65"/>
+      <c r="I9" s="55"/>
+      <c r="J9" s="52"/>
+      <c r="K9" s="55"/>
       <c r="L9" s="3"/>
       <c r="M9" s="2"/>
       <c r="N9" s="2"/>
@@ -1599,7 +1709,7 @@
       <c r="AA9" s="2"/>
     </row>
     <row r="10" spans="1:27" s="29" customFormat="1" ht="15.75" customHeight="1">
-      <c r="A10" s="49"/>
+      <c r="A10" s="58"/>
       <c r="B10" s="46"/>
       <c r="C10" s="46"/>
       <c r="D10" s="46"/>
@@ -1607,9 +1717,9 @@
       <c r="F10" s="30"/>
       <c r="G10" s="35"/>
       <c r="H10" s="35"/>
-      <c r="I10" s="54"/>
-      <c r="J10" s="66"/>
-      <c r="K10" s="54"/>
+      <c r="I10" s="55"/>
+      <c r="J10" s="52"/>
+      <c r="K10" s="55"/>
       <c r="L10" s="27"/>
       <c r="M10" s="28"/>
       <c r="N10" s="28"/>
@@ -1628,7 +1738,7 @@
       <c r="AA10" s="28"/>
     </row>
     <row r="11" spans="1:27">
-      <c r="A11" s="50"/>
+      <c r="A11" s="59"/>
       <c r="B11" s="47"/>
       <c r="C11" s="47"/>
       <c r="D11" s="47"/>
@@ -1636,9 +1746,9 @@
       <c r="F11" s="30"/>
       <c r="G11" s="35"/>
       <c r="H11" s="35"/>
-      <c r="I11" s="55"/>
-      <c r="J11" s="67"/>
-      <c r="K11" s="55"/>
+      <c r="I11" s="56"/>
+      <c r="J11" s="53"/>
+      <c r="K11" s="56"/>
       <c r="L11" s="3"/>
       <c r="M11" s="2"/>
       <c r="N11" s="2"/>
@@ -1657,7 +1767,7 @@
       <c r="AA11" s="2"/>
     </row>
     <row r="12" spans="1:27">
-      <c r="A12" s="48" t="s">
+      <c r="A12" s="57" t="s">
         <v>31</v>
       </c>
       <c r="B12" s="45" t="s">
@@ -1678,16 +1788,16 @@
       <c r="G12" s="45" t="s">
         <v>54</v>
       </c>
-      <c r="H12" s="63" t="s">
+      <c r="H12" s="64" t="s">
         <v>55</v>
       </c>
-      <c r="I12" s="53" t="s">
+      <c r="I12" s="54" t="s">
         <v>26</v>
       </c>
-      <c r="J12" s="65" t="s">
+      <c r="J12" s="51" t="s">
         <v>56</v>
       </c>
-      <c r="K12" s="53" t="s">
+      <c r="K12" s="54" t="s">
         <v>28</v>
       </c>
       <c r="L12" s="2"/>
@@ -1708,17 +1818,17 @@
       <c r="AA12" s="2"/>
     </row>
     <row r="13" spans="1:27">
-      <c r="A13" s="49"/>
+      <c r="A13" s="58"/>
       <c r="B13" s="46"/>
       <c r="C13" s="46"/>
       <c r="D13" s="46"/>
       <c r="E13" s="46"/>
       <c r="F13" s="47"/>
       <c r="G13" s="47"/>
-      <c r="H13" s="64"/>
-      <c r="I13" s="54"/>
-      <c r="J13" s="66"/>
-      <c r="K13" s="54"/>
+      <c r="H13" s="65"/>
+      <c r="I13" s="55"/>
+      <c r="J13" s="52"/>
+      <c r="K13" s="55"/>
       <c r="L13" s="2"/>
       <c r="M13" s="2"/>
       <c r="N13" s="2"/>
@@ -1737,7 +1847,7 @@
       <c r="AA13" s="2"/>
     </row>
     <row r="14" spans="1:27" s="29" customFormat="1">
-      <c r="A14" s="49"/>
+      <c r="A14" s="58"/>
       <c r="B14" s="46"/>
       <c r="C14" s="46"/>
       <c r="D14" s="46"/>
@@ -1745,9 +1855,9 @@
       <c r="F14" s="30"/>
       <c r="G14" s="35"/>
       <c r="H14" s="35"/>
-      <c r="I14" s="54"/>
-      <c r="J14" s="66"/>
-      <c r="K14" s="54"/>
+      <c r="I14" s="55"/>
+      <c r="J14" s="52"/>
+      <c r="K14" s="55"/>
       <c r="L14" s="28"/>
       <c r="M14" s="28"/>
       <c r="N14" s="28"/>
@@ -1766,7 +1876,7 @@
       <c r="AA14" s="28"/>
     </row>
     <row r="15" spans="1:27">
-      <c r="A15" s="50"/>
+      <c r="A15" s="59"/>
       <c r="B15" s="47"/>
       <c r="C15" s="47"/>
       <c r="D15" s="47"/>
@@ -1774,9 +1884,9 @@
       <c r="F15" s="30"/>
       <c r="G15" s="35"/>
       <c r="H15" s="35"/>
-      <c r="I15" s="55"/>
-      <c r="J15" s="67"/>
-      <c r="K15" s="55"/>
+      <c r="I15" s="56"/>
+      <c r="J15" s="53"/>
+      <c r="K15" s="56"/>
       <c r="L15" s="2"/>
       <c r="M15" s="2"/>
       <c r="N15" s="2"/>
@@ -1794,22 +1904,38 @@
       <c r="Z15" s="2"/>
       <c r="AA15" s="2"/>
     </row>
-    <row r="16" spans="1:27">
-      <c r="A16" s="48" t="s">
+    <row r="16" spans="1:27" ht="15.75" customHeight="1">
+      <c r="A16" s="71" t="s">
         <v>32</v>
       </c>
-      <c r="B16" s="45"/>
-      <c r="C16" s="45"/>
-      <c r="D16" s="45"/>
-      <c r="E16" s="45"/>
-      <c r="F16" s="30"/>
-      <c r="G16" s="44"/>
-      <c r="H16" s="44"/>
-      <c r="I16" s="53" t="s">
+      <c r="B16" s="45" t="s">
+        <v>63</v>
+      </c>
+      <c r="C16" s="45" t="s">
+        <v>64</v>
+      </c>
+      <c r="D16" s="45" t="s">
+        <v>65</v>
+      </c>
+      <c r="E16" s="45" t="s">
+        <v>83</v>
+      </c>
+      <c r="F16" s="30" t="s">
+        <v>53</v>
+      </c>
+      <c r="G16" s="35" t="s">
+        <v>54</v>
+      </c>
+      <c r="H16" s="35" t="s">
+        <v>66</v>
+      </c>
+      <c r="I16" s="54" t="s">
         <v>26</v>
       </c>
-      <c r="J16" s="65"/>
-      <c r="K16" s="53" t="s">
+      <c r="J16" s="51" t="s">
+        <v>56</v>
+      </c>
+      <c r="K16" s="54" t="s">
         <v>28</v>
       </c>
       <c r="L16" s="2"/>
@@ -1830,17 +1956,23 @@
       <c r="AA16" s="2"/>
     </row>
     <row r="17" spans="1:27" ht="16.5" customHeight="1">
-      <c r="A17" s="49"/>
+      <c r="A17" s="72"/>
       <c r="B17" s="46"/>
       <c r="C17" s="46"/>
       <c r="D17" s="46"/>
       <c r="E17" s="46"/>
-      <c r="F17" s="30"/>
-      <c r="G17" s="44"/>
-      <c r="H17" s="44"/>
-      <c r="I17" s="54"/>
-      <c r="J17" s="66"/>
-      <c r="K17" s="54"/>
+      <c r="F17" s="30" t="s">
+        <v>67</v>
+      </c>
+      <c r="G17" s="35" t="s">
+        <v>68</v>
+      </c>
+      <c r="H17" s="35" t="s">
+        <v>69</v>
+      </c>
+      <c r="I17" s="55"/>
+      <c r="J17" s="52"/>
+      <c r="K17" s="55"/>
       <c r="L17" s="2"/>
       <c r="M17" s="2"/>
       <c r="N17" s="2"/>
@@ -1858,18 +1990,24 @@
       <c r="Z17" s="2"/>
       <c r="AA17" s="2"/>
     </row>
-    <row r="18" spans="1:27" s="29" customFormat="1">
-      <c r="A18" s="49"/>
+    <row r="18" spans="1:27" s="29" customFormat="1" ht="25.5">
+      <c r="A18" s="72"/>
       <c r="B18" s="46"/>
       <c r="C18" s="46"/>
       <c r="D18" s="46"/>
       <c r="E18" s="46"/>
-      <c r="F18" s="30"/>
-      <c r="G18" s="44"/>
-      <c r="H18" s="44"/>
-      <c r="I18" s="54"/>
-      <c r="J18" s="66"/>
-      <c r="K18" s="54"/>
+      <c r="F18" s="30" t="s">
+        <v>70</v>
+      </c>
+      <c r="G18" s="35" t="s">
+        <v>71</v>
+      </c>
+      <c r="H18" s="35" t="s">
+        <v>72</v>
+      </c>
+      <c r="I18" s="55"/>
+      <c r="J18" s="52"/>
+      <c r="K18" s="55"/>
       <c r="L18" s="28"/>
       <c r="M18" s="28"/>
       <c r="N18" s="28"/>
@@ -1888,17 +2026,17 @@
       <c r="AA18" s="28"/>
     </row>
     <row r="19" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A19" s="50"/>
+      <c r="A19" s="73"/>
       <c r="B19" s="47"/>
       <c r="C19" s="47"/>
       <c r="D19" s="47"/>
       <c r="E19" s="47"/>
       <c r="F19" s="30"/>
-      <c r="G19" s="44"/>
-      <c r="H19" s="44"/>
-      <c r="I19" s="55"/>
-      <c r="J19" s="67"/>
-      <c r="K19" s="55"/>
+      <c r="G19" s="35"/>
+      <c r="H19" s="35"/>
+      <c r="I19" s="56"/>
+      <c r="J19" s="53"/>
+      <c r="K19" s="56"/>
       <c r="L19" s="2"/>
       <c r="M19" s="2"/>
       <c r="N19" s="2"/>
@@ -1917,21 +2055,37 @@
       <c r="AA19" s="2"/>
     </row>
     <row r="20" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A20" s="48" t="s">
+      <c r="A20" s="71" t="s">
         <v>33</v>
       </c>
-      <c r="B20" s="45"/>
-      <c r="C20" s="45"/>
-      <c r="D20" s="45"/>
-      <c r="E20" s="45"/>
-      <c r="F20" s="30"/>
-      <c r="G20" s="44"/>
-      <c r="H20" s="44"/>
-      <c r="I20" s="53" t="s">
+      <c r="B20" s="45" t="s">
+        <v>63</v>
+      </c>
+      <c r="C20" s="48" t="s">
+        <v>73</v>
+      </c>
+      <c r="D20" s="45" t="s">
+        <v>74</v>
+      </c>
+      <c r="E20" s="45" t="s">
+        <v>75</v>
+      </c>
+      <c r="F20" s="30" t="s">
+        <v>53</v>
+      </c>
+      <c r="G20" s="35" t="s">
+        <v>54</v>
+      </c>
+      <c r="H20" s="35" t="s">
+        <v>76</v>
+      </c>
+      <c r="I20" s="54" t="s">
         <v>26</v>
       </c>
-      <c r="J20" s="65"/>
-      <c r="K20" s="53" t="s">
+      <c r="J20" s="51" t="s">
+        <v>56</v>
+      </c>
+      <c r="K20" s="54" t="s">
         <v>28</v>
       </c>
       <c r="L20" s="2"/>
@@ -1952,17 +2106,21 @@
       <c r="AA20" s="2"/>
     </row>
     <row r="21" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A21" s="49"/>
+      <c r="A21" s="72"/>
       <c r="B21" s="46"/>
-      <c r="C21" s="46"/>
+      <c r="C21" s="49"/>
       <c r="D21" s="46"/>
       <c r="E21" s="46"/>
-      <c r="F21" s="30"/>
-      <c r="G21" s="44"/>
-      <c r="H21" s="44"/>
-      <c r="I21" s="54"/>
-      <c r="J21" s="66"/>
-      <c r="K21" s="54"/>
+      <c r="F21" s="30" t="s">
+        <v>67</v>
+      </c>
+      <c r="G21" s="35" t="s">
+        <v>77</v>
+      </c>
+      <c r="H21" s="35"/>
+      <c r="I21" s="55"/>
+      <c r="J21" s="52"/>
+      <c r="K21" s="55"/>
       <c r="L21" s="2"/>
       <c r="M21" s="2"/>
       <c r="N21" s="2"/>
@@ -1981,17 +2139,23 @@
       <c r="AA21" s="2"/>
     </row>
     <row r="22" spans="1:27" s="29" customFormat="1" ht="15.75" customHeight="1">
-      <c r="A22" s="49"/>
+      <c r="A22" s="72"/>
       <c r="B22" s="46"/>
-      <c r="C22" s="46"/>
+      <c r="C22" s="49"/>
       <c r="D22" s="46"/>
       <c r="E22" s="46"/>
-      <c r="F22" s="30"/>
-      <c r="G22" s="44"/>
-      <c r="H22" s="44"/>
-      <c r="I22" s="54"/>
-      <c r="J22" s="66"/>
-      <c r="K22" s="54"/>
+      <c r="F22" s="30" t="s">
+        <v>70</v>
+      </c>
+      <c r="G22" s="35" t="s">
+        <v>78</v>
+      </c>
+      <c r="H22" s="35" t="s">
+        <v>79</v>
+      </c>
+      <c r="I22" s="55"/>
+      <c r="J22" s="52"/>
+      <c r="K22" s="55"/>
       <c r="L22" s="28"/>
       <c r="M22" s="28"/>
       <c r="N22" s="28"/>
@@ -2010,17 +2174,17 @@
       <c r="AA22" s="28"/>
     </row>
     <row r="23" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A23" s="50"/>
+      <c r="A23" s="73"/>
       <c r="B23" s="47"/>
-      <c r="C23" s="47"/>
+      <c r="C23" s="50"/>
       <c r="D23" s="47"/>
       <c r="E23" s="47"/>
       <c r="F23" s="30"/>
-      <c r="G23" s="44"/>
-      <c r="H23" s="44"/>
-      <c r="I23" s="55"/>
-      <c r="J23" s="67"/>
-      <c r="K23" s="55"/>
+      <c r="G23" s="35"/>
+      <c r="H23" s="35"/>
+      <c r="I23" s="56"/>
+      <c r="J23" s="53"/>
+      <c r="K23" s="56"/>
       <c r="L23" s="2"/>
       <c r="M23" s="2"/>
       <c r="N23" s="2"/>
@@ -2039,21 +2203,37 @@
       <c r="AA23" s="2"/>
     </row>
     <row r="24" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A24" s="48" t="s">
+      <c r="A24" s="71" t="s">
         <v>34</v>
       </c>
-      <c r="B24" s="45"/>
-      <c r="C24" s="45"/>
-      <c r="D24" s="45"/>
-      <c r="E24" s="45"/>
-      <c r="F24" s="30"/>
-      <c r="G24" s="44"/>
-      <c r="H24" s="44"/>
-      <c r="I24" s="53" t="s">
+      <c r="B24" s="45" t="s">
+        <v>63</v>
+      </c>
+      <c r="C24" s="48" t="s">
+        <v>80</v>
+      </c>
+      <c r="D24" s="45" t="s">
+        <v>81</v>
+      </c>
+      <c r="E24" s="45" t="s">
+        <v>75</v>
+      </c>
+      <c r="F24" s="30" t="s">
+        <v>53</v>
+      </c>
+      <c r="G24" s="35" t="s">
+        <v>54</v>
+      </c>
+      <c r="H24" s="35" t="s">
+        <v>76</v>
+      </c>
+      <c r="I24" s="54" t="s">
         <v>26</v>
       </c>
-      <c r="J24" s="65"/>
-      <c r="K24" s="53" t="s">
+      <c r="J24" s="51" t="s">
+        <v>56</v>
+      </c>
+      <c r="K24" s="54" t="s">
         <v>28</v>
       </c>
       <c r="L24" s="2"/>
@@ -2074,17 +2254,21 @@
       <c r="AA24" s="2"/>
     </row>
     <row r="25" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A25" s="49"/>
+      <c r="A25" s="72"/>
       <c r="B25" s="46"/>
-      <c r="C25" s="46"/>
+      <c r="C25" s="49"/>
       <c r="D25" s="46"/>
       <c r="E25" s="46"/>
-      <c r="F25" s="30"/>
-      <c r="G25" s="44"/>
-      <c r="H25" s="44"/>
-      <c r="I25" s="54"/>
-      <c r="J25" s="66"/>
-      <c r="K25" s="54"/>
+      <c r="F25" s="30" t="s">
+        <v>67</v>
+      </c>
+      <c r="G25" s="35" t="s">
+        <v>77</v>
+      </c>
+      <c r="H25" s="35"/>
+      <c r="I25" s="55"/>
+      <c r="J25" s="52"/>
+      <c r="K25" s="55"/>
       <c r="L25" s="2"/>
       <c r="M25" s="2"/>
       <c r="N25" s="2"/>
@@ -2102,18 +2286,24 @@
       <c r="Z25" s="2"/>
       <c r="AA25" s="2"/>
     </row>
-    <row r="26" spans="1:27" s="29" customFormat="1" ht="15.75" customHeight="1">
-      <c r="A26" s="49"/>
+    <row r="26" spans="1:27" s="29" customFormat="1" ht="25.5">
+      <c r="A26" s="72"/>
       <c r="B26" s="46"/>
-      <c r="C26" s="46"/>
+      <c r="C26" s="49"/>
       <c r="D26" s="46"/>
       <c r="E26" s="46"/>
-      <c r="F26" s="30"/>
-      <c r="G26" s="44"/>
-      <c r="H26" s="44"/>
-      <c r="I26" s="54"/>
-      <c r="J26" s="66"/>
-      <c r="K26" s="54"/>
+      <c r="F26" s="30" t="s">
+        <v>70</v>
+      </c>
+      <c r="G26" s="35" t="s">
+        <v>78</v>
+      </c>
+      <c r="H26" s="35" t="s">
+        <v>82</v>
+      </c>
+      <c r="I26" s="55"/>
+      <c r="J26" s="52"/>
+      <c r="K26" s="55"/>
       <c r="L26" s="28"/>
       <c r="M26" s="28"/>
       <c r="N26" s="28"/>
@@ -2132,17 +2322,17 @@
       <c r="AA26" s="28"/>
     </row>
     <row r="27" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A27" s="50"/>
+      <c r="A27" s="73"/>
       <c r="B27" s="47"/>
-      <c r="C27" s="47"/>
+      <c r="C27" s="50"/>
       <c r="D27" s="47"/>
       <c r="E27" s="47"/>
       <c r="F27" s="30"/>
-      <c r="G27" s="44"/>
-      <c r="H27" s="44"/>
-      <c r="I27" s="55"/>
-      <c r="J27" s="67"/>
-      <c r="K27" s="55"/>
+      <c r="G27" s="35"/>
+      <c r="H27" s="35"/>
+      <c r="I27" s="56"/>
+      <c r="J27" s="53"/>
+      <c r="K27" s="56"/>
       <c r="L27" s="2"/>
       <c r="M27" s="2"/>
       <c r="N27" s="2"/>
@@ -2161,7 +2351,7 @@
       <c r="AA27" s="2"/>
     </row>
     <row r="28" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A28" s="48" t="s">
+      <c r="A28" s="57" t="s">
         <v>35</v>
       </c>
       <c r="B28" s="45"/>
@@ -2171,11 +2361,11 @@
       <c r="F28" s="30"/>
       <c r="G28" s="44"/>
       <c r="H28" s="44"/>
-      <c r="I28" s="53" t="s">
+      <c r="I28" s="54" t="s">
         <v>26</v>
       </c>
-      <c r="J28" s="65"/>
-      <c r="K28" s="53" t="s">
+      <c r="J28" s="51"/>
+      <c r="K28" s="54" t="s">
         <v>28</v>
       </c>
       <c r="L28" s="2"/>
@@ -2196,7 +2386,7 @@
       <c r="AA28" s="2"/>
     </row>
     <row r="29" spans="1:27">
-      <c r="A29" s="49"/>
+      <c r="A29" s="58"/>
       <c r="B29" s="46"/>
       <c r="C29" s="46"/>
       <c r="D29" s="46"/>
@@ -2204,9 +2394,9 @@
       <c r="F29" s="30"/>
       <c r="G29" s="44"/>
       <c r="H29" s="44"/>
-      <c r="I29" s="54"/>
-      <c r="J29" s="66"/>
-      <c r="K29" s="54"/>
+      <c r="I29" s="55"/>
+      <c r="J29" s="52"/>
+      <c r="K29" s="55"/>
       <c r="L29" s="2"/>
       <c r="M29" s="2"/>
       <c r="N29" s="2"/>
@@ -2225,7 +2415,7 @@
       <c r="AA29" s="2"/>
     </row>
     <row r="30" spans="1:27" s="29" customFormat="1" ht="15.75" customHeight="1">
-      <c r="A30" s="49"/>
+      <c r="A30" s="58"/>
       <c r="B30" s="46"/>
       <c r="C30" s="46"/>
       <c r="D30" s="46"/>
@@ -2233,9 +2423,9 @@
       <c r="F30" s="30"/>
       <c r="G30" s="44"/>
       <c r="H30" s="44"/>
-      <c r="I30" s="54"/>
-      <c r="J30" s="66"/>
-      <c r="K30" s="54"/>
+      <c r="I30" s="55"/>
+      <c r="J30" s="52"/>
+      <c r="K30" s="55"/>
       <c r="L30" s="28"/>
       <c r="M30" s="28"/>
       <c r="N30" s="28"/>
@@ -2254,7 +2444,7 @@
       <c r="AA30" s="28"/>
     </row>
     <row r="31" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A31" s="50"/>
+      <c r="A31" s="59"/>
       <c r="B31" s="47"/>
       <c r="C31" s="47"/>
       <c r="D31" s="47"/>
@@ -2262,9 +2452,9 @@
       <c r="F31" s="30"/>
       <c r="G31" s="44"/>
       <c r="H31" s="44"/>
-      <c r="I31" s="55"/>
-      <c r="J31" s="67"/>
-      <c r="K31" s="55"/>
+      <c r="I31" s="56"/>
+      <c r="J31" s="53"/>
+      <c r="K31" s="56"/>
       <c r="L31" s="2"/>
       <c r="M31" s="2"/>
       <c r="N31" s="2"/>
@@ -2283,7 +2473,7 @@
       <c r="AA31" s="2"/>
     </row>
     <row r="32" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A32" s="48" t="s">
+      <c r="A32" s="57" t="s">
         <v>36</v>
       </c>
       <c r="B32" s="45"/>
@@ -2293,11 +2483,11 @@
       <c r="F32" s="30"/>
       <c r="G32" s="35"/>
       <c r="H32" s="35"/>
-      <c r="I32" s="53" t="s">
+      <c r="I32" s="54" t="s">
         <v>26</v>
       </c>
-      <c r="J32" s="65"/>
-      <c r="K32" s="53" t="s">
+      <c r="J32" s="51"/>
+      <c r="K32" s="54" t="s">
         <v>28</v>
       </c>
       <c r="L32" s="2"/>
@@ -2318,7 +2508,7 @@
       <c r="AA32" s="2"/>
     </row>
     <row r="33" spans="1:27">
-      <c r="A33" s="49"/>
+      <c r="A33" s="58"/>
       <c r="B33" s="46"/>
       <c r="C33" s="46"/>
       <c r="D33" s="46"/>
@@ -2326,9 +2516,9 @@
       <c r="F33" s="30"/>
       <c r="G33" s="35"/>
       <c r="H33" s="35"/>
-      <c r="I33" s="54"/>
-      <c r="J33" s="66"/>
-      <c r="K33" s="54"/>
+      <c r="I33" s="55"/>
+      <c r="J33" s="52"/>
+      <c r="K33" s="55"/>
       <c r="L33" s="2"/>
       <c r="M33" s="2"/>
       <c r="N33" s="2"/>
@@ -2347,7 +2537,7 @@
       <c r="AA33" s="2"/>
     </row>
     <row r="34" spans="1:27">
-      <c r="A34" s="49"/>
+      <c r="A34" s="58"/>
       <c r="B34" s="46"/>
       <c r="C34" s="46"/>
       <c r="D34" s="46"/>
@@ -2355,9 +2545,9 @@
       <c r="F34" s="30"/>
       <c r="G34" s="35"/>
       <c r="H34" s="35"/>
-      <c r="I34" s="54"/>
-      <c r="J34" s="66"/>
-      <c r="K34" s="54"/>
+      <c r="I34" s="55"/>
+      <c r="J34" s="52"/>
+      <c r="K34" s="55"/>
       <c r="L34" s="2"/>
       <c r="M34" s="2"/>
       <c r="N34" s="2"/>
@@ -2376,7 +2566,7 @@
       <c r="AA34" s="2"/>
     </row>
     <row r="35" spans="1:27">
-      <c r="A35" s="50"/>
+      <c r="A35" s="59"/>
       <c r="B35" s="47"/>
       <c r="C35" s="47"/>
       <c r="D35" s="47"/>
@@ -2384,9 +2574,9 @@
       <c r="F35" s="30"/>
       <c r="G35" s="35"/>
       <c r="H35" s="35"/>
-      <c r="I35" s="55"/>
-      <c r="J35" s="67"/>
-      <c r="K35" s="55"/>
+      <c r="I35" s="56"/>
+      <c r="J35" s="53"/>
+      <c r="K35" s="56"/>
       <c r="L35" s="2"/>
       <c r="M35" s="2"/>
       <c r="N35" s="2"/>
@@ -2405,21 +2595,21 @@
       <c r="AA35" s="2"/>
     </row>
     <row r="36" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A36" s="48" t="s">
+      <c r="A36" s="57" t="s">
         <v>37</v>
       </c>
       <c r="B36" s="45"/>
-      <c r="C36" s="68"/>
+      <c r="C36" s="48"/>
       <c r="D36" s="45"/>
       <c r="E36" s="45"/>
       <c r="F36" s="30"/>
       <c r="G36" s="35"/>
       <c r="H36" s="35"/>
-      <c r="I36" s="53" t="s">
+      <c r="I36" s="54" t="s">
         <v>26</v>
       </c>
-      <c r="J36" s="65"/>
-      <c r="K36" s="53" t="s">
+      <c r="J36" s="51"/>
+      <c r="K36" s="54" t="s">
         <v>28</v>
       </c>
       <c r="L36" s="2"/>
@@ -2440,17 +2630,17 @@
       <c r="AA36" s="2"/>
     </row>
     <row r="37" spans="1:27">
-      <c r="A37" s="49"/>
+      <c r="A37" s="58"/>
       <c r="B37" s="46"/>
-      <c r="C37" s="69"/>
+      <c r="C37" s="49"/>
       <c r="D37" s="46"/>
       <c r="E37" s="46"/>
       <c r="F37" s="30"/>
       <c r="G37" s="35"/>
       <c r="H37" s="35"/>
-      <c r="I37" s="54"/>
-      <c r="J37" s="66"/>
-      <c r="K37" s="54"/>
+      <c r="I37" s="55"/>
+      <c r="J37" s="52"/>
+      <c r="K37" s="55"/>
       <c r="L37" s="2"/>
       <c r="M37" s="2"/>
       <c r="N37" s="2"/>
@@ -2469,17 +2659,17 @@
       <c r="AA37" s="2"/>
     </row>
     <row r="38" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A38" s="49"/>
+      <c r="A38" s="58"/>
       <c r="B38" s="46"/>
-      <c r="C38" s="69"/>
+      <c r="C38" s="49"/>
       <c r="D38" s="46"/>
       <c r="E38" s="46"/>
       <c r="F38" s="30"/>
       <c r="G38" s="35"/>
       <c r="H38" s="35"/>
-      <c r="I38" s="54"/>
-      <c r="J38" s="66"/>
-      <c r="K38" s="54"/>
+      <c r="I38" s="55"/>
+      <c r="J38" s="52"/>
+      <c r="K38" s="55"/>
       <c r="L38" s="2"/>
       <c r="M38" s="2"/>
       <c r="N38" s="2"/>
@@ -2498,17 +2688,17 @@
       <c r="AA38" s="2"/>
     </row>
     <row r="39" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A39" s="50"/>
+      <c r="A39" s="59"/>
       <c r="B39" s="47"/>
-      <c r="C39" s="70"/>
+      <c r="C39" s="50"/>
       <c r="D39" s="47"/>
       <c r="E39" s="47"/>
       <c r="F39" s="30"/>
       <c r="G39" s="35"/>
       <c r="H39" s="35"/>
-      <c r="I39" s="55"/>
-      <c r="J39" s="67"/>
-      <c r="K39" s="55"/>
+      <c r="I39" s="56"/>
+      <c r="J39" s="53"/>
+      <c r="K39" s="56"/>
       <c r="L39" s="2"/>
       <c r="M39" s="2"/>
       <c r="N39" s="2"/>
@@ -2527,21 +2717,21 @@
       <c r="AA39" s="2"/>
     </row>
     <row r="40" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A40" s="48" t="s">
+      <c r="A40" s="57" t="s">
         <v>38</v>
       </c>
       <c r="B40" s="45"/>
-      <c r="C40" s="68"/>
+      <c r="C40" s="48"/>
       <c r="D40" s="45"/>
       <c r="E40" s="45"/>
       <c r="F40" s="30"/>
       <c r="G40" s="35"/>
       <c r="H40" s="35"/>
-      <c r="I40" s="53" t="s">
+      <c r="I40" s="54" t="s">
         <v>26</v>
       </c>
-      <c r="J40" s="65"/>
-      <c r="K40" s="53" t="s">
+      <c r="J40" s="51"/>
+      <c r="K40" s="54" t="s">
         <v>28</v>
       </c>
       <c r="L40" s="2"/>
@@ -2562,17 +2752,17 @@
       <c r="AA40" s="2"/>
     </row>
     <row r="41" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A41" s="49"/>
+      <c r="A41" s="58"/>
       <c r="B41" s="46"/>
-      <c r="C41" s="69"/>
+      <c r="C41" s="49"/>
       <c r="D41" s="46"/>
       <c r="E41" s="46"/>
       <c r="F41" s="30"/>
       <c r="G41" s="35"/>
       <c r="H41" s="35"/>
-      <c r="I41" s="54"/>
-      <c r="J41" s="66"/>
-      <c r="K41" s="54"/>
+      <c r="I41" s="55"/>
+      <c r="J41" s="52"/>
+      <c r="K41" s="55"/>
       <c r="L41" s="2"/>
       <c r="M41" s="2"/>
       <c r="N41" s="2"/>
@@ -2591,17 +2781,17 @@
       <c r="AA41" s="2"/>
     </row>
     <row r="42" spans="1:27">
-      <c r="A42" s="49"/>
+      <c r="A42" s="58"/>
       <c r="B42" s="46"/>
-      <c r="C42" s="69"/>
+      <c r="C42" s="49"/>
       <c r="D42" s="46"/>
       <c r="E42" s="46"/>
       <c r="F42" s="30"/>
       <c r="G42" s="35"/>
       <c r="H42" s="35"/>
-      <c r="I42" s="54"/>
-      <c r="J42" s="66"/>
-      <c r="K42" s="54"/>
+      <c r="I42" s="55"/>
+      <c r="J42" s="52"/>
+      <c r="K42" s="55"/>
       <c r="L42" s="2"/>
       <c r="M42" s="2"/>
       <c r="N42" s="2"/>
@@ -2620,17 +2810,17 @@
       <c r="AA42" s="2"/>
     </row>
     <row r="43" spans="1:27" ht="18.75" customHeight="1">
-      <c r="A43" s="50"/>
+      <c r="A43" s="59"/>
       <c r="B43" s="47"/>
-      <c r="C43" s="70"/>
+      <c r="C43" s="50"/>
       <c r="D43" s="47"/>
       <c r="E43" s="47"/>
       <c r="F43" s="30"/>
       <c r="G43" s="35"/>
       <c r="H43" s="35"/>
-      <c r="I43" s="55"/>
-      <c r="J43" s="67"/>
-      <c r="K43" s="55"/>
+      <c r="I43" s="56"/>
+      <c r="J43" s="53"/>
+      <c r="K43" s="56"/>
       <c r="L43" s="2"/>
       <c r="M43" s="2"/>
       <c r="N43" s="2"/>
@@ -2649,7 +2839,7 @@
       <c r="AA43" s="2"/>
     </row>
     <row r="44" spans="1:27">
-      <c r="A44" s="48" t="s">
+      <c r="A44" s="57" t="s">
         <v>39</v>
       </c>
       <c r="B44" s="45"/>
@@ -2659,11 +2849,11 @@
       <c r="F44" s="30"/>
       <c r="G44" s="35"/>
       <c r="H44" s="35"/>
-      <c r="I44" s="53" t="s">
+      <c r="I44" s="54" t="s">
         <v>26</v>
       </c>
-      <c r="J44" s="65"/>
-      <c r="K44" s="53" t="s">
+      <c r="J44" s="51"/>
+      <c r="K44" s="54" t="s">
         <v>28</v>
       </c>
       <c r="L44" s="2"/>
@@ -2684,7 +2874,7 @@
       <c r="AA44" s="2"/>
     </row>
     <row r="45" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A45" s="49"/>
+      <c r="A45" s="58"/>
       <c r="B45" s="46"/>
       <c r="C45" s="46"/>
       <c r="D45" s="46"/>
@@ -2692,9 +2882,9 @@
       <c r="F45" s="30"/>
       <c r="G45" s="35"/>
       <c r="H45" s="35"/>
-      <c r="I45" s="54"/>
-      <c r="J45" s="66"/>
-      <c r="K45" s="54"/>
+      <c r="I45" s="55"/>
+      <c r="J45" s="52"/>
+      <c r="K45" s="55"/>
       <c r="L45" s="2"/>
       <c r="M45" s="2"/>
       <c r="N45" s="2"/>
@@ -2713,7 +2903,7 @@
       <c r="AA45" s="2"/>
     </row>
     <row r="46" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A46" s="49"/>
+      <c r="A46" s="58"/>
       <c r="B46" s="46"/>
       <c r="C46" s="46"/>
       <c r="D46" s="46"/>
@@ -2721,9 +2911,9 @@
       <c r="F46" s="30"/>
       <c r="G46" s="35"/>
       <c r="H46" s="35"/>
-      <c r="I46" s="54"/>
-      <c r="J46" s="66"/>
-      <c r="K46" s="54"/>
+      <c r="I46" s="55"/>
+      <c r="J46" s="52"/>
+      <c r="K46" s="55"/>
       <c r="L46" s="2"/>
       <c r="M46" s="2"/>
       <c r="N46" s="2"/>
@@ -2742,7 +2932,7 @@
       <c r="AA46" s="2"/>
     </row>
     <row r="47" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A47" s="50"/>
+      <c r="A47" s="59"/>
       <c r="B47" s="47"/>
       <c r="C47" s="47"/>
       <c r="D47" s="47"/>
@@ -2750,9 +2940,9 @@
       <c r="F47" s="30"/>
       <c r="G47" s="35"/>
       <c r="H47" s="35"/>
-      <c r="I47" s="55"/>
-      <c r="J47" s="67"/>
-      <c r="K47" s="55"/>
+      <c r="I47" s="56"/>
+      <c r="J47" s="53"/>
+      <c r="K47" s="56"/>
       <c r="L47" s="2"/>
       <c r="M47" s="2"/>
       <c r="N47" s="2"/>
@@ -2771,7 +2961,7 @@
       <c r="AA47" s="2"/>
     </row>
     <row r="48" spans="1:27">
-      <c r="A48" s="48" t="s">
+      <c r="A48" s="57" t="s">
         <v>40</v>
       </c>
       <c r="B48" s="45"/>
@@ -2781,11 +2971,11 @@
       <c r="F48" s="30"/>
       <c r="G48" s="35"/>
       <c r="H48" s="35"/>
-      <c r="I48" s="53" t="s">
+      <c r="I48" s="54" t="s">
         <v>26</v>
       </c>
-      <c r="J48" s="65"/>
-      <c r="K48" s="53" t="s">
+      <c r="J48" s="51"/>
+      <c r="K48" s="54" t="s">
         <v>28</v>
       </c>
       <c r="L48" s="2"/>
@@ -2806,7 +2996,7 @@
       <c r="AA48" s="2"/>
     </row>
     <row r="49" spans="1:27">
-      <c r="A49" s="49"/>
+      <c r="A49" s="58"/>
       <c r="B49" s="46"/>
       <c r="C49" s="46"/>
       <c r="D49" s="46"/>
@@ -2814,9 +3004,9 @@
       <c r="F49" s="30"/>
       <c r="G49" s="43"/>
       <c r="H49" s="43"/>
-      <c r="I49" s="54"/>
-      <c r="J49" s="66"/>
-      <c r="K49" s="54"/>
+      <c r="I49" s="55"/>
+      <c r="J49" s="52"/>
+      <c r="K49" s="55"/>
       <c r="L49" s="2"/>
       <c r="M49" s="2"/>
       <c r="N49" s="2"/>
@@ -2835,7 +3025,7 @@
       <c r="AA49" s="2"/>
     </row>
     <row r="50" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A50" s="49"/>
+      <c r="A50" s="58"/>
       <c r="B50" s="46"/>
       <c r="C50" s="46"/>
       <c r="D50" s="46"/>
@@ -2843,9 +3033,9 @@
       <c r="F50" s="30"/>
       <c r="G50" s="43"/>
       <c r="H50" s="43"/>
-      <c r="I50" s="54"/>
-      <c r="J50" s="66"/>
-      <c r="K50" s="54"/>
+      <c r="I50" s="55"/>
+      <c r="J50" s="52"/>
+      <c r="K50" s="55"/>
       <c r="L50" s="2"/>
       <c r="M50" s="2"/>
       <c r="N50" s="2"/>
@@ -2864,7 +3054,7 @@
       <c r="AA50" s="2"/>
     </row>
     <row r="51" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A51" s="50"/>
+      <c r="A51" s="59"/>
       <c r="B51" s="47"/>
       <c r="C51" s="47"/>
       <c r="D51" s="47"/>
@@ -2872,9 +3062,9 @@
       <c r="F51" s="30"/>
       <c r="G51" s="35"/>
       <c r="H51" s="35"/>
-      <c r="I51" s="55"/>
-      <c r="J51" s="67"/>
-      <c r="K51" s="55"/>
+      <c r="I51" s="56"/>
+      <c r="J51" s="53"/>
+      <c r="K51" s="56"/>
       <c r="L51" s="2"/>
       <c r="M51" s="2"/>
       <c r="N51" s="2"/>
@@ -2893,7 +3083,7 @@
       <c r="AA51" s="2"/>
     </row>
     <row r="52" spans="1:27">
-      <c r="A52" s="48" t="s">
+      <c r="A52" s="57" t="s">
         <v>41</v>
       </c>
       <c r="B52" s="45"/>
@@ -2903,11 +3093,11 @@
       <c r="F52" s="30"/>
       <c r="G52" s="35"/>
       <c r="H52" s="35"/>
-      <c r="I52" s="53" t="s">
+      <c r="I52" s="54" t="s">
         <v>26</v>
       </c>
-      <c r="J52" s="65"/>
-      <c r="K52" s="53" t="s">
+      <c r="J52" s="51"/>
+      <c r="K52" s="54" t="s">
         <v>28</v>
       </c>
       <c r="L52" s="2"/>
@@ -2928,7 +3118,7 @@
       <c r="AA52" s="2"/>
     </row>
     <row r="53" spans="1:27">
-      <c r="A53" s="49"/>
+      <c r="A53" s="58"/>
       <c r="B53" s="46"/>
       <c r="C53" s="46"/>
       <c r="D53" s="46"/>
@@ -2936,9 +3126,9 @@
       <c r="F53" s="30"/>
       <c r="G53" s="35"/>
       <c r="H53" s="35"/>
-      <c r="I53" s="54"/>
-      <c r="J53" s="66"/>
-      <c r="K53" s="54"/>
+      <c r="I53" s="55"/>
+      <c r="J53" s="52"/>
+      <c r="K53" s="55"/>
       <c r="L53" s="2"/>
       <c r="M53" s="2"/>
       <c r="N53" s="2"/>
@@ -2957,7 +3147,7 @@
       <c r="AA53" s="2"/>
     </row>
     <row r="54" spans="1:27">
-      <c r="A54" s="49"/>
+      <c r="A54" s="58"/>
       <c r="B54" s="46"/>
       <c r="C54" s="46"/>
       <c r="D54" s="46"/>
@@ -2965,9 +3155,9 @@
       <c r="F54" s="30"/>
       <c r="G54" s="35"/>
       <c r="H54" s="35"/>
-      <c r="I54" s="54"/>
-      <c r="J54" s="66"/>
-      <c r="K54" s="54"/>
+      <c r="I54" s="55"/>
+      <c r="J54" s="52"/>
+      <c r="K54" s="55"/>
       <c r="L54" s="2"/>
       <c r="M54" s="2"/>
       <c r="N54" s="2"/>
@@ -2986,7 +3176,7 @@
       <c r="AA54" s="2"/>
     </row>
     <row r="55" spans="1:27">
-      <c r="A55" s="50"/>
+      <c r="A55" s="59"/>
       <c r="B55" s="47"/>
       <c r="C55" s="47"/>
       <c r="D55" s="47"/>
@@ -2994,9 +3184,9 @@
       <c r="F55" s="30"/>
       <c r="G55" s="35"/>
       <c r="H55" s="35"/>
-      <c r="I55" s="55"/>
-      <c r="J55" s="67"/>
-      <c r="K55" s="55"/>
+      <c r="I55" s="56"/>
+      <c r="J55" s="53"/>
+      <c r="K55" s="56"/>
       <c r="L55" s="2"/>
       <c r="M55" s="2"/>
       <c r="N55" s="2"/>
@@ -3015,7 +3205,7 @@
       <c r="AA55" s="2"/>
     </row>
     <row r="56" spans="1:27">
-      <c r="A56" s="48" t="s">
+      <c r="A56" s="57" t="s">
         <v>42</v>
       </c>
       <c r="B56" s="45"/>
@@ -3025,11 +3215,11 @@
       <c r="F56" s="30"/>
       <c r="G56" s="35"/>
       <c r="H56" s="35"/>
-      <c r="I56" s="53" t="s">
+      <c r="I56" s="54" t="s">
         <v>26</v>
       </c>
-      <c r="J56" s="65"/>
-      <c r="K56" s="53" t="s">
+      <c r="J56" s="51"/>
+      <c r="K56" s="54" t="s">
         <v>28</v>
       </c>
       <c r="L56" s="2"/>
@@ -3050,7 +3240,7 @@
       <c r="AA56" s="2"/>
     </row>
     <row r="57" spans="1:27">
-      <c r="A57" s="49"/>
+      <c r="A57" s="58"/>
       <c r="B57" s="46"/>
       <c r="C57" s="46"/>
       <c r="D57" s="46"/>
@@ -3058,9 +3248,9 @@
       <c r="F57" s="30"/>
       <c r="G57" s="35"/>
       <c r="H57" s="35"/>
-      <c r="I57" s="54"/>
-      <c r="J57" s="66"/>
-      <c r="K57" s="54"/>
+      <c r="I57" s="55"/>
+      <c r="J57" s="52"/>
+      <c r="K57" s="55"/>
       <c r="L57" s="2"/>
       <c r="M57" s="2"/>
       <c r="N57" s="2"/>
@@ -3079,7 +3269,7 @@
       <c r="AA57" s="2"/>
     </row>
     <row r="58" spans="1:27">
-      <c r="A58" s="49"/>
+      <c r="A58" s="58"/>
       <c r="B58" s="46"/>
       <c r="C58" s="46"/>
       <c r="D58" s="46"/>
@@ -3087,9 +3277,9 @@
       <c r="F58" s="30"/>
       <c r="G58" s="35"/>
       <c r="H58" s="35"/>
-      <c r="I58" s="54"/>
-      <c r="J58" s="66"/>
-      <c r="K58" s="54"/>
+      <c r="I58" s="55"/>
+      <c r="J58" s="52"/>
+      <c r="K58" s="55"/>
       <c r="L58" s="2"/>
       <c r="M58" s="2"/>
       <c r="N58" s="2"/>
@@ -3108,7 +3298,7 @@
       <c r="AA58" s="2"/>
     </row>
     <row r="59" spans="1:27">
-      <c r="A59" s="50"/>
+      <c r="A59" s="59"/>
       <c r="B59" s="47"/>
       <c r="C59" s="47"/>
       <c r="D59" s="47"/>
@@ -3116,9 +3306,9 @@
       <c r="F59" s="30"/>
       <c r="G59" s="35"/>
       <c r="H59" s="35"/>
-      <c r="I59" s="55"/>
-      <c r="J59" s="67"/>
-      <c r="K59" s="55"/>
+      <c r="I59" s="56"/>
+      <c r="J59" s="53"/>
+      <c r="K59" s="56"/>
       <c r="L59" s="2"/>
       <c r="M59" s="2"/>
       <c r="N59" s="2"/>
@@ -3137,7 +3327,7 @@
       <c r="AA59" s="2"/>
     </row>
     <row r="60" spans="1:27">
-      <c r="A60" s="48" t="s">
+      <c r="A60" s="57" t="s">
         <v>43</v>
       </c>
       <c r="B60" s="45"/>
@@ -3147,11 +3337,11 @@
       <c r="F60" s="30"/>
       <c r="G60" s="35"/>
       <c r="H60" s="35"/>
-      <c r="I60" s="53" t="s">
+      <c r="I60" s="54" t="s">
         <v>26</v>
       </c>
-      <c r="J60" s="65"/>
-      <c r="K60" s="53" t="s">
+      <c r="J60" s="51"/>
+      <c r="K60" s="54" t="s">
         <v>28</v>
       </c>
       <c r="L60" s="2"/>
@@ -3172,7 +3362,7 @@
       <c r="AA60" s="2"/>
     </row>
     <row r="61" spans="1:27">
-      <c r="A61" s="49"/>
+      <c r="A61" s="58"/>
       <c r="B61" s="46"/>
       <c r="C61" s="46"/>
       <c r="D61" s="46"/>
@@ -3180,9 +3370,9 @@
       <c r="F61" s="30"/>
       <c r="G61" s="35"/>
       <c r="H61" s="35"/>
-      <c r="I61" s="54"/>
-      <c r="J61" s="66"/>
-      <c r="K61" s="54"/>
+      <c r="I61" s="55"/>
+      <c r="J61" s="52"/>
+      <c r="K61" s="55"/>
       <c r="L61" s="2"/>
       <c r="M61" s="2"/>
       <c r="N61" s="2"/>
@@ -3201,7 +3391,7 @@
       <c r="AA61" s="2"/>
     </row>
     <row r="62" spans="1:27">
-      <c r="A62" s="49"/>
+      <c r="A62" s="58"/>
       <c r="B62" s="46"/>
       <c r="C62" s="46"/>
       <c r="D62" s="46"/>
@@ -3209,9 +3399,9 @@
       <c r="F62" s="30"/>
       <c r="G62" s="35"/>
       <c r="H62" s="35"/>
-      <c r="I62" s="54"/>
-      <c r="J62" s="66"/>
-      <c r="K62" s="54"/>
+      <c r="I62" s="55"/>
+      <c r="J62" s="52"/>
+      <c r="K62" s="55"/>
       <c r="L62" s="2"/>
       <c r="M62" s="2"/>
       <c r="N62" s="2"/>
@@ -3230,7 +3420,7 @@
       <c r="AA62" s="2"/>
     </row>
     <row r="63" spans="1:27">
-      <c r="A63" s="50"/>
+      <c r="A63" s="59"/>
       <c r="B63" s="47"/>
       <c r="C63" s="47"/>
       <c r="D63" s="47"/>
@@ -3238,9 +3428,9 @@
       <c r="F63" s="30"/>
       <c r="G63" s="35"/>
       <c r="H63" s="36"/>
-      <c r="I63" s="55"/>
-      <c r="J63" s="67"/>
-      <c r="K63" s="55"/>
+      <c r="I63" s="56"/>
+      <c r="J63" s="53"/>
+      <c r="K63" s="56"/>
       <c r="L63" s="2"/>
       <c r="M63" s="2"/>
       <c r="N63" s="2"/>
@@ -3259,7 +3449,7 @@
       <c r="AA63" s="2"/>
     </row>
     <row r="64" spans="1:27">
-      <c r="A64" s="48" t="s">
+      <c r="A64" s="57" t="s">
         <v>44</v>
       </c>
       <c r="B64" s="45"/>
@@ -3269,11 +3459,11 @@
       <c r="F64" s="30"/>
       <c r="G64" s="35"/>
       <c r="H64" s="35"/>
-      <c r="I64" s="53" t="s">
+      <c r="I64" s="54" t="s">
         <v>26</v>
       </c>
-      <c r="J64" s="65"/>
-      <c r="K64" s="53" t="s">
+      <c r="J64" s="51"/>
+      <c r="K64" s="54" t="s">
         <v>28</v>
       </c>
       <c r="L64" s="2"/>
@@ -3294,7 +3484,7 @@
       <c r="AA64" s="2"/>
     </row>
     <row r="65" spans="1:27">
-      <c r="A65" s="49"/>
+      <c r="A65" s="58"/>
       <c r="B65" s="46"/>
       <c r="C65" s="46"/>
       <c r="D65" s="46"/>
@@ -3302,9 +3492,9 @@
       <c r="F65" s="30"/>
       <c r="G65" s="35"/>
       <c r="H65" s="35"/>
-      <c r="I65" s="54"/>
-      <c r="J65" s="66"/>
-      <c r="K65" s="54"/>
+      <c r="I65" s="55"/>
+      <c r="J65" s="52"/>
+      <c r="K65" s="55"/>
       <c r="L65" s="2"/>
       <c r="M65" s="2"/>
       <c r="N65" s="2"/>
@@ -3323,7 +3513,7 @@
       <c r="AA65" s="2"/>
     </row>
     <row r="66" spans="1:27">
-      <c r="A66" s="49"/>
+      <c r="A66" s="58"/>
       <c r="B66" s="46"/>
       <c r="C66" s="46"/>
       <c r="D66" s="46"/>
@@ -3331,9 +3521,9 @@
       <c r="F66" s="30"/>
       <c r="G66" s="35"/>
       <c r="H66" s="35"/>
-      <c r="I66" s="54"/>
-      <c r="J66" s="66"/>
-      <c r="K66" s="54"/>
+      <c r="I66" s="55"/>
+      <c r="J66" s="52"/>
+      <c r="K66" s="55"/>
       <c r="L66" s="2"/>
       <c r="M66" s="2"/>
       <c r="N66" s="2"/>
@@ -3352,7 +3542,7 @@
       <c r="AA66" s="2"/>
     </row>
     <row r="67" spans="1:27">
-      <c r="A67" s="50"/>
+      <c r="A67" s="59"/>
       <c r="B67" s="47"/>
       <c r="C67" s="47"/>
       <c r="D67" s="47"/>
@@ -3360,9 +3550,9 @@
       <c r="F67" s="30"/>
       <c r="G67" s="35"/>
       <c r="H67" s="36"/>
-      <c r="I67" s="55"/>
-      <c r="J67" s="67"/>
-      <c r="K67" s="55"/>
+      <c r="I67" s="56"/>
+      <c r="J67" s="53"/>
+      <c r="K67" s="56"/>
       <c r="L67" s="2"/>
       <c r="M67" s="2"/>
       <c r="N67" s="2"/>
@@ -3381,7 +3571,7 @@
       <c r="AA67" s="2"/>
     </row>
     <row r="68" spans="1:27">
-      <c r="A68" s="48" t="s">
+      <c r="A68" s="57" t="s">
         <v>45</v>
       </c>
       <c r="B68" s="45"/>
@@ -3391,11 +3581,11 @@
       <c r="F68" s="30"/>
       <c r="G68" s="35"/>
       <c r="H68" s="35"/>
-      <c r="I68" s="53" t="s">
+      <c r="I68" s="54" t="s">
         <v>26</v>
       </c>
-      <c r="J68" s="65"/>
-      <c r="K68" s="53" t="s">
+      <c r="J68" s="51"/>
+      <c r="K68" s="54" t="s">
         <v>28</v>
       </c>
       <c r="L68" s="2"/>
@@ -3416,7 +3606,7 @@
       <c r="AA68" s="2"/>
     </row>
     <row r="69" spans="1:27">
-      <c r="A69" s="49"/>
+      <c r="A69" s="58"/>
       <c r="B69" s="46"/>
       <c r="C69" s="46"/>
       <c r="D69" s="46"/>
@@ -3424,9 +3614,9 @@
       <c r="F69" s="30"/>
       <c r="G69" s="36"/>
       <c r="H69" s="36"/>
-      <c r="I69" s="54"/>
-      <c r="J69" s="66"/>
-      <c r="K69" s="54"/>
+      <c r="I69" s="55"/>
+      <c r="J69" s="52"/>
+      <c r="K69" s="55"/>
       <c r="L69" s="2"/>
       <c r="M69" s="2"/>
       <c r="N69" s="2"/>
@@ -3445,7 +3635,7 @@
       <c r="AA69" s="2"/>
     </row>
     <row r="70" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A70" s="49"/>
+      <c r="A70" s="58"/>
       <c r="B70" s="46"/>
       <c r="C70" s="46"/>
       <c r="D70" s="46"/>
@@ -3453,9 +3643,9 @@
       <c r="F70" s="30"/>
       <c r="G70" s="43"/>
       <c r="H70" s="43"/>
-      <c r="I70" s="54"/>
-      <c r="J70" s="66"/>
-      <c r="K70" s="54"/>
+      <c r="I70" s="55"/>
+      <c r="J70" s="52"/>
+      <c r="K70" s="55"/>
       <c r="L70" s="2"/>
       <c r="M70" s="2"/>
       <c r="N70" s="2"/>
@@ -3474,7 +3664,7 @@
       <c r="AA70" s="2"/>
     </row>
     <row r="71" spans="1:27">
-      <c r="A71" s="50"/>
+      <c r="A71" s="59"/>
       <c r="B71" s="47"/>
       <c r="C71" s="47"/>
       <c r="D71" s="47"/>
@@ -3482,9 +3672,9 @@
       <c r="F71" s="30"/>
       <c r="G71" s="43"/>
       <c r="H71" s="43"/>
-      <c r="I71" s="55"/>
-      <c r="J71" s="67"/>
-      <c r="K71" s="55"/>
+      <c r="I71" s="56"/>
+      <c r="J71" s="53"/>
+      <c r="K71" s="56"/>
       <c r="L71" s="2"/>
       <c r="M71" s="2"/>
       <c r="N71" s="2"/>
@@ -3503,7 +3693,7 @@
       <c r="AA71" s="2"/>
     </row>
     <row r="72" spans="1:27">
-      <c r="A72" s="48" t="s">
+      <c r="A72" s="57" t="s">
         <v>46</v>
       </c>
       <c r="B72" s="45"/>
@@ -3513,11 +3703,11 @@
       <c r="F72" s="30"/>
       <c r="G72" s="35"/>
       <c r="H72" s="35"/>
-      <c r="I72" s="53" t="s">
+      <c r="I72" s="54" t="s">
         <v>26</v>
       </c>
-      <c r="J72" s="65"/>
-      <c r="K72" s="53" t="s">
+      <c r="J72" s="51"/>
+      <c r="K72" s="54" t="s">
         <v>28</v>
       </c>
       <c r="L72" s="2"/>
@@ -3538,7 +3728,7 @@
       <c r="AA72" s="2"/>
     </row>
     <row r="73" spans="1:27">
-      <c r="A73" s="49"/>
+      <c r="A73" s="58"/>
       <c r="B73" s="46"/>
       <c r="C73" s="46"/>
       <c r="D73" s="46"/>
@@ -3546,9 +3736,9 @@
       <c r="F73" s="30"/>
       <c r="G73" s="36"/>
       <c r="H73" s="36"/>
-      <c r="I73" s="54"/>
-      <c r="J73" s="66"/>
-      <c r="K73" s="54"/>
+      <c r="I73" s="55"/>
+      <c r="J73" s="52"/>
+      <c r="K73" s="55"/>
       <c r="L73" s="2"/>
       <c r="M73" s="2"/>
       <c r="N73" s="2"/>
@@ -3567,7 +3757,7 @@
       <c r="AA73" s="2"/>
     </row>
     <row r="74" spans="1:27">
-      <c r="A74" s="49"/>
+      <c r="A74" s="58"/>
       <c r="B74" s="46"/>
       <c r="C74" s="46"/>
       <c r="D74" s="46"/>
@@ -3575,9 +3765,9 @@
       <c r="F74" s="30"/>
       <c r="G74" s="36"/>
       <c r="H74" s="36"/>
-      <c r="I74" s="54"/>
-      <c r="J74" s="66"/>
-      <c r="K74" s="54"/>
+      <c r="I74" s="55"/>
+      <c r="J74" s="52"/>
+      <c r="K74" s="55"/>
       <c r="L74" s="2"/>
       <c r="M74" s="2"/>
       <c r="N74" s="2"/>
@@ -3596,7 +3786,7 @@
       <c r="AA74" s="2"/>
     </row>
     <row r="75" spans="1:27">
-      <c r="A75" s="50"/>
+      <c r="A75" s="59"/>
       <c r="B75" s="47"/>
       <c r="C75" s="47"/>
       <c r="D75" s="47"/>
@@ -3604,9 +3794,9 @@
       <c r="F75" s="30"/>
       <c r="G75" s="35"/>
       <c r="H75" s="36"/>
-      <c r="I75" s="55"/>
-      <c r="J75" s="67"/>
-      <c r="K75" s="55"/>
+      <c r="I75" s="56"/>
+      <c r="J75" s="53"/>
+      <c r="K75" s="56"/>
       <c r="L75" s="2"/>
       <c r="M75" s="2"/>
       <c r="N75" s="2"/>
@@ -3625,7 +3815,7 @@
       <c r="AA75" s="2"/>
     </row>
     <row r="76" spans="1:27">
-      <c r="A76" s="48" t="s">
+      <c r="A76" s="57" t="s">
         <v>47</v>
       </c>
       <c r="B76" s="45"/>
@@ -3635,11 +3825,11 @@
       <c r="F76" s="30"/>
       <c r="G76" s="35"/>
       <c r="H76" s="35"/>
-      <c r="I76" s="53" t="s">
+      <c r="I76" s="54" t="s">
         <v>26</v>
       </c>
-      <c r="J76" s="65"/>
-      <c r="K76" s="53" t="s">
+      <c r="J76" s="51"/>
+      <c r="K76" s="54" t="s">
         <v>28</v>
       </c>
       <c r="L76" s="2"/>
@@ -3660,7 +3850,7 @@
       <c r="AA76" s="2"/>
     </row>
     <row r="77" spans="1:27">
-      <c r="A77" s="49"/>
+      <c r="A77" s="58"/>
       <c r="B77" s="46"/>
       <c r="C77" s="46"/>
       <c r="D77" s="46"/>
@@ -3668,9 +3858,9 @@
       <c r="F77" s="30"/>
       <c r="G77" s="35"/>
       <c r="H77" s="36"/>
-      <c r="I77" s="54"/>
-      <c r="J77" s="66"/>
-      <c r="K77" s="54"/>
+      <c r="I77" s="55"/>
+      <c r="J77" s="52"/>
+      <c r="K77" s="55"/>
       <c r="L77" s="2"/>
       <c r="M77" s="2"/>
       <c r="N77" s="2"/>
@@ -3689,7 +3879,7 @@
       <c r="AA77" s="2"/>
     </row>
     <row r="78" spans="1:27">
-      <c r="A78" s="49"/>
+      <c r="A78" s="58"/>
       <c r="B78" s="46"/>
       <c r="C78" s="46"/>
       <c r="D78" s="46"/>
@@ -3697,9 +3887,9 @@
       <c r="F78" s="30"/>
       <c r="G78" s="36"/>
       <c r="H78" s="36"/>
-      <c r="I78" s="54"/>
-      <c r="J78" s="66"/>
-      <c r="K78" s="54"/>
+      <c r="I78" s="55"/>
+      <c r="J78" s="52"/>
+      <c r="K78" s="55"/>
       <c r="L78" s="2"/>
       <c r="M78" s="2"/>
       <c r="N78" s="2"/>
@@ -3718,7 +3908,7 @@
       <c r="AA78" s="2"/>
     </row>
     <row r="79" spans="1:27">
-      <c r="A79" s="50"/>
+      <c r="A79" s="59"/>
       <c r="B79" s="47"/>
       <c r="C79" s="47"/>
       <c r="D79" s="47"/>
@@ -3726,9 +3916,9 @@
       <c r="F79" s="30"/>
       <c r="G79" s="35"/>
       <c r="H79" s="35"/>
-      <c r="I79" s="55"/>
-      <c r="J79" s="67"/>
-      <c r="K79" s="55"/>
+      <c r="I79" s="56"/>
+      <c r="J79" s="53"/>
+      <c r="K79" s="56"/>
       <c r="L79" s="2"/>
       <c r="M79" s="2"/>
       <c r="N79" s="2"/>
@@ -3747,21 +3937,21 @@
       <c r="AA79" s="2"/>
     </row>
     <row r="80" spans="1:27">
-      <c r="A80" s="48" t="s">
+      <c r="A80" s="57" t="s">
         <v>48</v>
       </c>
       <c r="B80" s="45"/>
-      <c r="C80" s="68"/>
+      <c r="C80" s="48"/>
       <c r="D80" s="45"/>
       <c r="E80" s="45"/>
       <c r="F80" s="30"/>
       <c r="G80" s="35"/>
       <c r="H80" s="35"/>
-      <c r="I80" s="53" t="s">
+      <c r="I80" s="54" t="s">
         <v>26</v>
       </c>
-      <c r="J80" s="65"/>
-      <c r="K80" s="53" t="s">
+      <c r="J80" s="51"/>
+      <c r="K80" s="54" t="s">
         <v>28</v>
       </c>
       <c r="L80" s="2"/>
@@ -3782,17 +3972,17 @@
       <c r="AA80" s="2"/>
     </row>
     <row r="81" spans="1:27">
-      <c r="A81" s="49"/>
+      <c r="A81" s="58"/>
       <c r="B81" s="46"/>
-      <c r="C81" s="69"/>
+      <c r="C81" s="49"/>
       <c r="D81" s="46"/>
       <c r="E81" s="46"/>
       <c r="F81" s="30"/>
       <c r="G81" s="35"/>
       <c r="H81" s="35"/>
-      <c r="I81" s="54"/>
-      <c r="J81" s="66"/>
-      <c r="K81" s="54"/>
+      <c r="I81" s="55"/>
+      <c r="J81" s="52"/>
+      <c r="K81" s="55"/>
       <c r="L81" s="2"/>
       <c r="M81" s="2"/>
       <c r="N81" s="2"/>
@@ -3811,17 +4001,17 @@
       <c r="AA81" s="2"/>
     </row>
     <row r="82" spans="1:27">
-      <c r="A82" s="49"/>
+      <c r="A82" s="58"/>
       <c r="B82" s="46"/>
-      <c r="C82" s="69"/>
+      <c r="C82" s="49"/>
       <c r="D82" s="46"/>
       <c r="E82" s="46"/>
       <c r="F82" s="30"/>
       <c r="G82" s="35"/>
       <c r="H82" s="35"/>
-      <c r="I82" s="54"/>
-      <c r="J82" s="66"/>
-      <c r="K82" s="54"/>
+      <c r="I82" s="55"/>
+      <c r="J82" s="52"/>
+      <c r="K82" s="55"/>
       <c r="L82" s="2"/>
       <c r="M82" s="2"/>
       <c r="N82" s="2"/>
@@ -3840,17 +4030,17 @@
       <c r="AA82" s="2"/>
     </row>
     <row r="83" spans="1:27">
-      <c r="A83" s="50"/>
+      <c r="A83" s="59"/>
       <c r="B83" s="47"/>
-      <c r="C83" s="70"/>
+      <c r="C83" s="50"/>
       <c r="D83" s="47"/>
       <c r="E83" s="47"/>
       <c r="F83" s="30"/>
       <c r="G83" s="35"/>
       <c r="H83" s="35"/>
-      <c r="I83" s="55"/>
-      <c r="J83" s="67"/>
-      <c r="K83" s="55"/>
+      <c r="I83" s="56"/>
+      <c r="J83" s="53"/>
+      <c r="K83" s="56"/>
       <c r="L83" s="2"/>
       <c r="M83" s="2"/>
       <c r="N83" s="2"/>
@@ -28578,42 +28768,124 @@
     </row>
   </sheetData>
   <mergeCells count="178">
-    <mergeCell ref="B36:B39"/>
-    <mergeCell ref="C36:C39"/>
-    <mergeCell ref="D36:D39"/>
-    <mergeCell ref="E36:E39"/>
-    <mergeCell ref="J44:J47"/>
-    <mergeCell ref="K44:K47"/>
-    <mergeCell ref="I48:I51"/>
-    <mergeCell ref="J48:J51"/>
-    <mergeCell ref="K48:K51"/>
-    <mergeCell ref="B48:B51"/>
-    <mergeCell ref="C48:C51"/>
-    <mergeCell ref="D48:D51"/>
-    <mergeCell ref="E48:E51"/>
-    <mergeCell ref="K40:K43"/>
-    <mergeCell ref="I40:I43"/>
-    <mergeCell ref="B40:B43"/>
-    <mergeCell ref="J36:J39"/>
-    <mergeCell ref="C40:C43"/>
-    <mergeCell ref="D40:D43"/>
-    <mergeCell ref="E40:E43"/>
-    <mergeCell ref="A76:A79"/>
-    <mergeCell ref="B76:B79"/>
-    <mergeCell ref="C76:C79"/>
-    <mergeCell ref="D76:D79"/>
-    <mergeCell ref="E76:E79"/>
-    <mergeCell ref="I76:I79"/>
-    <mergeCell ref="J76:J79"/>
-    <mergeCell ref="K76:K79"/>
-    <mergeCell ref="J80:J83"/>
-    <mergeCell ref="K80:K83"/>
-    <mergeCell ref="A80:A83"/>
-    <mergeCell ref="B80:B83"/>
-    <mergeCell ref="C80:C83"/>
-    <mergeCell ref="D80:D83"/>
-    <mergeCell ref="E80:E83"/>
-    <mergeCell ref="I80:I83"/>
+    <mergeCell ref="C32:C35"/>
+    <mergeCell ref="B32:B35"/>
+    <mergeCell ref="B28:B31"/>
+    <mergeCell ref="C4:C7"/>
+    <mergeCell ref="C8:C11"/>
+    <mergeCell ref="C12:C15"/>
+    <mergeCell ref="C16:C19"/>
+    <mergeCell ref="C20:C23"/>
+    <mergeCell ref="C24:C27"/>
+    <mergeCell ref="C28:C31"/>
+    <mergeCell ref="A4:A7"/>
+    <mergeCell ref="A8:A11"/>
+    <mergeCell ref="A12:A15"/>
+    <mergeCell ref="A16:A19"/>
+    <mergeCell ref="A20:A23"/>
+    <mergeCell ref="A24:A27"/>
+    <mergeCell ref="B24:B27"/>
+    <mergeCell ref="B20:B23"/>
+    <mergeCell ref="B16:B19"/>
+    <mergeCell ref="B12:B15"/>
+    <mergeCell ref="B8:B11"/>
+    <mergeCell ref="B4:B7"/>
+    <mergeCell ref="K2:K3"/>
+    <mergeCell ref="I4:I7"/>
+    <mergeCell ref="I8:I11"/>
+    <mergeCell ref="I12:I15"/>
+    <mergeCell ref="I16:I19"/>
+    <mergeCell ref="E28:E31"/>
+    <mergeCell ref="E2:E3"/>
+    <mergeCell ref="G12:G13"/>
+    <mergeCell ref="G8:G9"/>
+    <mergeCell ref="F12:F13"/>
+    <mergeCell ref="F4:F5"/>
+    <mergeCell ref="F8:F9"/>
+    <mergeCell ref="K28:K31"/>
+    <mergeCell ref="E16:E19"/>
+    <mergeCell ref="E20:E23"/>
+    <mergeCell ref="E24:E27"/>
+    <mergeCell ref="F2:H2"/>
+    <mergeCell ref="I2:I3"/>
+    <mergeCell ref="I20:I23"/>
+    <mergeCell ref="I24:I27"/>
+    <mergeCell ref="I28:I31"/>
+    <mergeCell ref="E4:E7"/>
+    <mergeCell ref="E8:E11"/>
+    <mergeCell ref="E12:E15"/>
+    <mergeCell ref="E32:E35"/>
+    <mergeCell ref="C2:C3"/>
+    <mergeCell ref="H4:H5"/>
+    <mergeCell ref="G4:G5"/>
+    <mergeCell ref="H8:H9"/>
+    <mergeCell ref="H12:H13"/>
+    <mergeCell ref="K32:K35"/>
+    <mergeCell ref="K36:K39"/>
+    <mergeCell ref="J4:J7"/>
+    <mergeCell ref="J8:J11"/>
+    <mergeCell ref="J12:J15"/>
+    <mergeCell ref="J16:J19"/>
+    <mergeCell ref="J20:J23"/>
+    <mergeCell ref="J24:J27"/>
+    <mergeCell ref="J28:J31"/>
+    <mergeCell ref="I32:I35"/>
+    <mergeCell ref="I36:I39"/>
+    <mergeCell ref="K4:K7"/>
+    <mergeCell ref="K8:K11"/>
+    <mergeCell ref="K12:K15"/>
+    <mergeCell ref="K16:K19"/>
+    <mergeCell ref="K20:K23"/>
+    <mergeCell ref="K24:K27"/>
+    <mergeCell ref="J2:J3"/>
+    <mergeCell ref="J32:J35"/>
+    <mergeCell ref="B2:B3"/>
+    <mergeCell ref="A2:A3"/>
+    <mergeCell ref="A52:A55"/>
+    <mergeCell ref="B52:B55"/>
+    <mergeCell ref="C56:C59"/>
+    <mergeCell ref="D56:D59"/>
+    <mergeCell ref="C52:C55"/>
+    <mergeCell ref="D52:D55"/>
+    <mergeCell ref="A44:A47"/>
+    <mergeCell ref="A48:A51"/>
+    <mergeCell ref="D24:D27"/>
+    <mergeCell ref="D20:D23"/>
+    <mergeCell ref="D16:D19"/>
+    <mergeCell ref="D12:D15"/>
+    <mergeCell ref="D8:D11"/>
+    <mergeCell ref="D4:D7"/>
+    <mergeCell ref="A28:A31"/>
+    <mergeCell ref="A32:A35"/>
+    <mergeCell ref="A36:A39"/>
+    <mergeCell ref="A40:A43"/>
+    <mergeCell ref="D32:D35"/>
+    <mergeCell ref="D28:D31"/>
+    <mergeCell ref="A56:A59"/>
+    <mergeCell ref="D2:D3"/>
+    <mergeCell ref="J52:J55"/>
+    <mergeCell ref="K52:K55"/>
+    <mergeCell ref="E52:E55"/>
+    <mergeCell ref="B44:B47"/>
+    <mergeCell ref="C44:C47"/>
+    <mergeCell ref="D44:D47"/>
+    <mergeCell ref="E44:E47"/>
+    <mergeCell ref="B64:B67"/>
+    <mergeCell ref="C64:C67"/>
+    <mergeCell ref="D64:D67"/>
+    <mergeCell ref="E64:E67"/>
+    <mergeCell ref="I64:I67"/>
+    <mergeCell ref="B60:B63"/>
+    <mergeCell ref="C60:C63"/>
+    <mergeCell ref="D60:D63"/>
+    <mergeCell ref="E60:E63"/>
+    <mergeCell ref="I60:I63"/>
+    <mergeCell ref="E56:E59"/>
+    <mergeCell ref="I52:I55"/>
+    <mergeCell ref="B56:B59"/>
+    <mergeCell ref="I56:I59"/>
+    <mergeCell ref="I44:I47"/>
+    <mergeCell ref="J40:J43"/>
     <mergeCell ref="A60:A63"/>
     <mergeCell ref="J56:J59"/>
     <mergeCell ref="K56:K59"/>
@@ -28638,170 +28910,108 @@
     <mergeCell ref="A64:A67"/>
     <mergeCell ref="J64:J67"/>
     <mergeCell ref="K64:K67"/>
-    <mergeCell ref="D2:D3"/>
-    <mergeCell ref="J52:J55"/>
-    <mergeCell ref="K52:K55"/>
-    <mergeCell ref="E52:E55"/>
-    <mergeCell ref="B44:B47"/>
-    <mergeCell ref="C44:C47"/>
-    <mergeCell ref="D44:D47"/>
-    <mergeCell ref="E44:E47"/>
-    <mergeCell ref="B64:B67"/>
-    <mergeCell ref="C64:C67"/>
-    <mergeCell ref="D64:D67"/>
-    <mergeCell ref="E64:E67"/>
-    <mergeCell ref="I64:I67"/>
-    <mergeCell ref="B60:B63"/>
-    <mergeCell ref="C60:C63"/>
-    <mergeCell ref="D60:D63"/>
-    <mergeCell ref="E60:E63"/>
-    <mergeCell ref="I60:I63"/>
-    <mergeCell ref="E56:E59"/>
-    <mergeCell ref="I52:I55"/>
-    <mergeCell ref="B56:B59"/>
-    <mergeCell ref="I56:I59"/>
-    <mergeCell ref="I44:I47"/>
-    <mergeCell ref="J40:J43"/>
-    <mergeCell ref="J32:J35"/>
-    <mergeCell ref="B2:B3"/>
-    <mergeCell ref="A2:A3"/>
-    <mergeCell ref="A52:A55"/>
-    <mergeCell ref="B52:B55"/>
-    <mergeCell ref="C56:C59"/>
-    <mergeCell ref="D56:D59"/>
-    <mergeCell ref="C52:C55"/>
-    <mergeCell ref="D52:D55"/>
-    <mergeCell ref="A44:A47"/>
-    <mergeCell ref="A48:A51"/>
-    <mergeCell ref="D24:D27"/>
-    <mergeCell ref="D20:D23"/>
-    <mergeCell ref="D16:D19"/>
-    <mergeCell ref="D12:D15"/>
-    <mergeCell ref="D8:D11"/>
-    <mergeCell ref="D4:D7"/>
-    <mergeCell ref="A28:A31"/>
-    <mergeCell ref="A32:A35"/>
-    <mergeCell ref="A36:A39"/>
-    <mergeCell ref="A40:A43"/>
-    <mergeCell ref="D32:D35"/>
-    <mergeCell ref="D28:D31"/>
-    <mergeCell ref="A56:A59"/>
-    <mergeCell ref="E32:E35"/>
-    <mergeCell ref="C2:C3"/>
-    <mergeCell ref="H4:H5"/>
-    <mergeCell ref="G4:G5"/>
-    <mergeCell ref="H8:H9"/>
-    <mergeCell ref="H12:H13"/>
-    <mergeCell ref="K32:K35"/>
-    <mergeCell ref="K36:K39"/>
-    <mergeCell ref="J4:J7"/>
-    <mergeCell ref="J8:J11"/>
-    <mergeCell ref="J12:J15"/>
-    <mergeCell ref="J16:J19"/>
-    <mergeCell ref="J20:J23"/>
-    <mergeCell ref="J24:J27"/>
-    <mergeCell ref="J28:J31"/>
-    <mergeCell ref="I32:I35"/>
-    <mergeCell ref="I36:I39"/>
-    <mergeCell ref="K4:K7"/>
-    <mergeCell ref="K8:K11"/>
-    <mergeCell ref="K12:K15"/>
-    <mergeCell ref="K16:K19"/>
-    <mergeCell ref="K20:K23"/>
-    <mergeCell ref="K24:K27"/>
-    <mergeCell ref="J2:J3"/>
-    <mergeCell ref="K2:K3"/>
-    <mergeCell ref="I4:I7"/>
-    <mergeCell ref="I8:I11"/>
-    <mergeCell ref="I12:I15"/>
-    <mergeCell ref="I16:I19"/>
-    <mergeCell ref="E28:E31"/>
-    <mergeCell ref="E2:E3"/>
-    <mergeCell ref="G12:G13"/>
-    <mergeCell ref="G8:G9"/>
-    <mergeCell ref="F12:F13"/>
-    <mergeCell ref="F4:F5"/>
-    <mergeCell ref="F8:F9"/>
-    <mergeCell ref="K28:K31"/>
-    <mergeCell ref="E16:E19"/>
-    <mergeCell ref="E20:E23"/>
-    <mergeCell ref="E24:E27"/>
-    <mergeCell ref="F2:H2"/>
-    <mergeCell ref="I2:I3"/>
-    <mergeCell ref="I20:I23"/>
-    <mergeCell ref="I24:I27"/>
-    <mergeCell ref="I28:I31"/>
-    <mergeCell ref="E4:E7"/>
-    <mergeCell ref="E8:E11"/>
-    <mergeCell ref="E12:E15"/>
-    <mergeCell ref="A4:A7"/>
-    <mergeCell ref="A8:A11"/>
-    <mergeCell ref="A12:A15"/>
-    <mergeCell ref="A16:A19"/>
-    <mergeCell ref="A20:A23"/>
-    <mergeCell ref="A24:A27"/>
-    <mergeCell ref="B24:B27"/>
-    <mergeCell ref="B20:B23"/>
-    <mergeCell ref="B16:B19"/>
-    <mergeCell ref="B12:B15"/>
-    <mergeCell ref="B8:B11"/>
-    <mergeCell ref="B4:B7"/>
-    <mergeCell ref="C32:C35"/>
-    <mergeCell ref="B32:B35"/>
-    <mergeCell ref="B28:B31"/>
-    <mergeCell ref="C4:C7"/>
-    <mergeCell ref="C8:C11"/>
-    <mergeCell ref="C12:C15"/>
-    <mergeCell ref="C16:C19"/>
-    <mergeCell ref="C20:C23"/>
-    <mergeCell ref="C24:C27"/>
-    <mergeCell ref="C28:C31"/>
+    <mergeCell ref="A76:A79"/>
+    <mergeCell ref="B76:B79"/>
+    <mergeCell ref="C76:C79"/>
+    <mergeCell ref="D76:D79"/>
+    <mergeCell ref="E76:E79"/>
+    <mergeCell ref="I76:I79"/>
+    <mergeCell ref="J76:J79"/>
+    <mergeCell ref="K76:K79"/>
+    <mergeCell ref="J80:J83"/>
+    <mergeCell ref="K80:K83"/>
+    <mergeCell ref="A80:A83"/>
+    <mergeCell ref="B80:B83"/>
+    <mergeCell ref="C80:C83"/>
+    <mergeCell ref="D80:D83"/>
+    <mergeCell ref="E80:E83"/>
+    <mergeCell ref="I80:I83"/>
+    <mergeCell ref="B36:B39"/>
+    <mergeCell ref="C36:C39"/>
+    <mergeCell ref="D36:D39"/>
+    <mergeCell ref="E36:E39"/>
+    <mergeCell ref="J44:J47"/>
+    <mergeCell ref="K44:K47"/>
+    <mergeCell ref="I48:I51"/>
+    <mergeCell ref="J48:J51"/>
+    <mergeCell ref="K48:K51"/>
+    <mergeCell ref="B48:B51"/>
+    <mergeCell ref="C48:C51"/>
+    <mergeCell ref="D48:D51"/>
+    <mergeCell ref="E48:E51"/>
+    <mergeCell ref="K40:K43"/>
+    <mergeCell ref="I40:I43"/>
+    <mergeCell ref="B40:B43"/>
+    <mergeCell ref="J36:J39"/>
+    <mergeCell ref="C40:C43"/>
+    <mergeCell ref="D40:D43"/>
+    <mergeCell ref="E40:E43"/>
   </mergeCells>
-  <conditionalFormatting sqref="I20 I16 I24 I28 I32 I36 I40 I44 I48 I52 I56 I60 I64 I68 I72 I76 I80">
-    <cfRule type="cellIs" dxfId="11" priority="105" operator="equal">
+  <conditionalFormatting sqref="I28 I32 I36 I40 I44 I48 I52 I56 I60 I64 I68 I72 I76 I80">
+    <cfRule type="cellIs" dxfId="15" priority="109" operator="equal">
       <formula>"TO DO"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I20 I16 I24 I28 I32 I36 I40 I44 I48 I52 I56 I60 I64 I68 I72 I76 I80">
-    <cfRule type="cellIs" dxfId="10" priority="106" operator="equal">
+  <conditionalFormatting sqref="I28 I32 I36 I40 I44 I48 I52 I56 I60 I64 I68 I72 I76 I80">
+    <cfRule type="cellIs" dxfId="14" priority="110" operator="equal">
       <formula>"IN PROGRESS"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I20 I16 I24 I28 I32 I36 I40 I44 I48 I52 I56 I60 I64 I68 I72 I76 I80">
-    <cfRule type="cellIs" dxfId="9" priority="107" operator="equal">
+  <conditionalFormatting sqref="I28 I32 I36 I40 I44 I48 I52 I56 I60 I64 I68 I72 I76 I80">
+    <cfRule type="cellIs" dxfId="13" priority="111" operator="equal">
       <formula>"REVIEWED"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I20 I16 I24 I28 I32 I36 I40 I44 I48 I52 I56 I60 I64 I68 I72 I76 I80">
-    <cfRule type="cellIs" dxfId="8" priority="108" operator="equal">
+  <conditionalFormatting sqref="I28 I32 I36 I40 I44 I48 I52 I56 I60 I64 I68 I72 I76 I80">
+    <cfRule type="cellIs" dxfId="12" priority="112" operator="equal">
       <formula>"IN REVIEW"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I4 I8 I12">
+    <cfRule type="cellIs" dxfId="11" priority="5" operator="equal">
+      <formula>"TO DO"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I4 I8 I12">
+    <cfRule type="cellIs" dxfId="10" priority="6" operator="equal">
+      <formula>"IN PROGRESS"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I4 I8 I12">
+    <cfRule type="cellIs" dxfId="9" priority="7" operator="equal">
+      <formula>"REVIEWED"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I4 I8 I12">
+    <cfRule type="cellIs" dxfId="8" priority="8" operator="equal">
+      <formula>"IN REVIEW"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I16 I20 I24">
     <cfRule type="cellIs" dxfId="7" priority="1" operator="equal">
       <formula>"TO DO"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I4 I8 I12">
+  <conditionalFormatting sqref="I16 I20 I24">
     <cfRule type="cellIs" dxfId="5" priority="2" operator="equal">
       <formula>"IN PROGRESS"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I4 I8 I12">
+  <conditionalFormatting sqref="I16 I20 I24">
     <cfRule type="cellIs" dxfId="3" priority="3" operator="equal">
       <formula>"REVIEWED"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I4 I8 I12">
+  <conditionalFormatting sqref="I16 I20 I24">
     <cfRule type="cellIs" dxfId="1" priority="4" operator="equal">
       <formula>"IN REVIEW"</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" sqref="I72 I76 I28 I40 I32 I20 I16 I24 I36 I48 I52 I44 I56 I60 I80 I64 I68 I4 I8 I12">
+    <dataValidation type="list" allowBlank="1" sqref="I72 I76 I28 I40 I32 I4 I8 I12 I36 I48 I52 I44 I56 I60 I80 I64 I68 I24 I16 I20">
       <formula1>"TO DO,In Progress,In Review,Reviewed"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" sqref="K76 K36 K40 K32 K28 K16 K20 K24 K48 K44 K52 K60 K56 K64 K68 K72 K80 K4 K12 K8">
+    <dataValidation type="list" allowBlank="1" sqref="K76 K36 K40 K32 K28 K4 K12 K8 K48 K44 K52 K60 K56 K64 K68 K72 K80 K20 K24 K16">
       <formula1>"Smoke,Regresión"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
Agrego casos de uso referentes a la gestion de usuarios en la web
</commit_message>
<xml_diff>
--- a/Testing 2024/template_caso_prueba-ISPC2024-sprint-1.xlsx
+++ b/Testing 2024/template_caso_prueba-ISPC2024-sprint-1.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="269" uniqueCount="130">
   <si>
     <t>Id</t>
   </si>
@@ -278,12 +278,150 @@
   <si>
     <t>El usuario debe estar situado en la home page</t>
   </si>
+  <si>
+    <t>Gestion de Usuarios</t>
+  </si>
+  <si>
+    <t>Click al botón de "Iniciar sesion"</t>
+  </si>
+  <si>
+    <t>El usuario hace click al botón de "Iniciar sesion"</t>
+  </si>
+  <si>
+    <t>Hacer click en "Iniciar sesion" en la navbar de la home page</t>
+  </si>
+  <si>
+    <t>Deberá mostrarse en pantalla un formulario de Inicio de sesion</t>
+  </si>
+  <si>
+    <t>Click al botón de "Crear cuenta"</t>
+  </si>
+  <si>
+    <t>El usuario hace click al botón de "Crear cuenta"</t>
+  </si>
+  <si>
+    <t>Hacer click en "Crear cuenta"  en la navbar de la home page</t>
+  </si>
+  <si>
+    <t>Deberá mostrarse en pantalla un formulario de registro</t>
+  </si>
+  <si>
+    <t>Registro exitoso de un usuario nuevo</t>
+  </si>
+  <si>
+    <t>Un nuevo usuario puede  registrarse con un email y una contraseña y acceder a la home page</t>
+  </si>
+  <si>
+    <t>Ser un usuario que no se haya registrado previamente en el sitio</t>
+  </si>
+  <si>
+    <t>El usuario ingresa sus credenciales (nombre, apellido, correo y contraseña)</t>
+  </si>
+  <si>
+    <t>Presiona el botón "crear cuenta"</t>
+  </si>
+  <si>
+    <t>El usuario se registra e ingresa a su perfil</t>
+  </si>
+  <si>
+    <t>4.</t>
+  </si>
+  <si>
+    <t>Login exitoso de un email y contraseña existentes</t>
+  </si>
+  <si>
+    <t>El usuario, previamente registrado, puede loguearse con su email y su contraseña y acceder a la home page</t>
+  </si>
+  <si>
+    <t>Ser un usuario registrado en el sitio con un email y contraseña existente</t>
+  </si>
+  <si>
+    <t>El usuario ingresa sus credenciales (correo y contraseña)</t>
+  </si>
+  <si>
+    <t>Presiona el botón "ingresar a mi cuenta"</t>
+  </si>
+  <si>
+    <t>El usuario se loguea e ingresa a su perfil</t>
+  </si>
+  <si>
+    <t>Login sin éxito: email y contraseña inexistentes</t>
+  </si>
+  <si>
+    <t>Un nuevo usuario intenta loguearse sin haberse registrado anteriormente</t>
+  </si>
+  <si>
+    <t>No tiene email ni contraseña registrados en el sitio</t>
+  </si>
+  <si>
+    <t>El usuario ingresa un correo y una contraseña</t>
+  </si>
+  <si>
+    <t>Se visualiza un mensaje que le indica que las credenciales no son válidas</t>
+  </si>
+  <si>
+    <t>Login sin éxito: email y/o contraseña incorrecta</t>
+  </si>
+  <si>
+    <t>El usuario previamente registrado intenta loguearse con un email o contraseña diferente las utilizadas al momento de haberse registrado</t>
+  </si>
+  <si>
+    <t>El usuario ingresa un correo o una contraseña incorrecta</t>
+  </si>
+  <si>
+    <t>Login sin éxito: email que no cumple con el formato correcto</t>
+  </si>
+  <si>
+    <t>Ingresar en el campo email un email con formato incorrecto, por ejemplo sin el @</t>
+  </si>
+  <si>
+    <t>Se visualiza un mensaje que dice que el email ingresado no cumple con el formato requerido</t>
+  </si>
+  <si>
+    <t>Login sin éxito: contraseña que no cumple con el formato correcto</t>
+  </si>
+  <si>
+    <t>Un nuevo usuario intenta registrarse con un email correcto y una contraseña incorrecta (la contraseña debe tener minimo 6 caracteres)</t>
+  </si>
+  <si>
+    <t>Ingresar en el campo email un email con formato correcto</t>
+  </si>
+  <si>
+    <t>Se visualiza el email ingresado</t>
+  </si>
+  <si>
+    <t>Ingresar en el campo contraseña una contraseña con menos caracteres de los requeridos</t>
+  </si>
+  <si>
+    <t>Cada caracter ingresado se visualiza como un punto o asterisco.</t>
+  </si>
+  <si>
+    <t>Se visualiza un mensaje diciendo que la contraseña no cumple con el formato requerido</t>
+  </si>
+  <si>
+    <t>Usuario registrado quiere registrarse nuevamente con el mismo email</t>
+  </si>
+  <si>
+    <t>Un usuario previamente registrado quiere registrarse nuevamente utilizando el mismo email</t>
+  </si>
+  <si>
+    <t>Ingresar el mismo email utilizado previamente al momento de registrarse</t>
+  </si>
+  <si>
+    <t>Ingresar la contraseña utilizada al momento de registrarse</t>
+  </si>
+  <si>
+    <t>Se visualiza un mensaje que dice "el email ingresado ya se encuentra registrado"</t>
+  </si>
+  <si>
+    <t>Un nuevo usuario intenta registrarse con un email que no cumplen con el formato correcto</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="13">
+  <fonts count="12">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -352,13 +490,8 @@
       <sz val="10"/>
       <name val="ArialMT"/>
     </font>
-    <font>
-      <sz val="10"/>
-      <color theme="8" tint="-0.249977111117893"/>
-      <name val="ArialMT"/>
-    </font>
   </fonts>
-  <fills count="12">
+  <fills count="13">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -422,6 +555,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor rgb="FFFFFFCC"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
         <bgColor rgb="FFFFFFCC"/>
       </patternFill>
     </fill>
@@ -696,7 +835,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="74">
+  <cellXfs count="76">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -791,9 +930,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -812,20 +948,6 @@
     <xf numFmtId="0" fontId="10" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="10" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -835,24 +957,26 @@
     <xf numFmtId="0" fontId="1" fillId="10" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="11" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="11" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="11" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -868,20 +992,41 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="11" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="11" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="11" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="12" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="12" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="12" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="16">
+  <dxfs count="20">
     <dxf>
       <fill>
         <patternFill patternType="solid">
@@ -935,6 +1080,38 @@
         <patternFill patternType="solid">
           <fgColor rgb="FFA2C4C9"/>
           <bgColor rgb="FFA2C4C9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFA2C4C9"/>
+          <bgColor rgb="FFA2C4C9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFCE5CD"/>
+          <bgColor rgb="FFFCE5CD"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF93C47D"/>
+          <bgColor rgb="FF93C47D"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFF2CC"/>
+          <bgColor rgb="FFFFF2CC"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1359,8 +1536,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AA935"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="60" workbookViewId="0">
-      <selection activeCell="G30" sqref="G30"/>
+    <sheetView tabSelected="1" topLeftCell="A50" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="60" workbookViewId="0">
+      <selection activeCell="D56" sqref="D56:D59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5703125" defaultRowHeight="12.75"/>
@@ -1409,33 +1586,33 @@
       <c r="AA1" s="2"/>
     </row>
     <row r="2" spans="1:27" s="31" customFormat="1" ht="15.75" customHeight="1">
-      <c r="A2" s="62" t="s">
+      <c r="A2" s="66" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="60" t="s">
+      <c r="B2" s="56" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="62" t="s">
+      <c r="C2" s="66" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="60" t="s">
+      <c r="D2" s="56" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="60" t="s">
+      <c r="E2" s="56" t="s">
         <v>4</v>
       </c>
-      <c r="F2" s="66" t="s">
+      <c r="F2" s="61" t="s">
         <v>5</v>
       </c>
-      <c r="G2" s="67"/>
-      <c r="H2" s="68"/>
-      <c r="I2" s="69" t="s">
+      <c r="G2" s="62"/>
+      <c r="H2" s="63"/>
+      <c r="I2" s="64" t="s">
         <v>6</v>
       </c>
-      <c r="J2" s="60" t="s">
+      <c r="J2" s="56" t="s">
         <v>7</v>
       </c>
-      <c r="K2" s="60" t="s">
+      <c r="K2" s="56" t="s">
         <v>27</v>
       </c>
       <c r="L2" s="32"/>
@@ -1456,11 +1633,11 @@
       <c r="AA2" s="33"/>
     </row>
     <row r="3" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A3" s="63"/>
-      <c r="B3" s="61"/>
-      <c r="C3" s="63"/>
-      <c r="D3" s="61"/>
-      <c r="E3" s="61"/>
+      <c r="A3" s="67"/>
+      <c r="B3" s="57"/>
+      <c r="C3" s="67"/>
+      <c r="D3" s="57"/>
+      <c r="E3" s="57"/>
       <c r="F3" s="34" t="s">
         <v>8</v>
       </c>
@@ -1470,9 +1647,9 @@
       <c r="H3" s="42" t="s">
         <v>10</v>
       </c>
-      <c r="I3" s="70"/>
-      <c r="J3" s="61"/>
-      <c r="K3" s="61"/>
+      <c r="I3" s="65"/>
+      <c r="J3" s="57"/>
+      <c r="K3" s="57"/>
       <c r="L3" s="3"/>
       <c r="M3" s="2"/>
       <c r="N3" s="2"/>
@@ -1491,37 +1668,37 @@
       <c r="AA3" s="2"/>
     </row>
     <row r="4" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A4" s="57" t="s">
+      <c r="A4" s="50" t="s">
         <v>29</v>
       </c>
-      <c r="B4" s="45" t="s">
+      <c r="B4" s="44" t="s">
         <v>49</v>
       </c>
-      <c r="C4" s="45" t="s">
+      <c r="C4" s="44" t="s">
         <v>50</v>
       </c>
-      <c r="D4" s="45" t="s">
+      <c r="D4" s="44" t="s">
         <v>51</v>
       </c>
-      <c r="E4" s="45" t="s">
+      <c r="E4" s="44" t="s">
         <v>52</v>
       </c>
-      <c r="F4" s="45" t="s">
+      <c r="F4" s="44" t="s">
         <v>53</v>
       </c>
-      <c r="G4" s="45" t="s">
+      <c r="G4" s="44" t="s">
         <v>54</v>
       </c>
-      <c r="H4" s="64" t="s">
+      <c r="H4" s="68" t="s">
         <v>55</v>
       </c>
-      <c r="I4" s="54" t="s">
+      <c r="I4" s="58" t="s">
         <v>26</v>
       </c>
-      <c r="J4" s="51" t="s">
+      <c r="J4" s="70" t="s">
         <v>56</v>
       </c>
-      <c r="K4" s="54" t="s">
+      <c r="K4" s="58" t="s">
         <v>28</v>
       </c>
       <c r="L4" s="3"/>
@@ -1542,17 +1719,17 @@
       <c r="AA4" s="2"/>
     </row>
     <row r="5" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A5" s="58"/>
-      <c r="B5" s="46"/>
-      <c r="C5" s="46"/>
-      <c r="D5" s="46"/>
-      <c r="E5" s="46"/>
-      <c r="F5" s="47"/>
-      <c r="G5" s="47"/>
-      <c r="H5" s="65"/>
-      <c r="I5" s="55"/>
-      <c r="J5" s="52"/>
-      <c r="K5" s="55"/>
+      <c r="A5" s="51"/>
+      <c r="B5" s="45"/>
+      <c r="C5" s="45"/>
+      <c r="D5" s="45"/>
+      <c r="E5" s="45"/>
+      <c r="F5" s="46"/>
+      <c r="G5" s="46"/>
+      <c r="H5" s="69"/>
+      <c r="I5" s="59"/>
+      <c r="J5" s="71"/>
+      <c r="K5" s="59"/>
       <c r="L5" s="3"/>
       <c r="M5" s="2"/>
       <c r="N5" s="2"/>
@@ -1571,17 +1748,17 @@
       <c r="AA5" s="2"/>
     </row>
     <row r="6" spans="1:27" s="29" customFormat="1" ht="15.75" customHeight="1">
-      <c r="A6" s="58"/>
-      <c r="B6" s="46"/>
-      <c r="C6" s="46"/>
-      <c r="D6" s="46"/>
-      <c r="E6" s="46"/>
+      <c r="A6" s="51"/>
+      <c r="B6" s="45"/>
+      <c r="C6" s="45"/>
+      <c r="D6" s="45"/>
+      <c r="E6" s="45"/>
       <c r="F6" s="30"/>
       <c r="G6" s="35"/>
       <c r="H6" s="35"/>
-      <c r="I6" s="55"/>
-      <c r="J6" s="52"/>
-      <c r="K6" s="55"/>
+      <c r="I6" s="59"/>
+      <c r="J6" s="71"/>
+      <c r="K6" s="59"/>
       <c r="L6" s="27"/>
       <c r="M6" s="28"/>
       <c r="N6" s="28"/>
@@ -1600,17 +1777,17 @@
       <c r="AA6" s="28"/>
     </row>
     <row r="7" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A7" s="59"/>
-      <c r="B7" s="47"/>
-      <c r="C7" s="47"/>
-      <c r="D7" s="47"/>
-      <c r="E7" s="47"/>
+      <c r="A7" s="52"/>
+      <c r="B7" s="46"/>
+      <c r="C7" s="46"/>
+      <c r="D7" s="46"/>
+      <c r="E7" s="46"/>
       <c r="F7" s="30"/>
       <c r="G7" s="35"/>
       <c r="H7" s="35"/>
-      <c r="I7" s="56"/>
-      <c r="J7" s="53"/>
-      <c r="K7" s="56"/>
+      <c r="I7" s="60"/>
+      <c r="J7" s="72"/>
+      <c r="K7" s="60"/>
       <c r="L7" s="3"/>
       <c r="M7" s="2"/>
       <c r="N7" s="2"/>
@@ -1629,37 +1806,37 @@
       <c r="AA7" s="2"/>
     </row>
     <row r="8" spans="1:27">
-      <c r="A8" s="57" t="s">
+      <c r="A8" s="50" t="s">
         <v>30</v>
       </c>
-      <c r="B8" s="45" t="s">
+      <c r="B8" s="44" t="s">
         <v>49</v>
       </c>
-      <c r="C8" s="45" t="s">
+      <c r="C8" s="44" t="s">
         <v>57</v>
       </c>
-      <c r="D8" s="45" t="s">
+      <c r="D8" s="44" t="s">
         <v>58</v>
       </c>
-      <c r="E8" s="45" t="s">
+      <c r="E8" s="44" t="s">
         <v>59</v>
       </c>
-      <c r="F8" s="45" t="s">
+      <c r="F8" s="44" t="s">
         <v>53</v>
       </c>
-      <c r="G8" s="45" t="s">
+      <c r="G8" s="44" t="s">
         <v>54</v>
       </c>
-      <c r="H8" s="64" t="s">
+      <c r="H8" s="68" t="s">
         <v>55</v>
       </c>
-      <c r="I8" s="54" t="s">
+      <c r="I8" s="58" t="s">
         <v>26</v>
       </c>
-      <c r="J8" s="51" t="s">
+      <c r="J8" s="70" t="s">
         <v>56</v>
       </c>
-      <c r="K8" s="54" t="s">
+      <c r="K8" s="58" t="s">
         <v>28</v>
       </c>
       <c r="L8" s="3"/>
@@ -1680,17 +1857,17 @@
       <c r="AA8" s="2"/>
     </row>
     <row r="9" spans="1:27">
-      <c r="A9" s="58"/>
-      <c r="B9" s="46"/>
-      <c r="C9" s="46"/>
-      <c r="D9" s="46"/>
-      <c r="E9" s="46"/>
-      <c r="F9" s="47"/>
-      <c r="G9" s="47"/>
-      <c r="H9" s="65"/>
-      <c r="I9" s="55"/>
-      <c r="J9" s="52"/>
-      <c r="K9" s="55"/>
+      <c r="A9" s="51"/>
+      <c r="B9" s="45"/>
+      <c r="C9" s="45"/>
+      <c r="D9" s="45"/>
+      <c r="E9" s="45"/>
+      <c r="F9" s="46"/>
+      <c r="G9" s="46"/>
+      <c r="H9" s="69"/>
+      <c r="I9" s="59"/>
+      <c r="J9" s="71"/>
+      <c r="K9" s="59"/>
       <c r="L9" s="3"/>
       <c r="M9" s="2"/>
       <c r="N9" s="2"/>
@@ -1709,17 +1886,17 @@
       <c r="AA9" s="2"/>
     </row>
     <row r="10" spans="1:27" s="29" customFormat="1" ht="15.75" customHeight="1">
-      <c r="A10" s="58"/>
-      <c r="B10" s="46"/>
-      <c r="C10" s="46"/>
-      <c r="D10" s="46"/>
-      <c r="E10" s="46"/>
+      <c r="A10" s="51"/>
+      <c r="B10" s="45"/>
+      <c r="C10" s="45"/>
+      <c r="D10" s="45"/>
+      <c r="E10" s="45"/>
       <c r="F10" s="30"/>
       <c r="G10" s="35"/>
       <c r="H10" s="35"/>
-      <c r="I10" s="55"/>
-      <c r="J10" s="52"/>
-      <c r="K10" s="55"/>
+      <c r="I10" s="59"/>
+      <c r="J10" s="71"/>
+      <c r="K10" s="59"/>
       <c r="L10" s="27"/>
       <c r="M10" s="28"/>
       <c r="N10" s="28"/>
@@ -1738,17 +1915,17 @@
       <c r="AA10" s="28"/>
     </row>
     <row r="11" spans="1:27">
-      <c r="A11" s="59"/>
-      <c r="B11" s="47"/>
-      <c r="C11" s="47"/>
-      <c r="D11" s="47"/>
-      <c r="E11" s="47"/>
+      <c r="A11" s="52"/>
+      <c r="B11" s="46"/>
+      <c r="C11" s="46"/>
+      <c r="D11" s="46"/>
+      <c r="E11" s="46"/>
       <c r="F11" s="30"/>
       <c r="G11" s="35"/>
       <c r="H11" s="35"/>
-      <c r="I11" s="56"/>
-      <c r="J11" s="53"/>
-      <c r="K11" s="56"/>
+      <c r="I11" s="60"/>
+      <c r="J11" s="72"/>
+      <c r="K11" s="60"/>
       <c r="L11" s="3"/>
       <c r="M11" s="2"/>
       <c r="N11" s="2"/>
@@ -1767,37 +1944,37 @@
       <c r="AA11" s="2"/>
     </row>
     <row r="12" spans="1:27">
-      <c r="A12" s="57" t="s">
+      <c r="A12" s="50" t="s">
         <v>31</v>
       </c>
-      <c r="B12" s="45" t="s">
+      <c r="B12" s="44" t="s">
         <v>49</v>
       </c>
-      <c r="C12" s="45" t="s">
+      <c r="C12" s="44" t="s">
         <v>60</v>
       </c>
-      <c r="D12" s="45" t="s">
+      <c r="D12" s="44" t="s">
         <v>61</v>
       </c>
-      <c r="E12" s="45" t="s">
+      <c r="E12" s="44" t="s">
         <v>62</v>
       </c>
-      <c r="F12" s="45" t="s">
+      <c r="F12" s="44" t="s">
         <v>53</v>
       </c>
-      <c r="G12" s="45" t="s">
+      <c r="G12" s="44" t="s">
         <v>54</v>
       </c>
-      <c r="H12" s="64" t="s">
+      <c r="H12" s="68" t="s">
         <v>55</v>
       </c>
-      <c r="I12" s="54" t="s">
+      <c r="I12" s="58" t="s">
         <v>26</v>
       </c>
-      <c r="J12" s="51" t="s">
+      <c r="J12" s="70" t="s">
         <v>56</v>
       </c>
-      <c r="K12" s="54" t="s">
+      <c r="K12" s="58" t="s">
         <v>28</v>
       </c>
       <c r="L12" s="2"/>
@@ -1818,17 +1995,17 @@
       <c r="AA12" s="2"/>
     </row>
     <row r="13" spans="1:27">
-      <c r="A13" s="58"/>
-      <c r="B13" s="46"/>
-      <c r="C13" s="46"/>
-      <c r="D13" s="46"/>
-      <c r="E13" s="46"/>
-      <c r="F13" s="47"/>
-      <c r="G13" s="47"/>
-      <c r="H13" s="65"/>
-      <c r="I13" s="55"/>
-      <c r="J13" s="52"/>
-      <c r="K13" s="55"/>
+      <c r="A13" s="51"/>
+      <c r="B13" s="45"/>
+      <c r="C13" s="45"/>
+      <c r="D13" s="45"/>
+      <c r="E13" s="45"/>
+      <c r="F13" s="46"/>
+      <c r="G13" s="46"/>
+      <c r="H13" s="69"/>
+      <c r="I13" s="59"/>
+      <c r="J13" s="71"/>
+      <c r="K13" s="59"/>
       <c r="L13" s="2"/>
       <c r="M13" s="2"/>
       <c r="N13" s="2"/>
@@ -1847,17 +2024,17 @@
       <c r="AA13" s="2"/>
     </row>
     <row r="14" spans="1:27" s="29" customFormat="1">
-      <c r="A14" s="58"/>
-      <c r="B14" s="46"/>
-      <c r="C14" s="46"/>
-      <c r="D14" s="46"/>
-      <c r="E14" s="46"/>
+      <c r="A14" s="51"/>
+      <c r="B14" s="45"/>
+      <c r="C14" s="45"/>
+      <c r="D14" s="45"/>
+      <c r="E14" s="45"/>
       <c r="F14" s="30"/>
       <c r="G14" s="35"/>
       <c r="H14" s="35"/>
-      <c r="I14" s="55"/>
-      <c r="J14" s="52"/>
-      <c r="K14" s="55"/>
+      <c r="I14" s="59"/>
+      <c r="J14" s="71"/>
+      <c r="K14" s="59"/>
       <c r="L14" s="28"/>
       <c r="M14" s="28"/>
       <c r="N14" s="28"/>
@@ -1876,17 +2053,17 @@
       <c r="AA14" s="28"/>
     </row>
     <row r="15" spans="1:27">
-      <c r="A15" s="59"/>
-      <c r="B15" s="47"/>
-      <c r="C15" s="47"/>
-      <c r="D15" s="47"/>
-      <c r="E15" s="47"/>
+      <c r="A15" s="52"/>
+      <c r="B15" s="46"/>
+      <c r="C15" s="46"/>
+      <c r="D15" s="46"/>
+      <c r="E15" s="46"/>
       <c r="F15" s="30"/>
       <c r="G15" s="35"/>
       <c r="H15" s="35"/>
-      <c r="I15" s="56"/>
-      <c r="J15" s="53"/>
-      <c r="K15" s="56"/>
+      <c r="I15" s="60"/>
+      <c r="J15" s="72"/>
+      <c r="K15" s="60"/>
       <c r="L15" s="2"/>
       <c r="M15" s="2"/>
       <c r="N15" s="2"/>
@@ -1905,19 +2082,19 @@
       <c r="AA15" s="2"/>
     </row>
     <row r="16" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A16" s="71" t="s">
+      <c r="A16" s="53" t="s">
         <v>32</v>
       </c>
-      <c r="B16" s="45" t="s">
+      <c r="B16" s="44" t="s">
         <v>63</v>
       </c>
-      <c r="C16" s="45" t="s">
+      <c r="C16" s="44" t="s">
         <v>64</v>
       </c>
-      <c r="D16" s="45" t="s">
+      <c r="D16" s="44" t="s">
         <v>65</v>
       </c>
-      <c r="E16" s="45" t="s">
+      <c r="E16" s="44" t="s">
         <v>83</v>
       </c>
       <c r="F16" s="30" t="s">
@@ -1929,13 +2106,13 @@
       <c r="H16" s="35" t="s">
         <v>66</v>
       </c>
-      <c r="I16" s="54" t="s">
+      <c r="I16" s="58" t="s">
         <v>26</v>
       </c>
-      <c r="J16" s="51" t="s">
+      <c r="J16" s="70" t="s">
         <v>56</v>
       </c>
-      <c r="K16" s="54" t="s">
+      <c r="K16" s="58" t="s">
         <v>28</v>
       </c>
       <c r="L16" s="2"/>
@@ -1956,11 +2133,11 @@
       <c r="AA16" s="2"/>
     </row>
     <row r="17" spans="1:27" ht="16.5" customHeight="1">
-      <c r="A17" s="72"/>
-      <c r="B17" s="46"/>
-      <c r="C17" s="46"/>
-      <c r="D17" s="46"/>
-      <c r="E17" s="46"/>
+      <c r="A17" s="54"/>
+      <c r="B17" s="45"/>
+      <c r="C17" s="45"/>
+      <c r="D17" s="45"/>
+      <c r="E17" s="45"/>
       <c r="F17" s="30" t="s">
         <v>67</v>
       </c>
@@ -1970,9 +2147,9 @@
       <c r="H17" s="35" t="s">
         <v>69</v>
       </c>
-      <c r="I17" s="55"/>
-      <c r="J17" s="52"/>
-      <c r="K17" s="55"/>
+      <c r="I17" s="59"/>
+      <c r="J17" s="71"/>
+      <c r="K17" s="59"/>
       <c r="L17" s="2"/>
       <c r="M17" s="2"/>
       <c r="N17" s="2"/>
@@ -1991,11 +2168,11 @@
       <c r="AA17" s="2"/>
     </row>
     <row r="18" spans="1:27" s="29" customFormat="1" ht="25.5">
-      <c r="A18" s="72"/>
-      <c r="B18" s="46"/>
-      <c r="C18" s="46"/>
-      <c r="D18" s="46"/>
-      <c r="E18" s="46"/>
+      <c r="A18" s="54"/>
+      <c r="B18" s="45"/>
+      <c r="C18" s="45"/>
+      <c r="D18" s="45"/>
+      <c r="E18" s="45"/>
       <c r="F18" s="30" t="s">
         <v>70</v>
       </c>
@@ -2005,9 +2182,9 @@
       <c r="H18" s="35" t="s">
         <v>72</v>
       </c>
-      <c r="I18" s="55"/>
-      <c r="J18" s="52"/>
-      <c r="K18" s="55"/>
+      <c r="I18" s="59"/>
+      <c r="J18" s="71"/>
+      <c r="K18" s="59"/>
       <c r="L18" s="28"/>
       <c r="M18" s="28"/>
       <c r="N18" s="28"/>
@@ -2026,17 +2203,17 @@
       <c r="AA18" s="28"/>
     </row>
     <row r="19" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A19" s="73"/>
-      <c r="B19" s="47"/>
-      <c r="C19" s="47"/>
-      <c r="D19" s="47"/>
-      <c r="E19" s="47"/>
+      <c r="A19" s="55"/>
+      <c r="B19" s="46"/>
+      <c r="C19" s="46"/>
+      <c r="D19" s="46"/>
+      <c r="E19" s="46"/>
       <c r="F19" s="30"/>
       <c r="G19" s="35"/>
       <c r="H19" s="35"/>
-      <c r="I19" s="56"/>
-      <c r="J19" s="53"/>
-      <c r="K19" s="56"/>
+      <c r="I19" s="60"/>
+      <c r="J19" s="72"/>
+      <c r="K19" s="60"/>
       <c r="L19" s="2"/>
       <c r="M19" s="2"/>
       <c r="N19" s="2"/>
@@ -2055,19 +2232,19 @@
       <c r="AA19" s="2"/>
     </row>
     <row r="20" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A20" s="71" t="s">
+      <c r="A20" s="53" t="s">
         <v>33</v>
       </c>
-      <c r="B20" s="45" t="s">
+      <c r="B20" s="44" t="s">
         <v>63</v>
       </c>
-      <c r="C20" s="48" t="s">
+      <c r="C20" s="47" t="s">
         <v>73</v>
       </c>
-      <c r="D20" s="45" t="s">
+      <c r="D20" s="44" t="s">
         <v>74</v>
       </c>
-      <c r="E20" s="45" t="s">
+      <c r="E20" s="44" t="s">
         <v>75</v>
       </c>
       <c r="F20" s="30" t="s">
@@ -2079,13 +2256,13 @@
       <c r="H20" s="35" t="s">
         <v>76</v>
       </c>
-      <c r="I20" s="54" t="s">
+      <c r="I20" s="58" t="s">
         <v>26</v>
       </c>
-      <c r="J20" s="51" t="s">
+      <c r="J20" s="70" t="s">
         <v>56</v>
       </c>
-      <c r="K20" s="54" t="s">
+      <c r="K20" s="58" t="s">
         <v>28</v>
       </c>
       <c r="L20" s="2"/>
@@ -2106,11 +2283,11 @@
       <c r="AA20" s="2"/>
     </row>
     <row r="21" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A21" s="72"/>
-      <c r="B21" s="46"/>
-      <c r="C21" s="49"/>
-      <c r="D21" s="46"/>
-      <c r="E21" s="46"/>
+      <c r="A21" s="54"/>
+      <c r="B21" s="45"/>
+      <c r="C21" s="48"/>
+      <c r="D21" s="45"/>
+      <c r="E21" s="45"/>
       <c r="F21" s="30" t="s">
         <v>67</v>
       </c>
@@ -2118,9 +2295,9 @@
         <v>77</v>
       </c>
       <c r="H21" s="35"/>
-      <c r="I21" s="55"/>
-      <c r="J21" s="52"/>
-      <c r="K21" s="55"/>
+      <c r="I21" s="59"/>
+      <c r="J21" s="71"/>
+      <c r="K21" s="59"/>
       <c r="L21" s="2"/>
       <c r="M21" s="2"/>
       <c r="N21" s="2"/>
@@ -2139,11 +2316,11 @@
       <c r="AA21" s="2"/>
     </row>
     <row r="22" spans="1:27" s="29" customFormat="1" ht="15.75" customHeight="1">
-      <c r="A22" s="72"/>
-      <c r="B22" s="46"/>
-      <c r="C22" s="49"/>
-      <c r="D22" s="46"/>
-      <c r="E22" s="46"/>
+      <c r="A22" s="54"/>
+      <c r="B22" s="45"/>
+      <c r="C22" s="48"/>
+      <c r="D22" s="45"/>
+      <c r="E22" s="45"/>
       <c r="F22" s="30" t="s">
         <v>70</v>
       </c>
@@ -2153,9 +2330,9 @@
       <c r="H22" s="35" t="s">
         <v>79</v>
       </c>
-      <c r="I22" s="55"/>
-      <c r="J22" s="52"/>
-      <c r="K22" s="55"/>
+      <c r="I22" s="59"/>
+      <c r="J22" s="71"/>
+      <c r="K22" s="59"/>
       <c r="L22" s="28"/>
       <c r="M22" s="28"/>
       <c r="N22" s="28"/>
@@ -2174,17 +2351,17 @@
       <c r="AA22" s="28"/>
     </row>
     <row r="23" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A23" s="73"/>
-      <c r="B23" s="47"/>
-      <c r="C23" s="50"/>
-      <c r="D23" s="47"/>
-      <c r="E23" s="47"/>
+      <c r="A23" s="55"/>
+      <c r="B23" s="46"/>
+      <c r="C23" s="49"/>
+      <c r="D23" s="46"/>
+      <c r="E23" s="46"/>
       <c r="F23" s="30"/>
       <c r="G23" s="35"/>
       <c r="H23" s="35"/>
-      <c r="I23" s="56"/>
-      <c r="J23" s="53"/>
-      <c r="K23" s="56"/>
+      <c r="I23" s="60"/>
+      <c r="J23" s="72"/>
+      <c r="K23" s="60"/>
       <c r="L23" s="2"/>
       <c r="M23" s="2"/>
       <c r="N23" s="2"/>
@@ -2203,19 +2380,19 @@
       <c r="AA23" s="2"/>
     </row>
     <row r="24" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A24" s="71" t="s">
+      <c r="A24" s="53" t="s">
         <v>34</v>
       </c>
-      <c r="B24" s="45" t="s">
+      <c r="B24" s="44" t="s">
         <v>63</v>
       </c>
-      <c r="C24" s="48" t="s">
+      <c r="C24" s="47" t="s">
         <v>80</v>
       </c>
-      <c r="D24" s="45" t="s">
+      <c r="D24" s="44" t="s">
         <v>81</v>
       </c>
-      <c r="E24" s="45" t="s">
+      <c r="E24" s="44" t="s">
         <v>75</v>
       </c>
       <c r="F24" s="30" t="s">
@@ -2227,13 +2404,13 @@
       <c r="H24" s="35" t="s">
         <v>76</v>
       </c>
-      <c r="I24" s="54" t="s">
+      <c r="I24" s="58" t="s">
         <v>26</v>
       </c>
-      <c r="J24" s="51" t="s">
+      <c r="J24" s="70" t="s">
         <v>56</v>
       </c>
-      <c r="K24" s="54" t="s">
+      <c r="K24" s="58" t="s">
         <v>28</v>
       </c>
       <c r="L24" s="2"/>
@@ -2254,11 +2431,11 @@
       <c r="AA24" s="2"/>
     </row>
     <row r="25" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A25" s="72"/>
-      <c r="B25" s="46"/>
-      <c r="C25" s="49"/>
-      <c r="D25" s="46"/>
-      <c r="E25" s="46"/>
+      <c r="A25" s="54"/>
+      <c r="B25" s="45"/>
+      <c r="C25" s="48"/>
+      <c r="D25" s="45"/>
+      <c r="E25" s="45"/>
       <c r="F25" s="30" t="s">
         <v>67</v>
       </c>
@@ -2266,9 +2443,9 @@
         <v>77</v>
       </c>
       <c r="H25" s="35"/>
-      <c r="I25" s="55"/>
-      <c r="J25" s="52"/>
-      <c r="K25" s="55"/>
+      <c r="I25" s="59"/>
+      <c r="J25" s="71"/>
+      <c r="K25" s="59"/>
       <c r="L25" s="2"/>
       <c r="M25" s="2"/>
       <c r="N25" s="2"/>
@@ -2287,11 +2464,11 @@
       <c r="AA25" s="2"/>
     </row>
     <row r="26" spans="1:27" s="29" customFormat="1" ht="25.5">
-      <c r="A26" s="72"/>
-      <c r="B26" s="46"/>
-      <c r="C26" s="49"/>
-      <c r="D26" s="46"/>
-      <c r="E26" s="46"/>
+      <c r="A26" s="54"/>
+      <c r="B26" s="45"/>
+      <c r="C26" s="48"/>
+      <c r="D26" s="45"/>
+      <c r="E26" s="45"/>
       <c r="F26" s="30" t="s">
         <v>70</v>
       </c>
@@ -2301,9 +2478,9 @@
       <c r="H26" s="35" t="s">
         <v>82</v>
       </c>
-      <c r="I26" s="55"/>
-      <c r="J26" s="52"/>
-      <c r="K26" s="55"/>
+      <c r="I26" s="59"/>
+      <c r="J26" s="71"/>
+      <c r="K26" s="59"/>
       <c r="L26" s="28"/>
       <c r="M26" s="28"/>
       <c r="N26" s="28"/>
@@ -2321,18 +2498,18 @@
       <c r="Z26" s="28"/>
       <c r="AA26" s="28"/>
     </row>
-    <row r="27" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A27" s="73"/>
-      <c r="B27" s="47"/>
-      <c r="C27" s="50"/>
-      <c r="D27" s="47"/>
-      <c r="E27" s="47"/>
+    <row r="27" spans="1:27" ht="18.75" customHeight="1">
+      <c r="A27" s="55"/>
+      <c r="B27" s="46"/>
+      <c r="C27" s="49"/>
+      <c r="D27" s="46"/>
+      <c r="E27" s="46"/>
       <c r="F27" s="30"/>
       <c r="G27" s="35"/>
       <c r="H27" s="35"/>
-      <c r="I27" s="56"/>
-      <c r="J27" s="53"/>
-      <c r="K27" s="56"/>
+      <c r="I27" s="60"/>
+      <c r="J27" s="72"/>
+      <c r="K27" s="60"/>
       <c r="L27" s="2"/>
       <c r="M27" s="2"/>
       <c r="N27" s="2"/>
@@ -2351,21 +2528,37 @@
       <c r="AA27" s="2"/>
     </row>
     <row r="28" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A28" s="57" t="s">
+      <c r="A28" s="73" t="s">
         <v>35</v>
       </c>
-      <c r="B28" s="45"/>
-      <c r="C28" s="45"/>
-      <c r="D28" s="45"/>
-      <c r="E28" s="45"/>
-      <c r="F28" s="30"/>
-      <c r="G28" s="44"/>
-      <c r="H28" s="44"/>
-      <c r="I28" s="54" t="s">
+      <c r="B28" s="44" t="s">
+        <v>84</v>
+      </c>
+      <c r="C28" s="44" t="s">
+        <v>85</v>
+      </c>
+      <c r="D28" s="44" t="s">
+        <v>86</v>
+      </c>
+      <c r="E28" s="44" t="s">
+        <v>83</v>
+      </c>
+      <c r="F28" s="30" t="s">
+        <v>53</v>
+      </c>
+      <c r="G28" s="35" t="s">
+        <v>87</v>
+      </c>
+      <c r="H28" s="35" t="s">
+        <v>88</v>
+      </c>
+      <c r="I28" s="58" t="s">
         <v>26</v>
       </c>
-      <c r="J28" s="51"/>
-      <c r="K28" s="54" t="s">
+      <c r="J28" s="70" t="s">
+        <v>56</v>
+      </c>
+      <c r="K28" s="58" t="s">
         <v>28</v>
       </c>
       <c r="L28" s="2"/>
@@ -2386,17 +2579,19 @@
       <c r="AA28" s="2"/>
     </row>
     <row r="29" spans="1:27">
-      <c r="A29" s="58"/>
-      <c r="B29" s="46"/>
-      <c r="C29" s="46"/>
-      <c r="D29" s="46"/>
-      <c r="E29" s="46"/>
-      <c r="F29" s="30"/>
-      <c r="G29" s="44"/>
-      <c r="H29" s="44"/>
-      <c r="I29" s="55"/>
-      <c r="J29" s="52"/>
-      <c r="K29" s="55"/>
+      <c r="A29" s="74"/>
+      <c r="B29" s="45"/>
+      <c r="C29" s="45"/>
+      <c r="D29" s="45"/>
+      <c r="E29" s="45"/>
+      <c r="F29" s="30" t="s">
+        <v>67</v>
+      </c>
+      <c r="G29" s="35"/>
+      <c r="H29" s="35"/>
+      <c r="I29" s="59"/>
+      <c r="J29" s="71"/>
+      <c r="K29" s="59"/>
       <c r="L29" s="2"/>
       <c r="M29" s="2"/>
       <c r="N29" s="2"/>
@@ -2415,17 +2610,17 @@
       <c r="AA29" s="2"/>
     </row>
     <row r="30" spans="1:27" s="29" customFormat="1" ht="15.75" customHeight="1">
-      <c r="A30" s="58"/>
-      <c r="B30" s="46"/>
-      <c r="C30" s="46"/>
-      <c r="D30" s="46"/>
-      <c r="E30" s="46"/>
+      <c r="A30" s="74"/>
+      <c r="B30" s="45"/>
+      <c r="C30" s="45"/>
+      <c r="D30" s="45"/>
+      <c r="E30" s="45"/>
       <c r="F30" s="30"/>
-      <c r="G30" s="44"/>
-      <c r="H30" s="44"/>
-      <c r="I30" s="55"/>
-      <c r="J30" s="52"/>
-      <c r="K30" s="55"/>
+      <c r="G30" s="35"/>
+      <c r="H30" s="35"/>
+      <c r="I30" s="59"/>
+      <c r="J30" s="71"/>
+      <c r="K30" s="59"/>
       <c r="L30" s="28"/>
       <c r="M30" s="28"/>
       <c r="N30" s="28"/>
@@ -2444,17 +2639,17 @@
       <c r="AA30" s="28"/>
     </row>
     <row r="31" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A31" s="59"/>
-      <c r="B31" s="47"/>
-      <c r="C31" s="47"/>
-      <c r="D31" s="47"/>
-      <c r="E31" s="47"/>
+      <c r="A31" s="75"/>
+      <c r="B31" s="46"/>
+      <c r="C31" s="46"/>
+      <c r="D31" s="46"/>
+      <c r="E31" s="46"/>
       <c r="F31" s="30"/>
-      <c r="G31" s="44"/>
-      <c r="H31" s="44"/>
-      <c r="I31" s="56"/>
-      <c r="J31" s="53"/>
-      <c r="K31" s="56"/>
+      <c r="G31" s="35"/>
+      <c r="H31" s="35"/>
+      <c r="I31" s="60"/>
+      <c r="J31" s="72"/>
+      <c r="K31" s="60"/>
       <c r="L31" s="2"/>
       <c r="M31" s="2"/>
       <c r="N31" s="2"/>
@@ -2473,21 +2668,37 @@
       <c r="AA31" s="2"/>
     </row>
     <row r="32" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A32" s="57" t="s">
+      <c r="A32" s="73" t="s">
         <v>36</v>
       </c>
-      <c r="B32" s="45"/>
-      <c r="C32" s="45"/>
-      <c r="D32" s="45"/>
-      <c r="E32" s="45"/>
-      <c r="F32" s="30"/>
-      <c r="G32" s="35"/>
-      <c r="H32" s="35"/>
-      <c r="I32" s="54" t="s">
+      <c r="B32" s="44" t="s">
+        <v>84</v>
+      </c>
+      <c r="C32" s="44" t="s">
+        <v>89</v>
+      </c>
+      <c r="D32" s="44" t="s">
+        <v>90</v>
+      </c>
+      <c r="E32" s="44" t="s">
+        <v>83</v>
+      </c>
+      <c r="F32" s="30" t="s">
+        <v>53</v>
+      </c>
+      <c r="G32" s="35" t="s">
+        <v>91</v>
+      </c>
+      <c r="H32" s="35" t="s">
+        <v>92</v>
+      </c>
+      <c r="I32" s="58" t="s">
         <v>26</v>
       </c>
-      <c r="J32" s="51"/>
-      <c r="K32" s="54" t="s">
+      <c r="J32" s="70" t="s">
+        <v>56</v>
+      </c>
+      <c r="K32" s="58" t="s">
         <v>28</v>
       </c>
       <c r="L32" s="2"/>
@@ -2508,17 +2719,17 @@
       <c r="AA32" s="2"/>
     </row>
     <row r="33" spans="1:27">
-      <c r="A33" s="58"/>
-      <c r="B33" s="46"/>
-      <c r="C33" s="46"/>
-      <c r="D33" s="46"/>
-      <c r="E33" s="46"/>
+      <c r="A33" s="74"/>
+      <c r="B33" s="45"/>
+      <c r="C33" s="45"/>
+      <c r="D33" s="45"/>
+      <c r="E33" s="45"/>
       <c r="F33" s="30"/>
-      <c r="G33" s="35"/>
-      <c r="H33" s="35"/>
-      <c r="I33" s="55"/>
-      <c r="J33" s="52"/>
-      <c r="K33" s="55"/>
+      <c r="G33" s="43"/>
+      <c r="H33" s="43"/>
+      <c r="I33" s="59"/>
+      <c r="J33" s="71"/>
+      <c r="K33" s="59"/>
       <c r="L33" s="2"/>
       <c r="M33" s="2"/>
       <c r="N33" s="2"/>
@@ -2537,17 +2748,17 @@
       <c r="AA33" s="2"/>
     </row>
     <row r="34" spans="1:27">
-      <c r="A34" s="58"/>
-      <c r="B34" s="46"/>
-      <c r="C34" s="46"/>
-      <c r="D34" s="46"/>
-      <c r="E34" s="46"/>
+      <c r="A34" s="74"/>
+      <c r="B34" s="45"/>
+      <c r="C34" s="45"/>
+      <c r="D34" s="45"/>
+      <c r="E34" s="45"/>
       <c r="F34" s="30"/>
-      <c r="G34" s="35"/>
-      <c r="H34" s="35"/>
-      <c r="I34" s="55"/>
-      <c r="J34" s="52"/>
-      <c r="K34" s="55"/>
+      <c r="G34" s="43"/>
+      <c r="H34" s="43"/>
+      <c r="I34" s="59"/>
+      <c r="J34" s="71"/>
+      <c r="K34" s="59"/>
       <c r="L34" s="2"/>
       <c r="M34" s="2"/>
       <c r="N34" s="2"/>
@@ -2566,17 +2777,17 @@
       <c r="AA34" s="2"/>
     </row>
     <row r="35" spans="1:27">
-      <c r="A35" s="59"/>
-      <c r="B35" s="47"/>
-      <c r="C35" s="47"/>
-      <c r="D35" s="47"/>
-      <c r="E35" s="47"/>
+      <c r="A35" s="75"/>
+      <c r="B35" s="46"/>
+      <c r="C35" s="46"/>
+      <c r="D35" s="46"/>
+      <c r="E35" s="46"/>
       <c r="F35" s="30"/>
       <c r="G35" s="35"/>
       <c r="H35" s="35"/>
-      <c r="I35" s="56"/>
-      <c r="J35" s="53"/>
-      <c r="K35" s="56"/>
+      <c r="I35" s="60"/>
+      <c r="J35" s="72"/>
+      <c r="K35" s="60"/>
       <c r="L35" s="2"/>
       <c r="M35" s="2"/>
       <c r="N35" s="2"/>
@@ -2595,21 +2806,37 @@
       <c r="AA35" s="2"/>
     </row>
     <row r="36" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A36" s="57" t="s">
+      <c r="A36" s="73" t="s">
         <v>37</v>
       </c>
-      <c r="B36" s="45"/>
-      <c r="C36" s="48"/>
-      <c r="D36" s="45"/>
-      <c r="E36" s="45"/>
-      <c r="F36" s="30"/>
-      <c r="G36" s="35"/>
-      <c r="H36" s="35"/>
-      <c r="I36" s="54" t="s">
+      <c r="B36" s="44" t="s">
+        <v>84</v>
+      </c>
+      <c r="C36" s="44" t="s">
+        <v>93</v>
+      </c>
+      <c r="D36" s="44" t="s">
+        <v>94</v>
+      </c>
+      <c r="E36" s="44" t="s">
+        <v>95</v>
+      </c>
+      <c r="F36" s="30" t="s">
+        <v>53</v>
+      </c>
+      <c r="G36" s="35" t="s">
+        <v>91</v>
+      </c>
+      <c r="H36" s="35" t="s">
+        <v>92</v>
+      </c>
+      <c r="I36" s="58" t="s">
         <v>26</v>
       </c>
-      <c r="J36" s="51"/>
-      <c r="K36" s="54" t="s">
+      <c r="J36" s="70" t="s">
+        <v>56</v>
+      </c>
+      <c r="K36" s="58" t="s">
         <v>28</v>
       </c>
       <c r="L36" s="2"/>
@@ -2629,18 +2856,22 @@
       <c r="Z36" s="2"/>
       <c r="AA36" s="2"/>
     </row>
-    <row r="37" spans="1:27">
-      <c r="A37" s="58"/>
-      <c r="B37" s="46"/>
-      <c r="C37" s="49"/>
-      <c r="D37" s="46"/>
-      <c r="E37" s="46"/>
-      <c r="F37" s="30"/>
-      <c r="G37" s="35"/>
+    <row r="37" spans="1:27" ht="25.5">
+      <c r="A37" s="74"/>
+      <c r="B37" s="45"/>
+      <c r="C37" s="45"/>
+      <c r="D37" s="45"/>
+      <c r="E37" s="45"/>
+      <c r="F37" s="30" t="s">
+        <v>67</v>
+      </c>
+      <c r="G37" s="35" t="s">
+        <v>96</v>
+      </c>
       <c r="H37" s="35"/>
-      <c r="I37" s="55"/>
-      <c r="J37" s="52"/>
-      <c r="K37" s="55"/>
+      <c r="I37" s="59"/>
+      <c r="J37" s="71"/>
+      <c r="K37" s="59"/>
       <c r="L37" s="2"/>
       <c r="M37" s="2"/>
       <c r="N37" s="2"/>
@@ -2659,17 +2890,23 @@
       <c r="AA37" s="2"/>
     </row>
     <row r="38" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A38" s="58"/>
-      <c r="B38" s="46"/>
-      <c r="C38" s="49"/>
-      <c r="D38" s="46"/>
-      <c r="E38" s="46"/>
-      <c r="F38" s="30"/>
-      <c r="G38" s="35"/>
-      <c r="H38" s="35"/>
-      <c r="I38" s="55"/>
-      <c r="J38" s="52"/>
-      <c r="K38" s="55"/>
+      <c r="A38" s="74"/>
+      <c r="B38" s="45"/>
+      <c r="C38" s="45"/>
+      <c r="D38" s="45"/>
+      <c r="E38" s="45"/>
+      <c r="F38" s="30" t="s">
+        <v>70</v>
+      </c>
+      <c r="G38" s="35" t="s">
+        <v>97</v>
+      </c>
+      <c r="H38" s="35" t="s">
+        <v>98</v>
+      </c>
+      <c r="I38" s="59"/>
+      <c r="J38" s="71"/>
+      <c r="K38" s="59"/>
       <c r="L38" s="2"/>
       <c r="M38" s="2"/>
       <c r="N38" s="2"/>
@@ -2688,17 +2925,19 @@
       <c r="AA38" s="2"/>
     </row>
     <row r="39" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A39" s="59"/>
-      <c r="B39" s="47"/>
-      <c r="C39" s="50"/>
-      <c r="D39" s="47"/>
-      <c r="E39" s="47"/>
-      <c r="F39" s="30"/>
+      <c r="A39" s="75"/>
+      <c r="B39" s="46"/>
+      <c r="C39" s="46"/>
+      <c r="D39" s="46"/>
+      <c r="E39" s="46"/>
+      <c r="F39" s="30" t="s">
+        <v>99</v>
+      </c>
       <c r="G39" s="35"/>
       <c r="H39" s="35"/>
-      <c r="I39" s="56"/>
-      <c r="J39" s="53"/>
-      <c r="K39" s="56"/>
+      <c r="I39" s="60"/>
+      <c r="J39" s="72"/>
+      <c r="K39" s="60"/>
       <c r="L39" s="2"/>
       <c r="M39" s="2"/>
       <c r="N39" s="2"/>
@@ -2717,21 +2956,37 @@
       <c r="AA39" s="2"/>
     </row>
     <row r="40" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A40" s="57" t="s">
+      <c r="A40" s="73" t="s">
         <v>38</v>
       </c>
-      <c r="B40" s="45"/>
-      <c r="C40" s="48"/>
-      <c r="D40" s="45"/>
-      <c r="E40" s="45"/>
-      <c r="F40" s="30"/>
-      <c r="G40" s="35"/>
-      <c r="H40" s="35"/>
-      <c r="I40" s="54" t="s">
+      <c r="B40" s="44" t="s">
+        <v>84</v>
+      </c>
+      <c r="C40" s="44" t="s">
+        <v>100</v>
+      </c>
+      <c r="D40" s="44" t="s">
+        <v>101</v>
+      </c>
+      <c r="E40" s="44" t="s">
+        <v>102</v>
+      </c>
+      <c r="F40" s="30" t="s">
+        <v>53</v>
+      </c>
+      <c r="G40" s="35" t="s">
+        <v>87</v>
+      </c>
+      <c r="H40" s="35" t="s">
+        <v>88</v>
+      </c>
+      <c r="I40" s="58" t="s">
         <v>26</v>
       </c>
-      <c r="J40" s="51"/>
-      <c r="K40" s="54" t="s">
+      <c r="J40" s="70" t="s">
+        <v>56</v>
+      </c>
+      <c r="K40" s="58" t="s">
         <v>28</v>
       </c>
       <c r="L40" s="2"/>
@@ -2752,17 +3007,21 @@
       <c r="AA40" s="2"/>
     </row>
     <row r="41" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A41" s="58"/>
-      <c r="B41" s="46"/>
-      <c r="C41" s="49"/>
-      <c r="D41" s="46"/>
-      <c r="E41" s="46"/>
-      <c r="F41" s="30"/>
-      <c r="G41" s="35"/>
+      <c r="A41" s="74"/>
+      <c r="B41" s="45"/>
+      <c r="C41" s="45"/>
+      <c r="D41" s="45"/>
+      <c r="E41" s="45"/>
+      <c r="F41" s="30" t="s">
+        <v>67</v>
+      </c>
+      <c r="G41" s="35" t="s">
+        <v>103</v>
+      </c>
       <c r="H41" s="35"/>
-      <c r="I41" s="55"/>
-      <c r="J41" s="52"/>
-      <c r="K41" s="55"/>
+      <c r="I41" s="59"/>
+      <c r="J41" s="71"/>
+      <c r="K41" s="59"/>
       <c r="L41" s="2"/>
       <c r="M41" s="2"/>
       <c r="N41" s="2"/>
@@ -2780,18 +3039,24 @@
       <c r="Z41" s="2"/>
       <c r="AA41" s="2"/>
     </row>
-    <row r="42" spans="1:27">
-      <c r="A42" s="58"/>
-      <c r="B42" s="46"/>
-      <c r="C42" s="49"/>
-      <c r="D42" s="46"/>
-      <c r="E42" s="46"/>
-      <c r="F42" s="30"/>
-      <c r="G42" s="35"/>
-      <c r="H42" s="35"/>
-      <c r="I42" s="55"/>
-      <c r="J42" s="52"/>
-      <c r="K42" s="55"/>
+    <row r="42" spans="1:27" ht="16.5" customHeight="1">
+      <c r="A42" s="74"/>
+      <c r="B42" s="45"/>
+      <c r="C42" s="45"/>
+      <c r="D42" s="45"/>
+      <c r="E42" s="45"/>
+      <c r="F42" s="30" t="s">
+        <v>70</v>
+      </c>
+      <c r="G42" s="35" t="s">
+        <v>104</v>
+      </c>
+      <c r="H42" s="35" t="s">
+        <v>105</v>
+      </c>
+      <c r="I42" s="59"/>
+      <c r="J42" s="71"/>
+      <c r="K42" s="59"/>
       <c r="L42" s="2"/>
       <c r="M42" s="2"/>
       <c r="N42" s="2"/>
@@ -2810,17 +3075,19 @@
       <c r="AA42" s="2"/>
     </row>
     <row r="43" spans="1:27" ht="18.75" customHeight="1">
-      <c r="A43" s="59"/>
-      <c r="B43" s="47"/>
-      <c r="C43" s="50"/>
-      <c r="D43" s="47"/>
-      <c r="E43" s="47"/>
-      <c r="F43" s="30"/>
+      <c r="A43" s="75"/>
+      <c r="B43" s="46"/>
+      <c r="C43" s="46"/>
+      <c r="D43" s="46"/>
+      <c r="E43" s="46"/>
+      <c r="F43" s="30" t="s">
+        <v>99</v>
+      </c>
       <c r="G43" s="35"/>
       <c r="H43" s="35"/>
-      <c r="I43" s="56"/>
-      <c r="J43" s="53"/>
-      <c r="K43" s="56"/>
+      <c r="I43" s="60"/>
+      <c r="J43" s="72"/>
+      <c r="K43" s="60"/>
       <c r="L43" s="2"/>
       <c r="M43" s="2"/>
       <c r="N43" s="2"/>
@@ -2838,22 +3105,38 @@
       <c r="Z43" s="2"/>
       <c r="AA43" s="2"/>
     </row>
-    <row r="44" spans="1:27">
-      <c r="A44" s="57" t="s">
+    <row r="44" spans="1:27" ht="25.5">
+      <c r="A44" s="73" t="s">
         <v>39</v>
       </c>
-      <c r="B44" s="45"/>
-      <c r="C44" s="45"/>
-      <c r="D44" s="45"/>
-      <c r="E44" s="45"/>
-      <c r="F44" s="30"/>
-      <c r="G44" s="35"/>
-      <c r="H44" s="35"/>
-      <c r="I44" s="54" t="s">
+      <c r="B44" s="44" t="s">
+        <v>84</v>
+      </c>
+      <c r="C44" s="44" t="s">
+        <v>106</v>
+      </c>
+      <c r="D44" s="44" t="s">
+        <v>107</v>
+      </c>
+      <c r="E44" s="44" t="s">
+        <v>108</v>
+      </c>
+      <c r="F44" s="30" t="s">
+        <v>53</v>
+      </c>
+      <c r="G44" s="35" t="s">
+        <v>87</v>
+      </c>
+      <c r="H44" s="35" t="s">
+        <v>88</v>
+      </c>
+      <c r="I44" s="58" t="s">
         <v>26</v>
       </c>
-      <c r="J44" s="51"/>
-      <c r="K44" s="54" t="s">
+      <c r="J44" s="70" t="s">
+        <v>56</v>
+      </c>
+      <c r="K44" s="58" t="s">
         <v>28</v>
       </c>
       <c r="L44" s="2"/>
@@ -2874,17 +3157,21 @@
       <c r="AA44" s="2"/>
     </row>
     <row r="45" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A45" s="58"/>
-      <c r="B45" s="46"/>
-      <c r="C45" s="46"/>
-      <c r="D45" s="46"/>
-      <c r="E45" s="46"/>
-      <c r="F45" s="30"/>
-      <c r="G45" s="35"/>
+      <c r="A45" s="74"/>
+      <c r="B45" s="45"/>
+      <c r="C45" s="45"/>
+      <c r="D45" s="45"/>
+      <c r="E45" s="45"/>
+      <c r="F45" s="30" t="s">
+        <v>67</v>
+      </c>
+      <c r="G45" s="35" t="s">
+        <v>109</v>
+      </c>
       <c r="H45" s="35"/>
-      <c r="I45" s="55"/>
-      <c r="J45" s="52"/>
-      <c r="K45" s="55"/>
+      <c r="I45" s="59"/>
+      <c r="J45" s="71"/>
+      <c r="K45" s="59"/>
       <c r="L45" s="2"/>
       <c r="M45" s="2"/>
       <c r="N45" s="2"/>
@@ -2902,18 +3189,24 @@
       <c r="Z45" s="2"/>
       <c r="AA45" s="2"/>
     </row>
-    <row r="46" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A46" s="58"/>
-      <c r="B46" s="46"/>
-      <c r="C46" s="46"/>
-      <c r="D46" s="46"/>
-      <c r="E46" s="46"/>
-      <c r="F46" s="30"/>
-      <c r="G46" s="35"/>
-      <c r="H46" s="35"/>
-      <c r="I46" s="55"/>
-      <c r="J46" s="52"/>
-      <c r="K46" s="55"/>
+    <row r="46" spans="1:27" ht="25.5">
+      <c r="A46" s="74"/>
+      <c r="B46" s="45"/>
+      <c r="C46" s="45"/>
+      <c r="D46" s="45"/>
+      <c r="E46" s="45"/>
+      <c r="F46" s="30" t="s">
+        <v>70</v>
+      </c>
+      <c r="G46" s="35" t="s">
+        <v>104</v>
+      </c>
+      <c r="H46" s="35" t="s">
+        <v>110</v>
+      </c>
+      <c r="I46" s="59"/>
+      <c r="J46" s="71"/>
+      <c r="K46" s="59"/>
       <c r="L46" s="2"/>
       <c r="M46" s="2"/>
       <c r="N46" s="2"/>
@@ -2932,17 +3225,19 @@
       <c r="AA46" s="2"/>
     </row>
     <row r="47" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A47" s="59"/>
-      <c r="B47" s="47"/>
-      <c r="C47" s="47"/>
-      <c r="D47" s="47"/>
-      <c r="E47" s="47"/>
-      <c r="F47" s="30"/>
+      <c r="A47" s="75"/>
+      <c r="B47" s="46"/>
+      <c r="C47" s="46"/>
+      <c r="D47" s="46"/>
+      <c r="E47" s="46"/>
+      <c r="F47" s="30" t="s">
+        <v>99</v>
+      </c>
       <c r="G47" s="35"/>
-      <c r="H47" s="35"/>
-      <c r="I47" s="56"/>
-      <c r="J47" s="53"/>
-      <c r="K47" s="56"/>
+      <c r="H47" s="36"/>
+      <c r="I47" s="60"/>
+      <c r="J47" s="72"/>
+      <c r="K47" s="60"/>
       <c r="L47" s="2"/>
       <c r="M47" s="2"/>
       <c r="N47" s="2"/>
@@ -2960,22 +3255,38 @@
       <c r="Z47" s="2"/>
       <c r="AA47" s="2"/>
     </row>
-    <row r="48" spans="1:27">
-      <c r="A48" s="57" t="s">
+    <row r="48" spans="1:27" ht="25.5">
+      <c r="A48" s="73" t="s">
         <v>40</v>
       </c>
-      <c r="B48" s="45"/>
-      <c r="C48" s="45"/>
-      <c r="D48" s="45"/>
-      <c r="E48" s="45"/>
-      <c r="F48" s="30"/>
-      <c r="G48" s="35"/>
-      <c r="H48" s="35"/>
-      <c r="I48" s="54" t="s">
+      <c r="B48" s="44" t="s">
+        <v>84</v>
+      </c>
+      <c r="C48" s="44" t="s">
+        <v>111</v>
+      </c>
+      <c r="D48" s="44" t="s">
+        <v>112</v>
+      </c>
+      <c r="E48" s="44" t="s">
+        <v>102</v>
+      </c>
+      <c r="F48" s="30" t="s">
+        <v>53</v>
+      </c>
+      <c r="G48" s="35" t="s">
+        <v>87</v>
+      </c>
+      <c r="H48" s="35" t="s">
+        <v>88</v>
+      </c>
+      <c r="I48" s="58" t="s">
         <v>26</v>
       </c>
-      <c r="J48" s="51"/>
-      <c r="K48" s="54" t="s">
+      <c r="J48" s="70" t="s">
+        <v>56</v>
+      </c>
+      <c r="K48" s="58" t="s">
         <v>28</v>
       </c>
       <c r="L48" s="2"/>
@@ -2995,18 +3306,22 @@
       <c r="Z48" s="2"/>
       <c r="AA48" s="2"/>
     </row>
-    <row r="49" spans="1:27">
-      <c r="A49" s="58"/>
-      <c r="B49" s="46"/>
-      <c r="C49" s="46"/>
-      <c r="D49" s="46"/>
-      <c r="E49" s="46"/>
-      <c r="F49" s="30"/>
-      <c r="G49" s="43"/>
-      <c r="H49" s="43"/>
-      <c r="I49" s="55"/>
-      <c r="J49" s="52"/>
-      <c r="K49" s="55"/>
+    <row r="49" spans="1:27" ht="15.75" customHeight="1">
+      <c r="A49" s="74"/>
+      <c r="B49" s="45"/>
+      <c r="C49" s="45"/>
+      <c r="D49" s="45"/>
+      <c r="E49" s="45"/>
+      <c r="F49" s="30" t="s">
+        <v>67</v>
+      </c>
+      <c r="G49" s="35" t="s">
+        <v>113</v>
+      </c>
+      <c r="H49" s="35"/>
+      <c r="I49" s="59"/>
+      <c r="J49" s="71"/>
+      <c r="K49" s="59"/>
       <c r="L49" s="2"/>
       <c r="M49" s="2"/>
       <c r="N49" s="2"/>
@@ -3024,18 +3339,24 @@
       <c r="Z49" s="2"/>
       <c r="AA49" s="2"/>
     </row>
-    <row r="50" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A50" s="58"/>
-      <c r="B50" s="46"/>
-      <c r="C50" s="46"/>
-      <c r="D50" s="46"/>
-      <c r="E50" s="46"/>
-      <c r="F50" s="30"/>
-      <c r="G50" s="43"/>
-      <c r="H50" s="43"/>
-      <c r="I50" s="55"/>
-      <c r="J50" s="52"/>
-      <c r="K50" s="55"/>
+    <row r="50" spans="1:27" ht="27" customHeight="1">
+      <c r="A50" s="74"/>
+      <c r="B50" s="45"/>
+      <c r="C50" s="45"/>
+      <c r="D50" s="45"/>
+      <c r="E50" s="45"/>
+      <c r="F50" s="30" t="s">
+        <v>70</v>
+      </c>
+      <c r="G50" s="35" t="s">
+        <v>104</v>
+      </c>
+      <c r="H50" s="35" t="s">
+        <v>110</v>
+      </c>
+      <c r="I50" s="59"/>
+      <c r="J50" s="71"/>
+      <c r="K50" s="59"/>
       <c r="L50" s="2"/>
       <c r="M50" s="2"/>
       <c r="N50" s="2"/>
@@ -3054,17 +3375,19 @@
       <c r="AA50" s="2"/>
     </row>
     <row r="51" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A51" s="59"/>
-      <c r="B51" s="47"/>
-      <c r="C51" s="47"/>
-      <c r="D51" s="47"/>
-      <c r="E51" s="47"/>
-      <c r="F51" s="30"/>
+      <c r="A51" s="75"/>
+      <c r="B51" s="46"/>
+      <c r="C51" s="46"/>
+      <c r="D51" s="46"/>
+      <c r="E51" s="46"/>
+      <c r="F51" s="30" t="s">
+        <v>99</v>
+      </c>
       <c r="G51" s="35"/>
-      <c r="H51" s="35"/>
-      <c r="I51" s="56"/>
-      <c r="J51" s="53"/>
-      <c r="K51" s="56"/>
+      <c r="H51" s="36"/>
+      <c r="I51" s="60"/>
+      <c r="J51" s="72"/>
+      <c r="K51" s="60"/>
       <c r="L51" s="2"/>
       <c r="M51" s="2"/>
       <c r="N51" s="2"/>
@@ -3082,22 +3405,38 @@
       <c r="Z51" s="2"/>
       <c r="AA51" s="2"/>
     </row>
-    <row r="52" spans="1:27">
-      <c r="A52" s="57" t="s">
+    <row r="52" spans="1:27" ht="25.5">
+      <c r="A52" s="73" t="s">
         <v>41</v>
       </c>
-      <c r="B52" s="45"/>
-      <c r="C52" s="45"/>
-      <c r="D52" s="45"/>
-      <c r="E52" s="45"/>
-      <c r="F52" s="30"/>
-      <c r="G52" s="35"/>
-      <c r="H52" s="35"/>
-      <c r="I52" s="54" t="s">
+      <c r="B52" s="44" t="s">
+        <v>84</v>
+      </c>
+      <c r="C52" s="44" t="s">
+        <v>114</v>
+      </c>
+      <c r="D52" s="44" t="s">
+        <v>129</v>
+      </c>
+      <c r="E52" s="44" t="s">
+        <v>95</v>
+      </c>
+      <c r="F52" s="30" t="s">
+        <v>53</v>
+      </c>
+      <c r="G52" s="35" t="s">
+        <v>91</v>
+      </c>
+      <c r="H52" s="35" t="s">
+        <v>92</v>
+      </c>
+      <c r="I52" s="58" t="s">
         <v>26</v>
       </c>
-      <c r="J52" s="51"/>
-      <c r="K52" s="54" t="s">
+      <c r="J52" s="70" t="s">
+        <v>56</v>
+      </c>
+      <c r="K52" s="58" t="s">
         <v>28</v>
       </c>
       <c r="L52" s="2"/>
@@ -3117,18 +3456,24 @@
       <c r="Z52" s="2"/>
       <c r="AA52" s="2"/>
     </row>
-    <row r="53" spans="1:27">
-      <c r="A53" s="58"/>
-      <c r="B53" s="46"/>
-      <c r="C53" s="46"/>
-      <c r="D53" s="46"/>
-      <c r="E53" s="46"/>
-      <c r="F53" s="30"/>
-      <c r="G53" s="35"/>
-      <c r="H53" s="35"/>
-      <c r="I53" s="55"/>
-      <c r="J53" s="52"/>
-      <c r="K53" s="55"/>
+    <row r="53" spans="1:27" ht="25.5">
+      <c r="A53" s="74"/>
+      <c r="B53" s="45"/>
+      <c r="C53" s="45"/>
+      <c r="D53" s="45"/>
+      <c r="E53" s="45"/>
+      <c r="F53" s="30" t="s">
+        <v>67</v>
+      </c>
+      <c r="G53" s="36" t="s">
+        <v>115</v>
+      </c>
+      <c r="H53" s="36" t="s">
+        <v>116</v>
+      </c>
+      <c r="I53" s="59"/>
+      <c r="J53" s="71"/>
+      <c r="K53" s="59"/>
       <c r="L53" s="2"/>
       <c r="M53" s="2"/>
       <c r="N53" s="2"/>
@@ -3146,18 +3491,18 @@
       <c r="Z53" s="2"/>
       <c r="AA53" s="2"/>
     </row>
-    <row r="54" spans="1:27">
-      <c r="A54" s="58"/>
-      <c r="B54" s="46"/>
-      <c r="C54" s="46"/>
-      <c r="D54" s="46"/>
-      <c r="E54" s="46"/>
+    <row r="54" spans="1:27" ht="13.5" customHeight="1">
+      <c r="A54" s="74"/>
+      <c r="B54" s="45"/>
+      <c r="C54" s="45"/>
+      <c r="D54" s="45"/>
+      <c r="E54" s="45"/>
       <c r="F54" s="30"/>
-      <c r="G54" s="35"/>
-      <c r="H54" s="35"/>
-      <c r="I54" s="55"/>
-      <c r="J54" s="52"/>
-      <c r="K54" s="55"/>
+      <c r="G54" s="43"/>
+      <c r="H54" s="43"/>
+      <c r="I54" s="59"/>
+      <c r="J54" s="71"/>
+      <c r="K54" s="59"/>
       <c r="L54" s="2"/>
       <c r="M54" s="2"/>
       <c r="N54" s="2"/>
@@ -3175,18 +3520,18 @@
       <c r="Z54" s="2"/>
       <c r="AA54" s="2"/>
     </row>
-    <row r="55" spans="1:27">
-      <c r="A55" s="59"/>
-      <c r="B55" s="47"/>
-      <c r="C55" s="47"/>
-      <c r="D55" s="47"/>
-      <c r="E55" s="47"/>
+    <row r="55" spans="1:27" ht="15" customHeight="1">
+      <c r="A55" s="75"/>
+      <c r="B55" s="46"/>
+      <c r="C55" s="46"/>
+      <c r="D55" s="46"/>
+      <c r="E55" s="46"/>
       <c r="F55" s="30"/>
-      <c r="G55" s="35"/>
-      <c r="H55" s="35"/>
-      <c r="I55" s="56"/>
-      <c r="J55" s="53"/>
-      <c r="K55" s="56"/>
+      <c r="G55" s="43"/>
+      <c r="H55" s="43"/>
+      <c r="I55" s="60"/>
+      <c r="J55" s="72"/>
+      <c r="K55" s="60"/>
       <c r="L55" s="2"/>
       <c r="M55" s="2"/>
       <c r="N55" s="2"/>
@@ -3204,22 +3549,38 @@
       <c r="Z55" s="2"/>
       <c r="AA55" s="2"/>
     </row>
-    <row r="56" spans="1:27">
-      <c r="A56" s="57" t="s">
+    <row r="56" spans="1:27" ht="25.5">
+      <c r="A56" s="73" t="s">
         <v>42</v>
       </c>
-      <c r="B56" s="45"/>
-      <c r="C56" s="45"/>
-      <c r="D56" s="45"/>
-      <c r="E56" s="45"/>
-      <c r="F56" s="30"/>
-      <c r="G56" s="35"/>
-      <c r="H56" s="35"/>
-      <c r="I56" s="54" t="s">
+      <c r="B56" s="44" t="s">
+        <v>84</v>
+      </c>
+      <c r="C56" s="44" t="s">
+        <v>117</v>
+      </c>
+      <c r="D56" s="44" t="s">
+        <v>118</v>
+      </c>
+      <c r="E56" s="44" t="s">
+        <v>95</v>
+      </c>
+      <c r="F56" s="30" t="s">
+        <v>53</v>
+      </c>
+      <c r="G56" s="35" t="s">
+        <v>91</v>
+      </c>
+      <c r="H56" s="35" t="s">
+        <v>92</v>
+      </c>
+      <c r="I56" s="58" t="s">
         <v>26</v>
       </c>
-      <c r="J56" s="51"/>
-      <c r="K56" s="54" t="s">
+      <c r="J56" s="70" t="s">
+        <v>56</v>
+      </c>
+      <c r="K56" s="58" t="s">
         <v>28</v>
       </c>
       <c r="L56" s="2"/>
@@ -3239,18 +3600,24 @@
       <c r="Z56" s="2"/>
       <c r="AA56" s="2"/>
     </row>
-    <row r="57" spans="1:27">
-      <c r="A57" s="58"/>
-      <c r="B57" s="46"/>
-      <c r="C57" s="46"/>
-      <c r="D57" s="46"/>
-      <c r="E57" s="46"/>
-      <c r="F57" s="30"/>
-      <c r="G57" s="35"/>
-      <c r="H57" s="35"/>
-      <c r="I57" s="55"/>
-      <c r="J57" s="52"/>
-      <c r="K57" s="55"/>
+    <row r="57" spans="1:27" ht="17.25" customHeight="1">
+      <c r="A57" s="74"/>
+      <c r="B57" s="45"/>
+      <c r="C57" s="45"/>
+      <c r="D57" s="45"/>
+      <c r="E57" s="45"/>
+      <c r="F57" s="30" t="s">
+        <v>67</v>
+      </c>
+      <c r="G57" s="36" t="s">
+        <v>119</v>
+      </c>
+      <c r="H57" s="36" t="s">
+        <v>120</v>
+      </c>
+      <c r="I57" s="59"/>
+      <c r="J57" s="71"/>
+      <c r="K57" s="59"/>
       <c r="L57" s="2"/>
       <c r="M57" s="2"/>
       <c r="N57" s="2"/>
@@ -3268,18 +3635,24 @@
       <c r="Z57" s="2"/>
       <c r="AA57" s="2"/>
     </row>
-    <row r="58" spans="1:27">
-      <c r="A58" s="58"/>
-      <c r="B58" s="46"/>
-      <c r="C58" s="46"/>
-      <c r="D58" s="46"/>
-      <c r="E58" s="46"/>
-      <c r="F58" s="30"/>
-      <c r="G58" s="35"/>
-      <c r="H58" s="35"/>
-      <c r="I58" s="55"/>
-      <c r="J58" s="52"/>
-      <c r="K58" s="55"/>
+    <row r="58" spans="1:27" ht="25.5">
+      <c r="A58" s="74"/>
+      <c r="B58" s="45"/>
+      <c r="C58" s="45"/>
+      <c r="D58" s="45"/>
+      <c r="E58" s="45"/>
+      <c r="F58" s="30" t="s">
+        <v>70</v>
+      </c>
+      <c r="G58" s="36" t="s">
+        <v>121</v>
+      </c>
+      <c r="H58" s="36" t="s">
+        <v>122</v>
+      </c>
+      <c r="I58" s="59"/>
+      <c r="J58" s="71"/>
+      <c r="K58" s="59"/>
       <c r="L58" s="2"/>
       <c r="M58" s="2"/>
       <c r="N58" s="2"/>
@@ -3297,18 +3670,24 @@
       <c r="Z58" s="2"/>
       <c r="AA58" s="2"/>
     </row>
-    <row r="59" spans="1:27">
-      <c r="A59" s="59"/>
-      <c r="B59" s="47"/>
-      <c r="C59" s="47"/>
-      <c r="D59" s="47"/>
-      <c r="E59" s="47"/>
-      <c r="F59" s="30"/>
-      <c r="G59" s="35"/>
-      <c r="H59" s="35"/>
-      <c r="I59" s="56"/>
-      <c r="J59" s="53"/>
-      <c r="K59" s="56"/>
+    <row r="59" spans="1:27" ht="25.5">
+      <c r="A59" s="75"/>
+      <c r="B59" s="46"/>
+      <c r="C59" s="46"/>
+      <c r="D59" s="46"/>
+      <c r="E59" s="46"/>
+      <c r="F59" s="30" t="s">
+        <v>99</v>
+      </c>
+      <c r="G59" s="35" t="s">
+        <v>104</v>
+      </c>
+      <c r="H59" s="36" t="s">
+        <v>123</v>
+      </c>
+      <c r="I59" s="60"/>
+      <c r="J59" s="72"/>
+      <c r="K59" s="60"/>
       <c r="L59" s="2"/>
       <c r="M59" s="2"/>
       <c r="N59" s="2"/>
@@ -3326,22 +3705,38 @@
       <c r="Z59" s="2"/>
       <c r="AA59" s="2"/>
     </row>
-    <row r="60" spans="1:27">
-      <c r="A60" s="57" t="s">
+    <row r="60" spans="1:27" ht="25.5">
+      <c r="A60" s="73" t="s">
         <v>43</v>
       </c>
-      <c r="B60" s="45"/>
-      <c r="C60" s="45"/>
-      <c r="D60" s="45"/>
-      <c r="E60" s="45"/>
-      <c r="F60" s="30"/>
-      <c r="G60" s="35"/>
-      <c r="H60" s="35"/>
-      <c r="I60" s="54" t="s">
+      <c r="B60" s="44" t="s">
+        <v>84</v>
+      </c>
+      <c r="C60" s="44" t="s">
+        <v>124</v>
+      </c>
+      <c r="D60" s="44" t="s">
+        <v>125</v>
+      </c>
+      <c r="E60" s="44" t="s">
+        <v>102</v>
+      </c>
+      <c r="F60" s="30" t="s">
+        <v>53</v>
+      </c>
+      <c r="G60" s="35" t="s">
+        <v>91</v>
+      </c>
+      <c r="H60" s="35" t="s">
+        <v>92</v>
+      </c>
+      <c r="I60" s="58" t="s">
         <v>26</v>
       </c>
-      <c r="J60" s="51"/>
-      <c r="K60" s="54" t="s">
+      <c r="J60" s="70" t="s">
+        <v>56</v>
+      </c>
+      <c r="K60" s="58" t="s">
         <v>28</v>
       </c>
       <c r="L60" s="2"/>
@@ -3361,18 +3756,24 @@
       <c r="Z60" s="2"/>
       <c r="AA60" s="2"/>
     </row>
-    <row r="61" spans="1:27">
-      <c r="A61" s="58"/>
-      <c r="B61" s="46"/>
-      <c r="C61" s="46"/>
-      <c r="D61" s="46"/>
-      <c r="E61" s="46"/>
-      <c r="F61" s="30"/>
-      <c r="G61" s="35"/>
-      <c r="H61" s="35"/>
-      <c r="I61" s="55"/>
-      <c r="J61" s="52"/>
-      <c r="K61" s="55"/>
+    <row r="61" spans="1:27" ht="25.5">
+      <c r="A61" s="74"/>
+      <c r="B61" s="45"/>
+      <c r="C61" s="45"/>
+      <c r="D61" s="45"/>
+      <c r="E61" s="45"/>
+      <c r="F61" s="30" t="s">
+        <v>67</v>
+      </c>
+      <c r="G61" s="35" t="s">
+        <v>126</v>
+      </c>
+      <c r="H61" s="36" t="s">
+        <v>120</v>
+      </c>
+      <c r="I61" s="59"/>
+      <c r="J61" s="71"/>
+      <c r="K61" s="59"/>
       <c r="L61" s="2"/>
       <c r="M61" s="2"/>
       <c r="N61" s="2"/>
@@ -3390,18 +3791,24 @@
       <c r="Z61" s="2"/>
       <c r="AA61" s="2"/>
     </row>
-    <row r="62" spans="1:27">
-      <c r="A62" s="58"/>
-      <c r="B62" s="46"/>
-      <c r="C62" s="46"/>
-      <c r="D62" s="46"/>
-      <c r="E62" s="46"/>
-      <c r="F62" s="30"/>
-      <c r="G62" s="35"/>
-      <c r="H62" s="35"/>
-      <c r="I62" s="55"/>
-      <c r="J62" s="52"/>
-      <c r="K62" s="55"/>
+    <row r="62" spans="1:27" ht="25.5">
+      <c r="A62" s="74"/>
+      <c r="B62" s="45"/>
+      <c r="C62" s="45"/>
+      <c r="D62" s="45"/>
+      <c r="E62" s="45"/>
+      <c r="F62" s="30" t="s">
+        <v>70</v>
+      </c>
+      <c r="G62" s="36" t="s">
+        <v>127</v>
+      </c>
+      <c r="H62" s="36" t="s">
+        <v>122</v>
+      </c>
+      <c r="I62" s="59"/>
+      <c r="J62" s="71"/>
+      <c r="K62" s="59"/>
       <c r="L62" s="2"/>
       <c r="M62" s="2"/>
       <c r="N62" s="2"/>
@@ -3419,18 +3826,24 @@
       <c r="Z62" s="2"/>
       <c r="AA62" s="2"/>
     </row>
-    <row r="63" spans="1:27">
-      <c r="A63" s="59"/>
-      <c r="B63" s="47"/>
-      <c r="C63" s="47"/>
-      <c r="D63" s="47"/>
-      <c r="E63" s="47"/>
-      <c r="F63" s="30"/>
-      <c r="G63" s="35"/>
-      <c r="H63" s="36"/>
-      <c r="I63" s="56"/>
-      <c r="J63" s="53"/>
-      <c r="K63" s="56"/>
+    <row r="63" spans="1:27" ht="25.5">
+      <c r="A63" s="75"/>
+      <c r="B63" s="46"/>
+      <c r="C63" s="46"/>
+      <c r="D63" s="46"/>
+      <c r="E63" s="46"/>
+      <c r="F63" s="30" t="s">
+        <v>99</v>
+      </c>
+      <c r="G63" s="35" t="s">
+        <v>97</v>
+      </c>
+      <c r="H63" s="35" t="s">
+        <v>128</v>
+      </c>
+      <c r="I63" s="60"/>
+      <c r="J63" s="72"/>
+      <c r="K63" s="60"/>
       <c r="L63" s="2"/>
       <c r="M63" s="2"/>
       <c r="N63" s="2"/>
@@ -3449,21 +3862,21 @@
       <c r="AA63" s="2"/>
     </row>
     <row r="64" spans="1:27">
-      <c r="A64" s="57" t="s">
+      <c r="A64" s="50" t="s">
         <v>44</v>
       </c>
-      <c r="B64" s="45"/>
-      <c r="C64" s="45"/>
-      <c r="D64" s="45"/>
-      <c r="E64" s="45"/>
+      <c r="B64" s="44"/>
+      <c r="C64" s="44"/>
+      <c r="D64" s="44"/>
+      <c r="E64" s="44"/>
       <c r="F64" s="30"/>
       <c r="G64" s="35"/>
       <c r="H64" s="35"/>
-      <c r="I64" s="54" t="s">
+      <c r="I64" s="58" t="s">
         <v>26</v>
       </c>
-      <c r="J64" s="51"/>
-      <c r="K64" s="54" t="s">
+      <c r="J64" s="70"/>
+      <c r="K64" s="58" t="s">
         <v>28</v>
       </c>
       <c r="L64" s="2"/>
@@ -3484,17 +3897,17 @@
       <c r="AA64" s="2"/>
     </row>
     <row r="65" spans="1:27">
-      <c r="A65" s="58"/>
-      <c r="B65" s="46"/>
-      <c r="C65" s="46"/>
-      <c r="D65" s="46"/>
-      <c r="E65" s="46"/>
+      <c r="A65" s="51"/>
+      <c r="B65" s="45"/>
+      <c r="C65" s="45"/>
+      <c r="D65" s="45"/>
+      <c r="E65" s="45"/>
       <c r="F65" s="30"/>
       <c r="G65" s="35"/>
       <c r="H65" s="35"/>
-      <c r="I65" s="55"/>
-      <c r="J65" s="52"/>
-      <c r="K65" s="55"/>
+      <c r="I65" s="59"/>
+      <c r="J65" s="71"/>
+      <c r="K65" s="59"/>
       <c r="L65" s="2"/>
       <c r="M65" s="2"/>
       <c r="N65" s="2"/>
@@ -3513,17 +3926,17 @@
       <c r="AA65" s="2"/>
     </row>
     <row r="66" spans="1:27">
-      <c r="A66" s="58"/>
-      <c r="B66" s="46"/>
-      <c r="C66" s="46"/>
-      <c r="D66" s="46"/>
-      <c r="E66" s="46"/>
+      <c r="A66" s="51"/>
+      <c r="B66" s="45"/>
+      <c r="C66" s="45"/>
+      <c r="D66" s="45"/>
+      <c r="E66" s="45"/>
       <c r="F66" s="30"/>
       <c r="G66" s="35"/>
       <c r="H66" s="35"/>
-      <c r="I66" s="55"/>
-      <c r="J66" s="52"/>
-      <c r="K66" s="55"/>
+      <c r="I66" s="59"/>
+      <c r="J66" s="71"/>
+      <c r="K66" s="59"/>
       <c r="L66" s="2"/>
       <c r="M66" s="2"/>
       <c r="N66" s="2"/>
@@ -3542,17 +3955,17 @@
       <c r="AA66" s="2"/>
     </row>
     <row r="67" spans="1:27">
-      <c r="A67" s="59"/>
-      <c r="B67" s="47"/>
-      <c r="C67" s="47"/>
-      <c r="D67" s="47"/>
-      <c r="E67" s="47"/>
+      <c r="A67" s="52"/>
+      <c r="B67" s="46"/>
+      <c r="C67" s="46"/>
+      <c r="D67" s="46"/>
+      <c r="E67" s="46"/>
       <c r="F67" s="30"/>
       <c r="G67" s="35"/>
       <c r="H67" s="36"/>
-      <c r="I67" s="56"/>
-      <c r="J67" s="53"/>
-      <c r="K67" s="56"/>
+      <c r="I67" s="60"/>
+      <c r="J67" s="72"/>
+      <c r="K67" s="60"/>
       <c r="L67" s="2"/>
       <c r="M67" s="2"/>
       <c r="N67" s="2"/>
@@ -3571,21 +3984,21 @@
       <c r="AA67" s="2"/>
     </row>
     <row r="68" spans="1:27">
-      <c r="A68" s="57" t="s">
+      <c r="A68" s="50" t="s">
         <v>45</v>
       </c>
-      <c r="B68" s="45"/>
-      <c r="C68" s="45"/>
-      <c r="D68" s="45"/>
-      <c r="E68" s="45"/>
+      <c r="B68" s="44"/>
+      <c r="C68" s="44"/>
+      <c r="D68" s="44"/>
+      <c r="E68" s="44"/>
       <c r="F68" s="30"/>
       <c r="G68" s="35"/>
       <c r="H68" s="35"/>
-      <c r="I68" s="54" t="s">
+      <c r="I68" s="58" t="s">
         <v>26</v>
       </c>
-      <c r="J68" s="51"/>
-      <c r="K68" s="54" t="s">
+      <c r="J68" s="70"/>
+      <c r="K68" s="58" t="s">
         <v>28</v>
       </c>
       <c r="L68" s="2"/>
@@ -3606,17 +4019,17 @@
       <c r="AA68" s="2"/>
     </row>
     <row r="69" spans="1:27">
-      <c r="A69" s="58"/>
-      <c r="B69" s="46"/>
-      <c r="C69" s="46"/>
-      <c r="D69" s="46"/>
-      <c r="E69" s="46"/>
+      <c r="A69" s="51"/>
+      <c r="B69" s="45"/>
+      <c r="C69" s="45"/>
+      <c r="D69" s="45"/>
+      <c r="E69" s="45"/>
       <c r="F69" s="30"/>
       <c r="G69" s="36"/>
       <c r="H69" s="36"/>
-      <c r="I69" s="55"/>
-      <c r="J69" s="52"/>
-      <c r="K69" s="55"/>
+      <c r="I69" s="59"/>
+      <c r="J69" s="71"/>
+      <c r="K69" s="59"/>
       <c r="L69" s="2"/>
       <c r="M69" s="2"/>
       <c r="N69" s="2"/>
@@ -3635,17 +4048,17 @@
       <c r="AA69" s="2"/>
     </row>
     <row r="70" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A70" s="58"/>
-      <c r="B70" s="46"/>
-      <c r="C70" s="46"/>
-      <c r="D70" s="46"/>
-      <c r="E70" s="46"/>
+      <c r="A70" s="51"/>
+      <c r="B70" s="45"/>
+      <c r="C70" s="45"/>
+      <c r="D70" s="45"/>
+      <c r="E70" s="45"/>
       <c r="F70" s="30"/>
       <c r="G70" s="43"/>
       <c r="H70" s="43"/>
-      <c r="I70" s="55"/>
-      <c r="J70" s="52"/>
-      <c r="K70" s="55"/>
+      <c r="I70" s="59"/>
+      <c r="J70" s="71"/>
+      <c r="K70" s="59"/>
       <c r="L70" s="2"/>
       <c r="M70" s="2"/>
       <c r="N70" s="2"/>
@@ -3664,17 +4077,17 @@
       <c r="AA70" s="2"/>
     </row>
     <row r="71" spans="1:27">
-      <c r="A71" s="59"/>
-      <c r="B71" s="47"/>
-      <c r="C71" s="47"/>
-      <c r="D71" s="47"/>
-      <c r="E71" s="47"/>
+      <c r="A71" s="52"/>
+      <c r="B71" s="46"/>
+      <c r="C71" s="46"/>
+      <c r="D71" s="46"/>
+      <c r="E71" s="46"/>
       <c r="F71" s="30"/>
       <c r="G71" s="43"/>
       <c r="H71" s="43"/>
-      <c r="I71" s="56"/>
-      <c r="J71" s="53"/>
-      <c r="K71" s="56"/>
+      <c r="I71" s="60"/>
+      <c r="J71" s="72"/>
+      <c r="K71" s="60"/>
       <c r="L71" s="2"/>
       <c r="M71" s="2"/>
       <c r="N71" s="2"/>
@@ -3693,21 +4106,21 @@
       <c r="AA71" s="2"/>
     </row>
     <row r="72" spans="1:27">
-      <c r="A72" s="57" t="s">
+      <c r="A72" s="50" t="s">
         <v>46</v>
       </c>
-      <c r="B72" s="45"/>
-      <c r="C72" s="45"/>
-      <c r="D72" s="45"/>
-      <c r="E72" s="45"/>
+      <c r="B72" s="44"/>
+      <c r="C72" s="44"/>
+      <c r="D72" s="44"/>
+      <c r="E72" s="44"/>
       <c r="F72" s="30"/>
       <c r="G72" s="35"/>
       <c r="H72" s="35"/>
-      <c r="I72" s="54" t="s">
+      <c r="I72" s="58" t="s">
         <v>26</v>
       </c>
-      <c r="J72" s="51"/>
-      <c r="K72" s="54" t="s">
+      <c r="J72" s="70"/>
+      <c r="K72" s="58" t="s">
         <v>28</v>
       </c>
       <c r="L72" s="2"/>
@@ -3728,17 +4141,17 @@
       <c r="AA72" s="2"/>
     </row>
     <row r="73" spans="1:27">
-      <c r="A73" s="58"/>
-      <c r="B73" s="46"/>
-      <c r="C73" s="46"/>
-      <c r="D73" s="46"/>
-      <c r="E73" s="46"/>
+      <c r="A73" s="51"/>
+      <c r="B73" s="45"/>
+      <c r="C73" s="45"/>
+      <c r="D73" s="45"/>
+      <c r="E73" s="45"/>
       <c r="F73" s="30"/>
       <c r="G73" s="36"/>
       <c r="H73" s="36"/>
-      <c r="I73" s="55"/>
-      <c r="J73" s="52"/>
-      <c r="K73" s="55"/>
+      <c r="I73" s="59"/>
+      <c r="J73" s="71"/>
+      <c r="K73" s="59"/>
       <c r="L73" s="2"/>
       <c r="M73" s="2"/>
       <c r="N73" s="2"/>
@@ -3757,17 +4170,17 @@
       <c r="AA73" s="2"/>
     </row>
     <row r="74" spans="1:27">
-      <c r="A74" s="58"/>
-      <c r="B74" s="46"/>
-      <c r="C74" s="46"/>
-      <c r="D74" s="46"/>
-      <c r="E74" s="46"/>
+      <c r="A74" s="51"/>
+      <c r="B74" s="45"/>
+      <c r="C74" s="45"/>
+      <c r="D74" s="45"/>
+      <c r="E74" s="45"/>
       <c r="F74" s="30"/>
       <c r="G74" s="36"/>
       <c r="H74" s="36"/>
-      <c r="I74" s="55"/>
-      <c r="J74" s="52"/>
-      <c r="K74" s="55"/>
+      <c r="I74" s="59"/>
+      <c r="J74" s="71"/>
+      <c r="K74" s="59"/>
       <c r="L74" s="2"/>
       <c r="M74" s="2"/>
       <c r="N74" s="2"/>
@@ -3786,17 +4199,17 @@
       <c r="AA74" s="2"/>
     </row>
     <row r="75" spans="1:27">
-      <c r="A75" s="59"/>
-      <c r="B75" s="47"/>
-      <c r="C75" s="47"/>
-      <c r="D75" s="47"/>
-      <c r="E75" s="47"/>
+      <c r="A75" s="52"/>
+      <c r="B75" s="46"/>
+      <c r="C75" s="46"/>
+      <c r="D75" s="46"/>
+      <c r="E75" s="46"/>
       <c r="F75" s="30"/>
       <c r="G75" s="35"/>
       <c r="H75" s="36"/>
-      <c r="I75" s="56"/>
-      <c r="J75" s="53"/>
-      <c r="K75" s="56"/>
+      <c r="I75" s="60"/>
+      <c r="J75" s="72"/>
+      <c r="K75" s="60"/>
       <c r="L75" s="2"/>
       <c r="M75" s="2"/>
       <c r="N75" s="2"/>
@@ -3815,21 +4228,21 @@
       <c r="AA75" s="2"/>
     </row>
     <row r="76" spans="1:27">
-      <c r="A76" s="57" t="s">
+      <c r="A76" s="50" t="s">
         <v>47</v>
       </c>
-      <c r="B76" s="45"/>
-      <c r="C76" s="45"/>
-      <c r="D76" s="45"/>
-      <c r="E76" s="45"/>
+      <c r="B76" s="44"/>
+      <c r="C76" s="44"/>
+      <c r="D76" s="44"/>
+      <c r="E76" s="44"/>
       <c r="F76" s="30"/>
       <c r="G76" s="35"/>
       <c r="H76" s="35"/>
-      <c r="I76" s="54" t="s">
+      <c r="I76" s="58" t="s">
         <v>26</v>
       </c>
-      <c r="J76" s="51"/>
-      <c r="K76" s="54" t="s">
+      <c r="J76" s="70"/>
+      <c r="K76" s="58" t="s">
         <v>28</v>
       </c>
       <c r="L76" s="2"/>
@@ -3850,17 +4263,17 @@
       <c r="AA76" s="2"/>
     </row>
     <row r="77" spans="1:27">
-      <c r="A77" s="58"/>
-      <c r="B77" s="46"/>
-      <c r="C77" s="46"/>
-      <c r="D77" s="46"/>
-      <c r="E77" s="46"/>
+      <c r="A77" s="51"/>
+      <c r="B77" s="45"/>
+      <c r="C77" s="45"/>
+      <c r="D77" s="45"/>
+      <c r="E77" s="45"/>
       <c r="F77" s="30"/>
       <c r="G77" s="35"/>
       <c r="H77" s="36"/>
-      <c r="I77" s="55"/>
-      <c r="J77" s="52"/>
-      <c r="K77" s="55"/>
+      <c r="I77" s="59"/>
+      <c r="J77" s="71"/>
+      <c r="K77" s="59"/>
       <c r="L77" s="2"/>
       <c r="M77" s="2"/>
       <c r="N77" s="2"/>
@@ -3879,17 +4292,17 @@
       <c r="AA77" s="2"/>
     </row>
     <row r="78" spans="1:27">
-      <c r="A78" s="58"/>
-      <c r="B78" s="46"/>
-      <c r="C78" s="46"/>
-      <c r="D78" s="46"/>
-      <c r="E78" s="46"/>
+      <c r="A78" s="51"/>
+      <c r="B78" s="45"/>
+      <c r="C78" s="45"/>
+      <c r="D78" s="45"/>
+      <c r="E78" s="45"/>
       <c r="F78" s="30"/>
       <c r="G78" s="36"/>
       <c r="H78" s="36"/>
-      <c r="I78" s="55"/>
-      <c r="J78" s="52"/>
-      <c r="K78" s="55"/>
+      <c r="I78" s="59"/>
+      <c r="J78" s="71"/>
+      <c r="K78" s="59"/>
       <c r="L78" s="2"/>
       <c r="M78" s="2"/>
       <c r="N78" s="2"/>
@@ -3908,17 +4321,17 @@
       <c r="AA78" s="2"/>
     </row>
     <row r="79" spans="1:27">
-      <c r="A79" s="59"/>
-      <c r="B79" s="47"/>
-      <c r="C79" s="47"/>
-      <c r="D79" s="47"/>
-      <c r="E79" s="47"/>
+      <c r="A79" s="52"/>
+      <c r="B79" s="46"/>
+      <c r="C79" s="46"/>
+      <c r="D79" s="46"/>
+      <c r="E79" s="46"/>
       <c r="F79" s="30"/>
       <c r="G79" s="35"/>
       <c r="H79" s="35"/>
-      <c r="I79" s="56"/>
-      <c r="J79" s="53"/>
-      <c r="K79" s="56"/>
+      <c r="I79" s="60"/>
+      <c r="J79" s="72"/>
+      <c r="K79" s="60"/>
       <c r="L79" s="2"/>
       <c r="M79" s="2"/>
       <c r="N79" s="2"/>
@@ -3937,21 +4350,21 @@
       <c r="AA79" s="2"/>
     </row>
     <row r="80" spans="1:27">
-      <c r="A80" s="57" t="s">
+      <c r="A80" s="50" t="s">
         <v>48</v>
       </c>
-      <c r="B80" s="45"/>
-      <c r="C80" s="48"/>
-      <c r="D80" s="45"/>
-      <c r="E80" s="45"/>
+      <c r="B80" s="44"/>
+      <c r="C80" s="47"/>
+      <c r="D80" s="44"/>
+      <c r="E80" s="44"/>
       <c r="F80" s="30"/>
       <c r="G80" s="35"/>
       <c r="H80" s="35"/>
-      <c r="I80" s="54" t="s">
+      <c r="I80" s="58" t="s">
         <v>26</v>
       </c>
-      <c r="J80" s="51"/>
-      <c r="K80" s="54" t="s">
+      <c r="J80" s="70"/>
+      <c r="K80" s="58" t="s">
         <v>28</v>
       </c>
       <c r="L80" s="2"/>
@@ -3972,17 +4385,17 @@
       <c r="AA80" s="2"/>
     </row>
     <row r="81" spans="1:27">
-      <c r="A81" s="58"/>
-      <c r="B81" s="46"/>
-      <c r="C81" s="49"/>
-      <c r="D81" s="46"/>
-      <c r="E81" s="46"/>
+      <c r="A81" s="51"/>
+      <c r="B81" s="45"/>
+      <c r="C81" s="48"/>
+      <c r="D81" s="45"/>
+      <c r="E81" s="45"/>
       <c r="F81" s="30"/>
       <c r="G81" s="35"/>
       <c r="H81" s="35"/>
-      <c r="I81" s="55"/>
-      <c r="J81" s="52"/>
-      <c r="K81" s="55"/>
+      <c r="I81" s="59"/>
+      <c r="J81" s="71"/>
+      <c r="K81" s="59"/>
       <c r="L81" s="2"/>
       <c r="M81" s="2"/>
       <c r="N81" s="2"/>
@@ -4001,17 +4414,17 @@
       <c r="AA81" s="2"/>
     </row>
     <row r="82" spans="1:27">
-      <c r="A82" s="58"/>
-      <c r="B82" s="46"/>
-      <c r="C82" s="49"/>
-      <c r="D82" s="46"/>
-      <c r="E82" s="46"/>
+      <c r="A82" s="51"/>
+      <c r="B82" s="45"/>
+      <c r="C82" s="48"/>
+      <c r="D82" s="45"/>
+      <c r="E82" s="45"/>
       <c r="F82" s="30"/>
       <c r="G82" s="35"/>
       <c r="H82" s="35"/>
-      <c r="I82" s="55"/>
-      <c r="J82" s="52"/>
-      <c r="K82" s="55"/>
+      <c r="I82" s="59"/>
+      <c r="J82" s="71"/>
+      <c r="K82" s="59"/>
       <c r="L82" s="2"/>
       <c r="M82" s="2"/>
       <c r="N82" s="2"/>
@@ -4030,17 +4443,17 @@
       <c r="AA82" s="2"/>
     </row>
     <row r="83" spans="1:27">
-      <c r="A83" s="59"/>
-      <c r="B83" s="47"/>
-      <c r="C83" s="50"/>
-      <c r="D83" s="47"/>
-      <c r="E83" s="47"/>
+      <c r="A83" s="52"/>
+      <c r="B83" s="46"/>
+      <c r="C83" s="49"/>
+      <c r="D83" s="46"/>
+      <c r="E83" s="46"/>
       <c r="F83" s="30"/>
       <c r="G83" s="35"/>
       <c r="H83" s="35"/>
-      <c r="I83" s="56"/>
-      <c r="J83" s="53"/>
-      <c r="K83" s="56"/>
+      <c r="I83" s="60"/>
+      <c r="J83" s="72"/>
+      <c r="K83" s="60"/>
       <c r="L83" s="2"/>
       <c r="M83" s="2"/>
       <c r="N83" s="2"/>
@@ -28768,28 +29181,138 @@
     </row>
   </sheetData>
   <mergeCells count="178">
-    <mergeCell ref="C32:C35"/>
-    <mergeCell ref="B32:B35"/>
-    <mergeCell ref="B28:B31"/>
-    <mergeCell ref="C4:C7"/>
-    <mergeCell ref="C8:C11"/>
-    <mergeCell ref="C12:C15"/>
-    <mergeCell ref="C16:C19"/>
-    <mergeCell ref="C20:C23"/>
-    <mergeCell ref="C24:C27"/>
-    <mergeCell ref="C28:C31"/>
-    <mergeCell ref="A4:A7"/>
-    <mergeCell ref="A8:A11"/>
-    <mergeCell ref="A12:A15"/>
-    <mergeCell ref="A16:A19"/>
-    <mergeCell ref="A20:A23"/>
-    <mergeCell ref="A24:A27"/>
-    <mergeCell ref="B24:B27"/>
-    <mergeCell ref="B20:B23"/>
-    <mergeCell ref="B16:B19"/>
-    <mergeCell ref="B12:B15"/>
-    <mergeCell ref="B8:B11"/>
-    <mergeCell ref="B4:B7"/>
+    <mergeCell ref="B36:B39"/>
+    <mergeCell ref="C36:C39"/>
+    <mergeCell ref="D36:D39"/>
+    <mergeCell ref="E36:E39"/>
+    <mergeCell ref="J44:J47"/>
+    <mergeCell ref="K44:K47"/>
+    <mergeCell ref="I48:I51"/>
+    <mergeCell ref="J48:J51"/>
+    <mergeCell ref="K48:K51"/>
+    <mergeCell ref="B48:B51"/>
+    <mergeCell ref="C48:C51"/>
+    <mergeCell ref="D48:D51"/>
+    <mergeCell ref="E48:E51"/>
+    <mergeCell ref="K40:K43"/>
+    <mergeCell ref="I40:I43"/>
+    <mergeCell ref="B40:B43"/>
+    <mergeCell ref="J36:J39"/>
+    <mergeCell ref="C40:C43"/>
+    <mergeCell ref="D40:D43"/>
+    <mergeCell ref="E40:E43"/>
+    <mergeCell ref="A76:A79"/>
+    <mergeCell ref="B76:B79"/>
+    <mergeCell ref="C76:C79"/>
+    <mergeCell ref="D76:D79"/>
+    <mergeCell ref="E76:E79"/>
+    <mergeCell ref="I76:I79"/>
+    <mergeCell ref="J76:J79"/>
+    <mergeCell ref="K76:K79"/>
+    <mergeCell ref="J80:J83"/>
+    <mergeCell ref="K80:K83"/>
+    <mergeCell ref="A80:A83"/>
+    <mergeCell ref="B80:B83"/>
+    <mergeCell ref="C80:C83"/>
+    <mergeCell ref="D80:D83"/>
+    <mergeCell ref="E80:E83"/>
+    <mergeCell ref="I80:I83"/>
+    <mergeCell ref="A60:A63"/>
+    <mergeCell ref="J56:J59"/>
+    <mergeCell ref="K56:K59"/>
+    <mergeCell ref="J60:J63"/>
+    <mergeCell ref="K60:K63"/>
+    <mergeCell ref="I68:I71"/>
+    <mergeCell ref="J68:J71"/>
+    <mergeCell ref="K68:K71"/>
+    <mergeCell ref="A72:A75"/>
+    <mergeCell ref="B72:B75"/>
+    <mergeCell ref="C72:C75"/>
+    <mergeCell ref="D72:D75"/>
+    <mergeCell ref="E72:E75"/>
+    <mergeCell ref="I72:I75"/>
+    <mergeCell ref="J72:J75"/>
+    <mergeCell ref="K72:K75"/>
+    <mergeCell ref="A68:A71"/>
+    <mergeCell ref="B68:B71"/>
+    <mergeCell ref="C68:C71"/>
+    <mergeCell ref="D68:D71"/>
+    <mergeCell ref="E68:E71"/>
+    <mergeCell ref="A64:A67"/>
+    <mergeCell ref="J64:J67"/>
+    <mergeCell ref="K64:K67"/>
+    <mergeCell ref="D2:D3"/>
+    <mergeCell ref="J52:J55"/>
+    <mergeCell ref="K52:K55"/>
+    <mergeCell ref="E52:E55"/>
+    <mergeCell ref="B44:B47"/>
+    <mergeCell ref="C44:C47"/>
+    <mergeCell ref="D44:D47"/>
+    <mergeCell ref="E44:E47"/>
+    <mergeCell ref="B64:B67"/>
+    <mergeCell ref="C64:C67"/>
+    <mergeCell ref="D64:D67"/>
+    <mergeCell ref="E64:E67"/>
+    <mergeCell ref="I64:I67"/>
+    <mergeCell ref="B60:B63"/>
+    <mergeCell ref="C60:C63"/>
+    <mergeCell ref="D60:D63"/>
+    <mergeCell ref="E60:E63"/>
+    <mergeCell ref="I60:I63"/>
+    <mergeCell ref="E56:E59"/>
+    <mergeCell ref="I52:I55"/>
+    <mergeCell ref="B56:B59"/>
+    <mergeCell ref="I56:I59"/>
+    <mergeCell ref="I44:I47"/>
+    <mergeCell ref="J40:J43"/>
+    <mergeCell ref="J32:J35"/>
+    <mergeCell ref="B2:B3"/>
+    <mergeCell ref="A2:A3"/>
+    <mergeCell ref="A52:A55"/>
+    <mergeCell ref="B52:B55"/>
+    <mergeCell ref="C56:C59"/>
+    <mergeCell ref="D56:D59"/>
+    <mergeCell ref="C52:C55"/>
+    <mergeCell ref="D52:D55"/>
+    <mergeCell ref="A44:A47"/>
+    <mergeCell ref="A48:A51"/>
+    <mergeCell ref="D24:D27"/>
+    <mergeCell ref="D20:D23"/>
+    <mergeCell ref="D16:D19"/>
+    <mergeCell ref="D12:D15"/>
+    <mergeCell ref="D8:D11"/>
+    <mergeCell ref="D4:D7"/>
+    <mergeCell ref="A28:A31"/>
+    <mergeCell ref="A32:A35"/>
+    <mergeCell ref="A36:A39"/>
+    <mergeCell ref="A40:A43"/>
+    <mergeCell ref="D32:D35"/>
+    <mergeCell ref="D28:D31"/>
+    <mergeCell ref="A56:A59"/>
+    <mergeCell ref="E32:E35"/>
+    <mergeCell ref="C2:C3"/>
+    <mergeCell ref="H4:H5"/>
+    <mergeCell ref="G4:G5"/>
+    <mergeCell ref="H8:H9"/>
+    <mergeCell ref="H12:H13"/>
+    <mergeCell ref="K32:K35"/>
+    <mergeCell ref="K36:K39"/>
+    <mergeCell ref="J4:J7"/>
+    <mergeCell ref="J8:J11"/>
+    <mergeCell ref="J12:J15"/>
+    <mergeCell ref="J16:J19"/>
+    <mergeCell ref="J20:J23"/>
+    <mergeCell ref="J24:J27"/>
+    <mergeCell ref="J28:J31"/>
+    <mergeCell ref="I32:I35"/>
+    <mergeCell ref="I36:I39"/>
+    <mergeCell ref="K4:K7"/>
+    <mergeCell ref="K8:K11"/>
+    <mergeCell ref="K12:K15"/>
+    <mergeCell ref="K16:K19"/>
+    <mergeCell ref="K20:K23"/>
+    <mergeCell ref="K24:K27"/>
+    <mergeCell ref="J2:J3"/>
     <mergeCell ref="K2:K3"/>
     <mergeCell ref="I4:I7"/>
     <mergeCell ref="I8:I11"/>
@@ -28814,201 +29337,111 @@
     <mergeCell ref="E4:E7"/>
     <mergeCell ref="E8:E11"/>
     <mergeCell ref="E12:E15"/>
-    <mergeCell ref="E32:E35"/>
-    <mergeCell ref="C2:C3"/>
-    <mergeCell ref="H4:H5"/>
-    <mergeCell ref="G4:G5"/>
-    <mergeCell ref="H8:H9"/>
-    <mergeCell ref="H12:H13"/>
-    <mergeCell ref="K32:K35"/>
-    <mergeCell ref="K36:K39"/>
-    <mergeCell ref="J4:J7"/>
-    <mergeCell ref="J8:J11"/>
-    <mergeCell ref="J12:J15"/>
-    <mergeCell ref="J16:J19"/>
-    <mergeCell ref="J20:J23"/>
-    <mergeCell ref="J24:J27"/>
-    <mergeCell ref="J28:J31"/>
-    <mergeCell ref="I32:I35"/>
-    <mergeCell ref="I36:I39"/>
-    <mergeCell ref="K4:K7"/>
-    <mergeCell ref="K8:K11"/>
-    <mergeCell ref="K12:K15"/>
-    <mergeCell ref="K16:K19"/>
-    <mergeCell ref="K20:K23"/>
-    <mergeCell ref="K24:K27"/>
-    <mergeCell ref="J2:J3"/>
-    <mergeCell ref="J32:J35"/>
-    <mergeCell ref="B2:B3"/>
-    <mergeCell ref="A2:A3"/>
-    <mergeCell ref="A52:A55"/>
-    <mergeCell ref="B52:B55"/>
-    <mergeCell ref="C56:C59"/>
-    <mergeCell ref="D56:D59"/>
-    <mergeCell ref="C52:C55"/>
-    <mergeCell ref="D52:D55"/>
-    <mergeCell ref="A44:A47"/>
-    <mergeCell ref="A48:A51"/>
-    <mergeCell ref="D24:D27"/>
-    <mergeCell ref="D20:D23"/>
-    <mergeCell ref="D16:D19"/>
-    <mergeCell ref="D12:D15"/>
-    <mergeCell ref="D8:D11"/>
-    <mergeCell ref="D4:D7"/>
-    <mergeCell ref="A28:A31"/>
-    <mergeCell ref="A32:A35"/>
-    <mergeCell ref="A36:A39"/>
-    <mergeCell ref="A40:A43"/>
-    <mergeCell ref="D32:D35"/>
-    <mergeCell ref="D28:D31"/>
-    <mergeCell ref="A56:A59"/>
-    <mergeCell ref="D2:D3"/>
-    <mergeCell ref="J52:J55"/>
-    <mergeCell ref="K52:K55"/>
-    <mergeCell ref="E52:E55"/>
-    <mergeCell ref="B44:B47"/>
-    <mergeCell ref="C44:C47"/>
-    <mergeCell ref="D44:D47"/>
-    <mergeCell ref="E44:E47"/>
-    <mergeCell ref="B64:B67"/>
-    <mergeCell ref="C64:C67"/>
-    <mergeCell ref="D64:D67"/>
-    <mergeCell ref="E64:E67"/>
-    <mergeCell ref="I64:I67"/>
-    <mergeCell ref="B60:B63"/>
-    <mergeCell ref="C60:C63"/>
-    <mergeCell ref="D60:D63"/>
-    <mergeCell ref="E60:E63"/>
-    <mergeCell ref="I60:I63"/>
-    <mergeCell ref="E56:E59"/>
-    <mergeCell ref="I52:I55"/>
-    <mergeCell ref="B56:B59"/>
-    <mergeCell ref="I56:I59"/>
-    <mergeCell ref="I44:I47"/>
-    <mergeCell ref="J40:J43"/>
-    <mergeCell ref="A60:A63"/>
-    <mergeCell ref="J56:J59"/>
-    <mergeCell ref="K56:K59"/>
-    <mergeCell ref="J60:J63"/>
-    <mergeCell ref="K60:K63"/>
-    <mergeCell ref="I68:I71"/>
-    <mergeCell ref="J68:J71"/>
-    <mergeCell ref="K68:K71"/>
-    <mergeCell ref="A72:A75"/>
-    <mergeCell ref="B72:B75"/>
-    <mergeCell ref="C72:C75"/>
-    <mergeCell ref="D72:D75"/>
-    <mergeCell ref="E72:E75"/>
-    <mergeCell ref="I72:I75"/>
-    <mergeCell ref="J72:J75"/>
-    <mergeCell ref="K72:K75"/>
-    <mergeCell ref="A68:A71"/>
-    <mergeCell ref="B68:B71"/>
-    <mergeCell ref="C68:C71"/>
-    <mergeCell ref="D68:D71"/>
-    <mergeCell ref="E68:E71"/>
-    <mergeCell ref="A64:A67"/>
-    <mergeCell ref="J64:J67"/>
-    <mergeCell ref="K64:K67"/>
-    <mergeCell ref="A76:A79"/>
-    <mergeCell ref="B76:B79"/>
-    <mergeCell ref="C76:C79"/>
-    <mergeCell ref="D76:D79"/>
-    <mergeCell ref="E76:E79"/>
-    <mergeCell ref="I76:I79"/>
-    <mergeCell ref="J76:J79"/>
-    <mergeCell ref="K76:K79"/>
-    <mergeCell ref="J80:J83"/>
-    <mergeCell ref="K80:K83"/>
-    <mergeCell ref="A80:A83"/>
-    <mergeCell ref="B80:B83"/>
-    <mergeCell ref="C80:C83"/>
-    <mergeCell ref="D80:D83"/>
-    <mergeCell ref="E80:E83"/>
-    <mergeCell ref="I80:I83"/>
-    <mergeCell ref="B36:B39"/>
-    <mergeCell ref="C36:C39"/>
-    <mergeCell ref="D36:D39"/>
-    <mergeCell ref="E36:E39"/>
-    <mergeCell ref="J44:J47"/>
-    <mergeCell ref="K44:K47"/>
-    <mergeCell ref="I48:I51"/>
-    <mergeCell ref="J48:J51"/>
-    <mergeCell ref="K48:K51"/>
-    <mergeCell ref="B48:B51"/>
-    <mergeCell ref="C48:C51"/>
-    <mergeCell ref="D48:D51"/>
-    <mergeCell ref="E48:E51"/>
-    <mergeCell ref="K40:K43"/>
-    <mergeCell ref="I40:I43"/>
-    <mergeCell ref="B40:B43"/>
-    <mergeCell ref="J36:J39"/>
-    <mergeCell ref="C40:C43"/>
-    <mergeCell ref="D40:D43"/>
-    <mergeCell ref="E40:E43"/>
+    <mergeCell ref="A4:A7"/>
+    <mergeCell ref="A8:A11"/>
+    <mergeCell ref="A12:A15"/>
+    <mergeCell ref="A16:A19"/>
+    <mergeCell ref="A20:A23"/>
+    <mergeCell ref="A24:A27"/>
+    <mergeCell ref="B24:B27"/>
+    <mergeCell ref="B20:B23"/>
+    <mergeCell ref="B16:B19"/>
+    <mergeCell ref="B12:B15"/>
+    <mergeCell ref="B8:B11"/>
+    <mergeCell ref="B4:B7"/>
+    <mergeCell ref="C32:C35"/>
+    <mergeCell ref="B32:B35"/>
+    <mergeCell ref="B28:B31"/>
+    <mergeCell ref="C4:C7"/>
+    <mergeCell ref="C8:C11"/>
+    <mergeCell ref="C12:C15"/>
+    <mergeCell ref="C16:C19"/>
+    <mergeCell ref="C20:C23"/>
+    <mergeCell ref="C24:C27"/>
+    <mergeCell ref="C28:C31"/>
   </mergeCells>
-  <conditionalFormatting sqref="I28 I32 I36 I40 I44 I48 I52 I56 I60 I64 I68 I72 I76 I80">
-    <cfRule type="cellIs" dxfId="15" priority="109" operator="equal">
+  <conditionalFormatting sqref="I64 I68 I72 I76 I80">
+    <cfRule type="cellIs" dxfId="19" priority="113" operator="equal">
       <formula>"TO DO"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I28 I32 I36 I40 I44 I48 I52 I56 I60 I64 I68 I72 I76 I80">
-    <cfRule type="cellIs" dxfId="14" priority="110" operator="equal">
+  <conditionalFormatting sqref="I64 I68 I72 I76 I80">
+    <cfRule type="cellIs" dxfId="18" priority="114" operator="equal">
       <formula>"IN PROGRESS"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I28 I32 I36 I40 I44 I48 I52 I56 I60 I64 I68 I72 I76 I80">
-    <cfRule type="cellIs" dxfId="13" priority="111" operator="equal">
+  <conditionalFormatting sqref="I64 I68 I72 I76 I80">
+    <cfRule type="cellIs" dxfId="17" priority="115" operator="equal">
       <formula>"REVIEWED"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I28 I32 I36 I40 I44 I48 I52 I56 I60 I64 I68 I72 I76 I80">
-    <cfRule type="cellIs" dxfId="12" priority="112" operator="equal">
+  <conditionalFormatting sqref="I64 I68 I72 I76 I80">
+    <cfRule type="cellIs" dxfId="16" priority="116" operator="equal">
       <formula>"IN REVIEW"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I4 I8 I12">
+    <cfRule type="cellIs" dxfId="15" priority="9" operator="equal">
+      <formula>"TO DO"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I4 I8 I12">
+    <cfRule type="cellIs" dxfId="14" priority="10" operator="equal">
+      <formula>"IN PROGRESS"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I4 I8 I12">
+    <cfRule type="cellIs" dxfId="13" priority="11" operator="equal">
+      <formula>"REVIEWED"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I4 I8 I12">
+    <cfRule type="cellIs" dxfId="12" priority="12" operator="equal">
+      <formula>"IN REVIEW"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I16 I20 I24">
     <cfRule type="cellIs" dxfId="11" priority="5" operator="equal">
       <formula>"TO DO"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I4 I8 I12">
+  <conditionalFormatting sqref="I16 I20 I24">
     <cfRule type="cellIs" dxfId="10" priority="6" operator="equal">
       <formula>"IN PROGRESS"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I4 I8 I12">
+  <conditionalFormatting sqref="I16 I20 I24">
     <cfRule type="cellIs" dxfId="9" priority="7" operator="equal">
       <formula>"REVIEWED"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I4 I8 I12">
+  <conditionalFormatting sqref="I16 I20 I24">
     <cfRule type="cellIs" dxfId="8" priority="8" operator="equal">
       <formula>"IN REVIEW"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I16 I20 I24">
+  <conditionalFormatting sqref="I28 I32 I36 I40 I44 I48 I52 I56 I60">
     <cfRule type="cellIs" dxfId="7" priority="1" operator="equal">
       <formula>"TO DO"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I16 I20 I24">
+  <conditionalFormatting sqref="I28 I32 I36 I40 I44 I48 I52 I56 I60">
     <cfRule type="cellIs" dxfId="5" priority="2" operator="equal">
       <formula>"IN PROGRESS"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I16 I20 I24">
+  <conditionalFormatting sqref="I28 I32 I36 I40 I44 I48 I52 I56 I60">
     <cfRule type="cellIs" dxfId="3" priority="3" operator="equal">
       <formula>"REVIEWED"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I16 I20 I24">
+  <conditionalFormatting sqref="I28 I32 I36 I40 I44 I48 I52 I56 I60">
     <cfRule type="cellIs" dxfId="1" priority="4" operator="equal">
       <formula>"IN REVIEW"</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" sqref="I72 I76 I28 I40 I32 I4 I8 I12 I36 I48 I52 I44 I56 I60 I80 I64 I68 I24 I16 I20">
+    <dataValidation type="list" allowBlank="1" sqref="I72 I76 I24 I16 I20 I4 I8 I12 I80 I64 I68 I32 I36 I28 I40 I44 I48 I52 I56 I60">
       <formula1>"TO DO,In Progress,In Review,Reviewed"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" sqref="K76 K36 K40 K32 K28 K4 K12 K8 K48 K44 K52 K60 K56 K64 K68 K72 K80 K20 K24 K16">

</xml_diff>

<commit_message>
Agrego casos de uso referentes a usabilidad en la web
</commit_message>
<xml_diff>
--- a/Testing 2024/template_caso_prueba-ISPC2024-sprint-1.xlsx
+++ b/Testing 2024/template_caso_prueba-ISPC2024-sprint-1.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="269" uniqueCount="130">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="285" uniqueCount="138">
   <si>
     <t>Id</t>
   </si>
@@ -416,6 +416,30 @@
   <si>
     <t>Un nuevo usuario intenta registrarse con un email que no cumplen con el formato correcto</t>
   </si>
+  <si>
+    <t>Acceder a la pantalla "Contactanos"</t>
+  </si>
+  <si>
+    <t>El usuario accede a la pantalla de "Contactanos" desde el navbar de la Homepage</t>
+  </si>
+  <si>
+    <t>Hacer click en "Contactanos" en la navbar de la home page</t>
+  </si>
+  <si>
+    <t>Deberá redirigirse al usuario a la página donde se muestren las maneras de contactarse y un formulario de contacto</t>
+  </si>
+  <si>
+    <t>Acceder a la pantalla "Sobre Nosotros"</t>
+  </si>
+  <si>
+    <t>El usuario accede a la pantalla de "Sobre Nosotros" desde el navbar de la Homepage</t>
+  </si>
+  <si>
+    <t>Hacer click en "Sobre Nosotros" en la navbar de la home page</t>
+  </si>
+  <si>
+    <t>Deberá redirigirse al usuario a la página donde se visualiza la información de Librería Franklin</t>
+  </si>
 </sst>
 </file>
 
@@ -491,7 +515,7 @@
       <name val="ArialMT"/>
     </font>
   </fonts>
-  <fills count="13">
+  <fills count="14">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -561,6 +585,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor rgb="FFFFFFCC"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.79998168889431442"/>
         <bgColor rgb="FFFFFFCC"/>
       </patternFill>
     </fill>
@@ -835,7 +865,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="76">
+  <cellXfs count="79">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -939,6 +969,29 @@
     <xf numFmtId="0" fontId="1" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="11" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -948,22 +1001,13 @@
     <xf numFmtId="0" fontId="10" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="10" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="12" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="10" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="12" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="10" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="11" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="11" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="11" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="12" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -972,11 +1016,18 @@
     <xf numFmtId="0" fontId="7" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -992,41 +1043,29 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="11" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="11" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="12" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="11" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="12" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="13" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="12" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="13" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="13" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="20">
+  <dxfs count="24">
     <dxf>
       <fill>
         <patternFill patternType="solid">
@@ -1080,6 +1119,38 @@
         <patternFill patternType="solid">
           <fgColor rgb="FFA2C4C9"/>
           <bgColor rgb="FFA2C4C9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFA2C4C9"/>
+          <bgColor rgb="FFA2C4C9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFCE5CD"/>
+          <bgColor rgb="FFFCE5CD"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF93C47D"/>
+          <bgColor rgb="FF93C47D"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFF2CC"/>
+          <bgColor rgb="FFFFF2CC"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1536,8 +1607,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AA935"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A50" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="60" workbookViewId="0">
-      <selection activeCell="D56" sqref="D56:D59"/>
+    <sheetView tabSelected="1" topLeftCell="A61" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="60" workbookViewId="0">
+      <selection activeCell="D72" sqref="D72:D75"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5703125" defaultRowHeight="12.75"/>
@@ -1586,33 +1657,33 @@
       <c r="AA1" s="2"/>
     </row>
     <row r="2" spans="1:27" s="31" customFormat="1" ht="15.75" customHeight="1">
-      <c r="A2" s="66" t="s">
+      <c r="A2" s="64" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="56" t="s">
+      <c r="B2" s="62" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="66" t="s">
+      <c r="C2" s="64" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="56" t="s">
+      <c r="D2" s="62" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="56" t="s">
+      <c r="E2" s="62" t="s">
         <v>4</v>
       </c>
-      <c r="F2" s="61" t="s">
+      <c r="F2" s="68" t="s">
         <v>5</v>
       </c>
-      <c r="G2" s="62"/>
-      <c r="H2" s="63"/>
-      <c r="I2" s="64" t="s">
+      <c r="G2" s="69"/>
+      <c r="H2" s="70"/>
+      <c r="I2" s="71" t="s">
         <v>6</v>
       </c>
-      <c r="J2" s="56" t="s">
+      <c r="J2" s="62" t="s">
         <v>7</v>
       </c>
-      <c r="K2" s="56" t="s">
+      <c r="K2" s="62" t="s">
         <v>27</v>
       </c>
       <c r="L2" s="32"/>
@@ -1633,11 +1704,11 @@
       <c r="AA2" s="33"/>
     </row>
     <row r="3" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A3" s="67"/>
-      <c r="B3" s="57"/>
-      <c r="C3" s="67"/>
-      <c r="D3" s="57"/>
-      <c r="E3" s="57"/>
+      <c r="A3" s="65"/>
+      <c r="B3" s="63"/>
+      <c r="C3" s="65"/>
+      <c r="D3" s="63"/>
+      <c r="E3" s="63"/>
       <c r="F3" s="34" t="s">
         <v>8</v>
       </c>
@@ -1647,9 +1718,9 @@
       <c r="H3" s="42" t="s">
         <v>10</v>
       </c>
-      <c r="I3" s="65"/>
-      <c r="J3" s="57"/>
-      <c r="K3" s="57"/>
+      <c r="I3" s="72"/>
+      <c r="J3" s="63"/>
+      <c r="K3" s="63"/>
       <c r="L3" s="3"/>
       <c r="M3" s="2"/>
       <c r="N3" s="2"/>
@@ -1668,7 +1739,7 @@
       <c r="AA3" s="2"/>
     </row>
     <row r="4" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A4" s="50" t="s">
+      <c r="A4" s="53" t="s">
         <v>29</v>
       </c>
       <c r="B4" s="44" t="s">
@@ -1689,16 +1760,16 @@
       <c r="G4" s="44" t="s">
         <v>54</v>
       </c>
-      <c r="H4" s="68" t="s">
+      <c r="H4" s="66" t="s">
         <v>55</v>
       </c>
-      <c r="I4" s="58" t="s">
+      <c r="I4" s="50" t="s">
         <v>26</v>
       </c>
-      <c r="J4" s="70" t="s">
+      <c r="J4" s="47" t="s">
         <v>56</v>
       </c>
-      <c r="K4" s="58" t="s">
+      <c r="K4" s="50" t="s">
         <v>28</v>
       </c>
       <c r="L4" s="3"/>
@@ -1719,17 +1790,17 @@
       <c r="AA4" s="2"/>
     </row>
     <row r="5" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A5" s="51"/>
+      <c r="A5" s="54"/>
       <c r="B5" s="45"/>
       <c r="C5" s="45"/>
       <c r="D5" s="45"/>
       <c r="E5" s="45"/>
       <c r="F5" s="46"/>
       <c r="G5" s="46"/>
-      <c r="H5" s="69"/>
-      <c r="I5" s="59"/>
-      <c r="J5" s="71"/>
-      <c r="K5" s="59"/>
+      <c r="H5" s="67"/>
+      <c r="I5" s="51"/>
+      <c r="J5" s="48"/>
+      <c r="K5" s="51"/>
       <c r="L5" s="3"/>
       <c r="M5" s="2"/>
       <c r="N5" s="2"/>
@@ -1748,7 +1819,7 @@
       <c r="AA5" s="2"/>
     </row>
     <row r="6" spans="1:27" s="29" customFormat="1" ht="15.75" customHeight="1">
-      <c r="A6" s="51"/>
+      <c r="A6" s="54"/>
       <c r="B6" s="45"/>
       <c r="C6" s="45"/>
       <c r="D6" s="45"/>
@@ -1756,9 +1827,9 @@
       <c r="F6" s="30"/>
       <c r="G6" s="35"/>
       <c r="H6" s="35"/>
-      <c r="I6" s="59"/>
-      <c r="J6" s="71"/>
-      <c r="K6" s="59"/>
+      <c r="I6" s="51"/>
+      <c r="J6" s="48"/>
+      <c r="K6" s="51"/>
       <c r="L6" s="27"/>
       <c r="M6" s="28"/>
       <c r="N6" s="28"/>
@@ -1777,7 +1848,7 @@
       <c r="AA6" s="28"/>
     </row>
     <row r="7" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A7" s="52"/>
+      <c r="A7" s="55"/>
       <c r="B7" s="46"/>
       <c r="C7" s="46"/>
       <c r="D7" s="46"/>
@@ -1785,9 +1856,9 @@
       <c r="F7" s="30"/>
       <c r="G7" s="35"/>
       <c r="H7" s="35"/>
-      <c r="I7" s="60"/>
-      <c r="J7" s="72"/>
-      <c r="K7" s="60"/>
+      <c r="I7" s="52"/>
+      <c r="J7" s="49"/>
+      <c r="K7" s="52"/>
       <c r="L7" s="3"/>
       <c r="M7" s="2"/>
       <c r="N7" s="2"/>
@@ -1806,7 +1877,7 @@
       <c r="AA7" s="2"/>
     </row>
     <row r="8" spans="1:27">
-      <c r="A8" s="50" t="s">
+      <c r="A8" s="53" t="s">
         <v>30</v>
       </c>
       <c r="B8" s="44" t="s">
@@ -1827,16 +1898,16 @@
       <c r="G8" s="44" t="s">
         <v>54</v>
       </c>
-      <c r="H8" s="68" t="s">
+      <c r="H8" s="66" t="s">
         <v>55</v>
       </c>
-      <c r="I8" s="58" t="s">
+      <c r="I8" s="50" t="s">
         <v>26</v>
       </c>
-      <c r="J8" s="70" t="s">
+      <c r="J8" s="47" t="s">
         <v>56</v>
       </c>
-      <c r="K8" s="58" t="s">
+      <c r="K8" s="50" t="s">
         <v>28</v>
       </c>
       <c r="L8" s="3"/>
@@ -1857,17 +1928,17 @@
       <c r="AA8" s="2"/>
     </row>
     <row r="9" spans="1:27">
-      <c r="A9" s="51"/>
+      <c r="A9" s="54"/>
       <c r="B9" s="45"/>
       <c r="C9" s="45"/>
       <c r="D9" s="45"/>
       <c r="E9" s="45"/>
       <c r="F9" s="46"/>
       <c r="G9" s="46"/>
-      <c r="H9" s="69"/>
-      <c r="I9" s="59"/>
-      <c r="J9" s="71"/>
-      <c r="K9" s="59"/>
+      <c r="H9" s="67"/>
+      <c r="I9" s="51"/>
+      <c r="J9" s="48"/>
+      <c r="K9" s="51"/>
       <c r="L9" s="3"/>
       <c r="M9" s="2"/>
       <c r="N9" s="2"/>
@@ -1886,7 +1957,7 @@
       <c r="AA9" s="2"/>
     </row>
     <row r="10" spans="1:27" s="29" customFormat="1" ht="15.75" customHeight="1">
-      <c r="A10" s="51"/>
+      <c r="A10" s="54"/>
       <c r="B10" s="45"/>
       <c r="C10" s="45"/>
       <c r="D10" s="45"/>
@@ -1894,9 +1965,9 @@
       <c r="F10" s="30"/>
       <c r="G10" s="35"/>
       <c r="H10" s="35"/>
-      <c r="I10" s="59"/>
-      <c r="J10" s="71"/>
-      <c r="K10" s="59"/>
+      <c r="I10" s="51"/>
+      <c r="J10" s="48"/>
+      <c r="K10" s="51"/>
       <c r="L10" s="27"/>
       <c r="M10" s="28"/>
       <c r="N10" s="28"/>
@@ -1915,7 +1986,7 @@
       <c r="AA10" s="28"/>
     </row>
     <row r="11" spans="1:27">
-      <c r="A11" s="52"/>
+      <c r="A11" s="55"/>
       <c r="B11" s="46"/>
       <c r="C11" s="46"/>
       <c r="D11" s="46"/>
@@ -1923,9 +1994,9 @@
       <c r="F11" s="30"/>
       <c r="G11" s="35"/>
       <c r="H11" s="35"/>
-      <c r="I11" s="60"/>
-      <c r="J11" s="72"/>
-      <c r="K11" s="60"/>
+      <c r="I11" s="52"/>
+      <c r="J11" s="49"/>
+      <c r="K11" s="52"/>
       <c r="L11" s="3"/>
       <c r="M11" s="2"/>
       <c r="N11" s="2"/>
@@ -1944,7 +2015,7 @@
       <c r="AA11" s="2"/>
     </row>
     <row r="12" spans="1:27">
-      <c r="A12" s="50" t="s">
+      <c r="A12" s="53" t="s">
         <v>31</v>
       </c>
       <c r="B12" s="44" t="s">
@@ -1965,16 +2036,16 @@
       <c r="G12" s="44" t="s">
         <v>54</v>
       </c>
-      <c r="H12" s="68" t="s">
+      <c r="H12" s="66" t="s">
         <v>55</v>
       </c>
-      <c r="I12" s="58" t="s">
+      <c r="I12" s="50" t="s">
         <v>26</v>
       </c>
-      <c r="J12" s="70" t="s">
+      <c r="J12" s="47" t="s">
         <v>56</v>
       </c>
-      <c r="K12" s="58" t="s">
+      <c r="K12" s="50" t="s">
         <v>28</v>
       </c>
       <c r="L12" s="2"/>
@@ -1995,17 +2066,17 @@
       <c r="AA12" s="2"/>
     </row>
     <row r="13" spans="1:27">
-      <c r="A13" s="51"/>
+      <c r="A13" s="54"/>
       <c r="B13" s="45"/>
       <c r="C13" s="45"/>
       <c r="D13" s="45"/>
       <c r="E13" s="45"/>
       <c r="F13" s="46"/>
       <c r="G13" s="46"/>
-      <c r="H13" s="69"/>
-      <c r="I13" s="59"/>
-      <c r="J13" s="71"/>
-      <c r="K13" s="59"/>
+      <c r="H13" s="67"/>
+      <c r="I13" s="51"/>
+      <c r="J13" s="48"/>
+      <c r="K13" s="51"/>
       <c r="L13" s="2"/>
       <c r="M13" s="2"/>
       <c r="N13" s="2"/>
@@ -2024,7 +2095,7 @@
       <c r="AA13" s="2"/>
     </row>
     <row r="14" spans="1:27" s="29" customFormat="1">
-      <c r="A14" s="51"/>
+      <c r="A14" s="54"/>
       <c r="B14" s="45"/>
       <c r="C14" s="45"/>
       <c r="D14" s="45"/>
@@ -2032,9 +2103,9 @@
       <c r="F14" s="30"/>
       <c r="G14" s="35"/>
       <c r="H14" s="35"/>
-      <c r="I14" s="59"/>
-      <c r="J14" s="71"/>
-      <c r="K14" s="59"/>
+      <c r="I14" s="51"/>
+      <c r="J14" s="48"/>
+      <c r="K14" s="51"/>
       <c r="L14" s="28"/>
       <c r="M14" s="28"/>
       <c r="N14" s="28"/>
@@ -2053,7 +2124,7 @@
       <c r="AA14" s="28"/>
     </row>
     <row r="15" spans="1:27">
-      <c r="A15" s="52"/>
+      <c r="A15" s="55"/>
       <c r="B15" s="46"/>
       <c r="C15" s="46"/>
       <c r="D15" s="46"/>
@@ -2061,9 +2132,9 @@
       <c r="F15" s="30"/>
       <c r="G15" s="35"/>
       <c r="H15" s="35"/>
-      <c r="I15" s="60"/>
-      <c r="J15" s="72"/>
-      <c r="K15" s="60"/>
+      <c r="I15" s="52"/>
+      <c r="J15" s="49"/>
+      <c r="K15" s="52"/>
       <c r="L15" s="2"/>
       <c r="M15" s="2"/>
       <c r="N15" s="2"/>
@@ -2082,7 +2153,7 @@
       <c r="AA15" s="2"/>
     </row>
     <row r="16" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A16" s="53" t="s">
+      <c r="A16" s="73" t="s">
         <v>32</v>
       </c>
       <c r="B16" s="44" t="s">
@@ -2106,13 +2177,13 @@
       <c r="H16" s="35" t="s">
         <v>66</v>
       </c>
-      <c r="I16" s="58" t="s">
+      <c r="I16" s="50" t="s">
         <v>26</v>
       </c>
-      <c r="J16" s="70" t="s">
+      <c r="J16" s="47" t="s">
         <v>56</v>
       </c>
-      <c r="K16" s="58" t="s">
+      <c r="K16" s="50" t="s">
         <v>28</v>
       </c>
       <c r="L16" s="2"/>
@@ -2133,7 +2204,7 @@
       <c r="AA16" s="2"/>
     </row>
     <row r="17" spans="1:27" ht="16.5" customHeight="1">
-      <c r="A17" s="54"/>
+      <c r="A17" s="74"/>
       <c r="B17" s="45"/>
       <c r="C17" s="45"/>
       <c r="D17" s="45"/>
@@ -2147,9 +2218,9 @@
       <c r="H17" s="35" t="s">
         <v>69</v>
       </c>
-      <c r="I17" s="59"/>
-      <c r="J17" s="71"/>
-      <c r="K17" s="59"/>
+      <c r="I17" s="51"/>
+      <c r="J17" s="48"/>
+      <c r="K17" s="51"/>
       <c r="L17" s="2"/>
       <c r="M17" s="2"/>
       <c r="N17" s="2"/>
@@ -2168,7 +2239,7 @@
       <c r="AA17" s="2"/>
     </row>
     <row r="18" spans="1:27" s="29" customFormat="1" ht="25.5">
-      <c r="A18" s="54"/>
+      <c r="A18" s="74"/>
       <c r="B18" s="45"/>
       <c r="C18" s="45"/>
       <c r="D18" s="45"/>
@@ -2182,9 +2253,9 @@
       <c r="H18" s="35" t="s">
         <v>72</v>
       </c>
-      <c r="I18" s="59"/>
-      <c r="J18" s="71"/>
-      <c r="K18" s="59"/>
+      <c r="I18" s="51"/>
+      <c r="J18" s="48"/>
+      <c r="K18" s="51"/>
       <c r="L18" s="28"/>
       <c r="M18" s="28"/>
       <c r="N18" s="28"/>
@@ -2203,7 +2274,7 @@
       <c r="AA18" s="28"/>
     </row>
     <row r="19" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A19" s="55"/>
+      <c r="A19" s="75"/>
       <c r="B19" s="46"/>
       <c r="C19" s="46"/>
       <c r="D19" s="46"/>
@@ -2211,9 +2282,9 @@
       <c r="F19" s="30"/>
       <c r="G19" s="35"/>
       <c r="H19" s="35"/>
-      <c r="I19" s="60"/>
-      <c r="J19" s="72"/>
-      <c r="K19" s="60"/>
+      <c r="I19" s="52"/>
+      <c r="J19" s="49"/>
+      <c r="K19" s="52"/>
       <c r="L19" s="2"/>
       <c r="M19" s="2"/>
       <c r="N19" s="2"/>
@@ -2232,13 +2303,13 @@
       <c r="AA19" s="2"/>
     </row>
     <row r="20" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A20" s="53" t="s">
+      <c r="A20" s="73" t="s">
         <v>33</v>
       </c>
       <c r="B20" s="44" t="s">
         <v>63</v>
       </c>
-      <c r="C20" s="47" t="s">
+      <c r="C20" s="56" t="s">
         <v>73</v>
       </c>
       <c r="D20" s="44" t="s">
@@ -2256,13 +2327,13 @@
       <c r="H20" s="35" t="s">
         <v>76</v>
       </c>
-      <c r="I20" s="58" t="s">
+      <c r="I20" s="50" t="s">
         <v>26</v>
       </c>
-      <c r="J20" s="70" t="s">
+      <c r="J20" s="47" t="s">
         <v>56</v>
       </c>
-      <c r="K20" s="58" t="s">
+      <c r="K20" s="50" t="s">
         <v>28</v>
       </c>
       <c r="L20" s="2"/>
@@ -2283,9 +2354,9 @@
       <c r="AA20" s="2"/>
     </row>
     <row r="21" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A21" s="54"/>
+      <c r="A21" s="74"/>
       <c r="B21" s="45"/>
-      <c r="C21" s="48"/>
+      <c r="C21" s="57"/>
       <c r="D21" s="45"/>
       <c r="E21" s="45"/>
       <c r="F21" s="30" t="s">
@@ -2295,9 +2366,9 @@
         <v>77</v>
       </c>
       <c r="H21" s="35"/>
-      <c r="I21" s="59"/>
-      <c r="J21" s="71"/>
-      <c r="K21" s="59"/>
+      <c r="I21" s="51"/>
+      <c r="J21" s="48"/>
+      <c r="K21" s="51"/>
       <c r="L21" s="2"/>
       <c r="M21" s="2"/>
       <c r="N21" s="2"/>
@@ -2316,9 +2387,9 @@
       <c r="AA21" s="2"/>
     </row>
     <row r="22" spans="1:27" s="29" customFormat="1" ht="15.75" customHeight="1">
-      <c r="A22" s="54"/>
+      <c r="A22" s="74"/>
       <c r="B22" s="45"/>
-      <c r="C22" s="48"/>
+      <c r="C22" s="57"/>
       <c r="D22" s="45"/>
       <c r="E22" s="45"/>
       <c r="F22" s="30" t="s">
@@ -2330,9 +2401,9 @@
       <c r="H22" s="35" t="s">
         <v>79</v>
       </c>
-      <c r="I22" s="59"/>
-      <c r="J22" s="71"/>
-      <c r="K22" s="59"/>
+      <c r="I22" s="51"/>
+      <c r="J22" s="48"/>
+      <c r="K22" s="51"/>
       <c r="L22" s="28"/>
       <c r="M22" s="28"/>
       <c r="N22" s="28"/>
@@ -2351,17 +2422,17 @@
       <c r="AA22" s="28"/>
     </row>
     <row r="23" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A23" s="55"/>
+      <c r="A23" s="75"/>
       <c r="B23" s="46"/>
-      <c r="C23" s="49"/>
+      <c r="C23" s="58"/>
       <c r="D23" s="46"/>
       <c r="E23" s="46"/>
       <c r="F23" s="30"/>
       <c r="G23" s="35"/>
       <c r="H23" s="35"/>
-      <c r="I23" s="60"/>
-      <c r="J23" s="72"/>
-      <c r="K23" s="60"/>
+      <c r="I23" s="52"/>
+      <c r="J23" s="49"/>
+      <c r="K23" s="52"/>
       <c r="L23" s="2"/>
       <c r="M23" s="2"/>
       <c r="N23" s="2"/>
@@ -2380,13 +2451,13 @@
       <c r="AA23" s="2"/>
     </row>
     <row r="24" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A24" s="53" t="s">
+      <c r="A24" s="73" t="s">
         <v>34</v>
       </c>
       <c r="B24" s="44" t="s">
         <v>63</v>
       </c>
-      <c r="C24" s="47" t="s">
+      <c r="C24" s="56" t="s">
         <v>80</v>
       </c>
       <c r="D24" s="44" t="s">
@@ -2404,13 +2475,13 @@
       <c r="H24" s="35" t="s">
         <v>76</v>
       </c>
-      <c r="I24" s="58" t="s">
+      <c r="I24" s="50" t="s">
         <v>26</v>
       </c>
-      <c r="J24" s="70" t="s">
+      <c r="J24" s="47" t="s">
         <v>56</v>
       </c>
-      <c r="K24" s="58" t="s">
+      <c r="K24" s="50" t="s">
         <v>28</v>
       </c>
       <c r="L24" s="2"/>
@@ -2431,9 +2502,9 @@
       <c r="AA24" s="2"/>
     </row>
     <row r="25" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A25" s="54"/>
+      <c r="A25" s="74"/>
       <c r="B25" s="45"/>
-      <c r="C25" s="48"/>
+      <c r="C25" s="57"/>
       <c r="D25" s="45"/>
       <c r="E25" s="45"/>
       <c r="F25" s="30" t="s">
@@ -2443,9 +2514,9 @@
         <v>77</v>
       </c>
       <c r="H25" s="35"/>
-      <c r="I25" s="59"/>
-      <c r="J25" s="71"/>
-      <c r="K25" s="59"/>
+      <c r="I25" s="51"/>
+      <c r="J25" s="48"/>
+      <c r="K25" s="51"/>
       <c r="L25" s="2"/>
       <c r="M25" s="2"/>
       <c r="N25" s="2"/>
@@ -2464,9 +2535,9 @@
       <c r="AA25" s="2"/>
     </row>
     <row r="26" spans="1:27" s="29" customFormat="1" ht="25.5">
-      <c r="A26" s="54"/>
+      <c r="A26" s="74"/>
       <c r="B26" s="45"/>
-      <c r="C26" s="48"/>
+      <c r="C26" s="57"/>
       <c r="D26" s="45"/>
       <c r="E26" s="45"/>
       <c r="F26" s="30" t="s">
@@ -2478,9 +2549,9 @@
       <c r="H26" s="35" t="s">
         <v>82</v>
       </c>
-      <c r="I26" s="59"/>
-      <c r="J26" s="71"/>
-      <c r="K26" s="59"/>
+      <c r="I26" s="51"/>
+      <c r="J26" s="48"/>
+      <c r="K26" s="51"/>
       <c r="L26" s="28"/>
       <c r="M26" s="28"/>
       <c r="N26" s="28"/>
@@ -2499,17 +2570,17 @@
       <c r="AA26" s="28"/>
     </row>
     <row r="27" spans="1:27" ht="18.75" customHeight="1">
-      <c r="A27" s="55"/>
+      <c r="A27" s="75"/>
       <c r="B27" s="46"/>
-      <c r="C27" s="49"/>
+      <c r="C27" s="58"/>
       <c r="D27" s="46"/>
       <c r="E27" s="46"/>
       <c r="F27" s="30"/>
       <c r="G27" s="35"/>
       <c r="H27" s="35"/>
-      <c r="I27" s="60"/>
-      <c r="J27" s="72"/>
-      <c r="K27" s="60"/>
+      <c r="I27" s="52"/>
+      <c r="J27" s="49"/>
+      <c r="K27" s="52"/>
       <c r="L27" s="2"/>
       <c r="M27" s="2"/>
       <c r="N27" s="2"/>
@@ -2528,7 +2599,7 @@
       <c r="AA27" s="2"/>
     </row>
     <row r="28" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A28" s="73" t="s">
+      <c r="A28" s="59" t="s">
         <v>35</v>
       </c>
       <c r="B28" s="44" t="s">
@@ -2552,13 +2623,13 @@
       <c r="H28" s="35" t="s">
         <v>88</v>
       </c>
-      <c r="I28" s="58" t="s">
+      <c r="I28" s="50" t="s">
         <v>26</v>
       </c>
-      <c r="J28" s="70" t="s">
+      <c r="J28" s="47" t="s">
         <v>56</v>
       </c>
-      <c r="K28" s="58" t="s">
+      <c r="K28" s="50" t="s">
         <v>28</v>
       </c>
       <c r="L28" s="2"/>
@@ -2579,7 +2650,7 @@
       <c r="AA28" s="2"/>
     </row>
     <row r="29" spans="1:27">
-      <c r="A29" s="74"/>
+      <c r="A29" s="60"/>
       <c r="B29" s="45"/>
       <c r="C29" s="45"/>
       <c r="D29" s="45"/>
@@ -2589,9 +2660,9 @@
       </c>
       <c r="G29" s="35"/>
       <c r="H29" s="35"/>
-      <c r="I29" s="59"/>
-      <c r="J29" s="71"/>
-      <c r="K29" s="59"/>
+      <c r="I29" s="51"/>
+      <c r="J29" s="48"/>
+      <c r="K29" s="51"/>
       <c r="L29" s="2"/>
       <c r="M29" s="2"/>
       <c r="N29" s="2"/>
@@ -2610,7 +2681,7 @@
       <c r="AA29" s="2"/>
     </row>
     <row r="30" spans="1:27" s="29" customFormat="1" ht="15.75" customHeight="1">
-      <c r="A30" s="74"/>
+      <c r="A30" s="60"/>
       <c r="B30" s="45"/>
       <c r="C30" s="45"/>
       <c r="D30" s="45"/>
@@ -2618,9 +2689,9 @@
       <c r="F30" s="30"/>
       <c r="G30" s="35"/>
       <c r="H30" s="35"/>
-      <c r="I30" s="59"/>
-      <c r="J30" s="71"/>
-      <c r="K30" s="59"/>
+      <c r="I30" s="51"/>
+      <c r="J30" s="48"/>
+      <c r="K30" s="51"/>
       <c r="L30" s="28"/>
       <c r="M30" s="28"/>
       <c r="N30" s="28"/>
@@ -2639,7 +2710,7 @@
       <c r="AA30" s="28"/>
     </row>
     <row r="31" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A31" s="75"/>
+      <c r="A31" s="61"/>
       <c r="B31" s="46"/>
       <c r="C31" s="46"/>
       <c r="D31" s="46"/>
@@ -2647,9 +2718,9 @@
       <c r="F31" s="30"/>
       <c r="G31" s="35"/>
       <c r="H31" s="35"/>
-      <c r="I31" s="60"/>
-      <c r="J31" s="72"/>
-      <c r="K31" s="60"/>
+      <c r="I31" s="52"/>
+      <c r="J31" s="49"/>
+      <c r="K31" s="52"/>
       <c r="L31" s="2"/>
       <c r="M31" s="2"/>
       <c r="N31" s="2"/>
@@ -2668,7 +2739,7 @@
       <c r="AA31" s="2"/>
     </row>
     <row r="32" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A32" s="73" t="s">
+      <c r="A32" s="59" t="s">
         <v>36</v>
       </c>
       <c r="B32" s="44" t="s">
@@ -2692,13 +2763,13 @@
       <c r="H32" s="35" t="s">
         <v>92</v>
       </c>
-      <c r="I32" s="58" t="s">
+      <c r="I32" s="50" t="s">
         <v>26</v>
       </c>
-      <c r="J32" s="70" t="s">
+      <c r="J32" s="47" t="s">
         <v>56</v>
       </c>
-      <c r="K32" s="58" t="s">
+      <c r="K32" s="50" t="s">
         <v>28</v>
       </c>
       <c r="L32" s="2"/>
@@ -2719,7 +2790,7 @@
       <c r="AA32" s="2"/>
     </row>
     <row r="33" spans="1:27">
-      <c r="A33" s="74"/>
+      <c r="A33" s="60"/>
       <c r="B33" s="45"/>
       <c r="C33" s="45"/>
       <c r="D33" s="45"/>
@@ -2727,9 +2798,9 @@
       <c r="F33" s="30"/>
       <c r="G33" s="43"/>
       <c r="H33" s="43"/>
-      <c r="I33" s="59"/>
-      <c r="J33" s="71"/>
-      <c r="K33" s="59"/>
+      <c r="I33" s="51"/>
+      <c r="J33" s="48"/>
+      <c r="K33" s="51"/>
       <c r="L33" s="2"/>
       <c r="M33" s="2"/>
       <c r="N33" s="2"/>
@@ -2748,7 +2819,7 @@
       <c r="AA33" s="2"/>
     </row>
     <row r="34" spans="1:27">
-      <c r="A34" s="74"/>
+      <c r="A34" s="60"/>
       <c r="B34" s="45"/>
       <c r="C34" s="45"/>
       <c r="D34" s="45"/>
@@ -2756,9 +2827,9 @@
       <c r="F34" s="30"/>
       <c r="G34" s="43"/>
       <c r="H34" s="43"/>
-      <c r="I34" s="59"/>
-      <c r="J34" s="71"/>
-      <c r="K34" s="59"/>
+      <c r="I34" s="51"/>
+      <c r="J34" s="48"/>
+      <c r="K34" s="51"/>
       <c r="L34" s="2"/>
       <c r="M34" s="2"/>
       <c r="N34" s="2"/>
@@ -2777,7 +2848,7 @@
       <c r="AA34" s="2"/>
     </row>
     <row r="35" spans="1:27">
-      <c r="A35" s="75"/>
+      <c r="A35" s="61"/>
       <c r="B35" s="46"/>
       <c r="C35" s="46"/>
       <c r="D35" s="46"/>
@@ -2785,9 +2856,9 @@
       <c r="F35" s="30"/>
       <c r="G35" s="35"/>
       <c r="H35" s="35"/>
-      <c r="I35" s="60"/>
-      <c r="J35" s="72"/>
-      <c r="K35" s="60"/>
+      <c r="I35" s="52"/>
+      <c r="J35" s="49"/>
+      <c r="K35" s="52"/>
       <c r="L35" s="2"/>
       <c r="M35" s="2"/>
       <c r="N35" s="2"/>
@@ -2806,7 +2877,7 @@
       <c r="AA35" s="2"/>
     </row>
     <row r="36" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A36" s="73" t="s">
+      <c r="A36" s="59" t="s">
         <v>37</v>
       </c>
       <c r="B36" s="44" t="s">
@@ -2830,13 +2901,13 @@
       <c r="H36" s="35" t="s">
         <v>92</v>
       </c>
-      <c r="I36" s="58" t="s">
+      <c r="I36" s="50" t="s">
         <v>26</v>
       </c>
-      <c r="J36" s="70" t="s">
+      <c r="J36" s="47" t="s">
         <v>56</v>
       </c>
-      <c r="K36" s="58" t="s">
+      <c r="K36" s="50" t="s">
         <v>28</v>
       </c>
       <c r="L36" s="2"/>
@@ -2857,7 +2928,7 @@
       <c r="AA36" s="2"/>
     </row>
     <row r="37" spans="1:27" ht="25.5">
-      <c r="A37" s="74"/>
+      <c r="A37" s="60"/>
       <c r="B37" s="45"/>
       <c r="C37" s="45"/>
       <c r="D37" s="45"/>
@@ -2869,9 +2940,9 @@
         <v>96</v>
       </c>
       <c r="H37" s="35"/>
-      <c r="I37" s="59"/>
-      <c r="J37" s="71"/>
-      <c r="K37" s="59"/>
+      <c r="I37" s="51"/>
+      <c r="J37" s="48"/>
+      <c r="K37" s="51"/>
       <c r="L37" s="2"/>
       <c r="M37" s="2"/>
       <c r="N37" s="2"/>
@@ -2890,7 +2961,7 @@
       <c r="AA37" s="2"/>
     </row>
     <row r="38" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A38" s="74"/>
+      <c r="A38" s="60"/>
       <c r="B38" s="45"/>
       <c r="C38" s="45"/>
       <c r="D38" s="45"/>
@@ -2904,9 +2975,9 @@
       <c r="H38" s="35" t="s">
         <v>98</v>
       </c>
-      <c r="I38" s="59"/>
-      <c r="J38" s="71"/>
-      <c r="K38" s="59"/>
+      <c r="I38" s="51"/>
+      <c r="J38" s="48"/>
+      <c r="K38" s="51"/>
       <c r="L38" s="2"/>
       <c r="M38" s="2"/>
       <c r="N38" s="2"/>
@@ -2925,7 +2996,7 @@
       <c r="AA38" s="2"/>
     </row>
     <row r="39" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A39" s="75"/>
+      <c r="A39" s="61"/>
       <c r="B39" s="46"/>
       <c r="C39" s="46"/>
       <c r="D39" s="46"/>
@@ -2935,9 +3006,9 @@
       </c>
       <c r="G39" s="35"/>
       <c r="H39" s="35"/>
-      <c r="I39" s="60"/>
-      <c r="J39" s="72"/>
-      <c r="K39" s="60"/>
+      <c r="I39" s="52"/>
+      <c r="J39" s="49"/>
+      <c r="K39" s="52"/>
       <c r="L39" s="2"/>
       <c r="M39" s="2"/>
       <c r="N39" s="2"/>
@@ -2956,7 +3027,7 @@
       <c r="AA39" s="2"/>
     </row>
     <row r="40" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A40" s="73" t="s">
+      <c r="A40" s="59" t="s">
         <v>38</v>
       </c>
       <c r="B40" s="44" t="s">
@@ -2980,13 +3051,13 @@
       <c r="H40" s="35" t="s">
         <v>88</v>
       </c>
-      <c r="I40" s="58" t="s">
+      <c r="I40" s="50" t="s">
         <v>26</v>
       </c>
-      <c r="J40" s="70" t="s">
+      <c r="J40" s="47" t="s">
         <v>56</v>
       </c>
-      <c r="K40" s="58" t="s">
+      <c r="K40" s="50" t="s">
         <v>28</v>
       </c>
       <c r="L40" s="2"/>
@@ -3007,7 +3078,7 @@
       <c r="AA40" s="2"/>
     </row>
     <row r="41" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A41" s="74"/>
+      <c r="A41" s="60"/>
       <c r="B41" s="45"/>
       <c r="C41" s="45"/>
       <c r="D41" s="45"/>
@@ -3019,9 +3090,9 @@
         <v>103</v>
       </c>
       <c r="H41" s="35"/>
-      <c r="I41" s="59"/>
-      <c r="J41" s="71"/>
-      <c r="K41" s="59"/>
+      <c r="I41" s="51"/>
+      <c r="J41" s="48"/>
+      <c r="K41" s="51"/>
       <c r="L41" s="2"/>
       <c r="M41" s="2"/>
       <c r="N41" s="2"/>
@@ -3040,7 +3111,7 @@
       <c r="AA41" s="2"/>
     </row>
     <row r="42" spans="1:27" ht="16.5" customHeight="1">
-      <c r="A42" s="74"/>
+      <c r="A42" s="60"/>
       <c r="B42" s="45"/>
       <c r="C42" s="45"/>
       <c r="D42" s="45"/>
@@ -3054,9 +3125,9 @@
       <c r="H42" s="35" t="s">
         <v>105</v>
       </c>
-      <c r="I42" s="59"/>
-      <c r="J42" s="71"/>
-      <c r="K42" s="59"/>
+      <c r="I42" s="51"/>
+      <c r="J42" s="48"/>
+      <c r="K42" s="51"/>
       <c r="L42" s="2"/>
       <c r="M42" s="2"/>
       <c r="N42" s="2"/>
@@ -3075,7 +3146,7 @@
       <c r="AA42" s="2"/>
     </row>
     <row r="43" spans="1:27" ht="18.75" customHeight="1">
-      <c r="A43" s="75"/>
+      <c r="A43" s="61"/>
       <c r="B43" s="46"/>
       <c r="C43" s="46"/>
       <c r="D43" s="46"/>
@@ -3085,9 +3156,9 @@
       </c>
       <c r="G43" s="35"/>
       <c r="H43" s="35"/>
-      <c r="I43" s="60"/>
-      <c r="J43" s="72"/>
-      <c r="K43" s="60"/>
+      <c r="I43" s="52"/>
+      <c r="J43" s="49"/>
+      <c r="K43" s="52"/>
       <c r="L43" s="2"/>
       <c r="M43" s="2"/>
       <c r="N43" s="2"/>
@@ -3106,7 +3177,7 @@
       <c r="AA43" s="2"/>
     </row>
     <row r="44" spans="1:27" ht="25.5">
-      <c r="A44" s="73" t="s">
+      <c r="A44" s="59" t="s">
         <v>39</v>
       </c>
       <c r="B44" s="44" t="s">
@@ -3130,13 +3201,13 @@
       <c r="H44" s="35" t="s">
         <v>88</v>
       </c>
-      <c r="I44" s="58" t="s">
+      <c r="I44" s="50" t="s">
         <v>26</v>
       </c>
-      <c r="J44" s="70" t="s">
+      <c r="J44" s="47" t="s">
         <v>56</v>
       </c>
-      <c r="K44" s="58" t="s">
+      <c r="K44" s="50" t="s">
         <v>28</v>
       </c>
       <c r="L44" s="2"/>
@@ -3157,7 +3228,7 @@
       <c r="AA44" s="2"/>
     </row>
     <row r="45" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A45" s="74"/>
+      <c r="A45" s="60"/>
       <c r="B45" s="45"/>
       <c r="C45" s="45"/>
       <c r="D45" s="45"/>
@@ -3169,9 +3240,9 @@
         <v>109</v>
       </c>
       <c r="H45" s="35"/>
-      <c r="I45" s="59"/>
-      <c r="J45" s="71"/>
-      <c r="K45" s="59"/>
+      <c r="I45" s="51"/>
+      <c r="J45" s="48"/>
+      <c r="K45" s="51"/>
       <c r="L45" s="2"/>
       <c r="M45" s="2"/>
       <c r="N45" s="2"/>
@@ -3190,7 +3261,7 @@
       <c r="AA45" s="2"/>
     </row>
     <row r="46" spans="1:27" ht="25.5">
-      <c r="A46" s="74"/>
+      <c r="A46" s="60"/>
       <c r="B46" s="45"/>
       <c r="C46" s="45"/>
       <c r="D46" s="45"/>
@@ -3204,9 +3275,9 @@
       <c r="H46" s="35" t="s">
         <v>110</v>
       </c>
-      <c r="I46" s="59"/>
-      <c r="J46" s="71"/>
-      <c r="K46" s="59"/>
+      <c r="I46" s="51"/>
+      <c r="J46" s="48"/>
+      <c r="K46" s="51"/>
       <c r="L46" s="2"/>
       <c r="M46" s="2"/>
       <c r="N46" s="2"/>
@@ -3225,7 +3296,7 @@
       <c r="AA46" s="2"/>
     </row>
     <row r="47" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A47" s="75"/>
+      <c r="A47" s="61"/>
       <c r="B47" s="46"/>
       <c r="C47" s="46"/>
       <c r="D47" s="46"/>
@@ -3235,9 +3306,9 @@
       </c>
       <c r="G47" s="35"/>
       <c r="H47" s="36"/>
-      <c r="I47" s="60"/>
-      <c r="J47" s="72"/>
-      <c r="K47" s="60"/>
+      <c r="I47" s="52"/>
+      <c r="J47" s="49"/>
+      <c r="K47" s="52"/>
       <c r="L47" s="2"/>
       <c r="M47" s="2"/>
       <c r="N47" s="2"/>
@@ -3256,7 +3327,7 @@
       <c r="AA47" s="2"/>
     </row>
     <row r="48" spans="1:27" ht="25.5">
-      <c r="A48" s="73" t="s">
+      <c r="A48" s="59" t="s">
         <v>40</v>
       </c>
       <c r="B48" s="44" t="s">
@@ -3280,13 +3351,13 @@
       <c r="H48" s="35" t="s">
         <v>88</v>
       </c>
-      <c r="I48" s="58" t="s">
+      <c r="I48" s="50" t="s">
         <v>26</v>
       </c>
-      <c r="J48" s="70" t="s">
+      <c r="J48" s="47" t="s">
         <v>56</v>
       </c>
-      <c r="K48" s="58" t="s">
+      <c r="K48" s="50" t="s">
         <v>28</v>
       </c>
       <c r="L48" s="2"/>
@@ -3307,7 +3378,7 @@
       <c r="AA48" s="2"/>
     </row>
     <row r="49" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A49" s="74"/>
+      <c r="A49" s="60"/>
       <c r="B49" s="45"/>
       <c r="C49" s="45"/>
       <c r="D49" s="45"/>
@@ -3319,9 +3390,9 @@
         <v>113</v>
       </c>
       <c r="H49" s="35"/>
-      <c r="I49" s="59"/>
-      <c r="J49" s="71"/>
-      <c r="K49" s="59"/>
+      <c r="I49" s="51"/>
+      <c r="J49" s="48"/>
+      <c r="K49" s="51"/>
       <c r="L49" s="2"/>
       <c r="M49" s="2"/>
       <c r="N49" s="2"/>
@@ -3340,7 +3411,7 @@
       <c r="AA49" s="2"/>
     </row>
     <row r="50" spans="1:27" ht="27" customHeight="1">
-      <c r="A50" s="74"/>
+      <c r="A50" s="60"/>
       <c r="B50" s="45"/>
       <c r="C50" s="45"/>
       <c r="D50" s="45"/>
@@ -3354,9 +3425,9 @@
       <c r="H50" s="35" t="s">
         <v>110</v>
       </c>
-      <c r="I50" s="59"/>
-      <c r="J50" s="71"/>
-      <c r="K50" s="59"/>
+      <c r="I50" s="51"/>
+      <c r="J50" s="48"/>
+      <c r="K50" s="51"/>
       <c r="L50" s="2"/>
       <c r="M50" s="2"/>
       <c r="N50" s="2"/>
@@ -3375,7 +3446,7 @@
       <c r="AA50" s="2"/>
     </row>
     <row r="51" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A51" s="75"/>
+      <c r="A51" s="61"/>
       <c r="B51" s="46"/>
       <c r="C51" s="46"/>
       <c r="D51" s="46"/>
@@ -3385,9 +3456,9 @@
       </c>
       <c r="G51" s="35"/>
       <c r="H51" s="36"/>
-      <c r="I51" s="60"/>
-      <c r="J51" s="72"/>
-      <c r="K51" s="60"/>
+      <c r="I51" s="52"/>
+      <c r="J51" s="49"/>
+      <c r="K51" s="52"/>
       <c r="L51" s="2"/>
       <c r="M51" s="2"/>
       <c r="N51" s="2"/>
@@ -3406,7 +3477,7 @@
       <c r="AA51" s="2"/>
     </row>
     <row r="52" spans="1:27" ht="25.5">
-      <c r="A52" s="73" t="s">
+      <c r="A52" s="59" t="s">
         <v>41</v>
       </c>
       <c r="B52" s="44" t="s">
@@ -3430,13 +3501,13 @@
       <c r="H52" s="35" t="s">
         <v>92</v>
       </c>
-      <c r="I52" s="58" t="s">
+      <c r="I52" s="50" t="s">
         <v>26</v>
       </c>
-      <c r="J52" s="70" t="s">
+      <c r="J52" s="47" t="s">
         <v>56</v>
       </c>
-      <c r="K52" s="58" t="s">
+      <c r="K52" s="50" t="s">
         <v>28</v>
       </c>
       <c r="L52" s="2"/>
@@ -3457,7 +3528,7 @@
       <c r="AA52" s="2"/>
     </row>
     <row r="53" spans="1:27" ht="25.5">
-      <c r="A53" s="74"/>
+      <c r="A53" s="60"/>
       <c r="B53" s="45"/>
       <c r="C53" s="45"/>
       <c r="D53" s="45"/>
@@ -3471,9 +3542,9 @@
       <c r="H53" s="36" t="s">
         <v>116</v>
       </c>
-      <c r="I53" s="59"/>
-      <c r="J53" s="71"/>
-      <c r="K53" s="59"/>
+      <c r="I53" s="51"/>
+      <c r="J53" s="48"/>
+      <c r="K53" s="51"/>
       <c r="L53" s="2"/>
       <c r="M53" s="2"/>
       <c r="N53" s="2"/>
@@ -3492,7 +3563,7 @@
       <c r="AA53" s="2"/>
     </row>
     <row r="54" spans="1:27" ht="13.5" customHeight="1">
-      <c r="A54" s="74"/>
+      <c r="A54" s="60"/>
       <c r="B54" s="45"/>
       <c r="C54" s="45"/>
       <c r="D54" s="45"/>
@@ -3500,9 +3571,9 @@
       <c r="F54" s="30"/>
       <c r="G54" s="43"/>
       <c r="H54" s="43"/>
-      <c r="I54" s="59"/>
-      <c r="J54" s="71"/>
-      <c r="K54" s="59"/>
+      <c r="I54" s="51"/>
+      <c r="J54" s="48"/>
+      <c r="K54" s="51"/>
       <c r="L54" s="2"/>
       <c r="M54" s="2"/>
       <c r="N54" s="2"/>
@@ -3521,7 +3592,7 @@
       <c r="AA54" s="2"/>
     </row>
     <row r="55" spans="1:27" ht="15" customHeight="1">
-      <c r="A55" s="75"/>
+      <c r="A55" s="61"/>
       <c r="B55" s="46"/>
       <c r="C55" s="46"/>
       <c r="D55" s="46"/>
@@ -3529,9 +3600,9 @@
       <c r="F55" s="30"/>
       <c r="G55" s="43"/>
       <c r="H55" s="43"/>
-      <c r="I55" s="60"/>
-      <c r="J55" s="72"/>
-      <c r="K55" s="60"/>
+      <c r="I55" s="52"/>
+      <c r="J55" s="49"/>
+      <c r="K55" s="52"/>
       <c r="L55" s="2"/>
       <c r="M55" s="2"/>
       <c r="N55" s="2"/>
@@ -3550,7 +3621,7 @@
       <c r="AA55" s="2"/>
     </row>
     <row r="56" spans="1:27" ht="25.5">
-      <c r="A56" s="73" t="s">
+      <c r="A56" s="59" t="s">
         <v>42</v>
       </c>
       <c r="B56" s="44" t="s">
@@ -3574,13 +3645,13 @@
       <c r="H56" s="35" t="s">
         <v>92</v>
       </c>
-      <c r="I56" s="58" t="s">
+      <c r="I56" s="50" t="s">
         <v>26</v>
       </c>
-      <c r="J56" s="70" t="s">
+      <c r="J56" s="47" t="s">
         <v>56</v>
       </c>
-      <c r="K56" s="58" t="s">
+      <c r="K56" s="50" t="s">
         <v>28</v>
       </c>
       <c r="L56" s="2"/>
@@ -3601,7 +3672,7 @@
       <c r="AA56" s="2"/>
     </row>
     <row r="57" spans="1:27" ht="17.25" customHeight="1">
-      <c r="A57" s="74"/>
+      <c r="A57" s="60"/>
       <c r="B57" s="45"/>
       <c r="C57" s="45"/>
       <c r="D57" s="45"/>
@@ -3615,9 +3686,9 @@
       <c r="H57" s="36" t="s">
         <v>120</v>
       </c>
-      <c r="I57" s="59"/>
-      <c r="J57" s="71"/>
-      <c r="K57" s="59"/>
+      <c r="I57" s="51"/>
+      <c r="J57" s="48"/>
+      <c r="K57" s="51"/>
       <c r="L57" s="2"/>
       <c r="M57" s="2"/>
       <c r="N57" s="2"/>
@@ -3636,7 +3707,7 @@
       <c r="AA57" s="2"/>
     </row>
     <row r="58" spans="1:27" ht="25.5">
-      <c r="A58" s="74"/>
+      <c r="A58" s="60"/>
       <c r="B58" s="45"/>
       <c r="C58" s="45"/>
       <c r="D58" s="45"/>
@@ -3650,9 +3721,9 @@
       <c r="H58" s="36" t="s">
         <v>122</v>
       </c>
-      <c r="I58" s="59"/>
-      <c r="J58" s="71"/>
-      <c r="K58" s="59"/>
+      <c r="I58" s="51"/>
+      <c r="J58" s="48"/>
+      <c r="K58" s="51"/>
       <c r="L58" s="2"/>
       <c r="M58" s="2"/>
       <c r="N58" s="2"/>
@@ -3671,7 +3742,7 @@
       <c r="AA58" s="2"/>
     </row>
     <row r="59" spans="1:27" ht="25.5">
-      <c r="A59" s="75"/>
+      <c r="A59" s="61"/>
       <c r="B59" s="46"/>
       <c r="C59" s="46"/>
       <c r="D59" s="46"/>
@@ -3685,9 +3756,9 @@
       <c r="H59" s="36" t="s">
         <v>123</v>
       </c>
-      <c r="I59" s="60"/>
-      <c r="J59" s="72"/>
-      <c r="K59" s="60"/>
+      <c r="I59" s="52"/>
+      <c r="J59" s="49"/>
+      <c r="K59" s="52"/>
       <c r="L59" s="2"/>
       <c r="M59" s="2"/>
       <c r="N59" s="2"/>
@@ -3706,7 +3777,7 @@
       <c r="AA59" s="2"/>
     </row>
     <row r="60" spans="1:27" ht="25.5">
-      <c r="A60" s="73" t="s">
+      <c r="A60" s="59" t="s">
         <v>43</v>
       </c>
       <c r="B60" s="44" t="s">
@@ -3730,13 +3801,13 @@
       <c r="H60" s="35" t="s">
         <v>92</v>
       </c>
-      <c r="I60" s="58" t="s">
+      <c r="I60" s="50" t="s">
         <v>26</v>
       </c>
-      <c r="J60" s="70" t="s">
+      <c r="J60" s="47" t="s">
         <v>56</v>
       </c>
-      <c r="K60" s="58" t="s">
+      <c r="K60" s="50" t="s">
         <v>28</v>
       </c>
       <c r="L60" s="2"/>
@@ -3757,7 +3828,7 @@
       <c r="AA60" s="2"/>
     </row>
     <row r="61" spans="1:27" ht="25.5">
-      <c r="A61" s="74"/>
+      <c r="A61" s="60"/>
       <c r="B61" s="45"/>
       <c r="C61" s="45"/>
       <c r="D61" s="45"/>
@@ -3771,9 +3842,9 @@
       <c r="H61" s="36" t="s">
         <v>120</v>
       </c>
-      <c r="I61" s="59"/>
-      <c r="J61" s="71"/>
-      <c r="K61" s="59"/>
+      <c r="I61" s="51"/>
+      <c r="J61" s="48"/>
+      <c r="K61" s="51"/>
       <c r="L61" s="2"/>
       <c r="M61" s="2"/>
       <c r="N61" s="2"/>
@@ -3792,7 +3863,7 @@
       <c r="AA61" s="2"/>
     </row>
     <row r="62" spans="1:27" ht="25.5">
-      <c r="A62" s="74"/>
+      <c r="A62" s="60"/>
       <c r="B62" s="45"/>
       <c r="C62" s="45"/>
       <c r="D62" s="45"/>
@@ -3806,9 +3877,9 @@
       <c r="H62" s="36" t="s">
         <v>122</v>
       </c>
-      <c r="I62" s="59"/>
-      <c r="J62" s="71"/>
-      <c r="K62" s="59"/>
+      <c r="I62" s="51"/>
+      <c r="J62" s="48"/>
+      <c r="K62" s="51"/>
       <c r="L62" s="2"/>
       <c r="M62" s="2"/>
       <c r="N62" s="2"/>
@@ -3827,7 +3898,7 @@
       <c r="AA62" s="2"/>
     </row>
     <row r="63" spans="1:27" ht="25.5">
-      <c r="A63" s="75"/>
+      <c r="A63" s="61"/>
       <c r="B63" s="46"/>
       <c r="C63" s="46"/>
       <c r="D63" s="46"/>
@@ -3841,9 +3912,9 @@
       <c r="H63" s="35" t="s">
         <v>128</v>
       </c>
-      <c r="I63" s="60"/>
-      <c r="J63" s="72"/>
-      <c r="K63" s="60"/>
+      <c r="I63" s="52"/>
+      <c r="J63" s="49"/>
+      <c r="K63" s="52"/>
       <c r="L63" s="2"/>
       <c r="M63" s="2"/>
       <c r="N63" s="2"/>
@@ -3861,22 +3932,38 @@
       <c r="Z63" s="2"/>
       <c r="AA63" s="2"/>
     </row>
-    <row r="64" spans="1:27">
-      <c r="A64" s="50" t="s">
+    <row r="64" spans="1:27" ht="25.5">
+      <c r="A64" s="76" t="s">
         <v>44</v>
       </c>
-      <c r="B64" s="44"/>
-      <c r="C64" s="44"/>
-      <c r="D64" s="44"/>
-      <c r="E64" s="44"/>
-      <c r="F64" s="30"/>
-      <c r="G64" s="35"/>
-      <c r="H64" s="35"/>
-      <c r="I64" s="58" t="s">
+      <c r="B64" s="44" t="s">
+        <v>49</v>
+      </c>
+      <c r="C64" s="56" t="s">
+        <v>130</v>
+      </c>
+      <c r="D64" s="44" t="s">
+        <v>131</v>
+      </c>
+      <c r="E64" s="44" t="s">
+        <v>83</v>
+      </c>
+      <c r="F64" s="30" t="s">
+        <v>53</v>
+      </c>
+      <c r="G64" s="35" t="s">
+        <v>132</v>
+      </c>
+      <c r="H64" s="35" t="s">
+        <v>133</v>
+      </c>
+      <c r="I64" s="50" t="s">
         <v>26</v>
       </c>
-      <c r="J64" s="70"/>
-      <c r="K64" s="58" t="s">
+      <c r="J64" s="47" t="s">
+        <v>56</v>
+      </c>
+      <c r="K64" s="50" t="s">
         <v>28</v>
       </c>
       <c r="L64" s="2"/>
@@ -3897,17 +3984,17 @@
       <c r="AA64" s="2"/>
     </row>
     <row r="65" spans="1:27">
-      <c r="A65" s="51"/>
+      <c r="A65" s="77"/>
       <c r="B65" s="45"/>
-      <c r="C65" s="45"/>
+      <c r="C65" s="57"/>
       <c r="D65" s="45"/>
       <c r="E65" s="45"/>
       <c r="F65" s="30"/>
       <c r="G65" s="35"/>
       <c r="H65" s="35"/>
-      <c r="I65" s="59"/>
-      <c r="J65" s="71"/>
-      <c r="K65" s="59"/>
+      <c r="I65" s="51"/>
+      <c r="J65" s="48"/>
+      <c r="K65" s="51"/>
       <c r="L65" s="2"/>
       <c r="M65" s="2"/>
       <c r="N65" s="2"/>
@@ -3926,17 +4013,17 @@
       <c r="AA65" s="2"/>
     </row>
     <row r="66" spans="1:27">
-      <c r="A66" s="51"/>
+      <c r="A66" s="77"/>
       <c r="B66" s="45"/>
-      <c r="C66" s="45"/>
+      <c r="C66" s="57"/>
       <c r="D66" s="45"/>
       <c r="E66" s="45"/>
       <c r="F66" s="30"/>
       <c r="G66" s="35"/>
       <c r="H66" s="35"/>
-      <c r="I66" s="59"/>
-      <c r="J66" s="71"/>
-      <c r="K66" s="59"/>
+      <c r="I66" s="51"/>
+      <c r="J66" s="48"/>
+      <c r="K66" s="51"/>
       <c r="L66" s="2"/>
       <c r="M66" s="2"/>
       <c r="N66" s="2"/>
@@ -3955,17 +4042,17 @@
       <c r="AA66" s="2"/>
     </row>
     <row r="67" spans="1:27">
-      <c r="A67" s="52"/>
+      <c r="A67" s="78"/>
       <c r="B67" s="46"/>
-      <c r="C67" s="46"/>
+      <c r="C67" s="58"/>
       <c r="D67" s="46"/>
       <c r="E67" s="46"/>
       <c r="F67" s="30"/>
       <c r="G67" s="35"/>
-      <c r="H67" s="36"/>
-      <c r="I67" s="60"/>
-      <c r="J67" s="72"/>
-      <c r="K67" s="60"/>
+      <c r="H67" s="35"/>
+      <c r="I67" s="52"/>
+      <c r="J67" s="49"/>
+      <c r="K67" s="52"/>
       <c r="L67" s="2"/>
       <c r="M67" s="2"/>
       <c r="N67" s="2"/>
@@ -3983,22 +4070,38 @@
       <c r="Z67" s="2"/>
       <c r="AA67" s="2"/>
     </row>
-    <row r="68" spans="1:27">
-      <c r="A68" s="50" t="s">
+    <row r="68" spans="1:27" ht="25.5">
+      <c r="A68" s="76" t="s">
         <v>45</v>
       </c>
-      <c r="B68" s="44"/>
-      <c r="C68" s="44"/>
-      <c r="D68" s="44"/>
-      <c r="E68" s="44"/>
-      <c r="F68" s="30"/>
-      <c r="G68" s="35"/>
-      <c r="H68" s="35"/>
-      <c r="I68" s="58" t="s">
+      <c r="B68" s="44" t="s">
+        <v>49</v>
+      </c>
+      <c r="C68" s="56" t="s">
+        <v>134</v>
+      </c>
+      <c r="D68" s="44" t="s">
+        <v>135</v>
+      </c>
+      <c r="E68" s="44" t="s">
+        <v>83</v>
+      </c>
+      <c r="F68" s="30" t="s">
+        <v>53</v>
+      </c>
+      <c r="G68" s="35" t="s">
+        <v>136</v>
+      </c>
+      <c r="H68" s="35" t="s">
+        <v>137</v>
+      </c>
+      <c r="I68" s="50" t="s">
         <v>26</v>
       </c>
-      <c r="J68" s="70"/>
-      <c r="K68" s="58" t="s">
+      <c r="J68" s="47" t="s">
+        <v>56</v>
+      </c>
+      <c r="K68" s="50" t="s">
         <v>28</v>
       </c>
       <c r="L68" s="2"/>
@@ -4019,17 +4122,17 @@
       <c r="AA68" s="2"/>
     </row>
     <row r="69" spans="1:27">
-      <c r="A69" s="51"/>
+      <c r="A69" s="77"/>
       <c r="B69" s="45"/>
-      <c r="C69" s="45"/>
+      <c r="C69" s="57"/>
       <c r="D69" s="45"/>
       <c r="E69" s="45"/>
       <c r="F69" s="30"/>
-      <c r="G69" s="36"/>
-      <c r="H69" s="36"/>
-      <c r="I69" s="59"/>
-      <c r="J69" s="71"/>
-      <c r="K69" s="59"/>
+      <c r="G69" s="35"/>
+      <c r="H69" s="35"/>
+      <c r="I69" s="51"/>
+      <c r="J69" s="48"/>
+      <c r="K69" s="51"/>
       <c r="L69" s="2"/>
       <c r="M69" s="2"/>
       <c r="N69" s="2"/>
@@ -4048,17 +4151,17 @@
       <c r="AA69" s="2"/>
     </row>
     <row r="70" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A70" s="51"/>
+      <c r="A70" s="77"/>
       <c r="B70" s="45"/>
-      <c r="C70" s="45"/>
+      <c r="C70" s="57"/>
       <c r="D70" s="45"/>
       <c r="E70" s="45"/>
       <c r="F70" s="30"/>
-      <c r="G70" s="43"/>
-      <c r="H70" s="43"/>
-      <c r="I70" s="59"/>
-      <c r="J70" s="71"/>
-      <c r="K70" s="59"/>
+      <c r="G70" s="35"/>
+      <c r="H70" s="35"/>
+      <c r="I70" s="51"/>
+      <c r="J70" s="48"/>
+      <c r="K70" s="51"/>
       <c r="L70" s="2"/>
       <c r="M70" s="2"/>
       <c r="N70" s="2"/>
@@ -4077,17 +4180,17 @@
       <c r="AA70" s="2"/>
     </row>
     <row r="71" spans="1:27">
-      <c r="A71" s="52"/>
+      <c r="A71" s="78"/>
       <c r="B71" s="46"/>
-      <c r="C71" s="46"/>
+      <c r="C71" s="58"/>
       <c r="D71" s="46"/>
       <c r="E71" s="46"/>
       <c r="F71" s="30"/>
-      <c r="G71" s="43"/>
-      <c r="H71" s="43"/>
-      <c r="I71" s="60"/>
-      <c r="J71" s="72"/>
-      <c r="K71" s="60"/>
+      <c r="G71" s="35"/>
+      <c r="H71" s="35"/>
+      <c r="I71" s="52"/>
+      <c r="J71" s="49"/>
+      <c r="K71" s="52"/>
       <c r="L71" s="2"/>
       <c r="M71" s="2"/>
       <c r="N71" s="2"/>
@@ -4106,7 +4209,7 @@
       <c r="AA71" s="2"/>
     </row>
     <row r="72" spans="1:27">
-      <c r="A72" s="50" t="s">
+      <c r="A72" s="53" t="s">
         <v>46</v>
       </c>
       <c r="B72" s="44"/>
@@ -4116,11 +4219,11 @@
       <c r="F72" s="30"/>
       <c r="G72" s="35"/>
       <c r="H72" s="35"/>
-      <c r="I72" s="58" t="s">
+      <c r="I72" s="50" t="s">
         <v>26</v>
       </c>
-      <c r="J72" s="70"/>
-      <c r="K72" s="58" t="s">
+      <c r="J72" s="47"/>
+      <c r="K72" s="50" t="s">
         <v>28</v>
       </c>
       <c r="L72" s="2"/>
@@ -4141,7 +4244,7 @@
       <c r="AA72" s="2"/>
     </row>
     <row r="73" spans="1:27">
-      <c r="A73" s="51"/>
+      <c r="A73" s="54"/>
       <c r="B73" s="45"/>
       <c r="C73" s="45"/>
       <c r="D73" s="45"/>
@@ -4149,9 +4252,9 @@
       <c r="F73" s="30"/>
       <c r="G73" s="36"/>
       <c r="H73" s="36"/>
-      <c r="I73" s="59"/>
-      <c r="J73" s="71"/>
-      <c r="K73" s="59"/>
+      <c r="I73" s="51"/>
+      <c r="J73" s="48"/>
+      <c r="K73" s="51"/>
       <c r="L73" s="2"/>
       <c r="M73" s="2"/>
       <c r="N73" s="2"/>
@@ -4170,7 +4273,7 @@
       <c r="AA73" s="2"/>
     </row>
     <row r="74" spans="1:27">
-      <c r="A74" s="51"/>
+      <c r="A74" s="54"/>
       <c r="B74" s="45"/>
       <c r="C74" s="45"/>
       <c r="D74" s="45"/>
@@ -4178,9 +4281,9 @@
       <c r="F74" s="30"/>
       <c r="G74" s="36"/>
       <c r="H74" s="36"/>
-      <c r="I74" s="59"/>
-      <c r="J74" s="71"/>
-      <c r="K74" s="59"/>
+      <c r="I74" s="51"/>
+      <c r="J74" s="48"/>
+      <c r="K74" s="51"/>
       <c r="L74" s="2"/>
       <c r="M74" s="2"/>
       <c r="N74" s="2"/>
@@ -4199,7 +4302,7 @@
       <c r="AA74" s="2"/>
     </row>
     <row r="75" spans="1:27">
-      <c r="A75" s="52"/>
+      <c r="A75" s="55"/>
       <c r="B75" s="46"/>
       <c r="C75" s="46"/>
       <c r="D75" s="46"/>
@@ -4207,9 +4310,9 @@
       <c r="F75" s="30"/>
       <c r="G75" s="35"/>
       <c r="H75" s="36"/>
-      <c r="I75" s="60"/>
-      <c r="J75" s="72"/>
-      <c r="K75" s="60"/>
+      <c r="I75" s="52"/>
+      <c r="J75" s="49"/>
+      <c r="K75" s="52"/>
       <c r="L75" s="2"/>
       <c r="M75" s="2"/>
       <c r="N75" s="2"/>
@@ -4228,7 +4331,7 @@
       <c r="AA75" s="2"/>
     </row>
     <row r="76" spans="1:27">
-      <c r="A76" s="50" t="s">
+      <c r="A76" s="53" t="s">
         <v>47</v>
       </c>
       <c r="B76" s="44"/>
@@ -4238,11 +4341,11 @@
       <c r="F76" s="30"/>
       <c r="G76" s="35"/>
       <c r="H76" s="35"/>
-      <c r="I76" s="58" t="s">
+      <c r="I76" s="50" t="s">
         <v>26</v>
       </c>
-      <c r="J76" s="70"/>
-      <c r="K76" s="58" t="s">
+      <c r="J76" s="47"/>
+      <c r="K76" s="50" t="s">
         <v>28</v>
       </c>
       <c r="L76" s="2"/>
@@ -4263,7 +4366,7 @@
       <c r="AA76" s="2"/>
     </row>
     <row r="77" spans="1:27">
-      <c r="A77" s="51"/>
+      <c r="A77" s="54"/>
       <c r="B77" s="45"/>
       <c r="C77" s="45"/>
       <c r="D77" s="45"/>
@@ -4271,9 +4374,9 @@
       <c r="F77" s="30"/>
       <c r="G77" s="35"/>
       <c r="H77" s="36"/>
-      <c r="I77" s="59"/>
-      <c r="J77" s="71"/>
-      <c r="K77" s="59"/>
+      <c r="I77" s="51"/>
+      <c r="J77" s="48"/>
+      <c r="K77" s="51"/>
       <c r="L77" s="2"/>
       <c r="M77" s="2"/>
       <c r="N77" s="2"/>
@@ -4292,7 +4395,7 @@
       <c r="AA77" s="2"/>
     </row>
     <row r="78" spans="1:27">
-      <c r="A78" s="51"/>
+      <c r="A78" s="54"/>
       <c r="B78" s="45"/>
       <c r="C78" s="45"/>
       <c r="D78" s="45"/>
@@ -4300,9 +4403,9 @@
       <c r="F78" s="30"/>
       <c r="G78" s="36"/>
       <c r="H78" s="36"/>
-      <c r="I78" s="59"/>
-      <c r="J78" s="71"/>
-      <c r="K78" s="59"/>
+      <c r="I78" s="51"/>
+      <c r="J78" s="48"/>
+      <c r="K78" s="51"/>
       <c r="L78" s="2"/>
       <c r="M78" s="2"/>
       <c r="N78" s="2"/>
@@ -4321,7 +4424,7 @@
       <c r="AA78" s="2"/>
     </row>
     <row r="79" spans="1:27">
-      <c r="A79" s="52"/>
+      <c r="A79" s="55"/>
       <c r="B79" s="46"/>
       <c r="C79" s="46"/>
       <c r="D79" s="46"/>
@@ -4329,9 +4432,9 @@
       <c r="F79" s="30"/>
       <c r="G79" s="35"/>
       <c r="H79" s="35"/>
-      <c r="I79" s="60"/>
-      <c r="J79" s="72"/>
-      <c r="K79" s="60"/>
+      <c r="I79" s="52"/>
+      <c r="J79" s="49"/>
+      <c r="K79" s="52"/>
       <c r="L79" s="2"/>
       <c r="M79" s="2"/>
       <c r="N79" s="2"/>
@@ -4350,21 +4453,21 @@
       <c r="AA79" s="2"/>
     </row>
     <row r="80" spans="1:27">
-      <c r="A80" s="50" t="s">
+      <c r="A80" s="53" t="s">
         <v>48</v>
       </c>
       <c r="B80" s="44"/>
-      <c r="C80" s="47"/>
+      <c r="C80" s="56"/>
       <c r="D80" s="44"/>
       <c r="E80" s="44"/>
       <c r="F80" s="30"/>
       <c r="G80" s="35"/>
       <c r="H80" s="35"/>
-      <c r="I80" s="58" t="s">
+      <c r="I80" s="50" t="s">
         <v>26</v>
       </c>
-      <c r="J80" s="70"/>
-      <c r="K80" s="58" t="s">
+      <c r="J80" s="47"/>
+      <c r="K80" s="50" t="s">
         <v>28</v>
       </c>
       <c r="L80" s="2"/>
@@ -4385,17 +4488,17 @@
       <c r="AA80" s="2"/>
     </row>
     <row r="81" spans="1:27">
-      <c r="A81" s="51"/>
+      <c r="A81" s="54"/>
       <c r="B81" s="45"/>
-      <c r="C81" s="48"/>
+      <c r="C81" s="57"/>
       <c r="D81" s="45"/>
       <c r="E81" s="45"/>
       <c r="F81" s="30"/>
       <c r="G81" s="35"/>
       <c r="H81" s="35"/>
-      <c r="I81" s="59"/>
-      <c r="J81" s="71"/>
-      <c r="K81" s="59"/>
+      <c r="I81" s="51"/>
+      <c r="J81" s="48"/>
+      <c r="K81" s="51"/>
       <c r="L81" s="2"/>
       <c r="M81" s="2"/>
       <c r="N81" s="2"/>
@@ -4414,17 +4517,17 @@
       <c r="AA81" s="2"/>
     </row>
     <row r="82" spans="1:27">
-      <c r="A82" s="51"/>
+      <c r="A82" s="54"/>
       <c r="B82" s="45"/>
-      <c r="C82" s="48"/>
+      <c r="C82" s="57"/>
       <c r="D82" s="45"/>
       <c r="E82" s="45"/>
       <c r="F82" s="30"/>
       <c r="G82" s="35"/>
       <c r="H82" s="35"/>
-      <c r="I82" s="59"/>
-      <c r="J82" s="71"/>
-      <c r="K82" s="59"/>
+      <c r="I82" s="51"/>
+      <c r="J82" s="48"/>
+      <c r="K82" s="51"/>
       <c r="L82" s="2"/>
       <c r="M82" s="2"/>
       <c r="N82" s="2"/>
@@ -4443,17 +4546,17 @@
       <c r="AA82" s="2"/>
     </row>
     <row r="83" spans="1:27">
-      <c r="A83" s="52"/>
+      <c r="A83" s="55"/>
       <c r="B83" s="46"/>
-      <c r="C83" s="49"/>
+      <c r="C83" s="58"/>
       <c r="D83" s="46"/>
       <c r="E83" s="46"/>
       <c r="F83" s="30"/>
       <c r="G83" s="35"/>
       <c r="H83" s="35"/>
-      <c r="I83" s="60"/>
-      <c r="J83" s="72"/>
-      <c r="K83" s="60"/>
+      <c r="I83" s="52"/>
+      <c r="J83" s="49"/>
+      <c r="K83" s="52"/>
       <c r="L83" s="2"/>
       <c r="M83" s="2"/>
       <c r="N83" s="2"/>
@@ -29181,42 +29284,124 @@
     </row>
   </sheetData>
   <mergeCells count="178">
-    <mergeCell ref="B36:B39"/>
-    <mergeCell ref="C36:C39"/>
-    <mergeCell ref="D36:D39"/>
-    <mergeCell ref="E36:E39"/>
-    <mergeCell ref="J44:J47"/>
-    <mergeCell ref="K44:K47"/>
-    <mergeCell ref="I48:I51"/>
-    <mergeCell ref="J48:J51"/>
-    <mergeCell ref="K48:K51"/>
-    <mergeCell ref="B48:B51"/>
-    <mergeCell ref="C48:C51"/>
-    <mergeCell ref="D48:D51"/>
-    <mergeCell ref="E48:E51"/>
-    <mergeCell ref="K40:K43"/>
-    <mergeCell ref="I40:I43"/>
-    <mergeCell ref="B40:B43"/>
-    <mergeCell ref="J36:J39"/>
-    <mergeCell ref="C40:C43"/>
-    <mergeCell ref="D40:D43"/>
-    <mergeCell ref="E40:E43"/>
-    <mergeCell ref="A76:A79"/>
-    <mergeCell ref="B76:B79"/>
-    <mergeCell ref="C76:C79"/>
-    <mergeCell ref="D76:D79"/>
-    <mergeCell ref="E76:E79"/>
-    <mergeCell ref="I76:I79"/>
-    <mergeCell ref="J76:J79"/>
-    <mergeCell ref="K76:K79"/>
-    <mergeCell ref="J80:J83"/>
-    <mergeCell ref="K80:K83"/>
-    <mergeCell ref="A80:A83"/>
-    <mergeCell ref="B80:B83"/>
-    <mergeCell ref="C80:C83"/>
-    <mergeCell ref="D80:D83"/>
-    <mergeCell ref="E80:E83"/>
-    <mergeCell ref="I80:I83"/>
+    <mergeCell ref="C32:C35"/>
+    <mergeCell ref="B32:B35"/>
+    <mergeCell ref="B28:B31"/>
+    <mergeCell ref="C4:C7"/>
+    <mergeCell ref="C8:C11"/>
+    <mergeCell ref="C12:C15"/>
+    <mergeCell ref="C16:C19"/>
+    <mergeCell ref="C20:C23"/>
+    <mergeCell ref="C24:C27"/>
+    <mergeCell ref="C28:C31"/>
+    <mergeCell ref="A4:A7"/>
+    <mergeCell ref="A8:A11"/>
+    <mergeCell ref="A12:A15"/>
+    <mergeCell ref="A16:A19"/>
+    <mergeCell ref="A20:A23"/>
+    <mergeCell ref="A24:A27"/>
+    <mergeCell ref="B24:B27"/>
+    <mergeCell ref="B20:B23"/>
+    <mergeCell ref="B16:B19"/>
+    <mergeCell ref="B12:B15"/>
+    <mergeCell ref="B8:B11"/>
+    <mergeCell ref="B4:B7"/>
+    <mergeCell ref="K2:K3"/>
+    <mergeCell ref="I4:I7"/>
+    <mergeCell ref="I8:I11"/>
+    <mergeCell ref="I12:I15"/>
+    <mergeCell ref="I16:I19"/>
+    <mergeCell ref="E28:E31"/>
+    <mergeCell ref="E2:E3"/>
+    <mergeCell ref="G12:G13"/>
+    <mergeCell ref="G8:G9"/>
+    <mergeCell ref="F12:F13"/>
+    <mergeCell ref="F4:F5"/>
+    <mergeCell ref="F8:F9"/>
+    <mergeCell ref="K28:K31"/>
+    <mergeCell ref="E16:E19"/>
+    <mergeCell ref="E20:E23"/>
+    <mergeCell ref="E24:E27"/>
+    <mergeCell ref="F2:H2"/>
+    <mergeCell ref="I2:I3"/>
+    <mergeCell ref="I20:I23"/>
+    <mergeCell ref="I24:I27"/>
+    <mergeCell ref="I28:I31"/>
+    <mergeCell ref="E4:E7"/>
+    <mergeCell ref="E8:E11"/>
+    <mergeCell ref="E12:E15"/>
+    <mergeCell ref="E32:E35"/>
+    <mergeCell ref="C2:C3"/>
+    <mergeCell ref="H4:H5"/>
+    <mergeCell ref="G4:G5"/>
+    <mergeCell ref="H8:H9"/>
+    <mergeCell ref="H12:H13"/>
+    <mergeCell ref="K32:K35"/>
+    <mergeCell ref="K36:K39"/>
+    <mergeCell ref="J4:J7"/>
+    <mergeCell ref="J8:J11"/>
+    <mergeCell ref="J12:J15"/>
+    <mergeCell ref="J16:J19"/>
+    <mergeCell ref="J20:J23"/>
+    <mergeCell ref="J24:J27"/>
+    <mergeCell ref="J28:J31"/>
+    <mergeCell ref="I32:I35"/>
+    <mergeCell ref="I36:I39"/>
+    <mergeCell ref="K4:K7"/>
+    <mergeCell ref="K8:K11"/>
+    <mergeCell ref="K12:K15"/>
+    <mergeCell ref="K16:K19"/>
+    <mergeCell ref="K20:K23"/>
+    <mergeCell ref="K24:K27"/>
+    <mergeCell ref="J2:J3"/>
+    <mergeCell ref="J32:J35"/>
+    <mergeCell ref="B2:B3"/>
+    <mergeCell ref="A2:A3"/>
+    <mergeCell ref="A52:A55"/>
+    <mergeCell ref="B52:B55"/>
+    <mergeCell ref="C56:C59"/>
+    <mergeCell ref="D56:D59"/>
+    <mergeCell ref="C52:C55"/>
+    <mergeCell ref="D52:D55"/>
+    <mergeCell ref="A44:A47"/>
+    <mergeCell ref="A48:A51"/>
+    <mergeCell ref="D24:D27"/>
+    <mergeCell ref="D20:D23"/>
+    <mergeCell ref="D16:D19"/>
+    <mergeCell ref="D12:D15"/>
+    <mergeCell ref="D8:D11"/>
+    <mergeCell ref="D4:D7"/>
+    <mergeCell ref="A28:A31"/>
+    <mergeCell ref="A32:A35"/>
+    <mergeCell ref="A36:A39"/>
+    <mergeCell ref="A40:A43"/>
+    <mergeCell ref="D32:D35"/>
+    <mergeCell ref="D28:D31"/>
+    <mergeCell ref="A56:A59"/>
+    <mergeCell ref="D2:D3"/>
+    <mergeCell ref="J52:J55"/>
+    <mergeCell ref="K52:K55"/>
+    <mergeCell ref="E52:E55"/>
+    <mergeCell ref="B44:B47"/>
+    <mergeCell ref="C44:C47"/>
+    <mergeCell ref="D44:D47"/>
+    <mergeCell ref="E44:E47"/>
+    <mergeCell ref="B64:B67"/>
+    <mergeCell ref="C64:C67"/>
+    <mergeCell ref="D64:D67"/>
+    <mergeCell ref="E64:E67"/>
+    <mergeCell ref="I64:I67"/>
+    <mergeCell ref="B60:B63"/>
+    <mergeCell ref="C60:C63"/>
+    <mergeCell ref="D60:D63"/>
+    <mergeCell ref="E60:E63"/>
+    <mergeCell ref="I60:I63"/>
+    <mergeCell ref="E56:E59"/>
+    <mergeCell ref="I52:I55"/>
+    <mergeCell ref="B56:B59"/>
+    <mergeCell ref="I56:I59"/>
+    <mergeCell ref="I44:I47"/>
+    <mergeCell ref="J40:J43"/>
     <mergeCell ref="A60:A63"/>
     <mergeCell ref="J56:J59"/>
     <mergeCell ref="K56:K59"/>
@@ -29241,207 +29426,145 @@
     <mergeCell ref="A64:A67"/>
     <mergeCell ref="J64:J67"/>
     <mergeCell ref="K64:K67"/>
-    <mergeCell ref="D2:D3"/>
-    <mergeCell ref="J52:J55"/>
-    <mergeCell ref="K52:K55"/>
-    <mergeCell ref="E52:E55"/>
-    <mergeCell ref="B44:B47"/>
-    <mergeCell ref="C44:C47"/>
-    <mergeCell ref="D44:D47"/>
-    <mergeCell ref="E44:E47"/>
-    <mergeCell ref="B64:B67"/>
-    <mergeCell ref="C64:C67"/>
-    <mergeCell ref="D64:D67"/>
-    <mergeCell ref="E64:E67"/>
-    <mergeCell ref="I64:I67"/>
-    <mergeCell ref="B60:B63"/>
-    <mergeCell ref="C60:C63"/>
-    <mergeCell ref="D60:D63"/>
-    <mergeCell ref="E60:E63"/>
-    <mergeCell ref="I60:I63"/>
-    <mergeCell ref="E56:E59"/>
-    <mergeCell ref="I52:I55"/>
-    <mergeCell ref="B56:B59"/>
-    <mergeCell ref="I56:I59"/>
-    <mergeCell ref="I44:I47"/>
-    <mergeCell ref="J40:J43"/>
-    <mergeCell ref="J32:J35"/>
-    <mergeCell ref="B2:B3"/>
-    <mergeCell ref="A2:A3"/>
-    <mergeCell ref="A52:A55"/>
-    <mergeCell ref="B52:B55"/>
-    <mergeCell ref="C56:C59"/>
-    <mergeCell ref="D56:D59"/>
-    <mergeCell ref="C52:C55"/>
-    <mergeCell ref="D52:D55"/>
-    <mergeCell ref="A44:A47"/>
-    <mergeCell ref="A48:A51"/>
-    <mergeCell ref="D24:D27"/>
-    <mergeCell ref="D20:D23"/>
-    <mergeCell ref="D16:D19"/>
-    <mergeCell ref="D12:D15"/>
-    <mergeCell ref="D8:D11"/>
-    <mergeCell ref="D4:D7"/>
-    <mergeCell ref="A28:A31"/>
-    <mergeCell ref="A32:A35"/>
-    <mergeCell ref="A36:A39"/>
-    <mergeCell ref="A40:A43"/>
-    <mergeCell ref="D32:D35"/>
-    <mergeCell ref="D28:D31"/>
-    <mergeCell ref="A56:A59"/>
-    <mergeCell ref="E32:E35"/>
-    <mergeCell ref="C2:C3"/>
-    <mergeCell ref="H4:H5"/>
-    <mergeCell ref="G4:G5"/>
-    <mergeCell ref="H8:H9"/>
-    <mergeCell ref="H12:H13"/>
-    <mergeCell ref="K32:K35"/>
-    <mergeCell ref="K36:K39"/>
-    <mergeCell ref="J4:J7"/>
-    <mergeCell ref="J8:J11"/>
-    <mergeCell ref="J12:J15"/>
-    <mergeCell ref="J16:J19"/>
-    <mergeCell ref="J20:J23"/>
-    <mergeCell ref="J24:J27"/>
-    <mergeCell ref="J28:J31"/>
-    <mergeCell ref="I32:I35"/>
-    <mergeCell ref="I36:I39"/>
-    <mergeCell ref="K4:K7"/>
-    <mergeCell ref="K8:K11"/>
-    <mergeCell ref="K12:K15"/>
-    <mergeCell ref="K16:K19"/>
-    <mergeCell ref="K20:K23"/>
-    <mergeCell ref="K24:K27"/>
-    <mergeCell ref="J2:J3"/>
-    <mergeCell ref="K2:K3"/>
-    <mergeCell ref="I4:I7"/>
-    <mergeCell ref="I8:I11"/>
-    <mergeCell ref="I12:I15"/>
-    <mergeCell ref="I16:I19"/>
-    <mergeCell ref="E28:E31"/>
-    <mergeCell ref="E2:E3"/>
-    <mergeCell ref="G12:G13"/>
-    <mergeCell ref="G8:G9"/>
-    <mergeCell ref="F12:F13"/>
-    <mergeCell ref="F4:F5"/>
-    <mergeCell ref="F8:F9"/>
-    <mergeCell ref="K28:K31"/>
-    <mergeCell ref="E16:E19"/>
-    <mergeCell ref="E20:E23"/>
-    <mergeCell ref="E24:E27"/>
-    <mergeCell ref="F2:H2"/>
-    <mergeCell ref="I2:I3"/>
-    <mergeCell ref="I20:I23"/>
-    <mergeCell ref="I24:I27"/>
-    <mergeCell ref="I28:I31"/>
-    <mergeCell ref="E4:E7"/>
-    <mergeCell ref="E8:E11"/>
-    <mergeCell ref="E12:E15"/>
-    <mergeCell ref="A4:A7"/>
-    <mergeCell ref="A8:A11"/>
-    <mergeCell ref="A12:A15"/>
-    <mergeCell ref="A16:A19"/>
-    <mergeCell ref="A20:A23"/>
-    <mergeCell ref="A24:A27"/>
-    <mergeCell ref="B24:B27"/>
-    <mergeCell ref="B20:B23"/>
-    <mergeCell ref="B16:B19"/>
-    <mergeCell ref="B12:B15"/>
-    <mergeCell ref="B8:B11"/>
-    <mergeCell ref="B4:B7"/>
-    <mergeCell ref="C32:C35"/>
-    <mergeCell ref="B32:B35"/>
-    <mergeCell ref="B28:B31"/>
-    <mergeCell ref="C4:C7"/>
-    <mergeCell ref="C8:C11"/>
-    <mergeCell ref="C12:C15"/>
-    <mergeCell ref="C16:C19"/>
-    <mergeCell ref="C20:C23"/>
-    <mergeCell ref="C24:C27"/>
-    <mergeCell ref="C28:C31"/>
+    <mergeCell ref="A76:A79"/>
+    <mergeCell ref="B76:B79"/>
+    <mergeCell ref="C76:C79"/>
+    <mergeCell ref="D76:D79"/>
+    <mergeCell ref="E76:E79"/>
+    <mergeCell ref="I76:I79"/>
+    <mergeCell ref="J76:J79"/>
+    <mergeCell ref="K76:K79"/>
+    <mergeCell ref="J80:J83"/>
+    <mergeCell ref="K80:K83"/>
+    <mergeCell ref="A80:A83"/>
+    <mergeCell ref="B80:B83"/>
+    <mergeCell ref="C80:C83"/>
+    <mergeCell ref="D80:D83"/>
+    <mergeCell ref="E80:E83"/>
+    <mergeCell ref="I80:I83"/>
+    <mergeCell ref="B36:B39"/>
+    <mergeCell ref="C36:C39"/>
+    <mergeCell ref="D36:D39"/>
+    <mergeCell ref="E36:E39"/>
+    <mergeCell ref="J44:J47"/>
+    <mergeCell ref="K44:K47"/>
+    <mergeCell ref="I48:I51"/>
+    <mergeCell ref="J48:J51"/>
+    <mergeCell ref="K48:K51"/>
+    <mergeCell ref="B48:B51"/>
+    <mergeCell ref="C48:C51"/>
+    <mergeCell ref="D48:D51"/>
+    <mergeCell ref="E48:E51"/>
+    <mergeCell ref="K40:K43"/>
+    <mergeCell ref="I40:I43"/>
+    <mergeCell ref="B40:B43"/>
+    <mergeCell ref="J36:J39"/>
+    <mergeCell ref="C40:C43"/>
+    <mergeCell ref="D40:D43"/>
+    <mergeCell ref="E40:E43"/>
   </mergeCells>
-  <conditionalFormatting sqref="I64 I68 I72 I76 I80">
-    <cfRule type="cellIs" dxfId="19" priority="113" operator="equal">
+  <conditionalFormatting sqref="I72 I76 I80">
+    <cfRule type="cellIs" dxfId="23" priority="117" operator="equal">
       <formula>"TO DO"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I64 I68 I72 I76 I80">
-    <cfRule type="cellIs" dxfId="18" priority="114" operator="equal">
+  <conditionalFormatting sqref="I72 I76 I80">
+    <cfRule type="cellIs" dxfId="22" priority="118" operator="equal">
       <formula>"IN PROGRESS"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I64 I68 I72 I76 I80">
-    <cfRule type="cellIs" dxfId="17" priority="115" operator="equal">
+  <conditionalFormatting sqref="I72 I76 I80">
+    <cfRule type="cellIs" dxfId="21" priority="119" operator="equal">
       <formula>"REVIEWED"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I64 I68 I72 I76 I80">
-    <cfRule type="cellIs" dxfId="16" priority="116" operator="equal">
+  <conditionalFormatting sqref="I72 I76 I80">
+    <cfRule type="cellIs" dxfId="20" priority="120" operator="equal">
       <formula>"IN REVIEW"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I4 I8 I12">
+    <cfRule type="cellIs" dxfId="19" priority="13" operator="equal">
+      <formula>"TO DO"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I4 I8 I12">
+    <cfRule type="cellIs" dxfId="18" priority="14" operator="equal">
+      <formula>"IN PROGRESS"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I4 I8 I12">
+    <cfRule type="cellIs" dxfId="17" priority="15" operator="equal">
+      <formula>"REVIEWED"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I4 I8 I12">
+    <cfRule type="cellIs" dxfId="16" priority="16" operator="equal">
+      <formula>"IN REVIEW"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I16 I20 I24">
     <cfRule type="cellIs" dxfId="15" priority="9" operator="equal">
       <formula>"TO DO"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I4 I8 I12">
+  <conditionalFormatting sqref="I16 I20 I24">
     <cfRule type="cellIs" dxfId="14" priority="10" operator="equal">
       <formula>"IN PROGRESS"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I4 I8 I12">
+  <conditionalFormatting sqref="I16 I20 I24">
     <cfRule type="cellIs" dxfId="13" priority="11" operator="equal">
       <formula>"REVIEWED"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I4 I8 I12">
+  <conditionalFormatting sqref="I16 I20 I24">
     <cfRule type="cellIs" dxfId="12" priority="12" operator="equal">
       <formula>"IN REVIEW"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I16 I20 I24">
+  <conditionalFormatting sqref="I28 I32 I36 I40 I44 I48 I52 I56 I60">
     <cfRule type="cellIs" dxfId="11" priority="5" operator="equal">
       <formula>"TO DO"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I16 I20 I24">
+  <conditionalFormatting sqref="I28 I32 I36 I40 I44 I48 I52 I56 I60">
     <cfRule type="cellIs" dxfId="10" priority="6" operator="equal">
       <formula>"IN PROGRESS"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I16 I20 I24">
+  <conditionalFormatting sqref="I28 I32 I36 I40 I44 I48 I52 I56 I60">
     <cfRule type="cellIs" dxfId="9" priority="7" operator="equal">
       <formula>"REVIEWED"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I16 I20 I24">
+  <conditionalFormatting sqref="I28 I32 I36 I40 I44 I48 I52 I56 I60">
     <cfRule type="cellIs" dxfId="8" priority="8" operator="equal">
       <formula>"IN REVIEW"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I28 I32 I36 I40 I44 I48 I52 I56 I60">
+  <conditionalFormatting sqref="I64 I68">
     <cfRule type="cellIs" dxfId="7" priority="1" operator="equal">
       <formula>"TO DO"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I28 I32 I36 I40 I44 I48 I52 I56 I60">
+  <conditionalFormatting sqref="I64 I68">
     <cfRule type="cellIs" dxfId="5" priority="2" operator="equal">
       <formula>"IN PROGRESS"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I28 I32 I36 I40 I44 I48 I52 I56 I60">
+  <conditionalFormatting sqref="I64 I68">
     <cfRule type="cellIs" dxfId="3" priority="3" operator="equal">
       <formula>"REVIEWED"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I28 I32 I36 I40 I44 I48 I52 I56 I60">
+  <conditionalFormatting sqref="I64 I68">
     <cfRule type="cellIs" dxfId="1" priority="4" operator="equal">
       <formula>"IN REVIEW"</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" sqref="I72 I76 I24 I16 I20 I4 I8 I12 I80 I64 I68 I32 I36 I28 I40 I44 I48 I52 I56 I60">
+    <dataValidation type="list" allowBlank="1" sqref="I72 I76 I24 I16 I20 I4 I8 I12 I80 I56 I60 I32 I36 I28 I40 I44 I48 I52 I64 I68">
       <formula1>"TO DO,In Progress,In Review,Reviewed"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" sqref="K76 K36 K40 K32 K28 K4 K12 K8 K48 K44 K52 K60 K56 K64 K68 K72 K80 K20 K24 K16">

</xml_diff>

<commit_message>
Agrego casos de uso referentes a la gestion del producto en la web
</commit_message>
<xml_diff>
--- a/Testing 2024/template_caso_prueba-ISPC2024-sprint-1.xlsx
+++ b/Testing 2024/template_caso_prueba-ISPC2024-sprint-1.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="285" uniqueCount="138">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="348" uniqueCount="164">
   <si>
     <t>Id</t>
   </si>
@@ -440,6 +440,84 @@
   <si>
     <t>Deberá redirigirse al usuario a la página donde se visualiza la información de Librería Franklin</t>
   </si>
+  <si>
+    <t>Gestion de Producto</t>
+  </si>
+  <si>
+    <t>Agregar un libro nuevo</t>
+  </si>
+  <si>
+    <t>El Administrador puede agregar un libro nuevo al catálogo de libros</t>
+  </si>
+  <si>
+    <t>Estar logueado con credenciales de Administrador y tener acceso a la BDD</t>
+  </si>
+  <si>
+    <t>Ingresar a postman</t>
+  </si>
+  <si>
+    <t>Se visualiza la pagina principal de postman</t>
+  </si>
+  <si>
+    <t>Copiar Url a testear, seleccionando metodo POST</t>
+  </si>
+  <si>
+    <t>Completar la info para crear el nuevo libro en la BDD</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Visualizar la información ingresada </t>
+  </si>
+  <si>
+    <t>Oprimir el boton "SEND"</t>
+  </si>
+  <si>
+    <t>Listar libros</t>
+  </si>
+  <si>
+    <t>El Administrador puede listar los libros del catálogo</t>
+  </si>
+  <si>
+    <t>Copiar Url a testear, seleccionando metodo GET</t>
+  </si>
+  <si>
+    <t>Se visualiza todas las categorias creadas status 200</t>
+  </si>
+  <si>
+    <t>Editar libro</t>
+  </si>
+  <si>
+    <t xml:space="preserve">El Administrador puede editar la información de un libro del catálogo </t>
+  </si>
+  <si>
+    <t>Copiar Url a testear, seleccionando metodo PUT</t>
+  </si>
+  <si>
+    <t>Completar el body con la info que necesitamos editar</t>
+  </si>
+  <si>
+    <t>Se visualizan los datos modificados, status 200</t>
+  </si>
+  <si>
+    <t>Eliminar libro</t>
+  </si>
+  <si>
+    <t>El Administrador puede eliminar un libro del catálogo</t>
+  </si>
+  <si>
+    <t>Copiar Url a testear con id especifico, seleccionando metodo DELETE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Se visualiza la info ingresada </t>
+  </si>
+  <si>
+    <t>Se visualiza status 200 ok, categoria eliminada</t>
+  </si>
+  <si>
+    <t>TC-021</t>
+  </si>
+  <si>
+    <t>Ver los datos del libro cargados en la BDD, status 201</t>
+  </si>
 </sst>
 </file>
 
@@ -515,7 +593,7 @@
       <name val="ArialMT"/>
     </font>
   </fonts>
-  <fills count="14">
+  <fills count="15">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -591,6 +669,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="5" tint="0.79998168889431442"/>
+        <bgColor rgb="FFFFFFCC"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF0CDF3"/>
         <bgColor rgb="FFFFFFCC"/>
       </patternFill>
     </fill>
@@ -865,7 +949,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="79">
+  <cellXfs count="86">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -960,15 +1044,26 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="11" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="7" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -978,27 +1073,22 @@
     <xf numFmtId="0" fontId="1" fillId="7" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="14" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="10" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="14" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="10" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="14" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="10" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="12" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1009,6 +1099,21 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="12" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="13" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="13" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="13" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1043,6 +1148,15 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="11" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1052,28 +1166,11 @@
     <xf numFmtId="0" fontId="1" fillId="11" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="13" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="13" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="13" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="24">
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFCE5CD"/>
-          <bgColor rgb="FFFCE5CD"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="20">
     <dxf>
       <fill>
         <patternFill patternType="solid">
@@ -1093,32 +1190,8 @@
     <dxf>
       <fill>
         <patternFill patternType="solid">
-          <fgColor rgb="FF93C47D"/>
-          <bgColor rgb="FF93C47D"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
           <fgColor rgb="FFFFF2CC"/>
           <bgColor rgb="FFFFF2CC"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFF2CC"/>
-          <bgColor rgb="FFFFF2CC"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFA2C4C9"/>
-          <bgColor rgb="FFA2C4C9"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1328,6 +1401,7 @@
       <rgbColor rgb="00333333"/>
     </indexedColors>
     <mruColors>
+      <color rgb="FFF0CDF3"/>
       <color rgb="FFF6DDBC"/>
     </mruColors>
   </colors>
@@ -1607,8 +1681,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AA935"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A61" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="60" workbookViewId="0">
-      <selection activeCell="D72" sqref="D72:D75"/>
+    <sheetView tabSelected="1" topLeftCell="A64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="60" workbookViewId="0">
+      <selection activeCell="H89" sqref="H89"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5703125" defaultRowHeight="12.75"/>
@@ -1657,33 +1731,33 @@
       <c r="AA1" s="2"/>
     </row>
     <row r="2" spans="1:27" s="31" customFormat="1" ht="15.75" customHeight="1">
-      <c r="A2" s="64" t="s">
+      <c r="A2" s="71" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="62" t="s">
+      <c r="B2" s="69" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="64" t="s">
+      <c r="C2" s="71" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="62" t="s">
+      <c r="D2" s="69" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="62" t="s">
+      <c r="E2" s="69" t="s">
         <v>4</v>
       </c>
-      <c r="F2" s="68" t="s">
+      <c r="F2" s="75" t="s">
         <v>5</v>
       </c>
-      <c r="G2" s="69"/>
-      <c r="H2" s="70"/>
-      <c r="I2" s="71" t="s">
+      <c r="G2" s="76"/>
+      <c r="H2" s="77"/>
+      <c r="I2" s="78" t="s">
         <v>6</v>
       </c>
-      <c r="J2" s="62" t="s">
+      <c r="J2" s="69" t="s">
         <v>7</v>
       </c>
-      <c r="K2" s="62" t="s">
+      <c r="K2" s="69" t="s">
         <v>27</v>
       </c>
       <c r="L2" s="32"/>
@@ -1704,11 +1778,11 @@
       <c r="AA2" s="33"/>
     </row>
     <row r="3" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A3" s="65"/>
-      <c r="B3" s="63"/>
-      <c r="C3" s="65"/>
-      <c r="D3" s="63"/>
-      <c r="E3" s="63"/>
+      <c r="A3" s="72"/>
+      <c r="B3" s="70"/>
+      <c r="C3" s="72"/>
+      <c r="D3" s="70"/>
+      <c r="E3" s="70"/>
       <c r="F3" s="34" t="s">
         <v>8</v>
       </c>
@@ -1718,9 +1792,9 @@
       <c r="H3" s="42" t="s">
         <v>10</v>
       </c>
-      <c r="I3" s="72"/>
-      <c r="J3" s="63"/>
-      <c r="K3" s="63"/>
+      <c r="I3" s="79"/>
+      <c r="J3" s="70"/>
+      <c r="K3" s="70"/>
       <c r="L3" s="3"/>
       <c r="M3" s="2"/>
       <c r="N3" s="2"/>
@@ -1739,37 +1813,37 @@
       <c r="AA3" s="2"/>
     </row>
     <row r="4" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A4" s="53" t="s">
+      <c r="A4" s="80" t="s">
         <v>29</v>
       </c>
-      <c r="B4" s="44" t="s">
+      <c r="B4" s="58" t="s">
         <v>49</v>
       </c>
-      <c r="C4" s="44" t="s">
+      <c r="C4" s="58" t="s">
         <v>50</v>
       </c>
-      <c r="D4" s="44" t="s">
+      <c r="D4" s="58" t="s">
         <v>51</v>
       </c>
-      <c r="E4" s="44" t="s">
+      <c r="E4" s="58" t="s">
         <v>52</v>
       </c>
-      <c r="F4" s="44" t="s">
+      <c r="F4" s="58" t="s">
         <v>53</v>
       </c>
-      <c r="G4" s="44" t="s">
+      <c r="G4" s="58" t="s">
         <v>54</v>
       </c>
-      <c r="H4" s="66" t="s">
+      <c r="H4" s="73" t="s">
         <v>55</v>
       </c>
-      <c r="I4" s="50" t="s">
+      <c r="I4" s="49" t="s">
         <v>26</v>
       </c>
-      <c r="J4" s="47" t="s">
+      <c r="J4" s="52" t="s">
         <v>56</v>
       </c>
-      <c r="K4" s="50" t="s">
+      <c r="K4" s="49" t="s">
         <v>28</v>
       </c>
       <c r="L4" s="3"/>
@@ -1790,17 +1864,17 @@
       <c r="AA4" s="2"/>
     </row>
     <row r="5" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A5" s="54"/>
-      <c r="B5" s="45"/>
-      <c r="C5" s="45"/>
-      <c r="D5" s="45"/>
-      <c r="E5" s="45"/>
-      <c r="F5" s="46"/>
-      <c r="G5" s="46"/>
-      <c r="H5" s="67"/>
-      <c r="I5" s="51"/>
-      <c r="J5" s="48"/>
-      <c r="K5" s="51"/>
+      <c r="A5" s="81"/>
+      <c r="B5" s="59"/>
+      <c r="C5" s="59"/>
+      <c r="D5" s="59"/>
+      <c r="E5" s="59"/>
+      <c r="F5" s="60"/>
+      <c r="G5" s="60"/>
+      <c r="H5" s="74"/>
+      <c r="I5" s="50"/>
+      <c r="J5" s="53"/>
+      <c r="K5" s="50"/>
       <c r="L5" s="3"/>
       <c r="M5" s="2"/>
       <c r="N5" s="2"/>
@@ -1819,17 +1893,17 @@
       <c r="AA5" s="2"/>
     </row>
     <row r="6" spans="1:27" s="29" customFormat="1" ht="15.75" customHeight="1">
-      <c r="A6" s="54"/>
-      <c r="B6" s="45"/>
-      <c r="C6" s="45"/>
-      <c r="D6" s="45"/>
-      <c r="E6" s="45"/>
+      <c r="A6" s="81"/>
+      <c r="B6" s="59"/>
+      <c r="C6" s="59"/>
+      <c r="D6" s="59"/>
+      <c r="E6" s="59"/>
       <c r="F6" s="30"/>
       <c r="G6" s="35"/>
       <c r="H6" s="35"/>
-      <c r="I6" s="51"/>
-      <c r="J6" s="48"/>
-      <c r="K6" s="51"/>
+      <c r="I6" s="50"/>
+      <c r="J6" s="53"/>
+      <c r="K6" s="50"/>
       <c r="L6" s="27"/>
       <c r="M6" s="28"/>
       <c r="N6" s="28"/>
@@ -1848,17 +1922,17 @@
       <c r="AA6" s="28"/>
     </row>
     <row r="7" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A7" s="55"/>
-      <c r="B7" s="46"/>
-      <c r="C7" s="46"/>
-      <c r="D7" s="46"/>
-      <c r="E7" s="46"/>
+      <c r="A7" s="82"/>
+      <c r="B7" s="60"/>
+      <c r="C7" s="60"/>
+      <c r="D7" s="60"/>
+      <c r="E7" s="60"/>
       <c r="F7" s="30"/>
       <c r="G7" s="35"/>
       <c r="H7" s="35"/>
-      <c r="I7" s="52"/>
-      <c r="J7" s="49"/>
-      <c r="K7" s="52"/>
+      <c r="I7" s="51"/>
+      <c r="J7" s="54"/>
+      <c r="K7" s="51"/>
       <c r="L7" s="3"/>
       <c r="M7" s="2"/>
       <c r="N7" s="2"/>
@@ -1877,37 +1951,37 @@
       <c r="AA7" s="2"/>
     </row>
     <row r="8" spans="1:27">
-      <c r="A8" s="53" t="s">
+      <c r="A8" s="80" t="s">
         <v>30</v>
       </c>
-      <c r="B8" s="44" t="s">
+      <c r="B8" s="58" t="s">
         <v>49</v>
       </c>
-      <c r="C8" s="44" t="s">
+      <c r="C8" s="58" t="s">
         <v>57</v>
       </c>
-      <c r="D8" s="44" t="s">
+      <c r="D8" s="58" t="s">
         <v>58</v>
       </c>
-      <c r="E8" s="44" t="s">
+      <c r="E8" s="58" t="s">
         <v>59</v>
       </c>
-      <c r="F8" s="44" t="s">
+      <c r="F8" s="58" t="s">
         <v>53</v>
       </c>
-      <c r="G8" s="44" t="s">
+      <c r="G8" s="58" t="s">
         <v>54</v>
       </c>
-      <c r="H8" s="66" t="s">
+      <c r="H8" s="73" t="s">
         <v>55</v>
       </c>
-      <c r="I8" s="50" t="s">
+      <c r="I8" s="49" t="s">
         <v>26</v>
       </c>
-      <c r="J8" s="47" t="s">
+      <c r="J8" s="52" t="s">
         <v>56</v>
       </c>
-      <c r="K8" s="50" t="s">
+      <c r="K8" s="49" t="s">
         <v>28</v>
       </c>
       <c r="L8" s="3"/>
@@ -1928,17 +2002,17 @@
       <c r="AA8" s="2"/>
     </row>
     <row r="9" spans="1:27">
-      <c r="A9" s="54"/>
-      <c r="B9" s="45"/>
-      <c r="C9" s="45"/>
-      <c r="D9" s="45"/>
-      <c r="E9" s="45"/>
-      <c r="F9" s="46"/>
-      <c r="G9" s="46"/>
-      <c r="H9" s="67"/>
-      <c r="I9" s="51"/>
-      <c r="J9" s="48"/>
-      <c r="K9" s="51"/>
+      <c r="A9" s="81"/>
+      <c r="B9" s="59"/>
+      <c r="C9" s="59"/>
+      <c r="D9" s="59"/>
+      <c r="E9" s="59"/>
+      <c r="F9" s="60"/>
+      <c r="G9" s="60"/>
+      <c r="H9" s="74"/>
+      <c r="I9" s="50"/>
+      <c r="J9" s="53"/>
+      <c r="K9" s="50"/>
       <c r="L9" s="3"/>
       <c r="M9" s="2"/>
       <c r="N9" s="2"/>
@@ -1957,17 +2031,17 @@
       <c r="AA9" s="2"/>
     </row>
     <row r="10" spans="1:27" s="29" customFormat="1" ht="15.75" customHeight="1">
-      <c r="A10" s="54"/>
-      <c r="B10" s="45"/>
-      <c r="C10" s="45"/>
-      <c r="D10" s="45"/>
-      <c r="E10" s="45"/>
+      <c r="A10" s="81"/>
+      <c r="B10" s="59"/>
+      <c r="C10" s="59"/>
+      <c r="D10" s="59"/>
+      <c r="E10" s="59"/>
       <c r="F10" s="30"/>
       <c r="G10" s="35"/>
       <c r="H10" s="35"/>
-      <c r="I10" s="51"/>
-      <c r="J10" s="48"/>
-      <c r="K10" s="51"/>
+      <c r="I10" s="50"/>
+      <c r="J10" s="53"/>
+      <c r="K10" s="50"/>
       <c r="L10" s="27"/>
       <c r="M10" s="28"/>
       <c r="N10" s="28"/>
@@ -1986,17 +2060,17 @@
       <c r="AA10" s="28"/>
     </row>
     <row r="11" spans="1:27">
-      <c r="A11" s="55"/>
-      <c r="B11" s="46"/>
-      <c r="C11" s="46"/>
-      <c r="D11" s="46"/>
-      <c r="E11" s="46"/>
+      <c r="A11" s="82"/>
+      <c r="B11" s="60"/>
+      <c r="C11" s="60"/>
+      <c r="D11" s="60"/>
+      <c r="E11" s="60"/>
       <c r="F11" s="30"/>
       <c r="G11" s="35"/>
       <c r="H11" s="35"/>
-      <c r="I11" s="52"/>
-      <c r="J11" s="49"/>
-      <c r="K11" s="52"/>
+      <c r="I11" s="51"/>
+      <c r="J11" s="54"/>
+      <c r="K11" s="51"/>
       <c r="L11" s="3"/>
       <c r="M11" s="2"/>
       <c r="N11" s="2"/>
@@ -2015,37 +2089,37 @@
       <c r="AA11" s="2"/>
     </row>
     <row r="12" spans="1:27">
-      <c r="A12" s="53" t="s">
+      <c r="A12" s="80" t="s">
         <v>31</v>
       </c>
-      <c r="B12" s="44" t="s">
+      <c r="B12" s="58" t="s">
         <v>49</v>
       </c>
-      <c r="C12" s="44" t="s">
+      <c r="C12" s="58" t="s">
         <v>60</v>
       </c>
-      <c r="D12" s="44" t="s">
+      <c r="D12" s="58" t="s">
         <v>61</v>
       </c>
-      <c r="E12" s="44" t="s">
+      <c r="E12" s="58" t="s">
         <v>62</v>
       </c>
-      <c r="F12" s="44" t="s">
+      <c r="F12" s="58" t="s">
         <v>53</v>
       </c>
-      <c r="G12" s="44" t="s">
+      <c r="G12" s="58" t="s">
         <v>54</v>
       </c>
-      <c r="H12" s="66" t="s">
+      <c r="H12" s="73" t="s">
         <v>55</v>
       </c>
-      <c r="I12" s="50" t="s">
+      <c r="I12" s="49" t="s">
         <v>26</v>
       </c>
-      <c r="J12" s="47" t="s">
+      <c r="J12" s="52" t="s">
         <v>56</v>
       </c>
-      <c r="K12" s="50" t="s">
+      <c r="K12" s="49" t="s">
         <v>28</v>
       </c>
       <c r="L12" s="2"/>
@@ -2066,17 +2140,17 @@
       <c r="AA12" s="2"/>
     </row>
     <row r="13" spans="1:27">
-      <c r="A13" s="54"/>
-      <c r="B13" s="45"/>
-      <c r="C13" s="45"/>
-      <c r="D13" s="45"/>
-      <c r="E13" s="45"/>
-      <c r="F13" s="46"/>
-      <c r="G13" s="46"/>
-      <c r="H13" s="67"/>
-      <c r="I13" s="51"/>
-      <c r="J13" s="48"/>
-      <c r="K13" s="51"/>
+      <c r="A13" s="81"/>
+      <c r="B13" s="59"/>
+      <c r="C13" s="59"/>
+      <c r="D13" s="59"/>
+      <c r="E13" s="59"/>
+      <c r="F13" s="60"/>
+      <c r="G13" s="60"/>
+      <c r="H13" s="74"/>
+      <c r="I13" s="50"/>
+      <c r="J13" s="53"/>
+      <c r="K13" s="50"/>
       <c r="L13" s="2"/>
       <c r="M13" s="2"/>
       <c r="N13" s="2"/>
@@ -2095,17 +2169,17 @@
       <c r="AA13" s="2"/>
     </row>
     <row r="14" spans="1:27" s="29" customFormat="1">
-      <c r="A14" s="54"/>
-      <c r="B14" s="45"/>
-      <c r="C14" s="45"/>
-      <c r="D14" s="45"/>
-      <c r="E14" s="45"/>
+      <c r="A14" s="81"/>
+      <c r="B14" s="59"/>
+      <c r="C14" s="59"/>
+      <c r="D14" s="59"/>
+      <c r="E14" s="59"/>
       <c r="F14" s="30"/>
       <c r="G14" s="35"/>
       <c r="H14" s="35"/>
-      <c r="I14" s="51"/>
-      <c r="J14" s="48"/>
-      <c r="K14" s="51"/>
+      <c r="I14" s="50"/>
+      <c r="J14" s="53"/>
+      <c r="K14" s="50"/>
       <c r="L14" s="28"/>
       <c r="M14" s="28"/>
       <c r="N14" s="28"/>
@@ -2124,17 +2198,17 @@
       <c r="AA14" s="28"/>
     </row>
     <row r="15" spans="1:27">
-      <c r="A15" s="55"/>
-      <c r="B15" s="46"/>
-      <c r="C15" s="46"/>
-      <c r="D15" s="46"/>
-      <c r="E15" s="46"/>
+      <c r="A15" s="82"/>
+      <c r="B15" s="60"/>
+      <c r="C15" s="60"/>
+      <c r="D15" s="60"/>
+      <c r="E15" s="60"/>
       <c r="F15" s="30"/>
       <c r="G15" s="35"/>
       <c r="H15" s="35"/>
-      <c r="I15" s="52"/>
-      <c r="J15" s="49"/>
-      <c r="K15" s="52"/>
+      <c r="I15" s="51"/>
+      <c r="J15" s="54"/>
+      <c r="K15" s="51"/>
       <c r="L15" s="2"/>
       <c r="M15" s="2"/>
       <c r="N15" s="2"/>
@@ -2153,19 +2227,19 @@
       <c r="AA15" s="2"/>
     </row>
     <row r="16" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A16" s="73" t="s">
+      <c r="A16" s="83" t="s">
         <v>32</v>
       </c>
-      <c r="B16" s="44" t="s">
+      <c r="B16" s="58" t="s">
         <v>63</v>
       </c>
-      <c r="C16" s="44" t="s">
+      <c r="C16" s="58" t="s">
         <v>64</v>
       </c>
-      <c r="D16" s="44" t="s">
+      <c r="D16" s="58" t="s">
         <v>65</v>
       </c>
-      <c r="E16" s="44" t="s">
+      <c r="E16" s="58" t="s">
         <v>83</v>
       </c>
       <c r="F16" s="30" t="s">
@@ -2177,13 +2251,13 @@
       <c r="H16" s="35" t="s">
         <v>66</v>
       </c>
-      <c r="I16" s="50" t="s">
+      <c r="I16" s="49" t="s">
         <v>26</v>
       </c>
-      <c r="J16" s="47" t="s">
+      <c r="J16" s="52" t="s">
         <v>56</v>
       </c>
-      <c r="K16" s="50" t="s">
+      <c r="K16" s="49" t="s">
         <v>28</v>
       </c>
       <c r="L16" s="2"/>
@@ -2204,11 +2278,11 @@
       <c r="AA16" s="2"/>
     </row>
     <row r="17" spans="1:27" ht="16.5" customHeight="1">
-      <c r="A17" s="74"/>
-      <c r="B17" s="45"/>
-      <c r="C17" s="45"/>
-      <c r="D17" s="45"/>
-      <c r="E17" s="45"/>
+      <c r="A17" s="84"/>
+      <c r="B17" s="59"/>
+      <c r="C17" s="59"/>
+      <c r="D17" s="59"/>
+      <c r="E17" s="59"/>
       <c r="F17" s="30" t="s">
         <v>67</v>
       </c>
@@ -2218,9 +2292,9 @@
       <c r="H17" s="35" t="s">
         <v>69</v>
       </c>
-      <c r="I17" s="51"/>
-      <c r="J17" s="48"/>
-      <c r="K17" s="51"/>
+      <c r="I17" s="50"/>
+      <c r="J17" s="53"/>
+      <c r="K17" s="50"/>
       <c r="L17" s="2"/>
       <c r="M17" s="2"/>
       <c r="N17" s="2"/>
@@ -2239,11 +2313,11 @@
       <c r="AA17" s="2"/>
     </row>
     <row r="18" spans="1:27" s="29" customFormat="1" ht="25.5">
-      <c r="A18" s="74"/>
-      <c r="B18" s="45"/>
-      <c r="C18" s="45"/>
-      <c r="D18" s="45"/>
-      <c r="E18" s="45"/>
+      <c r="A18" s="84"/>
+      <c r="B18" s="59"/>
+      <c r="C18" s="59"/>
+      <c r="D18" s="59"/>
+      <c r="E18" s="59"/>
       <c r="F18" s="30" t="s">
         <v>70</v>
       </c>
@@ -2253,9 +2327,9 @@
       <c r="H18" s="35" t="s">
         <v>72</v>
       </c>
-      <c r="I18" s="51"/>
-      <c r="J18" s="48"/>
-      <c r="K18" s="51"/>
+      <c r="I18" s="50"/>
+      <c r="J18" s="53"/>
+      <c r="K18" s="50"/>
       <c r="L18" s="28"/>
       <c r="M18" s="28"/>
       <c r="N18" s="28"/>
@@ -2274,17 +2348,17 @@
       <c r="AA18" s="28"/>
     </row>
     <row r="19" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A19" s="75"/>
-      <c r="B19" s="46"/>
-      <c r="C19" s="46"/>
-      <c r="D19" s="46"/>
-      <c r="E19" s="46"/>
+      <c r="A19" s="85"/>
+      <c r="B19" s="60"/>
+      <c r="C19" s="60"/>
+      <c r="D19" s="60"/>
+      <c r="E19" s="60"/>
       <c r="F19" s="30"/>
       <c r="G19" s="35"/>
       <c r="H19" s="35"/>
-      <c r="I19" s="52"/>
-      <c r="J19" s="49"/>
-      <c r="K19" s="52"/>
+      <c r="I19" s="51"/>
+      <c r="J19" s="54"/>
+      <c r="K19" s="51"/>
       <c r="L19" s="2"/>
       <c r="M19" s="2"/>
       <c r="N19" s="2"/>
@@ -2303,19 +2377,19 @@
       <c r="AA19" s="2"/>
     </row>
     <row r="20" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A20" s="73" t="s">
+      <c r="A20" s="83" t="s">
         <v>33</v>
       </c>
-      <c r="B20" s="44" t="s">
+      <c r="B20" s="58" t="s">
         <v>63</v>
       </c>
-      <c r="C20" s="56" t="s">
+      <c r="C20" s="46" t="s">
         <v>73</v>
       </c>
-      <c r="D20" s="44" t="s">
+      <c r="D20" s="58" t="s">
         <v>74</v>
       </c>
-      <c r="E20" s="44" t="s">
+      <c r="E20" s="58" t="s">
         <v>75</v>
       </c>
       <c r="F20" s="30" t="s">
@@ -2327,13 +2401,13 @@
       <c r="H20" s="35" t="s">
         <v>76</v>
       </c>
-      <c r="I20" s="50" t="s">
+      <c r="I20" s="49" t="s">
         <v>26</v>
       </c>
-      <c r="J20" s="47" t="s">
+      <c r="J20" s="52" t="s">
         <v>56</v>
       </c>
-      <c r="K20" s="50" t="s">
+      <c r="K20" s="49" t="s">
         <v>28</v>
       </c>
       <c r="L20" s="2"/>
@@ -2354,11 +2428,11 @@
       <c r="AA20" s="2"/>
     </row>
     <row r="21" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A21" s="74"/>
-      <c r="B21" s="45"/>
-      <c r="C21" s="57"/>
-      <c r="D21" s="45"/>
-      <c r="E21" s="45"/>
+      <c r="A21" s="84"/>
+      <c r="B21" s="59"/>
+      <c r="C21" s="67"/>
+      <c r="D21" s="59"/>
+      <c r="E21" s="59"/>
       <c r="F21" s="30" t="s">
         <v>67</v>
       </c>
@@ -2366,9 +2440,9 @@
         <v>77</v>
       </c>
       <c r="H21" s="35"/>
-      <c r="I21" s="51"/>
-      <c r="J21" s="48"/>
-      <c r="K21" s="51"/>
+      <c r="I21" s="50"/>
+      <c r="J21" s="53"/>
+      <c r="K21" s="50"/>
       <c r="L21" s="2"/>
       <c r="M21" s="2"/>
       <c r="N21" s="2"/>
@@ -2387,11 +2461,11 @@
       <c r="AA21" s="2"/>
     </row>
     <row r="22" spans="1:27" s="29" customFormat="1" ht="15.75" customHeight="1">
-      <c r="A22" s="74"/>
-      <c r="B22" s="45"/>
-      <c r="C22" s="57"/>
-      <c r="D22" s="45"/>
-      <c r="E22" s="45"/>
+      <c r="A22" s="84"/>
+      <c r="B22" s="59"/>
+      <c r="C22" s="67"/>
+      <c r="D22" s="59"/>
+      <c r="E22" s="59"/>
       <c r="F22" s="30" t="s">
         <v>70</v>
       </c>
@@ -2401,9 +2475,9 @@
       <c r="H22" s="35" t="s">
         <v>79</v>
       </c>
-      <c r="I22" s="51"/>
-      <c r="J22" s="48"/>
-      <c r="K22" s="51"/>
+      <c r="I22" s="50"/>
+      <c r="J22" s="53"/>
+      <c r="K22" s="50"/>
       <c r="L22" s="28"/>
       <c r="M22" s="28"/>
       <c r="N22" s="28"/>
@@ -2422,17 +2496,17 @@
       <c r="AA22" s="28"/>
     </row>
     <row r="23" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A23" s="75"/>
-      <c r="B23" s="46"/>
-      <c r="C23" s="58"/>
-      <c r="D23" s="46"/>
-      <c r="E23" s="46"/>
+      <c r="A23" s="85"/>
+      <c r="B23" s="60"/>
+      <c r="C23" s="68"/>
+      <c r="D23" s="60"/>
+      <c r="E23" s="60"/>
       <c r="F23" s="30"/>
       <c r="G23" s="35"/>
       <c r="H23" s="35"/>
-      <c r="I23" s="52"/>
-      <c r="J23" s="49"/>
-      <c r="K23" s="52"/>
+      <c r="I23" s="51"/>
+      <c r="J23" s="54"/>
+      <c r="K23" s="51"/>
       <c r="L23" s="2"/>
       <c r="M23" s="2"/>
       <c r="N23" s="2"/>
@@ -2451,19 +2525,19 @@
       <c r="AA23" s="2"/>
     </row>
     <row r="24" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A24" s="73" t="s">
+      <c r="A24" s="83" t="s">
         <v>34</v>
       </c>
-      <c r="B24" s="44" t="s">
+      <c r="B24" s="58" t="s">
         <v>63</v>
       </c>
-      <c r="C24" s="56" t="s">
+      <c r="C24" s="46" t="s">
         <v>80</v>
       </c>
-      <c r="D24" s="44" t="s">
+      <c r="D24" s="58" t="s">
         <v>81</v>
       </c>
-      <c r="E24" s="44" t="s">
+      <c r="E24" s="58" t="s">
         <v>75</v>
       </c>
       <c r="F24" s="30" t="s">
@@ -2475,13 +2549,13 @@
       <c r="H24" s="35" t="s">
         <v>76</v>
       </c>
-      <c r="I24" s="50" t="s">
+      <c r="I24" s="49" t="s">
         <v>26</v>
       </c>
-      <c r="J24" s="47" t="s">
+      <c r="J24" s="52" t="s">
         <v>56</v>
       </c>
-      <c r="K24" s="50" t="s">
+      <c r="K24" s="49" t="s">
         <v>28</v>
       </c>
       <c r="L24" s="2"/>
@@ -2502,11 +2576,11 @@
       <c r="AA24" s="2"/>
     </row>
     <row r="25" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A25" s="74"/>
-      <c r="B25" s="45"/>
-      <c r="C25" s="57"/>
-      <c r="D25" s="45"/>
-      <c r="E25" s="45"/>
+      <c r="A25" s="84"/>
+      <c r="B25" s="59"/>
+      <c r="C25" s="67"/>
+      <c r="D25" s="59"/>
+      <c r="E25" s="59"/>
       <c r="F25" s="30" t="s">
         <v>67</v>
       </c>
@@ -2514,9 +2588,9 @@
         <v>77</v>
       </c>
       <c r="H25" s="35"/>
-      <c r="I25" s="51"/>
-      <c r="J25" s="48"/>
-      <c r="K25" s="51"/>
+      <c r="I25" s="50"/>
+      <c r="J25" s="53"/>
+      <c r="K25" s="50"/>
       <c r="L25" s="2"/>
       <c r="M25" s="2"/>
       <c r="N25" s="2"/>
@@ -2535,11 +2609,11 @@
       <c r="AA25" s="2"/>
     </row>
     <row r="26" spans="1:27" s="29" customFormat="1" ht="25.5">
-      <c r="A26" s="74"/>
-      <c r="B26" s="45"/>
-      <c r="C26" s="57"/>
-      <c r="D26" s="45"/>
-      <c r="E26" s="45"/>
+      <c r="A26" s="84"/>
+      <c r="B26" s="59"/>
+      <c r="C26" s="67"/>
+      <c r="D26" s="59"/>
+      <c r="E26" s="59"/>
       <c r="F26" s="30" t="s">
         <v>70</v>
       </c>
@@ -2549,9 +2623,9 @@
       <c r="H26" s="35" t="s">
         <v>82</v>
       </c>
-      <c r="I26" s="51"/>
-      <c r="J26" s="48"/>
-      <c r="K26" s="51"/>
+      <c r="I26" s="50"/>
+      <c r="J26" s="53"/>
+      <c r="K26" s="50"/>
       <c r="L26" s="28"/>
       <c r="M26" s="28"/>
       <c r="N26" s="28"/>
@@ -2570,17 +2644,17 @@
       <c r="AA26" s="28"/>
     </row>
     <row r="27" spans="1:27" ht="18.75" customHeight="1">
-      <c r="A27" s="75"/>
-      <c r="B27" s="46"/>
-      <c r="C27" s="58"/>
-      <c r="D27" s="46"/>
-      <c r="E27" s="46"/>
+      <c r="A27" s="85"/>
+      <c r="B27" s="60"/>
+      <c r="C27" s="68"/>
+      <c r="D27" s="60"/>
+      <c r="E27" s="60"/>
       <c r="F27" s="30"/>
       <c r="G27" s="35"/>
       <c r="H27" s="35"/>
-      <c r="I27" s="52"/>
-      <c r="J27" s="49"/>
-      <c r="K27" s="52"/>
+      <c r="I27" s="51"/>
+      <c r="J27" s="54"/>
+      <c r="K27" s="51"/>
       <c r="L27" s="2"/>
       <c r="M27" s="2"/>
       <c r="N27" s="2"/>
@@ -2599,19 +2673,19 @@
       <c r="AA27" s="2"/>
     </row>
     <row r="28" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A28" s="59" t="s">
+      <c r="A28" s="61" t="s">
         <v>35</v>
       </c>
-      <c r="B28" s="44" t="s">
+      <c r="B28" s="58" t="s">
         <v>84</v>
       </c>
-      <c r="C28" s="44" t="s">
+      <c r="C28" s="58" t="s">
         <v>85</v>
       </c>
-      <c r="D28" s="44" t="s">
+      <c r="D28" s="58" t="s">
         <v>86</v>
       </c>
-      <c r="E28" s="44" t="s">
+      <c r="E28" s="58" t="s">
         <v>83</v>
       </c>
       <c r="F28" s="30" t="s">
@@ -2623,13 +2697,13 @@
       <c r="H28" s="35" t="s">
         <v>88</v>
       </c>
-      <c r="I28" s="50" t="s">
+      <c r="I28" s="49" t="s">
         <v>26</v>
       </c>
-      <c r="J28" s="47" t="s">
+      <c r="J28" s="52" t="s">
         <v>56</v>
       </c>
-      <c r="K28" s="50" t="s">
+      <c r="K28" s="49" t="s">
         <v>28</v>
       </c>
       <c r="L28" s="2"/>
@@ -2650,19 +2724,19 @@
       <c r="AA28" s="2"/>
     </row>
     <row r="29" spans="1:27">
-      <c r="A29" s="60"/>
-      <c r="B29" s="45"/>
-      <c r="C29" s="45"/>
-      <c r="D29" s="45"/>
-      <c r="E29" s="45"/>
+      <c r="A29" s="62"/>
+      <c r="B29" s="59"/>
+      <c r="C29" s="59"/>
+      <c r="D29" s="59"/>
+      <c r="E29" s="59"/>
       <c r="F29" s="30" t="s">
         <v>67</v>
       </c>
       <c r="G29" s="35"/>
       <c r="H29" s="35"/>
-      <c r="I29" s="51"/>
-      <c r="J29" s="48"/>
-      <c r="K29" s="51"/>
+      <c r="I29" s="50"/>
+      <c r="J29" s="53"/>
+      <c r="K29" s="50"/>
       <c r="L29" s="2"/>
       <c r="M29" s="2"/>
       <c r="N29" s="2"/>
@@ -2681,17 +2755,17 @@
       <c r="AA29" s="2"/>
     </row>
     <row r="30" spans="1:27" s="29" customFormat="1" ht="15.75" customHeight="1">
-      <c r="A30" s="60"/>
-      <c r="B30" s="45"/>
-      <c r="C30" s="45"/>
-      <c r="D30" s="45"/>
-      <c r="E30" s="45"/>
+      <c r="A30" s="62"/>
+      <c r="B30" s="59"/>
+      <c r="C30" s="59"/>
+      <c r="D30" s="59"/>
+      <c r="E30" s="59"/>
       <c r="F30" s="30"/>
       <c r="G30" s="35"/>
       <c r="H30" s="35"/>
-      <c r="I30" s="51"/>
-      <c r="J30" s="48"/>
-      <c r="K30" s="51"/>
+      <c r="I30" s="50"/>
+      <c r="J30" s="53"/>
+      <c r="K30" s="50"/>
       <c r="L30" s="28"/>
       <c r="M30" s="28"/>
       <c r="N30" s="28"/>
@@ -2710,17 +2784,17 @@
       <c r="AA30" s="28"/>
     </row>
     <row r="31" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A31" s="61"/>
-      <c r="B31" s="46"/>
-      <c r="C31" s="46"/>
-      <c r="D31" s="46"/>
-      <c r="E31" s="46"/>
+      <c r="A31" s="63"/>
+      <c r="B31" s="60"/>
+      <c r="C31" s="60"/>
+      <c r="D31" s="60"/>
+      <c r="E31" s="60"/>
       <c r="F31" s="30"/>
       <c r="G31" s="35"/>
       <c r="H31" s="35"/>
-      <c r="I31" s="52"/>
-      <c r="J31" s="49"/>
-      <c r="K31" s="52"/>
+      <c r="I31" s="51"/>
+      <c r="J31" s="54"/>
+      <c r="K31" s="51"/>
       <c r="L31" s="2"/>
       <c r="M31" s="2"/>
       <c r="N31" s="2"/>
@@ -2739,19 +2813,19 @@
       <c r="AA31" s="2"/>
     </row>
     <row r="32" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A32" s="59" t="s">
+      <c r="A32" s="61" t="s">
         <v>36</v>
       </c>
-      <c r="B32" s="44" t="s">
+      <c r="B32" s="58" t="s">
         <v>84</v>
       </c>
-      <c r="C32" s="44" t="s">
+      <c r="C32" s="58" t="s">
         <v>89</v>
       </c>
-      <c r="D32" s="44" t="s">
+      <c r="D32" s="58" t="s">
         <v>90</v>
       </c>
-      <c r="E32" s="44" t="s">
+      <c r="E32" s="58" t="s">
         <v>83</v>
       </c>
       <c r="F32" s="30" t="s">
@@ -2763,13 +2837,13 @@
       <c r="H32" s="35" t="s">
         <v>92</v>
       </c>
-      <c r="I32" s="50" t="s">
+      <c r="I32" s="49" t="s">
         <v>26</v>
       </c>
-      <c r="J32" s="47" t="s">
+      <c r="J32" s="52" t="s">
         <v>56</v>
       </c>
-      <c r="K32" s="50" t="s">
+      <c r="K32" s="49" t="s">
         <v>28</v>
       </c>
       <c r="L32" s="2"/>
@@ -2790,17 +2864,17 @@
       <c r="AA32" s="2"/>
     </row>
     <row r="33" spans="1:27">
-      <c r="A33" s="60"/>
-      <c r="B33" s="45"/>
-      <c r="C33" s="45"/>
-      <c r="D33" s="45"/>
-      <c r="E33" s="45"/>
+      <c r="A33" s="62"/>
+      <c r="B33" s="59"/>
+      <c r="C33" s="59"/>
+      <c r="D33" s="59"/>
+      <c r="E33" s="59"/>
       <c r="F33" s="30"/>
       <c r="G33" s="43"/>
       <c r="H33" s="43"/>
-      <c r="I33" s="51"/>
-      <c r="J33" s="48"/>
-      <c r="K33" s="51"/>
+      <c r="I33" s="50"/>
+      <c r="J33" s="53"/>
+      <c r="K33" s="50"/>
       <c r="L33" s="2"/>
       <c r="M33" s="2"/>
       <c r="N33" s="2"/>
@@ -2819,17 +2893,17 @@
       <c r="AA33" s="2"/>
     </row>
     <row r="34" spans="1:27">
-      <c r="A34" s="60"/>
-      <c r="B34" s="45"/>
-      <c r="C34" s="45"/>
-      <c r="D34" s="45"/>
-      <c r="E34" s="45"/>
+      <c r="A34" s="62"/>
+      <c r="B34" s="59"/>
+      <c r="C34" s="59"/>
+      <c r="D34" s="59"/>
+      <c r="E34" s="59"/>
       <c r="F34" s="30"/>
       <c r="G34" s="43"/>
       <c r="H34" s="43"/>
-      <c r="I34" s="51"/>
-      <c r="J34" s="48"/>
-      <c r="K34" s="51"/>
+      <c r="I34" s="50"/>
+      <c r="J34" s="53"/>
+      <c r="K34" s="50"/>
       <c r="L34" s="2"/>
       <c r="M34" s="2"/>
       <c r="N34" s="2"/>
@@ -2848,17 +2922,17 @@
       <c r="AA34" s="2"/>
     </row>
     <row r="35" spans="1:27">
-      <c r="A35" s="61"/>
-      <c r="B35" s="46"/>
-      <c r="C35" s="46"/>
-      <c r="D35" s="46"/>
-      <c r="E35" s="46"/>
+      <c r="A35" s="63"/>
+      <c r="B35" s="60"/>
+      <c r="C35" s="60"/>
+      <c r="D35" s="60"/>
+      <c r="E35" s="60"/>
       <c r="F35" s="30"/>
       <c r="G35" s="35"/>
       <c r="H35" s="35"/>
-      <c r="I35" s="52"/>
-      <c r="J35" s="49"/>
-      <c r="K35" s="52"/>
+      <c r="I35" s="51"/>
+      <c r="J35" s="54"/>
+      <c r="K35" s="51"/>
       <c r="L35" s="2"/>
       <c r="M35" s="2"/>
       <c r="N35" s="2"/>
@@ -2877,19 +2951,19 @@
       <c r="AA35" s="2"/>
     </row>
     <row r="36" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A36" s="59" t="s">
+      <c r="A36" s="61" t="s">
         <v>37</v>
       </c>
-      <c r="B36" s="44" t="s">
+      <c r="B36" s="58" t="s">
         <v>84</v>
       </c>
-      <c r="C36" s="44" t="s">
+      <c r="C36" s="58" t="s">
         <v>93</v>
       </c>
-      <c r="D36" s="44" t="s">
+      <c r="D36" s="58" t="s">
         <v>94</v>
       </c>
-      <c r="E36" s="44" t="s">
+      <c r="E36" s="58" t="s">
         <v>95</v>
       </c>
       <c r="F36" s="30" t="s">
@@ -2901,13 +2975,13 @@
       <c r="H36" s="35" t="s">
         <v>92</v>
       </c>
-      <c r="I36" s="50" t="s">
+      <c r="I36" s="49" t="s">
         <v>26</v>
       </c>
-      <c r="J36" s="47" t="s">
+      <c r="J36" s="52" t="s">
         <v>56</v>
       </c>
-      <c r="K36" s="50" t="s">
+      <c r="K36" s="49" t="s">
         <v>28</v>
       </c>
       <c r="L36" s="2"/>
@@ -2928,11 +3002,11 @@
       <c r="AA36" s="2"/>
     </row>
     <row r="37" spans="1:27" ht="25.5">
-      <c r="A37" s="60"/>
-      <c r="B37" s="45"/>
-      <c r="C37" s="45"/>
-      <c r="D37" s="45"/>
-      <c r="E37" s="45"/>
+      <c r="A37" s="62"/>
+      <c r="B37" s="59"/>
+      <c r="C37" s="59"/>
+      <c r="D37" s="59"/>
+      <c r="E37" s="59"/>
       <c r="F37" s="30" t="s">
         <v>67</v>
       </c>
@@ -2940,9 +3014,9 @@
         <v>96</v>
       </c>
       <c r="H37" s="35"/>
-      <c r="I37" s="51"/>
-      <c r="J37" s="48"/>
-      <c r="K37" s="51"/>
+      <c r="I37" s="50"/>
+      <c r="J37" s="53"/>
+      <c r="K37" s="50"/>
       <c r="L37" s="2"/>
       <c r="M37" s="2"/>
       <c r="N37" s="2"/>
@@ -2961,11 +3035,11 @@
       <c r="AA37" s="2"/>
     </row>
     <row r="38" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A38" s="60"/>
-      <c r="B38" s="45"/>
-      <c r="C38" s="45"/>
-      <c r="D38" s="45"/>
-      <c r="E38" s="45"/>
+      <c r="A38" s="62"/>
+      <c r="B38" s="59"/>
+      <c r="C38" s="59"/>
+      <c r="D38" s="59"/>
+      <c r="E38" s="59"/>
       <c r="F38" s="30" t="s">
         <v>70</v>
       </c>
@@ -2975,9 +3049,9 @@
       <c r="H38" s="35" t="s">
         <v>98</v>
       </c>
-      <c r="I38" s="51"/>
-      <c r="J38" s="48"/>
-      <c r="K38" s="51"/>
+      <c r="I38" s="50"/>
+      <c r="J38" s="53"/>
+      <c r="K38" s="50"/>
       <c r="L38" s="2"/>
       <c r="M38" s="2"/>
       <c r="N38" s="2"/>
@@ -2996,19 +3070,19 @@
       <c r="AA38" s="2"/>
     </row>
     <row r="39" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A39" s="61"/>
-      <c r="B39" s="46"/>
-      <c r="C39" s="46"/>
-      <c r="D39" s="46"/>
-      <c r="E39" s="46"/>
+      <c r="A39" s="63"/>
+      <c r="B39" s="60"/>
+      <c r="C39" s="60"/>
+      <c r="D39" s="60"/>
+      <c r="E39" s="60"/>
       <c r="F39" s="30" t="s">
         <v>99</v>
       </c>
       <c r="G39" s="35"/>
       <c r="H39" s="35"/>
-      <c r="I39" s="52"/>
-      <c r="J39" s="49"/>
-      <c r="K39" s="52"/>
+      <c r="I39" s="51"/>
+      <c r="J39" s="54"/>
+      <c r="K39" s="51"/>
       <c r="L39" s="2"/>
       <c r="M39" s="2"/>
       <c r="N39" s="2"/>
@@ -3027,19 +3101,19 @@
       <c r="AA39" s="2"/>
     </row>
     <row r="40" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A40" s="59" t="s">
+      <c r="A40" s="61" t="s">
         <v>38</v>
       </c>
-      <c r="B40" s="44" t="s">
+      <c r="B40" s="58" t="s">
         <v>84</v>
       </c>
-      <c r="C40" s="44" t="s">
+      <c r="C40" s="58" t="s">
         <v>100</v>
       </c>
-      <c r="D40" s="44" t="s">
+      <c r="D40" s="58" t="s">
         <v>101</v>
       </c>
-      <c r="E40" s="44" t="s">
+      <c r="E40" s="58" t="s">
         <v>102</v>
       </c>
       <c r="F40" s="30" t="s">
@@ -3051,13 +3125,13 @@
       <c r="H40" s="35" t="s">
         <v>88</v>
       </c>
-      <c r="I40" s="50" t="s">
+      <c r="I40" s="49" t="s">
         <v>26</v>
       </c>
-      <c r="J40" s="47" t="s">
+      <c r="J40" s="52" t="s">
         <v>56</v>
       </c>
-      <c r="K40" s="50" t="s">
+      <c r="K40" s="49" t="s">
         <v>28</v>
       </c>
       <c r="L40" s="2"/>
@@ -3078,11 +3152,11 @@
       <c r="AA40" s="2"/>
     </row>
     <row r="41" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A41" s="60"/>
-      <c r="B41" s="45"/>
-      <c r="C41" s="45"/>
-      <c r="D41" s="45"/>
-      <c r="E41" s="45"/>
+      <c r="A41" s="62"/>
+      <c r="B41" s="59"/>
+      <c r="C41" s="59"/>
+      <c r="D41" s="59"/>
+      <c r="E41" s="59"/>
       <c r="F41" s="30" t="s">
         <v>67</v>
       </c>
@@ -3090,9 +3164,9 @@
         <v>103</v>
       </c>
       <c r="H41" s="35"/>
-      <c r="I41" s="51"/>
-      <c r="J41" s="48"/>
-      <c r="K41" s="51"/>
+      <c r="I41" s="50"/>
+      <c r="J41" s="53"/>
+      <c r="K41" s="50"/>
       <c r="L41" s="2"/>
       <c r="M41" s="2"/>
       <c r="N41" s="2"/>
@@ -3111,11 +3185,11 @@
       <c r="AA41" s="2"/>
     </row>
     <row r="42" spans="1:27" ht="16.5" customHeight="1">
-      <c r="A42" s="60"/>
-      <c r="B42" s="45"/>
-      <c r="C42" s="45"/>
-      <c r="D42" s="45"/>
-      <c r="E42" s="45"/>
+      <c r="A42" s="62"/>
+      <c r="B42" s="59"/>
+      <c r="C42" s="59"/>
+      <c r="D42" s="59"/>
+      <c r="E42" s="59"/>
       <c r="F42" s="30" t="s">
         <v>70</v>
       </c>
@@ -3125,9 +3199,9 @@
       <c r="H42" s="35" t="s">
         <v>105</v>
       </c>
-      <c r="I42" s="51"/>
-      <c r="J42" s="48"/>
-      <c r="K42" s="51"/>
+      <c r="I42" s="50"/>
+      <c r="J42" s="53"/>
+      <c r="K42" s="50"/>
       <c r="L42" s="2"/>
       <c r="M42" s="2"/>
       <c r="N42" s="2"/>
@@ -3146,19 +3220,19 @@
       <c r="AA42" s="2"/>
     </row>
     <row r="43" spans="1:27" ht="18.75" customHeight="1">
-      <c r="A43" s="61"/>
-      <c r="B43" s="46"/>
-      <c r="C43" s="46"/>
-      <c r="D43" s="46"/>
-      <c r="E43" s="46"/>
+      <c r="A43" s="63"/>
+      <c r="B43" s="60"/>
+      <c r="C43" s="60"/>
+      <c r="D43" s="60"/>
+      <c r="E43" s="60"/>
       <c r="F43" s="30" t="s">
         <v>99</v>
       </c>
       <c r="G43" s="35"/>
       <c r="H43" s="35"/>
-      <c r="I43" s="52"/>
-      <c r="J43" s="49"/>
-      <c r="K43" s="52"/>
+      <c r="I43" s="51"/>
+      <c r="J43" s="54"/>
+      <c r="K43" s="51"/>
       <c r="L43" s="2"/>
       <c r="M43" s="2"/>
       <c r="N43" s="2"/>
@@ -3177,19 +3251,19 @@
       <c r="AA43" s="2"/>
     </row>
     <row r="44" spans="1:27" ht="25.5">
-      <c r="A44" s="59" t="s">
+      <c r="A44" s="61" t="s">
         <v>39</v>
       </c>
-      <c r="B44" s="44" t="s">
+      <c r="B44" s="58" t="s">
         <v>84</v>
       </c>
-      <c r="C44" s="44" t="s">
+      <c r="C44" s="58" t="s">
         <v>106</v>
       </c>
-      <c r="D44" s="44" t="s">
+      <c r="D44" s="58" t="s">
         <v>107</v>
       </c>
-      <c r="E44" s="44" t="s">
+      <c r="E44" s="58" t="s">
         <v>108</v>
       </c>
       <c r="F44" s="30" t="s">
@@ -3201,13 +3275,13 @@
       <c r="H44" s="35" t="s">
         <v>88</v>
       </c>
-      <c r="I44" s="50" t="s">
+      <c r="I44" s="49" t="s">
         <v>26</v>
       </c>
-      <c r="J44" s="47" t="s">
+      <c r="J44" s="52" t="s">
         <v>56</v>
       </c>
-      <c r="K44" s="50" t="s">
+      <c r="K44" s="49" t="s">
         <v>28</v>
       </c>
       <c r="L44" s="2"/>
@@ -3228,11 +3302,11 @@
       <c r="AA44" s="2"/>
     </row>
     <row r="45" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A45" s="60"/>
-      <c r="B45" s="45"/>
-      <c r="C45" s="45"/>
-      <c r="D45" s="45"/>
-      <c r="E45" s="45"/>
+      <c r="A45" s="62"/>
+      <c r="B45" s="59"/>
+      <c r="C45" s="59"/>
+      <c r="D45" s="59"/>
+      <c r="E45" s="59"/>
       <c r="F45" s="30" t="s">
         <v>67</v>
       </c>
@@ -3240,9 +3314,9 @@
         <v>109</v>
       </c>
       <c r="H45" s="35"/>
-      <c r="I45" s="51"/>
-      <c r="J45" s="48"/>
-      <c r="K45" s="51"/>
+      <c r="I45" s="50"/>
+      <c r="J45" s="53"/>
+      <c r="K45" s="50"/>
       <c r="L45" s="2"/>
       <c r="M45" s="2"/>
       <c r="N45" s="2"/>
@@ -3261,11 +3335,11 @@
       <c r="AA45" s="2"/>
     </row>
     <row r="46" spans="1:27" ht="25.5">
-      <c r="A46" s="60"/>
-      <c r="B46" s="45"/>
-      <c r="C46" s="45"/>
-      <c r="D46" s="45"/>
-      <c r="E46" s="45"/>
+      <c r="A46" s="62"/>
+      <c r="B46" s="59"/>
+      <c r="C46" s="59"/>
+      <c r="D46" s="59"/>
+      <c r="E46" s="59"/>
       <c r="F46" s="30" t="s">
         <v>70</v>
       </c>
@@ -3275,9 +3349,9 @@
       <c r="H46" s="35" t="s">
         <v>110</v>
       </c>
-      <c r="I46" s="51"/>
-      <c r="J46" s="48"/>
-      <c r="K46" s="51"/>
+      <c r="I46" s="50"/>
+      <c r="J46" s="53"/>
+      <c r="K46" s="50"/>
       <c r="L46" s="2"/>
       <c r="M46" s="2"/>
       <c r="N46" s="2"/>
@@ -3296,19 +3370,19 @@
       <c r="AA46" s="2"/>
     </row>
     <row r="47" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A47" s="61"/>
-      <c r="B47" s="46"/>
-      <c r="C47" s="46"/>
-      <c r="D47" s="46"/>
-      <c r="E47" s="46"/>
+      <c r="A47" s="63"/>
+      <c r="B47" s="60"/>
+      <c r="C47" s="60"/>
+      <c r="D47" s="60"/>
+      <c r="E47" s="60"/>
       <c r="F47" s="30" t="s">
         <v>99</v>
       </c>
       <c r="G47" s="35"/>
       <c r="H47" s="36"/>
-      <c r="I47" s="52"/>
-      <c r="J47" s="49"/>
-      <c r="K47" s="52"/>
+      <c r="I47" s="51"/>
+      <c r="J47" s="54"/>
+      <c r="K47" s="51"/>
       <c r="L47" s="2"/>
       <c r="M47" s="2"/>
       <c r="N47" s="2"/>
@@ -3327,19 +3401,19 @@
       <c r="AA47" s="2"/>
     </row>
     <row r="48" spans="1:27" ht="25.5">
-      <c r="A48" s="59" t="s">
+      <c r="A48" s="61" t="s">
         <v>40</v>
       </c>
-      <c r="B48" s="44" t="s">
+      <c r="B48" s="58" t="s">
         <v>84</v>
       </c>
-      <c r="C48" s="44" t="s">
+      <c r="C48" s="58" t="s">
         <v>111</v>
       </c>
-      <c r="D48" s="44" t="s">
+      <c r="D48" s="58" t="s">
         <v>112</v>
       </c>
-      <c r="E48" s="44" t="s">
+      <c r="E48" s="58" t="s">
         <v>102</v>
       </c>
       <c r="F48" s="30" t="s">
@@ -3351,13 +3425,13 @@
       <c r="H48" s="35" t="s">
         <v>88</v>
       </c>
-      <c r="I48" s="50" t="s">
+      <c r="I48" s="49" t="s">
         <v>26</v>
       </c>
-      <c r="J48" s="47" t="s">
+      <c r="J48" s="52" t="s">
         <v>56</v>
       </c>
-      <c r="K48" s="50" t="s">
+      <c r="K48" s="49" t="s">
         <v>28</v>
       </c>
       <c r="L48" s="2"/>
@@ -3378,11 +3452,11 @@
       <c r="AA48" s="2"/>
     </row>
     <row r="49" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A49" s="60"/>
-      <c r="B49" s="45"/>
-      <c r="C49" s="45"/>
-      <c r="D49" s="45"/>
-      <c r="E49" s="45"/>
+      <c r="A49" s="62"/>
+      <c r="B49" s="59"/>
+      <c r="C49" s="59"/>
+      <c r="D49" s="59"/>
+      <c r="E49" s="59"/>
       <c r="F49" s="30" t="s">
         <v>67</v>
       </c>
@@ -3390,9 +3464,9 @@
         <v>113</v>
       </c>
       <c r="H49" s="35"/>
-      <c r="I49" s="51"/>
-      <c r="J49" s="48"/>
-      <c r="K49" s="51"/>
+      <c r="I49" s="50"/>
+      <c r="J49" s="53"/>
+      <c r="K49" s="50"/>
       <c r="L49" s="2"/>
       <c r="M49" s="2"/>
       <c r="N49" s="2"/>
@@ -3411,11 +3485,11 @@
       <c r="AA49" s="2"/>
     </row>
     <row r="50" spans="1:27" ht="27" customHeight="1">
-      <c r="A50" s="60"/>
-      <c r="B50" s="45"/>
-      <c r="C50" s="45"/>
-      <c r="D50" s="45"/>
-      <c r="E50" s="45"/>
+      <c r="A50" s="62"/>
+      <c r="B50" s="59"/>
+      <c r="C50" s="59"/>
+      <c r="D50" s="59"/>
+      <c r="E50" s="59"/>
       <c r="F50" s="30" t="s">
         <v>70</v>
       </c>
@@ -3425,9 +3499,9 @@
       <c r="H50" s="35" t="s">
         <v>110</v>
       </c>
-      <c r="I50" s="51"/>
-      <c r="J50" s="48"/>
-      <c r="K50" s="51"/>
+      <c r="I50" s="50"/>
+      <c r="J50" s="53"/>
+      <c r="K50" s="50"/>
       <c r="L50" s="2"/>
       <c r="M50" s="2"/>
       <c r="N50" s="2"/>
@@ -3446,19 +3520,19 @@
       <c r="AA50" s="2"/>
     </row>
     <row r="51" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A51" s="61"/>
-      <c r="B51" s="46"/>
-      <c r="C51" s="46"/>
-      <c r="D51" s="46"/>
-      <c r="E51" s="46"/>
+      <c r="A51" s="63"/>
+      <c r="B51" s="60"/>
+      <c r="C51" s="60"/>
+      <c r="D51" s="60"/>
+      <c r="E51" s="60"/>
       <c r="F51" s="30" t="s">
         <v>99</v>
       </c>
       <c r="G51" s="35"/>
       <c r="H51" s="36"/>
-      <c r="I51" s="52"/>
-      <c r="J51" s="49"/>
-      <c r="K51" s="52"/>
+      <c r="I51" s="51"/>
+      <c r="J51" s="54"/>
+      <c r="K51" s="51"/>
       <c r="L51" s="2"/>
       <c r="M51" s="2"/>
       <c r="N51" s="2"/>
@@ -3477,19 +3551,19 @@
       <c r="AA51" s="2"/>
     </row>
     <row r="52" spans="1:27" ht="25.5">
-      <c r="A52" s="59" t="s">
+      <c r="A52" s="61" t="s">
         <v>41</v>
       </c>
-      <c r="B52" s="44" t="s">
+      <c r="B52" s="58" t="s">
         <v>84</v>
       </c>
-      <c r="C52" s="44" t="s">
+      <c r="C52" s="58" t="s">
         <v>114</v>
       </c>
-      <c r="D52" s="44" t="s">
+      <c r="D52" s="58" t="s">
         <v>129</v>
       </c>
-      <c r="E52" s="44" t="s">
+      <c r="E52" s="58" t="s">
         <v>95</v>
       </c>
       <c r="F52" s="30" t="s">
@@ -3501,13 +3575,13 @@
       <c r="H52" s="35" t="s">
         <v>92</v>
       </c>
-      <c r="I52" s="50" t="s">
+      <c r="I52" s="49" t="s">
         <v>26</v>
       </c>
-      <c r="J52" s="47" t="s">
+      <c r="J52" s="52" t="s">
         <v>56</v>
       </c>
-      <c r="K52" s="50" t="s">
+      <c r="K52" s="49" t="s">
         <v>28</v>
       </c>
       <c r="L52" s="2"/>
@@ -3528,11 +3602,11 @@
       <c r="AA52" s="2"/>
     </row>
     <row r="53" spans="1:27" ht="25.5">
-      <c r="A53" s="60"/>
-      <c r="B53" s="45"/>
-      <c r="C53" s="45"/>
-      <c r="D53" s="45"/>
-      <c r="E53" s="45"/>
+      <c r="A53" s="62"/>
+      <c r="B53" s="59"/>
+      <c r="C53" s="59"/>
+      <c r="D53" s="59"/>
+      <c r="E53" s="59"/>
       <c r="F53" s="30" t="s">
         <v>67</v>
       </c>
@@ -3542,9 +3616,9 @@
       <c r="H53" s="36" t="s">
         <v>116</v>
       </c>
-      <c r="I53" s="51"/>
-      <c r="J53" s="48"/>
-      <c r="K53" s="51"/>
+      <c r="I53" s="50"/>
+      <c r="J53" s="53"/>
+      <c r="K53" s="50"/>
       <c r="L53" s="2"/>
       <c r="M53" s="2"/>
       <c r="N53" s="2"/>
@@ -3563,17 +3637,17 @@
       <c r="AA53" s="2"/>
     </row>
     <row r="54" spans="1:27" ht="13.5" customHeight="1">
-      <c r="A54" s="60"/>
-      <c r="B54" s="45"/>
-      <c r="C54" s="45"/>
-      <c r="D54" s="45"/>
-      <c r="E54" s="45"/>
+      <c r="A54" s="62"/>
+      <c r="B54" s="59"/>
+      <c r="C54" s="59"/>
+      <c r="D54" s="59"/>
+      <c r="E54" s="59"/>
       <c r="F54" s="30"/>
       <c r="G54" s="43"/>
       <c r="H54" s="43"/>
-      <c r="I54" s="51"/>
-      <c r="J54" s="48"/>
-      <c r="K54" s="51"/>
+      <c r="I54" s="50"/>
+      <c r="J54" s="53"/>
+      <c r="K54" s="50"/>
       <c r="L54" s="2"/>
       <c r="M54" s="2"/>
       <c r="N54" s="2"/>
@@ -3592,17 +3666,17 @@
       <c r="AA54" s="2"/>
     </row>
     <row r="55" spans="1:27" ht="15" customHeight="1">
-      <c r="A55" s="61"/>
-      <c r="B55" s="46"/>
-      <c r="C55" s="46"/>
-      <c r="D55" s="46"/>
-      <c r="E55" s="46"/>
+      <c r="A55" s="63"/>
+      <c r="B55" s="60"/>
+      <c r="C55" s="60"/>
+      <c r="D55" s="60"/>
+      <c r="E55" s="60"/>
       <c r="F55" s="30"/>
       <c r="G55" s="43"/>
       <c r="H55" s="43"/>
-      <c r="I55" s="52"/>
-      <c r="J55" s="49"/>
-      <c r="K55" s="52"/>
+      <c r="I55" s="51"/>
+      <c r="J55" s="54"/>
+      <c r="K55" s="51"/>
       <c r="L55" s="2"/>
       <c r="M55" s="2"/>
       <c r="N55" s="2"/>
@@ -3621,19 +3695,19 @@
       <c r="AA55" s="2"/>
     </row>
     <row r="56" spans="1:27" ht="25.5">
-      <c r="A56" s="59" t="s">
+      <c r="A56" s="61" t="s">
         <v>42</v>
       </c>
-      <c r="B56" s="44" t="s">
+      <c r="B56" s="58" t="s">
         <v>84</v>
       </c>
-      <c r="C56" s="44" t="s">
+      <c r="C56" s="58" t="s">
         <v>117</v>
       </c>
-      <c r="D56" s="44" t="s">
+      <c r="D56" s="58" t="s">
         <v>118</v>
       </c>
-      <c r="E56" s="44" t="s">
+      <c r="E56" s="58" t="s">
         <v>95</v>
       </c>
       <c r="F56" s="30" t="s">
@@ -3645,13 +3719,13 @@
       <c r="H56" s="35" t="s">
         <v>92</v>
       </c>
-      <c r="I56" s="50" t="s">
+      <c r="I56" s="49" t="s">
         <v>26</v>
       </c>
-      <c r="J56" s="47" t="s">
+      <c r="J56" s="52" t="s">
         <v>56</v>
       </c>
-      <c r="K56" s="50" t="s">
+      <c r="K56" s="49" t="s">
         <v>28</v>
       </c>
       <c r="L56" s="2"/>
@@ -3672,11 +3746,11 @@
       <c r="AA56" s="2"/>
     </row>
     <row r="57" spans="1:27" ht="17.25" customHeight="1">
-      <c r="A57" s="60"/>
-      <c r="B57" s="45"/>
-      <c r="C57" s="45"/>
-      <c r="D57" s="45"/>
-      <c r="E57" s="45"/>
+      <c r="A57" s="62"/>
+      <c r="B57" s="59"/>
+      <c r="C57" s="59"/>
+      <c r="D57" s="59"/>
+      <c r="E57" s="59"/>
       <c r="F57" s="30" t="s">
         <v>67</v>
       </c>
@@ -3686,9 +3760,9 @@
       <c r="H57" s="36" t="s">
         <v>120</v>
       </c>
-      <c r="I57" s="51"/>
-      <c r="J57" s="48"/>
-      <c r="K57" s="51"/>
+      <c r="I57" s="50"/>
+      <c r="J57" s="53"/>
+      <c r="K57" s="50"/>
       <c r="L57" s="2"/>
       <c r="M57" s="2"/>
       <c r="N57" s="2"/>
@@ -3707,11 +3781,11 @@
       <c r="AA57" s="2"/>
     </row>
     <row r="58" spans="1:27" ht="25.5">
-      <c r="A58" s="60"/>
-      <c r="B58" s="45"/>
-      <c r="C58" s="45"/>
-      <c r="D58" s="45"/>
-      <c r="E58" s="45"/>
+      <c r="A58" s="62"/>
+      <c r="B58" s="59"/>
+      <c r="C58" s="59"/>
+      <c r="D58" s="59"/>
+      <c r="E58" s="59"/>
       <c r="F58" s="30" t="s">
         <v>70</v>
       </c>
@@ -3721,9 +3795,9 @@
       <c r="H58" s="36" t="s">
         <v>122</v>
       </c>
-      <c r="I58" s="51"/>
-      <c r="J58" s="48"/>
-      <c r="K58" s="51"/>
+      <c r="I58" s="50"/>
+      <c r="J58" s="53"/>
+      <c r="K58" s="50"/>
       <c r="L58" s="2"/>
       <c r="M58" s="2"/>
       <c r="N58" s="2"/>
@@ -3742,11 +3816,11 @@
       <c r="AA58" s="2"/>
     </row>
     <row r="59" spans="1:27" ht="25.5">
-      <c r="A59" s="61"/>
-      <c r="B59" s="46"/>
-      <c r="C59" s="46"/>
-      <c r="D59" s="46"/>
-      <c r="E59" s="46"/>
+      <c r="A59" s="63"/>
+      <c r="B59" s="60"/>
+      <c r="C59" s="60"/>
+      <c r="D59" s="60"/>
+      <c r="E59" s="60"/>
       <c r="F59" s="30" t="s">
         <v>99</v>
       </c>
@@ -3756,9 +3830,9 @@
       <c r="H59" s="36" t="s">
         <v>123</v>
       </c>
-      <c r="I59" s="52"/>
-      <c r="J59" s="49"/>
-      <c r="K59" s="52"/>
+      <c r="I59" s="51"/>
+      <c r="J59" s="54"/>
+      <c r="K59" s="51"/>
       <c r="L59" s="2"/>
       <c r="M59" s="2"/>
       <c r="N59" s="2"/>
@@ -3777,19 +3851,19 @@
       <c r="AA59" s="2"/>
     </row>
     <row r="60" spans="1:27" ht="25.5">
-      <c r="A60" s="59" t="s">
+      <c r="A60" s="61" t="s">
         <v>43</v>
       </c>
-      <c r="B60" s="44" t="s">
+      <c r="B60" s="58" t="s">
         <v>84</v>
       </c>
-      <c r="C60" s="44" t="s">
+      <c r="C60" s="58" t="s">
         <v>124</v>
       </c>
-      <c r="D60" s="44" t="s">
+      <c r="D60" s="58" t="s">
         <v>125</v>
       </c>
-      <c r="E60" s="44" t="s">
+      <c r="E60" s="58" t="s">
         <v>102</v>
       </c>
       <c r="F60" s="30" t="s">
@@ -3801,13 +3875,13 @@
       <c r="H60" s="35" t="s">
         <v>92</v>
       </c>
-      <c r="I60" s="50" t="s">
+      <c r="I60" s="49" t="s">
         <v>26</v>
       </c>
-      <c r="J60" s="47" t="s">
+      <c r="J60" s="52" t="s">
         <v>56</v>
       </c>
-      <c r="K60" s="50" t="s">
+      <c r="K60" s="49" t="s">
         <v>28</v>
       </c>
       <c r="L60" s="2"/>
@@ -3828,11 +3902,11 @@
       <c r="AA60" s="2"/>
     </row>
     <row r="61" spans="1:27" ht="25.5">
-      <c r="A61" s="60"/>
-      <c r="B61" s="45"/>
-      <c r="C61" s="45"/>
-      <c r="D61" s="45"/>
-      <c r="E61" s="45"/>
+      <c r="A61" s="62"/>
+      <c r="B61" s="59"/>
+      <c r="C61" s="59"/>
+      <c r="D61" s="59"/>
+      <c r="E61" s="59"/>
       <c r="F61" s="30" t="s">
         <v>67</v>
       </c>
@@ -3842,9 +3916,9 @@
       <c r="H61" s="36" t="s">
         <v>120</v>
       </c>
-      <c r="I61" s="51"/>
-      <c r="J61" s="48"/>
-      <c r="K61" s="51"/>
+      <c r="I61" s="50"/>
+      <c r="J61" s="53"/>
+      <c r="K61" s="50"/>
       <c r="L61" s="2"/>
       <c r="M61" s="2"/>
       <c r="N61" s="2"/>
@@ -3863,11 +3937,11 @@
       <c r="AA61" s="2"/>
     </row>
     <row r="62" spans="1:27" ht="25.5">
-      <c r="A62" s="60"/>
-      <c r="B62" s="45"/>
-      <c r="C62" s="45"/>
-      <c r="D62" s="45"/>
-      <c r="E62" s="45"/>
+      <c r="A62" s="62"/>
+      <c r="B62" s="59"/>
+      <c r="C62" s="59"/>
+      <c r="D62" s="59"/>
+      <c r="E62" s="59"/>
       <c r="F62" s="30" t="s">
         <v>70</v>
       </c>
@@ -3877,9 +3951,9 @@
       <c r="H62" s="36" t="s">
         <v>122</v>
       </c>
-      <c r="I62" s="51"/>
-      <c r="J62" s="48"/>
-      <c r="K62" s="51"/>
+      <c r="I62" s="50"/>
+      <c r="J62" s="53"/>
+      <c r="K62" s="50"/>
       <c r="L62" s="2"/>
       <c r="M62" s="2"/>
       <c r="N62" s="2"/>
@@ -3898,11 +3972,11 @@
       <c r="AA62" s="2"/>
     </row>
     <row r="63" spans="1:27" ht="25.5">
-      <c r="A63" s="61"/>
-      <c r="B63" s="46"/>
-      <c r="C63" s="46"/>
-      <c r="D63" s="46"/>
-      <c r="E63" s="46"/>
+      <c r="A63" s="63"/>
+      <c r="B63" s="60"/>
+      <c r="C63" s="60"/>
+      <c r="D63" s="60"/>
+      <c r="E63" s="60"/>
       <c r="F63" s="30" t="s">
         <v>99</v>
       </c>
@@ -3912,9 +3986,9 @@
       <c r="H63" s="35" t="s">
         <v>128</v>
       </c>
-      <c r="I63" s="52"/>
-      <c r="J63" s="49"/>
-      <c r="K63" s="52"/>
+      <c r="I63" s="51"/>
+      <c r="J63" s="54"/>
+      <c r="K63" s="51"/>
       <c r="L63" s="2"/>
       <c r="M63" s="2"/>
       <c r="N63" s="2"/>
@@ -3933,19 +4007,19 @@
       <c r="AA63" s="2"/>
     </row>
     <row r="64" spans="1:27" ht="25.5">
-      <c r="A64" s="76" t="s">
+      <c r="A64" s="64" t="s">
         <v>44</v>
       </c>
-      <c r="B64" s="44" t="s">
+      <c r="B64" s="58" t="s">
         <v>49</v>
       </c>
-      <c r="C64" s="56" t="s">
+      <c r="C64" s="46" t="s">
         <v>130</v>
       </c>
-      <c r="D64" s="44" t="s">
+      <c r="D64" s="58" t="s">
         <v>131</v>
       </c>
-      <c r="E64" s="44" t="s">
+      <c r="E64" s="58" t="s">
         <v>83</v>
       </c>
       <c r="F64" s="30" t="s">
@@ -3957,13 +4031,13 @@
       <c r="H64" s="35" t="s">
         <v>133</v>
       </c>
-      <c r="I64" s="50" t="s">
+      <c r="I64" s="49" t="s">
         <v>26</v>
       </c>
-      <c r="J64" s="47" t="s">
+      <c r="J64" s="52" t="s">
         <v>56</v>
       </c>
-      <c r="K64" s="50" t="s">
+      <c r="K64" s="49" t="s">
         <v>28</v>
       </c>
       <c r="L64" s="2"/>
@@ -3984,17 +4058,17 @@
       <c r="AA64" s="2"/>
     </row>
     <row r="65" spans="1:27">
-      <c r="A65" s="77"/>
-      <c r="B65" s="45"/>
-      <c r="C65" s="57"/>
-      <c r="D65" s="45"/>
-      <c r="E65" s="45"/>
+      <c r="A65" s="65"/>
+      <c r="B65" s="59"/>
+      <c r="C65" s="67"/>
+      <c r="D65" s="59"/>
+      <c r="E65" s="59"/>
       <c r="F65" s="30"/>
       <c r="G65" s="35"/>
       <c r="H65" s="35"/>
-      <c r="I65" s="51"/>
-      <c r="J65" s="48"/>
-      <c r="K65" s="51"/>
+      <c r="I65" s="50"/>
+      <c r="J65" s="53"/>
+      <c r="K65" s="50"/>
       <c r="L65" s="2"/>
       <c r="M65" s="2"/>
       <c r="N65" s="2"/>
@@ -4013,17 +4087,17 @@
       <c r="AA65" s="2"/>
     </row>
     <row r="66" spans="1:27">
-      <c r="A66" s="77"/>
-      <c r="B66" s="45"/>
-      <c r="C66" s="57"/>
-      <c r="D66" s="45"/>
-      <c r="E66" s="45"/>
+      <c r="A66" s="65"/>
+      <c r="B66" s="59"/>
+      <c r="C66" s="67"/>
+      <c r="D66" s="59"/>
+      <c r="E66" s="59"/>
       <c r="F66" s="30"/>
       <c r="G66" s="35"/>
       <c r="H66" s="35"/>
-      <c r="I66" s="51"/>
-      <c r="J66" s="48"/>
-      <c r="K66" s="51"/>
+      <c r="I66" s="50"/>
+      <c r="J66" s="53"/>
+      <c r="K66" s="50"/>
       <c r="L66" s="2"/>
       <c r="M66" s="2"/>
       <c r="N66" s="2"/>
@@ -4042,17 +4116,17 @@
       <c r="AA66" s="2"/>
     </row>
     <row r="67" spans="1:27">
-      <c r="A67" s="78"/>
-      <c r="B67" s="46"/>
-      <c r="C67" s="58"/>
-      <c r="D67" s="46"/>
-      <c r="E67" s="46"/>
+      <c r="A67" s="66"/>
+      <c r="B67" s="60"/>
+      <c r="C67" s="68"/>
+      <c r="D67" s="60"/>
+      <c r="E67" s="60"/>
       <c r="F67" s="30"/>
       <c r="G67" s="35"/>
       <c r="H67" s="35"/>
-      <c r="I67" s="52"/>
-      <c r="J67" s="49"/>
-      <c r="K67" s="52"/>
+      <c r="I67" s="51"/>
+      <c r="J67" s="54"/>
+      <c r="K67" s="51"/>
       <c r="L67" s="2"/>
       <c r="M67" s="2"/>
       <c r="N67" s="2"/>
@@ -4071,19 +4145,19 @@
       <c r="AA67" s="2"/>
     </row>
     <row r="68" spans="1:27" ht="25.5">
-      <c r="A68" s="76" t="s">
+      <c r="A68" s="64" t="s">
         <v>45</v>
       </c>
-      <c r="B68" s="44" t="s">
+      <c r="B68" s="58" t="s">
         <v>49</v>
       </c>
-      <c r="C68" s="56" t="s">
+      <c r="C68" s="46" t="s">
         <v>134</v>
       </c>
-      <c r="D68" s="44" t="s">
+      <c r="D68" s="58" t="s">
         <v>135</v>
       </c>
-      <c r="E68" s="44" t="s">
+      <c r="E68" s="58" t="s">
         <v>83</v>
       </c>
       <c r="F68" s="30" t="s">
@@ -4095,13 +4169,13 @@
       <c r="H68" s="35" t="s">
         <v>137</v>
       </c>
-      <c r="I68" s="50" t="s">
+      <c r="I68" s="49" t="s">
         <v>26</v>
       </c>
-      <c r="J68" s="47" t="s">
+      <c r="J68" s="52" t="s">
         <v>56</v>
       </c>
-      <c r="K68" s="50" t="s">
+      <c r="K68" s="49" t="s">
         <v>28</v>
       </c>
       <c r="L68" s="2"/>
@@ -4122,17 +4196,17 @@
       <c r="AA68" s="2"/>
     </row>
     <row r="69" spans="1:27">
-      <c r="A69" s="77"/>
-      <c r="B69" s="45"/>
-      <c r="C69" s="57"/>
-      <c r="D69" s="45"/>
-      <c r="E69" s="45"/>
+      <c r="A69" s="65"/>
+      <c r="B69" s="59"/>
+      <c r="C69" s="67"/>
+      <c r="D69" s="59"/>
+      <c r="E69" s="59"/>
       <c r="F69" s="30"/>
       <c r="G69" s="35"/>
       <c r="H69" s="35"/>
-      <c r="I69" s="51"/>
-      <c r="J69" s="48"/>
-      <c r="K69" s="51"/>
+      <c r="I69" s="50"/>
+      <c r="J69" s="53"/>
+      <c r="K69" s="50"/>
       <c r="L69" s="2"/>
       <c r="M69" s="2"/>
       <c r="N69" s="2"/>
@@ -4151,17 +4225,17 @@
       <c r="AA69" s="2"/>
     </row>
     <row r="70" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A70" s="77"/>
-      <c r="B70" s="45"/>
-      <c r="C70" s="57"/>
-      <c r="D70" s="45"/>
-      <c r="E70" s="45"/>
+      <c r="A70" s="65"/>
+      <c r="B70" s="59"/>
+      <c r="C70" s="67"/>
+      <c r="D70" s="59"/>
+      <c r="E70" s="59"/>
       <c r="F70" s="30"/>
       <c r="G70" s="35"/>
       <c r="H70" s="35"/>
-      <c r="I70" s="51"/>
-      <c r="J70" s="48"/>
-      <c r="K70" s="51"/>
+      <c r="I70" s="50"/>
+      <c r="J70" s="53"/>
+      <c r="K70" s="50"/>
       <c r="L70" s="2"/>
       <c r="M70" s="2"/>
       <c r="N70" s="2"/>
@@ -4180,17 +4254,17 @@
       <c r="AA70" s="2"/>
     </row>
     <row r="71" spans="1:27">
-      <c r="A71" s="78"/>
-      <c r="B71" s="46"/>
-      <c r="C71" s="58"/>
-      <c r="D71" s="46"/>
-      <c r="E71" s="46"/>
+      <c r="A71" s="66"/>
+      <c r="B71" s="60"/>
+      <c r="C71" s="68"/>
+      <c r="D71" s="60"/>
+      <c r="E71" s="60"/>
       <c r="F71" s="30"/>
       <c r="G71" s="35"/>
       <c r="H71" s="35"/>
-      <c r="I71" s="52"/>
-      <c r="J71" s="49"/>
-      <c r="K71" s="52"/>
+      <c r="I71" s="51"/>
+      <c r="J71" s="54"/>
+      <c r="K71" s="51"/>
       <c r="L71" s="2"/>
       <c r="M71" s="2"/>
       <c r="N71" s="2"/>
@@ -4209,21 +4283,37 @@
       <c r="AA71" s="2"/>
     </row>
     <row r="72" spans="1:27">
-      <c r="A72" s="53" t="s">
+      <c r="A72" s="55" t="s">
         <v>46</v>
       </c>
-      <c r="B72" s="44"/>
-      <c r="C72" s="44"/>
-      <c r="D72" s="44"/>
-      <c r="E72" s="44"/>
-      <c r="F72" s="30"/>
-      <c r="G72" s="35"/>
-      <c r="H72" s="35"/>
-      <c r="I72" s="50" t="s">
+      <c r="B72" s="46" t="s">
+        <v>138</v>
+      </c>
+      <c r="C72" s="46" t="s">
+        <v>139</v>
+      </c>
+      <c r="D72" s="46" t="s">
+        <v>140</v>
+      </c>
+      <c r="E72" s="46" t="s">
+        <v>141</v>
+      </c>
+      <c r="F72" s="44" t="s">
+        <v>53</v>
+      </c>
+      <c r="G72" s="45" t="s">
+        <v>142</v>
+      </c>
+      <c r="H72" s="45" t="s">
+        <v>143</v>
+      </c>
+      <c r="I72" s="49" t="s">
         <v>26</v>
       </c>
-      <c r="J72" s="47"/>
-      <c r="K72" s="50" t="s">
+      <c r="J72" s="52" t="s">
+        <v>56</v>
+      </c>
+      <c r="K72" s="49" t="s">
         <v>28</v>
       </c>
       <c r="L72" s="2"/>
@@ -4244,17 +4334,21 @@
       <c r="AA72" s="2"/>
     </row>
     <row r="73" spans="1:27">
-      <c r="A73" s="54"/>
-      <c r="B73" s="45"/>
-      <c r="C73" s="45"/>
-      <c r="D73" s="45"/>
-      <c r="E73" s="45"/>
-      <c r="F73" s="30"/>
-      <c r="G73" s="36"/>
-      <c r="H73" s="36"/>
-      <c r="I73" s="51"/>
-      <c r="J73" s="48"/>
-      <c r="K73" s="51"/>
+      <c r="A73" s="56"/>
+      <c r="B73" s="47"/>
+      <c r="C73" s="47"/>
+      <c r="D73" s="47"/>
+      <c r="E73" s="47"/>
+      <c r="F73" s="44" t="s">
+        <v>67</v>
+      </c>
+      <c r="G73" s="45" t="s">
+        <v>144</v>
+      </c>
+      <c r="H73" s="45"/>
+      <c r="I73" s="50"/>
+      <c r="J73" s="53"/>
+      <c r="K73" s="50"/>
       <c r="L73" s="2"/>
       <c r="M73" s="2"/>
       <c r="N73" s="2"/>
@@ -4273,17 +4367,23 @@
       <c r="AA73" s="2"/>
     </row>
     <row r="74" spans="1:27">
-      <c r="A74" s="54"/>
-      <c r="B74" s="45"/>
-      <c r="C74" s="45"/>
-      <c r="D74" s="45"/>
-      <c r="E74" s="45"/>
-      <c r="F74" s="30"/>
-      <c r="G74" s="36"/>
-      <c r="H74" s="36"/>
-      <c r="I74" s="51"/>
-      <c r="J74" s="48"/>
-      <c r="K74" s="51"/>
+      <c r="A74" s="56"/>
+      <c r="B74" s="47"/>
+      <c r="C74" s="47"/>
+      <c r="D74" s="47"/>
+      <c r="E74" s="47"/>
+      <c r="F74" s="44" t="s">
+        <v>70</v>
+      </c>
+      <c r="G74" s="45" t="s">
+        <v>145</v>
+      </c>
+      <c r="H74" s="45" t="s">
+        <v>146</v>
+      </c>
+      <c r="I74" s="50"/>
+      <c r="J74" s="53"/>
+      <c r="K74" s="50"/>
       <c r="L74" s="2"/>
       <c r="M74" s="2"/>
       <c r="N74" s="2"/>
@@ -4302,17 +4402,23 @@
       <c r="AA74" s="2"/>
     </row>
     <row r="75" spans="1:27">
-      <c r="A75" s="55"/>
-      <c r="B75" s="46"/>
-      <c r="C75" s="46"/>
-      <c r="D75" s="46"/>
-      <c r="E75" s="46"/>
-      <c r="F75" s="30"/>
-      <c r="G75" s="35"/>
-      <c r="H75" s="36"/>
-      <c r="I75" s="52"/>
-      <c r="J75" s="49"/>
-      <c r="K75" s="52"/>
+      <c r="A75" s="57"/>
+      <c r="B75" s="48"/>
+      <c r="C75" s="48"/>
+      <c r="D75" s="48"/>
+      <c r="E75" s="48"/>
+      <c r="F75" s="44" t="s">
+        <v>99</v>
+      </c>
+      <c r="G75" s="45" t="s">
+        <v>147</v>
+      </c>
+      <c r="H75" s="45" t="s">
+        <v>163</v>
+      </c>
+      <c r="I75" s="51"/>
+      <c r="J75" s="54"/>
+      <c r="K75" s="51"/>
       <c r="L75" s="2"/>
       <c r="M75" s="2"/>
       <c r="N75" s="2"/>
@@ -4331,21 +4437,37 @@
       <c r="AA75" s="2"/>
     </row>
     <row r="76" spans="1:27">
-      <c r="A76" s="53" t="s">
+      <c r="A76" s="55" t="s">
         <v>47</v>
       </c>
-      <c r="B76" s="44"/>
-      <c r="C76" s="44"/>
-      <c r="D76" s="44"/>
-      <c r="E76" s="44"/>
-      <c r="F76" s="30"/>
-      <c r="G76" s="35"/>
-      <c r="H76" s="35"/>
-      <c r="I76" s="50" t="s">
+      <c r="B76" s="46" t="s">
+        <v>138</v>
+      </c>
+      <c r="C76" s="46" t="s">
+        <v>148</v>
+      </c>
+      <c r="D76" s="46" t="s">
+        <v>149</v>
+      </c>
+      <c r="E76" s="46" t="s">
+        <v>141</v>
+      </c>
+      <c r="F76" s="44" t="s">
+        <v>53</v>
+      </c>
+      <c r="G76" s="45" t="s">
+        <v>142</v>
+      </c>
+      <c r="H76" s="45" t="s">
+        <v>143</v>
+      </c>
+      <c r="I76" s="49" t="s">
         <v>26</v>
       </c>
-      <c r="J76" s="47"/>
-      <c r="K76" s="50" t="s">
+      <c r="J76" s="52" t="s">
+        <v>56</v>
+      </c>
+      <c r="K76" s="49" t="s">
         <v>28</v>
       </c>
       <c r="L76" s="2"/>
@@ -4366,17 +4488,23 @@
       <c r="AA76" s="2"/>
     </row>
     <row r="77" spans="1:27">
-      <c r="A77" s="54"/>
-      <c r="B77" s="45"/>
-      <c r="C77" s="45"/>
-      <c r="D77" s="45"/>
-      <c r="E77" s="45"/>
-      <c r="F77" s="30"/>
-      <c r="G77" s="35"/>
-      <c r="H77" s="36"/>
-      <c r="I77" s="51"/>
-      <c r="J77" s="48"/>
-      <c r="K77" s="51"/>
+      <c r="A77" s="56"/>
+      <c r="B77" s="47"/>
+      <c r="C77" s="47"/>
+      <c r="D77" s="47"/>
+      <c r="E77" s="47"/>
+      <c r="F77" s="44" t="s">
+        <v>67</v>
+      </c>
+      <c r="G77" s="45" t="s">
+        <v>150</v>
+      </c>
+      <c r="H77" s="45" t="s">
+        <v>146</v>
+      </c>
+      <c r="I77" s="50"/>
+      <c r="J77" s="53"/>
+      <c r="K77" s="50"/>
       <c r="L77" s="2"/>
       <c r="M77" s="2"/>
       <c r="N77" s="2"/>
@@ -4395,17 +4523,23 @@
       <c r="AA77" s="2"/>
     </row>
     <row r="78" spans="1:27">
-      <c r="A78" s="54"/>
-      <c r="B78" s="45"/>
-      <c r="C78" s="45"/>
-      <c r="D78" s="45"/>
-      <c r="E78" s="45"/>
-      <c r="F78" s="30"/>
-      <c r="G78" s="36"/>
-      <c r="H78" s="36"/>
-      <c r="I78" s="51"/>
-      <c r="J78" s="48"/>
-      <c r="K78" s="51"/>
+      <c r="A78" s="56"/>
+      <c r="B78" s="47"/>
+      <c r="C78" s="47"/>
+      <c r="D78" s="47"/>
+      <c r="E78" s="47"/>
+      <c r="F78" s="44" t="s">
+        <v>70</v>
+      </c>
+      <c r="G78" s="45" t="s">
+        <v>147</v>
+      </c>
+      <c r="H78" s="45" t="s">
+        <v>151</v>
+      </c>
+      <c r="I78" s="50"/>
+      <c r="J78" s="53"/>
+      <c r="K78" s="50"/>
       <c r="L78" s="2"/>
       <c r="M78" s="2"/>
       <c r="N78" s="2"/>
@@ -4424,17 +4558,19 @@
       <c r="AA78" s="2"/>
     </row>
     <row r="79" spans="1:27">
-      <c r="A79" s="55"/>
-      <c r="B79" s="46"/>
-      <c r="C79" s="46"/>
-      <c r="D79" s="46"/>
-      <c r="E79" s="46"/>
-      <c r="F79" s="30"/>
-      <c r="G79" s="35"/>
-      <c r="H79" s="35"/>
-      <c r="I79" s="52"/>
-      <c r="J79" s="49"/>
-      <c r="K79" s="52"/>
+      <c r="A79" s="57"/>
+      <c r="B79" s="48"/>
+      <c r="C79" s="48"/>
+      <c r="D79" s="48"/>
+      <c r="E79" s="48"/>
+      <c r="F79" s="44" t="s">
+        <v>99</v>
+      </c>
+      <c r="G79" s="45"/>
+      <c r="H79" s="45"/>
+      <c r="I79" s="51"/>
+      <c r="J79" s="54"/>
+      <c r="K79" s="51"/>
       <c r="L79" s="2"/>
       <c r="M79" s="2"/>
       <c r="N79" s="2"/>
@@ -4453,21 +4589,37 @@
       <c r="AA79" s="2"/>
     </row>
     <row r="80" spans="1:27">
-      <c r="A80" s="53" t="s">
+      <c r="A80" s="55" t="s">
         <v>48</v>
       </c>
-      <c r="B80" s="44"/>
-      <c r="C80" s="56"/>
-      <c r="D80" s="44"/>
-      <c r="E80" s="44"/>
-      <c r="F80" s="30"/>
-      <c r="G80" s="35"/>
-      <c r="H80" s="35"/>
-      <c r="I80" s="50" t="s">
+      <c r="B80" s="46" t="s">
+        <v>138</v>
+      </c>
+      <c r="C80" s="46" t="s">
+        <v>152</v>
+      </c>
+      <c r="D80" s="46" t="s">
+        <v>153</v>
+      </c>
+      <c r="E80" s="46" t="s">
+        <v>141</v>
+      </c>
+      <c r="F80" s="44" t="s">
+        <v>53</v>
+      </c>
+      <c r="G80" s="45" t="s">
+        <v>142</v>
+      </c>
+      <c r="H80" s="45" t="s">
+        <v>143</v>
+      </c>
+      <c r="I80" s="49" t="s">
         <v>26</v>
       </c>
-      <c r="J80" s="47"/>
-      <c r="K80" s="50" t="s">
+      <c r="J80" s="52" t="s">
+        <v>56</v>
+      </c>
+      <c r="K80" s="49" t="s">
         <v>28</v>
       </c>
       <c r="L80" s="2"/>
@@ -4488,17 +4640,21 @@
       <c r="AA80" s="2"/>
     </row>
     <row r="81" spans="1:27">
-      <c r="A81" s="54"/>
-      <c r="B81" s="45"/>
-      <c r="C81" s="57"/>
-      <c r="D81" s="45"/>
-      <c r="E81" s="45"/>
-      <c r="F81" s="30"/>
-      <c r="G81" s="35"/>
-      <c r="H81" s="35"/>
-      <c r="I81" s="51"/>
-      <c r="J81" s="48"/>
-      <c r="K81" s="51"/>
+      <c r="A81" s="56"/>
+      <c r="B81" s="47"/>
+      <c r="C81" s="47"/>
+      <c r="D81" s="47"/>
+      <c r="E81" s="47"/>
+      <c r="F81" s="44" t="s">
+        <v>67</v>
+      </c>
+      <c r="G81" s="45" t="s">
+        <v>154</v>
+      </c>
+      <c r="H81" s="45"/>
+      <c r="I81" s="50"/>
+      <c r="J81" s="53"/>
+      <c r="K81" s="50"/>
       <c r="L81" s="2"/>
       <c r="M81" s="2"/>
       <c r="N81" s="2"/>
@@ -4517,17 +4673,23 @@
       <c r="AA81" s="2"/>
     </row>
     <row r="82" spans="1:27">
-      <c r="A82" s="54"/>
-      <c r="B82" s="45"/>
-      <c r="C82" s="57"/>
-      <c r="D82" s="45"/>
-      <c r="E82" s="45"/>
-      <c r="F82" s="30"/>
-      <c r="G82" s="35"/>
-      <c r="H82" s="35"/>
-      <c r="I82" s="51"/>
-      <c r="J82" s="48"/>
-      <c r="K82" s="51"/>
+      <c r="A82" s="56"/>
+      <c r="B82" s="47"/>
+      <c r="C82" s="47"/>
+      <c r="D82" s="47"/>
+      <c r="E82" s="47"/>
+      <c r="F82" s="44" t="s">
+        <v>70</v>
+      </c>
+      <c r="G82" s="45" t="s">
+        <v>155</v>
+      </c>
+      <c r="H82" s="45" t="s">
+        <v>146</v>
+      </c>
+      <c r="I82" s="50"/>
+      <c r="J82" s="53"/>
+      <c r="K82" s="50"/>
       <c r="L82" s="2"/>
       <c r="M82" s="2"/>
       <c r="N82" s="2"/>
@@ -4546,17 +4708,23 @@
       <c r="AA82" s="2"/>
     </row>
     <row r="83" spans="1:27">
-      <c r="A83" s="55"/>
-      <c r="B83" s="46"/>
-      <c r="C83" s="58"/>
-      <c r="D83" s="46"/>
-      <c r="E83" s="46"/>
-      <c r="F83" s="30"/>
-      <c r="G83" s="35"/>
-      <c r="H83" s="35"/>
-      <c r="I83" s="52"/>
-      <c r="J83" s="49"/>
-      <c r="K83" s="52"/>
+      <c r="A83" s="57"/>
+      <c r="B83" s="48"/>
+      <c r="C83" s="48"/>
+      <c r="D83" s="48"/>
+      <c r="E83" s="48"/>
+      <c r="F83" s="44" t="s">
+        <v>99</v>
+      </c>
+      <c r="G83" s="45" t="s">
+        <v>147</v>
+      </c>
+      <c r="H83" s="45" t="s">
+        <v>156</v>
+      </c>
+      <c r="I83" s="51"/>
+      <c r="J83" s="54"/>
+      <c r="K83" s="51"/>
       <c r="L83" s="2"/>
       <c r="M83" s="2"/>
       <c r="N83" s="2"/>
@@ -4575,16 +4743,36 @@
       <c r="AA83" s="2"/>
     </row>
     <row r="84" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A84" s="2"/>
-      <c r="B84" s="38"/>
-      <c r="C84" s="2"/>
-      <c r="D84" s="38"/>
-      <c r="E84" s="38"/>
-      <c r="F84" s="2"/>
-      <c r="G84" s="38"/>
-      <c r="H84" s="38"/>
-      <c r="I84" s="2"/>
-      <c r="J84" s="38"/>
+      <c r="A84" s="55" t="s">
+        <v>162</v>
+      </c>
+      <c r="B84" s="46" t="s">
+        <v>138</v>
+      </c>
+      <c r="C84" s="46" t="s">
+        <v>157</v>
+      </c>
+      <c r="D84" s="46" t="s">
+        <v>158</v>
+      </c>
+      <c r="E84" s="46" t="s">
+        <v>141</v>
+      </c>
+      <c r="F84" s="44" t="s">
+        <v>53</v>
+      </c>
+      <c r="G84" s="45" t="s">
+        <v>142</v>
+      </c>
+      <c r="H84" s="45" t="s">
+        <v>143</v>
+      </c>
+      <c r="I84" s="49" t="s">
+        <v>26</v>
+      </c>
+      <c r="J84" s="52" t="s">
+        <v>56</v>
+      </c>
       <c r="K84" s="2"/>
       <c r="L84" s="2"/>
       <c r="M84" s="2"/>
@@ -4603,17 +4791,23 @@
       <c r="Z84" s="2"/>
       <c r="AA84" s="2"/>
     </row>
-    <row r="85" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A85" s="2"/>
-      <c r="B85" s="38"/>
-      <c r="C85" s="2"/>
-      <c r="D85" s="38"/>
-      <c r="E85" s="38"/>
-      <c r="F85" s="2"/>
-      <c r="G85" s="38"/>
-      <c r="H85" s="38"/>
-      <c r="I85" s="2"/>
-      <c r="J85" s="38"/>
+    <row r="85" spans="1:27" ht="24" customHeight="1">
+      <c r="A85" s="56"/>
+      <c r="B85" s="47"/>
+      <c r="C85" s="47"/>
+      <c r="D85" s="47"/>
+      <c r="E85" s="47"/>
+      <c r="F85" s="44" t="s">
+        <v>67</v>
+      </c>
+      <c r="G85" s="45" t="s">
+        <v>159</v>
+      </c>
+      <c r="H85" s="45" t="s">
+        <v>160</v>
+      </c>
+      <c r="I85" s="50"/>
+      <c r="J85" s="53"/>
       <c r="K85" s="2"/>
       <c r="L85" s="2"/>
       <c r="M85" s="2"/>
@@ -4633,16 +4827,22 @@
       <c r="AA85" s="2"/>
     </row>
     <row r="86" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A86" s="2"/>
-      <c r="B86" s="38"/>
-      <c r="C86" s="2"/>
-      <c r="D86" s="38"/>
-      <c r="E86" s="38"/>
-      <c r="F86" s="2"/>
-      <c r="G86" s="38"/>
-      <c r="H86" s="38"/>
-      <c r="I86" s="2"/>
-      <c r="J86" s="38"/>
+      <c r="A86" s="56"/>
+      <c r="B86" s="47"/>
+      <c r="C86" s="47"/>
+      <c r="D86" s="47"/>
+      <c r="E86" s="47"/>
+      <c r="F86" s="44" t="s">
+        <v>70</v>
+      </c>
+      <c r="G86" s="45" t="s">
+        <v>147</v>
+      </c>
+      <c r="H86" s="45" t="s">
+        <v>161</v>
+      </c>
+      <c r="I86" s="50"/>
+      <c r="J86" s="53"/>
       <c r="K86" s="2"/>
       <c r="L86" s="2"/>
       <c r="M86" s="2"/>
@@ -4662,16 +4862,16 @@
       <c r="AA86" s="2"/>
     </row>
     <row r="87" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A87" s="2"/>
-      <c r="B87" s="38"/>
-      <c r="C87" s="2"/>
-      <c r="D87" s="38"/>
-      <c r="E87" s="38"/>
-      <c r="F87" s="2"/>
-      <c r="G87" s="38"/>
-      <c r="H87" s="38"/>
-      <c r="I87" s="2"/>
-      <c r="J87" s="38"/>
+      <c r="A87" s="57"/>
+      <c r="B87" s="48"/>
+      <c r="C87" s="48"/>
+      <c r="D87" s="48"/>
+      <c r="E87" s="48"/>
+      <c r="F87" s="44"/>
+      <c r="G87" s="45"/>
+      <c r="H87" s="45"/>
+      <c r="I87" s="51"/>
+      <c r="J87" s="54"/>
       <c r="K87" s="2"/>
       <c r="L87" s="2"/>
       <c r="M87" s="2"/>
@@ -29283,7 +29483,7 @@
       <c r="AA935" s="6"/>
     </row>
   </sheetData>
-  <mergeCells count="178">
+  <mergeCells count="185">
     <mergeCell ref="C32:C35"/>
     <mergeCell ref="B32:B35"/>
     <mergeCell ref="B28:B31"/>
@@ -29402,8 +29602,6 @@
     <mergeCell ref="I56:I59"/>
     <mergeCell ref="I44:I47"/>
     <mergeCell ref="J40:J43"/>
-    <mergeCell ref="A60:A63"/>
-    <mergeCell ref="J56:J59"/>
     <mergeCell ref="K56:K59"/>
     <mergeCell ref="J60:J63"/>
     <mergeCell ref="K60:K63"/>
@@ -29426,13 +29624,6 @@
     <mergeCell ref="A64:A67"/>
     <mergeCell ref="J64:J67"/>
     <mergeCell ref="K64:K67"/>
-    <mergeCell ref="A76:A79"/>
-    <mergeCell ref="B76:B79"/>
-    <mergeCell ref="C76:C79"/>
-    <mergeCell ref="D76:D79"/>
-    <mergeCell ref="E76:E79"/>
-    <mergeCell ref="I76:I79"/>
-    <mergeCell ref="J76:J79"/>
     <mergeCell ref="K76:K79"/>
     <mergeCell ref="J80:J83"/>
     <mergeCell ref="K80:K83"/>
@@ -29442,11 +29633,6 @@
     <mergeCell ref="D80:D83"/>
     <mergeCell ref="E80:E83"/>
     <mergeCell ref="I80:I83"/>
-    <mergeCell ref="B36:B39"/>
-    <mergeCell ref="C36:C39"/>
-    <mergeCell ref="D36:D39"/>
-    <mergeCell ref="E36:E39"/>
-    <mergeCell ref="J44:J47"/>
     <mergeCell ref="K44:K47"/>
     <mergeCell ref="I48:I51"/>
     <mergeCell ref="J48:J51"/>
@@ -29458,113 +29644,134 @@
     <mergeCell ref="K40:K43"/>
     <mergeCell ref="I40:I43"/>
     <mergeCell ref="B40:B43"/>
-    <mergeCell ref="J36:J39"/>
     <mergeCell ref="C40:C43"/>
     <mergeCell ref="D40:D43"/>
     <mergeCell ref="E40:E43"/>
+    <mergeCell ref="B84:B87"/>
+    <mergeCell ref="C84:C87"/>
+    <mergeCell ref="D84:D87"/>
+    <mergeCell ref="E84:E87"/>
+    <mergeCell ref="I84:I87"/>
+    <mergeCell ref="J84:J87"/>
+    <mergeCell ref="A84:A87"/>
+    <mergeCell ref="B36:B39"/>
+    <mergeCell ref="C36:C39"/>
+    <mergeCell ref="D36:D39"/>
+    <mergeCell ref="E36:E39"/>
+    <mergeCell ref="J44:J47"/>
+    <mergeCell ref="J36:J39"/>
+    <mergeCell ref="A76:A79"/>
+    <mergeCell ref="B76:B79"/>
+    <mergeCell ref="C76:C79"/>
+    <mergeCell ref="D76:D79"/>
+    <mergeCell ref="E76:E79"/>
+    <mergeCell ref="I76:I79"/>
+    <mergeCell ref="J76:J79"/>
+    <mergeCell ref="A60:A63"/>
+    <mergeCell ref="J56:J59"/>
   </mergeCells>
-  <conditionalFormatting sqref="I72 I76 I80">
-    <cfRule type="cellIs" dxfId="23" priority="117" operator="equal">
-      <formula>"TO DO"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I72 I76 I80">
-    <cfRule type="cellIs" dxfId="22" priority="118" operator="equal">
-      <formula>"IN PROGRESS"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I72 I76 I80">
-    <cfRule type="cellIs" dxfId="21" priority="119" operator="equal">
-      <formula>"REVIEWED"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I72 I76 I80">
-    <cfRule type="cellIs" dxfId="20" priority="120" operator="equal">
-      <formula>"IN REVIEW"</formula>
-    </cfRule>
-  </conditionalFormatting>
   <conditionalFormatting sqref="I4 I8 I12">
-    <cfRule type="cellIs" dxfId="19" priority="13" operator="equal">
+    <cfRule type="cellIs" dxfId="19" priority="17" operator="equal">
       <formula>"TO DO"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I4 I8 I12">
-    <cfRule type="cellIs" dxfId="18" priority="14" operator="equal">
+    <cfRule type="cellIs" dxfId="18" priority="18" operator="equal">
       <formula>"IN PROGRESS"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I4 I8 I12">
-    <cfRule type="cellIs" dxfId="17" priority="15" operator="equal">
+    <cfRule type="cellIs" dxfId="17" priority="19" operator="equal">
       <formula>"REVIEWED"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I4 I8 I12">
-    <cfRule type="cellIs" dxfId="16" priority="16" operator="equal">
+    <cfRule type="cellIs" dxfId="16" priority="20" operator="equal">
       <formula>"IN REVIEW"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I16 I20 I24">
-    <cfRule type="cellIs" dxfId="15" priority="9" operator="equal">
+    <cfRule type="cellIs" dxfId="15" priority="13" operator="equal">
       <formula>"TO DO"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I16 I20 I24">
-    <cfRule type="cellIs" dxfId="14" priority="10" operator="equal">
+    <cfRule type="cellIs" dxfId="14" priority="14" operator="equal">
       <formula>"IN PROGRESS"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I16 I20 I24">
-    <cfRule type="cellIs" dxfId="13" priority="11" operator="equal">
+    <cfRule type="cellIs" dxfId="13" priority="15" operator="equal">
       <formula>"REVIEWED"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I16 I20 I24">
-    <cfRule type="cellIs" dxfId="12" priority="12" operator="equal">
+    <cfRule type="cellIs" dxfId="12" priority="16" operator="equal">
       <formula>"IN REVIEW"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I28 I32 I36 I40 I44 I48 I52 I56 I60">
-    <cfRule type="cellIs" dxfId="11" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="11" priority="9" operator="equal">
       <formula>"TO DO"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I28 I32 I36 I40 I44 I48 I52 I56 I60">
-    <cfRule type="cellIs" dxfId="10" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="10" priority="10" operator="equal">
       <formula>"IN PROGRESS"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I28 I32 I36 I40 I44 I48 I52 I56 I60">
-    <cfRule type="cellIs" dxfId="9" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="9" priority="11" operator="equal">
       <formula>"REVIEWED"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I28 I32 I36 I40 I44 I48 I52 I56 I60">
-    <cfRule type="cellIs" dxfId="8" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="8" priority="12" operator="equal">
       <formula>"IN REVIEW"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I64 I68">
-    <cfRule type="cellIs" dxfId="7" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="7" priority="5" operator="equal">
       <formula>"TO DO"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I64 I68">
-    <cfRule type="cellIs" dxfId="5" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="6" priority="6" operator="equal">
       <formula>"IN PROGRESS"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I64 I68">
-    <cfRule type="cellIs" dxfId="3" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="5" priority="7" operator="equal">
       <formula>"REVIEWED"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I64 I68">
-    <cfRule type="cellIs" dxfId="1" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="4" priority="8" operator="equal">
+      <formula>"IN REVIEW"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I76 I72 I80 I84">
+    <cfRule type="cellIs" dxfId="3" priority="1" operator="equal">
+      <formula>"TO DO"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I76 I72 I80 I84">
+    <cfRule type="cellIs" dxfId="2" priority="2" operator="equal">
+      <formula>"IN PROGRESS"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I76 I72 I80 I84">
+    <cfRule type="cellIs" dxfId="1" priority="3" operator="equal">
+      <formula>"REVIEWED"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I76 I72 I80 I84">
+    <cfRule type="cellIs" dxfId="0" priority="4" operator="equal">
       <formula>"IN REVIEW"</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" sqref="I72 I76 I24 I16 I20 I4 I8 I12 I80 I56 I60 I32 I36 I28 I40 I44 I48 I52 I64 I68">
+    <dataValidation type="list" allowBlank="1" sqref="I52 I64 I24 I16 I20 I4 I8 I12 I68 I56 I60 I32 I36 I28 I40 I44 I48 I84 I76 I72 I80">
       <formula1>"TO DO,In Progress,In Review,Reviewed"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" sqref="K76 K36 K40 K32 K28 K4 K12 K8 K48 K44 K52 K60 K56 K64 K68 K72 K80 K20 K24 K16">

</xml_diff>

<commit_message>
Agrego Casos de Prueba referentes a la usabilidad de la web
</commit_message>
<xml_diff>
--- a/Testing 2024/template_caso_prueba-ISPC2024-sprint-1.xlsx
+++ b/Testing 2024/template_caso_prueba-ISPC2024-sprint-1.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="348" uniqueCount="164">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="363" uniqueCount="170">
   <si>
     <t>Id</t>
   </si>
@@ -518,6 +518,24 @@
   <si>
     <t>Ver los datos del libro cargados en la BDD, status 201</t>
   </si>
+  <si>
+    <t>El logotipo redirige a la home page</t>
+  </si>
+  <si>
+    <t>El logotipo debe ser cliqueable y redirigir a la home page</t>
+  </si>
+  <si>
+    <t>El usuario debe encontrarse situado en alguna seccion de la pagina diferente a la home page</t>
+  </si>
+  <si>
+    <t>Hace click en el logotipo</t>
+  </si>
+  <si>
+    <t>Se visualiza nuevamente la home page</t>
+  </si>
+  <si>
+    <t>TC-022</t>
+  </si>
 </sst>
 </file>
 
@@ -593,7 +611,7 @@
       <name val="ArialMT"/>
     </font>
   </fonts>
-  <fills count="15">
+  <fills count="16">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -675,6 +693,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFF0CDF3"/>
+        <bgColor rgb="FFFFFFCC"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF6DDBC"/>
         <bgColor rgb="FFFFFFCC"/>
       </patternFill>
     </fill>
@@ -949,7 +973,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="86">
+  <cellXfs count="93">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -1050,38 +1074,6 @@
     <xf numFmtId="0" fontId="11" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="14" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="14" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="14" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1091,62 +1083,14 @@
     <xf numFmtId="0" fontId="1" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="12" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="12" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="12" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="13" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="13" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="13" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="11" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="9" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="10" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1166,11 +1110,174 @@
     <xf numFmtId="0" fontId="1" fillId="11" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="9" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="12" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="12" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="12" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="14" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="14" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="14" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="13" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="13" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="13" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="15" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="15" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="15" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="20">
+  <dxfs count="28">
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFCE5CD"/>
+          <bgColor rgb="FFFCE5CD"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFCE5CD"/>
+          <bgColor rgb="FFFCE5CD"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF93C47D"/>
+          <bgColor rgb="FF93C47D"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF93C47D"/>
+          <bgColor rgb="FF93C47D"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFF2CC"/>
+          <bgColor rgb="FFFFF2CC"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFF2CC"/>
+          <bgColor rgb="FFFFF2CC"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFA2C4C9"/>
+          <bgColor rgb="FFA2C4C9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFA2C4C9"/>
+          <bgColor rgb="FFA2C4C9"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill patternType="solid">
@@ -1401,8 +1508,8 @@
       <rgbColor rgb="00333333"/>
     </indexedColors>
     <mruColors>
+      <color rgb="FFF6DDBC"/>
       <color rgb="FFF0CDF3"/>
-      <color rgb="FFF6DDBC"/>
     </mruColors>
   </colors>
   <extLst>
@@ -1681,8 +1788,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AA935"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="60" workbookViewId="0">
-      <selection activeCell="H89" sqref="H89"/>
+    <sheetView tabSelected="1" topLeftCell="A70" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="60" workbookViewId="0">
+      <selection activeCell="E95" sqref="E95"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5703125" defaultRowHeight="12.75"/>
@@ -1731,33 +1838,33 @@
       <c r="AA1" s="2"/>
     </row>
     <row r="2" spans="1:27" s="31" customFormat="1" ht="15.75" customHeight="1">
-      <c r="A2" s="71" t="s">
+      <c r="A2" s="68" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="69" t="s">
+      <c r="B2" s="58" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="71" t="s">
+      <c r="C2" s="68" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="69" t="s">
+      <c r="D2" s="58" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="69" t="s">
+      <c r="E2" s="58" t="s">
         <v>4</v>
       </c>
-      <c r="F2" s="75" t="s">
+      <c r="F2" s="63" t="s">
         <v>5</v>
       </c>
-      <c r="G2" s="76"/>
-      <c r="H2" s="77"/>
-      <c r="I2" s="78" t="s">
+      <c r="G2" s="64"/>
+      <c r="H2" s="65"/>
+      <c r="I2" s="66" t="s">
         <v>6</v>
       </c>
-      <c r="J2" s="69" t="s">
+      <c r="J2" s="58" t="s">
         <v>7</v>
       </c>
-      <c r="K2" s="69" t="s">
+      <c r="K2" s="58" t="s">
         <v>27</v>
       </c>
       <c r="L2" s="32"/>
@@ -1778,11 +1885,11 @@
       <c r="AA2" s="33"/>
     </row>
     <row r="3" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A3" s="72"/>
-      <c r="B3" s="70"/>
-      <c r="C3" s="72"/>
-      <c r="D3" s="70"/>
-      <c r="E3" s="70"/>
+      <c r="A3" s="69"/>
+      <c r="B3" s="59"/>
+      <c r="C3" s="69"/>
+      <c r="D3" s="59"/>
+      <c r="E3" s="59"/>
       <c r="F3" s="34" t="s">
         <v>8</v>
       </c>
@@ -1792,9 +1899,9 @@
       <c r="H3" s="42" t="s">
         <v>10</v>
       </c>
-      <c r="I3" s="79"/>
-      <c r="J3" s="70"/>
-      <c r="K3" s="70"/>
+      <c r="I3" s="67"/>
+      <c r="J3" s="59"/>
+      <c r="K3" s="59"/>
       <c r="L3" s="3"/>
       <c r="M3" s="2"/>
       <c r="N3" s="2"/>
@@ -1813,37 +1920,37 @@
       <c r="AA3" s="2"/>
     </row>
     <row r="4" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A4" s="80" t="s">
+      <c r="A4" s="52" t="s">
         <v>29</v>
       </c>
-      <c r="B4" s="58" t="s">
+      <c r="B4" s="46" t="s">
         <v>49</v>
       </c>
-      <c r="C4" s="58" t="s">
+      <c r="C4" s="46" t="s">
         <v>50</v>
       </c>
-      <c r="D4" s="58" t="s">
+      <c r="D4" s="46" t="s">
         <v>51</v>
       </c>
-      <c r="E4" s="58" t="s">
+      <c r="E4" s="46" t="s">
         <v>52</v>
       </c>
-      <c r="F4" s="58" t="s">
+      <c r="F4" s="46" t="s">
         <v>53</v>
       </c>
-      <c r="G4" s="58" t="s">
+      <c r="G4" s="46" t="s">
         <v>54</v>
       </c>
-      <c r="H4" s="73" t="s">
+      <c r="H4" s="70" t="s">
         <v>55</v>
       </c>
-      <c r="I4" s="49" t="s">
+      <c r="I4" s="60" t="s">
         <v>26</v>
       </c>
-      <c r="J4" s="52" t="s">
+      <c r="J4" s="72" t="s">
         <v>56</v>
       </c>
-      <c r="K4" s="49" t="s">
+      <c r="K4" s="60" t="s">
         <v>28</v>
       </c>
       <c r="L4" s="3"/>
@@ -1864,17 +1971,17 @@
       <c r="AA4" s="2"/>
     </row>
     <row r="5" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A5" s="81"/>
-      <c r="B5" s="59"/>
-      <c r="C5" s="59"/>
-      <c r="D5" s="59"/>
-      <c r="E5" s="59"/>
-      <c r="F5" s="60"/>
-      <c r="G5" s="60"/>
-      <c r="H5" s="74"/>
-      <c r="I5" s="50"/>
-      <c r="J5" s="53"/>
-      <c r="K5" s="50"/>
+      <c r="A5" s="53"/>
+      <c r="B5" s="47"/>
+      <c r="C5" s="47"/>
+      <c r="D5" s="47"/>
+      <c r="E5" s="47"/>
+      <c r="F5" s="48"/>
+      <c r="G5" s="48"/>
+      <c r="H5" s="71"/>
+      <c r="I5" s="61"/>
+      <c r="J5" s="73"/>
+      <c r="K5" s="61"/>
       <c r="L5" s="3"/>
       <c r="M5" s="2"/>
       <c r="N5" s="2"/>
@@ -1893,17 +2000,17 @@
       <c r="AA5" s="2"/>
     </row>
     <row r="6" spans="1:27" s="29" customFormat="1" ht="15.75" customHeight="1">
-      <c r="A6" s="81"/>
-      <c r="B6" s="59"/>
-      <c r="C6" s="59"/>
-      <c r="D6" s="59"/>
-      <c r="E6" s="59"/>
+      <c r="A6" s="53"/>
+      <c r="B6" s="47"/>
+      <c r="C6" s="47"/>
+      <c r="D6" s="47"/>
+      <c r="E6" s="47"/>
       <c r="F6" s="30"/>
       <c r="G6" s="35"/>
       <c r="H6" s="35"/>
-      <c r="I6" s="50"/>
-      <c r="J6" s="53"/>
-      <c r="K6" s="50"/>
+      <c r="I6" s="61"/>
+      <c r="J6" s="73"/>
+      <c r="K6" s="61"/>
       <c r="L6" s="27"/>
       <c r="M6" s="28"/>
       <c r="N6" s="28"/>
@@ -1922,17 +2029,17 @@
       <c r="AA6" s="28"/>
     </row>
     <row r="7" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A7" s="82"/>
-      <c r="B7" s="60"/>
-      <c r="C7" s="60"/>
-      <c r="D7" s="60"/>
-      <c r="E7" s="60"/>
+      <c r="A7" s="54"/>
+      <c r="B7" s="48"/>
+      <c r="C7" s="48"/>
+      <c r="D7" s="48"/>
+      <c r="E7" s="48"/>
       <c r="F7" s="30"/>
       <c r="G7" s="35"/>
       <c r="H7" s="35"/>
-      <c r="I7" s="51"/>
-      <c r="J7" s="54"/>
-      <c r="K7" s="51"/>
+      <c r="I7" s="62"/>
+      <c r="J7" s="74"/>
+      <c r="K7" s="62"/>
       <c r="L7" s="3"/>
       <c r="M7" s="2"/>
       <c r="N7" s="2"/>
@@ -1951,37 +2058,37 @@
       <c r="AA7" s="2"/>
     </row>
     <row r="8" spans="1:27">
-      <c r="A8" s="80" t="s">
+      <c r="A8" s="52" t="s">
         <v>30</v>
       </c>
-      <c r="B8" s="58" t="s">
+      <c r="B8" s="46" t="s">
         <v>49</v>
       </c>
-      <c r="C8" s="58" t="s">
+      <c r="C8" s="46" t="s">
         <v>57</v>
       </c>
-      <c r="D8" s="58" t="s">
+      <c r="D8" s="46" t="s">
         <v>58</v>
       </c>
-      <c r="E8" s="58" t="s">
+      <c r="E8" s="46" t="s">
         <v>59</v>
       </c>
-      <c r="F8" s="58" t="s">
+      <c r="F8" s="46" t="s">
         <v>53</v>
       </c>
-      <c r="G8" s="58" t="s">
+      <c r="G8" s="46" t="s">
         <v>54</v>
       </c>
-      <c r="H8" s="73" t="s">
+      <c r="H8" s="70" t="s">
         <v>55</v>
       </c>
-      <c r="I8" s="49" t="s">
+      <c r="I8" s="60" t="s">
         <v>26</v>
       </c>
-      <c r="J8" s="52" t="s">
+      <c r="J8" s="72" t="s">
         <v>56</v>
       </c>
-      <c r="K8" s="49" t="s">
+      <c r="K8" s="60" t="s">
         <v>28</v>
       </c>
       <c r="L8" s="3"/>
@@ -2002,17 +2109,17 @@
       <c r="AA8" s="2"/>
     </row>
     <row r="9" spans="1:27">
-      <c r="A9" s="81"/>
-      <c r="B9" s="59"/>
-      <c r="C9" s="59"/>
-      <c r="D9" s="59"/>
-      <c r="E9" s="59"/>
-      <c r="F9" s="60"/>
-      <c r="G9" s="60"/>
-      <c r="H9" s="74"/>
-      <c r="I9" s="50"/>
-      <c r="J9" s="53"/>
-      <c r="K9" s="50"/>
+      <c r="A9" s="53"/>
+      <c r="B9" s="47"/>
+      <c r="C9" s="47"/>
+      <c r="D9" s="47"/>
+      <c r="E9" s="47"/>
+      <c r="F9" s="48"/>
+      <c r="G9" s="48"/>
+      <c r="H9" s="71"/>
+      <c r="I9" s="61"/>
+      <c r="J9" s="73"/>
+      <c r="K9" s="61"/>
       <c r="L9" s="3"/>
       <c r="M9" s="2"/>
       <c r="N9" s="2"/>
@@ -2031,17 +2138,17 @@
       <c r="AA9" s="2"/>
     </row>
     <row r="10" spans="1:27" s="29" customFormat="1" ht="15.75" customHeight="1">
-      <c r="A10" s="81"/>
-      <c r="B10" s="59"/>
-      <c r="C10" s="59"/>
-      <c r="D10" s="59"/>
-      <c r="E10" s="59"/>
+      <c r="A10" s="53"/>
+      <c r="B10" s="47"/>
+      <c r="C10" s="47"/>
+      <c r="D10" s="47"/>
+      <c r="E10" s="47"/>
       <c r="F10" s="30"/>
       <c r="G10" s="35"/>
       <c r="H10" s="35"/>
-      <c r="I10" s="50"/>
-      <c r="J10" s="53"/>
-      <c r="K10" s="50"/>
+      <c r="I10" s="61"/>
+      <c r="J10" s="73"/>
+      <c r="K10" s="61"/>
       <c r="L10" s="27"/>
       <c r="M10" s="28"/>
       <c r="N10" s="28"/>
@@ -2060,17 +2167,17 @@
       <c r="AA10" s="28"/>
     </row>
     <row r="11" spans="1:27">
-      <c r="A11" s="82"/>
-      <c r="B11" s="60"/>
-      <c r="C11" s="60"/>
-      <c r="D11" s="60"/>
-      <c r="E11" s="60"/>
+      <c r="A11" s="54"/>
+      <c r="B11" s="48"/>
+      <c r="C11" s="48"/>
+      <c r="D11" s="48"/>
+      <c r="E11" s="48"/>
       <c r="F11" s="30"/>
       <c r="G11" s="35"/>
       <c r="H11" s="35"/>
-      <c r="I11" s="51"/>
-      <c r="J11" s="54"/>
-      <c r="K11" s="51"/>
+      <c r="I11" s="62"/>
+      <c r="J11" s="74"/>
+      <c r="K11" s="62"/>
       <c r="L11" s="3"/>
       <c r="M11" s="2"/>
       <c r="N11" s="2"/>
@@ -2089,37 +2196,37 @@
       <c r="AA11" s="2"/>
     </row>
     <row r="12" spans="1:27">
-      <c r="A12" s="80" t="s">
+      <c r="A12" s="52" t="s">
         <v>31</v>
       </c>
-      <c r="B12" s="58" t="s">
+      <c r="B12" s="46" t="s">
         <v>49</v>
       </c>
-      <c r="C12" s="58" t="s">
+      <c r="C12" s="46" t="s">
         <v>60</v>
       </c>
-      <c r="D12" s="58" t="s">
+      <c r="D12" s="46" t="s">
         <v>61</v>
       </c>
-      <c r="E12" s="58" t="s">
+      <c r="E12" s="46" t="s">
         <v>62</v>
       </c>
-      <c r="F12" s="58" t="s">
+      <c r="F12" s="46" t="s">
         <v>53</v>
       </c>
-      <c r="G12" s="58" t="s">
+      <c r="G12" s="46" t="s">
         <v>54</v>
       </c>
-      <c r="H12" s="73" t="s">
+      <c r="H12" s="70" t="s">
         <v>55</v>
       </c>
-      <c r="I12" s="49" t="s">
+      <c r="I12" s="60" t="s">
         <v>26</v>
       </c>
-      <c r="J12" s="52" t="s">
+      <c r="J12" s="72" t="s">
         <v>56</v>
       </c>
-      <c r="K12" s="49" t="s">
+      <c r="K12" s="60" t="s">
         <v>28</v>
       </c>
       <c r="L12" s="2"/>
@@ -2140,17 +2247,17 @@
       <c r="AA12" s="2"/>
     </row>
     <row r="13" spans="1:27">
-      <c r="A13" s="81"/>
-      <c r="B13" s="59"/>
-      <c r="C13" s="59"/>
-      <c r="D13" s="59"/>
-      <c r="E13" s="59"/>
-      <c r="F13" s="60"/>
-      <c r="G13" s="60"/>
-      <c r="H13" s="74"/>
-      <c r="I13" s="50"/>
-      <c r="J13" s="53"/>
-      <c r="K13" s="50"/>
+      <c r="A13" s="53"/>
+      <c r="B13" s="47"/>
+      <c r="C13" s="47"/>
+      <c r="D13" s="47"/>
+      <c r="E13" s="47"/>
+      <c r="F13" s="48"/>
+      <c r="G13" s="48"/>
+      <c r="H13" s="71"/>
+      <c r="I13" s="61"/>
+      <c r="J13" s="73"/>
+      <c r="K13" s="61"/>
       <c r="L13" s="2"/>
       <c r="M13" s="2"/>
       <c r="N13" s="2"/>
@@ -2169,17 +2276,17 @@
       <c r="AA13" s="2"/>
     </row>
     <row r="14" spans="1:27" s="29" customFormat="1">
-      <c r="A14" s="81"/>
-      <c r="B14" s="59"/>
-      <c r="C14" s="59"/>
-      <c r="D14" s="59"/>
-      <c r="E14" s="59"/>
+      <c r="A14" s="53"/>
+      <c r="B14" s="47"/>
+      <c r="C14" s="47"/>
+      <c r="D14" s="47"/>
+      <c r="E14" s="47"/>
       <c r="F14" s="30"/>
       <c r="G14" s="35"/>
       <c r="H14" s="35"/>
-      <c r="I14" s="50"/>
-      <c r="J14" s="53"/>
-      <c r="K14" s="50"/>
+      <c r="I14" s="61"/>
+      <c r="J14" s="73"/>
+      <c r="K14" s="61"/>
       <c r="L14" s="28"/>
       <c r="M14" s="28"/>
       <c r="N14" s="28"/>
@@ -2198,17 +2305,17 @@
       <c r="AA14" s="28"/>
     </row>
     <row r="15" spans="1:27">
-      <c r="A15" s="82"/>
-      <c r="B15" s="60"/>
-      <c r="C15" s="60"/>
-      <c r="D15" s="60"/>
-      <c r="E15" s="60"/>
+      <c r="A15" s="54"/>
+      <c r="B15" s="48"/>
+      <c r="C15" s="48"/>
+      <c r="D15" s="48"/>
+      <c r="E15" s="48"/>
       <c r="F15" s="30"/>
       <c r="G15" s="35"/>
       <c r="H15" s="35"/>
-      <c r="I15" s="51"/>
-      <c r="J15" s="54"/>
-      <c r="K15" s="51"/>
+      <c r="I15" s="62"/>
+      <c r="J15" s="74"/>
+      <c r="K15" s="62"/>
       <c r="L15" s="2"/>
       <c r="M15" s="2"/>
       <c r="N15" s="2"/>
@@ -2227,19 +2334,19 @@
       <c r="AA15" s="2"/>
     </row>
     <row r="16" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A16" s="83" t="s">
+      <c r="A16" s="55" t="s">
         <v>32</v>
       </c>
-      <c r="B16" s="58" t="s">
+      <c r="B16" s="46" t="s">
         <v>63</v>
       </c>
-      <c r="C16" s="58" t="s">
+      <c r="C16" s="46" t="s">
         <v>64</v>
       </c>
-      <c r="D16" s="58" t="s">
+      <c r="D16" s="46" t="s">
         <v>65</v>
       </c>
-      <c r="E16" s="58" t="s">
+      <c r="E16" s="46" t="s">
         <v>83</v>
       </c>
       <c r="F16" s="30" t="s">
@@ -2251,13 +2358,13 @@
       <c r="H16" s="35" t="s">
         <v>66</v>
       </c>
-      <c r="I16" s="49" t="s">
+      <c r="I16" s="60" t="s">
         <v>26</v>
       </c>
-      <c r="J16" s="52" t="s">
+      <c r="J16" s="72" t="s">
         <v>56</v>
       </c>
-      <c r="K16" s="49" t="s">
+      <c r="K16" s="60" t="s">
         <v>28</v>
       </c>
       <c r="L16" s="2"/>
@@ -2278,11 +2385,11 @@
       <c r="AA16" s="2"/>
     </row>
     <row r="17" spans="1:27" ht="16.5" customHeight="1">
-      <c r="A17" s="84"/>
-      <c r="B17" s="59"/>
-      <c r="C17" s="59"/>
-      <c r="D17" s="59"/>
-      <c r="E17" s="59"/>
+      <c r="A17" s="56"/>
+      <c r="B17" s="47"/>
+      <c r="C17" s="47"/>
+      <c r="D17" s="47"/>
+      <c r="E17" s="47"/>
       <c r="F17" s="30" t="s">
         <v>67</v>
       </c>
@@ -2292,9 +2399,9 @@
       <c r="H17" s="35" t="s">
         <v>69</v>
       </c>
-      <c r="I17" s="50"/>
-      <c r="J17" s="53"/>
-      <c r="K17" s="50"/>
+      <c r="I17" s="61"/>
+      <c r="J17" s="73"/>
+      <c r="K17" s="61"/>
       <c r="L17" s="2"/>
       <c r="M17" s="2"/>
       <c r="N17" s="2"/>
@@ -2313,11 +2420,11 @@
       <c r="AA17" s="2"/>
     </row>
     <row r="18" spans="1:27" s="29" customFormat="1" ht="25.5">
-      <c r="A18" s="84"/>
-      <c r="B18" s="59"/>
-      <c r="C18" s="59"/>
-      <c r="D18" s="59"/>
-      <c r="E18" s="59"/>
+      <c r="A18" s="56"/>
+      <c r="B18" s="47"/>
+      <c r="C18" s="47"/>
+      <c r="D18" s="47"/>
+      <c r="E18" s="47"/>
       <c r="F18" s="30" t="s">
         <v>70</v>
       </c>
@@ -2327,9 +2434,9 @@
       <c r="H18" s="35" t="s">
         <v>72</v>
       </c>
-      <c r="I18" s="50"/>
-      <c r="J18" s="53"/>
-      <c r="K18" s="50"/>
+      <c r="I18" s="61"/>
+      <c r="J18" s="73"/>
+      <c r="K18" s="61"/>
       <c r="L18" s="28"/>
       <c r="M18" s="28"/>
       <c r="N18" s="28"/>
@@ -2348,17 +2455,17 @@
       <c r="AA18" s="28"/>
     </row>
     <row r="19" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A19" s="85"/>
-      <c r="B19" s="60"/>
-      <c r="C19" s="60"/>
-      <c r="D19" s="60"/>
-      <c r="E19" s="60"/>
+      <c r="A19" s="57"/>
+      <c r="B19" s="48"/>
+      <c r="C19" s="48"/>
+      <c r="D19" s="48"/>
+      <c r="E19" s="48"/>
       <c r="F19" s="30"/>
       <c r="G19" s="35"/>
       <c r="H19" s="35"/>
-      <c r="I19" s="51"/>
-      <c r="J19" s="54"/>
-      <c r="K19" s="51"/>
+      <c r="I19" s="62"/>
+      <c r="J19" s="74"/>
+      <c r="K19" s="62"/>
       <c r="L19" s="2"/>
       <c r="M19" s="2"/>
       <c r="N19" s="2"/>
@@ -2377,19 +2484,19 @@
       <c r="AA19" s="2"/>
     </row>
     <row r="20" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A20" s="83" t="s">
+      <c r="A20" s="55" t="s">
         <v>33</v>
       </c>
-      <c r="B20" s="58" t="s">
+      <c r="B20" s="46" t="s">
         <v>63</v>
       </c>
-      <c r="C20" s="46" t="s">
+      <c r="C20" s="49" t="s">
         <v>73</v>
       </c>
-      <c r="D20" s="58" t="s">
+      <c r="D20" s="46" t="s">
         <v>74</v>
       </c>
-      <c r="E20" s="58" t="s">
+      <c r="E20" s="46" t="s">
         <v>75</v>
       </c>
       <c r="F20" s="30" t="s">
@@ -2401,13 +2508,13 @@
       <c r="H20" s="35" t="s">
         <v>76</v>
       </c>
-      <c r="I20" s="49" t="s">
+      <c r="I20" s="60" t="s">
         <v>26</v>
       </c>
-      <c r="J20" s="52" t="s">
+      <c r="J20" s="72" t="s">
         <v>56</v>
       </c>
-      <c r="K20" s="49" t="s">
+      <c r="K20" s="60" t="s">
         <v>28</v>
       </c>
       <c r="L20" s="2"/>
@@ -2428,11 +2535,11 @@
       <c r="AA20" s="2"/>
     </row>
     <row r="21" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A21" s="84"/>
-      <c r="B21" s="59"/>
-      <c r="C21" s="67"/>
-      <c r="D21" s="59"/>
-      <c r="E21" s="59"/>
+      <c r="A21" s="56"/>
+      <c r="B21" s="47"/>
+      <c r="C21" s="50"/>
+      <c r="D21" s="47"/>
+      <c r="E21" s="47"/>
       <c r="F21" s="30" t="s">
         <v>67</v>
       </c>
@@ -2440,9 +2547,9 @@
         <v>77</v>
       </c>
       <c r="H21" s="35"/>
-      <c r="I21" s="50"/>
-      <c r="J21" s="53"/>
-      <c r="K21" s="50"/>
+      <c r="I21" s="61"/>
+      <c r="J21" s="73"/>
+      <c r="K21" s="61"/>
       <c r="L21" s="2"/>
       <c r="M21" s="2"/>
       <c r="N21" s="2"/>
@@ -2461,11 +2568,11 @@
       <c r="AA21" s="2"/>
     </row>
     <row r="22" spans="1:27" s="29" customFormat="1" ht="15.75" customHeight="1">
-      <c r="A22" s="84"/>
-      <c r="B22" s="59"/>
-      <c r="C22" s="67"/>
-      <c r="D22" s="59"/>
-      <c r="E22" s="59"/>
+      <c r="A22" s="56"/>
+      <c r="B22" s="47"/>
+      <c r="C22" s="50"/>
+      <c r="D22" s="47"/>
+      <c r="E22" s="47"/>
       <c r="F22" s="30" t="s">
         <v>70</v>
       </c>
@@ -2475,9 +2582,9 @@
       <c r="H22" s="35" t="s">
         <v>79</v>
       </c>
-      <c r="I22" s="50"/>
-      <c r="J22" s="53"/>
-      <c r="K22" s="50"/>
+      <c r="I22" s="61"/>
+      <c r="J22" s="73"/>
+      <c r="K22" s="61"/>
       <c r="L22" s="28"/>
       <c r="M22" s="28"/>
       <c r="N22" s="28"/>
@@ -2496,17 +2603,17 @@
       <c r="AA22" s="28"/>
     </row>
     <row r="23" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A23" s="85"/>
-      <c r="B23" s="60"/>
-      <c r="C23" s="68"/>
-      <c r="D23" s="60"/>
-      <c r="E23" s="60"/>
+      <c r="A23" s="57"/>
+      <c r="B23" s="48"/>
+      <c r="C23" s="51"/>
+      <c r="D23" s="48"/>
+      <c r="E23" s="48"/>
       <c r="F23" s="30"/>
       <c r="G23" s="35"/>
       <c r="H23" s="35"/>
-      <c r="I23" s="51"/>
-      <c r="J23" s="54"/>
-      <c r="K23" s="51"/>
+      <c r="I23" s="62"/>
+      <c r="J23" s="74"/>
+      <c r="K23" s="62"/>
       <c r="L23" s="2"/>
       <c r="M23" s="2"/>
       <c r="N23" s="2"/>
@@ -2525,19 +2632,19 @@
       <c r="AA23" s="2"/>
     </row>
     <row r="24" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A24" s="83" t="s">
+      <c r="A24" s="55" t="s">
         <v>34</v>
       </c>
-      <c r="B24" s="58" t="s">
+      <c r="B24" s="46" t="s">
         <v>63</v>
       </c>
-      <c r="C24" s="46" t="s">
+      <c r="C24" s="49" t="s">
         <v>80</v>
       </c>
-      <c r="D24" s="58" t="s">
+      <c r="D24" s="46" t="s">
         <v>81</v>
       </c>
-      <c r="E24" s="58" t="s">
+      <c r="E24" s="46" t="s">
         <v>75</v>
       </c>
       <c r="F24" s="30" t="s">
@@ -2549,13 +2656,13 @@
       <c r="H24" s="35" t="s">
         <v>76</v>
       </c>
-      <c r="I24" s="49" t="s">
+      <c r="I24" s="60" t="s">
         <v>26</v>
       </c>
-      <c r="J24" s="52" t="s">
+      <c r="J24" s="72" t="s">
         <v>56</v>
       </c>
-      <c r="K24" s="49" t="s">
+      <c r="K24" s="60" t="s">
         <v>28</v>
       </c>
       <c r="L24" s="2"/>
@@ -2576,11 +2683,11 @@
       <c r="AA24" s="2"/>
     </row>
     <row r="25" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A25" s="84"/>
-      <c r="B25" s="59"/>
-      <c r="C25" s="67"/>
-      <c r="D25" s="59"/>
-      <c r="E25" s="59"/>
+      <c r="A25" s="56"/>
+      <c r="B25" s="47"/>
+      <c r="C25" s="50"/>
+      <c r="D25" s="47"/>
+      <c r="E25" s="47"/>
       <c r="F25" s="30" t="s">
         <v>67</v>
       </c>
@@ -2588,9 +2695,9 @@
         <v>77</v>
       </c>
       <c r="H25" s="35"/>
-      <c r="I25" s="50"/>
-      <c r="J25" s="53"/>
-      <c r="K25" s="50"/>
+      <c r="I25" s="61"/>
+      <c r="J25" s="73"/>
+      <c r="K25" s="61"/>
       <c r="L25" s="2"/>
       <c r="M25" s="2"/>
       <c r="N25" s="2"/>
@@ -2609,11 +2716,11 @@
       <c r="AA25" s="2"/>
     </row>
     <row r="26" spans="1:27" s="29" customFormat="1" ht="25.5">
-      <c r="A26" s="84"/>
-      <c r="B26" s="59"/>
-      <c r="C26" s="67"/>
-      <c r="D26" s="59"/>
-      <c r="E26" s="59"/>
+      <c r="A26" s="56"/>
+      <c r="B26" s="47"/>
+      <c r="C26" s="50"/>
+      <c r="D26" s="47"/>
+      <c r="E26" s="47"/>
       <c r="F26" s="30" t="s">
         <v>70</v>
       </c>
@@ -2623,9 +2730,9 @@
       <c r="H26" s="35" t="s">
         <v>82</v>
       </c>
-      <c r="I26" s="50"/>
-      <c r="J26" s="53"/>
-      <c r="K26" s="50"/>
+      <c r="I26" s="61"/>
+      <c r="J26" s="73"/>
+      <c r="K26" s="61"/>
       <c r="L26" s="28"/>
       <c r="M26" s="28"/>
       <c r="N26" s="28"/>
@@ -2644,17 +2751,17 @@
       <c r="AA26" s="28"/>
     </row>
     <row r="27" spans="1:27" ht="18.75" customHeight="1">
-      <c r="A27" s="85"/>
-      <c r="B27" s="60"/>
-      <c r="C27" s="68"/>
-      <c r="D27" s="60"/>
-      <c r="E27" s="60"/>
+      <c r="A27" s="57"/>
+      <c r="B27" s="48"/>
+      <c r="C27" s="51"/>
+      <c r="D27" s="48"/>
+      <c r="E27" s="48"/>
       <c r="F27" s="30"/>
       <c r="G27" s="35"/>
       <c r="H27" s="35"/>
-      <c r="I27" s="51"/>
-      <c r="J27" s="54"/>
-      <c r="K27" s="51"/>
+      <c r="I27" s="62"/>
+      <c r="J27" s="74"/>
+      <c r="K27" s="62"/>
       <c r="L27" s="2"/>
       <c r="M27" s="2"/>
       <c r="N27" s="2"/>
@@ -2673,19 +2780,19 @@
       <c r="AA27" s="2"/>
     </row>
     <row r="28" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A28" s="61" t="s">
+      <c r="A28" s="75" t="s">
         <v>35</v>
       </c>
-      <c r="B28" s="58" t="s">
+      <c r="B28" s="46" t="s">
         <v>84</v>
       </c>
-      <c r="C28" s="58" t="s">
+      <c r="C28" s="46" t="s">
         <v>85</v>
       </c>
-      <c r="D28" s="58" t="s">
+      <c r="D28" s="46" t="s">
         <v>86</v>
       </c>
-      <c r="E28" s="58" t="s">
+      <c r="E28" s="46" t="s">
         <v>83</v>
       </c>
       <c r="F28" s="30" t="s">
@@ -2697,13 +2804,13 @@
       <c r="H28" s="35" t="s">
         <v>88</v>
       </c>
-      <c r="I28" s="49" t="s">
+      <c r="I28" s="60" t="s">
         <v>26</v>
       </c>
-      <c r="J28" s="52" t="s">
+      <c r="J28" s="72" t="s">
         <v>56</v>
       </c>
-      <c r="K28" s="49" t="s">
+      <c r="K28" s="60" t="s">
         <v>28</v>
       </c>
       <c r="L28" s="2"/>
@@ -2724,19 +2831,19 @@
       <c r="AA28" s="2"/>
     </row>
     <row r="29" spans="1:27">
-      <c r="A29" s="62"/>
-      <c r="B29" s="59"/>
-      <c r="C29" s="59"/>
-      <c r="D29" s="59"/>
-      <c r="E29" s="59"/>
+      <c r="A29" s="76"/>
+      <c r="B29" s="47"/>
+      <c r="C29" s="47"/>
+      <c r="D29" s="47"/>
+      <c r="E29" s="47"/>
       <c r="F29" s="30" t="s">
         <v>67</v>
       </c>
       <c r="G29" s="35"/>
       <c r="H29" s="35"/>
-      <c r="I29" s="50"/>
-      <c r="J29" s="53"/>
-      <c r="K29" s="50"/>
+      <c r="I29" s="61"/>
+      <c r="J29" s="73"/>
+      <c r="K29" s="61"/>
       <c r="L29" s="2"/>
       <c r="M29" s="2"/>
       <c r="N29" s="2"/>
@@ -2755,17 +2862,17 @@
       <c r="AA29" s="2"/>
     </row>
     <row r="30" spans="1:27" s="29" customFormat="1" ht="15.75" customHeight="1">
-      <c r="A30" s="62"/>
-      <c r="B30" s="59"/>
-      <c r="C30" s="59"/>
-      <c r="D30" s="59"/>
-      <c r="E30" s="59"/>
+      <c r="A30" s="76"/>
+      <c r="B30" s="47"/>
+      <c r="C30" s="47"/>
+      <c r="D30" s="47"/>
+      <c r="E30" s="47"/>
       <c r="F30" s="30"/>
       <c r="G30" s="35"/>
       <c r="H30" s="35"/>
-      <c r="I30" s="50"/>
-      <c r="J30" s="53"/>
-      <c r="K30" s="50"/>
+      <c r="I30" s="61"/>
+      <c r="J30" s="73"/>
+      <c r="K30" s="61"/>
       <c r="L30" s="28"/>
       <c r="M30" s="28"/>
       <c r="N30" s="28"/>
@@ -2784,17 +2891,17 @@
       <c r="AA30" s="28"/>
     </row>
     <row r="31" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A31" s="63"/>
-      <c r="B31" s="60"/>
-      <c r="C31" s="60"/>
-      <c r="D31" s="60"/>
-      <c r="E31" s="60"/>
+      <c r="A31" s="77"/>
+      <c r="B31" s="48"/>
+      <c r="C31" s="48"/>
+      <c r="D31" s="48"/>
+      <c r="E31" s="48"/>
       <c r="F31" s="30"/>
       <c r="G31" s="35"/>
       <c r="H31" s="35"/>
-      <c r="I31" s="51"/>
-      <c r="J31" s="54"/>
-      <c r="K31" s="51"/>
+      <c r="I31" s="62"/>
+      <c r="J31" s="74"/>
+      <c r="K31" s="62"/>
       <c r="L31" s="2"/>
       <c r="M31" s="2"/>
       <c r="N31" s="2"/>
@@ -2813,19 +2920,19 @@
       <c r="AA31" s="2"/>
     </row>
     <row r="32" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A32" s="61" t="s">
+      <c r="A32" s="75" t="s">
         <v>36</v>
       </c>
-      <c r="B32" s="58" t="s">
+      <c r="B32" s="46" t="s">
         <v>84</v>
       </c>
-      <c r="C32" s="58" t="s">
+      <c r="C32" s="46" t="s">
         <v>89</v>
       </c>
-      <c r="D32" s="58" t="s">
+      <c r="D32" s="46" t="s">
         <v>90</v>
       </c>
-      <c r="E32" s="58" t="s">
+      <c r="E32" s="46" t="s">
         <v>83</v>
       </c>
       <c r="F32" s="30" t="s">
@@ -2837,13 +2944,13 @@
       <c r="H32" s="35" t="s">
         <v>92</v>
       </c>
-      <c r="I32" s="49" t="s">
+      <c r="I32" s="60" t="s">
         <v>26</v>
       </c>
-      <c r="J32" s="52" t="s">
+      <c r="J32" s="72" t="s">
         <v>56</v>
       </c>
-      <c r="K32" s="49" t="s">
+      <c r="K32" s="60" t="s">
         <v>28</v>
       </c>
       <c r="L32" s="2"/>
@@ -2864,17 +2971,17 @@
       <c r="AA32" s="2"/>
     </row>
     <row r="33" spans="1:27">
-      <c r="A33" s="62"/>
-      <c r="B33" s="59"/>
-      <c r="C33" s="59"/>
-      <c r="D33" s="59"/>
-      <c r="E33" s="59"/>
+      <c r="A33" s="76"/>
+      <c r="B33" s="47"/>
+      <c r="C33" s="47"/>
+      <c r="D33" s="47"/>
+      <c r="E33" s="47"/>
       <c r="F33" s="30"/>
       <c r="G33" s="43"/>
       <c r="H33" s="43"/>
-      <c r="I33" s="50"/>
-      <c r="J33" s="53"/>
-      <c r="K33" s="50"/>
+      <c r="I33" s="61"/>
+      <c r="J33" s="73"/>
+      <c r="K33" s="61"/>
       <c r="L33" s="2"/>
       <c r="M33" s="2"/>
       <c r="N33" s="2"/>
@@ -2893,17 +3000,17 @@
       <c r="AA33" s="2"/>
     </row>
     <row r="34" spans="1:27">
-      <c r="A34" s="62"/>
-      <c r="B34" s="59"/>
-      <c r="C34" s="59"/>
-      <c r="D34" s="59"/>
-      <c r="E34" s="59"/>
+      <c r="A34" s="76"/>
+      <c r="B34" s="47"/>
+      <c r="C34" s="47"/>
+      <c r="D34" s="47"/>
+      <c r="E34" s="47"/>
       <c r="F34" s="30"/>
       <c r="G34" s="43"/>
       <c r="H34" s="43"/>
-      <c r="I34" s="50"/>
-      <c r="J34" s="53"/>
-      <c r="K34" s="50"/>
+      <c r="I34" s="61"/>
+      <c r="J34" s="73"/>
+      <c r="K34" s="61"/>
       <c r="L34" s="2"/>
       <c r="M34" s="2"/>
       <c r="N34" s="2"/>
@@ -2922,17 +3029,17 @@
       <c r="AA34" s="2"/>
     </row>
     <row r="35" spans="1:27">
-      <c r="A35" s="63"/>
-      <c r="B35" s="60"/>
-      <c r="C35" s="60"/>
-      <c r="D35" s="60"/>
-      <c r="E35" s="60"/>
+      <c r="A35" s="77"/>
+      <c r="B35" s="48"/>
+      <c r="C35" s="48"/>
+      <c r="D35" s="48"/>
+      <c r="E35" s="48"/>
       <c r="F35" s="30"/>
       <c r="G35" s="35"/>
       <c r="H35" s="35"/>
-      <c r="I35" s="51"/>
-      <c r="J35" s="54"/>
-      <c r="K35" s="51"/>
+      <c r="I35" s="62"/>
+      <c r="J35" s="74"/>
+      <c r="K35" s="62"/>
       <c r="L35" s="2"/>
       <c r="M35" s="2"/>
       <c r="N35" s="2"/>
@@ -2951,19 +3058,19 @@
       <c r="AA35" s="2"/>
     </row>
     <row r="36" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A36" s="61" t="s">
+      <c r="A36" s="75" t="s">
         <v>37</v>
       </c>
-      <c r="B36" s="58" t="s">
+      <c r="B36" s="46" t="s">
         <v>84</v>
       </c>
-      <c r="C36" s="58" t="s">
+      <c r="C36" s="46" t="s">
         <v>93</v>
       </c>
-      <c r="D36" s="58" t="s">
+      <c r="D36" s="46" t="s">
         <v>94</v>
       </c>
-      <c r="E36" s="58" t="s">
+      <c r="E36" s="46" t="s">
         <v>95</v>
       </c>
       <c r="F36" s="30" t="s">
@@ -2975,13 +3082,13 @@
       <c r="H36" s="35" t="s">
         <v>92</v>
       </c>
-      <c r="I36" s="49" t="s">
+      <c r="I36" s="60" t="s">
         <v>26</v>
       </c>
-      <c r="J36" s="52" t="s">
+      <c r="J36" s="72" t="s">
         <v>56</v>
       </c>
-      <c r="K36" s="49" t="s">
+      <c r="K36" s="60" t="s">
         <v>28</v>
       </c>
       <c r="L36" s="2"/>
@@ -3002,11 +3109,11 @@
       <c r="AA36" s="2"/>
     </row>
     <row r="37" spans="1:27" ht="25.5">
-      <c r="A37" s="62"/>
-      <c r="B37" s="59"/>
-      <c r="C37" s="59"/>
-      <c r="D37" s="59"/>
-      <c r="E37" s="59"/>
+      <c r="A37" s="76"/>
+      <c r="B37" s="47"/>
+      <c r="C37" s="47"/>
+      <c r="D37" s="47"/>
+      <c r="E37" s="47"/>
       <c r="F37" s="30" t="s">
         <v>67</v>
       </c>
@@ -3014,9 +3121,9 @@
         <v>96</v>
       </c>
       <c r="H37" s="35"/>
-      <c r="I37" s="50"/>
-      <c r="J37" s="53"/>
-      <c r="K37" s="50"/>
+      <c r="I37" s="61"/>
+      <c r="J37" s="73"/>
+      <c r="K37" s="61"/>
       <c r="L37" s="2"/>
       <c r="M37" s="2"/>
       <c r="N37" s="2"/>
@@ -3035,11 +3142,11 @@
       <c r="AA37" s="2"/>
     </row>
     <row r="38" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A38" s="62"/>
-      <c r="B38" s="59"/>
-      <c r="C38" s="59"/>
-      <c r="D38" s="59"/>
-      <c r="E38" s="59"/>
+      <c r="A38" s="76"/>
+      <c r="B38" s="47"/>
+      <c r="C38" s="47"/>
+      <c r="D38" s="47"/>
+      <c r="E38" s="47"/>
       <c r="F38" s="30" t="s">
         <v>70</v>
       </c>
@@ -3049,9 +3156,9 @@
       <c r="H38" s="35" t="s">
         <v>98</v>
       </c>
-      <c r="I38" s="50"/>
-      <c r="J38" s="53"/>
-      <c r="K38" s="50"/>
+      <c r="I38" s="61"/>
+      <c r="J38" s="73"/>
+      <c r="K38" s="61"/>
       <c r="L38" s="2"/>
       <c r="M38" s="2"/>
       <c r="N38" s="2"/>
@@ -3070,19 +3177,19 @@
       <c r="AA38" s="2"/>
     </row>
     <row r="39" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A39" s="63"/>
-      <c r="B39" s="60"/>
-      <c r="C39" s="60"/>
-      <c r="D39" s="60"/>
-      <c r="E39" s="60"/>
+      <c r="A39" s="77"/>
+      <c r="B39" s="48"/>
+      <c r="C39" s="48"/>
+      <c r="D39" s="48"/>
+      <c r="E39" s="48"/>
       <c r="F39" s="30" t="s">
         <v>99</v>
       </c>
       <c r="G39" s="35"/>
       <c r="H39" s="35"/>
-      <c r="I39" s="51"/>
-      <c r="J39" s="54"/>
-      <c r="K39" s="51"/>
+      <c r="I39" s="62"/>
+      <c r="J39" s="74"/>
+      <c r="K39" s="62"/>
       <c r="L39" s="2"/>
       <c r="M39" s="2"/>
       <c r="N39" s="2"/>
@@ -3101,19 +3208,19 @@
       <c r="AA39" s="2"/>
     </row>
     <row r="40" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A40" s="61" t="s">
+      <c r="A40" s="75" t="s">
         <v>38</v>
       </c>
-      <c r="B40" s="58" t="s">
+      <c r="B40" s="46" t="s">
         <v>84</v>
       </c>
-      <c r="C40" s="58" t="s">
+      <c r="C40" s="46" t="s">
         <v>100</v>
       </c>
-      <c r="D40" s="58" t="s">
+      <c r="D40" s="46" t="s">
         <v>101</v>
       </c>
-      <c r="E40" s="58" t="s">
+      <c r="E40" s="46" t="s">
         <v>102</v>
       </c>
       <c r="F40" s="30" t="s">
@@ -3125,13 +3232,13 @@
       <c r="H40" s="35" t="s">
         <v>88</v>
       </c>
-      <c r="I40" s="49" t="s">
+      <c r="I40" s="60" t="s">
         <v>26</v>
       </c>
-      <c r="J40" s="52" t="s">
+      <c r="J40" s="72" t="s">
         <v>56</v>
       </c>
-      <c r="K40" s="49" t="s">
+      <c r="K40" s="60" t="s">
         <v>28</v>
       </c>
       <c r="L40" s="2"/>
@@ -3152,11 +3259,11 @@
       <c r="AA40" s="2"/>
     </row>
     <row r="41" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A41" s="62"/>
-      <c r="B41" s="59"/>
-      <c r="C41" s="59"/>
-      <c r="D41" s="59"/>
-      <c r="E41" s="59"/>
+      <c r="A41" s="76"/>
+      <c r="B41" s="47"/>
+      <c r="C41" s="47"/>
+      <c r="D41" s="47"/>
+      <c r="E41" s="47"/>
       <c r="F41" s="30" t="s">
         <v>67</v>
       </c>
@@ -3164,9 +3271,9 @@
         <v>103</v>
       </c>
       <c r="H41" s="35"/>
-      <c r="I41" s="50"/>
-      <c r="J41" s="53"/>
-      <c r="K41" s="50"/>
+      <c r="I41" s="61"/>
+      <c r="J41" s="73"/>
+      <c r="K41" s="61"/>
       <c r="L41" s="2"/>
       <c r="M41" s="2"/>
       <c r="N41" s="2"/>
@@ -3185,11 +3292,11 @@
       <c r="AA41" s="2"/>
     </row>
     <row r="42" spans="1:27" ht="16.5" customHeight="1">
-      <c r="A42" s="62"/>
-      <c r="B42" s="59"/>
-      <c r="C42" s="59"/>
-      <c r="D42" s="59"/>
-      <c r="E42" s="59"/>
+      <c r="A42" s="76"/>
+      <c r="B42" s="47"/>
+      <c r="C42" s="47"/>
+      <c r="D42" s="47"/>
+      <c r="E42" s="47"/>
       <c r="F42" s="30" t="s">
         <v>70</v>
       </c>
@@ -3199,9 +3306,9 @@
       <c r="H42" s="35" t="s">
         <v>105</v>
       </c>
-      <c r="I42" s="50"/>
-      <c r="J42" s="53"/>
-      <c r="K42" s="50"/>
+      <c r="I42" s="61"/>
+      <c r="J42" s="73"/>
+      <c r="K42" s="61"/>
       <c r="L42" s="2"/>
       <c r="M42" s="2"/>
       <c r="N42" s="2"/>
@@ -3220,19 +3327,19 @@
       <c r="AA42" s="2"/>
     </row>
     <row r="43" spans="1:27" ht="18.75" customHeight="1">
-      <c r="A43" s="63"/>
-      <c r="B43" s="60"/>
-      <c r="C43" s="60"/>
-      <c r="D43" s="60"/>
-      <c r="E43" s="60"/>
+      <c r="A43" s="77"/>
+      <c r="B43" s="48"/>
+      <c r="C43" s="48"/>
+      <c r="D43" s="48"/>
+      <c r="E43" s="48"/>
       <c r="F43" s="30" t="s">
         <v>99</v>
       </c>
       <c r="G43" s="35"/>
       <c r="H43" s="35"/>
-      <c r="I43" s="51"/>
-      <c r="J43" s="54"/>
-      <c r="K43" s="51"/>
+      <c r="I43" s="62"/>
+      <c r="J43" s="74"/>
+      <c r="K43" s="62"/>
       <c r="L43" s="2"/>
       <c r="M43" s="2"/>
       <c r="N43" s="2"/>
@@ -3251,19 +3358,19 @@
       <c r="AA43" s="2"/>
     </row>
     <row r="44" spans="1:27" ht="25.5">
-      <c r="A44" s="61" t="s">
+      <c r="A44" s="75" t="s">
         <v>39</v>
       </c>
-      <c r="B44" s="58" t="s">
+      <c r="B44" s="46" t="s">
         <v>84</v>
       </c>
-      <c r="C44" s="58" t="s">
+      <c r="C44" s="46" t="s">
         <v>106</v>
       </c>
-      <c r="D44" s="58" t="s">
+      <c r="D44" s="46" t="s">
         <v>107</v>
       </c>
-      <c r="E44" s="58" t="s">
+      <c r="E44" s="46" t="s">
         <v>108</v>
       </c>
       <c r="F44" s="30" t="s">
@@ -3275,13 +3382,13 @@
       <c r="H44" s="35" t="s">
         <v>88</v>
       </c>
-      <c r="I44" s="49" t="s">
+      <c r="I44" s="60" t="s">
         <v>26</v>
       </c>
-      <c r="J44" s="52" t="s">
+      <c r="J44" s="72" t="s">
         <v>56</v>
       </c>
-      <c r="K44" s="49" t="s">
+      <c r="K44" s="60" t="s">
         <v>28</v>
       </c>
       <c r="L44" s="2"/>
@@ -3302,11 +3409,11 @@
       <c r="AA44" s="2"/>
     </row>
     <row r="45" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A45" s="62"/>
-      <c r="B45" s="59"/>
-      <c r="C45" s="59"/>
-      <c r="D45" s="59"/>
-      <c r="E45" s="59"/>
+      <c r="A45" s="76"/>
+      <c r="B45" s="47"/>
+      <c r="C45" s="47"/>
+      <c r="D45" s="47"/>
+      <c r="E45" s="47"/>
       <c r="F45" s="30" t="s">
         <v>67</v>
       </c>
@@ -3314,9 +3421,9 @@
         <v>109</v>
       </c>
       <c r="H45" s="35"/>
-      <c r="I45" s="50"/>
-      <c r="J45" s="53"/>
-      <c r="K45" s="50"/>
+      <c r="I45" s="61"/>
+      <c r="J45" s="73"/>
+      <c r="K45" s="61"/>
       <c r="L45" s="2"/>
       <c r="M45" s="2"/>
       <c r="N45" s="2"/>
@@ -3335,11 +3442,11 @@
       <c r="AA45" s="2"/>
     </row>
     <row r="46" spans="1:27" ht="25.5">
-      <c r="A46" s="62"/>
-      <c r="B46" s="59"/>
-      <c r="C46" s="59"/>
-      <c r="D46" s="59"/>
-      <c r="E46" s="59"/>
+      <c r="A46" s="76"/>
+      <c r="B46" s="47"/>
+      <c r="C46" s="47"/>
+      <c r="D46" s="47"/>
+      <c r="E46" s="47"/>
       <c r="F46" s="30" t="s">
         <v>70</v>
       </c>
@@ -3349,9 +3456,9 @@
       <c r="H46" s="35" t="s">
         <v>110</v>
       </c>
-      <c r="I46" s="50"/>
-      <c r="J46" s="53"/>
-      <c r="K46" s="50"/>
+      <c r="I46" s="61"/>
+      <c r="J46" s="73"/>
+      <c r="K46" s="61"/>
       <c r="L46" s="2"/>
       <c r="M46" s="2"/>
       <c r="N46" s="2"/>
@@ -3370,19 +3477,19 @@
       <c r="AA46" s="2"/>
     </row>
     <row r="47" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A47" s="63"/>
-      <c r="B47" s="60"/>
-      <c r="C47" s="60"/>
-      <c r="D47" s="60"/>
-      <c r="E47" s="60"/>
+      <c r="A47" s="77"/>
+      <c r="B47" s="48"/>
+      <c r="C47" s="48"/>
+      <c r="D47" s="48"/>
+      <c r="E47" s="48"/>
       <c r="F47" s="30" t="s">
         <v>99</v>
       </c>
       <c r="G47" s="35"/>
       <c r="H47" s="36"/>
-      <c r="I47" s="51"/>
-      <c r="J47" s="54"/>
-      <c r="K47" s="51"/>
+      <c r="I47" s="62"/>
+      <c r="J47" s="74"/>
+      <c r="K47" s="62"/>
       <c r="L47" s="2"/>
       <c r="M47" s="2"/>
       <c r="N47" s="2"/>
@@ -3401,19 +3508,19 @@
       <c r="AA47" s="2"/>
     </row>
     <row r="48" spans="1:27" ht="25.5">
-      <c r="A48" s="61" t="s">
+      <c r="A48" s="75" t="s">
         <v>40</v>
       </c>
-      <c r="B48" s="58" t="s">
+      <c r="B48" s="46" t="s">
         <v>84</v>
       </c>
-      <c r="C48" s="58" t="s">
+      <c r="C48" s="46" t="s">
         <v>111</v>
       </c>
-      <c r="D48" s="58" t="s">
+      <c r="D48" s="46" t="s">
         <v>112</v>
       </c>
-      <c r="E48" s="58" t="s">
+      <c r="E48" s="46" t="s">
         <v>102</v>
       </c>
       <c r="F48" s="30" t="s">
@@ -3425,13 +3532,13 @@
       <c r="H48" s="35" t="s">
         <v>88</v>
       </c>
-      <c r="I48" s="49" t="s">
+      <c r="I48" s="60" t="s">
         <v>26</v>
       </c>
-      <c r="J48" s="52" t="s">
+      <c r="J48" s="72" t="s">
         <v>56</v>
       </c>
-      <c r="K48" s="49" t="s">
+      <c r="K48" s="60" t="s">
         <v>28</v>
       </c>
       <c r="L48" s="2"/>
@@ -3452,11 +3559,11 @@
       <c r="AA48" s="2"/>
     </row>
     <row r="49" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A49" s="62"/>
-      <c r="B49" s="59"/>
-      <c r="C49" s="59"/>
-      <c r="D49" s="59"/>
-      <c r="E49" s="59"/>
+      <c r="A49" s="76"/>
+      <c r="B49" s="47"/>
+      <c r="C49" s="47"/>
+      <c r="D49" s="47"/>
+      <c r="E49" s="47"/>
       <c r="F49" s="30" t="s">
         <v>67</v>
       </c>
@@ -3464,9 +3571,9 @@
         <v>113</v>
       </c>
       <c r="H49" s="35"/>
-      <c r="I49" s="50"/>
-      <c r="J49" s="53"/>
-      <c r="K49" s="50"/>
+      <c r="I49" s="61"/>
+      <c r="J49" s="73"/>
+      <c r="K49" s="61"/>
       <c r="L49" s="2"/>
       <c r="M49" s="2"/>
       <c r="N49" s="2"/>
@@ -3485,11 +3592,11 @@
       <c r="AA49" s="2"/>
     </row>
     <row r="50" spans="1:27" ht="27" customHeight="1">
-      <c r="A50" s="62"/>
-      <c r="B50" s="59"/>
-      <c r="C50" s="59"/>
-      <c r="D50" s="59"/>
-      <c r="E50" s="59"/>
+      <c r="A50" s="76"/>
+      <c r="B50" s="47"/>
+      <c r="C50" s="47"/>
+      <c r="D50" s="47"/>
+      <c r="E50" s="47"/>
       <c r="F50" s="30" t="s">
         <v>70</v>
       </c>
@@ -3499,9 +3606,9 @@
       <c r="H50" s="35" t="s">
         <v>110</v>
       </c>
-      <c r="I50" s="50"/>
-      <c r="J50" s="53"/>
-      <c r="K50" s="50"/>
+      <c r="I50" s="61"/>
+      <c r="J50" s="73"/>
+      <c r="K50" s="61"/>
       <c r="L50" s="2"/>
       <c r="M50" s="2"/>
       <c r="N50" s="2"/>
@@ -3520,19 +3627,19 @@
       <c r="AA50" s="2"/>
     </row>
     <row r="51" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A51" s="63"/>
-      <c r="B51" s="60"/>
-      <c r="C51" s="60"/>
-      <c r="D51" s="60"/>
-      <c r="E51" s="60"/>
+      <c r="A51" s="77"/>
+      <c r="B51" s="48"/>
+      <c r="C51" s="48"/>
+      <c r="D51" s="48"/>
+      <c r="E51" s="48"/>
       <c r="F51" s="30" t="s">
         <v>99</v>
       </c>
       <c r="G51" s="35"/>
       <c r="H51" s="36"/>
-      <c r="I51" s="51"/>
-      <c r="J51" s="54"/>
-      <c r="K51" s="51"/>
+      <c r="I51" s="62"/>
+      <c r="J51" s="74"/>
+      <c r="K51" s="62"/>
       <c r="L51" s="2"/>
       <c r="M51" s="2"/>
       <c r="N51" s="2"/>
@@ -3551,19 +3658,19 @@
       <c r="AA51" s="2"/>
     </row>
     <row r="52" spans="1:27" ht="25.5">
-      <c r="A52" s="61" t="s">
+      <c r="A52" s="75" t="s">
         <v>41</v>
       </c>
-      <c r="B52" s="58" t="s">
+      <c r="B52" s="46" t="s">
         <v>84</v>
       </c>
-      <c r="C52" s="58" t="s">
+      <c r="C52" s="46" t="s">
         <v>114</v>
       </c>
-      <c r="D52" s="58" t="s">
+      <c r="D52" s="46" t="s">
         <v>129</v>
       </c>
-      <c r="E52" s="58" t="s">
+      <c r="E52" s="46" t="s">
         <v>95</v>
       </c>
       <c r="F52" s="30" t="s">
@@ -3575,13 +3682,13 @@
       <c r="H52" s="35" t="s">
         <v>92</v>
       </c>
-      <c r="I52" s="49" t="s">
+      <c r="I52" s="60" t="s">
         <v>26</v>
       </c>
-      <c r="J52" s="52" t="s">
+      <c r="J52" s="72" t="s">
         <v>56</v>
       </c>
-      <c r="K52" s="49" t="s">
+      <c r="K52" s="60" t="s">
         <v>28</v>
       </c>
       <c r="L52" s="2"/>
@@ -3602,11 +3709,11 @@
       <c r="AA52" s="2"/>
     </row>
     <row r="53" spans="1:27" ht="25.5">
-      <c r="A53" s="62"/>
-      <c r="B53" s="59"/>
-      <c r="C53" s="59"/>
-      <c r="D53" s="59"/>
-      <c r="E53" s="59"/>
+      <c r="A53" s="76"/>
+      <c r="B53" s="47"/>
+      <c r="C53" s="47"/>
+      <c r="D53" s="47"/>
+      <c r="E53" s="47"/>
       <c r="F53" s="30" t="s">
         <v>67</v>
       </c>
@@ -3616,9 +3723,9 @@
       <c r="H53" s="36" t="s">
         <v>116</v>
       </c>
-      <c r="I53" s="50"/>
-      <c r="J53" s="53"/>
-      <c r="K53" s="50"/>
+      <c r="I53" s="61"/>
+      <c r="J53" s="73"/>
+      <c r="K53" s="61"/>
       <c r="L53" s="2"/>
       <c r="M53" s="2"/>
       <c r="N53" s="2"/>
@@ -3637,17 +3744,17 @@
       <c r="AA53" s="2"/>
     </row>
     <row r="54" spans="1:27" ht="13.5" customHeight="1">
-      <c r="A54" s="62"/>
-      <c r="B54" s="59"/>
-      <c r="C54" s="59"/>
-      <c r="D54" s="59"/>
-      <c r="E54" s="59"/>
+      <c r="A54" s="76"/>
+      <c r="B54" s="47"/>
+      <c r="C54" s="47"/>
+      <c r="D54" s="47"/>
+      <c r="E54" s="47"/>
       <c r="F54" s="30"/>
       <c r="G54" s="43"/>
       <c r="H54" s="43"/>
-      <c r="I54" s="50"/>
-      <c r="J54" s="53"/>
-      <c r="K54" s="50"/>
+      <c r="I54" s="61"/>
+      <c r="J54" s="73"/>
+      <c r="K54" s="61"/>
       <c r="L54" s="2"/>
       <c r="M54" s="2"/>
       <c r="N54" s="2"/>
@@ -3666,17 +3773,17 @@
       <c r="AA54" s="2"/>
     </row>
     <row r="55" spans="1:27" ht="15" customHeight="1">
-      <c r="A55" s="63"/>
-      <c r="B55" s="60"/>
-      <c r="C55" s="60"/>
-      <c r="D55" s="60"/>
-      <c r="E55" s="60"/>
+      <c r="A55" s="77"/>
+      <c r="B55" s="48"/>
+      <c r="C55" s="48"/>
+      <c r="D55" s="48"/>
+      <c r="E55" s="48"/>
       <c r="F55" s="30"/>
       <c r="G55" s="43"/>
       <c r="H55" s="43"/>
-      <c r="I55" s="51"/>
-      <c r="J55" s="54"/>
-      <c r="K55" s="51"/>
+      <c r="I55" s="62"/>
+      <c r="J55" s="74"/>
+      <c r="K55" s="62"/>
       <c r="L55" s="2"/>
       <c r="M55" s="2"/>
       <c r="N55" s="2"/>
@@ -3695,19 +3802,19 @@
       <c r="AA55" s="2"/>
     </row>
     <row r="56" spans="1:27" ht="25.5">
-      <c r="A56" s="61" t="s">
+      <c r="A56" s="75" t="s">
         <v>42</v>
       </c>
-      <c r="B56" s="58" t="s">
+      <c r="B56" s="46" t="s">
         <v>84</v>
       </c>
-      <c r="C56" s="58" t="s">
+      <c r="C56" s="46" t="s">
         <v>117</v>
       </c>
-      <c r="D56" s="58" t="s">
+      <c r="D56" s="46" t="s">
         <v>118</v>
       </c>
-      <c r="E56" s="58" t="s">
+      <c r="E56" s="46" t="s">
         <v>95</v>
       </c>
       <c r="F56" s="30" t="s">
@@ -3719,13 +3826,13 @@
       <c r="H56" s="35" t="s">
         <v>92</v>
       </c>
-      <c r="I56" s="49" t="s">
+      <c r="I56" s="60" t="s">
         <v>26</v>
       </c>
-      <c r="J56" s="52" t="s">
+      <c r="J56" s="72" t="s">
         <v>56</v>
       </c>
-      <c r="K56" s="49" t="s">
+      <c r="K56" s="60" t="s">
         <v>28</v>
       </c>
       <c r="L56" s="2"/>
@@ -3746,11 +3853,11 @@
       <c r="AA56" s="2"/>
     </row>
     <row r="57" spans="1:27" ht="17.25" customHeight="1">
-      <c r="A57" s="62"/>
-      <c r="B57" s="59"/>
-      <c r="C57" s="59"/>
-      <c r="D57" s="59"/>
-      <c r="E57" s="59"/>
+      <c r="A57" s="76"/>
+      <c r="B57" s="47"/>
+      <c r="C57" s="47"/>
+      <c r="D57" s="47"/>
+      <c r="E57" s="47"/>
       <c r="F57" s="30" t="s">
         <v>67</v>
       </c>
@@ -3760,9 +3867,9 @@
       <c r="H57" s="36" t="s">
         <v>120</v>
       </c>
-      <c r="I57" s="50"/>
-      <c r="J57" s="53"/>
-      <c r="K57" s="50"/>
+      <c r="I57" s="61"/>
+      <c r="J57" s="73"/>
+      <c r="K57" s="61"/>
       <c r="L57" s="2"/>
       <c r="M57" s="2"/>
       <c r="N57" s="2"/>
@@ -3781,11 +3888,11 @@
       <c r="AA57" s="2"/>
     </row>
     <row r="58" spans="1:27" ht="25.5">
-      <c r="A58" s="62"/>
-      <c r="B58" s="59"/>
-      <c r="C58" s="59"/>
-      <c r="D58" s="59"/>
-      <c r="E58" s="59"/>
+      <c r="A58" s="76"/>
+      <c r="B58" s="47"/>
+      <c r="C58" s="47"/>
+      <c r="D58" s="47"/>
+      <c r="E58" s="47"/>
       <c r="F58" s="30" t="s">
         <v>70</v>
       </c>
@@ -3795,9 +3902,9 @@
       <c r="H58" s="36" t="s">
         <v>122</v>
       </c>
-      <c r="I58" s="50"/>
-      <c r="J58" s="53"/>
-      <c r="K58" s="50"/>
+      <c r="I58" s="61"/>
+      <c r="J58" s="73"/>
+      <c r="K58" s="61"/>
       <c r="L58" s="2"/>
       <c r="M58" s="2"/>
       <c r="N58" s="2"/>
@@ -3816,11 +3923,11 @@
       <c r="AA58" s="2"/>
     </row>
     <row r="59" spans="1:27" ht="25.5">
-      <c r="A59" s="63"/>
-      <c r="B59" s="60"/>
-      <c r="C59" s="60"/>
-      <c r="D59" s="60"/>
-      <c r="E59" s="60"/>
+      <c r="A59" s="77"/>
+      <c r="B59" s="48"/>
+      <c r="C59" s="48"/>
+      <c r="D59" s="48"/>
+      <c r="E59" s="48"/>
       <c r="F59" s="30" t="s">
         <v>99</v>
       </c>
@@ -3830,9 +3937,9 @@
       <c r="H59" s="36" t="s">
         <v>123</v>
       </c>
-      <c r="I59" s="51"/>
-      <c r="J59" s="54"/>
-      <c r="K59" s="51"/>
+      <c r="I59" s="62"/>
+      <c r="J59" s="74"/>
+      <c r="K59" s="62"/>
       <c r="L59" s="2"/>
       <c r="M59" s="2"/>
       <c r="N59" s="2"/>
@@ -3851,19 +3958,19 @@
       <c r="AA59" s="2"/>
     </row>
     <row r="60" spans="1:27" ht="25.5">
-      <c r="A60" s="61" t="s">
+      <c r="A60" s="75" t="s">
         <v>43</v>
       </c>
-      <c r="B60" s="58" t="s">
+      <c r="B60" s="46" t="s">
         <v>84</v>
       </c>
-      <c r="C60" s="58" t="s">
+      <c r="C60" s="46" t="s">
         <v>124</v>
       </c>
-      <c r="D60" s="58" t="s">
+      <c r="D60" s="46" t="s">
         <v>125</v>
       </c>
-      <c r="E60" s="58" t="s">
+      <c r="E60" s="46" t="s">
         <v>102</v>
       </c>
       <c r="F60" s="30" t="s">
@@ -3875,13 +3982,13 @@
       <c r="H60" s="35" t="s">
         <v>92</v>
       </c>
-      <c r="I60" s="49" t="s">
+      <c r="I60" s="60" t="s">
         <v>26</v>
       </c>
-      <c r="J60" s="52" t="s">
+      <c r="J60" s="72" t="s">
         <v>56</v>
       </c>
-      <c r="K60" s="49" t="s">
+      <c r="K60" s="60" t="s">
         <v>28</v>
       </c>
       <c r="L60" s="2"/>
@@ -3902,11 +4009,11 @@
       <c r="AA60" s="2"/>
     </row>
     <row r="61" spans="1:27" ht="25.5">
-      <c r="A61" s="62"/>
-      <c r="B61" s="59"/>
-      <c r="C61" s="59"/>
-      <c r="D61" s="59"/>
-      <c r="E61" s="59"/>
+      <c r="A61" s="76"/>
+      <c r="B61" s="47"/>
+      <c r="C61" s="47"/>
+      <c r="D61" s="47"/>
+      <c r="E61" s="47"/>
       <c r="F61" s="30" t="s">
         <v>67</v>
       </c>
@@ -3916,9 +4023,9 @@
       <c r="H61" s="36" t="s">
         <v>120</v>
       </c>
-      <c r="I61" s="50"/>
-      <c r="J61" s="53"/>
-      <c r="K61" s="50"/>
+      <c r="I61" s="61"/>
+      <c r="J61" s="73"/>
+      <c r="K61" s="61"/>
       <c r="L61" s="2"/>
       <c r="M61" s="2"/>
       <c r="N61" s="2"/>
@@ -3937,11 +4044,11 @@
       <c r="AA61" s="2"/>
     </row>
     <row r="62" spans="1:27" ht="25.5">
-      <c r="A62" s="62"/>
-      <c r="B62" s="59"/>
-      <c r="C62" s="59"/>
-      <c r="D62" s="59"/>
-      <c r="E62" s="59"/>
+      <c r="A62" s="76"/>
+      <c r="B62" s="47"/>
+      <c r="C62" s="47"/>
+      <c r="D62" s="47"/>
+      <c r="E62" s="47"/>
       <c r="F62" s="30" t="s">
         <v>70</v>
       </c>
@@ -3951,9 +4058,9 @@
       <c r="H62" s="36" t="s">
         <v>122</v>
       </c>
-      <c r="I62" s="50"/>
-      <c r="J62" s="53"/>
-      <c r="K62" s="50"/>
+      <c r="I62" s="61"/>
+      <c r="J62" s="73"/>
+      <c r="K62" s="61"/>
       <c r="L62" s="2"/>
       <c r="M62" s="2"/>
       <c r="N62" s="2"/>
@@ -3972,11 +4079,11 @@
       <c r="AA62" s="2"/>
     </row>
     <row r="63" spans="1:27" ht="25.5">
-      <c r="A63" s="63"/>
-      <c r="B63" s="60"/>
-      <c r="C63" s="60"/>
-      <c r="D63" s="60"/>
-      <c r="E63" s="60"/>
+      <c r="A63" s="77"/>
+      <c r="B63" s="48"/>
+      <c r="C63" s="48"/>
+      <c r="D63" s="48"/>
+      <c r="E63" s="48"/>
       <c r="F63" s="30" t="s">
         <v>99</v>
       </c>
@@ -3986,9 +4093,9 @@
       <c r="H63" s="35" t="s">
         <v>128</v>
       </c>
-      <c r="I63" s="51"/>
-      <c r="J63" s="54"/>
-      <c r="K63" s="51"/>
+      <c r="I63" s="62"/>
+      <c r="J63" s="74"/>
+      <c r="K63" s="62"/>
       <c r="L63" s="2"/>
       <c r="M63" s="2"/>
       <c r="N63" s="2"/>
@@ -4007,19 +4114,19 @@
       <c r="AA63" s="2"/>
     </row>
     <row r="64" spans="1:27" ht="25.5">
-      <c r="A64" s="64" t="s">
+      <c r="A64" s="83" t="s">
         <v>44</v>
       </c>
-      <c r="B64" s="58" t="s">
+      <c r="B64" s="46" t="s">
         <v>49</v>
       </c>
-      <c r="C64" s="46" t="s">
+      <c r="C64" s="49" t="s">
         <v>130</v>
       </c>
-      <c r="D64" s="58" t="s">
+      <c r="D64" s="46" t="s">
         <v>131</v>
       </c>
-      <c r="E64" s="58" t="s">
+      <c r="E64" s="46" t="s">
         <v>83</v>
       </c>
       <c r="F64" s="30" t="s">
@@ -4031,13 +4138,13 @@
       <c r="H64" s="35" t="s">
         <v>133</v>
       </c>
-      <c r="I64" s="49" t="s">
+      <c r="I64" s="60" t="s">
         <v>26</v>
       </c>
-      <c r="J64" s="52" t="s">
+      <c r="J64" s="72" t="s">
         <v>56</v>
       </c>
-      <c r="K64" s="49" t="s">
+      <c r="K64" s="60" t="s">
         <v>28</v>
       </c>
       <c r="L64" s="2"/>
@@ -4058,17 +4165,17 @@
       <c r="AA64" s="2"/>
     </row>
     <row r="65" spans="1:27">
-      <c r="A65" s="65"/>
-      <c r="B65" s="59"/>
-      <c r="C65" s="67"/>
-      <c r="D65" s="59"/>
-      <c r="E65" s="59"/>
+      <c r="A65" s="84"/>
+      <c r="B65" s="47"/>
+      <c r="C65" s="50"/>
+      <c r="D65" s="47"/>
+      <c r="E65" s="47"/>
       <c r="F65" s="30"/>
       <c r="G65" s="35"/>
       <c r="H65" s="35"/>
-      <c r="I65" s="50"/>
-      <c r="J65" s="53"/>
-      <c r="K65" s="50"/>
+      <c r="I65" s="61"/>
+      <c r="J65" s="73"/>
+      <c r="K65" s="61"/>
       <c r="L65" s="2"/>
       <c r="M65" s="2"/>
       <c r="N65" s="2"/>
@@ -4087,17 +4194,17 @@
       <c r="AA65" s="2"/>
     </row>
     <row r="66" spans="1:27">
-      <c r="A66" s="65"/>
-      <c r="B66" s="59"/>
-      <c r="C66" s="67"/>
-      <c r="D66" s="59"/>
-      <c r="E66" s="59"/>
+      <c r="A66" s="84"/>
+      <c r="B66" s="47"/>
+      <c r="C66" s="50"/>
+      <c r="D66" s="47"/>
+      <c r="E66" s="47"/>
       <c r="F66" s="30"/>
       <c r="G66" s="35"/>
       <c r="H66" s="35"/>
-      <c r="I66" s="50"/>
-      <c r="J66" s="53"/>
-      <c r="K66" s="50"/>
+      <c r="I66" s="61"/>
+      <c r="J66" s="73"/>
+      <c r="K66" s="61"/>
       <c r="L66" s="2"/>
       <c r="M66" s="2"/>
       <c r="N66" s="2"/>
@@ -4116,17 +4223,17 @@
       <c r="AA66" s="2"/>
     </row>
     <row r="67" spans="1:27">
-      <c r="A67" s="66"/>
-      <c r="B67" s="60"/>
-      <c r="C67" s="68"/>
-      <c r="D67" s="60"/>
-      <c r="E67" s="60"/>
+      <c r="A67" s="85"/>
+      <c r="B67" s="48"/>
+      <c r="C67" s="51"/>
+      <c r="D67" s="48"/>
+      <c r="E67" s="48"/>
       <c r="F67" s="30"/>
       <c r="G67" s="35"/>
       <c r="H67" s="35"/>
-      <c r="I67" s="51"/>
-      <c r="J67" s="54"/>
-      <c r="K67" s="51"/>
+      <c r="I67" s="62"/>
+      <c r="J67" s="74"/>
+      <c r="K67" s="62"/>
       <c r="L67" s="2"/>
       <c r="M67" s="2"/>
       <c r="N67" s="2"/>
@@ -4145,19 +4252,19 @@
       <c r="AA67" s="2"/>
     </row>
     <row r="68" spans="1:27" ht="25.5">
-      <c r="A68" s="64" t="s">
+      <c r="A68" s="83" t="s">
         <v>45</v>
       </c>
-      <c r="B68" s="58" t="s">
+      <c r="B68" s="46" t="s">
         <v>49</v>
       </c>
-      <c r="C68" s="46" t="s">
+      <c r="C68" s="49" t="s">
         <v>134</v>
       </c>
-      <c r="D68" s="58" t="s">
+      <c r="D68" s="46" t="s">
         <v>135</v>
       </c>
-      <c r="E68" s="58" t="s">
+      <c r="E68" s="46" t="s">
         <v>83</v>
       </c>
       <c r="F68" s="30" t="s">
@@ -4169,13 +4276,13 @@
       <c r="H68" s="35" t="s">
         <v>137</v>
       </c>
-      <c r="I68" s="49" t="s">
+      <c r="I68" s="60" t="s">
         <v>26</v>
       </c>
-      <c r="J68" s="52" t="s">
+      <c r="J68" s="72" t="s">
         <v>56</v>
       </c>
-      <c r="K68" s="49" t="s">
+      <c r="K68" s="60" t="s">
         <v>28</v>
       </c>
       <c r="L68" s="2"/>
@@ -4196,17 +4303,17 @@
       <c r="AA68" s="2"/>
     </row>
     <row r="69" spans="1:27">
-      <c r="A69" s="65"/>
-      <c r="B69" s="59"/>
-      <c r="C69" s="67"/>
-      <c r="D69" s="59"/>
-      <c r="E69" s="59"/>
+      <c r="A69" s="84"/>
+      <c r="B69" s="47"/>
+      <c r="C69" s="50"/>
+      <c r="D69" s="47"/>
+      <c r="E69" s="47"/>
       <c r="F69" s="30"/>
       <c r="G69" s="35"/>
       <c r="H69" s="35"/>
-      <c r="I69" s="50"/>
-      <c r="J69" s="53"/>
-      <c r="K69" s="50"/>
+      <c r="I69" s="61"/>
+      <c r="J69" s="73"/>
+      <c r="K69" s="61"/>
       <c r="L69" s="2"/>
       <c r="M69" s="2"/>
       <c r="N69" s="2"/>
@@ -4225,17 +4332,17 @@
       <c r="AA69" s="2"/>
     </row>
     <row r="70" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A70" s="65"/>
-      <c r="B70" s="59"/>
-      <c r="C70" s="67"/>
-      <c r="D70" s="59"/>
-      <c r="E70" s="59"/>
+      <c r="A70" s="84"/>
+      <c r="B70" s="47"/>
+      <c r="C70" s="50"/>
+      <c r="D70" s="47"/>
+      <c r="E70" s="47"/>
       <c r="F70" s="30"/>
       <c r="G70" s="35"/>
       <c r="H70" s="35"/>
-      <c r="I70" s="50"/>
-      <c r="J70" s="53"/>
-      <c r="K70" s="50"/>
+      <c r="I70" s="61"/>
+      <c r="J70" s="73"/>
+      <c r="K70" s="61"/>
       <c r="L70" s="2"/>
       <c r="M70" s="2"/>
       <c r="N70" s="2"/>
@@ -4254,17 +4361,17 @@
       <c r="AA70" s="2"/>
     </row>
     <row r="71" spans="1:27">
-      <c r="A71" s="66"/>
-      <c r="B71" s="60"/>
-      <c r="C71" s="68"/>
-      <c r="D71" s="60"/>
-      <c r="E71" s="60"/>
+      <c r="A71" s="85"/>
+      <c r="B71" s="48"/>
+      <c r="C71" s="51"/>
+      <c r="D71" s="48"/>
+      <c r="E71" s="48"/>
       <c r="F71" s="30"/>
       <c r="G71" s="35"/>
       <c r="H71" s="35"/>
-      <c r="I71" s="51"/>
-      <c r="J71" s="54"/>
-      <c r="K71" s="51"/>
+      <c r="I71" s="62"/>
+      <c r="J71" s="74"/>
+      <c r="K71" s="62"/>
       <c r="L71" s="2"/>
       <c r="M71" s="2"/>
       <c r="N71" s="2"/>
@@ -4283,19 +4390,19 @@
       <c r="AA71" s="2"/>
     </row>
     <row r="72" spans="1:27">
-      <c r="A72" s="55" t="s">
+      <c r="A72" s="78" t="s">
         <v>46</v>
       </c>
-      <c r="B72" s="46" t="s">
+      <c r="B72" s="49" t="s">
         <v>138</v>
       </c>
-      <c r="C72" s="46" t="s">
+      <c r="C72" s="49" t="s">
         <v>139</v>
       </c>
-      <c r="D72" s="46" t="s">
+      <c r="D72" s="49" t="s">
         <v>140</v>
       </c>
-      <c r="E72" s="46" t="s">
+      <c r="E72" s="49" t="s">
         <v>141</v>
       </c>
       <c r="F72" s="44" t="s">
@@ -4307,13 +4414,13 @@
       <c r="H72" s="45" t="s">
         <v>143</v>
       </c>
-      <c r="I72" s="49" t="s">
+      <c r="I72" s="60" t="s">
         <v>26</v>
       </c>
-      <c r="J72" s="52" t="s">
+      <c r="J72" s="72" t="s">
         <v>56</v>
       </c>
-      <c r="K72" s="49" t="s">
+      <c r="K72" s="60" t="s">
         <v>28</v>
       </c>
       <c r="L72" s="2"/>
@@ -4334,11 +4441,11 @@
       <c r="AA72" s="2"/>
     </row>
     <row r="73" spans="1:27">
-      <c r="A73" s="56"/>
-      <c r="B73" s="47"/>
-      <c r="C73" s="47"/>
-      <c r="D73" s="47"/>
-      <c r="E73" s="47"/>
+      <c r="A73" s="79"/>
+      <c r="B73" s="81"/>
+      <c r="C73" s="81"/>
+      <c r="D73" s="81"/>
+      <c r="E73" s="81"/>
       <c r="F73" s="44" t="s">
         <v>67</v>
       </c>
@@ -4346,9 +4453,9 @@
         <v>144</v>
       </c>
       <c r="H73" s="45"/>
-      <c r="I73" s="50"/>
-      <c r="J73" s="53"/>
-      <c r="K73" s="50"/>
+      <c r="I73" s="61"/>
+      <c r="J73" s="73"/>
+      <c r="K73" s="61"/>
       <c r="L73" s="2"/>
       <c r="M73" s="2"/>
       <c r="N73" s="2"/>
@@ -4367,11 +4474,11 @@
       <c r="AA73" s="2"/>
     </row>
     <row r="74" spans="1:27">
-      <c r="A74" s="56"/>
-      <c r="B74" s="47"/>
-      <c r="C74" s="47"/>
-      <c r="D74" s="47"/>
-      <c r="E74" s="47"/>
+      <c r="A74" s="79"/>
+      <c r="B74" s="81"/>
+      <c r="C74" s="81"/>
+      <c r="D74" s="81"/>
+      <c r="E74" s="81"/>
       <c r="F74" s="44" t="s">
         <v>70</v>
       </c>
@@ -4381,9 +4488,9 @@
       <c r="H74" s="45" t="s">
         <v>146</v>
       </c>
-      <c r="I74" s="50"/>
-      <c r="J74" s="53"/>
-      <c r="K74" s="50"/>
+      <c r="I74" s="61"/>
+      <c r="J74" s="73"/>
+      <c r="K74" s="61"/>
       <c r="L74" s="2"/>
       <c r="M74" s="2"/>
       <c r="N74" s="2"/>
@@ -4402,11 +4509,11 @@
       <c r="AA74" s="2"/>
     </row>
     <row r="75" spans="1:27">
-      <c r="A75" s="57"/>
-      <c r="B75" s="48"/>
-      <c r="C75" s="48"/>
-      <c r="D75" s="48"/>
-      <c r="E75" s="48"/>
+      <c r="A75" s="80"/>
+      <c r="B75" s="82"/>
+      <c r="C75" s="82"/>
+      <c r="D75" s="82"/>
+      <c r="E75" s="82"/>
       <c r="F75" s="44" t="s">
         <v>99</v>
       </c>
@@ -4416,9 +4523,9 @@
       <c r="H75" s="45" t="s">
         <v>163</v>
       </c>
-      <c r="I75" s="51"/>
-      <c r="J75" s="54"/>
-      <c r="K75" s="51"/>
+      <c r="I75" s="62"/>
+      <c r="J75" s="74"/>
+      <c r="K75" s="62"/>
       <c r="L75" s="2"/>
       <c r="M75" s="2"/>
       <c r="N75" s="2"/>
@@ -4437,19 +4544,19 @@
       <c r="AA75" s="2"/>
     </row>
     <row r="76" spans="1:27">
-      <c r="A76" s="55" t="s">
+      <c r="A76" s="78" t="s">
         <v>47</v>
       </c>
-      <c r="B76" s="46" t="s">
+      <c r="B76" s="49" t="s">
         <v>138</v>
       </c>
-      <c r="C76" s="46" t="s">
+      <c r="C76" s="49" t="s">
         <v>148</v>
       </c>
-      <c r="D76" s="46" t="s">
+      <c r="D76" s="49" t="s">
         <v>149</v>
       </c>
-      <c r="E76" s="46" t="s">
+      <c r="E76" s="49" t="s">
         <v>141</v>
       </c>
       <c r="F76" s="44" t="s">
@@ -4461,13 +4568,13 @@
       <c r="H76" s="45" t="s">
         <v>143</v>
       </c>
-      <c r="I76" s="49" t="s">
+      <c r="I76" s="60" t="s">
         <v>26</v>
       </c>
-      <c r="J76" s="52" t="s">
+      <c r="J76" s="72" t="s">
         <v>56</v>
       </c>
-      <c r="K76" s="49" t="s">
+      <c r="K76" s="60" t="s">
         <v>28</v>
       </c>
       <c r="L76" s="2"/>
@@ -4488,11 +4595,11 @@
       <c r="AA76" s="2"/>
     </row>
     <row r="77" spans="1:27">
-      <c r="A77" s="56"/>
-      <c r="B77" s="47"/>
-      <c r="C77" s="47"/>
-      <c r="D77" s="47"/>
-      <c r="E77" s="47"/>
+      <c r="A77" s="79"/>
+      <c r="B77" s="81"/>
+      <c r="C77" s="81"/>
+      <c r="D77" s="81"/>
+      <c r="E77" s="81"/>
       <c r="F77" s="44" t="s">
         <v>67</v>
       </c>
@@ -4502,9 +4609,9 @@
       <c r="H77" s="45" t="s">
         <v>146</v>
       </c>
-      <c r="I77" s="50"/>
-      <c r="J77" s="53"/>
-      <c r="K77" s="50"/>
+      <c r="I77" s="61"/>
+      <c r="J77" s="73"/>
+      <c r="K77" s="61"/>
       <c r="L77" s="2"/>
       <c r="M77" s="2"/>
       <c r="N77" s="2"/>
@@ -4523,11 +4630,11 @@
       <c r="AA77" s="2"/>
     </row>
     <row r="78" spans="1:27">
-      <c r="A78" s="56"/>
-      <c r="B78" s="47"/>
-      <c r="C78" s="47"/>
-      <c r="D78" s="47"/>
-      <c r="E78" s="47"/>
+      <c r="A78" s="79"/>
+      <c r="B78" s="81"/>
+      <c r="C78" s="81"/>
+      <c r="D78" s="81"/>
+      <c r="E78" s="81"/>
       <c r="F78" s="44" t="s">
         <v>70</v>
       </c>
@@ -4537,9 +4644,9 @@
       <c r="H78" s="45" t="s">
         <v>151</v>
       </c>
-      <c r="I78" s="50"/>
-      <c r="J78" s="53"/>
-      <c r="K78" s="50"/>
+      <c r="I78" s="61"/>
+      <c r="J78" s="73"/>
+      <c r="K78" s="61"/>
       <c r="L78" s="2"/>
       <c r="M78" s="2"/>
       <c r="N78" s="2"/>
@@ -4558,19 +4665,19 @@
       <c r="AA78" s="2"/>
     </row>
     <row r="79" spans="1:27">
-      <c r="A79" s="57"/>
-      <c r="B79" s="48"/>
-      <c r="C79" s="48"/>
-      <c r="D79" s="48"/>
-      <c r="E79" s="48"/>
+      <c r="A79" s="80"/>
+      <c r="B79" s="82"/>
+      <c r="C79" s="82"/>
+      <c r="D79" s="82"/>
+      <c r="E79" s="82"/>
       <c r="F79" s="44" t="s">
         <v>99</v>
       </c>
       <c r="G79" s="45"/>
       <c r="H79" s="45"/>
-      <c r="I79" s="51"/>
-      <c r="J79" s="54"/>
-      <c r="K79" s="51"/>
+      <c r="I79" s="62"/>
+      <c r="J79" s="74"/>
+      <c r="K79" s="62"/>
       <c r="L79" s="2"/>
       <c r="M79" s="2"/>
       <c r="N79" s="2"/>
@@ -4589,19 +4696,19 @@
       <c r="AA79" s="2"/>
     </row>
     <row r="80" spans="1:27">
-      <c r="A80" s="55" t="s">
+      <c r="A80" s="78" t="s">
         <v>48</v>
       </c>
-      <c r="B80" s="46" t="s">
+      <c r="B80" s="49" t="s">
         <v>138</v>
       </c>
-      <c r="C80" s="46" t="s">
+      <c r="C80" s="49" t="s">
         <v>152</v>
       </c>
-      <c r="D80" s="46" t="s">
+      <c r="D80" s="49" t="s">
         <v>153</v>
       </c>
-      <c r="E80" s="46" t="s">
+      <c r="E80" s="49" t="s">
         <v>141</v>
       </c>
       <c r="F80" s="44" t="s">
@@ -4613,13 +4720,13 @@
       <c r="H80" s="45" t="s">
         <v>143</v>
       </c>
-      <c r="I80" s="49" t="s">
+      <c r="I80" s="60" t="s">
         <v>26</v>
       </c>
-      <c r="J80" s="52" t="s">
+      <c r="J80" s="72" t="s">
         <v>56</v>
       </c>
-      <c r="K80" s="49" t="s">
+      <c r="K80" s="60" t="s">
         <v>28</v>
       </c>
       <c r="L80" s="2"/>
@@ -4640,11 +4747,11 @@
       <c r="AA80" s="2"/>
     </row>
     <row r="81" spans="1:27">
-      <c r="A81" s="56"/>
-      <c r="B81" s="47"/>
-      <c r="C81" s="47"/>
-      <c r="D81" s="47"/>
-      <c r="E81" s="47"/>
+      <c r="A81" s="79"/>
+      <c r="B81" s="81"/>
+      <c r="C81" s="81"/>
+      <c r="D81" s="81"/>
+      <c r="E81" s="81"/>
       <c r="F81" s="44" t="s">
         <v>67</v>
       </c>
@@ -4652,9 +4759,9 @@
         <v>154</v>
       </c>
       <c r="H81" s="45"/>
-      <c r="I81" s="50"/>
-      <c r="J81" s="53"/>
-      <c r="K81" s="50"/>
+      <c r="I81" s="61"/>
+      <c r="J81" s="73"/>
+      <c r="K81" s="61"/>
       <c r="L81" s="2"/>
       <c r="M81" s="2"/>
       <c r="N81" s="2"/>
@@ -4673,11 +4780,11 @@
       <c r="AA81" s="2"/>
     </row>
     <row r="82" spans="1:27">
-      <c r="A82" s="56"/>
-      <c r="B82" s="47"/>
-      <c r="C82" s="47"/>
-      <c r="D82" s="47"/>
-      <c r="E82" s="47"/>
+      <c r="A82" s="79"/>
+      <c r="B82" s="81"/>
+      <c r="C82" s="81"/>
+      <c r="D82" s="81"/>
+      <c r="E82" s="81"/>
       <c r="F82" s="44" t="s">
         <v>70</v>
       </c>
@@ -4687,9 +4794,9 @@
       <c r="H82" s="45" t="s">
         <v>146</v>
       </c>
-      <c r="I82" s="50"/>
-      <c r="J82" s="53"/>
-      <c r="K82" s="50"/>
+      <c r="I82" s="61"/>
+      <c r="J82" s="73"/>
+      <c r="K82" s="61"/>
       <c r="L82" s="2"/>
       <c r="M82" s="2"/>
       <c r="N82" s="2"/>
@@ -4708,11 +4815,11 @@
       <c r="AA82" s="2"/>
     </row>
     <row r="83" spans="1:27">
-      <c r="A83" s="57"/>
-      <c r="B83" s="48"/>
-      <c r="C83" s="48"/>
-      <c r="D83" s="48"/>
-      <c r="E83" s="48"/>
+      <c r="A83" s="80"/>
+      <c r="B83" s="82"/>
+      <c r="C83" s="82"/>
+      <c r="D83" s="82"/>
+      <c r="E83" s="82"/>
       <c r="F83" s="44" t="s">
         <v>99</v>
       </c>
@@ -4722,9 +4829,9 @@
       <c r="H83" s="45" t="s">
         <v>156</v>
       </c>
-      <c r="I83" s="51"/>
-      <c r="J83" s="54"/>
-      <c r="K83" s="51"/>
+      <c r="I83" s="62"/>
+      <c r="J83" s="74"/>
+      <c r="K83" s="62"/>
       <c r="L83" s="2"/>
       <c r="M83" s="2"/>
       <c r="N83" s="2"/>
@@ -4743,19 +4850,19 @@
       <c r="AA83" s="2"/>
     </row>
     <row r="84" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A84" s="55" t="s">
+      <c r="A84" s="78" t="s">
         <v>162</v>
       </c>
-      <c r="B84" s="46" t="s">
+      <c r="B84" s="49" t="s">
         <v>138</v>
       </c>
-      <c r="C84" s="46" t="s">
+      <c r="C84" s="49" t="s">
         <v>157</v>
       </c>
-      <c r="D84" s="46" t="s">
+      <c r="D84" s="49" t="s">
         <v>158</v>
       </c>
-      <c r="E84" s="46" t="s">
+      <c r="E84" s="49" t="s">
         <v>141</v>
       </c>
       <c r="F84" s="44" t="s">
@@ -4767,13 +4874,15 @@
       <c r="H84" s="45" t="s">
         <v>143</v>
       </c>
-      <c r="I84" s="49" t="s">
+      <c r="I84" s="60" t="s">
         <v>26</v>
       </c>
-      <c r="J84" s="52" t="s">
+      <c r="J84" s="72" t="s">
         <v>56</v>
       </c>
-      <c r="K84" s="2"/>
+      <c r="K84" s="60" t="s">
+        <v>28</v>
+      </c>
       <c r="L84" s="2"/>
       <c r="M84" s="2"/>
       <c r="N84" s="2"/>
@@ -4792,11 +4901,11 @@
       <c r="AA84" s="2"/>
     </row>
     <row r="85" spans="1:27" ht="24" customHeight="1">
-      <c r="A85" s="56"/>
-      <c r="B85" s="47"/>
-      <c r="C85" s="47"/>
-      <c r="D85" s="47"/>
-      <c r="E85" s="47"/>
+      <c r="A85" s="79"/>
+      <c r="B85" s="81"/>
+      <c r="C85" s="81"/>
+      <c r="D85" s="81"/>
+      <c r="E85" s="81"/>
       <c r="F85" s="44" t="s">
         <v>67</v>
       </c>
@@ -4806,9 +4915,9 @@
       <c r="H85" s="45" t="s">
         <v>160</v>
       </c>
-      <c r="I85" s="50"/>
-      <c r="J85" s="53"/>
-      <c r="K85" s="2"/>
+      <c r="I85" s="61"/>
+      <c r="J85" s="73"/>
+      <c r="K85" s="61"/>
       <c r="L85" s="2"/>
       <c r="M85" s="2"/>
       <c r="N85" s="2"/>
@@ -4827,11 +4936,11 @@
       <c r="AA85" s="2"/>
     </row>
     <row r="86" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A86" s="56"/>
-      <c r="B86" s="47"/>
-      <c r="C86" s="47"/>
-      <c r="D86" s="47"/>
-      <c r="E86" s="47"/>
+      <c r="A86" s="79"/>
+      <c r="B86" s="81"/>
+      <c r="C86" s="81"/>
+      <c r="D86" s="81"/>
+      <c r="E86" s="81"/>
       <c r="F86" s="44" t="s">
         <v>70</v>
       </c>
@@ -4841,9 +4950,9 @@
       <c r="H86" s="45" t="s">
         <v>161</v>
       </c>
-      <c r="I86" s="50"/>
-      <c r="J86" s="53"/>
-      <c r="K86" s="2"/>
+      <c r="I86" s="61"/>
+      <c r="J86" s="73"/>
+      <c r="K86" s="61"/>
       <c r="L86" s="2"/>
       <c r="M86" s="2"/>
       <c r="N86" s="2"/>
@@ -4862,17 +4971,17 @@
       <c r="AA86" s="2"/>
     </row>
     <row r="87" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A87" s="57"/>
-      <c r="B87" s="48"/>
-      <c r="C87" s="48"/>
-      <c r="D87" s="48"/>
-      <c r="E87" s="48"/>
+      <c r="A87" s="80"/>
+      <c r="B87" s="82"/>
+      <c r="C87" s="82"/>
+      <c r="D87" s="82"/>
+      <c r="E87" s="82"/>
       <c r="F87" s="44"/>
       <c r="G87" s="45"/>
       <c r="H87" s="45"/>
-      <c r="I87" s="51"/>
-      <c r="J87" s="54"/>
-      <c r="K87" s="2"/>
+      <c r="I87" s="62"/>
+      <c r="J87" s="74"/>
+      <c r="K87" s="62"/>
       <c r="L87" s="2"/>
       <c r="M87" s="2"/>
       <c r="N87" s="2"/>
@@ -4891,17 +5000,39 @@
       <c r="AA87" s="2"/>
     </row>
     <row r="88" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A88" s="2"/>
-      <c r="B88" s="38"/>
-      <c r="C88" s="2"/>
-      <c r="D88" s="38"/>
-      <c r="E88" s="38"/>
-      <c r="F88" s="2"/>
-      <c r="G88" s="38"/>
-      <c r="H88" s="38"/>
-      <c r="I88" s="2"/>
-      <c r="J88" s="38"/>
-      <c r="K88" s="2"/>
+      <c r="A88" s="90" t="s">
+        <v>169</v>
+      </c>
+      <c r="B88" s="86" t="s">
+        <v>49</v>
+      </c>
+      <c r="C88" s="46" t="s">
+        <v>164</v>
+      </c>
+      <c r="D88" s="46" t="s">
+        <v>165</v>
+      </c>
+      <c r="E88" s="46" t="s">
+        <v>166</v>
+      </c>
+      <c r="F88" s="30" t="s">
+        <v>53</v>
+      </c>
+      <c r="G88" s="30" t="s">
+        <v>167</v>
+      </c>
+      <c r="H88" s="30" t="s">
+        <v>168</v>
+      </c>
+      <c r="I88" s="60" t="s">
+        <v>26</v>
+      </c>
+      <c r="J88" s="72" t="s">
+        <v>56</v>
+      </c>
+      <c r="K88" s="60" t="s">
+        <v>28</v>
+      </c>
       <c r="L88" s="2"/>
       <c r="M88" s="2"/>
       <c r="N88" s="2"/>
@@ -4920,17 +5051,19 @@
       <c r="AA88" s="2"/>
     </row>
     <row r="89" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A89" s="2"/>
-      <c r="B89" s="38"/>
-      <c r="C89" s="2"/>
-      <c r="D89" s="38"/>
-      <c r="E89" s="38"/>
-      <c r="F89" s="2"/>
-      <c r="G89" s="38"/>
-      <c r="H89" s="38"/>
-      <c r="I89" s="2"/>
-      <c r="J89" s="38"/>
-      <c r="K89" s="2"/>
+      <c r="A89" s="91"/>
+      <c r="B89" s="87"/>
+      <c r="C89" s="47"/>
+      <c r="D89" s="47"/>
+      <c r="E89" s="47"/>
+      <c r="F89" s="30" t="s">
+        <v>67</v>
+      </c>
+      <c r="G89" s="35"/>
+      <c r="H89" s="35"/>
+      <c r="I89" s="61"/>
+      <c r="J89" s="73"/>
+      <c r="K89" s="61"/>
       <c r="L89" s="2"/>
       <c r="M89" s="2"/>
       <c r="N89" s="2"/>
@@ -4949,17 +5082,19 @@
       <c r="AA89" s="2"/>
     </row>
     <row r="90" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A90" s="2"/>
-      <c r="B90" s="38"/>
-      <c r="C90" s="2"/>
-      <c r="D90" s="38"/>
-      <c r="E90" s="38"/>
-      <c r="F90" s="2"/>
-      <c r="G90" s="38"/>
-      <c r="H90" s="38"/>
-      <c r="I90" s="2"/>
-      <c r="J90" s="38"/>
-      <c r="K90" s="2"/>
+      <c r="A90" s="91"/>
+      <c r="B90" s="87"/>
+      <c r="C90" s="47"/>
+      <c r="D90" s="47"/>
+      <c r="E90" s="47"/>
+      <c r="F90" s="30" t="s">
+        <v>70</v>
+      </c>
+      <c r="G90" s="88"/>
+      <c r="H90" s="88"/>
+      <c r="I90" s="61"/>
+      <c r="J90" s="73"/>
+      <c r="K90" s="61"/>
       <c r="L90" s="2"/>
       <c r="M90" s="2"/>
       <c r="N90" s="2"/>
@@ -4978,17 +5113,19 @@
       <c r="AA90" s="2"/>
     </row>
     <row r="91" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A91" s="2"/>
-      <c r="B91" s="38"/>
-      <c r="C91" s="2"/>
-      <c r="D91" s="38"/>
-      <c r="E91" s="38"/>
-      <c r="F91" s="2"/>
-      <c r="G91" s="38"/>
-      <c r="H91" s="38"/>
-      <c r="I91" s="2"/>
-      <c r="J91" s="38"/>
-      <c r="K91" s="2"/>
+      <c r="A91" s="92"/>
+      <c r="B91" s="89"/>
+      <c r="C91" s="48"/>
+      <c r="D91" s="48"/>
+      <c r="E91" s="48"/>
+      <c r="F91" s="30" t="s">
+        <v>99</v>
+      </c>
+      <c r="G91" s="30"/>
+      <c r="H91" s="30"/>
+      <c r="I91" s="62"/>
+      <c r="J91" s="74"/>
+      <c r="K91" s="62"/>
       <c r="L91" s="2"/>
       <c r="M91" s="2"/>
       <c r="N91" s="2"/>
@@ -29483,29 +29620,155 @@
       <c r="AA935" s="6"/>
     </row>
   </sheetData>
-  <mergeCells count="185">
-    <mergeCell ref="C32:C35"/>
-    <mergeCell ref="B32:B35"/>
-    <mergeCell ref="B28:B31"/>
-    <mergeCell ref="C4:C7"/>
-    <mergeCell ref="C8:C11"/>
-    <mergeCell ref="C12:C15"/>
-    <mergeCell ref="C16:C19"/>
-    <mergeCell ref="C20:C23"/>
-    <mergeCell ref="C24:C27"/>
-    <mergeCell ref="C28:C31"/>
-    <mergeCell ref="A4:A7"/>
-    <mergeCell ref="A8:A11"/>
-    <mergeCell ref="A12:A15"/>
-    <mergeCell ref="A16:A19"/>
-    <mergeCell ref="A20:A23"/>
-    <mergeCell ref="A24:A27"/>
-    <mergeCell ref="B24:B27"/>
-    <mergeCell ref="B20:B23"/>
-    <mergeCell ref="B16:B19"/>
-    <mergeCell ref="B12:B15"/>
-    <mergeCell ref="B8:B11"/>
-    <mergeCell ref="B4:B7"/>
+  <mergeCells count="194">
+    <mergeCell ref="K84:K87"/>
+    <mergeCell ref="A88:A91"/>
+    <mergeCell ref="B88:B91"/>
+    <mergeCell ref="C88:C91"/>
+    <mergeCell ref="D88:D91"/>
+    <mergeCell ref="E88:E91"/>
+    <mergeCell ref="I88:I91"/>
+    <mergeCell ref="J88:J91"/>
+    <mergeCell ref="K88:K91"/>
+    <mergeCell ref="B84:B87"/>
+    <mergeCell ref="C84:C87"/>
+    <mergeCell ref="D84:D87"/>
+    <mergeCell ref="E84:E87"/>
+    <mergeCell ref="I84:I87"/>
+    <mergeCell ref="J84:J87"/>
+    <mergeCell ref="A84:A87"/>
+    <mergeCell ref="B36:B39"/>
+    <mergeCell ref="C36:C39"/>
+    <mergeCell ref="D36:D39"/>
+    <mergeCell ref="E36:E39"/>
+    <mergeCell ref="J44:J47"/>
+    <mergeCell ref="J36:J39"/>
+    <mergeCell ref="A76:A79"/>
+    <mergeCell ref="B76:B79"/>
+    <mergeCell ref="C76:C79"/>
+    <mergeCell ref="D76:D79"/>
+    <mergeCell ref="E76:E79"/>
+    <mergeCell ref="I76:I79"/>
+    <mergeCell ref="J76:J79"/>
+    <mergeCell ref="A60:A63"/>
+    <mergeCell ref="J56:J59"/>
+    <mergeCell ref="K44:K47"/>
+    <mergeCell ref="I48:I51"/>
+    <mergeCell ref="J48:J51"/>
+    <mergeCell ref="K48:K51"/>
+    <mergeCell ref="B48:B51"/>
+    <mergeCell ref="C48:C51"/>
+    <mergeCell ref="D48:D51"/>
+    <mergeCell ref="E48:E51"/>
+    <mergeCell ref="K40:K43"/>
+    <mergeCell ref="I40:I43"/>
+    <mergeCell ref="B40:B43"/>
+    <mergeCell ref="C40:C43"/>
+    <mergeCell ref="D40:D43"/>
+    <mergeCell ref="E40:E43"/>
+    <mergeCell ref="K76:K79"/>
+    <mergeCell ref="J80:J83"/>
+    <mergeCell ref="K80:K83"/>
+    <mergeCell ref="A80:A83"/>
+    <mergeCell ref="B80:B83"/>
+    <mergeCell ref="C80:C83"/>
+    <mergeCell ref="D80:D83"/>
+    <mergeCell ref="E80:E83"/>
+    <mergeCell ref="I80:I83"/>
+    <mergeCell ref="K56:K59"/>
+    <mergeCell ref="J60:J63"/>
+    <mergeCell ref="K60:K63"/>
+    <mergeCell ref="I68:I71"/>
+    <mergeCell ref="J68:J71"/>
+    <mergeCell ref="K68:K71"/>
+    <mergeCell ref="A72:A75"/>
+    <mergeCell ref="B72:B75"/>
+    <mergeCell ref="C72:C75"/>
+    <mergeCell ref="D72:D75"/>
+    <mergeCell ref="E72:E75"/>
+    <mergeCell ref="I72:I75"/>
+    <mergeCell ref="J72:J75"/>
+    <mergeCell ref="K72:K75"/>
+    <mergeCell ref="A68:A71"/>
+    <mergeCell ref="B68:B71"/>
+    <mergeCell ref="C68:C71"/>
+    <mergeCell ref="D68:D71"/>
+    <mergeCell ref="E68:E71"/>
+    <mergeCell ref="A64:A67"/>
+    <mergeCell ref="J64:J67"/>
+    <mergeCell ref="K64:K67"/>
+    <mergeCell ref="D2:D3"/>
+    <mergeCell ref="J52:J55"/>
+    <mergeCell ref="K52:K55"/>
+    <mergeCell ref="E52:E55"/>
+    <mergeCell ref="B44:B47"/>
+    <mergeCell ref="C44:C47"/>
+    <mergeCell ref="D44:D47"/>
+    <mergeCell ref="E44:E47"/>
+    <mergeCell ref="B64:B67"/>
+    <mergeCell ref="C64:C67"/>
+    <mergeCell ref="D64:D67"/>
+    <mergeCell ref="E64:E67"/>
+    <mergeCell ref="I64:I67"/>
+    <mergeCell ref="B60:B63"/>
+    <mergeCell ref="C60:C63"/>
+    <mergeCell ref="D60:D63"/>
+    <mergeCell ref="E60:E63"/>
+    <mergeCell ref="I60:I63"/>
+    <mergeCell ref="E56:E59"/>
+    <mergeCell ref="I52:I55"/>
+    <mergeCell ref="B56:B59"/>
+    <mergeCell ref="I56:I59"/>
+    <mergeCell ref="I44:I47"/>
+    <mergeCell ref="J40:J43"/>
+    <mergeCell ref="J32:J35"/>
+    <mergeCell ref="B2:B3"/>
+    <mergeCell ref="A2:A3"/>
+    <mergeCell ref="A52:A55"/>
+    <mergeCell ref="B52:B55"/>
+    <mergeCell ref="C56:C59"/>
+    <mergeCell ref="D56:D59"/>
+    <mergeCell ref="C52:C55"/>
+    <mergeCell ref="D52:D55"/>
+    <mergeCell ref="A44:A47"/>
+    <mergeCell ref="A48:A51"/>
+    <mergeCell ref="D24:D27"/>
+    <mergeCell ref="D20:D23"/>
+    <mergeCell ref="D16:D19"/>
+    <mergeCell ref="D12:D15"/>
+    <mergeCell ref="D8:D11"/>
+    <mergeCell ref="D4:D7"/>
+    <mergeCell ref="A28:A31"/>
+    <mergeCell ref="A32:A35"/>
+    <mergeCell ref="A36:A39"/>
+    <mergeCell ref="A40:A43"/>
+    <mergeCell ref="D32:D35"/>
+    <mergeCell ref="D28:D31"/>
+    <mergeCell ref="A56:A59"/>
+    <mergeCell ref="E32:E35"/>
+    <mergeCell ref="C2:C3"/>
+    <mergeCell ref="H4:H5"/>
+    <mergeCell ref="G4:G5"/>
+    <mergeCell ref="H8:H9"/>
+    <mergeCell ref="H12:H13"/>
+    <mergeCell ref="K32:K35"/>
+    <mergeCell ref="K36:K39"/>
+    <mergeCell ref="J4:J7"/>
+    <mergeCell ref="J8:J11"/>
+    <mergeCell ref="J12:J15"/>
+    <mergeCell ref="J16:J19"/>
+    <mergeCell ref="J20:J23"/>
+    <mergeCell ref="J24:J27"/>
+    <mergeCell ref="J28:J31"/>
+    <mergeCell ref="I32:I35"/>
+    <mergeCell ref="I36:I39"/>
+    <mergeCell ref="K4:K7"/>
+    <mergeCell ref="K8:K11"/>
+    <mergeCell ref="K12:K15"/>
+    <mergeCell ref="K16:K19"/>
+    <mergeCell ref="K20:K23"/>
+    <mergeCell ref="K24:K27"/>
+    <mergeCell ref="J2:J3"/>
     <mergeCell ref="K2:K3"/>
     <mergeCell ref="I4:I7"/>
     <mergeCell ref="I8:I11"/>
@@ -29530,251 +29793,154 @@
     <mergeCell ref="E4:E7"/>
     <mergeCell ref="E8:E11"/>
     <mergeCell ref="E12:E15"/>
-    <mergeCell ref="E32:E35"/>
-    <mergeCell ref="C2:C3"/>
-    <mergeCell ref="H4:H5"/>
-    <mergeCell ref="G4:G5"/>
-    <mergeCell ref="H8:H9"/>
-    <mergeCell ref="H12:H13"/>
-    <mergeCell ref="K32:K35"/>
-    <mergeCell ref="K36:K39"/>
-    <mergeCell ref="J4:J7"/>
-    <mergeCell ref="J8:J11"/>
-    <mergeCell ref="J12:J15"/>
-    <mergeCell ref="J16:J19"/>
-    <mergeCell ref="J20:J23"/>
-    <mergeCell ref="J24:J27"/>
-    <mergeCell ref="J28:J31"/>
-    <mergeCell ref="I32:I35"/>
-    <mergeCell ref="I36:I39"/>
-    <mergeCell ref="K4:K7"/>
-    <mergeCell ref="K8:K11"/>
-    <mergeCell ref="K12:K15"/>
-    <mergeCell ref="K16:K19"/>
-    <mergeCell ref="K20:K23"/>
-    <mergeCell ref="K24:K27"/>
-    <mergeCell ref="J2:J3"/>
-    <mergeCell ref="J32:J35"/>
-    <mergeCell ref="B2:B3"/>
-    <mergeCell ref="A2:A3"/>
-    <mergeCell ref="A52:A55"/>
-    <mergeCell ref="B52:B55"/>
-    <mergeCell ref="C56:C59"/>
-    <mergeCell ref="D56:D59"/>
-    <mergeCell ref="C52:C55"/>
-    <mergeCell ref="D52:D55"/>
-    <mergeCell ref="A44:A47"/>
-    <mergeCell ref="A48:A51"/>
-    <mergeCell ref="D24:D27"/>
-    <mergeCell ref="D20:D23"/>
-    <mergeCell ref="D16:D19"/>
-    <mergeCell ref="D12:D15"/>
-    <mergeCell ref="D8:D11"/>
-    <mergeCell ref="D4:D7"/>
-    <mergeCell ref="A28:A31"/>
-    <mergeCell ref="A32:A35"/>
-    <mergeCell ref="A36:A39"/>
-    <mergeCell ref="A40:A43"/>
-    <mergeCell ref="D32:D35"/>
-    <mergeCell ref="D28:D31"/>
-    <mergeCell ref="A56:A59"/>
-    <mergeCell ref="D2:D3"/>
-    <mergeCell ref="J52:J55"/>
-    <mergeCell ref="K52:K55"/>
-    <mergeCell ref="E52:E55"/>
-    <mergeCell ref="B44:B47"/>
-    <mergeCell ref="C44:C47"/>
-    <mergeCell ref="D44:D47"/>
-    <mergeCell ref="E44:E47"/>
-    <mergeCell ref="B64:B67"/>
-    <mergeCell ref="C64:C67"/>
-    <mergeCell ref="D64:D67"/>
-    <mergeCell ref="E64:E67"/>
-    <mergeCell ref="I64:I67"/>
-    <mergeCell ref="B60:B63"/>
-    <mergeCell ref="C60:C63"/>
-    <mergeCell ref="D60:D63"/>
-    <mergeCell ref="E60:E63"/>
-    <mergeCell ref="I60:I63"/>
-    <mergeCell ref="E56:E59"/>
-    <mergeCell ref="I52:I55"/>
-    <mergeCell ref="B56:B59"/>
-    <mergeCell ref="I56:I59"/>
-    <mergeCell ref="I44:I47"/>
-    <mergeCell ref="J40:J43"/>
-    <mergeCell ref="K56:K59"/>
-    <mergeCell ref="J60:J63"/>
-    <mergeCell ref="K60:K63"/>
-    <mergeCell ref="I68:I71"/>
-    <mergeCell ref="J68:J71"/>
-    <mergeCell ref="K68:K71"/>
-    <mergeCell ref="A72:A75"/>
-    <mergeCell ref="B72:B75"/>
-    <mergeCell ref="C72:C75"/>
-    <mergeCell ref="D72:D75"/>
-    <mergeCell ref="E72:E75"/>
-    <mergeCell ref="I72:I75"/>
-    <mergeCell ref="J72:J75"/>
-    <mergeCell ref="K72:K75"/>
-    <mergeCell ref="A68:A71"/>
-    <mergeCell ref="B68:B71"/>
-    <mergeCell ref="C68:C71"/>
-    <mergeCell ref="D68:D71"/>
-    <mergeCell ref="E68:E71"/>
-    <mergeCell ref="A64:A67"/>
-    <mergeCell ref="J64:J67"/>
-    <mergeCell ref="K64:K67"/>
-    <mergeCell ref="K76:K79"/>
-    <mergeCell ref="J80:J83"/>
-    <mergeCell ref="K80:K83"/>
-    <mergeCell ref="A80:A83"/>
-    <mergeCell ref="B80:B83"/>
-    <mergeCell ref="C80:C83"/>
-    <mergeCell ref="D80:D83"/>
-    <mergeCell ref="E80:E83"/>
-    <mergeCell ref="I80:I83"/>
-    <mergeCell ref="K44:K47"/>
-    <mergeCell ref="I48:I51"/>
-    <mergeCell ref="J48:J51"/>
-    <mergeCell ref="K48:K51"/>
-    <mergeCell ref="B48:B51"/>
-    <mergeCell ref="C48:C51"/>
-    <mergeCell ref="D48:D51"/>
-    <mergeCell ref="E48:E51"/>
-    <mergeCell ref="K40:K43"/>
-    <mergeCell ref="I40:I43"/>
-    <mergeCell ref="B40:B43"/>
-    <mergeCell ref="C40:C43"/>
-    <mergeCell ref="D40:D43"/>
-    <mergeCell ref="E40:E43"/>
-    <mergeCell ref="B84:B87"/>
-    <mergeCell ref="C84:C87"/>
-    <mergeCell ref="D84:D87"/>
-    <mergeCell ref="E84:E87"/>
-    <mergeCell ref="I84:I87"/>
-    <mergeCell ref="J84:J87"/>
-    <mergeCell ref="A84:A87"/>
-    <mergeCell ref="B36:B39"/>
-    <mergeCell ref="C36:C39"/>
-    <mergeCell ref="D36:D39"/>
-    <mergeCell ref="E36:E39"/>
-    <mergeCell ref="J44:J47"/>
-    <mergeCell ref="J36:J39"/>
-    <mergeCell ref="A76:A79"/>
-    <mergeCell ref="B76:B79"/>
-    <mergeCell ref="C76:C79"/>
-    <mergeCell ref="D76:D79"/>
-    <mergeCell ref="E76:E79"/>
-    <mergeCell ref="I76:I79"/>
-    <mergeCell ref="J76:J79"/>
-    <mergeCell ref="A60:A63"/>
-    <mergeCell ref="J56:J59"/>
+    <mergeCell ref="A4:A7"/>
+    <mergeCell ref="A8:A11"/>
+    <mergeCell ref="A12:A15"/>
+    <mergeCell ref="A16:A19"/>
+    <mergeCell ref="A20:A23"/>
+    <mergeCell ref="A24:A27"/>
+    <mergeCell ref="B24:B27"/>
+    <mergeCell ref="B20:B23"/>
+    <mergeCell ref="B16:B19"/>
+    <mergeCell ref="B12:B15"/>
+    <mergeCell ref="B8:B11"/>
+    <mergeCell ref="B4:B7"/>
+    <mergeCell ref="C32:C35"/>
+    <mergeCell ref="B32:B35"/>
+    <mergeCell ref="B28:B31"/>
+    <mergeCell ref="C4:C7"/>
+    <mergeCell ref="C8:C11"/>
+    <mergeCell ref="C12:C15"/>
+    <mergeCell ref="C16:C19"/>
+    <mergeCell ref="C20:C23"/>
+    <mergeCell ref="C24:C27"/>
+    <mergeCell ref="C28:C31"/>
   </mergeCells>
   <conditionalFormatting sqref="I4 I8 I12">
-    <cfRule type="cellIs" dxfId="19" priority="17" operator="equal">
+    <cfRule type="cellIs" dxfId="27" priority="21" operator="equal">
       <formula>"TO DO"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I4 I8 I12">
-    <cfRule type="cellIs" dxfId="18" priority="18" operator="equal">
+    <cfRule type="cellIs" dxfId="26" priority="22" operator="equal">
       <formula>"IN PROGRESS"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I4 I8 I12">
-    <cfRule type="cellIs" dxfId="17" priority="19" operator="equal">
+    <cfRule type="cellIs" dxfId="25" priority="23" operator="equal">
       <formula>"REVIEWED"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I4 I8 I12">
-    <cfRule type="cellIs" dxfId="16" priority="20" operator="equal">
+    <cfRule type="cellIs" dxfId="24" priority="24" operator="equal">
       <formula>"IN REVIEW"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I16 I20 I24">
-    <cfRule type="cellIs" dxfId="15" priority="13" operator="equal">
+    <cfRule type="cellIs" dxfId="23" priority="17" operator="equal">
       <formula>"TO DO"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I16 I20 I24">
-    <cfRule type="cellIs" dxfId="14" priority="14" operator="equal">
+    <cfRule type="cellIs" dxfId="22" priority="18" operator="equal">
       <formula>"IN PROGRESS"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I16 I20 I24">
-    <cfRule type="cellIs" dxfId="13" priority="15" operator="equal">
+    <cfRule type="cellIs" dxfId="21" priority="19" operator="equal">
       <formula>"REVIEWED"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I16 I20 I24">
-    <cfRule type="cellIs" dxfId="12" priority="16" operator="equal">
+    <cfRule type="cellIs" dxfId="20" priority="20" operator="equal">
       <formula>"IN REVIEW"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I28 I32 I36 I40 I44 I48 I52 I56 I60">
-    <cfRule type="cellIs" dxfId="11" priority="9" operator="equal">
+    <cfRule type="cellIs" dxfId="19" priority="13" operator="equal">
       <formula>"TO DO"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I28 I32 I36 I40 I44 I48 I52 I56 I60">
-    <cfRule type="cellIs" dxfId="10" priority="10" operator="equal">
+    <cfRule type="cellIs" dxfId="18" priority="14" operator="equal">
       <formula>"IN PROGRESS"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I28 I32 I36 I40 I44 I48 I52 I56 I60">
-    <cfRule type="cellIs" dxfId="9" priority="11" operator="equal">
+    <cfRule type="cellIs" dxfId="17" priority="15" operator="equal">
       <formula>"REVIEWED"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I28 I32 I36 I40 I44 I48 I52 I56 I60">
-    <cfRule type="cellIs" dxfId="8" priority="12" operator="equal">
+    <cfRule type="cellIs" dxfId="16" priority="16" operator="equal">
       <formula>"IN REVIEW"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I64 I68">
-    <cfRule type="cellIs" dxfId="7" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="15" priority="9" operator="equal">
       <formula>"TO DO"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I64 I68">
-    <cfRule type="cellIs" dxfId="6" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="14" priority="10" operator="equal">
       <formula>"IN PROGRESS"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I64 I68">
-    <cfRule type="cellIs" dxfId="5" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="13" priority="11" operator="equal">
       <formula>"REVIEWED"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I64 I68">
-    <cfRule type="cellIs" dxfId="4" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="12" priority="12" operator="equal">
       <formula>"IN REVIEW"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I76 I72 I80 I84">
-    <cfRule type="cellIs" dxfId="3" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="11" priority="5" operator="equal">
       <formula>"TO DO"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I76 I72 I80 I84">
-    <cfRule type="cellIs" dxfId="2" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="10" priority="6" operator="equal">
       <formula>"IN PROGRESS"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I76 I72 I80 I84">
-    <cfRule type="cellIs" dxfId="1" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="9" priority="7" operator="equal">
       <formula>"REVIEWED"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I76 I72 I80 I84">
-    <cfRule type="cellIs" dxfId="0" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="8" priority="8" operator="equal">
+      <formula>"IN REVIEW"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I88">
+    <cfRule type="cellIs" dxfId="7" priority="1" operator="equal">
+      <formula>"TO DO"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I88">
+    <cfRule type="cellIs" dxfId="5" priority="2" operator="equal">
+      <formula>"IN PROGRESS"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I88">
+    <cfRule type="cellIs" dxfId="3" priority="3" operator="equal">
+      <formula>"REVIEWED"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I88">
+    <cfRule type="cellIs" dxfId="1" priority="4" operator="equal">
       <formula>"IN REVIEW"</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" sqref="I52 I64 I24 I16 I20 I4 I8 I12 I68 I56 I60 I32 I36 I28 I40 I44 I48 I84 I76 I72 I80">
+    <dataValidation type="list" allowBlank="1" sqref="I52 I64 I24 I16 I20 I4 I8 I12 I68 I56 I60 I32 I36 I28 I40 I44 I48 I84 I76 I72 I80 I88">
       <formula1>"TO DO,In Progress,In Review,Reviewed"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" sqref="K76 K36 K40 K32 K28 K4 K12 K8 K48 K44 K52 K60 K56 K64 K68 K72 K80 K20 K24 K16">
+    <dataValidation type="list" allowBlank="1" sqref="K76 K36 K40 K32 K28 K4 K12 K8 K48 K44 K52 K60 K56 K64 K68 K72 K80 K20 K24 K16 K84 K88">
       <formula1>"Smoke,Regresión"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
Agrego Casos de Prueba referentes a la Gestion de Usuarios de la web
</commit_message>
<xml_diff>
--- a/Testing 2024/template_caso_prueba-ISPC2024-sprint-1.xlsx
+++ b/Testing 2024/template_caso_prueba-ISPC2024-sprint-1.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="363" uniqueCount="170">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="419" uniqueCount="190">
   <si>
     <t>Id</t>
   </si>
@@ -536,6 +536,66 @@
   <si>
     <t>TC-022</t>
   </si>
+  <si>
+    <t>Icono de cerrar bloque en formulario de login</t>
+  </si>
+  <si>
+    <t>Un usuario abre el formulario para loguearse y luego decide cerrarlo</t>
+  </si>
+  <si>
+    <t>El usuario debe visualizar el formulario de login</t>
+  </si>
+  <si>
+    <t>Oprimir el icono en forma de "X" en el extremo superior derecho</t>
+  </si>
+  <si>
+    <t>Deberá cerrarse el bloque</t>
+  </si>
+  <si>
+    <t>Icono de cerrar bloque en formulario de registro</t>
+  </si>
+  <si>
+    <t>Un usuario abre el formulario para registrarse y luego decide cerrarlo</t>
+  </si>
+  <si>
+    <t>El usuario debe visualizar el formulario de registro</t>
+  </si>
+  <si>
+    <t>El formulario de login tiene un link que redirecciona al formulario de registro</t>
+  </si>
+  <si>
+    <t>El formulario de login tiene en su parte inferior un texto con un link que redirecciona al formulario de registro</t>
+  </si>
+  <si>
+    <t>Hacer click en el texto/link que dice "registrarme" debajo del boton de "ingresar"</t>
+  </si>
+  <si>
+    <t>Se visualiza el formulario de Registro</t>
+  </si>
+  <si>
+    <t>El formulario de registro tiene un link que redirecciona al formulario de login</t>
+  </si>
+  <si>
+    <t>El formulario de registro tiene en su parte inferior un texto con un link que redirecciona al formulario de login</t>
+  </si>
+  <si>
+    <t>Hacer click en el texto/link que dice "iniciar sesion" debajo del boton de "crear cuenta"</t>
+  </si>
+  <si>
+    <t>Se visualiza el formulario de Login</t>
+  </si>
+  <si>
+    <t>TC-023</t>
+  </si>
+  <si>
+    <t>TC-024</t>
+  </si>
+  <si>
+    <t>TC-025</t>
+  </si>
+  <si>
+    <t>TC-026</t>
+  </si>
 </sst>
 </file>
 
@@ -703,7 +763,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="23">
+  <borders count="24">
     <border>
       <left/>
       <right/>
@@ -969,11 +1029,26 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="93">
+  <cellXfs count="94">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -1074,6 +1149,30 @@
     <xf numFmtId="0" fontId="11" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="15" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="15" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="15" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1083,14 +1182,89 @@
     <xf numFmtId="0" fontId="1" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="11" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="14" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="14" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="14" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="12" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="12" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="12" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="13" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="13" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="13" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="9" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="10" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1110,115 +1284,41 @@
     <xf numFmtId="0" fontId="1" fillId="11" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="9" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="12" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="12" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="12" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="14" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="14" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="14" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="13" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="13" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="13" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="15" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="15" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="15" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="28">
+  <dxfs count="32">
     <dxf>
       <fill>
         <patternFill patternType="solid">
           <fgColor rgb="FFFCE5CD"/>
           <bgColor rgb="FFFCE5CD"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF93C47D"/>
+          <bgColor rgb="FF93C47D"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFF2CC"/>
+          <bgColor rgb="FFFFF2CC"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFA2C4C9"/>
+          <bgColor rgb="FFA2C4C9"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1241,6 +1341,30 @@
     <dxf>
       <fill>
         <patternFill patternType="solid">
+          <fgColor rgb="FFFFF2CC"/>
+          <bgColor rgb="FFFFF2CC"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFA2C4C9"/>
+          <bgColor rgb="FFA2C4C9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFCE5CD"/>
+          <bgColor rgb="FFFCE5CD"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
           <fgColor rgb="FF93C47D"/>
           <bgColor rgb="FF93C47D"/>
         </patternFill>
@@ -1251,22 +1375,6 @@
         <patternFill patternType="solid">
           <fgColor rgb="FFFFF2CC"/>
           <bgColor rgb="FFFFF2CC"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFF2CC"/>
-          <bgColor rgb="FFFFF2CC"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFA2C4C9"/>
-          <bgColor rgb="FFA2C4C9"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1788,8 +1896,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AA935"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A70" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="60" workbookViewId="0">
-      <selection activeCell="E95" sqref="E95"/>
+    <sheetView tabSelected="1" topLeftCell="A93" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="60" workbookViewId="0">
+      <selection activeCell="M106" sqref="M106"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5703125" defaultRowHeight="12.75"/>
@@ -1838,33 +1946,33 @@
       <c r="AA1" s="2"/>
     </row>
     <row r="2" spans="1:27" s="31" customFormat="1" ht="15.75" customHeight="1">
-      <c r="A2" s="68" t="s">
+      <c r="A2" s="78" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="58" t="s">
+      <c r="B2" s="76" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="68" t="s">
+      <c r="C2" s="78" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="58" t="s">
+      <c r="D2" s="76" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="58" t="s">
+      <c r="E2" s="76" t="s">
         <v>4</v>
       </c>
-      <c r="F2" s="63" t="s">
+      <c r="F2" s="82" t="s">
         <v>5</v>
       </c>
-      <c r="G2" s="64"/>
-      <c r="H2" s="65"/>
-      <c r="I2" s="66" t="s">
+      <c r="G2" s="83"/>
+      <c r="H2" s="84"/>
+      <c r="I2" s="85" t="s">
         <v>6</v>
       </c>
-      <c r="J2" s="58" t="s">
+      <c r="J2" s="76" t="s">
         <v>7</v>
       </c>
-      <c r="K2" s="58" t="s">
+      <c r="K2" s="76" t="s">
         <v>27</v>
       </c>
       <c r="L2" s="32"/>
@@ -1885,11 +1993,11 @@
       <c r="AA2" s="33"/>
     </row>
     <row r="3" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A3" s="69"/>
-      <c r="B3" s="59"/>
-      <c r="C3" s="69"/>
-      <c r="D3" s="59"/>
-      <c r="E3" s="59"/>
+      <c r="A3" s="79"/>
+      <c r="B3" s="77"/>
+      <c r="C3" s="79"/>
+      <c r="D3" s="77"/>
+      <c r="E3" s="77"/>
       <c r="F3" s="34" t="s">
         <v>8</v>
       </c>
@@ -1899,9 +2007,9 @@
       <c r="H3" s="42" t="s">
         <v>10</v>
       </c>
-      <c r="I3" s="67"/>
-      <c r="J3" s="59"/>
-      <c r="K3" s="59"/>
+      <c r="I3" s="86"/>
+      <c r="J3" s="77"/>
+      <c r="K3" s="77"/>
       <c r="L3" s="3"/>
       <c r="M3" s="2"/>
       <c r="N3" s="2"/>
@@ -1920,37 +2028,37 @@
       <c r="AA3" s="2"/>
     </row>
     <row r="4" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A4" s="52" t="s">
+      <c r="A4" s="87" t="s">
         <v>29</v>
       </c>
-      <c r="B4" s="46" t="s">
+      <c r="B4" s="56" t="s">
         <v>49</v>
       </c>
-      <c r="C4" s="46" t="s">
+      <c r="C4" s="56" t="s">
         <v>50</v>
       </c>
-      <c r="D4" s="46" t="s">
+      <c r="D4" s="56" t="s">
         <v>51</v>
       </c>
-      <c r="E4" s="46" t="s">
+      <c r="E4" s="56" t="s">
         <v>52</v>
       </c>
-      <c r="F4" s="46" t="s">
+      <c r="F4" s="56" t="s">
         <v>53</v>
       </c>
-      <c r="G4" s="46" t="s">
+      <c r="G4" s="56" t="s">
         <v>54</v>
       </c>
-      <c r="H4" s="70" t="s">
+      <c r="H4" s="80" t="s">
         <v>55</v>
       </c>
-      <c r="I4" s="60" t="s">
+      <c r="I4" s="47" t="s">
         <v>26</v>
       </c>
-      <c r="J4" s="72" t="s">
+      <c r="J4" s="59" t="s">
         <v>56</v>
       </c>
-      <c r="K4" s="60" t="s">
+      <c r="K4" s="47" t="s">
         <v>28</v>
       </c>
       <c r="L4" s="3"/>
@@ -1971,17 +2079,17 @@
       <c r="AA4" s="2"/>
     </row>
     <row r="5" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A5" s="53"/>
-      <c r="B5" s="47"/>
-      <c r="C5" s="47"/>
-      <c r="D5" s="47"/>
-      <c r="E5" s="47"/>
-      <c r="F5" s="48"/>
-      <c r="G5" s="48"/>
-      <c r="H5" s="71"/>
-      <c r="I5" s="61"/>
-      <c r="J5" s="73"/>
-      <c r="K5" s="61"/>
+      <c r="A5" s="88"/>
+      <c r="B5" s="57"/>
+      <c r="C5" s="57"/>
+      <c r="D5" s="57"/>
+      <c r="E5" s="57"/>
+      <c r="F5" s="58"/>
+      <c r="G5" s="58"/>
+      <c r="H5" s="81"/>
+      <c r="I5" s="48"/>
+      <c r="J5" s="60"/>
+      <c r="K5" s="48"/>
       <c r="L5" s="3"/>
       <c r="M5" s="2"/>
       <c r="N5" s="2"/>
@@ -2000,17 +2108,17 @@
       <c r="AA5" s="2"/>
     </row>
     <row r="6" spans="1:27" s="29" customFormat="1" ht="15.75" customHeight="1">
-      <c r="A6" s="53"/>
-      <c r="B6" s="47"/>
-      <c r="C6" s="47"/>
-      <c r="D6" s="47"/>
-      <c r="E6" s="47"/>
+      <c r="A6" s="88"/>
+      <c r="B6" s="57"/>
+      <c r="C6" s="57"/>
+      <c r="D6" s="57"/>
+      <c r="E6" s="57"/>
       <c r="F6" s="30"/>
       <c r="G6" s="35"/>
       <c r="H6" s="35"/>
-      <c r="I6" s="61"/>
-      <c r="J6" s="73"/>
-      <c r="K6" s="61"/>
+      <c r="I6" s="48"/>
+      <c r="J6" s="60"/>
+      <c r="K6" s="48"/>
       <c r="L6" s="27"/>
       <c r="M6" s="28"/>
       <c r="N6" s="28"/>
@@ -2029,17 +2137,17 @@
       <c r="AA6" s="28"/>
     </row>
     <row r="7" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A7" s="54"/>
-      <c r="B7" s="48"/>
-      <c r="C7" s="48"/>
-      <c r="D7" s="48"/>
-      <c r="E7" s="48"/>
+      <c r="A7" s="89"/>
+      <c r="B7" s="58"/>
+      <c r="C7" s="58"/>
+      <c r="D7" s="58"/>
+      <c r="E7" s="58"/>
       <c r="F7" s="30"/>
       <c r="G7" s="35"/>
       <c r="H7" s="35"/>
-      <c r="I7" s="62"/>
-      <c r="J7" s="74"/>
-      <c r="K7" s="62"/>
+      <c r="I7" s="49"/>
+      <c r="J7" s="61"/>
+      <c r="K7" s="49"/>
       <c r="L7" s="3"/>
       <c r="M7" s="2"/>
       <c r="N7" s="2"/>
@@ -2058,37 +2166,37 @@
       <c r="AA7" s="2"/>
     </row>
     <row r="8" spans="1:27">
-      <c r="A8" s="52" t="s">
+      <c r="A8" s="87" t="s">
         <v>30</v>
       </c>
-      <c r="B8" s="46" t="s">
+      <c r="B8" s="56" t="s">
         <v>49</v>
       </c>
-      <c r="C8" s="46" t="s">
+      <c r="C8" s="56" t="s">
         <v>57</v>
       </c>
-      <c r="D8" s="46" t="s">
+      <c r="D8" s="56" t="s">
         <v>58</v>
       </c>
-      <c r="E8" s="46" t="s">
+      <c r="E8" s="56" t="s">
         <v>59</v>
       </c>
-      <c r="F8" s="46" t="s">
+      <c r="F8" s="56" t="s">
         <v>53</v>
       </c>
-      <c r="G8" s="46" t="s">
+      <c r="G8" s="56" t="s">
         <v>54</v>
       </c>
-      <c r="H8" s="70" t="s">
+      <c r="H8" s="80" t="s">
         <v>55</v>
       </c>
-      <c r="I8" s="60" t="s">
+      <c r="I8" s="47" t="s">
         <v>26</v>
       </c>
-      <c r="J8" s="72" t="s">
+      <c r="J8" s="59" t="s">
         <v>56</v>
       </c>
-      <c r="K8" s="60" t="s">
+      <c r="K8" s="47" t="s">
         <v>28</v>
       </c>
       <c r="L8" s="3"/>
@@ -2109,17 +2217,17 @@
       <c r="AA8" s="2"/>
     </row>
     <row r="9" spans="1:27">
-      <c r="A9" s="53"/>
-      <c r="B9" s="47"/>
-      <c r="C9" s="47"/>
-      <c r="D9" s="47"/>
-      <c r="E9" s="47"/>
-      <c r="F9" s="48"/>
-      <c r="G9" s="48"/>
-      <c r="H9" s="71"/>
-      <c r="I9" s="61"/>
-      <c r="J9" s="73"/>
-      <c r="K9" s="61"/>
+      <c r="A9" s="88"/>
+      <c r="B9" s="57"/>
+      <c r="C9" s="57"/>
+      <c r="D9" s="57"/>
+      <c r="E9" s="57"/>
+      <c r="F9" s="58"/>
+      <c r="G9" s="58"/>
+      <c r="H9" s="81"/>
+      <c r="I9" s="48"/>
+      <c r="J9" s="60"/>
+      <c r="K9" s="48"/>
       <c r="L9" s="3"/>
       <c r="M9" s="2"/>
       <c r="N9" s="2"/>
@@ -2138,17 +2246,17 @@
       <c r="AA9" s="2"/>
     </row>
     <row r="10" spans="1:27" s="29" customFormat="1" ht="15.75" customHeight="1">
-      <c r="A10" s="53"/>
-      <c r="B10" s="47"/>
-      <c r="C10" s="47"/>
-      <c r="D10" s="47"/>
-      <c r="E10" s="47"/>
+      <c r="A10" s="88"/>
+      <c r="B10" s="57"/>
+      <c r="C10" s="57"/>
+      <c r="D10" s="57"/>
+      <c r="E10" s="57"/>
       <c r="F10" s="30"/>
       <c r="G10" s="35"/>
       <c r="H10" s="35"/>
-      <c r="I10" s="61"/>
-      <c r="J10" s="73"/>
-      <c r="K10" s="61"/>
+      <c r="I10" s="48"/>
+      <c r="J10" s="60"/>
+      <c r="K10" s="48"/>
       <c r="L10" s="27"/>
       <c r="M10" s="28"/>
       <c r="N10" s="28"/>
@@ -2167,17 +2275,17 @@
       <c r="AA10" s="28"/>
     </row>
     <row r="11" spans="1:27">
-      <c r="A11" s="54"/>
-      <c r="B11" s="48"/>
-      <c r="C11" s="48"/>
-      <c r="D11" s="48"/>
-      <c r="E11" s="48"/>
+      <c r="A11" s="89"/>
+      <c r="B11" s="58"/>
+      <c r="C11" s="58"/>
+      <c r="D11" s="58"/>
+      <c r="E11" s="58"/>
       <c r="F11" s="30"/>
       <c r="G11" s="35"/>
       <c r="H11" s="35"/>
-      <c r="I11" s="62"/>
-      <c r="J11" s="74"/>
-      <c r="K11" s="62"/>
+      <c r="I11" s="49"/>
+      <c r="J11" s="61"/>
+      <c r="K11" s="49"/>
       <c r="L11" s="3"/>
       <c r="M11" s="2"/>
       <c r="N11" s="2"/>
@@ -2196,37 +2304,37 @@
       <c r="AA11" s="2"/>
     </row>
     <row r="12" spans="1:27">
-      <c r="A12" s="52" t="s">
+      <c r="A12" s="87" t="s">
         <v>31</v>
       </c>
-      <c r="B12" s="46" t="s">
+      <c r="B12" s="56" t="s">
         <v>49</v>
       </c>
-      <c r="C12" s="46" t="s">
+      <c r="C12" s="56" t="s">
         <v>60</v>
       </c>
-      <c r="D12" s="46" t="s">
+      <c r="D12" s="56" t="s">
         <v>61</v>
       </c>
-      <c r="E12" s="46" t="s">
+      <c r="E12" s="56" t="s">
         <v>62</v>
       </c>
-      <c r="F12" s="46" t="s">
+      <c r="F12" s="56" t="s">
         <v>53</v>
       </c>
-      <c r="G12" s="46" t="s">
+      <c r="G12" s="56" t="s">
         <v>54</v>
       </c>
-      <c r="H12" s="70" t="s">
+      <c r="H12" s="80" t="s">
         <v>55</v>
       </c>
-      <c r="I12" s="60" t="s">
+      <c r="I12" s="47" t="s">
         <v>26</v>
       </c>
-      <c r="J12" s="72" t="s">
+      <c r="J12" s="59" t="s">
         <v>56</v>
       </c>
-      <c r="K12" s="60" t="s">
+      <c r="K12" s="47" t="s">
         <v>28</v>
       </c>
       <c r="L12" s="2"/>
@@ -2247,17 +2355,17 @@
       <c r="AA12" s="2"/>
     </row>
     <row r="13" spans="1:27">
-      <c r="A13" s="53"/>
-      <c r="B13" s="47"/>
-      <c r="C13" s="47"/>
-      <c r="D13" s="47"/>
-      <c r="E13" s="47"/>
-      <c r="F13" s="48"/>
-      <c r="G13" s="48"/>
-      <c r="H13" s="71"/>
-      <c r="I13" s="61"/>
-      <c r="J13" s="73"/>
-      <c r="K13" s="61"/>
+      <c r="A13" s="88"/>
+      <c r="B13" s="57"/>
+      <c r="C13" s="57"/>
+      <c r="D13" s="57"/>
+      <c r="E13" s="57"/>
+      <c r="F13" s="58"/>
+      <c r="G13" s="58"/>
+      <c r="H13" s="81"/>
+      <c r="I13" s="48"/>
+      <c r="J13" s="60"/>
+      <c r="K13" s="48"/>
       <c r="L13" s="2"/>
       <c r="M13" s="2"/>
       <c r="N13" s="2"/>
@@ -2276,17 +2384,17 @@
       <c r="AA13" s="2"/>
     </row>
     <row r="14" spans="1:27" s="29" customFormat="1">
-      <c r="A14" s="53"/>
-      <c r="B14" s="47"/>
-      <c r="C14" s="47"/>
-      <c r="D14" s="47"/>
-      <c r="E14" s="47"/>
+      <c r="A14" s="88"/>
+      <c r="B14" s="57"/>
+      <c r="C14" s="57"/>
+      <c r="D14" s="57"/>
+      <c r="E14" s="57"/>
       <c r="F14" s="30"/>
       <c r="G14" s="35"/>
       <c r="H14" s="35"/>
-      <c r="I14" s="61"/>
-      <c r="J14" s="73"/>
-      <c r="K14" s="61"/>
+      <c r="I14" s="48"/>
+      <c r="J14" s="60"/>
+      <c r="K14" s="48"/>
       <c r="L14" s="28"/>
       <c r="M14" s="28"/>
       <c r="N14" s="28"/>
@@ -2305,17 +2413,17 @@
       <c r="AA14" s="28"/>
     </row>
     <row r="15" spans="1:27">
-      <c r="A15" s="54"/>
-      <c r="B15" s="48"/>
-      <c r="C15" s="48"/>
-      <c r="D15" s="48"/>
-      <c r="E15" s="48"/>
+      <c r="A15" s="89"/>
+      <c r="B15" s="58"/>
+      <c r="C15" s="58"/>
+      <c r="D15" s="58"/>
+      <c r="E15" s="58"/>
       <c r="F15" s="30"/>
       <c r="G15" s="35"/>
       <c r="H15" s="35"/>
-      <c r="I15" s="62"/>
-      <c r="J15" s="74"/>
-      <c r="K15" s="62"/>
+      <c r="I15" s="49"/>
+      <c r="J15" s="61"/>
+      <c r="K15" s="49"/>
       <c r="L15" s="2"/>
       <c r="M15" s="2"/>
       <c r="N15" s="2"/>
@@ -2334,19 +2442,19 @@
       <c r="AA15" s="2"/>
     </row>
     <row r="16" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A16" s="55" t="s">
+      <c r="A16" s="90" t="s">
         <v>32</v>
       </c>
-      <c r="B16" s="46" t="s">
+      <c r="B16" s="56" t="s">
         <v>63</v>
       </c>
-      <c r="C16" s="46" t="s">
+      <c r="C16" s="56" t="s">
         <v>64</v>
       </c>
-      <c r="D16" s="46" t="s">
+      <c r="D16" s="56" t="s">
         <v>65</v>
       </c>
-      <c r="E16" s="46" t="s">
+      <c r="E16" s="56" t="s">
         <v>83</v>
       </c>
       <c r="F16" s="30" t="s">
@@ -2358,13 +2466,13 @@
       <c r="H16" s="35" t="s">
         <v>66</v>
       </c>
-      <c r="I16" s="60" t="s">
+      <c r="I16" s="47" t="s">
         <v>26</v>
       </c>
-      <c r="J16" s="72" t="s">
+      <c r="J16" s="59" t="s">
         <v>56</v>
       </c>
-      <c r="K16" s="60" t="s">
+      <c r="K16" s="47" t="s">
         <v>28</v>
       </c>
       <c r="L16" s="2"/>
@@ -2385,11 +2493,11 @@
       <c r="AA16" s="2"/>
     </row>
     <row r="17" spans="1:27" ht="16.5" customHeight="1">
-      <c r="A17" s="56"/>
-      <c r="B17" s="47"/>
-      <c r="C17" s="47"/>
-      <c r="D17" s="47"/>
-      <c r="E17" s="47"/>
+      <c r="A17" s="91"/>
+      <c r="B17" s="57"/>
+      <c r="C17" s="57"/>
+      <c r="D17" s="57"/>
+      <c r="E17" s="57"/>
       <c r="F17" s="30" t="s">
         <v>67</v>
       </c>
@@ -2399,9 +2507,9 @@
       <c r="H17" s="35" t="s">
         <v>69</v>
       </c>
-      <c r="I17" s="61"/>
-      <c r="J17" s="73"/>
-      <c r="K17" s="61"/>
+      <c r="I17" s="48"/>
+      <c r="J17" s="60"/>
+      <c r="K17" s="48"/>
       <c r="L17" s="2"/>
       <c r="M17" s="2"/>
       <c r="N17" s="2"/>
@@ -2420,11 +2528,11 @@
       <c r="AA17" s="2"/>
     </row>
     <row r="18" spans="1:27" s="29" customFormat="1" ht="25.5">
-      <c r="A18" s="56"/>
-      <c r="B18" s="47"/>
-      <c r="C18" s="47"/>
-      <c r="D18" s="47"/>
-      <c r="E18" s="47"/>
+      <c r="A18" s="91"/>
+      <c r="B18" s="57"/>
+      <c r="C18" s="57"/>
+      <c r="D18" s="57"/>
+      <c r="E18" s="57"/>
       <c r="F18" s="30" t="s">
         <v>70</v>
       </c>
@@ -2434,9 +2542,9 @@
       <c r="H18" s="35" t="s">
         <v>72</v>
       </c>
-      <c r="I18" s="61"/>
-      <c r="J18" s="73"/>
-      <c r="K18" s="61"/>
+      <c r="I18" s="48"/>
+      <c r="J18" s="60"/>
+      <c r="K18" s="48"/>
       <c r="L18" s="28"/>
       <c r="M18" s="28"/>
       <c r="N18" s="28"/>
@@ -2455,17 +2563,17 @@
       <c r="AA18" s="28"/>
     </row>
     <row r="19" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A19" s="57"/>
-      <c r="B19" s="48"/>
-      <c r="C19" s="48"/>
-      <c r="D19" s="48"/>
-      <c r="E19" s="48"/>
+      <c r="A19" s="92"/>
+      <c r="B19" s="58"/>
+      <c r="C19" s="58"/>
+      <c r="D19" s="58"/>
+      <c r="E19" s="58"/>
       <c r="F19" s="30"/>
       <c r="G19" s="35"/>
       <c r="H19" s="35"/>
-      <c r="I19" s="62"/>
-      <c r="J19" s="74"/>
-      <c r="K19" s="62"/>
+      <c r="I19" s="49"/>
+      <c r="J19" s="61"/>
+      <c r="K19" s="49"/>
       <c r="L19" s="2"/>
       <c r="M19" s="2"/>
       <c r="N19" s="2"/>
@@ -2484,19 +2592,19 @@
       <c r="AA19" s="2"/>
     </row>
     <row r="20" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A20" s="55" t="s">
+      <c r="A20" s="90" t="s">
         <v>33</v>
       </c>
-      <c r="B20" s="46" t="s">
+      <c r="B20" s="56" t="s">
         <v>63</v>
       </c>
-      <c r="C20" s="49" t="s">
+      <c r="C20" s="62" t="s">
         <v>73</v>
       </c>
-      <c r="D20" s="46" t="s">
+      <c r="D20" s="56" t="s">
         <v>74</v>
       </c>
-      <c r="E20" s="46" t="s">
+      <c r="E20" s="56" t="s">
         <v>75</v>
       </c>
       <c r="F20" s="30" t="s">
@@ -2508,13 +2616,13 @@
       <c r="H20" s="35" t="s">
         <v>76</v>
       </c>
-      <c r="I20" s="60" t="s">
+      <c r="I20" s="47" t="s">
         <v>26</v>
       </c>
-      <c r="J20" s="72" t="s">
+      <c r="J20" s="59" t="s">
         <v>56</v>
       </c>
-      <c r="K20" s="60" t="s">
+      <c r="K20" s="47" t="s">
         <v>28</v>
       </c>
       <c r="L20" s="2"/>
@@ -2535,11 +2643,11 @@
       <c r="AA20" s="2"/>
     </row>
     <row r="21" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A21" s="56"/>
-      <c r="B21" s="47"/>
-      <c r="C21" s="50"/>
-      <c r="D21" s="47"/>
-      <c r="E21" s="47"/>
+      <c r="A21" s="91"/>
+      <c r="B21" s="57"/>
+      <c r="C21" s="74"/>
+      <c r="D21" s="57"/>
+      <c r="E21" s="57"/>
       <c r="F21" s="30" t="s">
         <v>67</v>
       </c>
@@ -2547,9 +2655,9 @@
         <v>77</v>
       </c>
       <c r="H21" s="35"/>
-      <c r="I21" s="61"/>
-      <c r="J21" s="73"/>
-      <c r="K21" s="61"/>
+      <c r="I21" s="48"/>
+      <c r="J21" s="60"/>
+      <c r="K21" s="48"/>
       <c r="L21" s="2"/>
       <c r="M21" s="2"/>
       <c r="N21" s="2"/>
@@ -2568,11 +2676,11 @@
       <c r="AA21" s="2"/>
     </row>
     <row r="22" spans="1:27" s="29" customFormat="1" ht="15.75" customHeight="1">
-      <c r="A22" s="56"/>
-      <c r="B22" s="47"/>
-      <c r="C22" s="50"/>
-      <c r="D22" s="47"/>
-      <c r="E22" s="47"/>
+      <c r="A22" s="91"/>
+      <c r="B22" s="57"/>
+      <c r="C22" s="74"/>
+      <c r="D22" s="57"/>
+      <c r="E22" s="57"/>
       <c r="F22" s="30" t="s">
         <v>70</v>
       </c>
@@ -2582,9 +2690,9 @@
       <c r="H22" s="35" t="s">
         <v>79</v>
       </c>
-      <c r="I22" s="61"/>
-      <c r="J22" s="73"/>
-      <c r="K22" s="61"/>
+      <c r="I22" s="48"/>
+      <c r="J22" s="60"/>
+      <c r="K22" s="48"/>
       <c r="L22" s="28"/>
       <c r="M22" s="28"/>
       <c r="N22" s="28"/>
@@ -2603,17 +2711,17 @@
       <c r="AA22" s="28"/>
     </row>
     <row r="23" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A23" s="57"/>
-      <c r="B23" s="48"/>
-      <c r="C23" s="51"/>
-      <c r="D23" s="48"/>
-      <c r="E23" s="48"/>
+      <c r="A23" s="92"/>
+      <c r="B23" s="58"/>
+      <c r="C23" s="75"/>
+      <c r="D23" s="58"/>
+      <c r="E23" s="58"/>
       <c r="F23" s="30"/>
       <c r="G23" s="35"/>
       <c r="H23" s="35"/>
-      <c r="I23" s="62"/>
-      <c r="J23" s="74"/>
-      <c r="K23" s="62"/>
+      <c r="I23" s="49"/>
+      <c r="J23" s="61"/>
+      <c r="K23" s="49"/>
       <c r="L23" s="2"/>
       <c r="M23" s="2"/>
       <c r="N23" s="2"/>
@@ -2632,19 +2740,19 @@
       <c r="AA23" s="2"/>
     </row>
     <row r="24" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A24" s="55" t="s">
+      <c r="A24" s="90" t="s">
         <v>34</v>
       </c>
-      <c r="B24" s="46" t="s">
+      <c r="B24" s="56" t="s">
         <v>63</v>
       </c>
-      <c r="C24" s="49" t="s">
+      <c r="C24" s="62" t="s">
         <v>80</v>
       </c>
-      <c r="D24" s="46" t="s">
+      <c r="D24" s="56" t="s">
         <v>81</v>
       </c>
-      <c r="E24" s="46" t="s">
+      <c r="E24" s="56" t="s">
         <v>75</v>
       </c>
       <c r="F24" s="30" t="s">
@@ -2656,13 +2764,13 @@
       <c r="H24" s="35" t="s">
         <v>76</v>
       </c>
-      <c r="I24" s="60" t="s">
+      <c r="I24" s="47" t="s">
         <v>26</v>
       </c>
-      <c r="J24" s="72" t="s">
+      <c r="J24" s="59" t="s">
         <v>56</v>
       </c>
-      <c r="K24" s="60" t="s">
+      <c r="K24" s="47" t="s">
         <v>28</v>
       </c>
       <c r="L24" s="2"/>
@@ -2683,11 +2791,11 @@
       <c r="AA24" s="2"/>
     </row>
     <row r="25" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A25" s="56"/>
-      <c r="B25" s="47"/>
-      <c r="C25" s="50"/>
-      <c r="D25" s="47"/>
-      <c r="E25" s="47"/>
+      <c r="A25" s="91"/>
+      <c r="B25" s="57"/>
+      <c r="C25" s="74"/>
+      <c r="D25" s="57"/>
+      <c r="E25" s="57"/>
       <c r="F25" s="30" t="s">
         <v>67</v>
       </c>
@@ -2695,9 +2803,9 @@
         <v>77</v>
       </c>
       <c r="H25" s="35"/>
-      <c r="I25" s="61"/>
-      <c r="J25" s="73"/>
-      <c r="K25" s="61"/>
+      <c r="I25" s="48"/>
+      <c r="J25" s="60"/>
+      <c r="K25" s="48"/>
       <c r="L25" s="2"/>
       <c r="M25" s="2"/>
       <c r="N25" s="2"/>
@@ -2716,11 +2824,11 @@
       <c r="AA25" s="2"/>
     </row>
     <row r="26" spans="1:27" s="29" customFormat="1" ht="25.5">
-      <c r="A26" s="56"/>
-      <c r="B26" s="47"/>
-      <c r="C26" s="50"/>
-      <c r="D26" s="47"/>
-      <c r="E26" s="47"/>
+      <c r="A26" s="91"/>
+      <c r="B26" s="57"/>
+      <c r="C26" s="74"/>
+      <c r="D26" s="57"/>
+      <c r="E26" s="57"/>
       <c r="F26" s="30" t="s">
         <v>70</v>
       </c>
@@ -2730,9 +2838,9 @@
       <c r="H26" s="35" t="s">
         <v>82</v>
       </c>
-      <c r="I26" s="61"/>
-      <c r="J26" s="73"/>
-      <c r="K26" s="61"/>
+      <c r="I26" s="48"/>
+      <c r="J26" s="60"/>
+      <c r="K26" s="48"/>
       <c r="L26" s="28"/>
       <c r="M26" s="28"/>
       <c r="N26" s="28"/>
@@ -2751,17 +2859,17 @@
       <c r="AA26" s="28"/>
     </row>
     <row r="27" spans="1:27" ht="18.75" customHeight="1">
-      <c r="A27" s="57"/>
-      <c r="B27" s="48"/>
-      <c r="C27" s="51"/>
-      <c r="D27" s="48"/>
-      <c r="E27" s="48"/>
+      <c r="A27" s="92"/>
+      <c r="B27" s="58"/>
+      <c r="C27" s="75"/>
+      <c r="D27" s="58"/>
+      <c r="E27" s="58"/>
       <c r="F27" s="30"/>
       <c r="G27" s="35"/>
       <c r="H27" s="35"/>
-      <c r="I27" s="62"/>
-      <c r="J27" s="74"/>
-      <c r="K27" s="62"/>
+      <c r="I27" s="49"/>
+      <c r="J27" s="61"/>
+      <c r="K27" s="49"/>
       <c r="L27" s="2"/>
       <c r="M27" s="2"/>
       <c r="N27" s="2"/>
@@ -2780,19 +2888,19 @@
       <c r="AA27" s="2"/>
     </row>
     <row r="28" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A28" s="75" t="s">
+      <c r="A28" s="68" t="s">
         <v>35</v>
       </c>
-      <c r="B28" s="46" t="s">
+      <c r="B28" s="56" t="s">
         <v>84</v>
       </c>
-      <c r="C28" s="46" t="s">
+      <c r="C28" s="56" t="s">
         <v>85</v>
       </c>
-      <c r="D28" s="46" t="s">
+      <c r="D28" s="56" t="s">
         <v>86</v>
       </c>
-      <c r="E28" s="46" t="s">
+      <c r="E28" s="56" t="s">
         <v>83</v>
       </c>
       <c r="F28" s="30" t="s">
@@ -2804,13 +2912,13 @@
       <c r="H28" s="35" t="s">
         <v>88</v>
       </c>
-      <c r="I28" s="60" t="s">
+      <c r="I28" s="47" t="s">
         <v>26</v>
       </c>
-      <c r="J28" s="72" t="s">
+      <c r="J28" s="59" t="s">
         <v>56</v>
       </c>
-      <c r="K28" s="60" t="s">
+      <c r="K28" s="47" t="s">
         <v>28</v>
       </c>
       <c r="L28" s="2"/>
@@ -2831,19 +2939,19 @@
       <c r="AA28" s="2"/>
     </row>
     <row r="29" spans="1:27">
-      <c r="A29" s="76"/>
-      <c r="B29" s="47"/>
-      <c r="C29" s="47"/>
-      <c r="D29" s="47"/>
-      <c r="E29" s="47"/>
+      <c r="A29" s="69"/>
+      <c r="B29" s="57"/>
+      <c r="C29" s="57"/>
+      <c r="D29" s="57"/>
+      <c r="E29" s="57"/>
       <c r="F29" s="30" t="s">
         <v>67</v>
       </c>
       <c r="G29" s="35"/>
       <c r="H29" s="35"/>
-      <c r="I29" s="61"/>
-      <c r="J29" s="73"/>
-      <c r="K29" s="61"/>
+      <c r="I29" s="48"/>
+      <c r="J29" s="60"/>
+      <c r="K29" s="48"/>
       <c r="L29" s="2"/>
       <c r="M29" s="2"/>
       <c r="N29" s="2"/>
@@ -2862,17 +2970,17 @@
       <c r="AA29" s="2"/>
     </row>
     <row r="30" spans="1:27" s="29" customFormat="1" ht="15.75" customHeight="1">
-      <c r="A30" s="76"/>
-      <c r="B30" s="47"/>
-      <c r="C30" s="47"/>
-      <c r="D30" s="47"/>
-      <c r="E30" s="47"/>
+      <c r="A30" s="69"/>
+      <c r="B30" s="57"/>
+      <c r="C30" s="57"/>
+      <c r="D30" s="57"/>
+      <c r="E30" s="57"/>
       <c r="F30" s="30"/>
       <c r="G30" s="35"/>
       <c r="H30" s="35"/>
-      <c r="I30" s="61"/>
-      <c r="J30" s="73"/>
-      <c r="K30" s="61"/>
+      <c r="I30" s="48"/>
+      <c r="J30" s="60"/>
+      <c r="K30" s="48"/>
       <c r="L30" s="28"/>
       <c r="M30" s="28"/>
       <c r="N30" s="28"/>
@@ -2891,17 +2999,17 @@
       <c r="AA30" s="28"/>
     </row>
     <row r="31" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A31" s="77"/>
-      <c r="B31" s="48"/>
-      <c r="C31" s="48"/>
-      <c r="D31" s="48"/>
-      <c r="E31" s="48"/>
+      <c r="A31" s="70"/>
+      <c r="B31" s="58"/>
+      <c r="C31" s="58"/>
+      <c r="D31" s="58"/>
+      <c r="E31" s="58"/>
       <c r="F31" s="30"/>
       <c r="G31" s="35"/>
       <c r="H31" s="35"/>
-      <c r="I31" s="62"/>
-      <c r="J31" s="74"/>
-      <c r="K31" s="62"/>
+      <c r="I31" s="49"/>
+      <c r="J31" s="61"/>
+      <c r="K31" s="49"/>
       <c r="L31" s="2"/>
       <c r="M31" s="2"/>
       <c r="N31" s="2"/>
@@ -2920,19 +3028,19 @@
       <c r="AA31" s="2"/>
     </row>
     <row r="32" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A32" s="75" t="s">
+      <c r="A32" s="68" t="s">
         <v>36</v>
       </c>
-      <c r="B32" s="46" t="s">
+      <c r="B32" s="56" t="s">
         <v>84</v>
       </c>
-      <c r="C32" s="46" t="s">
+      <c r="C32" s="56" t="s">
         <v>89</v>
       </c>
-      <c r="D32" s="46" t="s">
+      <c r="D32" s="56" t="s">
         <v>90</v>
       </c>
-      <c r="E32" s="46" t="s">
+      <c r="E32" s="56" t="s">
         <v>83</v>
       </c>
       <c r="F32" s="30" t="s">
@@ -2944,13 +3052,13 @@
       <c r="H32" s="35" t="s">
         <v>92</v>
       </c>
-      <c r="I32" s="60" t="s">
+      <c r="I32" s="47" t="s">
         <v>26</v>
       </c>
-      <c r="J32" s="72" t="s">
+      <c r="J32" s="59" t="s">
         <v>56</v>
       </c>
-      <c r="K32" s="60" t="s">
+      <c r="K32" s="47" t="s">
         <v>28</v>
       </c>
       <c r="L32" s="2"/>
@@ -2971,17 +3079,17 @@
       <c r="AA32" s="2"/>
     </row>
     <row r="33" spans="1:27">
-      <c r="A33" s="76"/>
-      <c r="B33" s="47"/>
-      <c r="C33" s="47"/>
-      <c r="D33" s="47"/>
-      <c r="E33" s="47"/>
+      <c r="A33" s="69"/>
+      <c r="B33" s="57"/>
+      <c r="C33" s="57"/>
+      <c r="D33" s="57"/>
+      <c r="E33" s="57"/>
       <c r="F33" s="30"/>
       <c r="G33" s="43"/>
       <c r="H33" s="43"/>
-      <c r="I33" s="61"/>
-      <c r="J33" s="73"/>
-      <c r="K33" s="61"/>
+      <c r="I33" s="48"/>
+      <c r="J33" s="60"/>
+      <c r="K33" s="48"/>
       <c r="L33" s="2"/>
       <c r="M33" s="2"/>
       <c r="N33" s="2"/>
@@ -3000,17 +3108,17 @@
       <c r="AA33" s="2"/>
     </row>
     <row r="34" spans="1:27">
-      <c r="A34" s="76"/>
-      <c r="B34" s="47"/>
-      <c r="C34" s="47"/>
-      <c r="D34" s="47"/>
-      <c r="E34" s="47"/>
+      <c r="A34" s="69"/>
+      <c r="B34" s="57"/>
+      <c r="C34" s="57"/>
+      <c r="D34" s="57"/>
+      <c r="E34" s="57"/>
       <c r="F34" s="30"/>
       <c r="G34" s="43"/>
       <c r="H34" s="43"/>
-      <c r="I34" s="61"/>
-      <c r="J34" s="73"/>
-      <c r="K34" s="61"/>
+      <c r="I34" s="48"/>
+      <c r="J34" s="60"/>
+      <c r="K34" s="48"/>
       <c r="L34" s="2"/>
       <c r="M34" s="2"/>
       <c r="N34" s="2"/>
@@ -3029,17 +3137,17 @@
       <c r="AA34" s="2"/>
     </row>
     <row r="35" spans="1:27">
-      <c r="A35" s="77"/>
-      <c r="B35" s="48"/>
-      <c r="C35" s="48"/>
-      <c r="D35" s="48"/>
-      <c r="E35" s="48"/>
+      <c r="A35" s="70"/>
+      <c r="B35" s="58"/>
+      <c r="C35" s="58"/>
+      <c r="D35" s="58"/>
+      <c r="E35" s="58"/>
       <c r="F35" s="30"/>
       <c r="G35" s="35"/>
       <c r="H35" s="35"/>
-      <c r="I35" s="62"/>
-      <c r="J35" s="74"/>
-      <c r="K35" s="62"/>
+      <c r="I35" s="49"/>
+      <c r="J35" s="61"/>
+      <c r="K35" s="49"/>
       <c r="L35" s="2"/>
       <c r="M35" s="2"/>
       <c r="N35" s="2"/>
@@ -3058,19 +3166,19 @@
       <c r="AA35" s="2"/>
     </row>
     <row r="36" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A36" s="75" t="s">
+      <c r="A36" s="68" t="s">
         <v>37</v>
       </c>
-      <c r="B36" s="46" t="s">
+      <c r="B36" s="56" t="s">
         <v>84</v>
       </c>
-      <c r="C36" s="46" t="s">
+      <c r="C36" s="56" t="s">
         <v>93</v>
       </c>
-      <c r="D36" s="46" t="s">
+      <c r="D36" s="56" t="s">
         <v>94</v>
       </c>
-      <c r="E36" s="46" t="s">
+      <c r="E36" s="56" t="s">
         <v>95</v>
       </c>
       <c r="F36" s="30" t="s">
@@ -3082,13 +3190,13 @@
       <c r="H36" s="35" t="s">
         <v>92</v>
       </c>
-      <c r="I36" s="60" t="s">
+      <c r="I36" s="47" t="s">
         <v>26</v>
       </c>
-      <c r="J36" s="72" t="s">
+      <c r="J36" s="59" t="s">
         <v>56</v>
       </c>
-      <c r="K36" s="60" t="s">
+      <c r="K36" s="47" t="s">
         <v>28</v>
       </c>
       <c r="L36" s="2"/>
@@ -3109,11 +3217,11 @@
       <c r="AA36" s="2"/>
     </row>
     <row r="37" spans="1:27" ht="25.5">
-      <c r="A37" s="76"/>
-      <c r="B37" s="47"/>
-      <c r="C37" s="47"/>
-      <c r="D37" s="47"/>
-      <c r="E37" s="47"/>
+      <c r="A37" s="69"/>
+      <c r="B37" s="57"/>
+      <c r="C37" s="57"/>
+      <c r="D37" s="57"/>
+      <c r="E37" s="57"/>
       <c r="F37" s="30" t="s">
         <v>67</v>
       </c>
@@ -3121,9 +3229,9 @@
         <v>96</v>
       </c>
       <c r="H37" s="35"/>
-      <c r="I37" s="61"/>
-      <c r="J37" s="73"/>
-      <c r="K37" s="61"/>
+      <c r="I37" s="48"/>
+      <c r="J37" s="60"/>
+      <c r="K37" s="48"/>
       <c r="L37" s="2"/>
       <c r="M37" s="2"/>
       <c r="N37" s="2"/>
@@ -3142,11 +3250,11 @@
       <c r="AA37" s="2"/>
     </row>
     <row r="38" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A38" s="76"/>
-      <c r="B38" s="47"/>
-      <c r="C38" s="47"/>
-      <c r="D38" s="47"/>
-      <c r="E38" s="47"/>
+      <c r="A38" s="69"/>
+      <c r="B38" s="57"/>
+      <c r="C38" s="57"/>
+      <c r="D38" s="57"/>
+      <c r="E38" s="57"/>
       <c r="F38" s="30" t="s">
         <v>70</v>
       </c>
@@ -3156,9 +3264,9 @@
       <c r="H38" s="35" t="s">
         <v>98</v>
       </c>
-      <c r="I38" s="61"/>
-      <c r="J38" s="73"/>
-      <c r="K38" s="61"/>
+      <c r="I38" s="48"/>
+      <c r="J38" s="60"/>
+      <c r="K38" s="48"/>
       <c r="L38" s="2"/>
       <c r="M38" s="2"/>
       <c r="N38" s="2"/>
@@ -3177,19 +3285,19 @@
       <c r="AA38" s="2"/>
     </row>
     <row r="39" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A39" s="77"/>
-      <c r="B39" s="48"/>
-      <c r="C39" s="48"/>
-      <c r="D39" s="48"/>
-      <c r="E39" s="48"/>
+      <c r="A39" s="70"/>
+      <c r="B39" s="58"/>
+      <c r="C39" s="58"/>
+      <c r="D39" s="58"/>
+      <c r="E39" s="58"/>
       <c r="F39" s="30" t="s">
         <v>99</v>
       </c>
       <c r="G39" s="35"/>
       <c r="H39" s="35"/>
-      <c r="I39" s="62"/>
-      <c r="J39" s="74"/>
-      <c r="K39" s="62"/>
+      <c r="I39" s="49"/>
+      <c r="J39" s="61"/>
+      <c r="K39" s="49"/>
       <c r="L39" s="2"/>
       <c r="M39" s="2"/>
       <c r="N39" s="2"/>
@@ -3208,19 +3316,19 @@
       <c r="AA39" s="2"/>
     </row>
     <row r="40" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A40" s="75" t="s">
+      <c r="A40" s="68" t="s">
         <v>38</v>
       </c>
-      <c r="B40" s="46" t="s">
+      <c r="B40" s="56" t="s">
         <v>84</v>
       </c>
-      <c r="C40" s="46" t="s">
+      <c r="C40" s="56" t="s">
         <v>100</v>
       </c>
-      <c r="D40" s="46" t="s">
+      <c r="D40" s="56" t="s">
         <v>101</v>
       </c>
-      <c r="E40" s="46" t="s">
+      <c r="E40" s="56" t="s">
         <v>102</v>
       </c>
       <c r="F40" s="30" t="s">
@@ -3232,13 +3340,13 @@
       <c r="H40" s="35" t="s">
         <v>88</v>
       </c>
-      <c r="I40" s="60" t="s">
+      <c r="I40" s="47" t="s">
         <v>26</v>
       </c>
-      <c r="J40" s="72" t="s">
+      <c r="J40" s="59" t="s">
         <v>56</v>
       </c>
-      <c r="K40" s="60" t="s">
+      <c r="K40" s="47" t="s">
         <v>28</v>
       </c>
       <c r="L40" s="2"/>
@@ -3259,11 +3367,11 @@
       <c r="AA40" s="2"/>
     </row>
     <row r="41" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A41" s="76"/>
-      <c r="B41" s="47"/>
-      <c r="C41" s="47"/>
-      <c r="D41" s="47"/>
-      <c r="E41" s="47"/>
+      <c r="A41" s="69"/>
+      <c r="B41" s="57"/>
+      <c r="C41" s="57"/>
+      <c r="D41" s="57"/>
+      <c r="E41" s="57"/>
       <c r="F41" s="30" t="s">
         <v>67</v>
       </c>
@@ -3271,9 +3379,9 @@
         <v>103</v>
       </c>
       <c r="H41" s="35"/>
-      <c r="I41" s="61"/>
-      <c r="J41" s="73"/>
-      <c r="K41" s="61"/>
+      <c r="I41" s="48"/>
+      <c r="J41" s="60"/>
+      <c r="K41" s="48"/>
       <c r="L41" s="2"/>
       <c r="M41" s="2"/>
       <c r="N41" s="2"/>
@@ -3292,11 +3400,11 @@
       <c r="AA41" s="2"/>
     </row>
     <row r="42" spans="1:27" ht="16.5" customHeight="1">
-      <c r="A42" s="76"/>
-      <c r="B42" s="47"/>
-      <c r="C42" s="47"/>
-      <c r="D42" s="47"/>
-      <c r="E42" s="47"/>
+      <c r="A42" s="69"/>
+      <c r="B42" s="57"/>
+      <c r="C42" s="57"/>
+      <c r="D42" s="57"/>
+      <c r="E42" s="57"/>
       <c r="F42" s="30" t="s">
         <v>70</v>
       </c>
@@ -3306,9 +3414,9 @@
       <c r="H42" s="35" t="s">
         <v>105</v>
       </c>
-      <c r="I42" s="61"/>
-      <c r="J42" s="73"/>
-      <c r="K42" s="61"/>
+      <c r="I42" s="48"/>
+      <c r="J42" s="60"/>
+      <c r="K42" s="48"/>
       <c r="L42" s="2"/>
       <c r="M42" s="2"/>
       <c r="N42" s="2"/>
@@ -3327,19 +3435,19 @@
       <c r="AA42" s="2"/>
     </row>
     <row r="43" spans="1:27" ht="18.75" customHeight="1">
-      <c r="A43" s="77"/>
-      <c r="B43" s="48"/>
-      <c r="C43" s="48"/>
-      <c r="D43" s="48"/>
-      <c r="E43" s="48"/>
+      <c r="A43" s="70"/>
+      <c r="B43" s="58"/>
+      <c r="C43" s="58"/>
+      <c r="D43" s="58"/>
+      <c r="E43" s="58"/>
       <c r="F43" s="30" t="s">
         <v>99</v>
       </c>
       <c r="G43" s="35"/>
       <c r="H43" s="35"/>
-      <c r="I43" s="62"/>
-      <c r="J43" s="74"/>
-      <c r="K43" s="62"/>
+      <c r="I43" s="49"/>
+      <c r="J43" s="61"/>
+      <c r="K43" s="49"/>
       <c r="L43" s="2"/>
       <c r="M43" s="2"/>
       <c r="N43" s="2"/>
@@ -3358,19 +3466,19 @@
       <c r="AA43" s="2"/>
     </row>
     <row r="44" spans="1:27" ht="25.5">
-      <c r="A44" s="75" t="s">
+      <c r="A44" s="68" t="s">
         <v>39</v>
       </c>
-      <c r="B44" s="46" t="s">
+      <c r="B44" s="56" t="s">
         <v>84</v>
       </c>
-      <c r="C44" s="46" t="s">
+      <c r="C44" s="56" t="s">
         <v>106</v>
       </c>
-      <c r="D44" s="46" t="s">
+      <c r="D44" s="56" t="s">
         <v>107</v>
       </c>
-      <c r="E44" s="46" t="s">
+      <c r="E44" s="56" t="s">
         <v>108</v>
       </c>
       <c r="F44" s="30" t="s">
@@ -3382,13 +3490,13 @@
       <c r="H44" s="35" t="s">
         <v>88</v>
       </c>
-      <c r="I44" s="60" t="s">
+      <c r="I44" s="47" t="s">
         <v>26</v>
       </c>
-      <c r="J44" s="72" t="s">
+      <c r="J44" s="59" t="s">
         <v>56</v>
       </c>
-      <c r="K44" s="60" t="s">
+      <c r="K44" s="47" t="s">
         <v>28</v>
       </c>
       <c r="L44" s="2"/>
@@ -3409,11 +3517,11 @@
       <c r="AA44" s="2"/>
     </row>
     <row r="45" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A45" s="76"/>
-      <c r="B45" s="47"/>
-      <c r="C45" s="47"/>
-      <c r="D45" s="47"/>
-      <c r="E45" s="47"/>
+      <c r="A45" s="69"/>
+      <c r="B45" s="57"/>
+      <c r="C45" s="57"/>
+      <c r="D45" s="57"/>
+      <c r="E45" s="57"/>
       <c r="F45" s="30" t="s">
         <v>67</v>
       </c>
@@ -3421,9 +3529,9 @@
         <v>109</v>
       </c>
       <c r="H45" s="35"/>
-      <c r="I45" s="61"/>
-      <c r="J45" s="73"/>
-      <c r="K45" s="61"/>
+      <c r="I45" s="48"/>
+      <c r="J45" s="60"/>
+      <c r="K45" s="48"/>
       <c r="L45" s="2"/>
       <c r="M45" s="2"/>
       <c r="N45" s="2"/>
@@ -3442,11 +3550,11 @@
       <c r="AA45" s="2"/>
     </row>
     <row r="46" spans="1:27" ht="25.5">
-      <c r="A46" s="76"/>
-      <c r="B46" s="47"/>
-      <c r="C46" s="47"/>
-      <c r="D46" s="47"/>
-      <c r="E46" s="47"/>
+      <c r="A46" s="69"/>
+      <c r="B46" s="57"/>
+      <c r="C46" s="57"/>
+      <c r="D46" s="57"/>
+      <c r="E46" s="57"/>
       <c r="F46" s="30" t="s">
         <v>70</v>
       </c>
@@ -3456,9 +3564,9 @@
       <c r="H46" s="35" t="s">
         <v>110</v>
       </c>
-      <c r="I46" s="61"/>
-      <c r="J46" s="73"/>
-      <c r="K46" s="61"/>
+      <c r="I46" s="48"/>
+      <c r="J46" s="60"/>
+      <c r="K46" s="48"/>
       <c r="L46" s="2"/>
       <c r="M46" s="2"/>
       <c r="N46" s="2"/>
@@ -3477,19 +3585,19 @@
       <c r="AA46" s="2"/>
     </row>
     <row r="47" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A47" s="77"/>
-      <c r="B47" s="48"/>
-      <c r="C47" s="48"/>
-      <c r="D47" s="48"/>
-      <c r="E47" s="48"/>
+      <c r="A47" s="70"/>
+      <c r="B47" s="58"/>
+      <c r="C47" s="58"/>
+      <c r="D47" s="58"/>
+      <c r="E47" s="58"/>
       <c r="F47" s="30" t="s">
         <v>99</v>
       </c>
       <c r="G47" s="35"/>
       <c r="H47" s="36"/>
-      <c r="I47" s="62"/>
-      <c r="J47" s="74"/>
-      <c r="K47" s="62"/>
+      <c r="I47" s="49"/>
+      <c r="J47" s="61"/>
+      <c r="K47" s="49"/>
       <c r="L47" s="2"/>
       <c r="M47" s="2"/>
       <c r="N47" s="2"/>
@@ -3508,19 +3616,19 @@
       <c r="AA47" s="2"/>
     </row>
     <row r="48" spans="1:27" ht="25.5">
-      <c r="A48" s="75" t="s">
+      <c r="A48" s="68" t="s">
         <v>40</v>
       </c>
-      <c r="B48" s="46" t="s">
+      <c r="B48" s="56" t="s">
         <v>84</v>
       </c>
-      <c r="C48" s="46" t="s">
+      <c r="C48" s="56" t="s">
         <v>111</v>
       </c>
-      <c r="D48" s="46" t="s">
+      <c r="D48" s="56" t="s">
         <v>112</v>
       </c>
-      <c r="E48" s="46" t="s">
+      <c r="E48" s="56" t="s">
         <v>102</v>
       </c>
       <c r="F48" s="30" t="s">
@@ -3532,13 +3640,13 @@
       <c r="H48" s="35" t="s">
         <v>88</v>
       </c>
-      <c r="I48" s="60" t="s">
+      <c r="I48" s="47" t="s">
         <v>26</v>
       </c>
-      <c r="J48" s="72" t="s">
+      <c r="J48" s="59" t="s">
         <v>56</v>
       </c>
-      <c r="K48" s="60" t="s">
+      <c r="K48" s="47" t="s">
         <v>28</v>
       </c>
       <c r="L48" s="2"/>
@@ -3559,11 +3667,11 @@
       <c r="AA48" s="2"/>
     </row>
     <row r="49" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A49" s="76"/>
-      <c r="B49" s="47"/>
-      <c r="C49" s="47"/>
-      <c r="D49" s="47"/>
-      <c r="E49" s="47"/>
+      <c r="A49" s="69"/>
+      <c r="B49" s="57"/>
+      <c r="C49" s="57"/>
+      <c r="D49" s="57"/>
+      <c r="E49" s="57"/>
       <c r="F49" s="30" t="s">
         <v>67</v>
       </c>
@@ -3571,9 +3679,9 @@
         <v>113</v>
       </c>
       <c r="H49" s="35"/>
-      <c r="I49" s="61"/>
-      <c r="J49" s="73"/>
-      <c r="K49" s="61"/>
+      <c r="I49" s="48"/>
+      <c r="J49" s="60"/>
+      <c r="K49" s="48"/>
       <c r="L49" s="2"/>
       <c r="M49" s="2"/>
       <c r="N49" s="2"/>
@@ -3592,11 +3700,11 @@
       <c r="AA49" s="2"/>
     </row>
     <row r="50" spans="1:27" ht="27" customHeight="1">
-      <c r="A50" s="76"/>
-      <c r="B50" s="47"/>
-      <c r="C50" s="47"/>
-      <c r="D50" s="47"/>
-      <c r="E50" s="47"/>
+      <c r="A50" s="69"/>
+      <c r="B50" s="57"/>
+      <c r="C50" s="57"/>
+      <c r="D50" s="57"/>
+      <c r="E50" s="57"/>
       <c r="F50" s="30" t="s">
         <v>70</v>
       </c>
@@ -3606,9 +3714,9 @@
       <c r="H50" s="35" t="s">
         <v>110</v>
       </c>
-      <c r="I50" s="61"/>
-      <c r="J50" s="73"/>
-      <c r="K50" s="61"/>
+      <c r="I50" s="48"/>
+      <c r="J50" s="60"/>
+      <c r="K50" s="48"/>
       <c r="L50" s="2"/>
       <c r="M50" s="2"/>
       <c r="N50" s="2"/>
@@ -3627,19 +3735,19 @@
       <c r="AA50" s="2"/>
     </row>
     <row r="51" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A51" s="77"/>
-      <c r="B51" s="48"/>
-      <c r="C51" s="48"/>
-      <c r="D51" s="48"/>
-      <c r="E51" s="48"/>
+      <c r="A51" s="70"/>
+      <c r="B51" s="58"/>
+      <c r="C51" s="58"/>
+      <c r="D51" s="58"/>
+      <c r="E51" s="58"/>
       <c r="F51" s="30" t="s">
         <v>99</v>
       </c>
       <c r="G51" s="35"/>
       <c r="H51" s="36"/>
-      <c r="I51" s="62"/>
-      <c r="J51" s="74"/>
-      <c r="K51" s="62"/>
+      <c r="I51" s="49"/>
+      <c r="J51" s="61"/>
+      <c r="K51" s="49"/>
       <c r="L51" s="2"/>
       <c r="M51" s="2"/>
       <c r="N51" s="2"/>
@@ -3658,19 +3766,19 @@
       <c r="AA51" s="2"/>
     </row>
     <row r="52" spans="1:27" ht="25.5">
-      <c r="A52" s="75" t="s">
+      <c r="A52" s="68" t="s">
         <v>41</v>
       </c>
-      <c r="B52" s="46" t="s">
+      <c r="B52" s="56" t="s">
         <v>84</v>
       </c>
-      <c r="C52" s="46" t="s">
+      <c r="C52" s="56" t="s">
         <v>114</v>
       </c>
-      <c r="D52" s="46" t="s">
+      <c r="D52" s="56" t="s">
         <v>129</v>
       </c>
-      <c r="E52" s="46" t="s">
+      <c r="E52" s="56" t="s">
         <v>95</v>
       </c>
       <c r="F52" s="30" t="s">
@@ -3682,13 +3790,13 @@
       <c r="H52" s="35" t="s">
         <v>92</v>
       </c>
-      <c r="I52" s="60" t="s">
+      <c r="I52" s="47" t="s">
         <v>26</v>
       </c>
-      <c r="J52" s="72" t="s">
+      <c r="J52" s="59" t="s">
         <v>56</v>
       </c>
-      <c r="K52" s="60" t="s">
+      <c r="K52" s="47" t="s">
         <v>28</v>
       </c>
       <c r="L52" s="2"/>
@@ -3709,11 +3817,11 @@
       <c r="AA52" s="2"/>
     </row>
     <row r="53" spans="1:27" ht="25.5">
-      <c r="A53" s="76"/>
-      <c r="B53" s="47"/>
-      <c r="C53" s="47"/>
-      <c r="D53" s="47"/>
-      <c r="E53" s="47"/>
+      <c r="A53" s="69"/>
+      <c r="B53" s="57"/>
+      <c r="C53" s="57"/>
+      <c r="D53" s="57"/>
+      <c r="E53" s="57"/>
       <c r="F53" s="30" t="s">
         <v>67</v>
       </c>
@@ -3723,9 +3831,9 @@
       <c r="H53" s="36" t="s">
         <v>116</v>
       </c>
-      <c r="I53" s="61"/>
-      <c r="J53" s="73"/>
-      <c r="K53" s="61"/>
+      <c r="I53" s="48"/>
+      <c r="J53" s="60"/>
+      <c r="K53" s="48"/>
       <c r="L53" s="2"/>
       <c r="M53" s="2"/>
       <c r="N53" s="2"/>
@@ -3744,17 +3852,17 @@
       <c r="AA53" s="2"/>
     </row>
     <row r="54" spans="1:27" ht="13.5" customHeight="1">
-      <c r="A54" s="76"/>
-      <c r="B54" s="47"/>
-      <c r="C54" s="47"/>
-      <c r="D54" s="47"/>
-      <c r="E54" s="47"/>
+      <c r="A54" s="69"/>
+      <c r="B54" s="57"/>
+      <c r="C54" s="57"/>
+      <c r="D54" s="57"/>
+      <c r="E54" s="57"/>
       <c r="F54" s="30"/>
       <c r="G54" s="43"/>
       <c r="H54" s="43"/>
-      <c r="I54" s="61"/>
-      <c r="J54" s="73"/>
-      <c r="K54" s="61"/>
+      <c r="I54" s="48"/>
+      <c r="J54" s="60"/>
+      <c r="K54" s="48"/>
       <c r="L54" s="2"/>
       <c r="M54" s="2"/>
       <c r="N54" s="2"/>
@@ -3773,17 +3881,17 @@
       <c r="AA54" s="2"/>
     </row>
     <row r="55" spans="1:27" ht="15" customHeight="1">
-      <c r="A55" s="77"/>
-      <c r="B55" s="48"/>
-      <c r="C55" s="48"/>
-      <c r="D55" s="48"/>
-      <c r="E55" s="48"/>
+      <c r="A55" s="70"/>
+      <c r="B55" s="58"/>
+      <c r="C55" s="58"/>
+      <c r="D55" s="58"/>
+      <c r="E55" s="58"/>
       <c r="F55" s="30"/>
       <c r="G55" s="43"/>
       <c r="H55" s="43"/>
-      <c r="I55" s="62"/>
-      <c r="J55" s="74"/>
-      <c r="K55" s="62"/>
+      <c r="I55" s="49"/>
+      <c r="J55" s="61"/>
+      <c r="K55" s="49"/>
       <c r="L55" s="2"/>
       <c r="M55" s="2"/>
       <c r="N55" s="2"/>
@@ -3802,19 +3910,19 @@
       <c r="AA55" s="2"/>
     </row>
     <row r="56" spans="1:27" ht="25.5">
-      <c r="A56" s="75" t="s">
+      <c r="A56" s="68" t="s">
         <v>42</v>
       </c>
-      <c r="B56" s="46" t="s">
+      <c r="B56" s="56" t="s">
         <v>84</v>
       </c>
-      <c r="C56" s="46" t="s">
+      <c r="C56" s="56" t="s">
         <v>117</v>
       </c>
-      <c r="D56" s="46" t="s">
+      <c r="D56" s="56" t="s">
         <v>118</v>
       </c>
-      <c r="E56" s="46" t="s">
+      <c r="E56" s="56" t="s">
         <v>95</v>
       </c>
       <c r="F56" s="30" t="s">
@@ -3826,13 +3934,13 @@
       <c r="H56" s="35" t="s">
         <v>92</v>
       </c>
-      <c r="I56" s="60" t="s">
+      <c r="I56" s="47" t="s">
         <v>26</v>
       </c>
-      <c r="J56" s="72" t="s">
+      <c r="J56" s="59" t="s">
         <v>56</v>
       </c>
-      <c r="K56" s="60" t="s">
+      <c r="K56" s="47" t="s">
         <v>28</v>
       </c>
       <c r="L56" s="2"/>
@@ -3853,11 +3961,11 @@
       <c r="AA56" s="2"/>
     </row>
     <row r="57" spans="1:27" ht="17.25" customHeight="1">
-      <c r="A57" s="76"/>
-      <c r="B57" s="47"/>
-      <c r="C57" s="47"/>
-      <c r="D57" s="47"/>
-      <c r="E57" s="47"/>
+      <c r="A57" s="69"/>
+      <c r="B57" s="57"/>
+      <c r="C57" s="57"/>
+      <c r="D57" s="57"/>
+      <c r="E57" s="57"/>
       <c r="F57" s="30" t="s">
         <v>67</v>
       </c>
@@ -3867,9 +3975,9 @@
       <c r="H57" s="36" t="s">
         <v>120</v>
       </c>
-      <c r="I57" s="61"/>
-      <c r="J57" s="73"/>
-      <c r="K57" s="61"/>
+      <c r="I57" s="48"/>
+      <c r="J57" s="60"/>
+      <c r="K57" s="48"/>
       <c r="L57" s="2"/>
       <c r="M57" s="2"/>
       <c r="N57" s="2"/>
@@ -3888,11 +3996,11 @@
       <c r="AA57" s="2"/>
     </row>
     <row r="58" spans="1:27" ht="25.5">
-      <c r="A58" s="76"/>
-      <c r="B58" s="47"/>
-      <c r="C58" s="47"/>
-      <c r="D58" s="47"/>
-      <c r="E58" s="47"/>
+      <c r="A58" s="69"/>
+      <c r="B58" s="57"/>
+      <c r="C58" s="57"/>
+      <c r="D58" s="57"/>
+      <c r="E58" s="57"/>
       <c r="F58" s="30" t="s">
         <v>70</v>
       </c>
@@ -3902,9 +4010,9 @@
       <c r="H58" s="36" t="s">
         <v>122</v>
       </c>
-      <c r="I58" s="61"/>
-      <c r="J58" s="73"/>
-      <c r="K58" s="61"/>
+      <c r="I58" s="48"/>
+      <c r="J58" s="60"/>
+      <c r="K58" s="48"/>
       <c r="L58" s="2"/>
       <c r="M58" s="2"/>
       <c r="N58" s="2"/>
@@ -3923,11 +4031,11 @@
       <c r="AA58" s="2"/>
     </row>
     <row r="59" spans="1:27" ht="25.5">
-      <c r="A59" s="77"/>
-      <c r="B59" s="48"/>
-      <c r="C59" s="48"/>
-      <c r="D59" s="48"/>
-      <c r="E59" s="48"/>
+      <c r="A59" s="70"/>
+      <c r="B59" s="58"/>
+      <c r="C59" s="58"/>
+      <c r="D59" s="58"/>
+      <c r="E59" s="58"/>
       <c r="F59" s="30" t="s">
         <v>99</v>
       </c>
@@ -3937,9 +4045,9 @@
       <c r="H59" s="36" t="s">
         <v>123</v>
       </c>
-      <c r="I59" s="62"/>
-      <c r="J59" s="74"/>
-      <c r="K59" s="62"/>
+      <c r="I59" s="49"/>
+      <c r="J59" s="61"/>
+      <c r="K59" s="49"/>
       <c r="L59" s="2"/>
       <c r="M59" s="2"/>
       <c r="N59" s="2"/>
@@ -3958,19 +4066,19 @@
       <c r="AA59" s="2"/>
     </row>
     <row r="60" spans="1:27" ht="25.5">
-      <c r="A60" s="75" t="s">
+      <c r="A60" s="68" t="s">
         <v>43</v>
       </c>
-      <c r="B60" s="46" t="s">
+      <c r="B60" s="56" t="s">
         <v>84</v>
       </c>
-      <c r="C60" s="46" t="s">
+      <c r="C60" s="56" t="s">
         <v>124</v>
       </c>
-      <c r="D60" s="46" t="s">
+      <c r="D60" s="56" t="s">
         <v>125</v>
       </c>
-      <c r="E60" s="46" t="s">
+      <c r="E60" s="56" t="s">
         <v>102</v>
       </c>
       <c r="F60" s="30" t="s">
@@ -3982,13 +4090,13 @@
       <c r="H60" s="35" t="s">
         <v>92</v>
       </c>
-      <c r="I60" s="60" t="s">
+      <c r="I60" s="47" t="s">
         <v>26</v>
       </c>
-      <c r="J60" s="72" t="s">
+      <c r="J60" s="59" t="s">
         <v>56</v>
       </c>
-      <c r="K60" s="60" t="s">
+      <c r="K60" s="47" t="s">
         <v>28</v>
       </c>
       <c r="L60" s="2"/>
@@ -4009,11 +4117,11 @@
       <c r="AA60" s="2"/>
     </row>
     <row r="61" spans="1:27" ht="25.5">
-      <c r="A61" s="76"/>
-      <c r="B61" s="47"/>
-      <c r="C61" s="47"/>
-      <c r="D61" s="47"/>
-      <c r="E61" s="47"/>
+      <c r="A61" s="69"/>
+      <c r="B61" s="57"/>
+      <c r="C61" s="57"/>
+      <c r="D61" s="57"/>
+      <c r="E61" s="57"/>
       <c r="F61" s="30" t="s">
         <v>67</v>
       </c>
@@ -4023,9 +4131,9 @@
       <c r="H61" s="36" t="s">
         <v>120</v>
       </c>
-      <c r="I61" s="61"/>
-      <c r="J61" s="73"/>
-      <c r="K61" s="61"/>
+      <c r="I61" s="48"/>
+      <c r="J61" s="60"/>
+      <c r="K61" s="48"/>
       <c r="L61" s="2"/>
       <c r="M61" s="2"/>
       <c r="N61" s="2"/>
@@ -4044,11 +4152,11 @@
       <c r="AA61" s="2"/>
     </row>
     <row r="62" spans="1:27" ht="25.5">
-      <c r="A62" s="76"/>
-      <c r="B62" s="47"/>
-      <c r="C62" s="47"/>
-      <c r="D62" s="47"/>
-      <c r="E62" s="47"/>
+      <c r="A62" s="69"/>
+      <c r="B62" s="57"/>
+      <c r="C62" s="57"/>
+      <c r="D62" s="57"/>
+      <c r="E62" s="57"/>
       <c r="F62" s="30" t="s">
         <v>70</v>
       </c>
@@ -4058,9 +4166,9 @@
       <c r="H62" s="36" t="s">
         <v>122</v>
       </c>
-      <c r="I62" s="61"/>
-      <c r="J62" s="73"/>
-      <c r="K62" s="61"/>
+      <c r="I62" s="48"/>
+      <c r="J62" s="60"/>
+      <c r="K62" s="48"/>
       <c r="L62" s="2"/>
       <c r="M62" s="2"/>
       <c r="N62" s="2"/>
@@ -4079,11 +4187,11 @@
       <c r="AA62" s="2"/>
     </row>
     <row r="63" spans="1:27" ht="25.5">
-      <c r="A63" s="77"/>
-      <c r="B63" s="48"/>
-      <c r="C63" s="48"/>
-      <c r="D63" s="48"/>
-      <c r="E63" s="48"/>
+      <c r="A63" s="70"/>
+      <c r="B63" s="58"/>
+      <c r="C63" s="58"/>
+      <c r="D63" s="58"/>
+      <c r="E63" s="58"/>
       <c r="F63" s="30" t="s">
         <v>99</v>
       </c>
@@ -4093,9 +4201,9 @@
       <c r="H63" s="35" t="s">
         <v>128</v>
       </c>
-      <c r="I63" s="62"/>
-      <c r="J63" s="74"/>
-      <c r="K63" s="62"/>
+      <c r="I63" s="49"/>
+      <c r="J63" s="61"/>
+      <c r="K63" s="49"/>
       <c r="L63" s="2"/>
       <c r="M63" s="2"/>
       <c r="N63" s="2"/>
@@ -4114,19 +4222,19 @@
       <c r="AA63" s="2"/>
     </row>
     <row r="64" spans="1:27" ht="25.5">
-      <c r="A64" s="83" t="s">
+      <c r="A64" s="71" t="s">
         <v>44</v>
       </c>
-      <c r="B64" s="46" t="s">
+      <c r="B64" s="56" t="s">
         <v>49</v>
       </c>
-      <c r="C64" s="49" t="s">
+      <c r="C64" s="62" t="s">
         <v>130</v>
       </c>
-      <c r="D64" s="46" t="s">
+      <c r="D64" s="56" t="s">
         <v>131</v>
       </c>
-      <c r="E64" s="46" t="s">
+      <c r="E64" s="56" t="s">
         <v>83</v>
       </c>
       <c r="F64" s="30" t="s">
@@ -4138,13 +4246,13 @@
       <c r="H64" s="35" t="s">
         <v>133</v>
       </c>
-      <c r="I64" s="60" t="s">
+      <c r="I64" s="47" t="s">
         <v>26</v>
       </c>
-      <c r="J64" s="72" t="s">
+      <c r="J64" s="59" t="s">
         <v>56</v>
       </c>
-      <c r="K64" s="60" t="s">
+      <c r="K64" s="47" t="s">
         <v>28</v>
       </c>
       <c r="L64" s="2"/>
@@ -4165,17 +4273,17 @@
       <c r="AA64" s="2"/>
     </row>
     <row r="65" spans="1:27">
-      <c r="A65" s="84"/>
-      <c r="B65" s="47"/>
-      <c r="C65" s="50"/>
-      <c r="D65" s="47"/>
-      <c r="E65" s="47"/>
+      <c r="A65" s="72"/>
+      <c r="B65" s="57"/>
+      <c r="C65" s="74"/>
+      <c r="D65" s="57"/>
+      <c r="E65" s="57"/>
       <c r="F65" s="30"/>
       <c r="G65" s="35"/>
       <c r="H65" s="35"/>
-      <c r="I65" s="61"/>
-      <c r="J65" s="73"/>
-      <c r="K65" s="61"/>
+      <c r="I65" s="48"/>
+      <c r="J65" s="60"/>
+      <c r="K65" s="48"/>
       <c r="L65" s="2"/>
       <c r="M65" s="2"/>
       <c r="N65" s="2"/>
@@ -4194,17 +4302,17 @@
       <c r="AA65" s="2"/>
     </row>
     <row r="66" spans="1:27">
-      <c r="A66" s="84"/>
-      <c r="B66" s="47"/>
-      <c r="C66" s="50"/>
-      <c r="D66" s="47"/>
-      <c r="E66" s="47"/>
+      <c r="A66" s="72"/>
+      <c r="B66" s="57"/>
+      <c r="C66" s="74"/>
+      <c r="D66" s="57"/>
+      <c r="E66" s="57"/>
       <c r="F66" s="30"/>
       <c r="G66" s="35"/>
       <c r="H66" s="35"/>
-      <c r="I66" s="61"/>
-      <c r="J66" s="73"/>
-      <c r="K66" s="61"/>
+      <c r="I66" s="48"/>
+      <c r="J66" s="60"/>
+      <c r="K66" s="48"/>
       <c r="L66" s="2"/>
       <c r="M66" s="2"/>
       <c r="N66" s="2"/>
@@ -4223,17 +4331,17 @@
       <c r="AA66" s="2"/>
     </row>
     <row r="67" spans="1:27">
-      <c r="A67" s="85"/>
-      <c r="B67" s="48"/>
-      <c r="C67" s="51"/>
-      <c r="D67" s="48"/>
-      <c r="E67" s="48"/>
+      <c r="A67" s="73"/>
+      <c r="B67" s="58"/>
+      <c r="C67" s="75"/>
+      <c r="D67" s="58"/>
+      <c r="E67" s="58"/>
       <c r="F67" s="30"/>
       <c r="G67" s="35"/>
       <c r="H67" s="35"/>
-      <c r="I67" s="62"/>
-      <c r="J67" s="74"/>
-      <c r="K67" s="62"/>
+      <c r="I67" s="49"/>
+      <c r="J67" s="61"/>
+      <c r="K67" s="49"/>
       <c r="L67" s="2"/>
       <c r="M67" s="2"/>
       <c r="N67" s="2"/>
@@ -4252,19 +4360,19 @@
       <c r="AA67" s="2"/>
     </row>
     <row r="68" spans="1:27" ht="25.5">
-      <c r="A68" s="83" t="s">
+      <c r="A68" s="71" t="s">
         <v>45</v>
       </c>
-      <c r="B68" s="46" t="s">
+      <c r="B68" s="56" t="s">
         <v>49</v>
       </c>
-      <c r="C68" s="49" t="s">
+      <c r="C68" s="62" t="s">
         <v>134</v>
       </c>
-      <c r="D68" s="46" t="s">
+      <c r="D68" s="56" t="s">
         <v>135</v>
       </c>
-      <c r="E68" s="46" t="s">
+      <c r="E68" s="56" t="s">
         <v>83</v>
       </c>
       <c r="F68" s="30" t="s">
@@ -4276,13 +4384,13 @@
       <c r="H68" s="35" t="s">
         <v>137</v>
       </c>
-      <c r="I68" s="60" t="s">
+      <c r="I68" s="47" t="s">
         <v>26</v>
       </c>
-      <c r="J68" s="72" t="s">
+      <c r="J68" s="59" t="s">
         <v>56</v>
       </c>
-      <c r="K68" s="60" t="s">
+      <c r="K68" s="47" t="s">
         <v>28</v>
       </c>
       <c r="L68" s="2"/>
@@ -4303,17 +4411,17 @@
       <c r="AA68" s="2"/>
     </row>
     <row r="69" spans="1:27">
-      <c r="A69" s="84"/>
-      <c r="B69" s="47"/>
-      <c r="C69" s="50"/>
-      <c r="D69" s="47"/>
-      <c r="E69" s="47"/>
+      <c r="A69" s="72"/>
+      <c r="B69" s="57"/>
+      <c r="C69" s="74"/>
+      <c r="D69" s="57"/>
+      <c r="E69" s="57"/>
       <c r="F69" s="30"/>
       <c r="G69" s="35"/>
       <c r="H69" s="35"/>
-      <c r="I69" s="61"/>
-      <c r="J69" s="73"/>
-      <c r="K69" s="61"/>
+      <c r="I69" s="48"/>
+      <c r="J69" s="60"/>
+      <c r="K69" s="48"/>
       <c r="L69" s="2"/>
       <c r="M69" s="2"/>
       <c r="N69" s="2"/>
@@ -4332,17 +4440,17 @@
       <c r="AA69" s="2"/>
     </row>
     <row r="70" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A70" s="84"/>
-      <c r="B70" s="47"/>
-      <c r="C70" s="50"/>
-      <c r="D70" s="47"/>
-      <c r="E70" s="47"/>
+      <c r="A70" s="72"/>
+      <c r="B70" s="57"/>
+      <c r="C70" s="74"/>
+      <c r="D70" s="57"/>
+      <c r="E70" s="57"/>
       <c r="F70" s="30"/>
       <c r="G70" s="35"/>
       <c r="H70" s="35"/>
-      <c r="I70" s="61"/>
-      <c r="J70" s="73"/>
-      <c r="K70" s="61"/>
+      <c r="I70" s="48"/>
+      <c r="J70" s="60"/>
+      <c r="K70" s="48"/>
       <c r="L70" s="2"/>
       <c r="M70" s="2"/>
       <c r="N70" s="2"/>
@@ -4361,17 +4469,17 @@
       <c r="AA70" s="2"/>
     </row>
     <row r="71" spans="1:27">
-      <c r="A71" s="85"/>
-      <c r="B71" s="48"/>
-      <c r="C71" s="51"/>
-      <c r="D71" s="48"/>
-      <c r="E71" s="48"/>
+      <c r="A71" s="73"/>
+      <c r="B71" s="58"/>
+      <c r="C71" s="75"/>
+      <c r="D71" s="58"/>
+      <c r="E71" s="58"/>
       <c r="F71" s="30"/>
       <c r="G71" s="35"/>
       <c r="H71" s="35"/>
-      <c r="I71" s="62"/>
-      <c r="J71" s="74"/>
-      <c r="K71" s="62"/>
+      <c r="I71" s="49"/>
+      <c r="J71" s="61"/>
+      <c r="K71" s="49"/>
       <c r="L71" s="2"/>
       <c r="M71" s="2"/>
       <c r="N71" s="2"/>
@@ -4390,19 +4498,19 @@
       <c r="AA71" s="2"/>
     </row>
     <row r="72" spans="1:27">
-      <c r="A72" s="78" t="s">
+      <c r="A72" s="65" t="s">
         <v>46</v>
       </c>
-      <c r="B72" s="49" t="s">
+      <c r="B72" s="62" t="s">
         <v>138</v>
       </c>
-      <c r="C72" s="49" t="s">
+      <c r="C72" s="62" t="s">
         <v>139</v>
       </c>
-      <c r="D72" s="49" t="s">
+      <c r="D72" s="62" t="s">
         <v>140</v>
       </c>
-      <c r="E72" s="49" t="s">
+      <c r="E72" s="62" t="s">
         <v>141</v>
       </c>
       <c r="F72" s="44" t="s">
@@ -4414,13 +4522,13 @@
       <c r="H72" s="45" t="s">
         <v>143</v>
       </c>
-      <c r="I72" s="60" t="s">
+      <c r="I72" s="47" t="s">
         <v>26</v>
       </c>
-      <c r="J72" s="72" t="s">
+      <c r="J72" s="59" t="s">
         <v>56</v>
       </c>
-      <c r="K72" s="60" t="s">
+      <c r="K72" s="47" t="s">
         <v>28</v>
       </c>
       <c r="L72" s="2"/>
@@ -4441,11 +4549,11 @@
       <c r="AA72" s="2"/>
     </row>
     <row r="73" spans="1:27">
-      <c r="A73" s="79"/>
-      <c r="B73" s="81"/>
-      <c r="C73" s="81"/>
-      <c r="D73" s="81"/>
-      <c r="E73" s="81"/>
+      <c r="A73" s="66"/>
+      <c r="B73" s="63"/>
+      <c r="C73" s="63"/>
+      <c r="D73" s="63"/>
+      <c r="E73" s="63"/>
       <c r="F73" s="44" t="s">
         <v>67</v>
       </c>
@@ -4453,9 +4561,9 @@
         <v>144</v>
       </c>
       <c r="H73" s="45"/>
-      <c r="I73" s="61"/>
-      <c r="J73" s="73"/>
-      <c r="K73" s="61"/>
+      <c r="I73" s="48"/>
+      <c r="J73" s="60"/>
+      <c r="K73" s="48"/>
       <c r="L73" s="2"/>
       <c r="M73" s="2"/>
       <c r="N73" s="2"/>
@@ -4474,11 +4582,11 @@
       <c r="AA73" s="2"/>
     </row>
     <row r="74" spans="1:27">
-      <c r="A74" s="79"/>
-      <c r="B74" s="81"/>
-      <c r="C74" s="81"/>
-      <c r="D74" s="81"/>
-      <c r="E74" s="81"/>
+      <c r="A74" s="66"/>
+      <c r="B74" s="63"/>
+      <c r="C74" s="63"/>
+      <c r="D74" s="63"/>
+      <c r="E74" s="63"/>
       <c r="F74" s="44" t="s">
         <v>70</v>
       </c>
@@ -4488,9 +4596,9 @@
       <c r="H74" s="45" t="s">
         <v>146</v>
       </c>
-      <c r="I74" s="61"/>
-      <c r="J74" s="73"/>
-      <c r="K74" s="61"/>
+      <c r="I74" s="48"/>
+      <c r="J74" s="60"/>
+      <c r="K74" s="48"/>
       <c r="L74" s="2"/>
       <c r="M74" s="2"/>
       <c r="N74" s="2"/>
@@ -4509,11 +4617,11 @@
       <c r="AA74" s="2"/>
     </row>
     <row r="75" spans="1:27">
-      <c r="A75" s="80"/>
-      <c r="B75" s="82"/>
-      <c r="C75" s="82"/>
-      <c r="D75" s="82"/>
-      <c r="E75" s="82"/>
+      <c r="A75" s="67"/>
+      <c r="B75" s="64"/>
+      <c r="C75" s="64"/>
+      <c r="D75" s="64"/>
+      <c r="E75" s="64"/>
       <c r="F75" s="44" t="s">
         <v>99</v>
       </c>
@@ -4523,9 +4631,9 @@
       <c r="H75" s="45" t="s">
         <v>163</v>
       </c>
-      <c r="I75" s="62"/>
-      <c r="J75" s="74"/>
-      <c r="K75" s="62"/>
+      <c r="I75" s="49"/>
+      <c r="J75" s="61"/>
+      <c r="K75" s="49"/>
       <c r="L75" s="2"/>
       <c r="M75" s="2"/>
       <c r="N75" s="2"/>
@@ -4544,19 +4652,19 @@
       <c r="AA75" s="2"/>
     </row>
     <row r="76" spans="1:27">
-      <c r="A76" s="78" t="s">
+      <c r="A76" s="65" t="s">
         <v>47</v>
       </c>
-      <c r="B76" s="49" t="s">
+      <c r="B76" s="62" t="s">
         <v>138</v>
       </c>
-      <c r="C76" s="49" t="s">
+      <c r="C76" s="62" t="s">
         <v>148</v>
       </c>
-      <c r="D76" s="49" t="s">
+      <c r="D76" s="62" t="s">
         <v>149</v>
       </c>
-      <c r="E76" s="49" t="s">
+      <c r="E76" s="62" t="s">
         <v>141</v>
       </c>
       <c r="F76" s="44" t="s">
@@ -4568,13 +4676,13 @@
       <c r="H76" s="45" t="s">
         <v>143</v>
       </c>
-      <c r="I76" s="60" t="s">
+      <c r="I76" s="47" t="s">
         <v>26</v>
       </c>
-      <c r="J76" s="72" t="s">
+      <c r="J76" s="59" t="s">
         <v>56</v>
       </c>
-      <c r="K76" s="60" t="s">
+      <c r="K76" s="47" t="s">
         <v>28</v>
       </c>
       <c r="L76" s="2"/>
@@ -4595,11 +4703,11 @@
       <c r="AA76" s="2"/>
     </row>
     <row r="77" spans="1:27">
-      <c r="A77" s="79"/>
-      <c r="B77" s="81"/>
-      <c r="C77" s="81"/>
-      <c r="D77" s="81"/>
-      <c r="E77" s="81"/>
+      <c r="A77" s="66"/>
+      <c r="B77" s="63"/>
+      <c r="C77" s="63"/>
+      <c r="D77" s="63"/>
+      <c r="E77" s="63"/>
       <c r="F77" s="44" t="s">
         <v>67</v>
       </c>
@@ -4609,9 +4717,9 @@
       <c r="H77" s="45" t="s">
         <v>146</v>
       </c>
-      <c r="I77" s="61"/>
-      <c r="J77" s="73"/>
-      <c r="K77" s="61"/>
+      <c r="I77" s="48"/>
+      <c r="J77" s="60"/>
+      <c r="K77" s="48"/>
       <c r="L77" s="2"/>
       <c r="M77" s="2"/>
       <c r="N77" s="2"/>
@@ -4630,11 +4738,11 @@
       <c r="AA77" s="2"/>
     </row>
     <row r="78" spans="1:27">
-      <c r="A78" s="79"/>
-      <c r="B78" s="81"/>
-      <c r="C78" s="81"/>
-      <c r="D78" s="81"/>
-      <c r="E78" s="81"/>
+      <c r="A78" s="66"/>
+      <c r="B78" s="63"/>
+      <c r="C78" s="63"/>
+      <c r="D78" s="63"/>
+      <c r="E78" s="63"/>
       <c r="F78" s="44" t="s">
         <v>70</v>
       </c>
@@ -4644,9 +4752,9 @@
       <c r="H78" s="45" t="s">
         <v>151</v>
       </c>
-      <c r="I78" s="61"/>
-      <c r="J78" s="73"/>
-      <c r="K78" s="61"/>
+      <c r="I78" s="48"/>
+      <c r="J78" s="60"/>
+      <c r="K78" s="48"/>
       <c r="L78" s="2"/>
       <c r="M78" s="2"/>
       <c r="N78" s="2"/>
@@ -4665,19 +4773,19 @@
       <c r="AA78" s="2"/>
     </row>
     <row r="79" spans="1:27">
-      <c r="A79" s="80"/>
-      <c r="B79" s="82"/>
-      <c r="C79" s="82"/>
-      <c r="D79" s="82"/>
-      <c r="E79" s="82"/>
+      <c r="A79" s="67"/>
+      <c r="B79" s="64"/>
+      <c r="C79" s="64"/>
+      <c r="D79" s="64"/>
+      <c r="E79" s="64"/>
       <c r="F79" s="44" t="s">
         <v>99</v>
       </c>
       <c r="G79" s="45"/>
       <c r="H79" s="45"/>
-      <c r="I79" s="62"/>
-      <c r="J79" s="74"/>
-      <c r="K79" s="62"/>
+      <c r="I79" s="49"/>
+      <c r="J79" s="61"/>
+      <c r="K79" s="49"/>
       <c r="L79" s="2"/>
       <c r="M79" s="2"/>
       <c r="N79" s="2"/>
@@ -4696,19 +4804,19 @@
       <c r="AA79" s="2"/>
     </row>
     <row r="80" spans="1:27">
-      <c r="A80" s="78" t="s">
+      <c r="A80" s="65" t="s">
         <v>48</v>
       </c>
-      <c r="B80" s="49" t="s">
+      <c r="B80" s="62" t="s">
         <v>138</v>
       </c>
-      <c r="C80" s="49" t="s">
+      <c r="C80" s="62" t="s">
         <v>152</v>
       </c>
-      <c r="D80" s="49" t="s">
+      <c r="D80" s="62" t="s">
         <v>153</v>
       </c>
-      <c r="E80" s="49" t="s">
+      <c r="E80" s="62" t="s">
         <v>141</v>
       </c>
       <c r="F80" s="44" t="s">
@@ -4720,13 +4828,13 @@
       <c r="H80" s="45" t="s">
         <v>143</v>
       </c>
-      <c r="I80" s="60" t="s">
+      <c r="I80" s="47" t="s">
         <v>26</v>
       </c>
-      <c r="J80" s="72" t="s">
+      <c r="J80" s="59" t="s">
         <v>56</v>
       </c>
-      <c r="K80" s="60" t="s">
+      <c r="K80" s="47" t="s">
         <v>28</v>
       </c>
       <c r="L80" s="2"/>
@@ -4747,11 +4855,11 @@
       <c r="AA80" s="2"/>
     </row>
     <row r="81" spans="1:27">
-      <c r="A81" s="79"/>
-      <c r="B81" s="81"/>
-      <c r="C81" s="81"/>
-      <c r="D81" s="81"/>
-      <c r="E81" s="81"/>
+      <c r="A81" s="66"/>
+      <c r="B81" s="63"/>
+      <c r="C81" s="63"/>
+      <c r="D81" s="63"/>
+      <c r="E81" s="63"/>
       <c r="F81" s="44" t="s">
         <v>67</v>
       </c>
@@ -4759,9 +4867,9 @@
         <v>154</v>
       </c>
       <c r="H81" s="45"/>
-      <c r="I81" s="61"/>
-      <c r="J81" s="73"/>
-      <c r="K81" s="61"/>
+      <c r="I81" s="48"/>
+      <c r="J81" s="60"/>
+      <c r="K81" s="48"/>
       <c r="L81" s="2"/>
       <c r="M81" s="2"/>
       <c r="N81" s="2"/>
@@ -4780,11 +4888,11 @@
       <c r="AA81" s="2"/>
     </row>
     <row r="82" spans="1:27">
-      <c r="A82" s="79"/>
-      <c r="B82" s="81"/>
-      <c r="C82" s="81"/>
-      <c r="D82" s="81"/>
-      <c r="E82" s="81"/>
+      <c r="A82" s="66"/>
+      <c r="B82" s="63"/>
+      <c r="C82" s="63"/>
+      <c r="D82" s="63"/>
+      <c r="E82" s="63"/>
       <c r="F82" s="44" t="s">
         <v>70</v>
       </c>
@@ -4794,9 +4902,9 @@
       <c r="H82" s="45" t="s">
         <v>146</v>
       </c>
-      <c r="I82" s="61"/>
-      <c r="J82" s="73"/>
-      <c r="K82" s="61"/>
+      <c r="I82" s="48"/>
+      <c r="J82" s="60"/>
+      <c r="K82" s="48"/>
       <c r="L82" s="2"/>
       <c r="M82" s="2"/>
       <c r="N82" s="2"/>
@@ -4815,11 +4923,11 @@
       <c r="AA82" s="2"/>
     </row>
     <row r="83" spans="1:27">
-      <c r="A83" s="80"/>
-      <c r="B83" s="82"/>
-      <c r="C83" s="82"/>
-      <c r="D83" s="82"/>
-      <c r="E83" s="82"/>
+      <c r="A83" s="67"/>
+      <c r="B83" s="64"/>
+      <c r="C83" s="64"/>
+      <c r="D83" s="64"/>
+      <c r="E83" s="64"/>
       <c r="F83" s="44" t="s">
         <v>99</v>
       </c>
@@ -4829,9 +4937,9 @@
       <c r="H83" s="45" t="s">
         <v>156</v>
       </c>
-      <c r="I83" s="62"/>
-      <c r="J83" s="74"/>
-      <c r="K83" s="62"/>
+      <c r="I83" s="49"/>
+      <c r="J83" s="61"/>
+      <c r="K83" s="49"/>
       <c r="L83" s="2"/>
       <c r="M83" s="2"/>
       <c r="N83" s="2"/>
@@ -4850,19 +4958,19 @@
       <c r="AA83" s="2"/>
     </row>
     <row r="84" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A84" s="78" t="s">
+      <c r="A84" s="65" t="s">
         <v>162</v>
       </c>
-      <c r="B84" s="49" t="s">
+      <c r="B84" s="62" t="s">
         <v>138</v>
       </c>
-      <c r="C84" s="49" t="s">
+      <c r="C84" s="62" t="s">
         <v>157</v>
       </c>
-      <c r="D84" s="49" t="s">
+      <c r="D84" s="62" t="s">
         <v>158</v>
       </c>
-      <c r="E84" s="49" t="s">
+      <c r="E84" s="62" t="s">
         <v>141</v>
       </c>
       <c r="F84" s="44" t="s">
@@ -4874,13 +4982,13 @@
       <c r="H84" s="45" t="s">
         <v>143</v>
       </c>
-      <c r="I84" s="60" t="s">
+      <c r="I84" s="47" t="s">
         <v>26</v>
       </c>
-      <c r="J84" s="72" t="s">
+      <c r="J84" s="59" t="s">
         <v>56</v>
       </c>
-      <c r="K84" s="60" t="s">
+      <c r="K84" s="47" t="s">
         <v>28</v>
       </c>
       <c r="L84" s="2"/>
@@ -4901,11 +5009,11 @@
       <c r="AA84" s="2"/>
     </row>
     <row r="85" spans="1:27" ht="24" customHeight="1">
-      <c r="A85" s="79"/>
-      <c r="B85" s="81"/>
-      <c r="C85" s="81"/>
-      <c r="D85" s="81"/>
-      <c r="E85" s="81"/>
+      <c r="A85" s="66"/>
+      <c r="B85" s="63"/>
+      <c r="C85" s="63"/>
+      <c r="D85" s="63"/>
+      <c r="E85" s="63"/>
       <c r="F85" s="44" t="s">
         <v>67</v>
       </c>
@@ -4915,9 +5023,9 @@
       <c r="H85" s="45" t="s">
         <v>160</v>
       </c>
-      <c r="I85" s="61"/>
-      <c r="J85" s="73"/>
-      <c r="K85" s="61"/>
+      <c r="I85" s="48"/>
+      <c r="J85" s="60"/>
+      <c r="K85" s="48"/>
       <c r="L85" s="2"/>
       <c r="M85" s="2"/>
       <c r="N85" s="2"/>
@@ -4936,11 +5044,11 @@
       <c r="AA85" s="2"/>
     </row>
     <row r="86" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A86" s="79"/>
-      <c r="B86" s="81"/>
-      <c r="C86" s="81"/>
-      <c r="D86" s="81"/>
-      <c r="E86" s="81"/>
+      <c r="A86" s="66"/>
+      <c r="B86" s="63"/>
+      <c r="C86" s="63"/>
+      <c r="D86" s="63"/>
+      <c r="E86" s="63"/>
       <c r="F86" s="44" t="s">
         <v>70</v>
       </c>
@@ -4950,9 +5058,9 @@
       <c r="H86" s="45" t="s">
         <v>161</v>
       </c>
-      <c r="I86" s="61"/>
-      <c r="J86" s="73"/>
-      <c r="K86" s="61"/>
+      <c r="I86" s="48"/>
+      <c r="J86" s="60"/>
+      <c r="K86" s="48"/>
       <c r="L86" s="2"/>
       <c r="M86" s="2"/>
       <c r="N86" s="2"/>
@@ -4971,17 +5079,17 @@
       <c r="AA86" s="2"/>
     </row>
     <row r="87" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A87" s="80"/>
-      <c r="B87" s="82"/>
-      <c r="C87" s="82"/>
-      <c r="D87" s="82"/>
-      <c r="E87" s="82"/>
+      <c r="A87" s="67"/>
+      <c r="B87" s="64"/>
+      <c r="C87" s="64"/>
+      <c r="D87" s="64"/>
+      <c r="E87" s="64"/>
       <c r="F87" s="44"/>
       <c r="G87" s="45"/>
       <c r="H87" s="45"/>
-      <c r="I87" s="62"/>
-      <c r="J87" s="74"/>
-      <c r="K87" s="62"/>
+      <c r="I87" s="49"/>
+      <c r="J87" s="61"/>
+      <c r="K87" s="49"/>
       <c r="L87" s="2"/>
       <c r="M87" s="2"/>
       <c r="N87" s="2"/>
@@ -5000,19 +5108,19 @@
       <c r="AA87" s="2"/>
     </row>
     <row r="88" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A88" s="90" t="s">
+      <c r="A88" s="50" t="s">
         <v>169</v>
       </c>
-      <c r="B88" s="86" t="s">
+      <c r="B88" s="53" t="s">
         <v>49</v>
       </c>
-      <c r="C88" s="46" t="s">
+      <c r="C88" s="56" t="s">
         <v>164</v>
       </c>
-      <c r="D88" s="46" t="s">
+      <c r="D88" s="56" t="s">
         <v>165</v>
       </c>
-      <c r="E88" s="46" t="s">
+      <c r="E88" s="56" t="s">
         <v>166</v>
       </c>
       <c r="F88" s="30" t="s">
@@ -5024,13 +5132,13 @@
       <c r="H88" s="30" t="s">
         <v>168</v>
       </c>
-      <c r="I88" s="60" t="s">
+      <c r="I88" s="47" t="s">
         <v>26</v>
       </c>
-      <c r="J88" s="72" t="s">
+      <c r="J88" s="59" t="s">
         <v>56</v>
       </c>
-      <c r="K88" s="60" t="s">
+      <c r="K88" s="47" t="s">
         <v>28</v>
       </c>
       <c r="L88" s="2"/>
@@ -5051,19 +5159,19 @@
       <c r="AA88" s="2"/>
     </row>
     <row r="89" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A89" s="91"/>
-      <c r="B89" s="87"/>
-      <c r="C89" s="47"/>
-      <c r="D89" s="47"/>
-      <c r="E89" s="47"/>
+      <c r="A89" s="51"/>
+      <c r="B89" s="54"/>
+      <c r="C89" s="57"/>
+      <c r="D89" s="57"/>
+      <c r="E89" s="57"/>
       <c r="F89" s="30" t="s">
         <v>67</v>
       </c>
       <c r="G89" s="35"/>
       <c r="H89" s="35"/>
-      <c r="I89" s="61"/>
-      <c r="J89" s="73"/>
-      <c r="K89" s="61"/>
+      <c r="I89" s="48"/>
+      <c r="J89" s="60"/>
+      <c r="K89" s="48"/>
       <c r="L89" s="2"/>
       <c r="M89" s="2"/>
       <c r="N89" s="2"/>
@@ -5082,19 +5190,19 @@
       <c r="AA89" s="2"/>
     </row>
     <row r="90" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A90" s="91"/>
-      <c r="B90" s="87"/>
-      <c r="C90" s="47"/>
-      <c r="D90" s="47"/>
-      <c r="E90" s="47"/>
+      <c r="A90" s="51"/>
+      <c r="B90" s="54"/>
+      <c r="C90" s="57"/>
+      <c r="D90" s="57"/>
+      <c r="E90" s="57"/>
       <c r="F90" s="30" t="s">
         <v>70</v>
       </c>
-      <c r="G90" s="88"/>
-      <c r="H90" s="88"/>
-      <c r="I90" s="61"/>
-      <c r="J90" s="73"/>
-      <c r="K90" s="61"/>
+      <c r="G90" s="46"/>
+      <c r="H90" s="46"/>
+      <c r="I90" s="48"/>
+      <c r="J90" s="60"/>
+      <c r="K90" s="48"/>
       <c r="L90" s="2"/>
       <c r="M90" s="2"/>
       <c r="N90" s="2"/>
@@ -5113,19 +5221,19 @@
       <c r="AA90" s="2"/>
     </row>
     <row r="91" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A91" s="92"/>
-      <c r="B91" s="89"/>
-      <c r="C91" s="48"/>
-      <c r="D91" s="48"/>
-      <c r="E91" s="48"/>
+      <c r="A91" s="52"/>
+      <c r="B91" s="55"/>
+      <c r="C91" s="58"/>
+      <c r="D91" s="58"/>
+      <c r="E91" s="58"/>
       <c r="F91" s="30" t="s">
         <v>99</v>
       </c>
       <c r="G91" s="30"/>
       <c r="H91" s="30"/>
-      <c r="I91" s="62"/>
-      <c r="J91" s="74"/>
-      <c r="K91" s="62"/>
+      <c r="I91" s="49"/>
+      <c r="J91" s="61"/>
+      <c r="K91" s="49"/>
       <c r="L91" s="2"/>
       <c r="M91" s="2"/>
       <c r="N91" s="2"/>
@@ -5143,18 +5251,40 @@
       <c r="Z91" s="2"/>
       <c r="AA91" s="2"/>
     </row>
-    <row r="92" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A92" s="2"/>
-      <c r="B92" s="38"/>
-      <c r="C92" s="2"/>
-      <c r="D92" s="38"/>
-      <c r="E92" s="38"/>
-      <c r="F92" s="2"/>
-      <c r="G92" s="38"/>
-      <c r="H92" s="38"/>
-      <c r="I92" s="2"/>
-      <c r="J92" s="38"/>
-      <c r="K92" s="2"/>
+    <row r="92" spans="1:27" ht="25.5" customHeight="1">
+      <c r="A92" s="68" t="s">
+        <v>186</v>
+      </c>
+      <c r="B92" s="56" t="s">
+        <v>84</v>
+      </c>
+      <c r="C92" s="56" t="s">
+        <v>170</v>
+      </c>
+      <c r="D92" s="56" t="s">
+        <v>171</v>
+      </c>
+      <c r="E92" s="56" t="s">
+        <v>172</v>
+      </c>
+      <c r="F92" s="30" t="s">
+        <v>53</v>
+      </c>
+      <c r="G92" s="35" t="s">
+        <v>173</v>
+      </c>
+      <c r="H92" s="30" t="s">
+        <v>174</v>
+      </c>
+      <c r="I92" s="47" t="s">
+        <v>26</v>
+      </c>
+      <c r="J92" s="59" t="s">
+        <v>56</v>
+      </c>
+      <c r="K92" s="47" t="s">
+        <v>28</v>
+      </c>
       <c r="L92" s="2"/>
       <c r="M92" s="2"/>
       <c r="N92" s="2"/>
@@ -5173,17 +5303,19 @@
       <c r="AA92" s="2"/>
     </row>
     <row r="93" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A93" s="2"/>
-      <c r="B93" s="38"/>
-      <c r="C93" s="2"/>
-      <c r="D93" s="38"/>
-      <c r="E93" s="38"/>
-      <c r="F93" s="2"/>
-      <c r="G93" s="38"/>
-      <c r="H93" s="38"/>
-      <c r="I93" s="2"/>
-      <c r="J93" s="38"/>
-      <c r="K93" s="2"/>
+      <c r="A93" s="69"/>
+      <c r="B93" s="57"/>
+      <c r="C93" s="57"/>
+      <c r="D93" s="57"/>
+      <c r="E93" s="57"/>
+      <c r="F93" s="30" t="s">
+        <v>67</v>
+      </c>
+      <c r="G93" s="35"/>
+      <c r="H93" s="30"/>
+      <c r="I93" s="48"/>
+      <c r="J93" s="60"/>
+      <c r="K93" s="48"/>
       <c r="L93" s="2"/>
       <c r="M93" s="2"/>
       <c r="N93" s="2"/>
@@ -5202,17 +5334,19 @@
       <c r="AA93" s="2"/>
     </row>
     <row r="94" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A94" s="2"/>
-      <c r="B94" s="38"/>
-      <c r="C94" s="2"/>
-      <c r="D94" s="38"/>
-      <c r="E94" s="38"/>
-      <c r="F94" s="2"/>
-      <c r="G94" s="38"/>
-      <c r="H94" s="38"/>
-      <c r="I94" s="2"/>
-      <c r="J94" s="38"/>
-      <c r="K94" s="2"/>
+      <c r="A94" s="69"/>
+      <c r="B94" s="57"/>
+      <c r="C94" s="57"/>
+      <c r="D94" s="57"/>
+      <c r="E94" s="57"/>
+      <c r="F94" s="30" t="s">
+        <v>70</v>
+      </c>
+      <c r="G94" s="46"/>
+      <c r="H94" s="46"/>
+      <c r="I94" s="48"/>
+      <c r="J94" s="60"/>
+      <c r="K94" s="48"/>
       <c r="L94" s="2"/>
       <c r="M94" s="2"/>
       <c r="N94" s="2"/>
@@ -5231,17 +5365,19 @@
       <c r="AA94" s="2"/>
     </row>
     <row r="95" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A95" s="2"/>
-      <c r="B95" s="38"/>
-      <c r="C95" s="2"/>
-      <c r="D95" s="38"/>
-      <c r="E95" s="38"/>
-      <c r="F95" s="2"/>
-      <c r="G95" s="38"/>
-      <c r="H95" s="38"/>
-      <c r="I95" s="2"/>
-      <c r="J95" s="38"/>
-      <c r="K95" s="2"/>
+      <c r="A95" s="70"/>
+      <c r="B95" s="58"/>
+      <c r="C95" s="58"/>
+      <c r="D95" s="58"/>
+      <c r="E95" s="58"/>
+      <c r="F95" s="30" t="s">
+        <v>99</v>
+      </c>
+      <c r="G95" s="30"/>
+      <c r="H95" s="30"/>
+      <c r="I95" s="49"/>
+      <c r="J95" s="61"/>
+      <c r="K95" s="49"/>
       <c r="L95" s="2"/>
       <c r="M95" s="2"/>
       <c r="N95" s="2"/>
@@ -5259,18 +5395,40 @@
       <c r="Z95" s="2"/>
       <c r="AA95" s="2"/>
     </row>
-    <row r="96" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A96" s="2"/>
-      <c r="B96" s="38"/>
-      <c r="C96" s="2"/>
-      <c r="D96" s="38"/>
-      <c r="E96" s="38"/>
-      <c r="F96" s="2"/>
-      <c r="G96" s="38"/>
-      <c r="H96" s="38"/>
-      <c r="I96" s="2"/>
-      <c r="J96" s="38"/>
-      <c r="K96" s="2"/>
+    <row r="96" spans="1:27" ht="26.25" customHeight="1">
+      <c r="A96" s="68" t="s">
+        <v>187</v>
+      </c>
+      <c r="B96" s="56" t="s">
+        <v>84</v>
+      </c>
+      <c r="C96" s="56" t="s">
+        <v>175</v>
+      </c>
+      <c r="D96" s="56" t="s">
+        <v>176</v>
+      </c>
+      <c r="E96" s="56" t="s">
+        <v>177</v>
+      </c>
+      <c r="F96" s="30" t="s">
+        <v>53</v>
+      </c>
+      <c r="G96" s="35" t="s">
+        <v>173</v>
+      </c>
+      <c r="H96" s="30" t="s">
+        <v>174</v>
+      </c>
+      <c r="I96" s="47" t="s">
+        <v>26</v>
+      </c>
+      <c r="J96" s="59" t="s">
+        <v>56</v>
+      </c>
+      <c r="K96" s="47" t="s">
+        <v>28</v>
+      </c>
       <c r="L96" s="2"/>
       <c r="M96" s="2"/>
       <c r="N96" s="2"/>
@@ -5289,17 +5447,19 @@
       <c r="AA96" s="2"/>
     </row>
     <row r="97" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A97" s="2"/>
-      <c r="B97" s="38"/>
-      <c r="C97" s="2"/>
-      <c r="D97" s="38"/>
-      <c r="E97" s="38"/>
-      <c r="F97" s="2"/>
-      <c r="G97" s="38"/>
-      <c r="H97" s="38"/>
-      <c r="I97" s="2"/>
-      <c r="J97" s="38"/>
-      <c r="K97" s="2"/>
+      <c r="A97" s="69"/>
+      <c r="B97" s="57"/>
+      <c r="C97" s="57"/>
+      <c r="D97" s="57"/>
+      <c r="E97" s="57"/>
+      <c r="F97" s="30" t="s">
+        <v>67</v>
+      </c>
+      <c r="G97" s="35"/>
+      <c r="H97" s="30"/>
+      <c r="I97" s="48"/>
+      <c r="J97" s="60"/>
+      <c r="K97" s="48"/>
       <c r="L97" s="2"/>
       <c r="M97" s="2"/>
       <c r="N97" s="2"/>
@@ -5318,17 +5478,19 @@
       <c r="AA97" s="2"/>
     </row>
     <row r="98" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A98" s="2"/>
-      <c r="B98" s="38"/>
-      <c r="C98" s="2"/>
-      <c r="D98" s="38"/>
-      <c r="E98" s="38"/>
-      <c r="F98" s="2"/>
-      <c r="G98" s="38"/>
-      <c r="H98" s="38"/>
-      <c r="I98" s="2"/>
-      <c r="J98" s="38"/>
-      <c r="K98" s="2"/>
+      <c r="A98" s="69"/>
+      <c r="B98" s="57"/>
+      <c r="C98" s="57"/>
+      <c r="D98" s="57"/>
+      <c r="E98" s="57"/>
+      <c r="F98" s="30" t="s">
+        <v>70</v>
+      </c>
+      <c r="G98" s="30"/>
+      <c r="H98" s="30"/>
+      <c r="I98" s="48"/>
+      <c r="J98" s="60"/>
+      <c r="K98" s="48"/>
       <c r="L98" s="2"/>
       <c r="M98" s="2"/>
       <c r="N98" s="2"/>
@@ -5347,17 +5509,19 @@
       <c r="AA98" s="2"/>
     </row>
     <row r="99" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A99" s="2"/>
-      <c r="B99" s="38"/>
-      <c r="C99" s="2"/>
-      <c r="D99" s="38"/>
-      <c r="E99" s="38"/>
-      <c r="F99" s="2"/>
-      <c r="G99" s="38"/>
-      <c r="H99" s="38"/>
-      <c r="I99" s="2"/>
-      <c r="J99" s="38"/>
-      <c r="K99" s="2"/>
+      <c r="A99" s="70"/>
+      <c r="B99" s="58"/>
+      <c r="C99" s="58"/>
+      <c r="D99" s="58"/>
+      <c r="E99" s="58"/>
+      <c r="F99" s="30" t="s">
+        <v>99</v>
+      </c>
+      <c r="G99" s="30"/>
+      <c r="H99" s="30"/>
+      <c r="I99" s="49"/>
+      <c r="J99" s="61"/>
+      <c r="K99" s="49"/>
       <c r="L99" s="2"/>
       <c r="M99" s="2"/>
       <c r="N99" s="2"/>
@@ -5375,18 +5539,40 @@
       <c r="Z99" s="2"/>
       <c r="AA99" s="2"/>
     </row>
-    <row r="100" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A100" s="2"/>
-      <c r="B100" s="38"/>
-      <c r="C100" s="2"/>
-      <c r="D100" s="38"/>
-      <c r="E100" s="38"/>
-      <c r="F100" s="2"/>
-      <c r="G100" s="38"/>
-      <c r="H100" s="38"/>
-      <c r="I100" s="2"/>
-      <c r="J100" s="38"/>
-      <c r="K100" s="2"/>
+    <row r="100" spans="1:27" ht="24.75" customHeight="1">
+      <c r="A100" s="68" t="s">
+        <v>188</v>
+      </c>
+      <c r="B100" s="56" t="s">
+        <v>84</v>
+      </c>
+      <c r="C100" s="56" t="s">
+        <v>178</v>
+      </c>
+      <c r="D100" s="56" t="s">
+        <v>179</v>
+      </c>
+      <c r="E100" s="56" t="s">
+        <v>172</v>
+      </c>
+      <c r="F100" s="30" t="s">
+        <v>53</v>
+      </c>
+      <c r="G100" s="35" t="s">
+        <v>180</v>
+      </c>
+      <c r="H100" s="30" t="s">
+        <v>181</v>
+      </c>
+      <c r="I100" s="47" t="s">
+        <v>26</v>
+      </c>
+      <c r="J100" s="59" t="s">
+        <v>56</v>
+      </c>
+      <c r="K100" s="47" t="s">
+        <v>28</v>
+      </c>
       <c r="L100" s="2"/>
       <c r="M100" s="2"/>
       <c r="N100" s="2"/>
@@ -5405,17 +5591,19 @@
       <c r="AA100" s="2"/>
     </row>
     <row r="101" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A101" s="2"/>
-      <c r="B101" s="38"/>
-      <c r="C101" s="2"/>
-      <c r="D101" s="38"/>
-      <c r="E101" s="38"/>
-      <c r="F101" s="2"/>
-      <c r="G101" s="38"/>
-      <c r="H101" s="38"/>
-      <c r="I101" s="2"/>
-      <c r="J101" s="38"/>
-      <c r="K101" s="2"/>
+      <c r="A101" s="69"/>
+      <c r="B101" s="57"/>
+      <c r="C101" s="57"/>
+      <c r="D101" s="57"/>
+      <c r="E101" s="57"/>
+      <c r="F101" s="30" t="s">
+        <v>67</v>
+      </c>
+      <c r="G101" s="35"/>
+      <c r="H101" s="30"/>
+      <c r="I101" s="48"/>
+      <c r="J101" s="60"/>
+      <c r="K101" s="48"/>
       <c r="L101" s="2"/>
       <c r="M101" s="2"/>
       <c r="N101" s="2"/>
@@ -5434,17 +5622,19 @@
       <c r="AA101" s="2"/>
     </row>
     <row r="102" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A102" s="2"/>
-      <c r="B102" s="38"/>
-      <c r="C102" s="2"/>
-      <c r="D102" s="38"/>
-      <c r="E102" s="38"/>
-      <c r="F102" s="2"/>
-      <c r="G102" s="38"/>
-      <c r="H102" s="38"/>
-      <c r="I102" s="2"/>
-      <c r="J102" s="38"/>
-      <c r="K102" s="2"/>
+      <c r="A102" s="69"/>
+      <c r="B102" s="57"/>
+      <c r="C102" s="57"/>
+      <c r="D102" s="57"/>
+      <c r="E102" s="57"/>
+      <c r="F102" s="30" t="s">
+        <v>70</v>
+      </c>
+      <c r="G102" s="46"/>
+      <c r="H102" s="46"/>
+      <c r="I102" s="48"/>
+      <c r="J102" s="60"/>
+      <c r="K102" s="48"/>
       <c r="L102" s="2"/>
       <c r="M102" s="2"/>
       <c r="N102" s="2"/>
@@ -5463,17 +5653,19 @@
       <c r="AA102" s="2"/>
     </row>
     <row r="103" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A103" s="2"/>
-      <c r="B103" s="38"/>
-      <c r="C103" s="2"/>
-      <c r="D103" s="38"/>
-      <c r="E103" s="38"/>
-      <c r="F103" s="2"/>
-      <c r="G103" s="38"/>
-      <c r="H103" s="38"/>
-      <c r="I103" s="2"/>
-      <c r="J103" s="38"/>
-      <c r="K103" s="2"/>
+      <c r="A103" s="70"/>
+      <c r="B103" s="58"/>
+      <c r="C103" s="58"/>
+      <c r="D103" s="58"/>
+      <c r="E103" s="58"/>
+      <c r="F103" s="30" t="s">
+        <v>99</v>
+      </c>
+      <c r="G103" s="46"/>
+      <c r="H103" s="46"/>
+      <c r="I103" s="49"/>
+      <c r="J103" s="61"/>
+      <c r="K103" s="49"/>
       <c r="L103" s="2"/>
       <c r="M103" s="2"/>
       <c r="N103" s="2"/>
@@ -5491,18 +5683,40 @@
       <c r="Z103" s="2"/>
       <c r="AA103" s="2"/>
     </row>
-    <row r="104" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A104" s="2"/>
-      <c r="B104" s="38"/>
-      <c r="C104" s="2"/>
-      <c r="D104" s="38"/>
-      <c r="E104" s="38"/>
-      <c r="F104" s="2"/>
-      <c r="G104" s="38"/>
-      <c r="H104" s="38"/>
-      <c r="I104" s="2"/>
-      <c r="J104" s="38"/>
-      <c r="K104" s="2"/>
+    <row r="104" spans="1:27" ht="24.75" customHeight="1">
+      <c r="A104" s="68" t="s">
+        <v>189</v>
+      </c>
+      <c r="B104" s="56" t="s">
+        <v>84</v>
+      </c>
+      <c r="C104" s="56" t="s">
+        <v>182</v>
+      </c>
+      <c r="D104" s="56" t="s">
+        <v>183</v>
+      </c>
+      <c r="E104" s="56" t="s">
+        <v>177</v>
+      </c>
+      <c r="F104" s="30" t="s">
+        <v>53</v>
+      </c>
+      <c r="G104" s="35" t="s">
+        <v>184</v>
+      </c>
+      <c r="H104" s="30" t="s">
+        <v>185</v>
+      </c>
+      <c r="I104" s="47" t="s">
+        <v>26</v>
+      </c>
+      <c r="J104" s="59" t="s">
+        <v>56</v>
+      </c>
+      <c r="K104" s="47" t="s">
+        <v>28</v>
+      </c>
       <c r="L104" s="2"/>
       <c r="M104" s="2"/>
       <c r="N104" s="2"/>
@@ -5521,17 +5735,19 @@
       <c r="AA104" s="2"/>
     </row>
     <row r="105" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A105" s="2"/>
-      <c r="B105" s="38"/>
-      <c r="C105" s="2"/>
-      <c r="D105" s="38"/>
-      <c r="E105" s="38"/>
-      <c r="F105" s="2"/>
-      <c r="G105" s="38"/>
-      <c r="H105" s="38"/>
-      <c r="I105" s="2"/>
-      <c r="J105" s="38"/>
-      <c r="K105" s="2"/>
+      <c r="A105" s="69"/>
+      <c r="B105" s="57"/>
+      <c r="C105" s="57"/>
+      <c r="D105" s="57"/>
+      <c r="E105" s="57"/>
+      <c r="F105" s="30" t="s">
+        <v>67</v>
+      </c>
+      <c r="G105" s="35"/>
+      <c r="H105" s="30"/>
+      <c r="I105" s="48"/>
+      <c r="J105" s="60"/>
+      <c r="K105" s="48"/>
       <c r="L105" s="2"/>
       <c r="M105" s="2"/>
       <c r="N105" s="2"/>
@@ -5550,17 +5766,19 @@
       <c r="AA105" s="2"/>
     </row>
     <row r="106" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A106" s="2"/>
-      <c r="B106" s="38"/>
-      <c r="C106" s="2"/>
-      <c r="D106" s="38"/>
-      <c r="E106" s="38"/>
-      <c r="F106" s="2"/>
-      <c r="G106" s="38"/>
-      <c r="H106" s="38"/>
-      <c r="I106" s="2"/>
-      <c r="J106" s="38"/>
-      <c r="K106" s="2"/>
+      <c r="A106" s="69"/>
+      <c r="B106" s="57"/>
+      <c r="C106" s="57"/>
+      <c r="D106" s="57"/>
+      <c r="E106" s="57"/>
+      <c r="F106" s="30" t="s">
+        <v>70</v>
+      </c>
+      <c r="G106" s="46"/>
+      <c r="H106" s="46"/>
+      <c r="I106" s="48"/>
+      <c r="J106" s="60"/>
+      <c r="K106" s="48"/>
       <c r="L106" s="2"/>
       <c r="M106" s="2"/>
       <c r="N106" s="2"/>
@@ -5579,17 +5797,19 @@
       <c r="AA106" s="2"/>
     </row>
     <row r="107" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A107" s="2"/>
-      <c r="B107" s="38"/>
-      <c r="C107" s="2"/>
-      <c r="D107" s="38"/>
-      <c r="E107" s="38"/>
-      <c r="F107" s="2"/>
-      <c r="G107" s="38"/>
-      <c r="H107" s="38"/>
-      <c r="I107" s="2"/>
-      <c r="J107" s="38"/>
-      <c r="K107" s="2"/>
+      <c r="A107" s="70"/>
+      <c r="B107" s="58"/>
+      <c r="C107" s="58"/>
+      <c r="D107" s="58"/>
+      <c r="E107" s="58"/>
+      <c r="F107" s="30" t="s">
+        <v>99</v>
+      </c>
+      <c r="G107" s="46"/>
+      <c r="H107" s="93"/>
+      <c r="I107" s="49"/>
+      <c r="J107" s="61"/>
+      <c r="K107" s="49"/>
       <c r="L107" s="2"/>
       <c r="M107" s="2"/>
       <c r="N107" s="2"/>
@@ -29620,83 +29840,133 @@
       <c r="AA935" s="6"/>
     </row>
   </sheetData>
-  <mergeCells count="194">
-    <mergeCell ref="K84:K87"/>
-    <mergeCell ref="A88:A91"/>
-    <mergeCell ref="B88:B91"/>
-    <mergeCell ref="C88:C91"/>
-    <mergeCell ref="D88:D91"/>
-    <mergeCell ref="E88:E91"/>
-    <mergeCell ref="I88:I91"/>
-    <mergeCell ref="J88:J91"/>
-    <mergeCell ref="K88:K91"/>
-    <mergeCell ref="B84:B87"/>
-    <mergeCell ref="C84:C87"/>
-    <mergeCell ref="D84:D87"/>
-    <mergeCell ref="E84:E87"/>
-    <mergeCell ref="I84:I87"/>
-    <mergeCell ref="J84:J87"/>
-    <mergeCell ref="A84:A87"/>
-    <mergeCell ref="B36:B39"/>
-    <mergeCell ref="C36:C39"/>
-    <mergeCell ref="D36:D39"/>
-    <mergeCell ref="E36:E39"/>
-    <mergeCell ref="J44:J47"/>
-    <mergeCell ref="J36:J39"/>
-    <mergeCell ref="A76:A79"/>
-    <mergeCell ref="B76:B79"/>
-    <mergeCell ref="C76:C79"/>
-    <mergeCell ref="D76:D79"/>
-    <mergeCell ref="E76:E79"/>
-    <mergeCell ref="I76:I79"/>
-    <mergeCell ref="J76:J79"/>
-    <mergeCell ref="A60:A63"/>
-    <mergeCell ref="J56:J59"/>
-    <mergeCell ref="K44:K47"/>
-    <mergeCell ref="I48:I51"/>
-    <mergeCell ref="J48:J51"/>
-    <mergeCell ref="K48:K51"/>
-    <mergeCell ref="B48:B51"/>
-    <mergeCell ref="C48:C51"/>
-    <mergeCell ref="D48:D51"/>
-    <mergeCell ref="E48:E51"/>
-    <mergeCell ref="K40:K43"/>
-    <mergeCell ref="I40:I43"/>
-    <mergeCell ref="B40:B43"/>
-    <mergeCell ref="C40:C43"/>
-    <mergeCell ref="D40:D43"/>
-    <mergeCell ref="E40:E43"/>
-    <mergeCell ref="K76:K79"/>
-    <mergeCell ref="J80:J83"/>
-    <mergeCell ref="K80:K83"/>
-    <mergeCell ref="A80:A83"/>
-    <mergeCell ref="B80:B83"/>
-    <mergeCell ref="C80:C83"/>
-    <mergeCell ref="D80:D83"/>
-    <mergeCell ref="E80:E83"/>
-    <mergeCell ref="I80:I83"/>
-    <mergeCell ref="K56:K59"/>
-    <mergeCell ref="J60:J63"/>
-    <mergeCell ref="K60:K63"/>
-    <mergeCell ref="I68:I71"/>
-    <mergeCell ref="J68:J71"/>
-    <mergeCell ref="K68:K71"/>
-    <mergeCell ref="A72:A75"/>
-    <mergeCell ref="B72:B75"/>
-    <mergeCell ref="C72:C75"/>
-    <mergeCell ref="D72:D75"/>
-    <mergeCell ref="E72:E75"/>
-    <mergeCell ref="I72:I75"/>
-    <mergeCell ref="J72:J75"/>
-    <mergeCell ref="K72:K75"/>
-    <mergeCell ref="A68:A71"/>
-    <mergeCell ref="B68:B71"/>
-    <mergeCell ref="C68:C71"/>
-    <mergeCell ref="D68:D71"/>
-    <mergeCell ref="E68:E71"/>
-    <mergeCell ref="A64:A67"/>
-    <mergeCell ref="J64:J67"/>
-    <mergeCell ref="K64:K67"/>
+  <mergeCells count="226">
+    <mergeCell ref="J92:J95"/>
+    <mergeCell ref="K92:K95"/>
+    <mergeCell ref="I96:I99"/>
+    <mergeCell ref="J96:J99"/>
+    <mergeCell ref="K96:K99"/>
+    <mergeCell ref="I100:I103"/>
+    <mergeCell ref="J100:J103"/>
+    <mergeCell ref="K100:K103"/>
+    <mergeCell ref="I104:I107"/>
+    <mergeCell ref="J104:J107"/>
+    <mergeCell ref="K104:K107"/>
+    <mergeCell ref="B104:B107"/>
+    <mergeCell ref="C104:C107"/>
+    <mergeCell ref="D104:D107"/>
+    <mergeCell ref="E104:E107"/>
+    <mergeCell ref="A92:A95"/>
+    <mergeCell ref="A96:A99"/>
+    <mergeCell ref="A100:A103"/>
+    <mergeCell ref="A104:A107"/>
+    <mergeCell ref="I92:I95"/>
+    <mergeCell ref="B92:B95"/>
+    <mergeCell ref="C92:C95"/>
+    <mergeCell ref="D92:D95"/>
+    <mergeCell ref="E92:E95"/>
+    <mergeCell ref="B96:B99"/>
+    <mergeCell ref="C96:C99"/>
+    <mergeCell ref="D96:D99"/>
+    <mergeCell ref="E96:E99"/>
+    <mergeCell ref="B100:B103"/>
+    <mergeCell ref="C100:C103"/>
+    <mergeCell ref="D100:D103"/>
+    <mergeCell ref="E100:E103"/>
+    <mergeCell ref="C32:C35"/>
+    <mergeCell ref="B32:B35"/>
+    <mergeCell ref="B28:B31"/>
+    <mergeCell ref="C4:C7"/>
+    <mergeCell ref="C8:C11"/>
+    <mergeCell ref="C12:C15"/>
+    <mergeCell ref="C16:C19"/>
+    <mergeCell ref="C20:C23"/>
+    <mergeCell ref="C24:C27"/>
+    <mergeCell ref="C28:C31"/>
+    <mergeCell ref="A4:A7"/>
+    <mergeCell ref="A8:A11"/>
+    <mergeCell ref="A12:A15"/>
+    <mergeCell ref="A16:A19"/>
+    <mergeCell ref="A20:A23"/>
+    <mergeCell ref="A24:A27"/>
+    <mergeCell ref="B24:B27"/>
+    <mergeCell ref="B20:B23"/>
+    <mergeCell ref="B16:B19"/>
+    <mergeCell ref="B12:B15"/>
+    <mergeCell ref="B8:B11"/>
+    <mergeCell ref="B4:B7"/>
+    <mergeCell ref="K2:K3"/>
+    <mergeCell ref="I4:I7"/>
+    <mergeCell ref="I8:I11"/>
+    <mergeCell ref="I12:I15"/>
+    <mergeCell ref="I16:I19"/>
+    <mergeCell ref="E28:E31"/>
+    <mergeCell ref="E2:E3"/>
+    <mergeCell ref="G12:G13"/>
+    <mergeCell ref="G8:G9"/>
+    <mergeCell ref="F12:F13"/>
+    <mergeCell ref="F4:F5"/>
+    <mergeCell ref="F8:F9"/>
+    <mergeCell ref="K28:K31"/>
+    <mergeCell ref="E16:E19"/>
+    <mergeCell ref="E20:E23"/>
+    <mergeCell ref="E24:E27"/>
+    <mergeCell ref="F2:H2"/>
+    <mergeCell ref="I2:I3"/>
+    <mergeCell ref="I20:I23"/>
+    <mergeCell ref="I24:I27"/>
+    <mergeCell ref="I28:I31"/>
+    <mergeCell ref="E4:E7"/>
+    <mergeCell ref="E8:E11"/>
+    <mergeCell ref="E12:E15"/>
+    <mergeCell ref="E32:E35"/>
+    <mergeCell ref="C2:C3"/>
+    <mergeCell ref="H4:H5"/>
+    <mergeCell ref="G4:G5"/>
+    <mergeCell ref="H8:H9"/>
+    <mergeCell ref="H12:H13"/>
+    <mergeCell ref="K32:K35"/>
+    <mergeCell ref="K36:K39"/>
+    <mergeCell ref="J4:J7"/>
+    <mergeCell ref="J8:J11"/>
+    <mergeCell ref="J12:J15"/>
+    <mergeCell ref="J16:J19"/>
+    <mergeCell ref="J20:J23"/>
+    <mergeCell ref="J24:J27"/>
+    <mergeCell ref="J28:J31"/>
+    <mergeCell ref="I32:I35"/>
+    <mergeCell ref="I36:I39"/>
+    <mergeCell ref="K4:K7"/>
+    <mergeCell ref="K8:K11"/>
+    <mergeCell ref="K12:K15"/>
+    <mergeCell ref="K16:K19"/>
+    <mergeCell ref="K20:K23"/>
+    <mergeCell ref="K24:K27"/>
+    <mergeCell ref="J2:J3"/>
+    <mergeCell ref="J32:J35"/>
+    <mergeCell ref="B2:B3"/>
+    <mergeCell ref="A2:A3"/>
+    <mergeCell ref="A52:A55"/>
+    <mergeCell ref="B52:B55"/>
+    <mergeCell ref="C56:C59"/>
+    <mergeCell ref="D56:D59"/>
+    <mergeCell ref="C52:C55"/>
+    <mergeCell ref="D52:D55"/>
+    <mergeCell ref="A44:A47"/>
+    <mergeCell ref="A48:A51"/>
+    <mergeCell ref="D24:D27"/>
+    <mergeCell ref="D20:D23"/>
+    <mergeCell ref="D16:D19"/>
+    <mergeCell ref="D12:D15"/>
+    <mergeCell ref="D8:D11"/>
+    <mergeCell ref="D4:D7"/>
+    <mergeCell ref="A28:A31"/>
+    <mergeCell ref="A32:A35"/>
+    <mergeCell ref="A36:A39"/>
+    <mergeCell ref="A40:A43"/>
+    <mergeCell ref="D32:D35"/>
+    <mergeCell ref="D28:D31"/>
+    <mergeCell ref="A56:A59"/>
     <mergeCell ref="D2:D3"/>
     <mergeCell ref="J52:J55"/>
     <mergeCell ref="K52:K55"/>
@@ -29721,226 +29991,208 @@
     <mergeCell ref="I56:I59"/>
     <mergeCell ref="I44:I47"/>
     <mergeCell ref="J40:J43"/>
-    <mergeCell ref="J32:J35"/>
-    <mergeCell ref="B2:B3"/>
-    <mergeCell ref="A2:A3"/>
-    <mergeCell ref="A52:A55"/>
-    <mergeCell ref="B52:B55"/>
-    <mergeCell ref="C56:C59"/>
-    <mergeCell ref="D56:D59"/>
-    <mergeCell ref="C52:C55"/>
-    <mergeCell ref="D52:D55"/>
-    <mergeCell ref="A44:A47"/>
-    <mergeCell ref="A48:A51"/>
-    <mergeCell ref="D24:D27"/>
-    <mergeCell ref="D20:D23"/>
-    <mergeCell ref="D16:D19"/>
-    <mergeCell ref="D12:D15"/>
-    <mergeCell ref="D8:D11"/>
-    <mergeCell ref="D4:D7"/>
-    <mergeCell ref="A28:A31"/>
-    <mergeCell ref="A32:A35"/>
-    <mergeCell ref="A36:A39"/>
-    <mergeCell ref="A40:A43"/>
-    <mergeCell ref="D32:D35"/>
-    <mergeCell ref="D28:D31"/>
-    <mergeCell ref="A56:A59"/>
-    <mergeCell ref="E32:E35"/>
-    <mergeCell ref="C2:C3"/>
-    <mergeCell ref="H4:H5"/>
-    <mergeCell ref="G4:G5"/>
-    <mergeCell ref="H8:H9"/>
-    <mergeCell ref="H12:H13"/>
-    <mergeCell ref="K32:K35"/>
-    <mergeCell ref="K36:K39"/>
-    <mergeCell ref="J4:J7"/>
-    <mergeCell ref="J8:J11"/>
-    <mergeCell ref="J12:J15"/>
-    <mergeCell ref="J16:J19"/>
-    <mergeCell ref="J20:J23"/>
-    <mergeCell ref="J24:J27"/>
-    <mergeCell ref="J28:J31"/>
-    <mergeCell ref="I32:I35"/>
-    <mergeCell ref="I36:I39"/>
-    <mergeCell ref="K4:K7"/>
-    <mergeCell ref="K8:K11"/>
-    <mergeCell ref="K12:K15"/>
-    <mergeCell ref="K16:K19"/>
-    <mergeCell ref="K20:K23"/>
-    <mergeCell ref="K24:K27"/>
-    <mergeCell ref="J2:J3"/>
-    <mergeCell ref="K2:K3"/>
-    <mergeCell ref="I4:I7"/>
-    <mergeCell ref="I8:I11"/>
-    <mergeCell ref="I12:I15"/>
-    <mergeCell ref="I16:I19"/>
-    <mergeCell ref="E28:E31"/>
-    <mergeCell ref="E2:E3"/>
-    <mergeCell ref="G12:G13"/>
-    <mergeCell ref="G8:G9"/>
-    <mergeCell ref="F12:F13"/>
-    <mergeCell ref="F4:F5"/>
-    <mergeCell ref="F8:F9"/>
-    <mergeCell ref="K28:K31"/>
-    <mergeCell ref="E16:E19"/>
-    <mergeCell ref="E20:E23"/>
-    <mergeCell ref="E24:E27"/>
-    <mergeCell ref="F2:H2"/>
-    <mergeCell ref="I2:I3"/>
-    <mergeCell ref="I20:I23"/>
-    <mergeCell ref="I24:I27"/>
-    <mergeCell ref="I28:I31"/>
-    <mergeCell ref="E4:E7"/>
-    <mergeCell ref="E8:E11"/>
-    <mergeCell ref="E12:E15"/>
-    <mergeCell ref="A4:A7"/>
-    <mergeCell ref="A8:A11"/>
-    <mergeCell ref="A12:A15"/>
-    <mergeCell ref="A16:A19"/>
-    <mergeCell ref="A20:A23"/>
-    <mergeCell ref="A24:A27"/>
-    <mergeCell ref="B24:B27"/>
-    <mergeCell ref="B20:B23"/>
-    <mergeCell ref="B16:B19"/>
-    <mergeCell ref="B12:B15"/>
-    <mergeCell ref="B8:B11"/>
-    <mergeCell ref="B4:B7"/>
-    <mergeCell ref="C32:C35"/>
-    <mergeCell ref="B32:B35"/>
-    <mergeCell ref="B28:B31"/>
-    <mergeCell ref="C4:C7"/>
-    <mergeCell ref="C8:C11"/>
-    <mergeCell ref="C12:C15"/>
-    <mergeCell ref="C16:C19"/>
-    <mergeCell ref="C20:C23"/>
-    <mergeCell ref="C24:C27"/>
-    <mergeCell ref="C28:C31"/>
+    <mergeCell ref="K56:K59"/>
+    <mergeCell ref="J60:J63"/>
+    <mergeCell ref="K60:K63"/>
+    <mergeCell ref="I68:I71"/>
+    <mergeCell ref="J68:J71"/>
+    <mergeCell ref="K68:K71"/>
+    <mergeCell ref="A72:A75"/>
+    <mergeCell ref="B72:B75"/>
+    <mergeCell ref="C72:C75"/>
+    <mergeCell ref="D72:D75"/>
+    <mergeCell ref="E72:E75"/>
+    <mergeCell ref="I72:I75"/>
+    <mergeCell ref="J72:J75"/>
+    <mergeCell ref="K72:K75"/>
+    <mergeCell ref="A68:A71"/>
+    <mergeCell ref="B68:B71"/>
+    <mergeCell ref="C68:C71"/>
+    <mergeCell ref="D68:D71"/>
+    <mergeCell ref="E68:E71"/>
+    <mergeCell ref="A64:A67"/>
+    <mergeCell ref="J64:J67"/>
+    <mergeCell ref="K64:K67"/>
+    <mergeCell ref="K76:K79"/>
+    <mergeCell ref="J80:J83"/>
+    <mergeCell ref="K80:K83"/>
+    <mergeCell ref="A80:A83"/>
+    <mergeCell ref="B80:B83"/>
+    <mergeCell ref="C80:C83"/>
+    <mergeCell ref="D80:D83"/>
+    <mergeCell ref="E80:E83"/>
+    <mergeCell ref="I80:I83"/>
+    <mergeCell ref="K44:K47"/>
+    <mergeCell ref="I48:I51"/>
+    <mergeCell ref="J48:J51"/>
+    <mergeCell ref="K48:K51"/>
+    <mergeCell ref="B48:B51"/>
+    <mergeCell ref="C48:C51"/>
+    <mergeCell ref="D48:D51"/>
+    <mergeCell ref="E48:E51"/>
+    <mergeCell ref="K40:K43"/>
+    <mergeCell ref="I40:I43"/>
+    <mergeCell ref="B40:B43"/>
+    <mergeCell ref="C40:C43"/>
+    <mergeCell ref="D40:D43"/>
+    <mergeCell ref="E40:E43"/>
+    <mergeCell ref="B36:B39"/>
+    <mergeCell ref="C36:C39"/>
+    <mergeCell ref="D36:D39"/>
+    <mergeCell ref="E36:E39"/>
+    <mergeCell ref="J44:J47"/>
+    <mergeCell ref="J36:J39"/>
+    <mergeCell ref="A76:A79"/>
+    <mergeCell ref="B76:B79"/>
+    <mergeCell ref="C76:C79"/>
+    <mergeCell ref="D76:D79"/>
+    <mergeCell ref="E76:E79"/>
+    <mergeCell ref="I76:I79"/>
+    <mergeCell ref="J76:J79"/>
+    <mergeCell ref="A60:A63"/>
+    <mergeCell ref="J56:J59"/>
+    <mergeCell ref="K84:K87"/>
+    <mergeCell ref="A88:A91"/>
+    <mergeCell ref="B88:B91"/>
+    <mergeCell ref="C88:C91"/>
+    <mergeCell ref="D88:D91"/>
+    <mergeCell ref="E88:E91"/>
+    <mergeCell ref="I88:I91"/>
+    <mergeCell ref="J88:J91"/>
+    <mergeCell ref="K88:K91"/>
+    <mergeCell ref="B84:B87"/>
+    <mergeCell ref="C84:C87"/>
+    <mergeCell ref="D84:D87"/>
+    <mergeCell ref="E84:E87"/>
+    <mergeCell ref="I84:I87"/>
+    <mergeCell ref="J84:J87"/>
+    <mergeCell ref="A84:A87"/>
   </mergeCells>
   <conditionalFormatting sqref="I4 I8 I12">
-    <cfRule type="cellIs" dxfId="27" priority="21" operator="equal">
+    <cfRule type="cellIs" dxfId="31" priority="21" operator="equal">
       <formula>"TO DO"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I4 I8 I12">
-    <cfRule type="cellIs" dxfId="26" priority="22" operator="equal">
+    <cfRule type="cellIs" dxfId="30" priority="22" operator="equal">
       <formula>"IN PROGRESS"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I4 I8 I12">
-    <cfRule type="cellIs" dxfId="25" priority="23" operator="equal">
+    <cfRule type="cellIs" dxfId="29" priority="23" operator="equal">
       <formula>"REVIEWED"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I4 I8 I12">
-    <cfRule type="cellIs" dxfId="24" priority="24" operator="equal">
+    <cfRule type="cellIs" dxfId="28" priority="24" operator="equal">
       <formula>"IN REVIEW"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I16 I20 I24">
-    <cfRule type="cellIs" dxfId="23" priority="17" operator="equal">
+    <cfRule type="cellIs" dxfId="27" priority="17" operator="equal">
       <formula>"TO DO"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I16 I20 I24">
-    <cfRule type="cellIs" dxfId="22" priority="18" operator="equal">
+    <cfRule type="cellIs" dxfId="26" priority="18" operator="equal">
       <formula>"IN PROGRESS"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I16 I20 I24">
-    <cfRule type="cellIs" dxfId="21" priority="19" operator="equal">
+    <cfRule type="cellIs" dxfId="25" priority="19" operator="equal">
       <formula>"REVIEWED"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I16 I20 I24">
-    <cfRule type="cellIs" dxfId="20" priority="20" operator="equal">
+    <cfRule type="cellIs" dxfId="24" priority="20" operator="equal">
       <formula>"IN REVIEW"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I28 I32 I36 I40 I44 I48 I52 I56 I60">
-    <cfRule type="cellIs" dxfId="19" priority="13" operator="equal">
+    <cfRule type="cellIs" dxfId="23" priority="13" operator="equal">
       <formula>"TO DO"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I28 I32 I36 I40 I44 I48 I52 I56 I60">
-    <cfRule type="cellIs" dxfId="18" priority="14" operator="equal">
+    <cfRule type="cellIs" dxfId="22" priority="14" operator="equal">
       <formula>"IN PROGRESS"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I28 I32 I36 I40 I44 I48 I52 I56 I60">
-    <cfRule type="cellIs" dxfId="17" priority="15" operator="equal">
+    <cfRule type="cellIs" dxfId="21" priority="15" operator="equal">
       <formula>"REVIEWED"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I28 I32 I36 I40 I44 I48 I52 I56 I60">
-    <cfRule type="cellIs" dxfId="16" priority="16" operator="equal">
+    <cfRule type="cellIs" dxfId="20" priority="16" operator="equal">
       <formula>"IN REVIEW"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I64 I68">
-    <cfRule type="cellIs" dxfId="15" priority="9" operator="equal">
+    <cfRule type="cellIs" dxfId="19" priority="9" operator="equal">
       <formula>"TO DO"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I64 I68">
-    <cfRule type="cellIs" dxfId="14" priority="10" operator="equal">
+    <cfRule type="cellIs" dxfId="18" priority="10" operator="equal">
       <formula>"IN PROGRESS"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I64 I68">
-    <cfRule type="cellIs" dxfId="13" priority="11" operator="equal">
+    <cfRule type="cellIs" dxfId="17" priority="11" operator="equal">
       <formula>"REVIEWED"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I64 I68">
-    <cfRule type="cellIs" dxfId="12" priority="12" operator="equal">
+    <cfRule type="cellIs" dxfId="16" priority="12" operator="equal">
       <formula>"IN REVIEW"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I76 I72 I80 I84">
-    <cfRule type="cellIs" dxfId="11" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="15" priority="5" operator="equal">
       <formula>"TO DO"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I76 I72 I80 I84">
-    <cfRule type="cellIs" dxfId="10" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="14" priority="6" operator="equal">
       <formula>"IN PROGRESS"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I76 I72 I80 I84">
-    <cfRule type="cellIs" dxfId="9" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="13" priority="7" operator="equal">
       <formula>"REVIEWED"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I76 I72 I80 I84">
-    <cfRule type="cellIs" dxfId="8" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="12" priority="8" operator="equal">
       <formula>"IN REVIEW"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I88">
-    <cfRule type="cellIs" dxfId="7" priority="1" operator="equal">
+  <conditionalFormatting sqref="I88 I92 I96 I100 I104">
+    <cfRule type="cellIs" dxfId="11" priority="1" operator="equal">
       <formula>"TO DO"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I88">
-    <cfRule type="cellIs" dxfId="5" priority="2" operator="equal">
+  <conditionalFormatting sqref="I88 I92 I96 I100 I104">
+    <cfRule type="cellIs" dxfId="10" priority="2" operator="equal">
       <formula>"IN PROGRESS"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I88">
-    <cfRule type="cellIs" dxfId="3" priority="3" operator="equal">
+  <conditionalFormatting sqref="I88 I92 I96 I100 I104">
+    <cfRule type="cellIs" dxfId="9" priority="3" operator="equal">
       <formula>"REVIEWED"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I88">
-    <cfRule type="cellIs" dxfId="1" priority="4" operator="equal">
+  <conditionalFormatting sqref="I88 I92 I96 I100 I104">
+    <cfRule type="cellIs" dxfId="8" priority="4" operator="equal">
       <formula>"IN REVIEW"</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" sqref="I52 I64 I24 I16 I20 I4 I8 I12 I68 I56 I60 I32 I36 I28 I40 I44 I48 I84 I76 I72 I80 I88">
+    <dataValidation type="list" allowBlank="1" sqref="I52 I64 I24 I16 I20 I4 I8 I12 I68 I56 I60 I32 I36 I28 I40 I44 I48 I84 I76 I72 I80 I88 I92 I96 I100 I104">
       <formula1>"TO DO,In Progress,In Review,Reviewed"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" sqref="K76 K36 K40 K32 K28 K4 K12 K8 K48 K44 K52 K60 K56 K64 K68 K72 K80 K20 K24 K16 K84 K88">
+    <dataValidation type="list" allowBlank="1" sqref="K76 K36 K40 K32 K28 K4 K12 K8 K48 K44 K52 K60 K56 K64 K68 K72 K80 K20 K24 K16 K84 K88 K92 K96 K100 K104">
       <formula1>"Smoke,Regresión"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
Agrego Casos de Prueba referentes a la visualizacion de productos de la web
</commit_message>
<xml_diff>
--- a/Testing 2024/template_caso_prueba-ISPC2024-sprint-1.xlsx
+++ b/Testing 2024/template_caso_prueba-ISPC2024-sprint-1.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="419" uniqueCount="190">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="444" uniqueCount="202">
   <si>
     <t>Id</t>
   </si>
@@ -596,6 +596,42 @@
   <si>
     <t>TC-026</t>
   </si>
+  <si>
+    <t>Visualización de Productos</t>
+  </si>
+  <si>
+    <t>El usuario (registrado o no) debe estar situado en la home page</t>
+  </si>
+  <si>
+    <t>Visualizar las Categorias</t>
+  </si>
+  <si>
+    <t>Ingresar a la url http://cartech2022.sytes.net/</t>
+  </si>
+  <si>
+    <t>Visualizar las categorias disponibles la home page</t>
+  </si>
+  <si>
+    <t>Visualizar el detalle de un libro</t>
+  </si>
+  <si>
+    <t>El usuario accede al detalle de un libro con información mas detallada</t>
+  </si>
+  <si>
+    <t>El usuario hace click sobre uno de los libros</t>
+  </si>
+  <si>
+    <t>Se visualiza el detalle del libro: Titulo, autor, disponibilidad, precio, resumen, editorial ISBN, cantidad de paginas, clasificacion, fecha de publicacion y un boton para agregar el libro al carrito de compras</t>
+  </si>
+  <si>
+    <t>TC-027</t>
+  </si>
+  <si>
+    <t>TC-028</t>
+  </si>
+  <si>
+    <t>El usuario debe poder visualizar en la Home Page las Categorias disponibles</t>
+  </si>
 </sst>
 </file>
 
@@ -671,7 +707,7 @@
       <name val="ArialMT"/>
     </font>
   </fonts>
-  <fills count="16">
+  <fills count="15">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -746,24 +782,18 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.79998168889431442"/>
-        <bgColor rgb="FFFFFFCC"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FFF0CDF3"/>
         <bgColor rgb="FFFFFFCC"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF6DDBC"/>
+        <fgColor rgb="FFFDCDCD"/>
         <bgColor rgb="FFFFFFCC"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="24">
+  <borders count="25">
     <border>
       <left/>
       <right/>
@@ -1044,11 +1074,22 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="94">
+  <cellXfs count="92">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -1150,38 +1191,7 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="15" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="15" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="15" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="7" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1191,23 +1201,19 @@
     <xf numFmtId="0" fontId="1" fillId="7" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="14" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="14" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="14" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="12" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1218,53 +1224,14 @@
     <xf numFmtId="0" fontId="1" fillId="12" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="13" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="13" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="13" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="11" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="9" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="10" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1284,44 +1251,80 @@
     <xf numFmtId="0" fontId="1" fillId="11" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="9" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="13" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="13" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="13" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="14" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="14" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="14" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="32">
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFCE5CD"/>
-          <bgColor rgb="FFFCE5CD"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FF93C47D"/>
-          <bgColor rgb="FF93C47D"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFF2CC"/>
-          <bgColor rgb="FFFFF2CC"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFA2C4C9"/>
-          <bgColor rgb="FFA2C4C9"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="28">
     <dxf>
       <fill>
         <patternFill patternType="solid">
@@ -1616,6 +1619,7 @@
       <rgbColor rgb="00333333"/>
     </indexedColors>
     <mruColors>
+      <color rgb="FFFDCDCD"/>
       <color rgb="FFF6DDBC"/>
       <color rgb="FFF0CDF3"/>
     </mruColors>
@@ -1894,10 +1898,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AA935"/>
+  <dimension ref="A1:AA931"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A93" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="60" workbookViewId="0">
-      <selection activeCell="M106" sqref="M106"/>
+    <sheetView tabSelected="1" topLeftCell="A106" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="60" workbookViewId="0">
+      <selection activeCell="C119" sqref="C119"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5703125" defaultRowHeight="12.75"/>
@@ -1946,33 +1950,33 @@
       <c r="AA1" s="2"/>
     </row>
     <row r="2" spans="1:27" s="31" customFormat="1" ht="15.75" customHeight="1">
-      <c r="A2" s="78" t="s">
+      <c r="A2" s="76" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="76" t="s">
+      <c r="B2" s="69" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="78" t="s">
+      <c r="C2" s="76" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="76" t="s">
+      <c r="D2" s="69" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="76" t="s">
+      <c r="E2" s="69" t="s">
         <v>4</v>
       </c>
-      <c r="F2" s="82" t="s">
+      <c r="F2" s="71" t="s">
         <v>5</v>
       </c>
-      <c r="G2" s="83"/>
-      <c r="H2" s="84"/>
-      <c r="I2" s="85" t="s">
+      <c r="G2" s="72"/>
+      <c r="H2" s="73"/>
+      <c r="I2" s="74" t="s">
         <v>6</v>
       </c>
-      <c r="J2" s="76" t="s">
+      <c r="J2" s="69" t="s">
         <v>7</v>
       </c>
-      <c r="K2" s="76" t="s">
+      <c r="K2" s="69" t="s">
         <v>27</v>
       </c>
       <c r="L2" s="32"/>
@@ -1993,11 +1997,11 @@
       <c r="AA2" s="33"/>
     </row>
     <row r="3" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A3" s="79"/>
-      <c r="B3" s="77"/>
-      <c r="C3" s="79"/>
-      <c r="D3" s="77"/>
-      <c r="E3" s="77"/>
+      <c r="A3" s="77"/>
+      <c r="B3" s="70"/>
+      <c r="C3" s="77"/>
+      <c r="D3" s="70"/>
+      <c r="E3" s="70"/>
       <c r="F3" s="34" t="s">
         <v>8</v>
       </c>
@@ -2007,9 +2011,9 @@
       <c r="H3" s="42" t="s">
         <v>10</v>
       </c>
-      <c r="I3" s="86"/>
-      <c r="J3" s="77"/>
-      <c r="K3" s="77"/>
+      <c r="I3" s="75"/>
+      <c r="J3" s="70"/>
+      <c r="K3" s="70"/>
       <c r="L3" s="3"/>
       <c r="M3" s="2"/>
       <c r="N3" s="2"/>
@@ -2028,37 +2032,37 @@
       <c r="AA3" s="2"/>
     </row>
     <row r="4" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A4" s="87" t="s">
+      <c r="A4" s="63" t="s">
         <v>29</v>
       </c>
-      <c r="B4" s="56" t="s">
+      <c r="B4" s="54" t="s">
         <v>49</v>
       </c>
-      <c r="C4" s="56" t="s">
+      <c r="C4" s="54" t="s">
         <v>50</v>
       </c>
-      <c r="D4" s="56" t="s">
+      <c r="D4" s="54" t="s">
         <v>51</v>
       </c>
-      <c r="E4" s="56" t="s">
+      <c r="E4" s="54" t="s">
         <v>52</v>
       </c>
-      <c r="F4" s="56" t="s">
+      <c r="F4" s="54" t="s">
         <v>53</v>
       </c>
-      <c r="G4" s="56" t="s">
+      <c r="G4" s="54" t="s">
         <v>54</v>
       </c>
-      <c r="H4" s="80" t="s">
+      <c r="H4" s="78" t="s">
         <v>55</v>
       </c>
-      <c r="I4" s="47" t="s">
+      <c r="I4" s="51" t="s">
         <v>26</v>
       </c>
-      <c r="J4" s="59" t="s">
+      <c r="J4" s="48" t="s">
         <v>56</v>
       </c>
-      <c r="K4" s="47" t="s">
+      <c r="K4" s="51" t="s">
         <v>28</v>
       </c>
       <c r="L4" s="3"/>
@@ -2079,17 +2083,17 @@
       <c r="AA4" s="2"/>
     </row>
     <row r="5" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A5" s="88"/>
-      <c r="B5" s="57"/>
-      <c r="C5" s="57"/>
-      <c r="D5" s="57"/>
-      <c r="E5" s="57"/>
-      <c r="F5" s="58"/>
-      <c r="G5" s="58"/>
-      <c r="H5" s="81"/>
-      <c r="I5" s="48"/>
-      <c r="J5" s="60"/>
-      <c r="K5" s="48"/>
+      <c r="A5" s="64"/>
+      <c r="B5" s="55"/>
+      <c r="C5" s="55"/>
+      <c r="D5" s="55"/>
+      <c r="E5" s="55"/>
+      <c r="F5" s="56"/>
+      <c r="G5" s="56"/>
+      <c r="H5" s="79"/>
+      <c r="I5" s="52"/>
+      <c r="J5" s="49"/>
+      <c r="K5" s="52"/>
       <c r="L5" s="3"/>
       <c r="M5" s="2"/>
       <c r="N5" s="2"/>
@@ -2108,17 +2112,17 @@
       <c r="AA5" s="2"/>
     </row>
     <row r="6" spans="1:27" s="29" customFormat="1" ht="15.75" customHeight="1">
-      <c r="A6" s="88"/>
-      <c r="B6" s="57"/>
-      <c r="C6" s="57"/>
-      <c r="D6" s="57"/>
-      <c r="E6" s="57"/>
+      <c r="A6" s="64"/>
+      <c r="B6" s="55"/>
+      <c r="C6" s="55"/>
+      <c r="D6" s="55"/>
+      <c r="E6" s="55"/>
       <c r="F6" s="30"/>
       <c r="G6" s="35"/>
       <c r="H6" s="35"/>
-      <c r="I6" s="48"/>
-      <c r="J6" s="60"/>
-      <c r="K6" s="48"/>
+      <c r="I6" s="52"/>
+      <c r="J6" s="49"/>
+      <c r="K6" s="52"/>
       <c r="L6" s="27"/>
       <c r="M6" s="28"/>
       <c r="N6" s="28"/>
@@ -2137,17 +2141,17 @@
       <c r="AA6" s="28"/>
     </row>
     <row r="7" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A7" s="89"/>
-      <c r="B7" s="58"/>
-      <c r="C7" s="58"/>
-      <c r="D7" s="58"/>
-      <c r="E7" s="58"/>
+      <c r="A7" s="65"/>
+      <c r="B7" s="56"/>
+      <c r="C7" s="56"/>
+      <c r="D7" s="56"/>
+      <c r="E7" s="56"/>
       <c r="F7" s="30"/>
       <c r="G7" s="35"/>
       <c r="H7" s="35"/>
-      <c r="I7" s="49"/>
-      <c r="J7" s="61"/>
-      <c r="K7" s="49"/>
+      <c r="I7" s="53"/>
+      <c r="J7" s="50"/>
+      <c r="K7" s="53"/>
       <c r="L7" s="3"/>
       <c r="M7" s="2"/>
       <c r="N7" s="2"/>
@@ -2166,37 +2170,37 @@
       <c r="AA7" s="2"/>
     </row>
     <row r="8" spans="1:27">
-      <c r="A8" s="87" t="s">
+      <c r="A8" s="63" t="s">
         <v>30</v>
       </c>
-      <c r="B8" s="56" t="s">
+      <c r="B8" s="54" t="s">
         <v>49</v>
       </c>
-      <c r="C8" s="56" t="s">
+      <c r="C8" s="54" t="s">
         <v>57</v>
       </c>
-      <c r="D8" s="56" t="s">
+      <c r="D8" s="54" t="s">
         <v>58</v>
       </c>
-      <c r="E8" s="56" t="s">
+      <c r="E8" s="54" t="s">
         <v>59</v>
       </c>
-      <c r="F8" s="56" t="s">
+      <c r="F8" s="54" t="s">
         <v>53</v>
       </c>
-      <c r="G8" s="56" t="s">
+      <c r="G8" s="54" t="s">
         <v>54</v>
       </c>
-      <c r="H8" s="80" t="s">
+      <c r="H8" s="78" t="s">
         <v>55</v>
       </c>
-      <c r="I8" s="47" t="s">
+      <c r="I8" s="51" t="s">
         <v>26</v>
       </c>
-      <c r="J8" s="59" t="s">
+      <c r="J8" s="48" t="s">
         <v>56</v>
       </c>
-      <c r="K8" s="47" t="s">
+      <c r="K8" s="51" t="s">
         <v>28</v>
       </c>
       <c r="L8" s="3"/>
@@ -2217,17 +2221,17 @@
       <c r="AA8" s="2"/>
     </row>
     <row r="9" spans="1:27">
-      <c r="A9" s="88"/>
-      <c r="B9" s="57"/>
-      <c r="C9" s="57"/>
-      <c r="D9" s="57"/>
-      <c r="E9" s="57"/>
-      <c r="F9" s="58"/>
-      <c r="G9" s="58"/>
-      <c r="H9" s="81"/>
-      <c r="I9" s="48"/>
-      <c r="J9" s="60"/>
-      <c r="K9" s="48"/>
+      <c r="A9" s="64"/>
+      <c r="B9" s="55"/>
+      <c r="C9" s="55"/>
+      <c r="D9" s="55"/>
+      <c r="E9" s="55"/>
+      <c r="F9" s="56"/>
+      <c r="G9" s="56"/>
+      <c r="H9" s="79"/>
+      <c r="I9" s="52"/>
+      <c r="J9" s="49"/>
+      <c r="K9" s="52"/>
       <c r="L9" s="3"/>
       <c r="M9" s="2"/>
       <c r="N9" s="2"/>
@@ -2246,17 +2250,17 @@
       <c r="AA9" s="2"/>
     </row>
     <row r="10" spans="1:27" s="29" customFormat="1" ht="15.75" customHeight="1">
-      <c r="A10" s="88"/>
-      <c r="B10" s="57"/>
-      <c r="C10" s="57"/>
-      <c r="D10" s="57"/>
-      <c r="E10" s="57"/>
+      <c r="A10" s="64"/>
+      <c r="B10" s="55"/>
+      <c r="C10" s="55"/>
+      <c r="D10" s="55"/>
+      <c r="E10" s="55"/>
       <c r="F10" s="30"/>
       <c r="G10" s="35"/>
       <c r="H10" s="35"/>
-      <c r="I10" s="48"/>
-      <c r="J10" s="60"/>
-      <c r="K10" s="48"/>
+      <c r="I10" s="52"/>
+      <c r="J10" s="49"/>
+      <c r="K10" s="52"/>
       <c r="L10" s="27"/>
       <c r="M10" s="28"/>
       <c r="N10" s="28"/>
@@ -2275,17 +2279,17 @@
       <c r="AA10" s="28"/>
     </row>
     <row r="11" spans="1:27">
-      <c r="A11" s="89"/>
-      <c r="B11" s="58"/>
-      <c r="C11" s="58"/>
-      <c r="D11" s="58"/>
-      <c r="E11" s="58"/>
+      <c r="A11" s="65"/>
+      <c r="B11" s="56"/>
+      <c r="C11" s="56"/>
+      <c r="D11" s="56"/>
+      <c r="E11" s="56"/>
       <c r="F11" s="30"/>
       <c r="G11" s="35"/>
       <c r="H11" s="35"/>
-      <c r="I11" s="49"/>
-      <c r="J11" s="61"/>
-      <c r="K11" s="49"/>
+      <c r="I11" s="53"/>
+      <c r="J11" s="50"/>
+      <c r="K11" s="53"/>
       <c r="L11" s="3"/>
       <c r="M11" s="2"/>
       <c r="N11" s="2"/>
@@ -2304,37 +2308,37 @@
       <c r="AA11" s="2"/>
     </row>
     <row r="12" spans="1:27">
-      <c r="A12" s="87" t="s">
+      <c r="A12" s="63" t="s">
         <v>31</v>
       </c>
-      <c r="B12" s="56" t="s">
+      <c r="B12" s="54" t="s">
         <v>49</v>
       </c>
-      <c r="C12" s="56" t="s">
+      <c r="C12" s="54" t="s">
         <v>60</v>
       </c>
-      <c r="D12" s="56" t="s">
+      <c r="D12" s="54" t="s">
         <v>61</v>
       </c>
-      <c r="E12" s="56" t="s">
+      <c r="E12" s="54" t="s">
         <v>62</v>
       </c>
-      <c r="F12" s="56" t="s">
+      <c r="F12" s="54" t="s">
         <v>53</v>
       </c>
-      <c r="G12" s="56" t="s">
+      <c r="G12" s="54" t="s">
         <v>54</v>
       </c>
-      <c r="H12" s="80" t="s">
+      <c r="H12" s="78" t="s">
         <v>55</v>
       </c>
-      <c r="I12" s="47" t="s">
+      <c r="I12" s="51" t="s">
         <v>26</v>
       </c>
-      <c r="J12" s="59" t="s">
+      <c r="J12" s="48" t="s">
         <v>56</v>
       </c>
-      <c r="K12" s="47" t="s">
+      <c r="K12" s="51" t="s">
         <v>28</v>
       </c>
       <c r="L12" s="2"/>
@@ -2355,17 +2359,17 @@
       <c r="AA12" s="2"/>
     </row>
     <row r="13" spans="1:27">
-      <c r="A13" s="88"/>
-      <c r="B13" s="57"/>
-      <c r="C13" s="57"/>
-      <c r="D13" s="57"/>
-      <c r="E13" s="57"/>
-      <c r="F13" s="58"/>
-      <c r="G13" s="58"/>
-      <c r="H13" s="81"/>
-      <c r="I13" s="48"/>
-      <c r="J13" s="60"/>
-      <c r="K13" s="48"/>
+      <c r="A13" s="64"/>
+      <c r="B13" s="55"/>
+      <c r="C13" s="55"/>
+      <c r="D13" s="55"/>
+      <c r="E13" s="55"/>
+      <c r="F13" s="56"/>
+      <c r="G13" s="56"/>
+      <c r="H13" s="79"/>
+      <c r="I13" s="52"/>
+      <c r="J13" s="49"/>
+      <c r="K13" s="52"/>
       <c r="L13" s="2"/>
       <c r="M13" s="2"/>
       <c r="N13" s="2"/>
@@ -2384,17 +2388,17 @@
       <c r="AA13" s="2"/>
     </row>
     <row r="14" spans="1:27" s="29" customFormat="1">
-      <c r="A14" s="88"/>
-      <c r="B14" s="57"/>
-      <c r="C14" s="57"/>
-      <c r="D14" s="57"/>
-      <c r="E14" s="57"/>
+      <c r="A14" s="64"/>
+      <c r="B14" s="55"/>
+      <c r="C14" s="55"/>
+      <c r="D14" s="55"/>
+      <c r="E14" s="55"/>
       <c r="F14" s="30"/>
       <c r="G14" s="35"/>
       <c r="H14" s="35"/>
-      <c r="I14" s="48"/>
-      <c r="J14" s="60"/>
-      <c r="K14" s="48"/>
+      <c r="I14" s="52"/>
+      <c r="J14" s="49"/>
+      <c r="K14" s="52"/>
       <c r="L14" s="28"/>
       <c r="M14" s="28"/>
       <c r="N14" s="28"/>
@@ -2413,17 +2417,17 @@
       <c r="AA14" s="28"/>
     </row>
     <row r="15" spans="1:27">
-      <c r="A15" s="89"/>
-      <c r="B15" s="58"/>
-      <c r="C15" s="58"/>
-      <c r="D15" s="58"/>
-      <c r="E15" s="58"/>
+      <c r="A15" s="65"/>
+      <c r="B15" s="56"/>
+      <c r="C15" s="56"/>
+      <c r="D15" s="56"/>
+      <c r="E15" s="56"/>
       <c r="F15" s="30"/>
       <c r="G15" s="35"/>
       <c r="H15" s="35"/>
-      <c r="I15" s="49"/>
-      <c r="J15" s="61"/>
-      <c r="K15" s="49"/>
+      <c r="I15" s="53"/>
+      <c r="J15" s="50"/>
+      <c r="K15" s="53"/>
       <c r="L15" s="2"/>
       <c r="M15" s="2"/>
       <c r="N15" s="2"/>
@@ -2442,19 +2446,19 @@
       <c r="AA15" s="2"/>
     </row>
     <row r="16" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A16" s="90" t="s">
+      <c r="A16" s="66" t="s">
         <v>32</v>
       </c>
-      <c r="B16" s="56" t="s">
+      <c r="B16" s="54" t="s">
         <v>63</v>
       </c>
-      <c r="C16" s="56" t="s">
+      <c r="C16" s="54" t="s">
         <v>64</v>
       </c>
-      <c r="D16" s="56" t="s">
+      <c r="D16" s="54" t="s">
         <v>65</v>
       </c>
-      <c r="E16" s="56" t="s">
+      <c r="E16" s="54" t="s">
         <v>83</v>
       </c>
       <c r="F16" s="30" t="s">
@@ -2466,13 +2470,13 @@
       <c r="H16" s="35" t="s">
         <v>66</v>
       </c>
-      <c r="I16" s="47" t="s">
+      <c r="I16" s="51" t="s">
         <v>26</v>
       </c>
-      <c r="J16" s="59" t="s">
+      <c r="J16" s="48" t="s">
         <v>56</v>
       </c>
-      <c r="K16" s="47" t="s">
+      <c r="K16" s="51" t="s">
         <v>28</v>
       </c>
       <c r="L16" s="2"/>
@@ -2493,11 +2497,11 @@
       <c r="AA16" s="2"/>
     </row>
     <row r="17" spans="1:27" ht="16.5" customHeight="1">
-      <c r="A17" s="91"/>
-      <c r="B17" s="57"/>
-      <c r="C17" s="57"/>
-      <c r="D17" s="57"/>
-      <c r="E17" s="57"/>
+      <c r="A17" s="67"/>
+      <c r="B17" s="55"/>
+      <c r="C17" s="55"/>
+      <c r="D17" s="55"/>
+      <c r="E17" s="55"/>
       <c r="F17" s="30" t="s">
         <v>67</v>
       </c>
@@ -2507,9 +2511,9 @@
       <c r="H17" s="35" t="s">
         <v>69</v>
       </c>
-      <c r="I17" s="48"/>
-      <c r="J17" s="60"/>
-      <c r="K17" s="48"/>
+      <c r="I17" s="52"/>
+      <c r="J17" s="49"/>
+      <c r="K17" s="52"/>
       <c r="L17" s="2"/>
       <c r="M17" s="2"/>
       <c r="N17" s="2"/>
@@ -2528,11 +2532,11 @@
       <c r="AA17" s="2"/>
     </row>
     <row r="18" spans="1:27" s="29" customFormat="1" ht="25.5">
-      <c r="A18" s="91"/>
-      <c r="B18" s="57"/>
-      <c r="C18" s="57"/>
-      <c r="D18" s="57"/>
-      <c r="E18" s="57"/>
+      <c r="A18" s="67"/>
+      <c r="B18" s="55"/>
+      <c r="C18" s="55"/>
+      <c r="D18" s="55"/>
+      <c r="E18" s="55"/>
       <c r="F18" s="30" t="s">
         <v>70</v>
       </c>
@@ -2542,9 +2546,9 @@
       <c r="H18" s="35" t="s">
         <v>72</v>
       </c>
-      <c r="I18" s="48"/>
-      <c r="J18" s="60"/>
-      <c r="K18" s="48"/>
+      <c r="I18" s="52"/>
+      <c r="J18" s="49"/>
+      <c r="K18" s="52"/>
       <c r="L18" s="28"/>
       <c r="M18" s="28"/>
       <c r="N18" s="28"/>
@@ -2563,17 +2567,17 @@
       <c r="AA18" s="28"/>
     </row>
     <row r="19" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A19" s="92"/>
-      <c r="B19" s="58"/>
-      <c r="C19" s="58"/>
-      <c r="D19" s="58"/>
-      <c r="E19" s="58"/>
+      <c r="A19" s="68"/>
+      <c r="B19" s="56"/>
+      <c r="C19" s="56"/>
+      <c r="D19" s="56"/>
+      <c r="E19" s="56"/>
       <c r="F19" s="30"/>
       <c r="G19" s="35"/>
       <c r="H19" s="35"/>
-      <c r="I19" s="49"/>
-      <c r="J19" s="61"/>
-      <c r="K19" s="49"/>
+      <c r="I19" s="53"/>
+      <c r="J19" s="50"/>
+      <c r="K19" s="53"/>
       <c r="L19" s="2"/>
       <c r="M19" s="2"/>
       <c r="N19" s="2"/>
@@ -2592,19 +2596,19 @@
       <c r="AA19" s="2"/>
     </row>
     <row r="20" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A20" s="90" t="s">
+      <c r="A20" s="66" t="s">
         <v>33</v>
       </c>
-      <c r="B20" s="56" t="s">
+      <c r="B20" s="54" t="s">
         <v>63</v>
       </c>
-      <c r="C20" s="62" t="s">
+      <c r="C20" s="60" t="s">
         <v>73</v>
       </c>
-      <c r="D20" s="56" t="s">
+      <c r="D20" s="54" t="s">
         <v>74</v>
       </c>
-      <c r="E20" s="56" t="s">
+      <c r="E20" s="54" t="s">
         <v>75</v>
       </c>
       <c r="F20" s="30" t="s">
@@ -2616,13 +2620,13 @@
       <c r="H20" s="35" t="s">
         <v>76</v>
       </c>
-      <c r="I20" s="47" t="s">
+      <c r="I20" s="51" t="s">
         <v>26</v>
       </c>
-      <c r="J20" s="59" t="s">
+      <c r="J20" s="48" t="s">
         <v>56</v>
       </c>
-      <c r="K20" s="47" t="s">
+      <c r="K20" s="51" t="s">
         <v>28</v>
       </c>
       <c r="L20" s="2"/>
@@ -2643,11 +2647,11 @@
       <c r="AA20" s="2"/>
     </row>
     <row r="21" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A21" s="91"/>
-      <c r="B21" s="57"/>
-      <c r="C21" s="74"/>
-      <c r="D21" s="57"/>
-      <c r="E21" s="57"/>
+      <c r="A21" s="67"/>
+      <c r="B21" s="55"/>
+      <c r="C21" s="61"/>
+      <c r="D21" s="55"/>
+      <c r="E21" s="55"/>
       <c r="F21" s="30" t="s">
         <v>67</v>
       </c>
@@ -2655,9 +2659,9 @@
         <v>77</v>
       </c>
       <c r="H21" s="35"/>
-      <c r="I21" s="48"/>
-      <c r="J21" s="60"/>
-      <c r="K21" s="48"/>
+      <c r="I21" s="52"/>
+      <c r="J21" s="49"/>
+      <c r="K21" s="52"/>
       <c r="L21" s="2"/>
       <c r="M21" s="2"/>
       <c r="N21" s="2"/>
@@ -2676,11 +2680,11 @@
       <c r="AA21" s="2"/>
     </row>
     <row r="22" spans="1:27" s="29" customFormat="1" ht="15.75" customHeight="1">
-      <c r="A22" s="91"/>
-      <c r="B22" s="57"/>
-      <c r="C22" s="74"/>
-      <c r="D22" s="57"/>
-      <c r="E22" s="57"/>
+      <c r="A22" s="67"/>
+      <c r="B22" s="55"/>
+      <c r="C22" s="61"/>
+      <c r="D22" s="55"/>
+      <c r="E22" s="55"/>
       <c r="F22" s="30" t="s">
         <v>70</v>
       </c>
@@ -2690,9 +2694,9 @@
       <c r="H22" s="35" t="s">
         <v>79</v>
       </c>
-      <c r="I22" s="48"/>
-      <c r="J22" s="60"/>
-      <c r="K22" s="48"/>
+      <c r="I22" s="52"/>
+      <c r="J22" s="49"/>
+      <c r="K22" s="52"/>
       <c r="L22" s="28"/>
       <c r="M22" s="28"/>
       <c r="N22" s="28"/>
@@ -2711,17 +2715,17 @@
       <c r="AA22" s="28"/>
     </row>
     <row r="23" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A23" s="92"/>
-      <c r="B23" s="58"/>
-      <c r="C23" s="75"/>
-      <c r="D23" s="58"/>
-      <c r="E23" s="58"/>
+      <c r="A23" s="68"/>
+      <c r="B23" s="56"/>
+      <c r="C23" s="62"/>
+      <c r="D23" s="56"/>
+      <c r="E23" s="56"/>
       <c r="F23" s="30"/>
       <c r="G23" s="35"/>
       <c r="H23" s="35"/>
-      <c r="I23" s="49"/>
-      <c r="J23" s="61"/>
-      <c r="K23" s="49"/>
+      <c r="I23" s="53"/>
+      <c r="J23" s="50"/>
+      <c r="K23" s="53"/>
       <c r="L23" s="2"/>
       <c r="M23" s="2"/>
       <c r="N23" s="2"/>
@@ -2740,19 +2744,19 @@
       <c r="AA23" s="2"/>
     </row>
     <row r="24" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A24" s="90" t="s">
+      <c r="A24" s="66" t="s">
         <v>34</v>
       </c>
-      <c r="B24" s="56" t="s">
+      <c r="B24" s="54" t="s">
         <v>63</v>
       </c>
-      <c r="C24" s="62" t="s">
+      <c r="C24" s="60" t="s">
         <v>80</v>
       </c>
-      <c r="D24" s="56" t="s">
+      <c r="D24" s="54" t="s">
         <v>81</v>
       </c>
-      <c r="E24" s="56" t="s">
+      <c r="E24" s="54" t="s">
         <v>75</v>
       </c>
       <c r="F24" s="30" t="s">
@@ -2764,13 +2768,13 @@
       <c r="H24" s="35" t="s">
         <v>76</v>
       </c>
-      <c r="I24" s="47" t="s">
+      <c r="I24" s="51" t="s">
         <v>26</v>
       </c>
-      <c r="J24" s="59" t="s">
+      <c r="J24" s="48" t="s">
         <v>56</v>
       </c>
-      <c r="K24" s="47" t="s">
+      <c r="K24" s="51" t="s">
         <v>28</v>
       </c>
       <c r="L24" s="2"/>
@@ -2791,11 +2795,11 @@
       <c r="AA24" s="2"/>
     </row>
     <row r="25" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A25" s="91"/>
-      <c r="B25" s="57"/>
-      <c r="C25" s="74"/>
-      <c r="D25" s="57"/>
-      <c r="E25" s="57"/>
+      <c r="A25" s="67"/>
+      <c r="B25" s="55"/>
+      <c r="C25" s="61"/>
+      <c r="D25" s="55"/>
+      <c r="E25" s="55"/>
       <c r="F25" s="30" t="s">
         <v>67</v>
       </c>
@@ -2803,9 +2807,9 @@
         <v>77</v>
       </c>
       <c r="H25" s="35"/>
-      <c r="I25" s="48"/>
-      <c r="J25" s="60"/>
-      <c r="K25" s="48"/>
+      <c r="I25" s="52"/>
+      <c r="J25" s="49"/>
+      <c r="K25" s="52"/>
       <c r="L25" s="2"/>
       <c r="M25" s="2"/>
       <c r="N25" s="2"/>
@@ -2824,11 +2828,11 @@
       <c r="AA25" s="2"/>
     </row>
     <row r="26" spans="1:27" s="29" customFormat="1" ht="25.5">
-      <c r="A26" s="91"/>
-      <c r="B26" s="57"/>
-      <c r="C26" s="74"/>
-      <c r="D26" s="57"/>
-      <c r="E26" s="57"/>
+      <c r="A26" s="67"/>
+      <c r="B26" s="55"/>
+      <c r="C26" s="61"/>
+      <c r="D26" s="55"/>
+      <c r="E26" s="55"/>
       <c r="F26" s="30" t="s">
         <v>70</v>
       </c>
@@ -2838,9 +2842,9 @@
       <c r="H26" s="35" t="s">
         <v>82</v>
       </c>
-      <c r="I26" s="48"/>
-      <c r="J26" s="60"/>
-      <c r="K26" s="48"/>
+      <c r="I26" s="52"/>
+      <c r="J26" s="49"/>
+      <c r="K26" s="52"/>
       <c r="L26" s="28"/>
       <c r="M26" s="28"/>
       <c r="N26" s="28"/>
@@ -2859,17 +2863,17 @@
       <c r="AA26" s="28"/>
     </row>
     <row r="27" spans="1:27" ht="18.75" customHeight="1">
-      <c r="A27" s="92"/>
-      <c r="B27" s="58"/>
-      <c r="C27" s="75"/>
-      <c r="D27" s="58"/>
-      <c r="E27" s="58"/>
+      <c r="A27" s="68"/>
+      <c r="B27" s="56"/>
+      <c r="C27" s="62"/>
+      <c r="D27" s="56"/>
+      <c r="E27" s="56"/>
       <c r="F27" s="30"/>
       <c r="G27" s="35"/>
       <c r="H27" s="35"/>
-      <c r="I27" s="49"/>
-      <c r="J27" s="61"/>
-      <c r="K27" s="49"/>
+      <c r="I27" s="53"/>
+      <c r="J27" s="50"/>
+      <c r="K27" s="53"/>
       <c r="L27" s="2"/>
       <c r="M27" s="2"/>
       <c r="N27" s="2"/>
@@ -2888,19 +2892,19 @@
       <c r="AA27" s="2"/>
     </row>
     <row r="28" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A28" s="68" t="s">
+      <c r="A28" s="57" t="s">
         <v>35</v>
       </c>
-      <c r="B28" s="56" t="s">
+      <c r="B28" s="54" t="s">
         <v>84</v>
       </c>
-      <c r="C28" s="56" t="s">
+      <c r="C28" s="54" t="s">
         <v>85</v>
       </c>
-      <c r="D28" s="56" t="s">
+      <c r="D28" s="54" t="s">
         <v>86</v>
       </c>
-      <c r="E28" s="56" t="s">
+      <c r="E28" s="54" t="s">
         <v>83</v>
       </c>
       <c r="F28" s="30" t="s">
@@ -2912,13 +2916,13 @@
       <c r="H28" s="35" t="s">
         <v>88</v>
       </c>
-      <c r="I28" s="47" t="s">
+      <c r="I28" s="51" t="s">
         <v>26</v>
       </c>
-      <c r="J28" s="59" t="s">
+      <c r="J28" s="48" t="s">
         <v>56</v>
       </c>
-      <c r="K28" s="47" t="s">
+      <c r="K28" s="51" t="s">
         <v>28</v>
       </c>
       <c r="L28" s="2"/>
@@ -2939,19 +2943,19 @@
       <c r="AA28" s="2"/>
     </row>
     <row r="29" spans="1:27">
-      <c r="A29" s="69"/>
-      <c r="B29" s="57"/>
-      <c r="C29" s="57"/>
-      <c r="D29" s="57"/>
-      <c r="E29" s="57"/>
+      <c r="A29" s="58"/>
+      <c r="B29" s="55"/>
+      <c r="C29" s="55"/>
+      <c r="D29" s="55"/>
+      <c r="E29" s="55"/>
       <c r="F29" s="30" t="s">
         <v>67</v>
       </c>
       <c r="G29" s="35"/>
       <c r="H29" s="35"/>
-      <c r="I29" s="48"/>
-      <c r="J29" s="60"/>
-      <c r="K29" s="48"/>
+      <c r="I29" s="52"/>
+      <c r="J29" s="49"/>
+      <c r="K29" s="52"/>
       <c r="L29" s="2"/>
       <c r="M29" s="2"/>
       <c r="N29" s="2"/>
@@ -2970,17 +2974,17 @@
       <c r="AA29" s="2"/>
     </row>
     <row r="30" spans="1:27" s="29" customFormat="1" ht="15.75" customHeight="1">
-      <c r="A30" s="69"/>
-      <c r="B30" s="57"/>
-      <c r="C30" s="57"/>
-      <c r="D30" s="57"/>
-      <c r="E30" s="57"/>
+      <c r="A30" s="58"/>
+      <c r="B30" s="55"/>
+      <c r="C30" s="55"/>
+      <c r="D30" s="55"/>
+      <c r="E30" s="55"/>
       <c r="F30" s="30"/>
       <c r="G30" s="35"/>
       <c r="H30" s="35"/>
-      <c r="I30" s="48"/>
-      <c r="J30" s="60"/>
-      <c r="K30" s="48"/>
+      <c r="I30" s="52"/>
+      <c r="J30" s="49"/>
+      <c r="K30" s="52"/>
       <c r="L30" s="28"/>
       <c r="M30" s="28"/>
       <c r="N30" s="28"/>
@@ -2999,17 +3003,17 @@
       <c r="AA30" s="28"/>
     </row>
     <row r="31" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A31" s="70"/>
-      <c r="B31" s="58"/>
-      <c r="C31" s="58"/>
-      <c r="D31" s="58"/>
-      <c r="E31" s="58"/>
+      <c r="A31" s="59"/>
+      <c r="B31" s="56"/>
+      <c r="C31" s="56"/>
+      <c r="D31" s="56"/>
+      <c r="E31" s="56"/>
       <c r="F31" s="30"/>
       <c r="G31" s="35"/>
       <c r="H31" s="35"/>
-      <c r="I31" s="49"/>
-      <c r="J31" s="61"/>
-      <c r="K31" s="49"/>
+      <c r="I31" s="53"/>
+      <c r="J31" s="50"/>
+      <c r="K31" s="53"/>
       <c r="L31" s="2"/>
       <c r="M31" s="2"/>
       <c r="N31" s="2"/>
@@ -3028,19 +3032,19 @@
       <c r="AA31" s="2"/>
     </row>
     <row r="32" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A32" s="68" t="s">
+      <c r="A32" s="57" t="s">
         <v>36</v>
       </c>
-      <c r="B32" s="56" t="s">
+      <c r="B32" s="54" t="s">
         <v>84</v>
       </c>
-      <c r="C32" s="56" t="s">
+      <c r="C32" s="54" t="s">
         <v>89</v>
       </c>
-      <c r="D32" s="56" t="s">
+      <c r="D32" s="54" t="s">
         <v>90</v>
       </c>
-      <c r="E32" s="56" t="s">
+      <c r="E32" s="54" t="s">
         <v>83</v>
       </c>
       <c r="F32" s="30" t="s">
@@ -3052,13 +3056,13 @@
       <c r="H32" s="35" t="s">
         <v>92</v>
       </c>
-      <c r="I32" s="47" t="s">
+      <c r="I32" s="51" t="s">
         <v>26</v>
       </c>
-      <c r="J32" s="59" t="s">
+      <c r="J32" s="48" t="s">
         <v>56</v>
       </c>
-      <c r="K32" s="47" t="s">
+      <c r="K32" s="51" t="s">
         <v>28</v>
       </c>
       <c r="L32" s="2"/>
@@ -3079,17 +3083,17 @@
       <c r="AA32" s="2"/>
     </row>
     <row r="33" spans="1:27">
-      <c r="A33" s="69"/>
-      <c r="B33" s="57"/>
-      <c r="C33" s="57"/>
-      <c r="D33" s="57"/>
-      <c r="E33" s="57"/>
+      <c r="A33" s="58"/>
+      <c r="B33" s="55"/>
+      <c r="C33" s="55"/>
+      <c r="D33" s="55"/>
+      <c r="E33" s="55"/>
       <c r="F33" s="30"/>
       <c r="G33" s="43"/>
       <c r="H33" s="43"/>
-      <c r="I33" s="48"/>
-      <c r="J33" s="60"/>
-      <c r="K33" s="48"/>
+      <c r="I33" s="52"/>
+      <c r="J33" s="49"/>
+      <c r="K33" s="52"/>
       <c r="L33" s="2"/>
       <c r="M33" s="2"/>
       <c r="N33" s="2"/>
@@ -3108,17 +3112,17 @@
       <c r="AA33" s="2"/>
     </row>
     <row r="34" spans="1:27">
-      <c r="A34" s="69"/>
-      <c r="B34" s="57"/>
-      <c r="C34" s="57"/>
-      <c r="D34" s="57"/>
-      <c r="E34" s="57"/>
+      <c r="A34" s="58"/>
+      <c r="B34" s="55"/>
+      <c r="C34" s="55"/>
+      <c r="D34" s="55"/>
+      <c r="E34" s="55"/>
       <c r="F34" s="30"/>
       <c r="G34" s="43"/>
       <c r="H34" s="43"/>
-      <c r="I34" s="48"/>
-      <c r="J34" s="60"/>
-      <c r="K34" s="48"/>
+      <c r="I34" s="52"/>
+      <c r="J34" s="49"/>
+      <c r="K34" s="52"/>
       <c r="L34" s="2"/>
       <c r="M34" s="2"/>
       <c r="N34" s="2"/>
@@ -3137,17 +3141,17 @@
       <c r="AA34" s="2"/>
     </row>
     <row r="35" spans="1:27">
-      <c r="A35" s="70"/>
-      <c r="B35" s="58"/>
-      <c r="C35" s="58"/>
-      <c r="D35" s="58"/>
-      <c r="E35" s="58"/>
+      <c r="A35" s="59"/>
+      <c r="B35" s="56"/>
+      <c r="C35" s="56"/>
+      <c r="D35" s="56"/>
+      <c r="E35" s="56"/>
       <c r="F35" s="30"/>
       <c r="G35" s="35"/>
       <c r="H35" s="35"/>
-      <c r="I35" s="49"/>
-      <c r="J35" s="61"/>
-      <c r="K35" s="49"/>
+      <c r="I35" s="53"/>
+      <c r="J35" s="50"/>
+      <c r="K35" s="53"/>
       <c r="L35" s="2"/>
       <c r="M35" s="2"/>
       <c r="N35" s="2"/>
@@ -3166,19 +3170,19 @@
       <c r="AA35" s="2"/>
     </row>
     <row r="36" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A36" s="68" t="s">
+      <c r="A36" s="57" t="s">
         <v>37</v>
       </c>
-      <c r="B36" s="56" t="s">
+      <c r="B36" s="54" t="s">
         <v>84</v>
       </c>
-      <c r="C36" s="56" t="s">
+      <c r="C36" s="54" t="s">
         <v>93</v>
       </c>
-      <c r="D36" s="56" t="s">
+      <c r="D36" s="54" t="s">
         <v>94</v>
       </c>
-      <c r="E36" s="56" t="s">
+      <c r="E36" s="54" t="s">
         <v>95</v>
       </c>
       <c r="F36" s="30" t="s">
@@ -3190,13 +3194,13 @@
       <c r="H36" s="35" t="s">
         <v>92</v>
       </c>
-      <c r="I36" s="47" t="s">
+      <c r="I36" s="51" t="s">
         <v>26</v>
       </c>
-      <c r="J36" s="59" t="s">
+      <c r="J36" s="48" t="s">
         <v>56</v>
       </c>
-      <c r="K36" s="47" t="s">
+      <c r="K36" s="51" t="s">
         <v>28</v>
       </c>
       <c r="L36" s="2"/>
@@ -3217,11 +3221,11 @@
       <c r="AA36" s="2"/>
     </row>
     <row r="37" spans="1:27" ht="25.5">
-      <c r="A37" s="69"/>
-      <c r="B37" s="57"/>
-      <c r="C37" s="57"/>
-      <c r="D37" s="57"/>
-      <c r="E37" s="57"/>
+      <c r="A37" s="58"/>
+      <c r="B37" s="55"/>
+      <c r="C37" s="55"/>
+      <c r="D37" s="55"/>
+      <c r="E37" s="55"/>
       <c r="F37" s="30" t="s">
         <v>67</v>
       </c>
@@ -3229,9 +3233,9 @@
         <v>96</v>
       </c>
       <c r="H37" s="35"/>
-      <c r="I37" s="48"/>
-      <c r="J37" s="60"/>
-      <c r="K37" s="48"/>
+      <c r="I37" s="52"/>
+      <c r="J37" s="49"/>
+      <c r="K37" s="52"/>
       <c r="L37" s="2"/>
       <c r="M37" s="2"/>
       <c r="N37" s="2"/>
@@ -3250,11 +3254,11 @@
       <c r="AA37" s="2"/>
     </row>
     <row r="38" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A38" s="69"/>
-      <c r="B38" s="57"/>
-      <c r="C38" s="57"/>
-      <c r="D38" s="57"/>
-      <c r="E38" s="57"/>
+      <c r="A38" s="58"/>
+      <c r="B38" s="55"/>
+      <c r="C38" s="55"/>
+      <c r="D38" s="55"/>
+      <c r="E38" s="55"/>
       <c r="F38" s="30" t="s">
         <v>70</v>
       </c>
@@ -3264,9 +3268,9 @@
       <c r="H38" s="35" t="s">
         <v>98</v>
       </c>
-      <c r="I38" s="48"/>
-      <c r="J38" s="60"/>
-      <c r="K38" s="48"/>
+      <c r="I38" s="52"/>
+      <c r="J38" s="49"/>
+      <c r="K38" s="52"/>
       <c r="L38" s="2"/>
       <c r="M38" s="2"/>
       <c r="N38" s="2"/>
@@ -3285,19 +3289,19 @@
       <c r="AA38" s="2"/>
     </row>
     <row r="39" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A39" s="70"/>
-      <c r="B39" s="58"/>
-      <c r="C39" s="58"/>
-      <c r="D39" s="58"/>
-      <c r="E39" s="58"/>
+      <c r="A39" s="59"/>
+      <c r="B39" s="56"/>
+      <c r="C39" s="56"/>
+      <c r="D39" s="56"/>
+      <c r="E39" s="56"/>
       <c r="F39" s="30" t="s">
         <v>99</v>
       </c>
       <c r="G39" s="35"/>
       <c r="H39" s="35"/>
-      <c r="I39" s="49"/>
-      <c r="J39" s="61"/>
-      <c r="K39" s="49"/>
+      <c r="I39" s="53"/>
+      <c r="J39" s="50"/>
+      <c r="K39" s="53"/>
       <c r="L39" s="2"/>
       <c r="M39" s="2"/>
       <c r="N39" s="2"/>
@@ -3316,19 +3320,19 @@
       <c r="AA39" s="2"/>
     </row>
     <row r="40" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A40" s="68" t="s">
+      <c r="A40" s="57" t="s">
         <v>38</v>
       </c>
-      <c r="B40" s="56" t="s">
+      <c r="B40" s="54" t="s">
         <v>84</v>
       </c>
-      <c r="C40" s="56" t="s">
+      <c r="C40" s="54" t="s">
         <v>100</v>
       </c>
-      <c r="D40" s="56" t="s">
+      <c r="D40" s="54" t="s">
         <v>101</v>
       </c>
-      <c r="E40" s="56" t="s">
+      <c r="E40" s="54" t="s">
         <v>102</v>
       </c>
       <c r="F40" s="30" t="s">
@@ -3340,13 +3344,13 @@
       <c r="H40" s="35" t="s">
         <v>88</v>
       </c>
-      <c r="I40" s="47" t="s">
+      <c r="I40" s="51" t="s">
         <v>26</v>
       </c>
-      <c r="J40" s="59" t="s">
+      <c r="J40" s="48" t="s">
         <v>56</v>
       </c>
-      <c r="K40" s="47" t="s">
+      <c r="K40" s="51" t="s">
         <v>28</v>
       </c>
       <c r="L40" s="2"/>
@@ -3367,11 +3371,11 @@
       <c r="AA40" s="2"/>
     </row>
     <row r="41" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A41" s="69"/>
-      <c r="B41" s="57"/>
-      <c r="C41" s="57"/>
-      <c r="D41" s="57"/>
-      <c r="E41" s="57"/>
+      <c r="A41" s="58"/>
+      <c r="B41" s="55"/>
+      <c r="C41" s="55"/>
+      <c r="D41" s="55"/>
+      <c r="E41" s="55"/>
       <c r="F41" s="30" t="s">
         <v>67</v>
       </c>
@@ -3379,9 +3383,9 @@
         <v>103</v>
       </c>
       <c r="H41" s="35"/>
-      <c r="I41" s="48"/>
-      <c r="J41" s="60"/>
-      <c r="K41" s="48"/>
+      <c r="I41" s="52"/>
+      <c r="J41" s="49"/>
+      <c r="K41" s="52"/>
       <c r="L41" s="2"/>
       <c r="M41" s="2"/>
       <c r="N41" s="2"/>
@@ -3400,11 +3404,11 @@
       <c r="AA41" s="2"/>
     </row>
     <row r="42" spans="1:27" ht="16.5" customHeight="1">
-      <c r="A42" s="69"/>
-      <c r="B42" s="57"/>
-      <c r="C42" s="57"/>
-      <c r="D42" s="57"/>
-      <c r="E42" s="57"/>
+      <c r="A42" s="58"/>
+      <c r="B42" s="55"/>
+      <c r="C42" s="55"/>
+      <c r="D42" s="55"/>
+      <c r="E42" s="55"/>
       <c r="F42" s="30" t="s">
         <v>70</v>
       </c>
@@ -3414,9 +3418,9 @@
       <c r="H42" s="35" t="s">
         <v>105</v>
       </c>
-      <c r="I42" s="48"/>
-      <c r="J42" s="60"/>
-      <c r="K42" s="48"/>
+      <c r="I42" s="52"/>
+      <c r="J42" s="49"/>
+      <c r="K42" s="52"/>
       <c r="L42" s="2"/>
       <c r="M42" s="2"/>
       <c r="N42" s="2"/>
@@ -3435,19 +3439,19 @@
       <c r="AA42" s="2"/>
     </row>
     <row r="43" spans="1:27" ht="18.75" customHeight="1">
-      <c r="A43" s="70"/>
-      <c r="B43" s="58"/>
-      <c r="C43" s="58"/>
-      <c r="D43" s="58"/>
-      <c r="E43" s="58"/>
+      <c r="A43" s="59"/>
+      <c r="B43" s="56"/>
+      <c r="C43" s="56"/>
+      <c r="D43" s="56"/>
+      <c r="E43" s="56"/>
       <c r="F43" s="30" t="s">
         <v>99</v>
       </c>
       <c r="G43" s="35"/>
       <c r="H43" s="35"/>
-      <c r="I43" s="49"/>
-      <c r="J43" s="61"/>
-      <c r="K43" s="49"/>
+      <c r="I43" s="53"/>
+      <c r="J43" s="50"/>
+      <c r="K43" s="53"/>
       <c r="L43" s="2"/>
       <c r="M43" s="2"/>
       <c r="N43" s="2"/>
@@ -3466,19 +3470,19 @@
       <c r="AA43" s="2"/>
     </row>
     <row r="44" spans="1:27" ht="25.5">
-      <c r="A44" s="68" t="s">
+      <c r="A44" s="57" t="s">
         <v>39</v>
       </c>
-      <c r="B44" s="56" t="s">
+      <c r="B44" s="54" t="s">
         <v>84</v>
       </c>
-      <c r="C44" s="56" t="s">
+      <c r="C44" s="54" t="s">
         <v>106</v>
       </c>
-      <c r="D44" s="56" t="s">
+      <c r="D44" s="54" t="s">
         <v>107</v>
       </c>
-      <c r="E44" s="56" t="s">
+      <c r="E44" s="54" t="s">
         <v>108</v>
       </c>
       <c r="F44" s="30" t="s">
@@ -3490,13 +3494,13 @@
       <c r="H44" s="35" t="s">
         <v>88</v>
       </c>
-      <c r="I44" s="47" t="s">
+      <c r="I44" s="51" t="s">
         <v>26</v>
       </c>
-      <c r="J44" s="59" t="s">
+      <c r="J44" s="48" t="s">
         <v>56</v>
       </c>
-      <c r="K44" s="47" t="s">
+      <c r="K44" s="51" t="s">
         <v>28</v>
       </c>
       <c r="L44" s="2"/>
@@ -3517,11 +3521,11 @@
       <c r="AA44" s="2"/>
     </row>
     <row r="45" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A45" s="69"/>
-      <c r="B45" s="57"/>
-      <c r="C45" s="57"/>
-      <c r="D45" s="57"/>
-      <c r="E45" s="57"/>
+      <c r="A45" s="58"/>
+      <c r="B45" s="55"/>
+      <c r="C45" s="55"/>
+      <c r="D45" s="55"/>
+      <c r="E45" s="55"/>
       <c r="F45" s="30" t="s">
         <v>67</v>
       </c>
@@ -3529,9 +3533,9 @@
         <v>109</v>
       </c>
       <c r="H45" s="35"/>
-      <c r="I45" s="48"/>
-      <c r="J45" s="60"/>
-      <c r="K45" s="48"/>
+      <c r="I45" s="52"/>
+      <c r="J45" s="49"/>
+      <c r="K45" s="52"/>
       <c r="L45" s="2"/>
       <c r="M45" s="2"/>
       <c r="N45" s="2"/>
@@ -3550,11 +3554,11 @@
       <c r="AA45" s="2"/>
     </row>
     <row r="46" spans="1:27" ht="25.5">
-      <c r="A46" s="69"/>
-      <c r="B46" s="57"/>
-      <c r="C46" s="57"/>
-      <c r="D46" s="57"/>
-      <c r="E46" s="57"/>
+      <c r="A46" s="58"/>
+      <c r="B46" s="55"/>
+      <c r="C46" s="55"/>
+      <c r="D46" s="55"/>
+      <c r="E46" s="55"/>
       <c r="F46" s="30" t="s">
         <v>70</v>
       </c>
@@ -3564,9 +3568,9 @@
       <c r="H46" s="35" t="s">
         <v>110</v>
       </c>
-      <c r="I46" s="48"/>
-      <c r="J46" s="60"/>
-      <c r="K46" s="48"/>
+      <c r="I46" s="52"/>
+      <c r="J46" s="49"/>
+      <c r="K46" s="52"/>
       <c r="L46" s="2"/>
       <c r="M46" s="2"/>
       <c r="N46" s="2"/>
@@ -3585,19 +3589,19 @@
       <c r="AA46" s="2"/>
     </row>
     <row r="47" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A47" s="70"/>
-      <c r="B47" s="58"/>
-      <c r="C47" s="58"/>
-      <c r="D47" s="58"/>
-      <c r="E47" s="58"/>
+      <c r="A47" s="59"/>
+      <c r="B47" s="56"/>
+      <c r="C47" s="56"/>
+      <c r="D47" s="56"/>
+      <c r="E47" s="56"/>
       <c r="F47" s="30" t="s">
         <v>99</v>
       </c>
       <c r="G47" s="35"/>
       <c r="H47" s="36"/>
-      <c r="I47" s="49"/>
-      <c r="J47" s="61"/>
-      <c r="K47" s="49"/>
+      <c r="I47" s="53"/>
+      <c r="J47" s="50"/>
+      <c r="K47" s="53"/>
       <c r="L47" s="2"/>
       <c r="M47" s="2"/>
       <c r="N47" s="2"/>
@@ -3616,19 +3620,19 @@
       <c r="AA47" s="2"/>
     </row>
     <row r="48" spans="1:27" ht="25.5">
-      <c r="A48" s="68" t="s">
+      <c r="A48" s="57" t="s">
         <v>40</v>
       </c>
-      <c r="B48" s="56" t="s">
+      <c r="B48" s="54" t="s">
         <v>84</v>
       </c>
-      <c r="C48" s="56" t="s">
+      <c r="C48" s="54" t="s">
         <v>111</v>
       </c>
-      <c r="D48" s="56" t="s">
+      <c r="D48" s="54" t="s">
         <v>112</v>
       </c>
-      <c r="E48" s="56" t="s">
+      <c r="E48" s="54" t="s">
         <v>102</v>
       </c>
       <c r="F48" s="30" t="s">
@@ -3640,13 +3644,13 @@
       <c r="H48" s="35" t="s">
         <v>88</v>
       </c>
-      <c r="I48" s="47" t="s">
+      <c r="I48" s="51" t="s">
         <v>26</v>
       </c>
-      <c r="J48" s="59" t="s">
+      <c r="J48" s="48" t="s">
         <v>56</v>
       </c>
-      <c r="K48" s="47" t="s">
+      <c r="K48" s="51" t="s">
         <v>28</v>
       </c>
       <c r="L48" s="2"/>
@@ -3667,11 +3671,11 @@
       <c r="AA48" s="2"/>
     </row>
     <row r="49" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A49" s="69"/>
-      <c r="B49" s="57"/>
-      <c r="C49" s="57"/>
-      <c r="D49" s="57"/>
-      <c r="E49" s="57"/>
+      <c r="A49" s="58"/>
+      <c r="B49" s="55"/>
+      <c r="C49" s="55"/>
+      <c r="D49" s="55"/>
+      <c r="E49" s="55"/>
       <c r="F49" s="30" t="s">
         <v>67</v>
       </c>
@@ -3679,9 +3683,9 @@
         <v>113</v>
       </c>
       <c r="H49" s="35"/>
-      <c r="I49" s="48"/>
-      <c r="J49" s="60"/>
-      <c r="K49" s="48"/>
+      <c r="I49" s="52"/>
+      <c r="J49" s="49"/>
+      <c r="K49" s="52"/>
       <c r="L49" s="2"/>
       <c r="M49" s="2"/>
       <c r="N49" s="2"/>
@@ -3700,11 +3704,11 @@
       <c r="AA49" s="2"/>
     </row>
     <row r="50" spans="1:27" ht="27" customHeight="1">
-      <c r="A50" s="69"/>
-      <c r="B50" s="57"/>
-      <c r="C50" s="57"/>
-      <c r="D50" s="57"/>
-      <c r="E50" s="57"/>
+      <c r="A50" s="58"/>
+      <c r="B50" s="55"/>
+      <c r="C50" s="55"/>
+      <c r="D50" s="55"/>
+      <c r="E50" s="55"/>
       <c r="F50" s="30" t="s">
         <v>70</v>
       </c>
@@ -3714,9 +3718,9 @@
       <c r="H50" s="35" t="s">
         <v>110</v>
       </c>
-      <c r="I50" s="48"/>
-      <c r="J50" s="60"/>
-      <c r="K50" s="48"/>
+      <c r="I50" s="52"/>
+      <c r="J50" s="49"/>
+      <c r="K50" s="52"/>
       <c r="L50" s="2"/>
       <c r="M50" s="2"/>
       <c r="N50" s="2"/>
@@ -3735,19 +3739,19 @@
       <c r="AA50" s="2"/>
     </row>
     <row r="51" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A51" s="70"/>
-      <c r="B51" s="58"/>
-      <c r="C51" s="58"/>
-      <c r="D51" s="58"/>
-      <c r="E51" s="58"/>
+      <c r="A51" s="59"/>
+      <c r="B51" s="56"/>
+      <c r="C51" s="56"/>
+      <c r="D51" s="56"/>
+      <c r="E51" s="56"/>
       <c r="F51" s="30" t="s">
         <v>99</v>
       </c>
       <c r="G51" s="35"/>
       <c r="H51" s="36"/>
-      <c r="I51" s="49"/>
-      <c r="J51" s="61"/>
-      <c r="K51" s="49"/>
+      <c r="I51" s="53"/>
+      <c r="J51" s="50"/>
+      <c r="K51" s="53"/>
       <c r="L51" s="2"/>
       <c r="M51" s="2"/>
       <c r="N51" s="2"/>
@@ -3766,19 +3770,19 @@
       <c r="AA51" s="2"/>
     </row>
     <row r="52" spans="1:27" ht="25.5">
-      <c r="A52" s="68" t="s">
+      <c r="A52" s="57" t="s">
         <v>41</v>
       </c>
-      <c r="B52" s="56" t="s">
+      <c r="B52" s="54" t="s">
         <v>84</v>
       </c>
-      <c r="C52" s="56" t="s">
+      <c r="C52" s="54" t="s">
         <v>114</v>
       </c>
-      <c r="D52" s="56" t="s">
+      <c r="D52" s="54" t="s">
         <v>129</v>
       </c>
-      <c r="E52" s="56" t="s">
+      <c r="E52" s="54" t="s">
         <v>95</v>
       </c>
       <c r="F52" s="30" t="s">
@@ -3790,13 +3794,13 @@
       <c r="H52" s="35" t="s">
         <v>92</v>
       </c>
-      <c r="I52" s="47" t="s">
+      <c r="I52" s="51" t="s">
         <v>26</v>
       </c>
-      <c r="J52" s="59" t="s">
+      <c r="J52" s="48" t="s">
         <v>56</v>
       </c>
-      <c r="K52" s="47" t="s">
+      <c r="K52" s="51" t="s">
         <v>28</v>
       </c>
       <c r="L52" s="2"/>
@@ -3817,11 +3821,11 @@
       <c r="AA52" s="2"/>
     </row>
     <row r="53" spans="1:27" ht="25.5">
-      <c r="A53" s="69"/>
-      <c r="B53" s="57"/>
-      <c r="C53" s="57"/>
-      <c r="D53" s="57"/>
-      <c r="E53" s="57"/>
+      <c r="A53" s="58"/>
+      <c r="B53" s="55"/>
+      <c r="C53" s="55"/>
+      <c r="D53" s="55"/>
+      <c r="E53" s="55"/>
       <c r="F53" s="30" t="s">
         <v>67</v>
       </c>
@@ -3831,9 +3835,9 @@
       <c r="H53" s="36" t="s">
         <v>116</v>
       </c>
-      <c r="I53" s="48"/>
-      <c r="J53" s="60"/>
-      <c r="K53" s="48"/>
+      <c r="I53" s="52"/>
+      <c r="J53" s="49"/>
+      <c r="K53" s="52"/>
       <c r="L53" s="2"/>
       <c r="M53" s="2"/>
       <c r="N53" s="2"/>
@@ -3852,17 +3856,17 @@
       <c r="AA53" s="2"/>
     </row>
     <row r="54" spans="1:27" ht="13.5" customHeight="1">
-      <c r="A54" s="69"/>
-      <c r="B54" s="57"/>
-      <c r="C54" s="57"/>
-      <c r="D54" s="57"/>
-      <c r="E54" s="57"/>
+      <c r="A54" s="58"/>
+      <c r="B54" s="55"/>
+      <c r="C54" s="55"/>
+      <c r="D54" s="55"/>
+      <c r="E54" s="55"/>
       <c r="F54" s="30"/>
       <c r="G54" s="43"/>
       <c r="H54" s="43"/>
-      <c r="I54" s="48"/>
-      <c r="J54" s="60"/>
-      <c r="K54" s="48"/>
+      <c r="I54" s="52"/>
+      <c r="J54" s="49"/>
+      <c r="K54" s="52"/>
       <c r="L54" s="2"/>
       <c r="M54" s="2"/>
       <c r="N54" s="2"/>
@@ -3881,17 +3885,17 @@
       <c r="AA54" s="2"/>
     </row>
     <row r="55" spans="1:27" ht="15" customHeight="1">
-      <c r="A55" s="70"/>
-      <c r="B55" s="58"/>
-      <c r="C55" s="58"/>
-      <c r="D55" s="58"/>
-      <c r="E55" s="58"/>
+      <c r="A55" s="59"/>
+      <c r="B55" s="56"/>
+      <c r="C55" s="56"/>
+      <c r="D55" s="56"/>
+      <c r="E55" s="56"/>
       <c r="F55" s="30"/>
       <c r="G55" s="43"/>
       <c r="H55" s="43"/>
-      <c r="I55" s="49"/>
-      <c r="J55" s="61"/>
-      <c r="K55" s="49"/>
+      <c r="I55" s="53"/>
+      <c r="J55" s="50"/>
+      <c r="K55" s="53"/>
       <c r="L55" s="2"/>
       <c r="M55" s="2"/>
       <c r="N55" s="2"/>
@@ -3910,19 +3914,19 @@
       <c r="AA55" s="2"/>
     </row>
     <row r="56" spans="1:27" ht="25.5">
-      <c r="A56" s="68" t="s">
+      <c r="A56" s="57" t="s">
         <v>42</v>
       </c>
-      <c r="B56" s="56" t="s">
+      <c r="B56" s="54" t="s">
         <v>84</v>
       </c>
-      <c r="C56" s="56" t="s">
+      <c r="C56" s="54" t="s">
         <v>117</v>
       </c>
-      <c r="D56" s="56" t="s">
+      <c r="D56" s="54" t="s">
         <v>118</v>
       </c>
-      <c r="E56" s="56" t="s">
+      <c r="E56" s="54" t="s">
         <v>95</v>
       </c>
       <c r="F56" s="30" t="s">
@@ -3934,13 +3938,13 @@
       <c r="H56" s="35" t="s">
         <v>92</v>
       </c>
-      <c r="I56" s="47" t="s">
+      <c r="I56" s="51" t="s">
         <v>26</v>
       </c>
-      <c r="J56" s="59" t="s">
+      <c r="J56" s="48" t="s">
         <v>56</v>
       </c>
-      <c r="K56" s="47" t="s">
+      <c r="K56" s="51" t="s">
         <v>28</v>
       </c>
       <c r="L56" s="2"/>
@@ -3961,11 +3965,11 @@
       <c r="AA56" s="2"/>
     </row>
     <row r="57" spans="1:27" ht="17.25" customHeight="1">
-      <c r="A57" s="69"/>
-      <c r="B57" s="57"/>
-      <c r="C57" s="57"/>
-      <c r="D57" s="57"/>
-      <c r="E57" s="57"/>
+      <c r="A57" s="58"/>
+      <c r="B57" s="55"/>
+      <c r="C57" s="55"/>
+      <c r="D57" s="55"/>
+      <c r="E57" s="55"/>
       <c r="F57" s="30" t="s">
         <v>67</v>
       </c>
@@ -3975,9 +3979,9 @@
       <c r="H57" s="36" t="s">
         <v>120</v>
       </c>
-      <c r="I57" s="48"/>
-      <c r="J57" s="60"/>
-      <c r="K57" s="48"/>
+      <c r="I57" s="52"/>
+      <c r="J57" s="49"/>
+      <c r="K57" s="52"/>
       <c r="L57" s="2"/>
       <c r="M57" s="2"/>
       <c r="N57" s="2"/>
@@ -3996,11 +4000,11 @@
       <c r="AA57" s="2"/>
     </row>
     <row r="58" spans="1:27" ht="25.5">
-      <c r="A58" s="69"/>
-      <c r="B58" s="57"/>
-      <c r="C58" s="57"/>
-      <c r="D58" s="57"/>
-      <c r="E58" s="57"/>
+      <c r="A58" s="58"/>
+      <c r="B58" s="55"/>
+      <c r="C58" s="55"/>
+      <c r="D58" s="55"/>
+      <c r="E58" s="55"/>
       <c r="F58" s="30" t="s">
         <v>70</v>
       </c>
@@ -4010,9 +4014,9 @@
       <c r="H58" s="36" t="s">
         <v>122</v>
       </c>
-      <c r="I58" s="48"/>
-      <c r="J58" s="60"/>
-      <c r="K58" s="48"/>
+      <c r="I58" s="52"/>
+      <c r="J58" s="49"/>
+      <c r="K58" s="52"/>
       <c r="L58" s="2"/>
       <c r="M58" s="2"/>
       <c r="N58" s="2"/>
@@ -4031,11 +4035,11 @@
       <c r="AA58" s="2"/>
     </row>
     <row r="59" spans="1:27" ht="25.5">
-      <c r="A59" s="70"/>
-      <c r="B59" s="58"/>
-      <c r="C59" s="58"/>
-      <c r="D59" s="58"/>
-      <c r="E59" s="58"/>
+      <c r="A59" s="59"/>
+      <c r="B59" s="56"/>
+      <c r="C59" s="56"/>
+      <c r="D59" s="56"/>
+      <c r="E59" s="56"/>
       <c r="F59" s="30" t="s">
         <v>99</v>
       </c>
@@ -4045,9 +4049,9 @@
       <c r="H59" s="36" t="s">
         <v>123</v>
       </c>
-      <c r="I59" s="49"/>
-      <c r="J59" s="61"/>
-      <c r="K59" s="49"/>
+      <c r="I59" s="53"/>
+      <c r="J59" s="50"/>
+      <c r="K59" s="53"/>
       <c r="L59" s="2"/>
       <c r="M59" s="2"/>
       <c r="N59" s="2"/>
@@ -4066,19 +4070,19 @@
       <c r="AA59" s="2"/>
     </row>
     <row r="60" spans="1:27" ht="25.5">
-      <c r="A60" s="68" t="s">
+      <c r="A60" s="57" t="s">
         <v>43</v>
       </c>
-      <c r="B60" s="56" t="s">
+      <c r="B60" s="54" t="s">
         <v>84</v>
       </c>
-      <c r="C60" s="56" t="s">
+      <c r="C60" s="54" t="s">
         <v>124</v>
       </c>
-      <c r="D60" s="56" t="s">
+      <c r="D60" s="54" t="s">
         <v>125</v>
       </c>
-      <c r="E60" s="56" t="s">
+      <c r="E60" s="54" t="s">
         <v>102</v>
       </c>
       <c r="F60" s="30" t="s">
@@ -4090,13 +4094,13 @@
       <c r="H60" s="35" t="s">
         <v>92</v>
       </c>
-      <c r="I60" s="47" t="s">
+      <c r="I60" s="51" t="s">
         <v>26</v>
       </c>
-      <c r="J60" s="59" t="s">
+      <c r="J60" s="48" t="s">
         <v>56</v>
       </c>
-      <c r="K60" s="47" t="s">
+      <c r="K60" s="51" t="s">
         <v>28</v>
       </c>
       <c r="L60" s="2"/>
@@ -4117,11 +4121,11 @@
       <c r="AA60" s="2"/>
     </row>
     <row r="61" spans="1:27" ht="25.5">
-      <c r="A61" s="69"/>
-      <c r="B61" s="57"/>
-      <c r="C61" s="57"/>
-      <c r="D61" s="57"/>
-      <c r="E61" s="57"/>
+      <c r="A61" s="58"/>
+      <c r="B61" s="55"/>
+      <c r="C61" s="55"/>
+      <c r="D61" s="55"/>
+      <c r="E61" s="55"/>
       <c r="F61" s="30" t="s">
         <v>67</v>
       </c>
@@ -4131,9 +4135,9 @@
       <c r="H61" s="36" t="s">
         <v>120</v>
       </c>
-      <c r="I61" s="48"/>
-      <c r="J61" s="60"/>
-      <c r="K61" s="48"/>
+      <c r="I61" s="52"/>
+      <c r="J61" s="49"/>
+      <c r="K61" s="52"/>
       <c r="L61" s="2"/>
       <c r="M61" s="2"/>
       <c r="N61" s="2"/>
@@ -4152,11 +4156,11 @@
       <c r="AA61" s="2"/>
     </row>
     <row r="62" spans="1:27" ht="25.5">
-      <c r="A62" s="69"/>
-      <c r="B62" s="57"/>
-      <c r="C62" s="57"/>
-      <c r="D62" s="57"/>
-      <c r="E62" s="57"/>
+      <c r="A62" s="58"/>
+      <c r="B62" s="55"/>
+      <c r="C62" s="55"/>
+      <c r="D62" s="55"/>
+      <c r="E62" s="55"/>
       <c r="F62" s="30" t="s">
         <v>70</v>
       </c>
@@ -4166,9 +4170,9 @@
       <c r="H62" s="36" t="s">
         <v>122</v>
       </c>
-      <c r="I62" s="48"/>
-      <c r="J62" s="60"/>
-      <c r="K62" s="48"/>
+      <c r="I62" s="52"/>
+      <c r="J62" s="49"/>
+      <c r="K62" s="52"/>
       <c r="L62" s="2"/>
       <c r="M62" s="2"/>
       <c r="N62" s="2"/>
@@ -4187,11 +4191,11 @@
       <c r="AA62" s="2"/>
     </row>
     <row r="63" spans="1:27" ht="25.5">
-      <c r="A63" s="70"/>
-      <c r="B63" s="58"/>
-      <c r="C63" s="58"/>
-      <c r="D63" s="58"/>
-      <c r="E63" s="58"/>
+      <c r="A63" s="59"/>
+      <c r="B63" s="56"/>
+      <c r="C63" s="56"/>
+      <c r="D63" s="56"/>
+      <c r="E63" s="56"/>
       <c r="F63" s="30" t="s">
         <v>99</v>
       </c>
@@ -4201,9 +4205,9 @@
       <c r="H63" s="35" t="s">
         <v>128</v>
       </c>
-      <c r="I63" s="49"/>
-      <c r="J63" s="61"/>
-      <c r="K63" s="49"/>
+      <c r="I63" s="53"/>
+      <c r="J63" s="50"/>
+      <c r="K63" s="53"/>
       <c r="L63" s="2"/>
       <c r="M63" s="2"/>
       <c r="N63" s="2"/>
@@ -4222,19 +4226,19 @@
       <c r="AA63" s="2"/>
     </row>
     <row r="64" spans="1:27" ht="25.5">
-      <c r="A64" s="71" t="s">
+      <c r="A64" s="63" t="s">
         <v>44</v>
       </c>
-      <c r="B64" s="56" t="s">
+      <c r="B64" s="54" t="s">
         <v>49</v>
       </c>
-      <c r="C64" s="62" t="s">
+      <c r="C64" s="60" t="s">
         <v>130</v>
       </c>
-      <c r="D64" s="56" t="s">
+      <c r="D64" s="54" t="s">
         <v>131</v>
       </c>
-      <c r="E64" s="56" t="s">
+      <c r="E64" s="54" t="s">
         <v>83</v>
       </c>
       <c r="F64" s="30" t="s">
@@ -4246,13 +4250,13 @@
       <c r="H64" s="35" t="s">
         <v>133</v>
       </c>
-      <c r="I64" s="47" t="s">
+      <c r="I64" s="51" t="s">
         <v>26</v>
       </c>
-      <c r="J64" s="59" t="s">
+      <c r="J64" s="48" t="s">
         <v>56</v>
       </c>
-      <c r="K64" s="47" t="s">
+      <c r="K64" s="51" t="s">
         <v>28</v>
       </c>
       <c r="L64" s="2"/>
@@ -4273,17 +4277,17 @@
       <c r="AA64" s="2"/>
     </row>
     <row r="65" spans="1:27">
-      <c r="A65" s="72"/>
-      <c r="B65" s="57"/>
-      <c r="C65" s="74"/>
-      <c r="D65" s="57"/>
-      <c r="E65" s="57"/>
+      <c r="A65" s="64"/>
+      <c r="B65" s="55"/>
+      <c r="C65" s="61"/>
+      <c r="D65" s="55"/>
+      <c r="E65" s="55"/>
       <c r="F65" s="30"/>
       <c r="G65" s="35"/>
       <c r="H65" s="35"/>
-      <c r="I65" s="48"/>
-      <c r="J65" s="60"/>
-      <c r="K65" s="48"/>
+      <c r="I65" s="52"/>
+      <c r="J65" s="49"/>
+      <c r="K65" s="52"/>
       <c r="L65" s="2"/>
       <c r="M65" s="2"/>
       <c r="N65" s="2"/>
@@ -4302,17 +4306,17 @@
       <c r="AA65" s="2"/>
     </row>
     <row r="66" spans="1:27">
-      <c r="A66" s="72"/>
-      <c r="B66" s="57"/>
-      <c r="C66" s="74"/>
-      <c r="D66" s="57"/>
-      <c r="E66" s="57"/>
+      <c r="A66" s="64"/>
+      <c r="B66" s="55"/>
+      <c r="C66" s="61"/>
+      <c r="D66" s="55"/>
+      <c r="E66" s="55"/>
       <c r="F66" s="30"/>
       <c r="G66" s="35"/>
       <c r="H66" s="35"/>
-      <c r="I66" s="48"/>
-      <c r="J66" s="60"/>
-      <c r="K66" s="48"/>
+      <c r="I66" s="52"/>
+      <c r="J66" s="49"/>
+      <c r="K66" s="52"/>
       <c r="L66" s="2"/>
       <c r="M66" s="2"/>
       <c r="N66" s="2"/>
@@ -4331,17 +4335,17 @@
       <c r="AA66" s="2"/>
     </row>
     <row r="67" spans="1:27">
-      <c r="A67" s="73"/>
-      <c r="B67" s="58"/>
-      <c r="C67" s="75"/>
-      <c r="D67" s="58"/>
-      <c r="E67" s="58"/>
+      <c r="A67" s="65"/>
+      <c r="B67" s="56"/>
+      <c r="C67" s="62"/>
+      <c r="D67" s="56"/>
+      <c r="E67" s="56"/>
       <c r="F67" s="30"/>
       <c r="G67" s="35"/>
       <c r="H67" s="35"/>
-      <c r="I67" s="49"/>
-      <c r="J67" s="61"/>
-      <c r="K67" s="49"/>
+      <c r="I67" s="53"/>
+      <c r="J67" s="50"/>
+      <c r="K67" s="53"/>
       <c r="L67" s="2"/>
       <c r="M67" s="2"/>
       <c r="N67" s="2"/>
@@ -4360,19 +4364,19 @@
       <c r="AA67" s="2"/>
     </row>
     <row r="68" spans="1:27" ht="25.5">
-      <c r="A68" s="71" t="s">
+      <c r="A68" s="63" t="s">
         <v>45</v>
       </c>
-      <c r="B68" s="56" t="s">
+      <c r="B68" s="54" t="s">
         <v>49</v>
       </c>
-      <c r="C68" s="62" t="s">
+      <c r="C68" s="60" t="s">
         <v>134</v>
       </c>
-      <c r="D68" s="56" t="s">
+      <c r="D68" s="54" t="s">
         <v>135</v>
       </c>
-      <c r="E68" s="56" t="s">
+      <c r="E68" s="54" t="s">
         <v>83</v>
       </c>
       <c r="F68" s="30" t="s">
@@ -4384,13 +4388,13 @@
       <c r="H68" s="35" t="s">
         <v>137</v>
       </c>
-      <c r="I68" s="47" t="s">
+      <c r="I68" s="51" t="s">
         <v>26</v>
       </c>
-      <c r="J68" s="59" t="s">
+      <c r="J68" s="48" t="s">
         <v>56</v>
       </c>
-      <c r="K68" s="47" t="s">
+      <c r="K68" s="51" t="s">
         <v>28</v>
       </c>
       <c r="L68" s="2"/>
@@ -4411,17 +4415,17 @@
       <c r="AA68" s="2"/>
     </row>
     <row r="69" spans="1:27">
-      <c r="A69" s="72"/>
-      <c r="B69" s="57"/>
-      <c r="C69" s="74"/>
-      <c r="D69" s="57"/>
-      <c r="E69" s="57"/>
+      <c r="A69" s="64"/>
+      <c r="B69" s="55"/>
+      <c r="C69" s="61"/>
+      <c r="D69" s="55"/>
+      <c r="E69" s="55"/>
       <c r="F69" s="30"/>
       <c r="G69" s="35"/>
       <c r="H69" s="35"/>
-      <c r="I69" s="48"/>
-      <c r="J69" s="60"/>
-      <c r="K69" s="48"/>
+      <c r="I69" s="52"/>
+      <c r="J69" s="49"/>
+      <c r="K69" s="52"/>
       <c r="L69" s="2"/>
       <c r="M69" s="2"/>
       <c r="N69" s="2"/>
@@ -4440,17 +4444,17 @@
       <c r="AA69" s="2"/>
     </row>
     <row r="70" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A70" s="72"/>
-      <c r="B70" s="57"/>
-      <c r="C70" s="74"/>
-      <c r="D70" s="57"/>
-      <c r="E70" s="57"/>
+      <c r="A70" s="64"/>
+      <c r="B70" s="55"/>
+      <c r="C70" s="61"/>
+      <c r="D70" s="55"/>
+      <c r="E70" s="55"/>
       <c r="F70" s="30"/>
       <c r="G70" s="35"/>
       <c r="H70" s="35"/>
-      <c r="I70" s="48"/>
-      <c r="J70" s="60"/>
-      <c r="K70" s="48"/>
+      <c r="I70" s="52"/>
+      <c r="J70" s="49"/>
+      <c r="K70" s="52"/>
       <c r="L70" s="2"/>
       <c r="M70" s="2"/>
       <c r="N70" s="2"/>
@@ -4469,17 +4473,17 @@
       <c r="AA70" s="2"/>
     </row>
     <row r="71" spans="1:27">
-      <c r="A71" s="73"/>
-      <c r="B71" s="58"/>
-      <c r="C71" s="75"/>
-      <c r="D71" s="58"/>
-      <c r="E71" s="58"/>
+      <c r="A71" s="65"/>
+      <c r="B71" s="56"/>
+      <c r="C71" s="62"/>
+      <c r="D71" s="56"/>
+      <c r="E71" s="56"/>
       <c r="F71" s="30"/>
       <c r="G71" s="35"/>
       <c r="H71" s="35"/>
-      <c r="I71" s="49"/>
-      <c r="J71" s="61"/>
-      <c r="K71" s="49"/>
+      <c r="I71" s="53"/>
+      <c r="J71" s="50"/>
+      <c r="K71" s="53"/>
       <c r="L71" s="2"/>
       <c r="M71" s="2"/>
       <c r="N71" s="2"/>
@@ -4498,19 +4502,19 @@
       <c r="AA71" s="2"/>
     </row>
     <row r="72" spans="1:27">
-      <c r="A72" s="65" t="s">
+      <c r="A72" s="80" t="s">
         <v>46</v>
       </c>
-      <c r="B72" s="62" t="s">
+      <c r="B72" s="60" t="s">
         <v>138</v>
       </c>
-      <c r="C72" s="62" t="s">
+      <c r="C72" s="60" t="s">
         <v>139</v>
       </c>
-      <c r="D72" s="62" t="s">
+      <c r="D72" s="60" t="s">
         <v>140</v>
       </c>
-      <c r="E72" s="62" t="s">
+      <c r="E72" s="60" t="s">
         <v>141</v>
       </c>
       <c r="F72" s="44" t="s">
@@ -4522,13 +4526,13 @@
       <c r="H72" s="45" t="s">
         <v>143</v>
       </c>
-      <c r="I72" s="47" t="s">
+      <c r="I72" s="51" t="s">
         <v>26</v>
       </c>
-      <c r="J72" s="59" t="s">
+      <c r="J72" s="48" t="s">
         <v>56</v>
       </c>
-      <c r="K72" s="47" t="s">
+      <c r="K72" s="51" t="s">
         <v>28</v>
       </c>
       <c r="L72" s="2"/>
@@ -4549,11 +4553,11 @@
       <c r="AA72" s="2"/>
     </row>
     <row r="73" spans="1:27">
-      <c r="A73" s="66"/>
-      <c r="B73" s="63"/>
-      <c r="C73" s="63"/>
-      <c r="D73" s="63"/>
-      <c r="E73" s="63"/>
+      <c r="A73" s="81"/>
+      <c r="B73" s="83"/>
+      <c r="C73" s="83"/>
+      <c r="D73" s="83"/>
+      <c r="E73" s="83"/>
       <c r="F73" s="44" t="s">
         <v>67</v>
       </c>
@@ -4561,9 +4565,9 @@
         <v>144</v>
       </c>
       <c r="H73" s="45"/>
-      <c r="I73" s="48"/>
-      <c r="J73" s="60"/>
-      <c r="K73" s="48"/>
+      <c r="I73" s="52"/>
+      <c r="J73" s="49"/>
+      <c r="K73" s="52"/>
       <c r="L73" s="2"/>
       <c r="M73" s="2"/>
       <c r="N73" s="2"/>
@@ -4582,11 +4586,11 @@
       <c r="AA73" s="2"/>
     </row>
     <row r="74" spans="1:27">
-      <c r="A74" s="66"/>
-      <c r="B74" s="63"/>
-      <c r="C74" s="63"/>
-      <c r="D74" s="63"/>
-      <c r="E74" s="63"/>
+      <c r="A74" s="81"/>
+      <c r="B74" s="83"/>
+      <c r="C74" s="83"/>
+      <c r="D74" s="83"/>
+      <c r="E74" s="83"/>
       <c r="F74" s="44" t="s">
         <v>70</v>
       </c>
@@ -4596,9 +4600,9 @@
       <c r="H74" s="45" t="s">
         <v>146</v>
       </c>
-      <c r="I74" s="48"/>
-      <c r="J74" s="60"/>
-      <c r="K74" s="48"/>
+      <c r="I74" s="52"/>
+      <c r="J74" s="49"/>
+      <c r="K74" s="52"/>
       <c r="L74" s="2"/>
       <c r="M74" s="2"/>
       <c r="N74" s="2"/>
@@ -4617,11 +4621,11 @@
       <c r="AA74" s="2"/>
     </row>
     <row r="75" spans="1:27">
-      <c r="A75" s="67"/>
-      <c r="B75" s="64"/>
-      <c r="C75" s="64"/>
-      <c r="D75" s="64"/>
-      <c r="E75" s="64"/>
+      <c r="A75" s="82"/>
+      <c r="B75" s="84"/>
+      <c r="C75" s="84"/>
+      <c r="D75" s="84"/>
+      <c r="E75" s="84"/>
       <c r="F75" s="44" t="s">
         <v>99</v>
       </c>
@@ -4631,9 +4635,9 @@
       <c r="H75" s="45" t="s">
         <v>163</v>
       </c>
-      <c r="I75" s="49"/>
-      <c r="J75" s="61"/>
-      <c r="K75" s="49"/>
+      <c r="I75" s="53"/>
+      <c r="J75" s="50"/>
+      <c r="K75" s="53"/>
       <c r="L75" s="2"/>
       <c r="M75" s="2"/>
       <c r="N75" s="2"/>
@@ -4652,19 +4656,19 @@
       <c r="AA75" s="2"/>
     </row>
     <row r="76" spans="1:27">
-      <c r="A76" s="65" t="s">
+      <c r="A76" s="80" t="s">
         <v>47</v>
       </c>
-      <c r="B76" s="62" t="s">
+      <c r="B76" s="60" t="s">
         <v>138</v>
       </c>
-      <c r="C76" s="62" t="s">
+      <c r="C76" s="60" t="s">
         <v>148</v>
       </c>
-      <c r="D76" s="62" t="s">
+      <c r="D76" s="60" t="s">
         <v>149</v>
       </c>
-      <c r="E76" s="62" t="s">
+      <c r="E76" s="60" t="s">
         <v>141</v>
       </c>
       <c r="F76" s="44" t="s">
@@ -4676,13 +4680,13 @@
       <c r="H76" s="45" t="s">
         <v>143</v>
       </c>
-      <c r="I76" s="47" t="s">
+      <c r="I76" s="51" t="s">
         <v>26</v>
       </c>
-      <c r="J76" s="59" t="s">
+      <c r="J76" s="48" t="s">
         <v>56</v>
       </c>
-      <c r="K76" s="47" t="s">
+      <c r="K76" s="51" t="s">
         <v>28</v>
       </c>
       <c r="L76" s="2"/>
@@ -4703,11 +4707,11 @@
       <c r="AA76" s="2"/>
     </row>
     <row r="77" spans="1:27">
-      <c r="A77" s="66"/>
-      <c r="B77" s="63"/>
-      <c r="C77" s="63"/>
-      <c r="D77" s="63"/>
-      <c r="E77" s="63"/>
+      <c r="A77" s="81"/>
+      <c r="B77" s="83"/>
+      <c r="C77" s="83"/>
+      <c r="D77" s="83"/>
+      <c r="E77" s="83"/>
       <c r="F77" s="44" t="s">
         <v>67</v>
       </c>
@@ -4717,9 +4721,9 @@
       <c r="H77" s="45" t="s">
         <v>146</v>
       </c>
-      <c r="I77" s="48"/>
-      <c r="J77" s="60"/>
-      <c r="K77" s="48"/>
+      <c r="I77" s="52"/>
+      <c r="J77" s="49"/>
+      <c r="K77" s="52"/>
       <c r="L77" s="2"/>
       <c r="M77" s="2"/>
       <c r="N77" s="2"/>
@@ -4738,11 +4742,11 @@
       <c r="AA77" s="2"/>
     </row>
     <row r="78" spans="1:27">
-      <c r="A78" s="66"/>
-      <c r="B78" s="63"/>
-      <c r="C78" s="63"/>
-      <c r="D78" s="63"/>
-      <c r="E78" s="63"/>
+      <c r="A78" s="81"/>
+      <c r="B78" s="83"/>
+      <c r="C78" s="83"/>
+      <c r="D78" s="83"/>
+      <c r="E78" s="83"/>
       <c r="F78" s="44" t="s">
         <v>70</v>
       </c>
@@ -4752,9 +4756,9 @@
       <c r="H78" s="45" t="s">
         <v>151</v>
       </c>
-      <c r="I78" s="48"/>
-      <c r="J78" s="60"/>
-      <c r="K78" s="48"/>
+      <c r="I78" s="52"/>
+      <c r="J78" s="49"/>
+      <c r="K78" s="52"/>
       <c r="L78" s="2"/>
       <c r="M78" s="2"/>
       <c r="N78" s="2"/>
@@ -4773,19 +4777,19 @@
       <c r="AA78" s="2"/>
     </row>
     <row r="79" spans="1:27">
-      <c r="A79" s="67"/>
-      <c r="B79" s="64"/>
-      <c r="C79" s="64"/>
-      <c r="D79" s="64"/>
-      <c r="E79" s="64"/>
+      <c r="A79" s="82"/>
+      <c r="B79" s="84"/>
+      <c r="C79" s="84"/>
+      <c r="D79" s="84"/>
+      <c r="E79" s="84"/>
       <c r="F79" s="44" t="s">
         <v>99</v>
       </c>
       <c r="G79" s="45"/>
       <c r="H79" s="45"/>
-      <c r="I79" s="49"/>
-      <c r="J79" s="61"/>
-      <c r="K79" s="49"/>
+      <c r="I79" s="53"/>
+      <c r="J79" s="50"/>
+      <c r="K79" s="53"/>
       <c r="L79" s="2"/>
       <c r="M79" s="2"/>
       <c r="N79" s="2"/>
@@ -4804,19 +4808,19 @@
       <c r="AA79" s="2"/>
     </row>
     <row r="80" spans="1:27">
-      <c r="A80" s="65" t="s">
+      <c r="A80" s="80" t="s">
         <v>48</v>
       </c>
-      <c r="B80" s="62" t="s">
+      <c r="B80" s="60" t="s">
         <v>138</v>
       </c>
-      <c r="C80" s="62" t="s">
+      <c r="C80" s="60" t="s">
         <v>152</v>
       </c>
-      <c r="D80" s="62" t="s">
+      <c r="D80" s="60" t="s">
         <v>153</v>
       </c>
-      <c r="E80" s="62" t="s">
+      <c r="E80" s="60" t="s">
         <v>141</v>
       </c>
       <c r="F80" s="44" t="s">
@@ -4828,13 +4832,13 @@
       <c r="H80" s="45" t="s">
         <v>143</v>
       </c>
-      <c r="I80" s="47" t="s">
+      <c r="I80" s="51" t="s">
         <v>26</v>
       </c>
-      <c r="J80" s="59" t="s">
+      <c r="J80" s="48" t="s">
         <v>56</v>
       </c>
-      <c r="K80" s="47" t="s">
+      <c r="K80" s="51" t="s">
         <v>28</v>
       </c>
       <c r="L80" s="2"/>
@@ -4855,11 +4859,11 @@
       <c r="AA80" s="2"/>
     </row>
     <row r="81" spans="1:27">
-      <c r="A81" s="66"/>
-      <c r="B81" s="63"/>
-      <c r="C81" s="63"/>
-      <c r="D81" s="63"/>
-      <c r="E81" s="63"/>
+      <c r="A81" s="81"/>
+      <c r="B81" s="83"/>
+      <c r="C81" s="83"/>
+      <c r="D81" s="83"/>
+      <c r="E81" s="83"/>
       <c r="F81" s="44" t="s">
         <v>67</v>
       </c>
@@ -4867,9 +4871,9 @@
         <v>154</v>
       </c>
       <c r="H81" s="45"/>
-      <c r="I81" s="48"/>
-      <c r="J81" s="60"/>
-      <c r="K81" s="48"/>
+      <c r="I81" s="52"/>
+      <c r="J81" s="49"/>
+      <c r="K81" s="52"/>
       <c r="L81" s="2"/>
       <c r="M81" s="2"/>
       <c r="N81" s="2"/>
@@ -4888,11 +4892,11 @@
       <c r="AA81" s="2"/>
     </row>
     <row r="82" spans="1:27">
-      <c r="A82" s="66"/>
-      <c r="B82" s="63"/>
-      <c r="C82" s="63"/>
-      <c r="D82" s="63"/>
-      <c r="E82" s="63"/>
+      <c r="A82" s="81"/>
+      <c r="B82" s="83"/>
+      <c r="C82" s="83"/>
+      <c r="D82" s="83"/>
+      <c r="E82" s="83"/>
       <c r="F82" s="44" t="s">
         <v>70</v>
       </c>
@@ -4902,9 +4906,9 @@
       <c r="H82" s="45" t="s">
         <v>146</v>
       </c>
-      <c r="I82" s="48"/>
-      <c r="J82" s="60"/>
-      <c r="K82" s="48"/>
+      <c r="I82" s="52"/>
+      <c r="J82" s="49"/>
+      <c r="K82" s="52"/>
       <c r="L82" s="2"/>
       <c r="M82" s="2"/>
       <c r="N82" s="2"/>
@@ -4923,11 +4927,11 @@
       <c r="AA82" s="2"/>
     </row>
     <row r="83" spans="1:27">
-      <c r="A83" s="67"/>
-      <c r="B83" s="64"/>
-      <c r="C83" s="64"/>
-      <c r="D83" s="64"/>
-      <c r="E83" s="64"/>
+      <c r="A83" s="82"/>
+      <c r="B83" s="84"/>
+      <c r="C83" s="84"/>
+      <c r="D83" s="84"/>
+      <c r="E83" s="84"/>
       <c r="F83" s="44" t="s">
         <v>99</v>
       </c>
@@ -4937,9 +4941,9 @@
       <c r="H83" s="45" t="s">
         <v>156</v>
       </c>
-      <c r="I83" s="49"/>
-      <c r="J83" s="61"/>
-      <c r="K83" s="49"/>
+      <c r="I83" s="53"/>
+      <c r="J83" s="50"/>
+      <c r="K83" s="53"/>
       <c r="L83" s="2"/>
       <c r="M83" s="2"/>
       <c r="N83" s="2"/>
@@ -4958,19 +4962,19 @@
       <c r="AA83" s="2"/>
     </row>
     <row r="84" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A84" s="65" t="s">
+      <c r="A84" s="80" t="s">
         <v>162</v>
       </c>
-      <c r="B84" s="62" t="s">
+      <c r="B84" s="60" t="s">
         <v>138</v>
       </c>
-      <c r="C84" s="62" t="s">
+      <c r="C84" s="60" t="s">
         <v>157</v>
       </c>
-      <c r="D84" s="62" t="s">
+      <c r="D84" s="60" t="s">
         <v>158</v>
       </c>
-      <c r="E84" s="62" t="s">
+      <c r="E84" s="60" t="s">
         <v>141</v>
       </c>
       <c r="F84" s="44" t="s">
@@ -4982,13 +4986,13 @@
       <c r="H84" s="45" t="s">
         <v>143</v>
       </c>
-      <c r="I84" s="47" t="s">
+      <c r="I84" s="51" t="s">
         <v>26</v>
       </c>
-      <c r="J84" s="59" t="s">
+      <c r="J84" s="48" t="s">
         <v>56</v>
       </c>
-      <c r="K84" s="47" t="s">
+      <c r="K84" s="51" t="s">
         <v>28</v>
       </c>
       <c r="L84" s="2"/>
@@ -5009,11 +5013,11 @@
       <c r="AA84" s="2"/>
     </row>
     <row r="85" spans="1:27" ht="24" customHeight="1">
-      <c r="A85" s="66"/>
-      <c r="B85" s="63"/>
-      <c r="C85" s="63"/>
-      <c r="D85" s="63"/>
-      <c r="E85" s="63"/>
+      <c r="A85" s="81"/>
+      <c r="B85" s="83"/>
+      <c r="C85" s="83"/>
+      <c r="D85" s="83"/>
+      <c r="E85" s="83"/>
       <c r="F85" s="44" t="s">
         <v>67</v>
       </c>
@@ -5023,9 +5027,9 @@
       <c r="H85" s="45" t="s">
         <v>160</v>
       </c>
-      <c r="I85" s="48"/>
-      <c r="J85" s="60"/>
-      <c r="K85" s="48"/>
+      <c r="I85" s="52"/>
+      <c r="J85" s="49"/>
+      <c r="K85" s="52"/>
       <c r="L85" s="2"/>
       <c r="M85" s="2"/>
       <c r="N85" s="2"/>
@@ -5044,11 +5048,11 @@
       <c r="AA85" s="2"/>
     </row>
     <row r="86" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A86" s="66"/>
-      <c r="B86" s="63"/>
-      <c r="C86" s="63"/>
-      <c r="D86" s="63"/>
-      <c r="E86" s="63"/>
+      <c r="A86" s="81"/>
+      <c r="B86" s="83"/>
+      <c r="C86" s="83"/>
+      <c r="D86" s="83"/>
+      <c r="E86" s="83"/>
       <c r="F86" s="44" t="s">
         <v>70</v>
       </c>
@@ -5058,9 +5062,9 @@
       <c r="H86" s="45" t="s">
         <v>161</v>
       </c>
-      <c r="I86" s="48"/>
-      <c r="J86" s="60"/>
-      <c r="K86" s="48"/>
+      <c r="I86" s="52"/>
+      <c r="J86" s="49"/>
+      <c r="K86" s="52"/>
       <c r="L86" s="2"/>
       <c r="M86" s="2"/>
       <c r="N86" s="2"/>
@@ -5079,17 +5083,17 @@
       <c r="AA86" s="2"/>
     </row>
     <row r="87" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A87" s="67"/>
-      <c r="B87" s="64"/>
-      <c r="C87" s="64"/>
-      <c r="D87" s="64"/>
-      <c r="E87" s="64"/>
+      <c r="A87" s="82"/>
+      <c r="B87" s="84"/>
+      <c r="C87" s="84"/>
+      <c r="D87" s="84"/>
+      <c r="E87" s="84"/>
       <c r="F87" s="44"/>
       <c r="G87" s="45"/>
       <c r="H87" s="45"/>
-      <c r="I87" s="49"/>
-      <c r="J87" s="61"/>
-      <c r="K87" s="49"/>
+      <c r="I87" s="53"/>
+      <c r="J87" s="50"/>
+      <c r="K87" s="53"/>
       <c r="L87" s="2"/>
       <c r="M87" s="2"/>
       <c r="N87" s="2"/>
@@ -5108,19 +5112,19 @@
       <c r="AA87" s="2"/>
     </row>
     <row r="88" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A88" s="50" t="s">
+      <c r="A88" s="63" t="s">
         <v>169</v>
       </c>
-      <c r="B88" s="53" t="s">
+      <c r="B88" s="85" t="s">
         <v>49</v>
       </c>
-      <c r="C88" s="56" t="s">
+      <c r="C88" s="54" t="s">
         <v>164</v>
       </c>
-      <c r="D88" s="56" t="s">
+      <c r="D88" s="54" t="s">
         <v>165</v>
       </c>
-      <c r="E88" s="56" t="s">
+      <c r="E88" s="54" t="s">
         <v>166</v>
       </c>
       <c r="F88" s="30" t="s">
@@ -5132,13 +5136,13 @@
       <c r="H88" s="30" t="s">
         <v>168</v>
       </c>
-      <c r="I88" s="47" t="s">
+      <c r="I88" s="51" t="s">
         <v>26</v>
       </c>
-      <c r="J88" s="59" t="s">
+      <c r="J88" s="48" t="s">
         <v>56</v>
       </c>
-      <c r="K88" s="47" t="s">
+      <c r="K88" s="51" t="s">
         <v>28</v>
       </c>
       <c r="L88" s="2"/>
@@ -5159,19 +5163,19 @@
       <c r="AA88" s="2"/>
     </row>
     <row r="89" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A89" s="51"/>
-      <c r="B89" s="54"/>
-      <c r="C89" s="57"/>
-      <c r="D89" s="57"/>
-      <c r="E89" s="57"/>
+      <c r="A89" s="64"/>
+      <c r="B89" s="86"/>
+      <c r="C89" s="55"/>
+      <c r="D89" s="55"/>
+      <c r="E89" s="55"/>
       <c r="F89" s="30" t="s">
         <v>67</v>
       </c>
       <c r="G89" s="35"/>
       <c r="H89" s="35"/>
-      <c r="I89" s="48"/>
-      <c r="J89" s="60"/>
-      <c r="K89" s="48"/>
+      <c r="I89" s="52"/>
+      <c r="J89" s="49"/>
+      <c r="K89" s="52"/>
       <c r="L89" s="2"/>
       <c r="M89" s="2"/>
       <c r="N89" s="2"/>
@@ -5190,19 +5194,19 @@
       <c r="AA89" s="2"/>
     </row>
     <row r="90" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A90" s="51"/>
-      <c r="B90" s="54"/>
-      <c r="C90" s="57"/>
-      <c r="D90" s="57"/>
-      <c r="E90" s="57"/>
+      <c r="A90" s="64"/>
+      <c r="B90" s="86"/>
+      <c r="C90" s="55"/>
+      <c r="D90" s="55"/>
+      <c r="E90" s="55"/>
       <c r="F90" s="30" t="s">
         <v>70</v>
       </c>
       <c r="G90" s="46"/>
       <c r="H90" s="46"/>
-      <c r="I90" s="48"/>
-      <c r="J90" s="60"/>
-      <c r="K90" s="48"/>
+      <c r="I90" s="52"/>
+      <c r="J90" s="49"/>
+      <c r="K90" s="52"/>
       <c r="L90" s="2"/>
       <c r="M90" s="2"/>
       <c r="N90" s="2"/>
@@ -5221,19 +5225,19 @@
       <c r="AA90" s="2"/>
     </row>
     <row r="91" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A91" s="52"/>
-      <c r="B91" s="55"/>
-      <c r="C91" s="58"/>
-      <c r="D91" s="58"/>
-      <c r="E91" s="58"/>
+      <c r="A91" s="65"/>
+      <c r="B91" s="87"/>
+      <c r="C91" s="56"/>
+      <c r="D91" s="56"/>
+      <c r="E91" s="56"/>
       <c r="F91" s="30" t="s">
         <v>99</v>
       </c>
       <c r="G91" s="30"/>
       <c r="H91" s="30"/>
-      <c r="I91" s="49"/>
-      <c r="J91" s="61"/>
-      <c r="K91" s="49"/>
+      <c r="I91" s="53"/>
+      <c r="J91" s="50"/>
+      <c r="K91" s="53"/>
       <c r="L91" s="2"/>
       <c r="M91" s="2"/>
       <c r="N91" s="2"/>
@@ -5252,19 +5256,19 @@
       <c r="AA91" s="2"/>
     </row>
     <row r="92" spans="1:27" ht="25.5" customHeight="1">
-      <c r="A92" s="68" t="s">
+      <c r="A92" s="57" t="s">
         <v>186</v>
       </c>
-      <c r="B92" s="56" t="s">
+      <c r="B92" s="54" t="s">
         <v>84</v>
       </c>
-      <c r="C92" s="56" t="s">
+      <c r="C92" s="54" t="s">
         <v>170</v>
       </c>
-      <c r="D92" s="56" t="s">
+      <c r="D92" s="54" t="s">
         <v>171</v>
       </c>
-      <c r="E92" s="56" t="s">
+      <c r="E92" s="54" t="s">
         <v>172</v>
       </c>
       <c r="F92" s="30" t="s">
@@ -5276,13 +5280,13 @@
       <c r="H92" s="30" t="s">
         <v>174</v>
       </c>
-      <c r="I92" s="47" t="s">
+      <c r="I92" s="51" t="s">
         <v>26</v>
       </c>
-      <c r="J92" s="59" t="s">
+      <c r="J92" s="48" t="s">
         <v>56</v>
       </c>
-      <c r="K92" s="47" t="s">
+      <c r="K92" s="51" t="s">
         <v>28</v>
       </c>
       <c r="L92" s="2"/>
@@ -5303,19 +5307,19 @@
       <c r="AA92" s="2"/>
     </row>
     <row r="93" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A93" s="69"/>
-      <c r="B93" s="57"/>
-      <c r="C93" s="57"/>
-      <c r="D93" s="57"/>
-      <c r="E93" s="57"/>
+      <c r="A93" s="58"/>
+      <c r="B93" s="55"/>
+      <c r="C93" s="55"/>
+      <c r="D93" s="55"/>
+      <c r="E93" s="55"/>
       <c r="F93" s="30" t="s">
         <v>67</v>
       </c>
       <c r="G93" s="35"/>
       <c r="H93" s="30"/>
-      <c r="I93" s="48"/>
-      <c r="J93" s="60"/>
-      <c r="K93" s="48"/>
+      <c r="I93" s="52"/>
+      <c r="J93" s="49"/>
+      <c r="K93" s="52"/>
       <c r="L93" s="2"/>
       <c r="M93" s="2"/>
       <c r="N93" s="2"/>
@@ -5334,19 +5338,19 @@
       <c r="AA93" s="2"/>
     </row>
     <row r="94" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A94" s="69"/>
-      <c r="B94" s="57"/>
-      <c r="C94" s="57"/>
-      <c r="D94" s="57"/>
-      <c r="E94" s="57"/>
+      <c r="A94" s="58"/>
+      <c r="B94" s="55"/>
+      <c r="C94" s="55"/>
+      <c r="D94" s="55"/>
+      <c r="E94" s="55"/>
       <c r="F94" s="30" t="s">
         <v>70</v>
       </c>
       <c r="G94" s="46"/>
       <c r="H94" s="46"/>
-      <c r="I94" s="48"/>
-      <c r="J94" s="60"/>
-      <c r="K94" s="48"/>
+      <c r="I94" s="52"/>
+      <c r="J94" s="49"/>
+      <c r="K94" s="52"/>
       <c r="L94" s="2"/>
       <c r="M94" s="2"/>
       <c r="N94" s="2"/>
@@ -5365,19 +5369,19 @@
       <c r="AA94" s="2"/>
     </row>
     <row r="95" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A95" s="70"/>
-      <c r="B95" s="58"/>
-      <c r="C95" s="58"/>
-      <c r="D95" s="58"/>
-      <c r="E95" s="58"/>
+      <c r="A95" s="59"/>
+      <c r="B95" s="56"/>
+      <c r="C95" s="56"/>
+      <c r="D95" s="56"/>
+      <c r="E95" s="56"/>
       <c r="F95" s="30" t="s">
         <v>99</v>
       </c>
       <c r="G95" s="30"/>
       <c r="H95" s="30"/>
-      <c r="I95" s="49"/>
-      <c r="J95" s="61"/>
-      <c r="K95" s="49"/>
+      <c r="I95" s="53"/>
+      <c r="J95" s="50"/>
+      <c r="K95" s="53"/>
       <c r="L95" s="2"/>
       <c r="M95" s="2"/>
       <c r="N95" s="2"/>
@@ -5396,19 +5400,19 @@
       <c r="AA95" s="2"/>
     </row>
     <row r="96" spans="1:27" ht="26.25" customHeight="1">
-      <c r="A96" s="68" t="s">
+      <c r="A96" s="57" t="s">
         <v>187</v>
       </c>
-      <c r="B96" s="56" t="s">
+      <c r="B96" s="54" t="s">
         <v>84</v>
       </c>
-      <c r="C96" s="56" t="s">
+      <c r="C96" s="54" t="s">
         <v>175</v>
       </c>
-      <c r="D96" s="56" t="s">
+      <c r="D96" s="54" t="s">
         <v>176</v>
       </c>
-      <c r="E96" s="56" t="s">
+      <c r="E96" s="54" t="s">
         <v>177</v>
       </c>
       <c r="F96" s="30" t="s">
@@ -5420,13 +5424,13 @@
       <c r="H96" s="30" t="s">
         <v>174</v>
       </c>
-      <c r="I96" s="47" t="s">
+      <c r="I96" s="51" t="s">
         <v>26</v>
       </c>
-      <c r="J96" s="59" t="s">
+      <c r="J96" s="48" t="s">
         <v>56</v>
       </c>
-      <c r="K96" s="47" t="s">
+      <c r="K96" s="51" t="s">
         <v>28</v>
       </c>
       <c r="L96" s="2"/>
@@ -5447,19 +5451,19 @@
       <c r="AA96" s="2"/>
     </row>
     <row r="97" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A97" s="69"/>
-      <c r="B97" s="57"/>
-      <c r="C97" s="57"/>
-      <c r="D97" s="57"/>
-      <c r="E97" s="57"/>
+      <c r="A97" s="58"/>
+      <c r="B97" s="55"/>
+      <c r="C97" s="55"/>
+      <c r="D97" s="55"/>
+      <c r="E97" s="55"/>
       <c r="F97" s="30" t="s">
         <v>67</v>
       </c>
       <c r="G97" s="35"/>
       <c r="H97" s="30"/>
-      <c r="I97" s="48"/>
-      <c r="J97" s="60"/>
-      <c r="K97" s="48"/>
+      <c r="I97" s="52"/>
+      <c r="J97" s="49"/>
+      <c r="K97" s="52"/>
       <c r="L97" s="2"/>
       <c r="M97" s="2"/>
       <c r="N97" s="2"/>
@@ -5478,19 +5482,19 @@
       <c r="AA97" s="2"/>
     </row>
     <row r="98" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A98" s="69"/>
-      <c r="B98" s="57"/>
-      <c r="C98" s="57"/>
-      <c r="D98" s="57"/>
-      <c r="E98" s="57"/>
+      <c r="A98" s="58"/>
+      <c r="B98" s="55"/>
+      <c r="C98" s="55"/>
+      <c r="D98" s="55"/>
+      <c r="E98" s="55"/>
       <c r="F98" s="30" t="s">
         <v>70</v>
       </c>
       <c r="G98" s="30"/>
       <c r="H98" s="30"/>
-      <c r="I98" s="48"/>
-      <c r="J98" s="60"/>
-      <c r="K98" s="48"/>
+      <c r="I98" s="52"/>
+      <c r="J98" s="49"/>
+      <c r="K98" s="52"/>
       <c r="L98" s="2"/>
       <c r="M98" s="2"/>
       <c r="N98" s="2"/>
@@ -5509,19 +5513,19 @@
       <c r="AA98" s="2"/>
     </row>
     <row r="99" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A99" s="70"/>
-      <c r="B99" s="58"/>
-      <c r="C99" s="58"/>
-      <c r="D99" s="58"/>
-      <c r="E99" s="58"/>
+      <c r="A99" s="59"/>
+      <c r="B99" s="56"/>
+      <c r="C99" s="56"/>
+      <c r="D99" s="56"/>
+      <c r="E99" s="56"/>
       <c r="F99" s="30" t="s">
         <v>99</v>
       </c>
       <c r="G99" s="30"/>
       <c r="H99" s="30"/>
-      <c r="I99" s="49"/>
-      <c r="J99" s="61"/>
-      <c r="K99" s="49"/>
+      <c r="I99" s="53"/>
+      <c r="J99" s="50"/>
+      <c r="K99" s="53"/>
       <c r="L99" s="2"/>
       <c r="M99" s="2"/>
       <c r="N99" s="2"/>
@@ -5540,19 +5544,19 @@
       <c r="AA99" s="2"/>
     </row>
     <row r="100" spans="1:27" ht="24.75" customHeight="1">
-      <c r="A100" s="68" t="s">
+      <c r="A100" s="57" t="s">
         <v>188</v>
       </c>
-      <c r="B100" s="56" t="s">
+      <c r="B100" s="54" t="s">
         <v>84</v>
       </c>
-      <c r="C100" s="56" t="s">
+      <c r="C100" s="54" t="s">
         <v>178</v>
       </c>
-      <c r="D100" s="56" t="s">
+      <c r="D100" s="54" t="s">
         <v>179</v>
       </c>
-      <c r="E100" s="56" t="s">
+      <c r="E100" s="54" t="s">
         <v>172</v>
       </c>
       <c r="F100" s="30" t="s">
@@ -5564,13 +5568,13 @@
       <c r="H100" s="30" t="s">
         <v>181</v>
       </c>
-      <c r="I100" s="47" t="s">
+      <c r="I100" s="51" t="s">
         <v>26</v>
       </c>
-      <c r="J100" s="59" t="s">
+      <c r="J100" s="48" t="s">
         <v>56</v>
       </c>
-      <c r="K100" s="47" t="s">
+      <c r="K100" s="51" t="s">
         <v>28</v>
       </c>
       <c r="L100" s="2"/>
@@ -5591,19 +5595,19 @@
       <c r="AA100" s="2"/>
     </row>
     <row r="101" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A101" s="69"/>
-      <c r="B101" s="57"/>
-      <c r="C101" s="57"/>
-      <c r="D101" s="57"/>
-      <c r="E101" s="57"/>
+      <c r="A101" s="58"/>
+      <c r="B101" s="55"/>
+      <c r="C101" s="55"/>
+      <c r="D101" s="55"/>
+      <c r="E101" s="55"/>
       <c r="F101" s="30" t="s">
         <v>67</v>
       </c>
       <c r="G101" s="35"/>
       <c r="H101" s="30"/>
-      <c r="I101" s="48"/>
-      <c r="J101" s="60"/>
-      <c r="K101" s="48"/>
+      <c r="I101" s="52"/>
+      <c r="J101" s="49"/>
+      <c r="K101" s="52"/>
       <c r="L101" s="2"/>
       <c r="M101" s="2"/>
       <c r="N101" s="2"/>
@@ -5622,19 +5626,19 @@
       <c r="AA101" s="2"/>
     </row>
     <row r="102" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A102" s="69"/>
-      <c r="B102" s="57"/>
-      <c r="C102" s="57"/>
-      <c r="D102" s="57"/>
-      <c r="E102" s="57"/>
+      <c r="A102" s="58"/>
+      <c r="B102" s="55"/>
+      <c r="C102" s="55"/>
+      <c r="D102" s="55"/>
+      <c r="E102" s="55"/>
       <c r="F102" s="30" t="s">
         <v>70</v>
       </c>
       <c r="G102" s="46"/>
       <c r="H102" s="46"/>
-      <c r="I102" s="48"/>
-      <c r="J102" s="60"/>
-      <c r="K102" s="48"/>
+      <c r="I102" s="52"/>
+      <c r="J102" s="49"/>
+      <c r="K102" s="52"/>
       <c r="L102" s="2"/>
       <c r="M102" s="2"/>
       <c r="N102" s="2"/>
@@ -5653,19 +5657,19 @@
       <c r="AA102" s="2"/>
     </row>
     <row r="103" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A103" s="70"/>
-      <c r="B103" s="58"/>
-      <c r="C103" s="58"/>
-      <c r="D103" s="58"/>
-      <c r="E103" s="58"/>
+      <c r="A103" s="59"/>
+      <c r="B103" s="56"/>
+      <c r="C103" s="56"/>
+      <c r="D103" s="56"/>
+      <c r="E103" s="56"/>
       <c r="F103" s="30" t="s">
         <v>99</v>
       </c>
       <c r="G103" s="46"/>
       <c r="H103" s="46"/>
-      <c r="I103" s="49"/>
-      <c r="J103" s="61"/>
-      <c r="K103" s="49"/>
+      <c r="I103" s="53"/>
+      <c r="J103" s="50"/>
+      <c r="K103" s="53"/>
       <c r="L103" s="2"/>
       <c r="M103" s="2"/>
       <c r="N103" s="2"/>
@@ -5684,19 +5688,19 @@
       <c r="AA103" s="2"/>
     </row>
     <row r="104" spans="1:27" ht="24.75" customHeight="1">
-      <c r="A104" s="68" t="s">
+      <c r="A104" s="57" t="s">
         <v>189</v>
       </c>
-      <c r="B104" s="56" t="s">
+      <c r="B104" s="54" t="s">
         <v>84</v>
       </c>
-      <c r="C104" s="56" t="s">
+      <c r="C104" s="54" t="s">
         <v>182</v>
       </c>
-      <c r="D104" s="56" t="s">
+      <c r="D104" s="54" t="s">
         <v>183</v>
       </c>
-      <c r="E104" s="56" t="s">
+      <c r="E104" s="54" t="s">
         <v>177</v>
       </c>
       <c r="F104" s="30" t="s">
@@ -5708,13 +5712,13 @@
       <c r="H104" s="30" t="s">
         <v>185</v>
       </c>
-      <c r="I104" s="47" t="s">
+      <c r="I104" s="51" t="s">
         <v>26</v>
       </c>
-      <c r="J104" s="59" t="s">
+      <c r="J104" s="48" t="s">
         <v>56</v>
       </c>
-      <c r="K104" s="47" t="s">
+      <c r="K104" s="51" t="s">
         <v>28</v>
       </c>
       <c r="L104" s="2"/>
@@ -5735,19 +5739,19 @@
       <c r="AA104" s="2"/>
     </row>
     <row r="105" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A105" s="69"/>
-      <c r="B105" s="57"/>
-      <c r="C105" s="57"/>
-      <c r="D105" s="57"/>
-      <c r="E105" s="57"/>
+      <c r="A105" s="58"/>
+      <c r="B105" s="55"/>
+      <c r="C105" s="55"/>
+      <c r="D105" s="55"/>
+      <c r="E105" s="55"/>
       <c r="F105" s="30" t="s">
         <v>67</v>
       </c>
       <c r="G105" s="35"/>
       <c r="H105" s="30"/>
-      <c r="I105" s="48"/>
-      <c r="J105" s="60"/>
-      <c r="K105" s="48"/>
+      <c r="I105" s="52"/>
+      <c r="J105" s="49"/>
+      <c r="K105" s="52"/>
       <c r="L105" s="2"/>
       <c r="M105" s="2"/>
       <c r="N105" s="2"/>
@@ -5766,19 +5770,19 @@
       <c r="AA105" s="2"/>
     </row>
     <row r="106" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A106" s="69"/>
-      <c r="B106" s="57"/>
-      <c r="C106" s="57"/>
-      <c r="D106" s="57"/>
-      <c r="E106" s="57"/>
+      <c r="A106" s="58"/>
+      <c r="B106" s="55"/>
+      <c r="C106" s="55"/>
+      <c r="D106" s="55"/>
+      <c r="E106" s="55"/>
       <c r="F106" s="30" t="s">
         <v>70</v>
       </c>
       <c r="G106" s="46"/>
       <c r="H106" s="46"/>
-      <c r="I106" s="48"/>
-      <c r="J106" s="60"/>
-      <c r="K106" s="48"/>
+      <c r="I106" s="52"/>
+      <c r="J106" s="49"/>
+      <c r="K106" s="52"/>
       <c r="L106" s="2"/>
       <c r="M106" s="2"/>
       <c r="N106" s="2"/>
@@ -5797,19 +5801,19 @@
       <c r="AA106" s="2"/>
     </row>
     <row r="107" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A107" s="70"/>
-      <c r="B107" s="58"/>
-      <c r="C107" s="58"/>
-      <c r="D107" s="58"/>
-      <c r="E107" s="58"/>
+      <c r="A107" s="59"/>
+      <c r="B107" s="56"/>
+      <c r="C107" s="56"/>
+      <c r="D107" s="56"/>
+      <c r="E107" s="56"/>
       <c r="F107" s="30" t="s">
         <v>99</v>
       </c>
       <c r="G107" s="46"/>
-      <c r="H107" s="93"/>
-      <c r="I107" s="49"/>
-      <c r="J107" s="61"/>
-      <c r="K107" s="49"/>
+      <c r="H107" s="47"/>
+      <c r="I107" s="53"/>
+      <c r="J107" s="50"/>
+      <c r="K107" s="53"/>
       <c r="L107" s="2"/>
       <c r="M107" s="2"/>
       <c r="N107" s="2"/>
@@ -5828,17 +5832,39 @@
       <c r="AA107" s="2"/>
     </row>
     <row r="108" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A108" s="2"/>
-      <c r="B108" s="38"/>
-      <c r="C108" s="2"/>
-      <c r="D108" s="38"/>
-      <c r="E108" s="38"/>
-      <c r="F108" s="2"/>
-      <c r="G108" s="38"/>
-      <c r="H108" s="38"/>
-      <c r="I108" s="2"/>
-      <c r="J108" s="38"/>
-      <c r="K108" s="2"/>
+      <c r="A108" s="89" t="s">
+        <v>199</v>
+      </c>
+      <c r="B108" s="54" t="s">
+        <v>190</v>
+      </c>
+      <c r="C108" s="54" t="s">
+        <v>192</v>
+      </c>
+      <c r="D108" s="54" t="s">
+        <v>201</v>
+      </c>
+      <c r="E108" s="54" t="s">
+        <v>191</v>
+      </c>
+      <c r="F108" s="30" t="s">
+        <v>53</v>
+      </c>
+      <c r="G108" s="30" t="s">
+        <v>193</v>
+      </c>
+      <c r="H108" s="30" t="s">
+        <v>194</v>
+      </c>
+      <c r="I108" s="51" t="s">
+        <v>26</v>
+      </c>
+      <c r="J108" s="48" t="s">
+        <v>56</v>
+      </c>
+      <c r="K108" s="51" t="s">
+        <v>28</v>
+      </c>
       <c r="L108" s="2"/>
       <c r="M108" s="2"/>
       <c r="N108" s="2"/>
@@ -5857,17 +5883,19 @@
       <c r="AA108" s="2"/>
     </row>
     <row r="109" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A109" s="2"/>
-      <c r="B109" s="38"/>
-      <c r="C109" s="2"/>
-      <c r="D109" s="38"/>
-      <c r="E109" s="38"/>
-      <c r="F109" s="2"/>
-      <c r="G109" s="38"/>
-      <c r="H109" s="38"/>
-      <c r="I109" s="2"/>
-      <c r="J109" s="38"/>
-      <c r="K109" s="2"/>
+      <c r="A109" s="90"/>
+      <c r="B109" s="55"/>
+      <c r="C109" s="55"/>
+      <c r="D109" s="55"/>
+      <c r="E109" s="55"/>
+      <c r="F109" s="30" t="s">
+        <v>67</v>
+      </c>
+      <c r="G109" s="30"/>
+      <c r="H109" s="30"/>
+      <c r="I109" s="52"/>
+      <c r="J109" s="49"/>
+      <c r="K109" s="52"/>
       <c r="L109" s="2"/>
       <c r="M109" s="2"/>
       <c r="N109" s="2"/>
@@ -5886,17 +5914,19 @@
       <c r="AA109" s="2"/>
     </row>
     <row r="110" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A110" s="2"/>
-      <c r="B110" s="38"/>
-      <c r="C110" s="2"/>
-      <c r="D110" s="38"/>
-      <c r="E110" s="38"/>
-      <c r="F110" s="2"/>
-      <c r="G110" s="38"/>
-      <c r="H110" s="38"/>
-      <c r="I110" s="2"/>
-      <c r="J110" s="38"/>
-      <c r="K110" s="2"/>
+      <c r="A110" s="90"/>
+      <c r="B110" s="55"/>
+      <c r="C110" s="55"/>
+      <c r="D110" s="55"/>
+      <c r="E110" s="55"/>
+      <c r="F110" s="30" t="s">
+        <v>70</v>
+      </c>
+      <c r="G110" s="30"/>
+      <c r="H110" s="30"/>
+      <c r="I110" s="52"/>
+      <c r="J110" s="49"/>
+      <c r="K110" s="52"/>
       <c r="L110" s="2"/>
       <c r="M110" s="2"/>
       <c r="N110" s="2"/>
@@ -5915,17 +5945,19 @@
       <c r="AA110" s="2"/>
     </row>
     <row r="111" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A111" s="2"/>
-      <c r="B111" s="38"/>
-      <c r="C111" s="2"/>
-      <c r="D111" s="38"/>
-      <c r="E111" s="38"/>
-      <c r="F111" s="2"/>
-      <c r="G111" s="38"/>
-      <c r="H111" s="38"/>
-      <c r="I111" s="2"/>
-      <c r="J111" s="38"/>
-      <c r="K111" s="2"/>
+      <c r="A111" s="91"/>
+      <c r="B111" s="55"/>
+      <c r="C111" s="56"/>
+      <c r="D111" s="56"/>
+      <c r="E111" s="56"/>
+      <c r="F111" s="30" t="s">
+        <v>99</v>
+      </c>
+      <c r="G111" s="30"/>
+      <c r="H111" s="30"/>
+      <c r="I111" s="53"/>
+      <c r="J111" s="50"/>
+      <c r="K111" s="53"/>
       <c r="L111" s="2"/>
       <c r="M111" s="2"/>
       <c r="N111" s="2"/>
@@ -5944,17 +5976,39 @@
       <c r="AA111" s="2"/>
     </row>
     <row r="112" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A112" s="2"/>
-      <c r="B112" s="38"/>
-      <c r="C112" s="2"/>
-      <c r="D112" s="38"/>
-      <c r="E112" s="38"/>
-      <c r="F112" s="2"/>
-      <c r="G112" s="38"/>
-      <c r="H112" s="38"/>
-      <c r="I112" s="2"/>
-      <c r="J112" s="38"/>
-      <c r="K112" s="2"/>
+      <c r="A112" s="89" t="s">
+        <v>200</v>
+      </c>
+      <c r="B112" s="54" t="s">
+        <v>190</v>
+      </c>
+      <c r="C112" s="54" t="s">
+        <v>195</v>
+      </c>
+      <c r="D112" s="54" t="s">
+        <v>196</v>
+      </c>
+      <c r="E112" s="54" t="s">
+        <v>83</v>
+      </c>
+      <c r="F112" s="85" t="s">
+        <v>53</v>
+      </c>
+      <c r="G112" s="85" t="s">
+        <v>197</v>
+      </c>
+      <c r="H112" s="78" t="s">
+        <v>198</v>
+      </c>
+      <c r="I112" s="51" t="s">
+        <v>26</v>
+      </c>
+      <c r="J112" s="48" t="s">
+        <v>56</v>
+      </c>
+      <c r="K112" s="51" t="s">
+        <v>28</v>
+      </c>
       <c r="L112" s="2"/>
       <c r="M112" s="2"/>
       <c r="N112" s="2"/>
@@ -5973,17 +6027,17 @@
       <c r="AA112" s="2"/>
     </row>
     <row r="113" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A113" s="2"/>
-      <c r="B113" s="38"/>
-      <c r="C113" s="2"/>
-      <c r="D113" s="38"/>
-      <c r="E113" s="38"/>
-      <c r="F113" s="2"/>
-      <c r="G113" s="38"/>
-      <c r="H113" s="38"/>
-      <c r="I113" s="2"/>
-      <c r="J113" s="38"/>
-      <c r="K113" s="2"/>
+      <c r="A113" s="90"/>
+      <c r="B113" s="55"/>
+      <c r="C113" s="55"/>
+      <c r="D113" s="55"/>
+      <c r="E113" s="55"/>
+      <c r="F113" s="86"/>
+      <c r="G113" s="86"/>
+      <c r="H113" s="88"/>
+      <c r="I113" s="52"/>
+      <c r="J113" s="49"/>
+      <c r="K113" s="52"/>
       <c r="L113" s="2"/>
       <c r="M113" s="2"/>
       <c r="N113" s="2"/>
@@ -6002,17 +6056,17 @@
       <c r="AA113" s="2"/>
     </row>
     <row r="114" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A114" s="2"/>
-      <c r="B114" s="38"/>
-      <c r="C114" s="2"/>
-      <c r="D114" s="38"/>
-      <c r="E114" s="38"/>
-      <c r="F114" s="2"/>
-      <c r="G114" s="38"/>
-      <c r="H114" s="38"/>
-      <c r="I114" s="2"/>
-      <c r="J114" s="38"/>
-      <c r="K114" s="2"/>
+      <c r="A114" s="90"/>
+      <c r="B114" s="55"/>
+      <c r="C114" s="55"/>
+      <c r="D114" s="55"/>
+      <c r="E114" s="55"/>
+      <c r="F114" s="86"/>
+      <c r="G114" s="86"/>
+      <c r="H114" s="88"/>
+      <c r="I114" s="52"/>
+      <c r="J114" s="49"/>
+      <c r="K114" s="52"/>
       <c r="L114" s="2"/>
       <c r="M114" s="2"/>
       <c r="N114" s="2"/>
@@ -6031,17 +6085,17 @@
       <c r="AA114" s="2"/>
     </row>
     <row r="115" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A115" s="2"/>
-      <c r="B115" s="38"/>
-      <c r="C115" s="2"/>
-      <c r="D115" s="38"/>
-      <c r="E115" s="38"/>
-      <c r="F115" s="2"/>
-      <c r="G115" s="38"/>
-      <c r="H115" s="38"/>
-      <c r="I115" s="2"/>
-      <c r="J115" s="38"/>
-      <c r="K115" s="2"/>
+      <c r="A115" s="91"/>
+      <c r="B115" s="56"/>
+      <c r="C115" s="56"/>
+      <c r="D115" s="56"/>
+      <c r="E115" s="56"/>
+      <c r="F115" s="87"/>
+      <c r="G115" s="87"/>
+      <c r="H115" s="79"/>
+      <c r="I115" s="53"/>
+      <c r="J115" s="50"/>
+      <c r="K115" s="53"/>
       <c r="L115" s="2"/>
       <c r="M115" s="2"/>
       <c r="N115" s="2"/>
@@ -8380,120 +8434,120 @@
       <c r="AA195" s="2"/>
     </row>
     <row r="196" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A196" s="2"/>
-      <c r="B196" s="38"/>
-      <c r="C196" s="2"/>
-      <c r="D196" s="38"/>
-      <c r="E196" s="38"/>
-      <c r="F196" s="2"/>
-      <c r="G196" s="38"/>
-      <c r="H196" s="38"/>
-      <c r="I196" s="2"/>
-      <c r="J196" s="38"/>
-      <c r="K196" s="2"/>
-      <c r="L196" s="2"/>
-      <c r="M196" s="2"/>
-      <c r="N196" s="2"/>
-      <c r="O196" s="2"/>
-      <c r="P196" s="2"/>
-      <c r="Q196" s="2"/>
-      <c r="R196" s="2"/>
-      <c r="S196" s="2"/>
-      <c r="T196" s="2"/>
-      <c r="U196" s="2"/>
-      <c r="V196" s="2"/>
-      <c r="W196" s="2"/>
-      <c r="X196" s="2"/>
-      <c r="Y196" s="2"/>
-      <c r="Z196" s="2"/>
-      <c r="AA196" s="2"/>
+      <c r="A196" s="7"/>
+      <c r="B196" s="39"/>
+      <c r="C196" s="7"/>
+      <c r="D196" s="39"/>
+      <c r="E196" s="39"/>
+      <c r="F196" s="7"/>
+      <c r="G196" s="39"/>
+      <c r="H196" s="39"/>
+      <c r="I196" s="7"/>
+      <c r="J196" s="39"/>
+      <c r="K196" s="7"/>
+      <c r="L196" s="7"/>
+      <c r="M196" s="7"/>
+      <c r="N196" s="7"/>
+      <c r="O196" s="7"/>
+      <c r="P196" s="7"/>
+      <c r="Q196" s="7"/>
+      <c r="R196" s="7"/>
+      <c r="S196" s="7"/>
+      <c r="T196" s="7"/>
+      <c r="U196" s="7"/>
+      <c r="V196" s="7"/>
+      <c r="W196" s="7"/>
+      <c r="X196" s="7"/>
+      <c r="Y196" s="7"/>
+      <c r="Z196" s="7"/>
+      <c r="AA196" s="7"/>
     </row>
     <row r="197" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A197" s="2"/>
-      <c r="B197" s="38"/>
-      <c r="C197" s="2"/>
-      <c r="D197" s="38"/>
-      <c r="E197" s="38"/>
-      <c r="F197" s="2"/>
-      <c r="G197" s="38"/>
-      <c r="H197" s="38"/>
-      <c r="I197" s="2"/>
-      <c r="J197" s="38"/>
-      <c r="K197" s="2"/>
-      <c r="L197" s="2"/>
-      <c r="M197" s="2"/>
-      <c r="N197" s="2"/>
-      <c r="O197" s="2"/>
-      <c r="P197" s="2"/>
-      <c r="Q197" s="2"/>
-      <c r="R197" s="2"/>
-      <c r="S197" s="2"/>
-      <c r="T197" s="2"/>
-      <c r="U197" s="2"/>
-      <c r="V197" s="2"/>
-      <c r="W197" s="2"/>
-      <c r="X197" s="2"/>
-      <c r="Y197" s="2"/>
-      <c r="Z197" s="2"/>
-      <c r="AA197" s="2"/>
+      <c r="A197" s="6"/>
+      <c r="B197" s="40"/>
+      <c r="C197" s="6"/>
+      <c r="D197" s="40"/>
+      <c r="E197" s="40"/>
+      <c r="F197" s="6"/>
+      <c r="G197" s="40"/>
+      <c r="H197" s="40"/>
+      <c r="I197" s="6"/>
+      <c r="J197" s="40"/>
+      <c r="K197" s="6"/>
+      <c r="L197" s="6"/>
+      <c r="M197" s="6"/>
+      <c r="N197" s="6"/>
+      <c r="O197" s="6"/>
+      <c r="P197" s="6"/>
+      <c r="Q197" s="6"/>
+      <c r="R197" s="6"/>
+      <c r="S197" s="6"/>
+      <c r="T197" s="6"/>
+      <c r="U197" s="6"/>
+      <c r="V197" s="6"/>
+      <c r="W197" s="6"/>
+      <c r="X197" s="6"/>
+      <c r="Y197" s="6"/>
+      <c r="Z197" s="6"/>
+      <c r="AA197" s="6"/>
     </row>
     <row r="198" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A198" s="2"/>
-      <c r="B198" s="38"/>
-      <c r="C198" s="2"/>
-      <c r="D198" s="38"/>
-      <c r="E198" s="38"/>
-      <c r="F198" s="2"/>
-      <c r="G198" s="38"/>
-      <c r="H198" s="38"/>
-      <c r="I198" s="2"/>
-      <c r="J198" s="38"/>
-      <c r="K198" s="2"/>
-      <c r="L198" s="2"/>
-      <c r="M198" s="2"/>
-      <c r="N198" s="2"/>
-      <c r="O198" s="2"/>
-      <c r="P198" s="2"/>
-      <c r="Q198" s="2"/>
-      <c r="R198" s="2"/>
-      <c r="S198" s="2"/>
-      <c r="T198" s="2"/>
-      <c r="U198" s="2"/>
-      <c r="V198" s="2"/>
-      <c r="W198" s="2"/>
-      <c r="X198" s="2"/>
-      <c r="Y198" s="2"/>
-      <c r="Z198" s="2"/>
-      <c r="AA198" s="2"/>
+      <c r="A198" s="7"/>
+      <c r="B198" s="39"/>
+      <c r="C198" s="7"/>
+      <c r="D198" s="39"/>
+      <c r="E198" s="39"/>
+      <c r="F198" s="7"/>
+      <c r="G198" s="39"/>
+      <c r="H198" s="39"/>
+      <c r="I198" s="7"/>
+      <c r="J198" s="39"/>
+      <c r="K198" s="7"/>
+      <c r="L198" s="7"/>
+      <c r="M198" s="7"/>
+      <c r="N198" s="7"/>
+      <c r="O198" s="7"/>
+      <c r="P198" s="7"/>
+      <c r="Q198" s="7"/>
+      <c r="R198" s="7"/>
+      <c r="S198" s="7"/>
+      <c r="T198" s="7"/>
+      <c r="U198" s="7"/>
+      <c r="V198" s="7"/>
+      <c r="W198" s="7"/>
+      <c r="X198" s="7"/>
+      <c r="Y198" s="7"/>
+      <c r="Z198" s="7"/>
+      <c r="AA198" s="7"/>
     </row>
     <row r="199" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A199" s="2"/>
-      <c r="B199" s="38"/>
-      <c r="C199" s="2"/>
-      <c r="D199" s="38"/>
-      <c r="E199" s="38"/>
-      <c r="F199" s="2"/>
-      <c r="G199" s="38"/>
-      <c r="H199" s="38"/>
-      <c r="I199" s="2"/>
-      <c r="J199" s="38"/>
-      <c r="K199" s="2"/>
-      <c r="L199" s="2"/>
-      <c r="M199" s="2"/>
-      <c r="N199" s="2"/>
-      <c r="O199" s="2"/>
-      <c r="P199" s="2"/>
-      <c r="Q199" s="2"/>
-      <c r="R199" s="2"/>
-      <c r="S199" s="2"/>
-      <c r="T199" s="2"/>
-      <c r="U199" s="2"/>
-      <c r="V199" s="2"/>
-      <c r="W199" s="2"/>
-      <c r="X199" s="2"/>
-      <c r="Y199" s="2"/>
-      <c r="Z199" s="2"/>
-      <c r="AA199" s="2"/>
+      <c r="A199" s="6"/>
+      <c r="B199" s="40"/>
+      <c r="C199" s="6"/>
+      <c r="D199" s="40"/>
+      <c r="E199" s="40"/>
+      <c r="F199" s="6"/>
+      <c r="G199" s="40"/>
+      <c r="H199" s="40"/>
+      <c r="I199" s="6"/>
+      <c r="J199" s="40"/>
+      <c r="K199" s="6"/>
+      <c r="L199" s="6"/>
+      <c r="M199" s="6"/>
+      <c r="N199" s="6"/>
+      <c r="O199" s="6"/>
+      <c r="P199" s="6"/>
+      <c r="Q199" s="6"/>
+      <c r="R199" s="6"/>
+      <c r="S199" s="6"/>
+      <c r="T199" s="6"/>
+      <c r="U199" s="6"/>
+      <c r="V199" s="6"/>
+      <c r="W199" s="6"/>
+      <c r="X199" s="6"/>
+      <c r="Y199" s="6"/>
+      <c r="Z199" s="6"/>
+      <c r="AA199" s="6"/>
     </row>
     <row r="200" spans="1:27" ht="15.75" customHeight="1">
       <c r="A200" s="7"/>
@@ -29723,178 +29777,175 @@
       <c r="Z931" s="6"/>
       <c r="AA931" s="6"/>
     </row>
-    <row r="932" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A932" s="7"/>
-      <c r="B932" s="39"/>
-      <c r="C932" s="7"/>
-      <c r="D932" s="39"/>
-      <c r="E932" s="39"/>
-      <c r="F932" s="7"/>
-      <c r="G932" s="39"/>
-      <c r="H932" s="39"/>
-      <c r="I932" s="7"/>
-      <c r="J932" s="39"/>
-      <c r="K932" s="7"/>
-      <c r="L932" s="7"/>
-      <c r="M932" s="7"/>
-      <c r="N932" s="7"/>
-      <c r="O932" s="7"/>
-      <c r="P932" s="7"/>
-      <c r="Q932" s="7"/>
-      <c r="R932" s="7"/>
-      <c r="S932" s="7"/>
-      <c r="T932" s="7"/>
-      <c r="U932" s="7"/>
-      <c r="V932" s="7"/>
-      <c r="W932" s="7"/>
-      <c r="X932" s="7"/>
-      <c r="Y932" s="7"/>
-      <c r="Z932" s="7"/>
-      <c r="AA932" s="7"/>
-    </row>
-    <row r="933" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A933" s="6"/>
-      <c r="B933" s="40"/>
-      <c r="C933" s="6"/>
-      <c r="D933" s="40"/>
-      <c r="E933" s="40"/>
-      <c r="F933" s="6"/>
-      <c r="G933" s="40"/>
-      <c r="H933" s="40"/>
-      <c r="I933" s="6"/>
-      <c r="J933" s="40"/>
-      <c r="K933" s="6"/>
-      <c r="L933" s="6"/>
-      <c r="M933" s="6"/>
-      <c r="N933" s="6"/>
-      <c r="O933" s="6"/>
-      <c r="P933" s="6"/>
-      <c r="Q933" s="6"/>
-      <c r="R933" s="6"/>
-      <c r="S933" s="6"/>
-      <c r="T933" s="6"/>
-      <c r="U933" s="6"/>
-      <c r="V933" s="6"/>
-      <c r="W933" s="6"/>
-      <c r="X933" s="6"/>
-      <c r="Y933" s="6"/>
-      <c r="Z933" s="6"/>
-      <c r="AA933" s="6"/>
-    </row>
-    <row r="934" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A934" s="7"/>
-      <c r="B934" s="39"/>
-      <c r="C934" s="7"/>
-      <c r="D934" s="39"/>
-      <c r="E934" s="39"/>
-      <c r="F934" s="7"/>
-      <c r="G934" s="39"/>
-      <c r="H934" s="39"/>
-      <c r="I934" s="7"/>
-      <c r="J934" s="39"/>
-      <c r="K934" s="7"/>
-      <c r="L934" s="7"/>
-      <c r="M934" s="7"/>
-      <c r="N934" s="7"/>
-      <c r="O934" s="7"/>
-      <c r="P934" s="7"/>
-      <c r="Q934" s="7"/>
-      <c r="R934" s="7"/>
-      <c r="S934" s="7"/>
-      <c r="T934" s="7"/>
-      <c r="U934" s="7"/>
-      <c r="V934" s="7"/>
-      <c r="W934" s="7"/>
-      <c r="X934" s="7"/>
-      <c r="Y934" s="7"/>
-      <c r="Z934" s="7"/>
-      <c r="AA934" s="7"/>
-    </row>
-    <row r="935" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A935" s="6"/>
-      <c r="B935" s="40"/>
-      <c r="C935" s="6"/>
-      <c r="D935" s="40"/>
-      <c r="E935" s="40"/>
-      <c r="F935" s="6"/>
-      <c r="G935" s="40"/>
-      <c r="H935" s="40"/>
-      <c r="I935" s="6"/>
-      <c r="J935" s="40"/>
-      <c r="K935" s="6"/>
-      <c r="L935" s="6"/>
-      <c r="M935" s="6"/>
-      <c r="N935" s="6"/>
-      <c r="O935" s="6"/>
-      <c r="P935" s="6"/>
-      <c r="Q935" s="6"/>
-      <c r="R935" s="6"/>
-      <c r="S935" s="6"/>
-      <c r="T935" s="6"/>
-      <c r="U935" s="6"/>
-      <c r="V935" s="6"/>
-      <c r="W935" s="6"/>
-      <c r="X935" s="6"/>
-      <c r="Y935" s="6"/>
-      <c r="Z935" s="6"/>
-      <c r="AA935" s="6"/>
-    </row>
   </sheetData>
-  <mergeCells count="226">
-    <mergeCell ref="J92:J95"/>
-    <mergeCell ref="K92:K95"/>
-    <mergeCell ref="I96:I99"/>
-    <mergeCell ref="J96:J99"/>
-    <mergeCell ref="K96:K99"/>
-    <mergeCell ref="I100:I103"/>
-    <mergeCell ref="J100:J103"/>
-    <mergeCell ref="K100:K103"/>
-    <mergeCell ref="I104:I107"/>
-    <mergeCell ref="J104:J107"/>
-    <mergeCell ref="K104:K107"/>
-    <mergeCell ref="B104:B107"/>
-    <mergeCell ref="C104:C107"/>
-    <mergeCell ref="D104:D107"/>
-    <mergeCell ref="E104:E107"/>
-    <mergeCell ref="A92:A95"/>
-    <mergeCell ref="A96:A99"/>
-    <mergeCell ref="A100:A103"/>
-    <mergeCell ref="A104:A107"/>
-    <mergeCell ref="I92:I95"/>
-    <mergeCell ref="B92:B95"/>
-    <mergeCell ref="C92:C95"/>
-    <mergeCell ref="D92:D95"/>
-    <mergeCell ref="E92:E95"/>
-    <mergeCell ref="B96:B99"/>
-    <mergeCell ref="C96:C99"/>
-    <mergeCell ref="D96:D99"/>
-    <mergeCell ref="E96:E99"/>
-    <mergeCell ref="B100:B103"/>
-    <mergeCell ref="C100:C103"/>
-    <mergeCell ref="D100:D103"/>
-    <mergeCell ref="E100:E103"/>
-    <mergeCell ref="C32:C35"/>
-    <mergeCell ref="B32:B35"/>
-    <mergeCell ref="B28:B31"/>
-    <mergeCell ref="C4:C7"/>
-    <mergeCell ref="C8:C11"/>
-    <mergeCell ref="C12:C15"/>
-    <mergeCell ref="C16:C19"/>
-    <mergeCell ref="C20:C23"/>
-    <mergeCell ref="C24:C27"/>
-    <mergeCell ref="C28:C31"/>
-    <mergeCell ref="A4:A7"/>
-    <mergeCell ref="A8:A11"/>
-    <mergeCell ref="A12:A15"/>
-    <mergeCell ref="A16:A19"/>
-    <mergeCell ref="A20:A23"/>
-    <mergeCell ref="A24:A27"/>
-    <mergeCell ref="B24:B27"/>
-    <mergeCell ref="B20:B23"/>
-    <mergeCell ref="B16:B19"/>
-    <mergeCell ref="B12:B15"/>
-    <mergeCell ref="B8:B11"/>
-    <mergeCell ref="B4:B7"/>
+  <mergeCells count="245">
+    <mergeCell ref="I108:I111"/>
+    <mergeCell ref="J108:J111"/>
+    <mergeCell ref="K108:K111"/>
+    <mergeCell ref="I112:I115"/>
+    <mergeCell ref="J112:J115"/>
+    <mergeCell ref="K112:K115"/>
+    <mergeCell ref="B112:B115"/>
+    <mergeCell ref="C112:C115"/>
+    <mergeCell ref="D112:D115"/>
+    <mergeCell ref="E112:E115"/>
+    <mergeCell ref="F112:F115"/>
+    <mergeCell ref="G112:G115"/>
+    <mergeCell ref="H112:H115"/>
+    <mergeCell ref="A108:A111"/>
+    <mergeCell ref="A112:A115"/>
+    <mergeCell ref="B108:B111"/>
+    <mergeCell ref="C108:C111"/>
+    <mergeCell ref="D108:D111"/>
+    <mergeCell ref="E108:E111"/>
+    <mergeCell ref="K84:K87"/>
+    <mergeCell ref="A88:A91"/>
+    <mergeCell ref="B88:B91"/>
+    <mergeCell ref="C88:C91"/>
+    <mergeCell ref="D88:D91"/>
+    <mergeCell ref="E88:E91"/>
+    <mergeCell ref="I88:I91"/>
+    <mergeCell ref="J88:J91"/>
+    <mergeCell ref="K88:K91"/>
+    <mergeCell ref="B84:B87"/>
+    <mergeCell ref="C84:C87"/>
+    <mergeCell ref="D84:D87"/>
+    <mergeCell ref="E84:E87"/>
+    <mergeCell ref="I84:I87"/>
+    <mergeCell ref="J84:J87"/>
+    <mergeCell ref="A84:A87"/>
+    <mergeCell ref="B36:B39"/>
+    <mergeCell ref="C36:C39"/>
+    <mergeCell ref="D36:D39"/>
+    <mergeCell ref="E36:E39"/>
+    <mergeCell ref="J44:J47"/>
+    <mergeCell ref="J36:J39"/>
+    <mergeCell ref="A76:A79"/>
+    <mergeCell ref="B76:B79"/>
+    <mergeCell ref="C76:C79"/>
+    <mergeCell ref="D76:D79"/>
+    <mergeCell ref="E76:E79"/>
+    <mergeCell ref="I76:I79"/>
+    <mergeCell ref="J76:J79"/>
+    <mergeCell ref="A60:A63"/>
+    <mergeCell ref="J56:J59"/>
+    <mergeCell ref="K44:K47"/>
+    <mergeCell ref="I48:I51"/>
+    <mergeCell ref="J48:J51"/>
+    <mergeCell ref="K48:K51"/>
+    <mergeCell ref="B48:B51"/>
+    <mergeCell ref="C48:C51"/>
+    <mergeCell ref="D48:D51"/>
+    <mergeCell ref="E48:E51"/>
+    <mergeCell ref="K40:K43"/>
+    <mergeCell ref="I40:I43"/>
+    <mergeCell ref="B40:B43"/>
+    <mergeCell ref="C40:C43"/>
+    <mergeCell ref="D40:D43"/>
+    <mergeCell ref="E40:E43"/>
+    <mergeCell ref="K76:K79"/>
+    <mergeCell ref="J80:J83"/>
+    <mergeCell ref="K80:K83"/>
+    <mergeCell ref="A80:A83"/>
+    <mergeCell ref="B80:B83"/>
+    <mergeCell ref="C80:C83"/>
+    <mergeCell ref="D80:D83"/>
+    <mergeCell ref="E80:E83"/>
+    <mergeCell ref="I80:I83"/>
+    <mergeCell ref="K56:K59"/>
+    <mergeCell ref="J60:J63"/>
+    <mergeCell ref="K60:K63"/>
+    <mergeCell ref="I68:I71"/>
+    <mergeCell ref="J68:J71"/>
+    <mergeCell ref="K68:K71"/>
+    <mergeCell ref="A72:A75"/>
+    <mergeCell ref="B72:B75"/>
+    <mergeCell ref="C72:C75"/>
+    <mergeCell ref="D72:D75"/>
+    <mergeCell ref="E72:E75"/>
+    <mergeCell ref="I72:I75"/>
+    <mergeCell ref="J72:J75"/>
+    <mergeCell ref="K72:K75"/>
+    <mergeCell ref="A68:A71"/>
+    <mergeCell ref="B68:B71"/>
+    <mergeCell ref="C68:C71"/>
+    <mergeCell ref="D68:D71"/>
+    <mergeCell ref="E68:E71"/>
+    <mergeCell ref="A64:A67"/>
+    <mergeCell ref="J64:J67"/>
+    <mergeCell ref="K64:K67"/>
+    <mergeCell ref="D2:D3"/>
+    <mergeCell ref="J52:J55"/>
+    <mergeCell ref="K52:K55"/>
+    <mergeCell ref="E52:E55"/>
+    <mergeCell ref="B44:B47"/>
+    <mergeCell ref="C44:C47"/>
+    <mergeCell ref="D44:D47"/>
+    <mergeCell ref="E44:E47"/>
+    <mergeCell ref="B64:B67"/>
+    <mergeCell ref="C64:C67"/>
+    <mergeCell ref="D64:D67"/>
+    <mergeCell ref="E64:E67"/>
+    <mergeCell ref="I64:I67"/>
+    <mergeCell ref="B60:B63"/>
+    <mergeCell ref="C60:C63"/>
+    <mergeCell ref="D60:D63"/>
+    <mergeCell ref="E60:E63"/>
+    <mergeCell ref="I60:I63"/>
+    <mergeCell ref="E56:E59"/>
+    <mergeCell ref="I52:I55"/>
+    <mergeCell ref="B56:B59"/>
+    <mergeCell ref="I56:I59"/>
+    <mergeCell ref="I44:I47"/>
+    <mergeCell ref="J40:J43"/>
+    <mergeCell ref="J32:J35"/>
+    <mergeCell ref="B2:B3"/>
+    <mergeCell ref="A2:A3"/>
+    <mergeCell ref="A52:A55"/>
+    <mergeCell ref="B52:B55"/>
+    <mergeCell ref="C56:C59"/>
+    <mergeCell ref="D56:D59"/>
+    <mergeCell ref="C52:C55"/>
+    <mergeCell ref="D52:D55"/>
+    <mergeCell ref="A44:A47"/>
+    <mergeCell ref="A48:A51"/>
+    <mergeCell ref="D24:D27"/>
+    <mergeCell ref="D20:D23"/>
+    <mergeCell ref="D16:D19"/>
+    <mergeCell ref="D12:D15"/>
+    <mergeCell ref="D8:D11"/>
+    <mergeCell ref="D4:D7"/>
+    <mergeCell ref="A28:A31"/>
+    <mergeCell ref="A32:A35"/>
+    <mergeCell ref="A36:A39"/>
+    <mergeCell ref="A40:A43"/>
+    <mergeCell ref="D32:D35"/>
+    <mergeCell ref="D28:D31"/>
+    <mergeCell ref="A56:A59"/>
+    <mergeCell ref="E32:E35"/>
+    <mergeCell ref="C2:C3"/>
+    <mergeCell ref="H4:H5"/>
+    <mergeCell ref="G4:G5"/>
+    <mergeCell ref="H8:H9"/>
+    <mergeCell ref="H12:H13"/>
+    <mergeCell ref="K32:K35"/>
+    <mergeCell ref="K36:K39"/>
+    <mergeCell ref="J4:J7"/>
+    <mergeCell ref="J8:J11"/>
+    <mergeCell ref="J12:J15"/>
+    <mergeCell ref="J16:J19"/>
+    <mergeCell ref="J20:J23"/>
+    <mergeCell ref="J24:J27"/>
+    <mergeCell ref="J28:J31"/>
+    <mergeCell ref="I32:I35"/>
+    <mergeCell ref="I36:I39"/>
+    <mergeCell ref="K4:K7"/>
+    <mergeCell ref="K8:K11"/>
+    <mergeCell ref="K12:K15"/>
+    <mergeCell ref="K16:K19"/>
+    <mergeCell ref="K20:K23"/>
+    <mergeCell ref="K24:K27"/>
+    <mergeCell ref="J2:J3"/>
     <mergeCell ref="K2:K3"/>
     <mergeCell ref="I4:I7"/>
     <mergeCell ref="I8:I11"/>
@@ -29919,280 +29970,186 @@
     <mergeCell ref="E4:E7"/>
     <mergeCell ref="E8:E11"/>
     <mergeCell ref="E12:E15"/>
-    <mergeCell ref="E32:E35"/>
-    <mergeCell ref="C2:C3"/>
-    <mergeCell ref="H4:H5"/>
-    <mergeCell ref="G4:G5"/>
-    <mergeCell ref="H8:H9"/>
-    <mergeCell ref="H12:H13"/>
-    <mergeCell ref="K32:K35"/>
-    <mergeCell ref="K36:K39"/>
-    <mergeCell ref="J4:J7"/>
-    <mergeCell ref="J8:J11"/>
-    <mergeCell ref="J12:J15"/>
-    <mergeCell ref="J16:J19"/>
-    <mergeCell ref="J20:J23"/>
-    <mergeCell ref="J24:J27"/>
-    <mergeCell ref="J28:J31"/>
-    <mergeCell ref="I32:I35"/>
-    <mergeCell ref="I36:I39"/>
-    <mergeCell ref="K4:K7"/>
-    <mergeCell ref="K8:K11"/>
-    <mergeCell ref="K12:K15"/>
-    <mergeCell ref="K16:K19"/>
-    <mergeCell ref="K20:K23"/>
-    <mergeCell ref="K24:K27"/>
-    <mergeCell ref="J2:J3"/>
-    <mergeCell ref="J32:J35"/>
-    <mergeCell ref="B2:B3"/>
-    <mergeCell ref="A2:A3"/>
-    <mergeCell ref="A52:A55"/>
-    <mergeCell ref="B52:B55"/>
-    <mergeCell ref="C56:C59"/>
-    <mergeCell ref="D56:D59"/>
-    <mergeCell ref="C52:C55"/>
-    <mergeCell ref="D52:D55"/>
-    <mergeCell ref="A44:A47"/>
-    <mergeCell ref="A48:A51"/>
-    <mergeCell ref="D24:D27"/>
-    <mergeCell ref="D20:D23"/>
-    <mergeCell ref="D16:D19"/>
-    <mergeCell ref="D12:D15"/>
-    <mergeCell ref="D8:D11"/>
-    <mergeCell ref="D4:D7"/>
-    <mergeCell ref="A28:A31"/>
-    <mergeCell ref="A32:A35"/>
-    <mergeCell ref="A36:A39"/>
-    <mergeCell ref="A40:A43"/>
-    <mergeCell ref="D32:D35"/>
-    <mergeCell ref="D28:D31"/>
-    <mergeCell ref="A56:A59"/>
-    <mergeCell ref="D2:D3"/>
-    <mergeCell ref="J52:J55"/>
-    <mergeCell ref="K52:K55"/>
-    <mergeCell ref="E52:E55"/>
-    <mergeCell ref="B44:B47"/>
-    <mergeCell ref="C44:C47"/>
-    <mergeCell ref="D44:D47"/>
-    <mergeCell ref="E44:E47"/>
-    <mergeCell ref="B64:B67"/>
-    <mergeCell ref="C64:C67"/>
-    <mergeCell ref="D64:D67"/>
-    <mergeCell ref="E64:E67"/>
-    <mergeCell ref="I64:I67"/>
-    <mergeCell ref="B60:B63"/>
-    <mergeCell ref="C60:C63"/>
-    <mergeCell ref="D60:D63"/>
-    <mergeCell ref="E60:E63"/>
-    <mergeCell ref="I60:I63"/>
-    <mergeCell ref="E56:E59"/>
-    <mergeCell ref="I52:I55"/>
-    <mergeCell ref="B56:B59"/>
-    <mergeCell ref="I56:I59"/>
-    <mergeCell ref="I44:I47"/>
-    <mergeCell ref="J40:J43"/>
-    <mergeCell ref="K56:K59"/>
-    <mergeCell ref="J60:J63"/>
-    <mergeCell ref="K60:K63"/>
-    <mergeCell ref="I68:I71"/>
-    <mergeCell ref="J68:J71"/>
-    <mergeCell ref="K68:K71"/>
-    <mergeCell ref="A72:A75"/>
-    <mergeCell ref="B72:B75"/>
-    <mergeCell ref="C72:C75"/>
-    <mergeCell ref="D72:D75"/>
-    <mergeCell ref="E72:E75"/>
-    <mergeCell ref="I72:I75"/>
-    <mergeCell ref="J72:J75"/>
-    <mergeCell ref="K72:K75"/>
-    <mergeCell ref="A68:A71"/>
-    <mergeCell ref="B68:B71"/>
-    <mergeCell ref="C68:C71"/>
-    <mergeCell ref="D68:D71"/>
-    <mergeCell ref="E68:E71"/>
-    <mergeCell ref="A64:A67"/>
-    <mergeCell ref="J64:J67"/>
-    <mergeCell ref="K64:K67"/>
-    <mergeCell ref="K76:K79"/>
-    <mergeCell ref="J80:J83"/>
-    <mergeCell ref="K80:K83"/>
-    <mergeCell ref="A80:A83"/>
-    <mergeCell ref="B80:B83"/>
-    <mergeCell ref="C80:C83"/>
-    <mergeCell ref="D80:D83"/>
-    <mergeCell ref="E80:E83"/>
-    <mergeCell ref="I80:I83"/>
-    <mergeCell ref="K44:K47"/>
-    <mergeCell ref="I48:I51"/>
-    <mergeCell ref="J48:J51"/>
-    <mergeCell ref="K48:K51"/>
-    <mergeCell ref="B48:B51"/>
-    <mergeCell ref="C48:C51"/>
-    <mergeCell ref="D48:D51"/>
-    <mergeCell ref="E48:E51"/>
-    <mergeCell ref="K40:K43"/>
-    <mergeCell ref="I40:I43"/>
-    <mergeCell ref="B40:B43"/>
-    <mergeCell ref="C40:C43"/>
-    <mergeCell ref="D40:D43"/>
-    <mergeCell ref="E40:E43"/>
-    <mergeCell ref="B36:B39"/>
-    <mergeCell ref="C36:C39"/>
-    <mergeCell ref="D36:D39"/>
-    <mergeCell ref="E36:E39"/>
-    <mergeCell ref="J44:J47"/>
-    <mergeCell ref="J36:J39"/>
-    <mergeCell ref="A76:A79"/>
-    <mergeCell ref="B76:B79"/>
-    <mergeCell ref="C76:C79"/>
-    <mergeCell ref="D76:D79"/>
-    <mergeCell ref="E76:E79"/>
-    <mergeCell ref="I76:I79"/>
-    <mergeCell ref="J76:J79"/>
-    <mergeCell ref="A60:A63"/>
-    <mergeCell ref="J56:J59"/>
-    <mergeCell ref="K84:K87"/>
-    <mergeCell ref="A88:A91"/>
-    <mergeCell ref="B88:B91"/>
-    <mergeCell ref="C88:C91"/>
-    <mergeCell ref="D88:D91"/>
-    <mergeCell ref="E88:E91"/>
-    <mergeCell ref="I88:I91"/>
-    <mergeCell ref="J88:J91"/>
-    <mergeCell ref="K88:K91"/>
-    <mergeCell ref="B84:B87"/>
-    <mergeCell ref="C84:C87"/>
-    <mergeCell ref="D84:D87"/>
-    <mergeCell ref="E84:E87"/>
-    <mergeCell ref="I84:I87"/>
-    <mergeCell ref="J84:J87"/>
-    <mergeCell ref="A84:A87"/>
+    <mergeCell ref="A4:A7"/>
+    <mergeCell ref="A8:A11"/>
+    <mergeCell ref="A12:A15"/>
+    <mergeCell ref="A16:A19"/>
+    <mergeCell ref="A20:A23"/>
+    <mergeCell ref="A24:A27"/>
+    <mergeCell ref="B24:B27"/>
+    <mergeCell ref="B20:B23"/>
+    <mergeCell ref="B16:B19"/>
+    <mergeCell ref="B12:B15"/>
+    <mergeCell ref="B8:B11"/>
+    <mergeCell ref="B4:B7"/>
+    <mergeCell ref="C32:C35"/>
+    <mergeCell ref="B32:B35"/>
+    <mergeCell ref="B28:B31"/>
+    <mergeCell ref="C4:C7"/>
+    <mergeCell ref="C8:C11"/>
+    <mergeCell ref="C12:C15"/>
+    <mergeCell ref="C16:C19"/>
+    <mergeCell ref="C20:C23"/>
+    <mergeCell ref="C24:C27"/>
+    <mergeCell ref="C28:C31"/>
+    <mergeCell ref="B104:B107"/>
+    <mergeCell ref="C104:C107"/>
+    <mergeCell ref="D104:D107"/>
+    <mergeCell ref="E104:E107"/>
+    <mergeCell ref="A92:A95"/>
+    <mergeCell ref="A96:A99"/>
+    <mergeCell ref="A100:A103"/>
+    <mergeCell ref="A104:A107"/>
+    <mergeCell ref="I92:I95"/>
+    <mergeCell ref="B92:B95"/>
+    <mergeCell ref="C92:C95"/>
+    <mergeCell ref="D92:D95"/>
+    <mergeCell ref="E92:E95"/>
+    <mergeCell ref="B96:B99"/>
+    <mergeCell ref="C96:C99"/>
+    <mergeCell ref="D96:D99"/>
+    <mergeCell ref="E96:E99"/>
+    <mergeCell ref="B100:B103"/>
+    <mergeCell ref="C100:C103"/>
+    <mergeCell ref="D100:D103"/>
+    <mergeCell ref="E100:E103"/>
+    <mergeCell ref="J92:J95"/>
+    <mergeCell ref="K92:K95"/>
+    <mergeCell ref="I96:I99"/>
+    <mergeCell ref="J96:J99"/>
+    <mergeCell ref="K96:K99"/>
+    <mergeCell ref="I100:I103"/>
+    <mergeCell ref="J100:J103"/>
+    <mergeCell ref="K100:K103"/>
+    <mergeCell ref="I104:I107"/>
+    <mergeCell ref="J104:J107"/>
+    <mergeCell ref="K104:K107"/>
   </mergeCells>
   <conditionalFormatting sqref="I4 I8 I12">
-    <cfRule type="cellIs" dxfId="31" priority="21" operator="equal">
+    <cfRule type="cellIs" dxfId="27" priority="21" operator="equal">
       <formula>"TO DO"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I4 I8 I12">
-    <cfRule type="cellIs" dxfId="30" priority="22" operator="equal">
+    <cfRule type="cellIs" dxfId="26" priority="22" operator="equal">
       <formula>"IN PROGRESS"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I4 I8 I12">
-    <cfRule type="cellIs" dxfId="29" priority="23" operator="equal">
+    <cfRule type="cellIs" dxfId="25" priority="23" operator="equal">
       <formula>"REVIEWED"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I4 I8 I12">
-    <cfRule type="cellIs" dxfId="28" priority="24" operator="equal">
+    <cfRule type="cellIs" dxfId="24" priority="24" operator="equal">
       <formula>"IN REVIEW"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I16 I20 I24">
-    <cfRule type="cellIs" dxfId="27" priority="17" operator="equal">
+    <cfRule type="cellIs" dxfId="23" priority="17" operator="equal">
       <formula>"TO DO"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I16 I20 I24">
-    <cfRule type="cellIs" dxfId="26" priority="18" operator="equal">
+    <cfRule type="cellIs" dxfId="22" priority="18" operator="equal">
       <formula>"IN PROGRESS"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I16 I20 I24">
-    <cfRule type="cellIs" dxfId="25" priority="19" operator="equal">
+    <cfRule type="cellIs" dxfId="21" priority="19" operator="equal">
       <formula>"REVIEWED"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I16 I20 I24">
-    <cfRule type="cellIs" dxfId="24" priority="20" operator="equal">
+    <cfRule type="cellIs" dxfId="20" priority="20" operator="equal">
       <formula>"IN REVIEW"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I28 I32 I36 I40 I44 I48 I52 I56 I60">
-    <cfRule type="cellIs" dxfId="23" priority="13" operator="equal">
+    <cfRule type="cellIs" dxfId="19" priority="13" operator="equal">
       <formula>"TO DO"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I28 I32 I36 I40 I44 I48 I52 I56 I60">
-    <cfRule type="cellIs" dxfId="22" priority="14" operator="equal">
+    <cfRule type="cellIs" dxfId="18" priority="14" operator="equal">
       <formula>"IN PROGRESS"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I28 I32 I36 I40 I44 I48 I52 I56 I60">
-    <cfRule type="cellIs" dxfId="21" priority="15" operator="equal">
+    <cfRule type="cellIs" dxfId="17" priority="15" operator="equal">
       <formula>"REVIEWED"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I28 I32 I36 I40 I44 I48 I52 I56 I60">
-    <cfRule type="cellIs" dxfId="20" priority="16" operator="equal">
+    <cfRule type="cellIs" dxfId="16" priority="16" operator="equal">
       <formula>"IN REVIEW"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I64 I68">
-    <cfRule type="cellIs" dxfId="19" priority="9" operator="equal">
+    <cfRule type="cellIs" dxfId="15" priority="9" operator="equal">
       <formula>"TO DO"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I64 I68">
-    <cfRule type="cellIs" dxfId="18" priority="10" operator="equal">
+    <cfRule type="cellIs" dxfId="14" priority="10" operator="equal">
       <formula>"IN PROGRESS"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I64 I68">
-    <cfRule type="cellIs" dxfId="17" priority="11" operator="equal">
+    <cfRule type="cellIs" dxfId="13" priority="11" operator="equal">
       <formula>"REVIEWED"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I64 I68">
-    <cfRule type="cellIs" dxfId="16" priority="12" operator="equal">
+    <cfRule type="cellIs" dxfId="12" priority="12" operator="equal">
       <formula>"IN REVIEW"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I76 I72 I80 I84">
-    <cfRule type="cellIs" dxfId="15" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="11" priority="5" operator="equal">
       <formula>"TO DO"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I76 I72 I80 I84">
-    <cfRule type="cellIs" dxfId="14" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="10" priority="6" operator="equal">
       <formula>"IN PROGRESS"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I76 I72 I80 I84">
-    <cfRule type="cellIs" dxfId="13" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="9" priority="7" operator="equal">
       <formula>"REVIEWED"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I76 I72 I80 I84">
-    <cfRule type="cellIs" dxfId="12" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="8" priority="8" operator="equal">
       <formula>"IN REVIEW"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I88 I92 I96 I100 I104">
-    <cfRule type="cellIs" dxfId="11" priority="1" operator="equal">
+  <conditionalFormatting sqref="I88 I92 I96 I100 I104 I108 I112">
+    <cfRule type="cellIs" dxfId="7" priority="1" operator="equal">
       <formula>"TO DO"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I88 I92 I96 I100 I104">
-    <cfRule type="cellIs" dxfId="10" priority="2" operator="equal">
+  <conditionalFormatting sqref="I88 I92 I96 I100 I104 I108 I112">
+    <cfRule type="cellIs" dxfId="6" priority="2" operator="equal">
       <formula>"IN PROGRESS"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I88 I92 I96 I100 I104">
-    <cfRule type="cellIs" dxfId="9" priority="3" operator="equal">
+  <conditionalFormatting sqref="I88 I92 I96 I100 I104 I108 I112">
+    <cfRule type="cellIs" dxfId="5" priority="3" operator="equal">
       <formula>"REVIEWED"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I88 I92 I96 I100 I104">
-    <cfRule type="cellIs" dxfId="8" priority="4" operator="equal">
+  <conditionalFormatting sqref="I88 I92 I96 I100 I104 I108 I112">
+    <cfRule type="cellIs" dxfId="4" priority="4" operator="equal">
       <formula>"IN REVIEW"</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" sqref="I52 I64 I24 I16 I20 I4 I8 I12 I68 I56 I60 I32 I36 I28 I40 I44 I48 I84 I76 I72 I80 I88 I92 I96 I100 I104">
+    <dataValidation type="list" allowBlank="1" sqref="I52 I64 I24 I16 I20 I4 I8 I12 I68 I56 I60 I32 I36 I28 I40 I44 I48 I84 I76 I72 I80 I88 I92 I96 I100 I104 I108 I112">
       <formula1>"TO DO,In Progress,In Review,Reviewed"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" sqref="K76 K36 K40 K32 K28 K4 K12 K8 K48 K44 K52 K60 K56 K64 K68 K72 K80 K20 K24 K16 K84 K88 K92 K96 K100 K104">
+    <dataValidation type="list" allowBlank="1" sqref="K76 K36 K40 K32 K28 K4 K12 K8 K48 K44 K52 K60 K56 K64 K68 K72 K80 K20 K24 K16 K84 K88 K92 K96 K100 K104 K108 K112">
       <formula1>"Smoke,Regresión"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
Agrego Casos de Prueba referentes a la Gestion de Productos de la web
</commit_message>
<xml_diff>
--- a/Testing 2024/template_caso_prueba-ISPC2024-sprint-1.xlsx
+++ b/Testing 2024/template_caso_prueba-ISPC2024-sprint-1.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="444" uniqueCount="202">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="493" uniqueCount="226">
   <si>
     <t>Id</t>
   </si>
@@ -600,9 +600,6 @@
     <t>Visualización de Productos</t>
   </si>
   <si>
-    <t>El usuario (registrado o no) debe estar situado en la home page</t>
-  </si>
-  <si>
     <t>Visualizar las Categorias</t>
   </si>
   <si>
@@ -631,6 +628,81 @@
   </si>
   <si>
     <t>El usuario debe poder visualizar en la Home Page las Categorias disponibles</t>
+  </si>
+  <si>
+    <t>Gestion de productos</t>
+  </si>
+  <si>
+    <t>Agregar un libro al carrito</t>
+  </si>
+  <si>
+    <t>Agregar un libro al carrito de compras</t>
+  </si>
+  <si>
+    <t>El usuario hace click en el botón "agregar al carrito"</t>
+  </si>
+  <si>
+    <t>Se redirige al carrito de compras y se muestra el libro agregado, el precio total, un botón para eliminar el libro, la opción para seguir comprando y un botón de Iniciar compra</t>
+  </si>
+  <si>
+    <t>Generar compra</t>
+  </si>
+  <si>
+    <t>Una vez agregados los libros al carrito el usuario puede generar la compra</t>
+  </si>
+  <si>
+    <t>El usuario hace click en el botón "Iniciar compra"</t>
+  </si>
+  <si>
+    <t>Se redirige a la pagina para cargar los datos personales, los datos de envío y un botón "Pagar"</t>
+  </si>
+  <si>
+    <t>Seleccionar medio de pago</t>
+  </si>
+  <si>
+    <t>El usuario selecciona el medio de pago</t>
+  </si>
+  <si>
+    <t>El usuario hace click en el botón "Pagar"</t>
+  </si>
+  <si>
+    <t>Se redirige a la pagina para cargar los datos de la tarjeta, o el pago en el local, un  link para volver al carrito y un botón "Confirmar compra"</t>
+  </si>
+  <si>
+    <t>Confirmar compra</t>
+  </si>
+  <si>
+    <t xml:space="preserve">El usuario confirma la compra </t>
+  </si>
+  <si>
+    <t>El usuario hace click en el botón  "Confirmar compra"</t>
+  </si>
+  <si>
+    <t>Visualiza un mensaje de "pago realizado con éxito", el número de órden y un botón para volver al catálogo</t>
+  </si>
+  <si>
+    <t>TC-029</t>
+  </si>
+  <si>
+    <t>TC-030</t>
+  </si>
+  <si>
+    <t>TC-031</t>
+  </si>
+  <si>
+    <t>TC-032</t>
+  </si>
+  <si>
+    <t>El usuario debe estar situado en la página de detalle del producto</t>
+  </si>
+  <si>
+    <t>El usuario debe estar situado en la página de Carrito</t>
+  </si>
+  <si>
+    <t>El usuario debe estar situado en la página de Selección de envío</t>
+  </si>
+  <si>
+    <t>El usuario debe estar situado en la página de selección de medios de pago</t>
   </si>
 </sst>
 </file>
@@ -1089,7 +1161,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="92">
+  <cellXfs count="94">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -1192,6 +1264,11 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="7" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1201,11 +1278,6 @@
     <xf numFmtId="0" fontId="1" fillId="7" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1214,6 +1286,60 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="14" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="14" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="14" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="13" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="13" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="13" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="12" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1224,38 +1350,23 @@
     <xf numFmtId="0" fontId="1" fillId="12" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="10" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="10" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="10" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="10" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="11" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="11" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="11" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1272,53 +1383,20 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="11" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="11" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="13" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="11" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="13" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="13" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="14" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="14" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="14" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1900,8 +1978,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AA931"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A106" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="60" workbookViewId="0">
-      <selection activeCell="C119" sqref="C119"/>
+    <sheetView tabSelected="1" topLeftCell="F113" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="60" workbookViewId="0">
+      <selection activeCell="M130" sqref="M130"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5703125" defaultRowHeight="12.75"/>
@@ -1950,33 +2028,33 @@
       <c r="AA1" s="2"/>
     </row>
     <row r="2" spans="1:27" s="31" customFormat="1" ht="15.75" customHeight="1">
-      <c r="A2" s="76" t="s">
+      <c r="A2" s="82" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="69" t="s">
+      <c r="B2" s="80" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="76" t="s">
+      <c r="C2" s="82" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="69" t="s">
+      <c r="D2" s="80" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="69" t="s">
+      <c r="E2" s="80" t="s">
         <v>4</v>
       </c>
-      <c r="F2" s="71" t="s">
+      <c r="F2" s="84" t="s">
         <v>5</v>
       </c>
-      <c r="G2" s="72"/>
-      <c r="H2" s="73"/>
-      <c r="I2" s="74" t="s">
+      <c r="G2" s="85"/>
+      <c r="H2" s="86"/>
+      <c r="I2" s="87" t="s">
         <v>6</v>
       </c>
-      <c r="J2" s="69" t="s">
+      <c r="J2" s="80" t="s">
         <v>7</v>
       </c>
-      <c r="K2" s="69" t="s">
+      <c r="K2" s="80" t="s">
         <v>27</v>
       </c>
       <c r="L2" s="32"/>
@@ -1997,11 +2075,11 @@
       <c r="AA2" s="33"/>
     </row>
     <row r="3" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A3" s="77"/>
-      <c r="B3" s="70"/>
-      <c r="C3" s="77"/>
-      <c r="D3" s="70"/>
-      <c r="E3" s="70"/>
+      <c r="A3" s="83"/>
+      <c r="B3" s="81"/>
+      <c r="C3" s="83"/>
+      <c r="D3" s="81"/>
+      <c r="E3" s="81"/>
       <c r="F3" s="34" t="s">
         <v>8</v>
       </c>
@@ -2011,9 +2089,9 @@
       <c r="H3" s="42" t="s">
         <v>10</v>
       </c>
-      <c r="I3" s="75"/>
-      <c r="J3" s="70"/>
-      <c r="K3" s="70"/>
+      <c r="I3" s="88"/>
+      <c r="J3" s="81"/>
+      <c r="K3" s="81"/>
       <c r="L3" s="3"/>
       <c r="M3" s="2"/>
       <c r="N3" s="2"/>
@@ -2032,7 +2110,7 @@
       <c r="AA3" s="2"/>
     </row>
     <row r="4" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A4" s="63" t="s">
+      <c r="A4" s="66" t="s">
         <v>29</v>
       </c>
       <c r="B4" s="54" t="s">
@@ -2053,16 +2131,16 @@
       <c r="G4" s="54" t="s">
         <v>54</v>
       </c>
-      <c r="H4" s="78" t="s">
+      <c r="H4" s="60" t="s">
         <v>55</v>
       </c>
-      <c r="I4" s="51" t="s">
+      <c r="I4" s="48" t="s">
         <v>26</v>
       </c>
-      <c r="J4" s="48" t="s">
+      <c r="J4" s="51" t="s">
         <v>56</v>
       </c>
-      <c r="K4" s="51" t="s">
+      <c r="K4" s="48" t="s">
         <v>28</v>
       </c>
       <c r="L4" s="3"/>
@@ -2083,17 +2161,17 @@
       <c r="AA4" s="2"/>
     </row>
     <row r="5" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A5" s="64"/>
+      <c r="A5" s="67"/>
       <c r="B5" s="55"/>
       <c r="C5" s="55"/>
       <c r="D5" s="55"/>
       <c r="E5" s="55"/>
       <c r="F5" s="56"/>
       <c r="G5" s="56"/>
-      <c r="H5" s="79"/>
-      <c r="I5" s="52"/>
-      <c r="J5" s="49"/>
-      <c r="K5" s="52"/>
+      <c r="H5" s="62"/>
+      <c r="I5" s="49"/>
+      <c r="J5" s="52"/>
+      <c r="K5" s="49"/>
       <c r="L5" s="3"/>
       <c r="M5" s="2"/>
       <c r="N5" s="2"/>
@@ -2112,7 +2190,7 @@
       <c r="AA5" s="2"/>
     </row>
     <row r="6" spans="1:27" s="29" customFormat="1" ht="15.75" customHeight="1">
-      <c r="A6" s="64"/>
+      <c r="A6" s="67"/>
       <c r="B6" s="55"/>
       <c r="C6" s="55"/>
       <c r="D6" s="55"/>
@@ -2120,9 +2198,9 @@
       <c r="F6" s="30"/>
       <c r="G6" s="35"/>
       <c r="H6" s="35"/>
-      <c r="I6" s="52"/>
-      <c r="J6" s="49"/>
-      <c r="K6" s="52"/>
+      <c r="I6" s="49"/>
+      <c r="J6" s="52"/>
+      <c r="K6" s="49"/>
       <c r="L6" s="27"/>
       <c r="M6" s="28"/>
       <c r="N6" s="28"/>
@@ -2141,7 +2219,7 @@
       <c r="AA6" s="28"/>
     </row>
     <row r="7" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A7" s="65"/>
+      <c r="A7" s="68"/>
       <c r="B7" s="56"/>
       <c r="C7" s="56"/>
       <c r="D7" s="56"/>
@@ -2149,9 +2227,9 @@
       <c r="F7" s="30"/>
       <c r="G7" s="35"/>
       <c r="H7" s="35"/>
-      <c r="I7" s="53"/>
-      <c r="J7" s="50"/>
-      <c r="K7" s="53"/>
+      <c r="I7" s="50"/>
+      <c r="J7" s="53"/>
+      <c r="K7" s="50"/>
       <c r="L7" s="3"/>
       <c r="M7" s="2"/>
       <c r="N7" s="2"/>
@@ -2170,7 +2248,7 @@
       <c r="AA7" s="2"/>
     </row>
     <row r="8" spans="1:27">
-      <c r="A8" s="63" t="s">
+      <c r="A8" s="66" t="s">
         <v>30</v>
       </c>
       <c r="B8" s="54" t="s">
@@ -2191,16 +2269,16 @@
       <c r="G8" s="54" t="s">
         <v>54</v>
       </c>
-      <c r="H8" s="78" t="s">
+      <c r="H8" s="60" t="s">
         <v>55</v>
       </c>
-      <c r="I8" s="51" t="s">
+      <c r="I8" s="48" t="s">
         <v>26</v>
       </c>
-      <c r="J8" s="48" t="s">
+      <c r="J8" s="51" t="s">
         <v>56</v>
       </c>
-      <c r="K8" s="51" t="s">
+      <c r="K8" s="48" t="s">
         <v>28</v>
       </c>
       <c r="L8" s="3"/>
@@ -2221,17 +2299,17 @@
       <c r="AA8" s="2"/>
     </row>
     <row r="9" spans="1:27">
-      <c r="A9" s="64"/>
+      <c r="A9" s="67"/>
       <c r="B9" s="55"/>
       <c r="C9" s="55"/>
       <c r="D9" s="55"/>
       <c r="E9" s="55"/>
       <c r="F9" s="56"/>
       <c r="G9" s="56"/>
-      <c r="H9" s="79"/>
-      <c r="I9" s="52"/>
-      <c r="J9" s="49"/>
-      <c r="K9" s="52"/>
+      <c r="H9" s="62"/>
+      <c r="I9" s="49"/>
+      <c r="J9" s="52"/>
+      <c r="K9" s="49"/>
       <c r="L9" s="3"/>
       <c r="M9" s="2"/>
       <c r="N9" s="2"/>
@@ -2250,7 +2328,7 @@
       <c r="AA9" s="2"/>
     </row>
     <row r="10" spans="1:27" s="29" customFormat="1" ht="15.75" customHeight="1">
-      <c r="A10" s="64"/>
+      <c r="A10" s="67"/>
       <c r="B10" s="55"/>
       <c r="C10" s="55"/>
       <c r="D10" s="55"/>
@@ -2258,9 +2336,9 @@
       <c r="F10" s="30"/>
       <c r="G10" s="35"/>
       <c r="H10" s="35"/>
-      <c r="I10" s="52"/>
-      <c r="J10" s="49"/>
-      <c r="K10" s="52"/>
+      <c r="I10" s="49"/>
+      <c r="J10" s="52"/>
+      <c r="K10" s="49"/>
       <c r="L10" s="27"/>
       <c r="M10" s="28"/>
       <c r="N10" s="28"/>
@@ -2279,7 +2357,7 @@
       <c r="AA10" s="28"/>
     </row>
     <row r="11" spans="1:27">
-      <c r="A11" s="65"/>
+      <c r="A11" s="68"/>
       <c r="B11" s="56"/>
       <c r="C11" s="56"/>
       <c r="D11" s="56"/>
@@ -2287,9 +2365,9 @@
       <c r="F11" s="30"/>
       <c r="G11" s="35"/>
       <c r="H11" s="35"/>
-      <c r="I11" s="53"/>
-      <c r="J11" s="50"/>
-      <c r="K11" s="53"/>
+      <c r="I11" s="50"/>
+      <c r="J11" s="53"/>
+      <c r="K11" s="50"/>
       <c r="L11" s="3"/>
       <c r="M11" s="2"/>
       <c r="N11" s="2"/>
@@ -2308,7 +2386,7 @@
       <c r="AA11" s="2"/>
     </row>
     <row r="12" spans="1:27">
-      <c r="A12" s="63" t="s">
+      <c r="A12" s="66" t="s">
         <v>31</v>
       </c>
       <c r="B12" s="54" t="s">
@@ -2329,16 +2407,16 @@
       <c r="G12" s="54" t="s">
         <v>54</v>
       </c>
-      <c r="H12" s="78" t="s">
+      <c r="H12" s="60" t="s">
         <v>55</v>
       </c>
-      <c r="I12" s="51" t="s">
+      <c r="I12" s="48" t="s">
         <v>26</v>
       </c>
-      <c r="J12" s="48" t="s">
+      <c r="J12" s="51" t="s">
         <v>56</v>
       </c>
-      <c r="K12" s="51" t="s">
+      <c r="K12" s="48" t="s">
         <v>28</v>
       </c>
       <c r="L12" s="2"/>
@@ -2359,17 +2437,17 @@
       <c r="AA12" s="2"/>
     </row>
     <row r="13" spans="1:27">
-      <c r="A13" s="64"/>
+      <c r="A13" s="67"/>
       <c r="B13" s="55"/>
       <c r="C13" s="55"/>
       <c r="D13" s="55"/>
       <c r="E13" s="55"/>
       <c r="F13" s="56"/>
       <c r="G13" s="56"/>
-      <c r="H13" s="79"/>
-      <c r="I13" s="52"/>
-      <c r="J13" s="49"/>
-      <c r="K13" s="52"/>
+      <c r="H13" s="62"/>
+      <c r="I13" s="49"/>
+      <c r="J13" s="52"/>
+      <c r="K13" s="49"/>
       <c r="L13" s="2"/>
       <c r="M13" s="2"/>
       <c r="N13" s="2"/>
@@ -2388,7 +2466,7 @@
       <c r="AA13" s="2"/>
     </row>
     <row r="14" spans="1:27" s="29" customFormat="1">
-      <c r="A14" s="64"/>
+      <c r="A14" s="67"/>
       <c r="B14" s="55"/>
       <c r="C14" s="55"/>
       <c r="D14" s="55"/>
@@ -2396,9 +2474,9 @@
       <c r="F14" s="30"/>
       <c r="G14" s="35"/>
       <c r="H14" s="35"/>
-      <c r="I14" s="52"/>
-      <c r="J14" s="49"/>
-      <c r="K14" s="52"/>
+      <c r="I14" s="49"/>
+      <c r="J14" s="52"/>
+      <c r="K14" s="49"/>
       <c r="L14" s="28"/>
       <c r="M14" s="28"/>
       <c r="N14" s="28"/>
@@ -2417,7 +2495,7 @@
       <c r="AA14" s="28"/>
     </row>
     <row r="15" spans="1:27">
-      <c r="A15" s="65"/>
+      <c r="A15" s="68"/>
       <c r="B15" s="56"/>
       <c r="C15" s="56"/>
       <c r="D15" s="56"/>
@@ -2425,9 +2503,9 @@
       <c r="F15" s="30"/>
       <c r="G15" s="35"/>
       <c r="H15" s="35"/>
-      <c r="I15" s="53"/>
-      <c r="J15" s="50"/>
-      <c r="K15" s="53"/>
+      <c r="I15" s="50"/>
+      <c r="J15" s="53"/>
+      <c r="K15" s="50"/>
       <c r="L15" s="2"/>
       <c r="M15" s="2"/>
       <c r="N15" s="2"/>
@@ -2446,7 +2524,7 @@
       <c r="AA15" s="2"/>
     </row>
     <row r="16" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A16" s="66" t="s">
+      <c r="A16" s="89" t="s">
         <v>32</v>
       </c>
       <c r="B16" s="54" t="s">
@@ -2470,13 +2548,13 @@
       <c r="H16" s="35" t="s">
         <v>66</v>
       </c>
-      <c r="I16" s="51" t="s">
+      <c r="I16" s="48" t="s">
         <v>26</v>
       </c>
-      <c r="J16" s="48" t="s">
+      <c r="J16" s="51" t="s">
         <v>56</v>
       </c>
-      <c r="K16" s="51" t="s">
+      <c r="K16" s="48" t="s">
         <v>28</v>
       </c>
       <c r="L16" s="2"/>
@@ -2497,7 +2575,7 @@
       <c r="AA16" s="2"/>
     </row>
     <row r="17" spans="1:27" ht="16.5" customHeight="1">
-      <c r="A17" s="67"/>
+      <c r="A17" s="90"/>
       <c r="B17" s="55"/>
       <c r="C17" s="55"/>
       <c r="D17" s="55"/>
@@ -2511,9 +2589,9 @@
       <c r="H17" s="35" t="s">
         <v>69</v>
       </c>
-      <c r="I17" s="52"/>
-      <c r="J17" s="49"/>
-      <c r="K17" s="52"/>
+      <c r="I17" s="49"/>
+      <c r="J17" s="52"/>
+      <c r="K17" s="49"/>
       <c r="L17" s="2"/>
       <c r="M17" s="2"/>
       <c r="N17" s="2"/>
@@ -2532,7 +2610,7 @@
       <c r="AA17" s="2"/>
     </row>
     <row r="18" spans="1:27" s="29" customFormat="1" ht="25.5">
-      <c r="A18" s="67"/>
+      <c r="A18" s="90"/>
       <c r="B18" s="55"/>
       <c r="C18" s="55"/>
       <c r="D18" s="55"/>
@@ -2546,9 +2624,9 @@
       <c r="H18" s="35" t="s">
         <v>72</v>
       </c>
-      <c r="I18" s="52"/>
-      <c r="J18" s="49"/>
-      <c r="K18" s="52"/>
+      <c r="I18" s="49"/>
+      <c r="J18" s="52"/>
+      <c r="K18" s="49"/>
       <c r="L18" s="28"/>
       <c r="M18" s="28"/>
       <c r="N18" s="28"/>
@@ -2567,7 +2645,7 @@
       <c r="AA18" s="28"/>
     </row>
     <row r="19" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A19" s="68"/>
+      <c r="A19" s="91"/>
       <c r="B19" s="56"/>
       <c r="C19" s="56"/>
       <c r="D19" s="56"/>
@@ -2575,9 +2653,9 @@
       <c r="F19" s="30"/>
       <c r="G19" s="35"/>
       <c r="H19" s="35"/>
-      <c r="I19" s="53"/>
-      <c r="J19" s="50"/>
-      <c r="K19" s="53"/>
+      <c r="I19" s="50"/>
+      <c r="J19" s="53"/>
+      <c r="K19" s="50"/>
       <c r="L19" s="2"/>
       <c r="M19" s="2"/>
       <c r="N19" s="2"/>
@@ -2596,13 +2674,13 @@
       <c r="AA19" s="2"/>
     </row>
     <row r="20" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A20" s="66" t="s">
+      <c r="A20" s="89" t="s">
         <v>33</v>
       </c>
       <c r="B20" s="54" t="s">
         <v>63</v>
       </c>
-      <c r="C20" s="60" t="s">
+      <c r="C20" s="69" t="s">
         <v>73</v>
       </c>
       <c r="D20" s="54" t="s">
@@ -2620,13 +2698,13 @@
       <c r="H20" s="35" t="s">
         <v>76</v>
       </c>
-      <c r="I20" s="51" t="s">
+      <c r="I20" s="48" t="s">
         <v>26</v>
       </c>
-      <c r="J20" s="48" t="s">
+      <c r="J20" s="51" t="s">
         <v>56</v>
       </c>
-      <c r="K20" s="51" t="s">
+      <c r="K20" s="48" t="s">
         <v>28</v>
       </c>
       <c r="L20" s="2"/>
@@ -2647,9 +2725,9 @@
       <c r="AA20" s="2"/>
     </row>
     <row r="21" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A21" s="67"/>
+      <c r="A21" s="90"/>
       <c r="B21" s="55"/>
-      <c r="C21" s="61"/>
+      <c r="C21" s="78"/>
       <c r="D21" s="55"/>
       <c r="E21" s="55"/>
       <c r="F21" s="30" t="s">
@@ -2659,9 +2737,9 @@
         <v>77</v>
       </c>
       <c r="H21" s="35"/>
-      <c r="I21" s="52"/>
-      <c r="J21" s="49"/>
-      <c r="K21" s="52"/>
+      <c r="I21" s="49"/>
+      <c r="J21" s="52"/>
+      <c r="K21" s="49"/>
       <c r="L21" s="2"/>
       <c r="M21" s="2"/>
       <c r="N21" s="2"/>
@@ -2680,9 +2758,9 @@
       <c r="AA21" s="2"/>
     </row>
     <row r="22" spans="1:27" s="29" customFormat="1" ht="15.75" customHeight="1">
-      <c r="A22" s="67"/>
+      <c r="A22" s="90"/>
       <c r="B22" s="55"/>
-      <c r="C22" s="61"/>
+      <c r="C22" s="78"/>
       <c r="D22" s="55"/>
       <c r="E22" s="55"/>
       <c r="F22" s="30" t="s">
@@ -2694,9 +2772,9 @@
       <c r="H22" s="35" t="s">
         <v>79</v>
       </c>
-      <c r="I22" s="52"/>
-      <c r="J22" s="49"/>
-      <c r="K22" s="52"/>
+      <c r="I22" s="49"/>
+      <c r="J22" s="52"/>
+      <c r="K22" s="49"/>
       <c r="L22" s="28"/>
       <c r="M22" s="28"/>
       <c r="N22" s="28"/>
@@ -2715,17 +2793,17 @@
       <c r="AA22" s="28"/>
     </row>
     <row r="23" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A23" s="68"/>
+      <c r="A23" s="91"/>
       <c r="B23" s="56"/>
-      <c r="C23" s="62"/>
+      <c r="C23" s="79"/>
       <c r="D23" s="56"/>
       <c r="E23" s="56"/>
       <c r="F23" s="30"/>
       <c r="G23" s="35"/>
       <c r="H23" s="35"/>
-      <c r="I23" s="53"/>
-      <c r="J23" s="50"/>
-      <c r="K23" s="53"/>
+      <c r="I23" s="50"/>
+      <c r="J23" s="53"/>
+      <c r="K23" s="50"/>
       <c r="L23" s="2"/>
       <c r="M23" s="2"/>
       <c r="N23" s="2"/>
@@ -2744,13 +2822,13 @@
       <c r="AA23" s="2"/>
     </row>
     <row r="24" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A24" s="66" t="s">
+      <c r="A24" s="89" t="s">
         <v>34</v>
       </c>
       <c r="B24" s="54" t="s">
         <v>63</v>
       </c>
-      <c r="C24" s="60" t="s">
+      <c r="C24" s="69" t="s">
         <v>80</v>
       </c>
       <c r="D24" s="54" t="s">
@@ -2768,13 +2846,13 @@
       <c r="H24" s="35" t="s">
         <v>76</v>
       </c>
-      <c r="I24" s="51" t="s">
+      <c r="I24" s="48" t="s">
         <v>26</v>
       </c>
-      <c r="J24" s="48" t="s">
+      <c r="J24" s="51" t="s">
         <v>56</v>
       </c>
-      <c r="K24" s="51" t="s">
+      <c r="K24" s="48" t="s">
         <v>28</v>
       </c>
       <c r="L24" s="2"/>
@@ -2795,9 +2873,9 @@
       <c r="AA24" s="2"/>
     </row>
     <row r="25" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A25" s="67"/>
+      <c r="A25" s="90"/>
       <c r="B25" s="55"/>
-      <c r="C25" s="61"/>
+      <c r="C25" s="78"/>
       <c r="D25" s="55"/>
       <c r="E25" s="55"/>
       <c r="F25" s="30" t="s">
@@ -2807,9 +2885,9 @@
         <v>77</v>
       </c>
       <c r="H25" s="35"/>
-      <c r="I25" s="52"/>
-      <c r="J25" s="49"/>
-      <c r="K25" s="52"/>
+      <c r="I25" s="49"/>
+      <c r="J25" s="52"/>
+      <c r="K25" s="49"/>
       <c r="L25" s="2"/>
       <c r="M25" s="2"/>
       <c r="N25" s="2"/>
@@ -2828,9 +2906,9 @@
       <c r="AA25" s="2"/>
     </row>
     <row r="26" spans="1:27" s="29" customFormat="1" ht="25.5">
-      <c r="A26" s="67"/>
+      <c r="A26" s="90"/>
       <c r="B26" s="55"/>
-      <c r="C26" s="61"/>
+      <c r="C26" s="78"/>
       <c r="D26" s="55"/>
       <c r="E26" s="55"/>
       <c r="F26" s="30" t="s">
@@ -2842,9 +2920,9 @@
       <c r="H26" s="35" t="s">
         <v>82</v>
       </c>
-      <c r="I26" s="52"/>
-      <c r="J26" s="49"/>
-      <c r="K26" s="52"/>
+      <c r="I26" s="49"/>
+      <c r="J26" s="52"/>
+      <c r="K26" s="49"/>
       <c r="L26" s="28"/>
       <c r="M26" s="28"/>
       <c r="N26" s="28"/>
@@ -2863,17 +2941,17 @@
       <c r="AA26" s="28"/>
     </row>
     <row r="27" spans="1:27" ht="18.75" customHeight="1">
-      <c r="A27" s="68"/>
+      <c r="A27" s="91"/>
       <c r="B27" s="56"/>
-      <c r="C27" s="62"/>
+      <c r="C27" s="79"/>
       <c r="D27" s="56"/>
       <c r="E27" s="56"/>
       <c r="F27" s="30"/>
       <c r="G27" s="35"/>
       <c r="H27" s="35"/>
-      <c r="I27" s="53"/>
-      <c r="J27" s="50"/>
-      <c r="K27" s="53"/>
+      <c r="I27" s="50"/>
+      <c r="J27" s="53"/>
+      <c r="K27" s="50"/>
       <c r="L27" s="2"/>
       <c r="M27" s="2"/>
       <c r="N27" s="2"/>
@@ -2892,7 +2970,7 @@
       <c r="AA27" s="2"/>
     </row>
     <row r="28" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A28" s="57" t="s">
+      <c r="A28" s="75" t="s">
         <v>35</v>
       </c>
       <c r="B28" s="54" t="s">
@@ -2916,13 +2994,13 @@
       <c r="H28" s="35" t="s">
         <v>88</v>
       </c>
-      <c r="I28" s="51" t="s">
+      <c r="I28" s="48" t="s">
         <v>26</v>
       </c>
-      <c r="J28" s="48" t="s">
+      <c r="J28" s="51" t="s">
         <v>56</v>
       </c>
-      <c r="K28" s="51" t="s">
+      <c r="K28" s="48" t="s">
         <v>28</v>
       </c>
       <c r="L28" s="2"/>
@@ -2943,7 +3021,7 @@
       <c r="AA28" s="2"/>
     </row>
     <row r="29" spans="1:27">
-      <c r="A29" s="58"/>
+      <c r="A29" s="76"/>
       <c r="B29" s="55"/>
       <c r="C29" s="55"/>
       <c r="D29" s="55"/>
@@ -2953,9 +3031,9 @@
       </c>
       <c r="G29" s="35"/>
       <c r="H29" s="35"/>
-      <c r="I29" s="52"/>
-      <c r="J29" s="49"/>
-      <c r="K29" s="52"/>
+      <c r="I29" s="49"/>
+      <c r="J29" s="52"/>
+      <c r="K29" s="49"/>
       <c r="L29" s="2"/>
       <c r="M29" s="2"/>
       <c r="N29" s="2"/>
@@ -2974,7 +3052,7 @@
       <c r="AA29" s="2"/>
     </row>
     <row r="30" spans="1:27" s="29" customFormat="1" ht="15.75" customHeight="1">
-      <c r="A30" s="58"/>
+      <c r="A30" s="76"/>
       <c r="B30" s="55"/>
       <c r="C30" s="55"/>
       <c r="D30" s="55"/>
@@ -2982,9 +3060,9 @@
       <c r="F30" s="30"/>
       <c r="G30" s="35"/>
       <c r="H30" s="35"/>
-      <c r="I30" s="52"/>
-      <c r="J30" s="49"/>
-      <c r="K30" s="52"/>
+      <c r="I30" s="49"/>
+      <c r="J30" s="52"/>
+      <c r="K30" s="49"/>
       <c r="L30" s="28"/>
       <c r="M30" s="28"/>
       <c r="N30" s="28"/>
@@ -3003,7 +3081,7 @@
       <c r="AA30" s="28"/>
     </row>
     <row r="31" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A31" s="59"/>
+      <c r="A31" s="77"/>
       <c r="B31" s="56"/>
       <c r="C31" s="56"/>
       <c r="D31" s="56"/>
@@ -3011,9 +3089,9 @@
       <c r="F31" s="30"/>
       <c r="G31" s="35"/>
       <c r="H31" s="35"/>
-      <c r="I31" s="53"/>
-      <c r="J31" s="50"/>
-      <c r="K31" s="53"/>
+      <c r="I31" s="50"/>
+      <c r="J31" s="53"/>
+      <c r="K31" s="50"/>
       <c r="L31" s="2"/>
       <c r="M31" s="2"/>
       <c r="N31" s="2"/>
@@ -3032,7 +3110,7 @@
       <c r="AA31" s="2"/>
     </row>
     <row r="32" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A32" s="57" t="s">
+      <c r="A32" s="75" t="s">
         <v>36</v>
       </c>
       <c r="B32" s="54" t="s">
@@ -3056,13 +3134,13 @@
       <c r="H32" s="35" t="s">
         <v>92</v>
       </c>
-      <c r="I32" s="51" t="s">
+      <c r="I32" s="48" t="s">
         <v>26</v>
       </c>
-      <c r="J32" s="48" t="s">
+      <c r="J32" s="51" t="s">
         <v>56</v>
       </c>
-      <c r="K32" s="51" t="s">
+      <c r="K32" s="48" t="s">
         <v>28</v>
       </c>
       <c r="L32" s="2"/>
@@ -3083,7 +3161,7 @@
       <c r="AA32" s="2"/>
     </row>
     <row r="33" spans="1:27">
-      <c r="A33" s="58"/>
+      <c r="A33" s="76"/>
       <c r="B33" s="55"/>
       <c r="C33" s="55"/>
       <c r="D33" s="55"/>
@@ -3091,9 +3169,9 @@
       <c r="F33" s="30"/>
       <c r="G33" s="43"/>
       <c r="H33" s="43"/>
-      <c r="I33" s="52"/>
-      <c r="J33" s="49"/>
-      <c r="K33" s="52"/>
+      <c r="I33" s="49"/>
+      <c r="J33" s="52"/>
+      <c r="K33" s="49"/>
       <c r="L33" s="2"/>
       <c r="M33" s="2"/>
       <c r="N33" s="2"/>
@@ -3112,7 +3190,7 @@
       <c r="AA33" s="2"/>
     </row>
     <row r="34" spans="1:27">
-      <c r="A34" s="58"/>
+      <c r="A34" s="76"/>
       <c r="B34" s="55"/>
       <c r="C34" s="55"/>
       <c r="D34" s="55"/>
@@ -3120,9 +3198,9 @@
       <c r="F34" s="30"/>
       <c r="G34" s="43"/>
       <c r="H34" s="43"/>
-      <c r="I34" s="52"/>
-      <c r="J34" s="49"/>
-      <c r="K34" s="52"/>
+      <c r="I34" s="49"/>
+      <c r="J34" s="52"/>
+      <c r="K34" s="49"/>
       <c r="L34" s="2"/>
       <c r="M34" s="2"/>
       <c r="N34" s="2"/>
@@ -3141,7 +3219,7 @@
       <c r="AA34" s="2"/>
     </row>
     <row r="35" spans="1:27">
-      <c r="A35" s="59"/>
+      <c r="A35" s="77"/>
       <c r="B35" s="56"/>
       <c r="C35" s="56"/>
       <c r="D35" s="56"/>
@@ -3149,9 +3227,9 @@
       <c r="F35" s="30"/>
       <c r="G35" s="35"/>
       <c r="H35" s="35"/>
-      <c r="I35" s="53"/>
-      <c r="J35" s="50"/>
-      <c r="K35" s="53"/>
+      <c r="I35" s="50"/>
+      <c r="J35" s="53"/>
+      <c r="K35" s="50"/>
       <c r="L35" s="2"/>
       <c r="M35" s="2"/>
       <c r="N35" s="2"/>
@@ -3170,7 +3248,7 @@
       <c r="AA35" s="2"/>
     </row>
     <row r="36" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A36" s="57" t="s">
+      <c r="A36" s="75" t="s">
         <v>37</v>
       </c>
       <c r="B36" s="54" t="s">
@@ -3194,13 +3272,13 @@
       <c r="H36" s="35" t="s">
         <v>92</v>
       </c>
-      <c r="I36" s="51" t="s">
+      <c r="I36" s="48" t="s">
         <v>26</v>
       </c>
-      <c r="J36" s="48" t="s">
+      <c r="J36" s="51" t="s">
         <v>56</v>
       </c>
-      <c r="K36" s="51" t="s">
+      <c r="K36" s="48" t="s">
         <v>28</v>
       </c>
       <c r="L36" s="2"/>
@@ -3221,7 +3299,7 @@
       <c r="AA36" s="2"/>
     </row>
     <row r="37" spans="1:27" ht="25.5">
-      <c r="A37" s="58"/>
+      <c r="A37" s="76"/>
       <c r="B37" s="55"/>
       <c r="C37" s="55"/>
       <c r="D37" s="55"/>
@@ -3233,9 +3311,9 @@
         <v>96</v>
       </c>
       <c r="H37" s="35"/>
-      <c r="I37" s="52"/>
-      <c r="J37" s="49"/>
-      <c r="K37" s="52"/>
+      <c r="I37" s="49"/>
+      <c r="J37" s="52"/>
+      <c r="K37" s="49"/>
       <c r="L37" s="2"/>
       <c r="M37" s="2"/>
       <c r="N37" s="2"/>
@@ -3254,7 +3332,7 @@
       <c r="AA37" s="2"/>
     </row>
     <row r="38" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A38" s="58"/>
+      <c r="A38" s="76"/>
       <c r="B38" s="55"/>
       <c r="C38" s="55"/>
       <c r="D38" s="55"/>
@@ -3268,9 +3346,9 @@
       <c r="H38" s="35" t="s">
         <v>98</v>
       </c>
-      <c r="I38" s="52"/>
-      <c r="J38" s="49"/>
-      <c r="K38" s="52"/>
+      <c r="I38" s="49"/>
+      <c r="J38" s="52"/>
+      <c r="K38" s="49"/>
       <c r="L38" s="2"/>
       <c r="M38" s="2"/>
       <c r="N38" s="2"/>
@@ -3289,7 +3367,7 @@
       <c r="AA38" s="2"/>
     </row>
     <row r="39" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A39" s="59"/>
+      <c r="A39" s="77"/>
       <c r="B39" s="56"/>
       <c r="C39" s="56"/>
       <c r="D39" s="56"/>
@@ -3299,9 +3377,9 @@
       </c>
       <c r="G39" s="35"/>
       <c r="H39" s="35"/>
-      <c r="I39" s="53"/>
-      <c r="J39" s="50"/>
-      <c r="K39" s="53"/>
+      <c r="I39" s="50"/>
+      <c r="J39" s="53"/>
+      <c r="K39" s="50"/>
       <c r="L39" s="2"/>
       <c r="M39" s="2"/>
       <c r="N39" s="2"/>
@@ -3320,7 +3398,7 @@
       <c r="AA39" s="2"/>
     </row>
     <row r="40" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A40" s="57" t="s">
+      <c r="A40" s="75" t="s">
         <v>38</v>
       </c>
       <c r="B40" s="54" t="s">
@@ -3344,13 +3422,13 @@
       <c r="H40" s="35" t="s">
         <v>88</v>
       </c>
-      <c r="I40" s="51" t="s">
+      <c r="I40" s="48" t="s">
         <v>26</v>
       </c>
-      <c r="J40" s="48" t="s">
+      <c r="J40" s="51" t="s">
         <v>56</v>
       </c>
-      <c r="K40" s="51" t="s">
+      <c r="K40" s="48" t="s">
         <v>28</v>
       </c>
       <c r="L40" s="2"/>
@@ -3371,7 +3449,7 @@
       <c r="AA40" s="2"/>
     </row>
     <row r="41" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A41" s="58"/>
+      <c r="A41" s="76"/>
       <c r="B41" s="55"/>
       <c r="C41" s="55"/>
       <c r="D41" s="55"/>
@@ -3383,9 +3461,9 @@
         <v>103</v>
       </c>
       <c r="H41" s="35"/>
-      <c r="I41" s="52"/>
-      <c r="J41" s="49"/>
-      <c r="K41" s="52"/>
+      <c r="I41" s="49"/>
+      <c r="J41" s="52"/>
+      <c r="K41" s="49"/>
       <c r="L41" s="2"/>
       <c r="M41" s="2"/>
       <c r="N41" s="2"/>
@@ -3404,7 +3482,7 @@
       <c r="AA41" s="2"/>
     </row>
     <row r="42" spans="1:27" ht="16.5" customHeight="1">
-      <c r="A42" s="58"/>
+      <c r="A42" s="76"/>
       <c r="B42" s="55"/>
       <c r="C42" s="55"/>
       <c r="D42" s="55"/>
@@ -3418,9 +3496,9 @@
       <c r="H42" s="35" t="s">
         <v>105</v>
       </c>
-      <c r="I42" s="52"/>
-      <c r="J42" s="49"/>
-      <c r="K42" s="52"/>
+      <c r="I42" s="49"/>
+      <c r="J42" s="52"/>
+      <c r="K42" s="49"/>
       <c r="L42" s="2"/>
       <c r="M42" s="2"/>
       <c r="N42" s="2"/>
@@ -3439,7 +3517,7 @@
       <c r="AA42" s="2"/>
     </row>
     <row r="43" spans="1:27" ht="18.75" customHeight="1">
-      <c r="A43" s="59"/>
+      <c r="A43" s="77"/>
       <c r="B43" s="56"/>
       <c r="C43" s="56"/>
       <c r="D43" s="56"/>
@@ -3449,9 +3527,9 @@
       </c>
       <c r="G43" s="35"/>
       <c r="H43" s="35"/>
-      <c r="I43" s="53"/>
-      <c r="J43" s="50"/>
-      <c r="K43" s="53"/>
+      <c r="I43" s="50"/>
+      <c r="J43" s="53"/>
+      <c r="K43" s="50"/>
       <c r="L43" s="2"/>
       <c r="M43" s="2"/>
       <c r="N43" s="2"/>
@@ -3470,7 +3548,7 @@
       <c r="AA43" s="2"/>
     </row>
     <row r="44" spans="1:27" ht="25.5">
-      <c r="A44" s="57" t="s">
+      <c r="A44" s="75" t="s">
         <v>39</v>
       </c>
       <c r="B44" s="54" t="s">
@@ -3494,13 +3572,13 @@
       <c r="H44" s="35" t="s">
         <v>88</v>
       </c>
-      <c r="I44" s="51" t="s">
+      <c r="I44" s="48" t="s">
         <v>26</v>
       </c>
-      <c r="J44" s="48" t="s">
+      <c r="J44" s="51" t="s">
         <v>56</v>
       </c>
-      <c r="K44" s="51" t="s">
+      <c r="K44" s="48" t="s">
         <v>28</v>
       </c>
       <c r="L44" s="2"/>
@@ -3521,7 +3599,7 @@
       <c r="AA44" s="2"/>
     </row>
     <row r="45" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A45" s="58"/>
+      <c r="A45" s="76"/>
       <c r="B45" s="55"/>
       <c r="C45" s="55"/>
       <c r="D45" s="55"/>
@@ -3533,9 +3611,9 @@
         <v>109</v>
       </c>
       <c r="H45" s="35"/>
-      <c r="I45" s="52"/>
-      <c r="J45" s="49"/>
-      <c r="K45" s="52"/>
+      <c r="I45" s="49"/>
+      <c r="J45" s="52"/>
+      <c r="K45" s="49"/>
       <c r="L45" s="2"/>
       <c r="M45" s="2"/>
       <c r="N45" s="2"/>
@@ -3554,7 +3632,7 @@
       <c r="AA45" s="2"/>
     </row>
     <row r="46" spans="1:27" ht="25.5">
-      <c r="A46" s="58"/>
+      <c r="A46" s="76"/>
       <c r="B46" s="55"/>
       <c r="C46" s="55"/>
       <c r="D46" s="55"/>
@@ -3568,9 +3646,9 @@
       <c r="H46" s="35" t="s">
         <v>110</v>
       </c>
-      <c r="I46" s="52"/>
-      <c r="J46" s="49"/>
-      <c r="K46" s="52"/>
+      <c r="I46" s="49"/>
+      <c r="J46" s="52"/>
+      <c r="K46" s="49"/>
       <c r="L46" s="2"/>
       <c r="M46" s="2"/>
       <c r="N46" s="2"/>
@@ -3589,7 +3667,7 @@
       <c r="AA46" s="2"/>
     </row>
     <row r="47" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A47" s="59"/>
+      <c r="A47" s="77"/>
       <c r="B47" s="56"/>
       <c r="C47" s="56"/>
       <c r="D47" s="56"/>
@@ -3599,9 +3677,9 @@
       </c>
       <c r="G47" s="35"/>
       <c r="H47" s="36"/>
-      <c r="I47" s="53"/>
-      <c r="J47" s="50"/>
-      <c r="K47" s="53"/>
+      <c r="I47" s="50"/>
+      <c r="J47" s="53"/>
+      <c r="K47" s="50"/>
       <c r="L47" s="2"/>
       <c r="M47" s="2"/>
       <c r="N47" s="2"/>
@@ -3620,7 +3698,7 @@
       <c r="AA47" s="2"/>
     </row>
     <row r="48" spans="1:27" ht="25.5">
-      <c r="A48" s="57" t="s">
+      <c r="A48" s="75" t="s">
         <v>40</v>
       </c>
       <c r="B48" s="54" t="s">
@@ -3644,13 +3722,13 @@
       <c r="H48" s="35" t="s">
         <v>88</v>
       </c>
-      <c r="I48" s="51" t="s">
+      <c r="I48" s="48" t="s">
         <v>26</v>
       </c>
-      <c r="J48" s="48" t="s">
+      <c r="J48" s="51" t="s">
         <v>56</v>
       </c>
-      <c r="K48" s="51" t="s">
+      <c r="K48" s="48" t="s">
         <v>28</v>
       </c>
       <c r="L48" s="2"/>
@@ -3671,7 +3749,7 @@
       <c r="AA48" s="2"/>
     </row>
     <row r="49" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A49" s="58"/>
+      <c r="A49" s="76"/>
       <c r="B49" s="55"/>
       <c r="C49" s="55"/>
       <c r="D49" s="55"/>
@@ -3683,9 +3761,9 @@
         <v>113</v>
       </c>
       <c r="H49" s="35"/>
-      <c r="I49" s="52"/>
-      <c r="J49" s="49"/>
-      <c r="K49" s="52"/>
+      <c r="I49" s="49"/>
+      <c r="J49" s="52"/>
+      <c r="K49" s="49"/>
       <c r="L49" s="2"/>
       <c r="M49" s="2"/>
       <c r="N49" s="2"/>
@@ -3704,7 +3782,7 @@
       <c r="AA49" s="2"/>
     </row>
     <row r="50" spans="1:27" ht="27" customHeight="1">
-      <c r="A50" s="58"/>
+      <c r="A50" s="76"/>
       <c r="B50" s="55"/>
       <c r="C50" s="55"/>
       <c r="D50" s="55"/>
@@ -3718,9 +3796,9 @@
       <c r="H50" s="35" t="s">
         <v>110</v>
       </c>
-      <c r="I50" s="52"/>
-      <c r="J50" s="49"/>
-      <c r="K50" s="52"/>
+      <c r="I50" s="49"/>
+      <c r="J50" s="52"/>
+      <c r="K50" s="49"/>
       <c r="L50" s="2"/>
       <c r="M50" s="2"/>
       <c r="N50" s="2"/>
@@ -3739,7 +3817,7 @@
       <c r="AA50" s="2"/>
     </row>
     <row r="51" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A51" s="59"/>
+      <c r="A51" s="77"/>
       <c r="B51" s="56"/>
       <c r="C51" s="56"/>
       <c r="D51" s="56"/>
@@ -3749,9 +3827,9 @@
       </c>
       <c r="G51" s="35"/>
       <c r="H51" s="36"/>
-      <c r="I51" s="53"/>
-      <c r="J51" s="50"/>
-      <c r="K51" s="53"/>
+      <c r="I51" s="50"/>
+      <c r="J51" s="53"/>
+      <c r="K51" s="50"/>
       <c r="L51" s="2"/>
       <c r="M51" s="2"/>
       <c r="N51" s="2"/>
@@ -3770,7 +3848,7 @@
       <c r="AA51" s="2"/>
     </row>
     <row r="52" spans="1:27" ht="25.5">
-      <c r="A52" s="57" t="s">
+      <c r="A52" s="75" t="s">
         <v>41</v>
       </c>
       <c r="B52" s="54" t="s">
@@ -3794,13 +3872,13 @@
       <c r="H52" s="35" t="s">
         <v>92</v>
       </c>
-      <c r="I52" s="51" t="s">
+      <c r="I52" s="48" t="s">
         <v>26</v>
       </c>
-      <c r="J52" s="48" t="s">
+      <c r="J52" s="51" t="s">
         <v>56</v>
       </c>
-      <c r="K52" s="51" t="s">
+      <c r="K52" s="48" t="s">
         <v>28</v>
       </c>
       <c r="L52" s="2"/>
@@ -3821,7 +3899,7 @@
       <c r="AA52" s="2"/>
     </row>
     <row r="53" spans="1:27" ht="25.5">
-      <c r="A53" s="58"/>
+      <c r="A53" s="76"/>
       <c r="B53" s="55"/>
       <c r="C53" s="55"/>
       <c r="D53" s="55"/>
@@ -3835,9 +3913,9 @@
       <c r="H53" s="36" t="s">
         <v>116</v>
       </c>
-      <c r="I53" s="52"/>
-      <c r="J53" s="49"/>
-      <c r="K53" s="52"/>
+      <c r="I53" s="49"/>
+      <c r="J53" s="52"/>
+      <c r="K53" s="49"/>
       <c r="L53" s="2"/>
       <c r="M53" s="2"/>
       <c r="N53" s="2"/>
@@ -3856,7 +3934,7 @@
       <c r="AA53" s="2"/>
     </row>
     <row r="54" spans="1:27" ht="13.5" customHeight="1">
-      <c r="A54" s="58"/>
+      <c r="A54" s="76"/>
       <c r="B54" s="55"/>
       <c r="C54" s="55"/>
       <c r="D54" s="55"/>
@@ -3864,9 +3942,9 @@
       <c r="F54" s="30"/>
       <c r="G54" s="43"/>
       <c r="H54" s="43"/>
-      <c r="I54" s="52"/>
-      <c r="J54" s="49"/>
-      <c r="K54" s="52"/>
+      <c r="I54" s="49"/>
+      <c r="J54" s="52"/>
+      <c r="K54" s="49"/>
       <c r="L54" s="2"/>
       <c r="M54" s="2"/>
       <c r="N54" s="2"/>
@@ -3885,7 +3963,7 @@
       <c r="AA54" s="2"/>
     </row>
     <row r="55" spans="1:27" ht="15" customHeight="1">
-      <c r="A55" s="59"/>
+      <c r="A55" s="77"/>
       <c r="B55" s="56"/>
       <c r="C55" s="56"/>
       <c r="D55" s="56"/>
@@ -3893,9 +3971,9 @@
       <c r="F55" s="30"/>
       <c r="G55" s="43"/>
       <c r="H55" s="43"/>
-      <c r="I55" s="53"/>
-      <c r="J55" s="50"/>
-      <c r="K55" s="53"/>
+      <c r="I55" s="50"/>
+      <c r="J55" s="53"/>
+      <c r="K55" s="50"/>
       <c r="L55" s="2"/>
       <c r="M55" s="2"/>
       <c r="N55" s="2"/>
@@ -3914,7 +3992,7 @@
       <c r="AA55" s="2"/>
     </row>
     <row r="56" spans="1:27" ht="25.5">
-      <c r="A56" s="57" t="s">
+      <c r="A56" s="75" t="s">
         <v>42</v>
       </c>
       <c r="B56" s="54" t="s">
@@ -3938,13 +4016,13 @@
       <c r="H56" s="35" t="s">
         <v>92</v>
       </c>
-      <c r="I56" s="51" t="s">
+      <c r="I56" s="48" t="s">
         <v>26</v>
       </c>
-      <c r="J56" s="48" t="s">
+      <c r="J56" s="51" t="s">
         <v>56</v>
       </c>
-      <c r="K56" s="51" t="s">
+      <c r="K56" s="48" t="s">
         <v>28</v>
       </c>
       <c r="L56" s="2"/>
@@ -3965,7 +4043,7 @@
       <c r="AA56" s="2"/>
     </row>
     <row r="57" spans="1:27" ht="17.25" customHeight="1">
-      <c r="A57" s="58"/>
+      <c r="A57" s="76"/>
       <c r="B57" s="55"/>
       <c r="C57" s="55"/>
       <c r="D57" s="55"/>
@@ -3979,9 +4057,9 @@
       <c r="H57" s="36" t="s">
         <v>120</v>
       </c>
-      <c r="I57" s="52"/>
-      <c r="J57" s="49"/>
-      <c r="K57" s="52"/>
+      <c r="I57" s="49"/>
+      <c r="J57" s="52"/>
+      <c r="K57" s="49"/>
       <c r="L57" s="2"/>
       <c r="M57" s="2"/>
       <c r="N57" s="2"/>
@@ -4000,7 +4078,7 @@
       <c r="AA57" s="2"/>
     </row>
     <row r="58" spans="1:27" ht="25.5">
-      <c r="A58" s="58"/>
+      <c r="A58" s="76"/>
       <c r="B58" s="55"/>
       <c r="C58" s="55"/>
       <c r="D58" s="55"/>
@@ -4014,9 +4092,9 @@
       <c r="H58" s="36" t="s">
         <v>122</v>
       </c>
-      <c r="I58" s="52"/>
-      <c r="J58" s="49"/>
-      <c r="K58" s="52"/>
+      <c r="I58" s="49"/>
+      <c r="J58" s="52"/>
+      <c r="K58" s="49"/>
       <c r="L58" s="2"/>
       <c r="M58" s="2"/>
       <c r="N58" s="2"/>
@@ -4035,7 +4113,7 @@
       <c r="AA58" s="2"/>
     </row>
     <row r="59" spans="1:27" ht="25.5">
-      <c r="A59" s="59"/>
+      <c r="A59" s="77"/>
       <c r="B59" s="56"/>
       <c r="C59" s="56"/>
       <c r="D59" s="56"/>
@@ -4049,9 +4127,9 @@
       <c r="H59" s="36" t="s">
         <v>123</v>
       </c>
-      <c r="I59" s="53"/>
-      <c r="J59" s="50"/>
-      <c r="K59" s="53"/>
+      <c r="I59" s="50"/>
+      <c r="J59" s="53"/>
+      <c r="K59" s="50"/>
       <c r="L59" s="2"/>
       <c r="M59" s="2"/>
       <c r="N59" s="2"/>
@@ -4070,7 +4148,7 @@
       <c r="AA59" s="2"/>
     </row>
     <row r="60" spans="1:27" ht="25.5">
-      <c r="A60" s="57" t="s">
+      <c r="A60" s="75" t="s">
         <v>43</v>
       </c>
       <c r="B60" s="54" t="s">
@@ -4094,13 +4172,13 @@
       <c r="H60" s="35" t="s">
         <v>92</v>
       </c>
-      <c r="I60" s="51" t="s">
+      <c r="I60" s="48" t="s">
         <v>26</v>
       </c>
-      <c r="J60" s="48" t="s">
+      <c r="J60" s="51" t="s">
         <v>56</v>
       </c>
-      <c r="K60" s="51" t="s">
+      <c r="K60" s="48" t="s">
         <v>28</v>
       </c>
       <c r="L60" s="2"/>
@@ -4121,7 +4199,7 @@
       <c r="AA60" s="2"/>
     </row>
     <row r="61" spans="1:27" ht="25.5">
-      <c r="A61" s="58"/>
+      <c r="A61" s="76"/>
       <c r="B61" s="55"/>
       <c r="C61" s="55"/>
       <c r="D61" s="55"/>
@@ -4135,9 +4213,9 @@
       <c r="H61" s="36" t="s">
         <v>120</v>
       </c>
-      <c r="I61" s="52"/>
-      <c r="J61" s="49"/>
-      <c r="K61" s="52"/>
+      <c r="I61" s="49"/>
+      <c r="J61" s="52"/>
+      <c r="K61" s="49"/>
       <c r="L61" s="2"/>
       <c r="M61" s="2"/>
       <c r="N61" s="2"/>
@@ -4156,7 +4234,7 @@
       <c r="AA61" s="2"/>
     </row>
     <row r="62" spans="1:27" ht="25.5">
-      <c r="A62" s="58"/>
+      <c r="A62" s="76"/>
       <c r="B62" s="55"/>
       <c r="C62" s="55"/>
       <c r="D62" s="55"/>
@@ -4170,9 +4248,9 @@
       <c r="H62" s="36" t="s">
         <v>122</v>
       </c>
-      <c r="I62" s="52"/>
-      <c r="J62" s="49"/>
-      <c r="K62" s="52"/>
+      <c r="I62" s="49"/>
+      <c r="J62" s="52"/>
+      <c r="K62" s="49"/>
       <c r="L62" s="2"/>
       <c r="M62" s="2"/>
       <c r="N62" s="2"/>
@@ -4191,7 +4269,7 @@
       <c r="AA62" s="2"/>
     </row>
     <row r="63" spans="1:27" ht="25.5">
-      <c r="A63" s="59"/>
+      <c r="A63" s="77"/>
       <c r="B63" s="56"/>
       <c r="C63" s="56"/>
       <c r="D63" s="56"/>
@@ -4205,9 +4283,9 @@
       <c r="H63" s="35" t="s">
         <v>128</v>
       </c>
-      <c r="I63" s="53"/>
-      <c r="J63" s="50"/>
-      <c r="K63" s="53"/>
+      <c r="I63" s="50"/>
+      <c r="J63" s="53"/>
+      <c r="K63" s="50"/>
       <c r="L63" s="2"/>
       <c r="M63" s="2"/>
       <c r="N63" s="2"/>
@@ -4226,13 +4304,13 @@
       <c r="AA63" s="2"/>
     </row>
     <row r="64" spans="1:27" ht="25.5">
-      <c r="A64" s="63" t="s">
+      <c r="A64" s="66" t="s">
         <v>44</v>
       </c>
       <c r="B64" s="54" t="s">
         <v>49</v>
       </c>
-      <c r="C64" s="60" t="s">
+      <c r="C64" s="69" t="s">
         <v>130</v>
       </c>
       <c r="D64" s="54" t="s">
@@ -4250,13 +4328,13 @@
       <c r="H64" s="35" t="s">
         <v>133</v>
       </c>
-      <c r="I64" s="51" t="s">
+      <c r="I64" s="48" t="s">
         <v>26</v>
       </c>
-      <c r="J64" s="48" t="s">
+      <c r="J64" s="51" t="s">
         <v>56</v>
       </c>
-      <c r="K64" s="51" t="s">
+      <c r="K64" s="48" t="s">
         <v>28</v>
       </c>
       <c r="L64" s="2"/>
@@ -4277,17 +4355,17 @@
       <c r="AA64" s="2"/>
     </row>
     <row r="65" spans="1:27">
-      <c r="A65" s="64"/>
+      <c r="A65" s="67"/>
       <c r="B65" s="55"/>
-      <c r="C65" s="61"/>
+      <c r="C65" s="78"/>
       <c r="D65" s="55"/>
       <c r="E65" s="55"/>
       <c r="F65" s="30"/>
       <c r="G65" s="35"/>
       <c r="H65" s="35"/>
-      <c r="I65" s="52"/>
-      <c r="J65" s="49"/>
-      <c r="K65" s="52"/>
+      <c r="I65" s="49"/>
+      <c r="J65" s="52"/>
+      <c r="K65" s="49"/>
       <c r="L65" s="2"/>
       <c r="M65" s="2"/>
       <c r="N65" s="2"/>
@@ -4306,17 +4384,17 @@
       <c r="AA65" s="2"/>
     </row>
     <row r="66" spans="1:27">
-      <c r="A66" s="64"/>
+      <c r="A66" s="67"/>
       <c r="B66" s="55"/>
-      <c r="C66" s="61"/>
+      <c r="C66" s="78"/>
       <c r="D66" s="55"/>
       <c r="E66" s="55"/>
       <c r="F66" s="30"/>
       <c r="G66" s="35"/>
       <c r="H66" s="35"/>
-      <c r="I66" s="52"/>
-      <c r="J66" s="49"/>
-      <c r="K66" s="52"/>
+      <c r="I66" s="49"/>
+      <c r="J66" s="52"/>
+      <c r="K66" s="49"/>
       <c r="L66" s="2"/>
       <c r="M66" s="2"/>
       <c r="N66" s="2"/>
@@ -4335,17 +4413,17 @@
       <c r="AA66" s="2"/>
     </row>
     <row r="67" spans="1:27">
-      <c r="A67" s="65"/>
+      <c r="A67" s="68"/>
       <c r="B67" s="56"/>
-      <c r="C67" s="62"/>
+      <c r="C67" s="79"/>
       <c r="D67" s="56"/>
       <c r="E67" s="56"/>
       <c r="F67" s="30"/>
       <c r="G67" s="35"/>
       <c r="H67" s="35"/>
-      <c r="I67" s="53"/>
-      <c r="J67" s="50"/>
-      <c r="K67" s="53"/>
+      <c r="I67" s="50"/>
+      <c r="J67" s="53"/>
+      <c r="K67" s="50"/>
       <c r="L67" s="2"/>
       <c r="M67" s="2"/>
       <c r="N67" s="2"/>
@@ -4364,13 +4442,13 @@
       <c r="AA67" s="2"/>
     </row>
     <row r="68" spans="1:27" ht="25.5">
-      <c r="A68" s="63" t="s">
+      <c r="A68" s="66" t="s">
         <v>45</v>
       </c>
       <c r="B68" s="54" t="s">
         <v>49</v>
       </c>
-      <c r="C68" s="60" t="s">
+      <c r="C68" s="69" t="s">
         <v>134</v>
       </c>
       <c r="D68" s="54" t="s">
@@ -4388,13 +4466,13 @@
       <c r="H68" s="35" t="s">
         <v>137</v>
       </c>
-      <c r="I68" s="51" t="s">
+      <c r="I68" s="48" t="s">
         <v>26</v>
       </c>
-      <c r="J68" s="48" t="s">
+      <c r="J68" s="51" t="s">
         <v>56</v>
       </c>
-      <c r="K68" s="51" t="s">
+      <c r="K68" s="48" t="s">
         <v>28</v>
       </c>
       <c r="L68" s="2"/>
@@ -4415,17 +4493,17 @@
       <c r="AA68" s="2"/>
     </row>
     <row r="69" spans="1:27">
-      <c r="A69" s="64"/>
+      <c r="A69" s="67"/>
       <c r="B69" s="55"/>
-      <c r="C69" s="61"/>
+      <c r="C69" s="78"/>
       <c r="D69" s="55"/>
       <c r="E69" s="55"/>
       <c r="F69" s="30"/>
       <c r="G69" s="35"/>
       <c r="H69" s="35"/>
-      <c r="I69" s="52"/>
-      <c r="J69" s="49"/>
-      <c r="K69" s="52"/>
+      <c r="I69" s="49"/>
+      <c r="J69" s="52"/>
+      <c r="K69" s="49"/>
       <c r="L69" s="2"/>
       <c r="M69" s="2"/>
       <c r="N69" s="2"/>
@@ -4444,17 +4522,17 @@
       <c r="AA69" s="2"/>
     </row>
     <row r="70" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A70" s="64"/>
+      <c r="A70" s="67"/>
       <c r="B70" s="55"/>
-      <c r="C70" s="61"/>
+      <c r="C70" s="78"/>
       <c r="D70" s="55"/>
       <c r="E70" s="55"/>
       <c r="F70" s="30"/>
       <c r="G70" s="35"/>
       <c r="H70" s="35"/>
-      <c r="I70" s="52"/>
-      <c r="J70" s="49"/>
-      <c r="K70" s="52"/>
+      <c r="I70" s="49"/>
+      <c r="J70" s="52"/>
+      <c r="K70" s="49"/>
       <c r="L70" s="2"/>
       <c r="M70" s="2"/>
       <c r="N70" s="2"/>
@@ -4473,17 +4551,17 @@
       <c r="AA70" s="2"/>
     </row>
     <row r="71" spans="1:27">
-      <c r="A71" s="65"/>
+      <c r="A71" s="68"/>
       <c r="B71" s="56"/>
-      <c r="C71" s="62"/>
+      <c r="C71" s="79"/>
       <c r="D71" s="56"/>
       <c r="E71" s="56"/>
       <c r="F71" s="30"/>
       <c r="G71" s="35"/>
       <c r="H71" s="35"/>
-      <c r="I71" s="53"/>
-      <c r="J71" s="50"/>
-      <c r="K71" s="53"/>
+      <c r="I71" s="50"/>
+      <c r="J71" s="53"/>
+      <c r="K71" s="50"/>
       <c r="L71" s="2"/>
       <c r="M71" s="2"/>
       <c r="N71" s="2"/>
@@ -4502,19 +4580,19 @@
       <c r="AA71" s="2"/>
     </row>
     <row r="72" spans="1:27">
-      <c r="A72" s="80" t="s">
+      <c r="A72" s="72" t="s">
         <v>46</v>
       </c>
-      <c r="B72" s="60" t="s">
+      <c r="B72" s="69" t="s">
         <v>138</v>
       </c>
-      <c r="C72" s="60" t="s">
+      <c r="C72" s="69" t="s">
         <v>139</v>
       </c>
-      <c r="D72" s="60" t="s">
+      <c r="D72" s="69" t="s">
         <v>140</v>
       </c>
-      <c r="E72" s="60" t="s">
+      <c r="E72" s="69" t="s">
         <v>141</v>
       </c>
       <c r="F72" s="44" t="s">
@@ -4526,13 +4604,13 @@
       <c r="H72" s="45" t="s">
         <v>143</v>
       </c>
-      <c r="I72" s="51" t="s">
+      <c r="I72" s="48" t="s">
         <v>26</v>
       </c>
-      <c r="J72" s="48" t="s">
+      <c r="J72" s="51" t="s">
         <v>56</v>
       </c>
-      <c r="K72" s="51" t="s">
+      <c r="K72" s="48" t="s">
         <v>28</v>
       </c>
       <c r="L72" s="2"/>
@@ -4553,11 +4631,11 @@
       <c r="AA72" s="2"/>
     </row>
     <row r="73" spans="1:27">
-      <c r="A73" s="81"/>
-      <c r="B73" s="83"/>
-      <c r="C73" s="83"/>
-      <c r="D73" s="83"/>
-      <c r="E73" s="83"/>
+      <c r="A73" s="73"/>
+      <c r="B73" s="70"/>
+      <c r="C73" s="70"/>
+      <c r="D73" s="70"/>
+      <c r="E73" s="70"/>
       <c r="F73" s="44" t="s">
         <v>67</v>
       </c>
@@ -4565,9 +4643,9 @@
         <v>144</v>
       </c>
       <c r="H73" s="45"/>
-      <c r="I73" s="52"/>
-      <c r="J73" s="49"/>
-      <c r="K73" s="52"/>
+      <c r="I73" s="49"/>
+      <c r="J73" s="52"/>
+      <c r="K73" s="49"/>
       <c r="L73" s="2"/>
       <c r="M73" s="2"/>
       <c r="N73" s="2"/>
@@ -4586,11 +4664,11 @@
       <c r="AA73" s="2"/>
     </row>
     <row r="74" spans="1:27">
-      <c r="A74" s="81"/>
-      <c r="B74" s="83"/>
-      <c r="C74" s="83"/>
-      <c r="D74" s="83"/>
-      <c r="E74" s="83"/>
+      <c r="A74" s="73"/>
+      <c r="B74" s="70"/>
+      <c r="C74" s="70"/>
+      <c r="D74" s="70"/>
+      <c r="E74" s="70"/>
       <c r="F74" s="44" t="s">
         <v>70</v>
       </c>
@@ -4600,9 +4678,9 @@
       <c r="H74" s="45" t="s">
         <v>146</v>
       </c>
-      <c r="I74" s="52"/>
-      <c r="J74" s="49"/>
-      <c r="K74" s="52"/>
+      <c r="I74" s="49"/>
+      <c r="J74" s="52"/>
+      <c r="K74" s="49"/>
       <c r="L74" s="2"/>
       <c r="M74" s="2"/>
       <c r="N74" s="2"/>
@@ -4621,11 +4699,11 @@
       <c r="AA74" s="2"/>
     </row>
     <row r="75" spans="1:27">
-      <c r="A75" s="82"/>
-      <c r="B75" s="84"/>
-      <c r="C75" s="84"/>
-      <c r="D75" s="84"/>
-      <c r="E75" s="84"/>
+      <c r="A75" s="74"/>
+      <c r="B75" s="71"/>
+      <c r="C75" s="71"/>
+      <c r="D75" s="71"/>
+      <c r="E75" s="71"/>
       <c r="F75" s="44" t="s">
         <v>99</v>
       </c>
@@ -4635,9 +4713,9 @@
       <c r="H75" s="45" t="s">
         <v>163</v>
       </c>
-      <c r="I75" s="53"/>
-      <c r="J75" s="50"/>
-      <c r="K75" s="53"/>
+      <c r="I75" s="50"/>
+      <c r="J75" s="53"/>
+      <c r="K75" s="50"/>
       <c r="L75" s="2"/>
       <c r="M75" s="2"/>
       <c r="N75" s="2"/>
@@ -4656,19 +4734,19 @@
       <c r="AA75" s="2"/>
     </row>
     <row r="76" spans="1:27">
-      <c r="A76" s="80" t="s">
+      <c r="A76" s="72" t="s">
         <v>47</v>
       </c>
-      <c r="B76" s="60" t="s">
+      <c r="B76" s="69" t="s">
         <v>138</v>
       </c>
-      <c r="C76" s="60" t="s">
+      <c r="C76" s="69" t="s">
         <v>148</v>
       </c>
-      <c r="D76" s="60" t="s">
+      <c r="D76" s="69" t="s">
         <v>149</v>
       </c>
-      <c r="E76" s="60" t="s">
+      <c r="E76" s="69" t="s">
         <v>141</v>
       </c>
       <c r="F76" s="44" t="s">
@@ -4680,13 +4758,13 @@
       <c r="H76" s="45" t="s">
         <v>143</v>
       </c>
-      <c r="I76" s="51" t="s">
+      <c r="I76" s="48" t="s">
         <v>26</v>
       </c>
-      <c r="J76" s="48" t="s">
+      <c r="J76" s="51" t="s">
         <v>56</v>
       </c>
-      <c r="K76" s="51" t="s">
+      <c r="K76" s="48" t="s">
         <v>28</v>
       </c>
       <c r="L76" s="2"/>
@@ -4707,11 +4785,11 @@
       <c r="AA76" s="2"/>
     </row>
     <row r="77" spans="1:27">
-      <c r="A77" s="81"/>
-      <c r="B77" s="83"/>
-      <c r="C77" s="83"/>
-      <c r="D77" s="83"/>
-      <c r="E77" s="83"/>
+      <c r="A77" s="73"/>
+      <c r="B77" s="70"/>
+      <c r="C77" s="70"/>
+      <c r="D77" s="70"/>
+      <c r="E77" s="70"/>
       <c r="F77" s="44" t="s">
         <v>67</v>
       </c>
@@ -4721,9 +4799,9 @@
       <c r="H77" s="45" t="s">
         <v>146</v>
       </c>
-      <c r="I77" s="52"/>
-      <c r="J77" s="49"/>
-      <c r="K77" s="52"/>
+      <c r="I77" s="49"/>
+      <c r="J77" s="52"/>
+      <c r="K77" s="49"/>
       <c r="L77" s="2"/>
       <c r="M77" s="2"/>
       <c r="N77" s="2"/>
@@ -4742,11 +4820,11 @@
       <c r="AA77" s="2"/>
     </row>
     <row r="78" spans="1:27">
-      <c r="A78" s="81"/>
-      <c r="B78" s="83"/>
-      <c r="C78" s="83"/>
-      <c r="D78" s="83"/>
-      <c r="E78" s="83"/>
+      <c r="A78" s="73"/>
+      <c r="B78" s="70"/>
+      <c r="C78" s="70"/>
+      <c r="D78" s="70"/>
+      <c r="E78" s="70"/>
       <c r="F78" s="44" t="s">
         <v>70</v>
       </c>
@@ -4756,9 +4834,9 @@
       <c r="H78" s="45" t="s">
         <v>151</v>
       </c>
-      <c r="I78" s="52"/>
-      <c r="J78" s="49"/>
-      <c r="K78" s="52"/>
+      <c r="I78" s="49"/>
+      <c r="J78" s="52"/>
+      <c r="K78" s="49"/>
       <c r="L78" s="2"/>
       <c r="M78" s="2"/>
       <c r="N78" s="2"/>
@@ -4777,19 +4855,19 @@
       <c r="AA78" s="2"/>
     </row>
     <row r="79" spans="1:27">
-      <c r="A79" s="82"/>
-      <c r="B79" s="84"/>
-      <c r="C79" s="84"/>
-      <c r="D79" s="84"/>
-      <c r="E79" s="84"/>
+      <c r="A79" s="74"/>
+      <c r="B79" s="71"/>
+      <c r="C79" s="71"/>
+      <c r="D79" s="71"/>
+      <c r="E79" s="71"/>
       <c r="F79" s="44" t="s">
         <v>99</v>
       </c>
       <c r="G79" s="45"/>
       <c r="H79" s="45"/>
-      <c r="I79" s="53"/>
-      <c r="J79" s="50"/>
-      <c r="K79" s="53"/>
+      <c r="I79" s="50"/>
+      <c r="J79" s="53"/>
+      <c r="K79" s="50"/>
       <c r="L79" s="2"/>
       <c r="M79" s="2"/>
       <c r="N79" s="2"/>
@@ -4808,19 +4886,19 @@
       <c r="AA79" s="2"/>
     </row>
     <row r="80" spans="1:27">
-      <c r="A80" s="80" t="s">
+      <c r="A80" s="72" t="s">
         <v>48</v>
       </c>
-      <c r="B80" s="60" t="s">
+      <c r="B80" s="69" t="s">
         <v>138</v>
       </c>
-      <c r="C80" s="60" t="s">
+      <c r="C80" s="69" t="s">
         <v>152</v>
       </c>
-      <c r="D80" s="60" t="s">
+      <c r="D80" s="69" t="s">
         <v>153</v>
       </c>
-      <c r="E80" s="60" t="s">
+      <c r="E80" s="69" t="s">
         <v>141</v>
       </c>
       <c r="F80" s="44" t="s">
@@ -4832,13 +4910,13 @@
       <c r="H80" s="45" t="s">
         <v>143</v>
       </c>
-      <c r="I80" s="51" t="s">
+      <c r="I80" s="48" t="s">
         <v>26</v>
       </c>
-      <c r="J80" s="48" t="s">
+      <c r="J80" s="51" t="s">
         <v>56</v>
       </c>
-      <c r="K80" s="51" t="s">
+      <c r="K80" s="48" t="s">
         <v>28</v>
       </c>
       <c r="L80" s="2"/>
@@ -4859,11 +4937,11 @@
       <c r="AA80" s="2"/>
     </row>
     <row r="81" spans="1:27">
-      <c r="A81" s="81"/>
-      <c r="B81" s="83"/>
-      <c r="C81" s="83"/>
-      <c r="D81" s="83"/>
-      <c r="E81" s="83"/>
+      <c r="A81" s="73"/>
+      <c r="B81" s="70"/>
+      <c r="C81" s="70"/>
+      <c r="D81" s="70"/>
+      <c r="E81" s="70"/>
       <c r="F81" s="44" t="s">
         <v>67</v>
       </c>
@@ -4871,9 +4949,9 @@
         <v>154</v>
       </c>
       <c r="H81" s="45"/>
-      <c r="I81" s="52"/>
-      <c r="J81" s="49"/>
-      <c r="K81" s="52"/>
+      <c r="I81" s="49"/>
+      <c r="J81" s="52"/>
+      <c r="K81" s="49"/>
       <c r="L81" s="2"/>
       <c r="M81" s="2"/>
       <c r="N81" s="2"/>
@@ -4892,11 +4970,11 @@
       <c r="AA81" s="2"/>
     </row>
     <row r="82" spans="1:27">
-      <c r="A82" s="81"/>
-      <c r="B82" s="83"/>
-      <c r="C82" s="83"/>
-      <c r="D82" s="83"/>
-      <c r="E82" s="83"/>
+      <c r="A82" s="73"/>
+      <c r="B82" s="70"/>
+      <c r="C82" s="70"/>
+      <c r="D82" s="70"/>
+      <c r="E82" s="70"/>
       <c r="F82" s="44" t="s">
         <v>70</v>
       </c>
@@ -4906,9 +4984,9 @@
       <c r="H82" s="45" t="s">
         <v>146</v>
       </c>
-      <c r="I82" s="52"/>
-      <c r="J82" s="49"/>
-      <c r="K82" s="52"/>
+      <c r="I82" s="49"/>
+      <c r="J82" s="52"/>
+      <c r="K82" s="49"/>
       <c r="L82" s="2"/>
       <c r="M82" s="2"/>
       <c r="N82" s="2"/>
@@ -4927,11 +5005,11 @@
       <c r="AA82" s="2"/>
     </row>
     <row r="83" spans="1:27">
-      <c r="A83" s="82"/>
-      <c r="B83" s="84"/>
-      <c r="C83" s="84"/>
-      <c r="D83" s="84"/>
-      <c r="E83" s="84"/>
+      <c r="A83" s="74"/>
+      <c r="B83" s="71"/>
+      <c r="C83" s="71"/>
+      <c r="D83" s="71"/>
+      <c r="E83" s="71"/>
       <c r="F83" s="44" t="s">
         <v>99</v>
       </c>
@@ -4941,9 +5019,9 @@
       <c r="H83" s="45" t="s">
         <v>156</v>
       </c>
-      <c r="I83" s="53"/>
-      <c r="J83" s="50"/>
-      <c r="K83" s="53"/>
+      <c r="I83" s="50"/>
+      <c r="J83" s="53"/>
+      <c r="K83" s="50"/>
       <c r="L83" s="2"/>
       <c r="M83" s="2"/>
       <c r="N83" s="2"/>
@@ -4962,19 +5040,19 @@
       <c r="AA83" s="2"/>
     </row>
     <row r="84" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A84" s="80" t="s">
+      <c r="A84" s="72" t="s">
         <v>162</v>
       </c>
-      <c r="B84" s="60" t="s">
+      <c r="B84" s="69" t="s">
         <v>138</v>
       </c>
-      <c r="C84" s="60" t="s">
+      <c r="C84" s="69" t="s">
         <v>157</v>
       </c>
-      <c r="D84" s="60" t="s">
+      <c r="D84" s="69" t="s">
         <v>158</v>
       </c>
-      <c r="E84" s="60" t="s">
+      <c r="E84" s="69" t="s">
         <v>141</v>
       </c>
       <c r="F84" s="44" t="s">
@@ -4986,13 +5064,13 @@
       <c r="H84" s="45" t="s">
         <v>143</v>
       </c>
-      <c r="I84" s="51" t="s">
+      <c r="I84" s="48" t="s">
         <v>26</v>
       </c>
-      <c r="J84" s="48" t="s">
+      <c r="J84" s="51" t="s">
         <v>56</v>
       </c>
-      <c r="K84" s="51" t="s">
+      <c r="K84" s="48" t="s">
         <v>28</v>
       </c>
       <c r="L84" s="2"/>
@@ -5013,11 +5091,11 @@
       <c r="AA84" s="2"/>
     </row>
     <row r="85" spans="1:27" ht="24" customHeight="1">
-      <c r="A85" s="81"/>
-      <c r="B85" s="83"/>
-      <c r="C85" s="83"/>
-      <c r="D85" s="83"/>
-      <c r="E85" s="83"/>
+      <c r="A85" s="73"/>
+      <c r="B85" s="70"/>
+      <c r="C85" s="70"/>
+      <c r="D85" s="70"/>
+      <c r="E85" s="70"/>
       <c r="F85" s="44" t="s">
         <v>67</v>
       </c>
@@ -5027,9 +5105,9 @@
       <c r="H85" s="45" t="s">
         <v>160</v>
       </c>
-      <c r="I85" s="52"/>
-      <c r="J85" s="49"/>
-      <c r="K85" s="52"/>
+      <c r="I85" s="49"/>
+      <c r="J85" s="52"/>
+      <c r="K85" s="49"/>
       <c r="L85" s="2"/>
       <c r="M85" s="2"/>
       <c r="N85" s="2"/>
@@ -5048,11 +5126,11 @@
       <c r="AA85" s="2"/>
     </row>
     <row r="86" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A86" s="81"/>
-      <c r="B86" s="83"/>
-      <c r="C86" s="83"/>
-      <c r="D86" s="83"/>
-      <c r="E86" s="83"/>
+      <c r="A86" s="73"/>
+      <c r="B86" s="70"/>
+      <c r="C86" s="70"/>
+      <c r="D86" s="70"/>
+      <c r="E86" s="70"/>
       <c r="F86" s="44" t="s">
         <v>70</v>
       </c>
@@ -5062,9 +5140,9 @@
       <c r="H86" s="45" t="s">
         <v>161</v>
       </c>
-      <c r="I86" s="52"/>
-      <c r="J86" s="49"/>
-      <c r="K86" s="52"/>
+      <c r="I86" s="49"/>
+      <c r="J86" s="52"/>
+      <c r="K86" s="49"/>
       <c r="L86" s="2"/>
       <c r="M86" s="2"/>
       <c r="N86" s="2"/>
@@ -5083,17 +5161,17 @@
       <c r="AA86" s="2"/>
     </row>
     <row r="87" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A87" s="82"/>
-      <c r="B87" s="84"/>
-      <c r="C87" s="84"/>
-      <c r="D87" s="84"/>
-      <c r="E87" s="84"/>
+      <c r="A87" s="74"/>
+      <c r="B87" s="71"/>
+      <c r="C87" s="71"/>
+      <c r="D87" s="71"/>
+      <c r="E87" s="71"/>
       <c r="F87" s="44"/>
       <c r="G87" s="45"/>
       <c r="H87" s="45"/>
-      <c r="I87" s="53"/>
-      <c r="J87" s="50"/>
-      <c r="K87" s="53"/>
+      <c r="I87" s="50"/>
+      <c r="J87" s="53"/>
+      <c r="K87" s="50"/>
       <c r="L87" s="2"/>
       <c r="M87" s="2"/>
       <c r="N87" s="2"/>
@@ -5112,10 +5190,10 @@
       <c r="AA87" s="2"/>
     </row>
     <row r="88" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A88" s="63" t="s">
+      <c r="A88" s="66" t="s">
         <v>169</v>
       </c>
-      <c r="B88" s="85" t="s">
+      <c r="B88" s="57" t="s">
         <v>49</v>
       </c>
       <c r="C88" s="54" t="s">
@@ -5136,13 +5214,13 @@
       <c r="H88" s="30" t="s">
         <v>168</v>
       </c>
-      <c r="I88" s="51" t="s">
+      <c r="I88" s="48" t="s">
         <v>26</v>
       </c>
-      <c r="J88" s="48" t="s">
+      <c r="J88" s="51" t="s">
         <v>56</v>
       </c>
-      <c r="K88" s="51" t="s">
+      <c r="K88" s="48" t="s">
         <v>28</v>
       </c>
       <c r="L88" s="2"/>
@@ -5163,8 +5241,8 @@
       <c r="AA88" s="2"/>
     </row>
     <row r="89" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A89" s="64"/>
-      <c r="B89" s="86"/>
+      <c r="A89" s="67"/>
+      <c r="B89" s="58"/>
       <c r="C89" s="55"/>
       <c r="D89" s="55"/>
       <c r="E89" s="55"/>
@@ -5173,9 +5251,9 @@
       </c>
       <c r="G89" s="35"/>
       <c r="H89" s="35"/>
-      <c r="I89" s="52"/>
-      <c r="J89" s="49"/>
-      <c r="K89" s="52"/>
+      <c r="I89" s="49"/>
+      <c r="J89" s="52"/>
+      <c r="K89" s="49"/>
       <c r="L89" s="2"/>
       <c r="M89" s="2"/>
       <c r="N89" s="2"/>
@@ -5194,8 +5272,8 @@
       <c r="AA89" s="2"/>
     </row>
     <row r="90" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A90" s="64"/>
-      <c r="B90" s="86"/>
+      <c r="A90" s="67"/>
+      <c r="B90" s="58"/>
       <c r="C90" s="55"/>
       <c r="D90" s="55"/>
       <c r="E90" s="55"/>
@@ -5204,9 +5282,9 @@
       </c>
       <c r="G90" s="46"/>
       <c r="H90" s="46"/>
-      <c r="I90" s="52"/>
-      <c r="J90" s="49"/>
-      <c r="K90" s="52"/>
+      <c r="I90" s="49"/>
+      <c r="J90" s="52"/>
+      <c r="K90" s="49"/>
       <c r="L90" s="2"/>
       <c r="M90" s="2"/>
       <c r="N90" s="2"/>
@@ -5225,8 +5303,8 @@
       <c r="AA90" s="2"/>
     </row>
     <row r="91" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A91" s="65"/>
-      <c r="B91" s="87"/>
+      <c r="A91" s="68"/>
+      <c r="B91" s="59"/>
       <c r="C91" s="56"/>
       <c r="D91" s="56"/>
       <c r="E91" s="56"/>
@@ -5235,9 +5313,9 @@
       </c>
       <c r="G91" s="30"/>
       <c r="H91" s="30"/>
-      <c r="I91" s="53"/>
-      <c r="J91" s="50"/>
-      <c r="K91" s="53"/>
+      <c r="I91" s="50"/>
+      <c r="J91" s="53"/>
+      <c r="K91" s="50"/>
       <c r="L91" s="2"/>
       <c r="M91" s="2"/>
       <c r="N91" s="2"/>
@@ -5256,7 +5334,7 @@
       <c r="AA91" s="2"/>
     </row>
     <row r="92" spans="1:27" ht="25.5" customHeight="1">
-      <c r="A92" s="57" t="s">
+      <c r="A92" s="75" t="s">
         <v>186</v>
       </c>
       <c r="B92" s="54" t="s">
@@ -5280,13 +5358,13 @@
       <c r="H92" s="30" t="s">
         <v>174</v>
       </c>
-      <c r="I92" s="51" t="s">
+      <c r="I92" s="48" t="s">
         <v>26</v>
       </c>
-      <c r="J92" s="48" t="s">
+      <c r="J92" s="51" t="s">
         <v>56</v>
       </c>
-      <c r="K92" s="51" t="s">
+      <c r="K92" s="48" t="s">
         <v>28</v>
       </c>
       <c r="L92" s="2"/>
@@ -5307,7 +5385,7 @@
       <c r="AA92" s="2"/>
     </row>
     <row r="93" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A93" s="58"/>
+      <c r="A93" s="76"/>
       <c r="B93" s="55"/>
       <c r="C93" s="55"/>
       <c r="D93" s="55"/>
@@ -5317,9 +5395,9 @@
       </c>
       <c r="G93" s="35"/>
       <c r="H93" s="30"/>
-      <c r="I93" s="52"/>
-      <c r="J93" s="49"/>
-      <c r="K93" s="52"/>
+      <c r="I93" s="49"/>
+      <c r="J93" s="52"/>
+      <c r="K93" s="49"/>
       <c r="L93" s="2"/>
       <c r="M93" s="2"/>
       <c r="N93" s="2"/>
@@ -5338,7 +5416,7 @@
       <c r="AA93" s="2"/>
     </row>
     <row r="94" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A94" s="58"/>
+      <c r="A94" s="76"/>
       <c r="B94" s="55"/>
       <c r="C94" s="55"/>
       <c r="D94" s="55"/>
@@ -5348,9 +5426,9 @@
       </c>
       <c r="G94" s="46"/>
       <c r="H94" s="46"/>
-      <c r="I94" s="52"/>
-      <c r="J94" s="49"/>
-      <c r="K94" s="52"/>
+      <c r="I94" s="49"/>
+      <c r="J94" s="52"/>
+      <c r="K94" s="49"/>
       <c r="L94" s="2"/>
       <c r="M94" s="2"/>
       <c r="N94" s="2"/>
@@ -5369,7 +5447,7 @@
       <c r="AA94" s="2"/>
     </row>
     <row r="95" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A95" s="59"/>
+      <c r="A95" s="77"/>
       <c r="B95" s="56"/>
       <c r="C95" s="56"/>
       <c r="D95" s="56"/>
@@ -5379,9 +5457,9 @@
       </c>
       <c r="G95" s="30"/>
       <c r="H95" s="30"/>
-      <c r="I95" s="53"/>
-      <c r="J95" s="50"/>
-      <c r="K95" s="53"/>
+      <c r="I95" s="50"/>
+      <c r="J95" s="53"/>
+      <c r="K95" s="50"/>
       <c r="L95" s="2"/>
       <c r="M95" s="2"/>
       <c r="N95" s="2"/>
@@ -5400,7 +5478,7 @@
       <c r="AA95" s="2"/>
     </row>
     <row r="96" spans="1:27" ht="26.25" customHeight="1">
-      <c r="A96" s="57" t="s">
+      <c r="A96" s="75" t="s">
         <v>187</v>
       </c>
       <c r="B96" s="54" t="s">
@@ -5424,13 +5502,13 @@
       <c r="H96" s="30" t="s">
         <v>174</v>
       </c>
-      <c r="I96" s="51" t="s">
+      <c r="I96" s="48" t="s">
         <v>26</v>
       </c>
-      <c r="J96" s="48" t="s">
+      <c r="J96" s="51" t="s">
         <v>56</v>
       </c>
-      <c r="K96" s="51" t="s">
+      <c r="K96" s="48" t="s">
         <v>28</v>
       </c>
       <c r="L96" s="2"/>
@@ -5451,7 +5529,7 @@
       <c r="AA96" s="2"/>
     </row>
     <row r="97" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A97" s="58"/>
+      <c r="A97" s="76"/>
       <c r="B97" s="55"/>
       <c r="C97" s="55"/>
       <c r="D97" s="55"/>
@@ -5461,9 +5539,9 @@
       </c>
       <c r="G97" s="35"/>
       <c r="H97" s="30"/>
-      <c r="I97" s="52"/>
-      <c r="J97" s="49"/>
-      <c r="K97" s="52"/>
+      <c r="I97" s="49"/>
+      <c r="J97" s="52"/>
+      <c r="K97" s="49"/>
       <c r="L97" s="2"/>
       <c r="M97" s="2"/>
       <c r="N97" s="2"/>
@@ -5482,7 +5560,7 @@
       <c r="AA97" s="2"/>
     </row>
     <row r="98" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A98" s="58"/>
+      <c r="A98" s="76"/>
       <c r="B98" s="55"/>
       <c r="C98" s="55"/>
       <c r="D98" s="55"/>
@@ -5492,9 +5570,9 @@
       </c>
       <c r="G98" s="30"/>
       <c r="H98" s="30"/>
-      <c r="I98" s="52"/>
-      <c r="J98" s="49"/>
-      <c r="K98" s="52"/>
+      <c r="I98" s="49"/>
+      <c r="J98" s="52"/>
+      <c r="K98" s="49"/>
       <c r="L98" s="2"/>
       <c r="M98" s="2"/>
       <c r="N98" s="2"/>
@@ -5513,7 +5591,7 @@
       <c r="AA98" s="2"/>
     </row>
     <row r="99" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A99" s="59"/>
+      <c r="A99" s="77"/>
       <c r="B99" s="56"/>
       <c r="C99" s="56"/>
       <c r="D99" s="56"/>
@@ -5523,9 +5601,9 @@
       </c>
       <c r="G99" s="30"/>
       <c r="H99" s="30"/>
-      <c r="I99" s="53"/>
-      <c r="J99" s="50"/>
-      <c r="K99" s="53"/>
+      <c r="I99" s="50"/>
+      <c r="J99" s="53"/>
+      <c r="K99" s="50"/>
       <c r="L99" s="2"/>
       <c r="M99" s="2"/>
       <c r="N99" s="2"/>
@@ -5544,7 +5622,7 @@
       <c r="AA99" s="2"/>
     </row>
     <row r="100" spans="1:27" ht="24.75" customHeight="1">
-      <c r="A100" s="57" t="s">
+      <c r="A100" s="75" t="s">
         <v>188</v>
       </c>
       <c r="B100" s="54" t="s">
@@ -5568,13 +5646,13 @@
       <c r="H100" s="30" t="s">
         <v>181</v>
       </c>
-      <c r="I100" s="51" t="s">
+      <c r="I100" s="48" t="s">
         <v>26</v>
       </c>
-      <c r="J100" s="48" t="s">
+      <c r="J100" s="51" t="s">
         <v>56</v>
       </c>
-      <c r="K100" s="51" t="s">
+      <c r="K100" s="48" t="s">
         <v>28</v>
       </c>
       <c r="L100" s="2"/>
@@ -5595,7 +5673,7 @@
       <c r="AA100" s="2"/>
     </row>
     <row r="101" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A101" s="58"/>
+      <c r="A101" s="76"/>
       <c r="B101" s="55"/>
       <c r="C101" s="55"/>
       <c r="D101" s="55"/>
@@ -5605,9 +5683,9 @@
       </c>
       <c r="G101" s="35"/>
       <c r="H101" s="30"/>
-      <c r="I101" s="52"/>
-      <c r="J101" s="49"/>
-      <c r="K101" s="52"/>
+      <c r="I101" s="49"/>
+      <c r="J101" s="52"/>
+      <c r="K101" s="49"/>
       <c r="L101" s="2"/>
       <c r="M101" s="2"/>
       <c r="N101" s="2"/>
@@ -5626,7 +5704,7 @@
       <c r="AA101" s="2"/>
     </row>
     <row r="102" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A102" s="58"/>
+      <c r="A102" s="76"/>
       <c r="B102" s="55"/>
       <c r="C102" s="55"/>
       <c r="D102" s="55"/>
@@ -5636,9 +5714,9 @@
       </c>
       <c r="G102" s="46"/>
       <c r="H102" s="46"/>
-      <c r="I102" s="52"/>
-      <c r="J102" s="49"/>
-      <c r="K102" s="52"/>
+      <c r="I102" s="49"/>
+      <c r="J102" s="52"/>
+      <c r="K102" s="49"/>
       <c r="L102" s="2"/>
       <c r="M102" s="2"/>
       <c r="N102" s="2"/>
@@ -5657,7 +5735,7 @@
       <c r="AA102" s="2"/>
     </row>
     <row r="103" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A103" s="59"/>
+      <c r="A103" s="77"/>
       <c r="B103" s="56"/>
       <c r="C103" s="56"/>
       <c r="D103" s="56"/>
@@ -5667,9 +5745,9 @@
       </c>
       <c r="G103" s="46"/>
       <c r="H103" s="46"/>
-      <c r="I103" s="53"/>
-      <c r="J103" s="50"/>
-      <c r="K103" s="53"/>
+      <c r="I103" s="50"/>
+      <c r="J103" s="53"/>
+      <c r="K103" s="50"/>
       <c r="L103" s="2"/>
       <c r="M103" s="2"/>
       <c r="N103" s="2"/>
@@ -5688,7 +5766,7 @@
       <c r="AA103" s="2"/>
     </row>
     <row r="104" spans="1:27" ht="24.75" customHeight="1">
-      <c r="A104" s="57" t="s">
+      <c r="A104" s="75" t="s">
         <v>189</v>
       </c>
       <c r="B104" s="54" t="s">
@@ -5712,13 +5790,13 @@
       <c r="H104" s="30" t="s">
         <v>185</v>
       </c>
-      <c r="I104" s="51" t="s">
+      <c r="I104" s="48" t="s">
         <v>26</v>
       </c>
-      <c r="J104" s="48" t="s">
+      <c r="J104" s="51" t="s">
         <v>56</v>
       </c>
-      <c r="K104" s="51" t="s">
+      <c r="K104" s="48" t="s">
         <v>28</v>
       </c>
       <c r="L104" s="2"/>
@@ -5739,7 +5817,7 @@
       <c r="AA104" s="2"/>
     </row>
     <row r="105" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A105" s="58"/>
+      <c r="A105" s="76"/>
       <c r="B105" s="55"/>
       <c r="C105" s="55"/>
       <c r="D105" s="55"/>
@@ -5749,9 +5827,9 @@
       </c>
       <c r="G105" s="35"/>
       <c r="H105" s="30"/>
-      <c r="I105" s="52"/>
-      <c r="J105" s="49"/>
-      <c r="K105" s="52"/>
+      <c r="I105" s="49"/>
+      <c r="J105" s="52"/>
+      <c r="K105" s="49"/>
       <c r="L105" s="2"/>
       <c r="M105" s="2"/>
       <c r="N105" s="2"/>
@@ -5770,7 +5848,7 @@
       <c r="AA105" s="2"/>
     </row>
     <row r="106" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A106" s="58"/>
+      <c r="A106" s="76"/>
       <c r="B106" s="55"/>
       <c r="C106" s="55"/>
       <c r="D106" s="55"/>
@@ -5780,9 +5858,9 @@
       </c>
       <c r="G106" s="46"/>
       <c r="H106" s="46"/>
-      <c r="I106" s="52"/>
-      <c r="J106" s="49"/>
-      <c r="K106" s="52"/>
+      <c r="I106" s="49"/>
+      <c r="J106" s="52"/>
+      <c r="K106" s="49"/>
       <c r="L106" s="2"/>
       <c r="M106" s="2"/>
       <c r="N106" s="2"/>
@@ -5801,7 +5879,7 @@
       <c r="AA106" s="2"/>
     </row>
     <row r="107" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A107" s="59"/>
+      <c r="A107" s="77"/>
       <c r="B107" s="56"/>
       <c r="C107" s="56"/>
       <c r="D107" s="56"/>
@@ -5811,9 +5889,9 @@
       </c>
       <c r="G107" s="46"/>
       <c r="H107" s="47"/>
-      <c r="I107" s="53"/>
-      <c r="J107" s="50"/>
-      <c r="K107" s="53"/>
+      <c r="I107" s="50"/>
+      <c r="J107" s="53"/>
+      <c r="K107" s="50"/>
       <c r="L107" s="2"/>
       <c r="M107" s="2"/>
       <c r="N107" s="2"/>
@@ -5832,37 +5910,37 @@
       <c r="AA107" s="2"/>
     </row>
     <row r="108" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A108" s="89" t="s">
-        <v>199</v>
+      <c r="A108" s="63" t="s">
+        <v>198</v>
       </c>
       <c r="B108" s="54" t="s">
         <v>190</v>
       </c>
       <c r="C108" s="54" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="D108" s="54" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="E108" s="54" t="s">
-        <v>191</v>
+        <v>83</v>
       </c>
       <c r="F108" s="30" t="s">
         <v>53</v>
       </c>
       <c r="G108" s="30" t="s">
+        <v>192</v>
+      </c>
+      <c r="H108" s="30" t="s">
         <v>193</v>
       </c>
-      <c r="H108" s="30" t="s">
-        <v>194</v>
-      </c>
-      <c r="I108" s="51" t="s">
+      <c r="I108" s="48" t="s">
         <v>26</v>
       </c>
-      <c r="J108" s="48" t="s">
+      <c r="J108" s="51" t="s">
         <v>56</v>
       </c>
-      <c r="K108" s="51" t="s">
+      <c r="K108" s="48" t="s">
         <v>28</v>
       </c>
       <c r="L108" s="2"/>
@@ -5883,7 +5961,7 @@
       <c r="AA108" s="2"/>
     </row>
     <row r="109" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A109" s="90"/>
+      <c r="A109" s="64"/>
       <c r="B109" s="55"/>
       <c r="C109" s="55"/>
       <c r="D109" s="55"/>
@@ -5893,9 +5971,9 @@
       </c>
       <c r="G109" s="30"/>
       <c r="H109" s="30"/>
-      <c r="I109" s="52"/>
-      <c r="J109" s="49"/>
-      <c r="K109" s="52"/>
+      <c r="I109" s="49"/>
+      <c r="J109" s="52"/>
+      <c r="K109" s="49"/>
       <c r="L109" s="2"/>
       <c r="M109" s="2"/>
       <c r="N109" s="2"/>
@@ -5914,7 +5992,7 @@
       <c r="AA109" s="2"/>
     </row>
     <row r="110" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A110" s="90"/>
+      <c r="A110" s="64"/>
       <c r="B110" s="55"/>
       <c r="C110" s="55"/>
       <c r="D110" s="55"/>
@@ -5924,9 +6002,9 @@
       </c>
       <c r="G110" s="30"/>
       <c r="H110" s="30"/>
-      <c r="I110" s="52"/>
-      <c r="J110" s="49"/>
-      <c r="K110" s="52"/>
+      <c r="I110" s="49"/>
+      <c r="J110" s="52"/>
+      <c r="K110" s="49"/>
       <c r="L110" s="2"/>
       <c r="M110" s="2"/>
       <c r="N110" s="2"/>
@@ -5945,7 +6023,7 @@
       <c r="AA110" s="2"/>
     </row>
     <row r="111" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A111" s="91"/>
+      <c r="A111" s="65"/>
       <c r="B111" s="55"/>
       <c r="C111" s="56"/>
       <c r="D111" s="56"/>
@@ -5955,9 +6033,9 @@
       </c>
       <c r="G111" s="30"/>
       <c r="H111" s="30"/>
-      <c r="I111" s="53"/>
-      <c r="J111" s="50"/>
-      <c r="K111" s="53"/>
+      <c r="I111" s="50"/>
+      <c r="J111" s="53"/>
+      <c r="K111" s="50"/>
       <c r="L111" s="2"/>
       <c r="M111" s="2"/>
       <c r="N111" s="2"/>
@@ -5976,37 +6054,37 @@
       <c r="AA111" s="2"/>
     </row>
     <row r="112" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A112" s="89" t="s">
-        <v>200</v>
+      <c r="A112" s="63" t="s">
+        <v>199</v>
       </c>
       <c r="B112" s="54" t="s">
         <v>190</v>
       </c>
       <c r="C112" s="54" t="s">
+        <v>194</v>
+      </c>
+      <c r="D112" s="54" t="s">
         <v>195</v>
-      </c>
-      <c r="D112" s="54" t="s">
-        <v>196</v>
       </c>
       <c r="E112" s="54" t="s">
         <v>83</v>
       </c>
-      <c r="F112" s="85" t="s">
+      <c r="F112" s="57" t="s">
         <v>53</v>
       </c>
-      <c r="G112" s="85" t="s">
+      <c r="G112" s="57" t="s">
+        <v>196</v>
+      </c>
+      <c r="H112" s="60" t="s">
         <v>197</v>
       </c>
-      <c r="H112" s="78" t="s">
-        <v>198</v>
-      </c>
-      <c r="I112" s="51" t="s">
+      <c r="I112" s="48" t="s">
         <v>26</v>
       </c>
-      <c r="J112" s="48" t="s">
+      <c r="J112" s="51" t="s">
         <v>56</v>
       </c>
-      <c r="K112" s="51" t="s">
+      <c r="K112" s="48" t="s">
         <v>28</v>
       </c>
       <c r="L112" s="2"/>
@@ -6027,17 +6105,17 @@
       <c r="AA112" s="2"/>
     </row>
     <row r="113" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A113" s="90"/>
+      <c r="A113" s="64"/>
       <c r="B113" s="55"/>
       <c r="C113" s="55"/>
       <c r="D113" s="55"/>
       <c r="E113" s="55"/>
-      <c r="F113" s="86"/>
-      <c r="G113" s="86"/>
-      <c r="H113" s="88"/>
-      <c r="I113" s="52"/>
-      <c r="J113" s="49"/>
-      <c r="K113" s="52"/>
+      <c r="F113" s="58"/>
+      <c r="G113" s="58"/>
+      <c r="H113" s="61"/>
+      <c r="I113" s="49"/>
+      <c r="J113" s="52"/>
+      <c r="K113" s="49"/>
       <c r="L113" s="2"/>
       <c r="M113" s="2"/>
       <c r="N113" s="2"/>
@@ -6056,17 +6134,17 @@
       <c r="AA113" s="2"/>
     </row>
     <row r="114" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A114" s="90"/>
+      <c r="A114" s="64"/>
       <c r="B114" s="55"/>
       <c r="C114" s="55"/>
       <c r="D114" s="55"/>
       <c r="E114" s="55"/>
-      <c r="F114" s="86"/>
-      <c r="G114" s="86"/>
-      <c r="H114" s="88"/>
-      <c r="I114" s="52"/>
-      <c r="J114" s="49"/>
-      <c r="K114" s="52"/>
+      <c r="F114" s="58"/>
+      <c r="G114" s="58"/>
+      <c r="H114" s="61"/>
+      <c r="I114" s="49"/>
+      <c r="J114" s="52"/>
+      <c r="K114" s="49"/>
       <c r="L114" s="2"/>
       <c r="M114" s="2"/>
       <c r="N114" s="2"/>
@@ -6085,17 +6163,17 @@
       <c r="AA114" s="2"/>
     </row>
     <row r="115" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A115" s="91"/>
+      <c r="A115" s="65"/>
       <c r="B115" s="56"/>
       <c r="C115" s="56"/>
       <c r="D115" s="56"/>
       <c r="E115" s="56"/>
-      <c r="F115" s="87"/>
-      <c r="G115" s="87"/>
-      <c r="H115" s="79"/>
-      <c r="I115" s="53"/>
-      <c r="J115" s="50"/>
-      <c r="K115" s="53"/>
+      <c r="F115" s="59"/>
+      <c r="G115" s="59"/>
+      <c r="H115" s="62"/>
+      <c r="I115" s="50"/>
+      <c r="J115" s="53"/>
+      <c r="K115" s="50"/>
       <c r="L115" s="2"/>
       <c r="M115" s="2"/>
       <c r="N115" s="2"/>
@@ -6114,17 +6192,39 @@
       <c r="AA115" s="2"/>
     </row>
     <row r="116" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A116" s="2"/>
-      <c r="B116" s="38"/>
-      <c r="C116" s="2"/>
-      <c r="D116" s="38"/>
-      <c r="E116" s="38"/>
-      <c r="F116" s="2"/>
-      <c r="G116" s="38"/>
-      <c r="H116" s="38"/>
-      <c r="I116" s="2"/>
-      <c r="J116" s="38"/>
-      <c r="K116" s="2"/>
+      <c r="A116" s="63" t="s">
+        <v>218</v>
+      </c>
+      <c r="B116" s="54" t="s">
+        <v>201</v>
+      </c>
+      <c r="C116" s="54" t="s">
+        <v>202</v>
+      </c>
+      <c r="D116" s="54" t="s">
+        <v>203</v>
+      </c>
+      <c r="E116" s="54" t="s">
+        <v>222</v>
+      </c>
+      <c r="F116" s="57" t="s">
+        <v>53</v>
+      </c>
+      <c r="G116" s="54" t="s">
+        <v>204</v>
+      </c>
+      <c r="H116" s="60" t="s">
+        <v>205</v>
+      </c>
+      <c r="I116" s="48" t="s">
+        <v>26</v>
+      </c>
+      <c r="J116" s="51" t="s">
+        <v>56</v>
+      </c>
+      <c r="K116" s="48" t="s">
+        <v>28</v>
+      </c>
       <c r="L116" s="2"/>
       <c r="M116" s="2"/>
       <c r="N116" s="2"/>
@@ -6143,17 +6243,17 @@
       <c r="AA116" s="2"/>
     </row>
     <row r="117" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A117" s="2"/>
-      <c r="B117" s="38"/>
-      <c r="C117" s="2"/>
-      <c r="D117" s="38"/>
-      <c r="E117" s="38"/>
-      <c r="F117" s="2"/>
-      <c r="G117" s="38"/>
-      <c r="H117" s="38"/>
-      <c r="I117" s="2"/>
-      <c r="J117" s="38"/>
-      <c r="K117" s="2"/>
+      <c r="A117" s="64"/>
+      <c r="B117" s="55"/>
+      <c r="C117" s="55"/>
+      <c r="D117" s="55"/>
+      <c r="E117" s="55"/>
+      <c r="F117" s="58"/>
+      <c r="G117" s="55"/>
+      <c r="H117" s="61"/>
+      <c r="I117" s="49"/>
+      <c r="J117" s="52"/>
+      <c r="K117" s="49"/>
       <c r="L117" s="2"/>
       <c r="M117" s="2"/>
       <c r="N117" s="2"/>
@@ -6172,17 +6272,17 @@
       <c r="AA117" s="2"/>
     </row>
     <row r="118" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A118" s="2"/>
-      <c r="B118" s="38"/>
-      <c r="C118" s="2"/>
-      <c r="D118" s="38"/>
-      <c r="E118" s="38"/>
-      <c r="F118" s="2"/>
-      <c r="G118" s="38"/>
-      <c r="H118" s="38"/>
-      <c r="I118" s="2"/>
-      <c r="J118" s="38"/>
-      <c r="K118" s="2"/>
+      <c r="A118" s="64"/>
+      <c r="B118" s="55"/>
+      <c r="C118" s="55"/>
+      <c r="D118" s="55"/>
+      <c r="E118" s="55"/>
+      <c r="F118" s="59"/>
+      <c r="G118" s="55"/>
+      <c r="H118" s="61"/>
+      <c r="I118" s="49"/>
+      <c r="J118" s="52"/>
+      <c r="K118" s="49"/>
       <c r="L118" s="2"/>
       <c r="M118" s="2"/>
       <c r="N118" s="2"/>
@@ -6201,17 +6301,19 @@
       <c r="AA118" s="2"/>
     </row>
     <row r="119" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A119" s="2"/>
-      <c r="B119" s="38"/>
-      <c r="C119" s="2"/>
-      <c r="D119" s="38"/>
-      <c r="E119" s="38"/>
-      <c r="F119" s="2"/>
-      <c r="G119" s="38"/>
-      <c r="H119" s="38"/>
-      <c r="I119" s="2"/>
-      <c r="J119" s="38"/>
-      <c r="K119" s="2"/>
+      <c r="A119" s="65"/>
+      <c r="B119" s="56"/>
+      <c r="C119" s="56"/>
+      <c r="D119" s="56"/>
+      <c r="E119" s="56"/>
+      <c r="F119" s="30" t="s">
+        <v>67</v>
+      </c>
+      <c r="G119" s="92"/>
+      <c r="H119" s="93"/>
+      <c r="I119" s="50"/>
+      <c r="J119" s="53"/>
+      <c r="K119" s="50"/>
       <c r="L119" s="2"/>
       <c r="M119" s="2"/>
       <c r="N119" s="2"/>
@@ -6230,17 +6332,39 @@
       <c r="AA119" s="2"/>
     </row>
     <row r="120" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A120" s="2"/>
-      <c r="B120" s="38"/>
-      <c r="C120" s="2"/>
-      <c r="D120" s="38"/>
-      <c r="E120" s="38"/>
-      <c r="F120" s="2"/>
-      <c r="G120" s="38"/>
-      <c r="H120" s="38"/>
-      <c r="I120" s="2"/>
-      <c r="J120" s="38"/>
-      <c r="K120" s="2"/>
+      <c r="A120" s="63" t="s">
+        <v>219</v>
+      </c>
+      <c r="B120" s="54" t="s">
+        <v>201</v>
+      </c>
+      <c r="C120" s="54" t="s">
+        <v>206</v>
+      </c>
+      <c r="D120" s="54" t="s">
+        <v>207</v>
+      </c>
+      <c r="E120" s="54" t="s">
+        <v>223</v>
+      </c>
+      <c r="F120" s="57" t="s">
+        <v>53</v>
+      </c>
+      <c r="G120" s="54" t="s">
+        <v>208</v>
+      </c>
+      <c r="H120" s="60" t="s">
+        <v>209</v>
+      </c>
+      <c r="I120" s="48" t="s">
+        <v>26</v>
+      </c>
+      <c r="J120" s="51" t="s">
+        <v>56</v>
+      </c>
+      <c r="K120" s="48" t="s">
+        <v>28</v>
+      </c>
       <c r="L120" s="2"/>
       <c r="M120" s="2"/>
       <c r="N120" s="2"/>
@@ -6259,17 +6383,17 @@
       <c r="AA120" s="2"/>
     </row>
     <row r="121" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A121" s="2"/>
-      <c r="B121" s="38"/>
-      <c r="C121" s="2"/>
-      <c r="D121" s="38"/>
-      <c r="E121" s="38"/>
-      <c r="F121" s="2"/>
-      <c r="G121" s="38"/>
-      <c r="H121" s="38"/>
-      <c r="I121" s="2"/>
-      <c r="J121" s="38"/>
-      <c r="K121" s="2"/>
+      <c r="A121" s="64"/>
+      <c r="B121" s="55"/>
+      <c r="C121" s="55"/>
+      <c r="D121" s="55"/>
+      <c r="E121" s="55"/>
+      <c r="F121" s="58"/>
+      <c r="G121" s="55"/>
+      <c r="H121" s="61"/>
+      <c r="I121" s="49"/>
+      <c r="J121" s="52"/>
+      <c r="K121" s="49"/>
       <c r="L121" s="2"/>
       <c r="M121" s="2"/>
       <c r="N121" s="2"/>
@@ -6288,17 +6412,17 @@
       <c r="AA121" s="2"/>
     </row>
     <row r="122" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A122" s="2"/>
-      <c r="B122" s="38"/>
-      <c r="C122" s="2"/>
-      <c r="D122" s="38"/>
-      <c r="E122" s="38"/>
-      <c r="F122" s="2"/>
-      <c r="G122" s="38"/>
-      <c r="H122" s="38"/>
-      <c r="I122" s="2"/>
-      <c r="J122" s="38"/>
-      <c r="K122" s="2"/>
+      <c r="A122" s="64"/>
+      <c r="B122" s="55"/>
+      <c r="C122" s="55"/>
+      <c r="D122" s="55"/>
+      <c r="E122" s="55"/>
+      <c r="F122" s="59"/>
+      <c r="G122" s="55"/>
+      <c r="H122" s="61"/>
+      <c r="I122" s="49"/>
+      <c r="J122" s="52"/>
+      <c r="K122" s="49"/>
       <c r="L122" s="2"/>
       <c r="M122" s="2"/>
       <c r="N122" s="2"/>
@@ -6317,17 +6441,19 @@
       <c r="AA122" s="2"/>
     </row>
     <row r="123" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A123" s="2"/>
-      <c r="B123" s="38"/>
-      <c r="C123" s="2"/>
-      <c r="D123" s="38"/>
-      <c r="E123" s="38"/>
-      <c r="F123" s="2"/>
-      <c r="G123" s="38"/>
-      <c r="H123" s="38"/>
-      <c r="I123" s="2"/>
-      <c r="J123" s="38"/>
-      <c r="K123" s="2"/>
+      <c r="A123" s="65"/>
+      <c r="B123" s="56"/>
+      <c r="C123" s="56"/>
+      <c r="D123" s="56"/>
+      <c r="E123" s="56"/>
+      <c r="F123" s="30" t="s">
+        <v>67</v>
+      </c>
+      <c r="G123" s="30"/>
+      <c r="H123" s="30"/>
+      <c r="I123" s="50"/>
+      <c r="J123" s="53"/>
+      <c r="K123" s="50"/>
       <c r="L123" s="2"/>
       <c r="M123" s="2"/>
       <c r="N123" s="2"/>
@@ -6346,17 +6472,39 @@
       <c r="AA123" s="2"/>
     </row>
     <row r="124" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A124" s="2"/>
-      <c r="B124" s="38"/>
-      <c r="C124" s="2"/>
-      <c r="D124" s="38"/>
-      <c r="E124" s="38"/>
-      <c r="F124" s="2"/>
-      <c r="G124" s="38"/>
-      <c r="H124" s="38"/>
-      <c r="I124" s="2"/>
-      <c r="J124" s="38"/>
-      <c r="K124" s="2"/>
+      <c r="A124" s="63" t="s">
+        <v>220</v>
+      </c>
+      <c r="B124" s="54" t="s">
+        <v>201</v>
+      </c>
+      <c r="C124" s="54" t="s">
+        <v>210</v>
+      </c>
+      <c r="D124" s="54" t="s">
+        <v>211</v>
+      </c>
+      <c r="E124" s="54" t="s">
+        <v>224</v>
+      </c>
+      <c r="F124" s="57" t="s">
+        <v>53</v>
+      </c>
+      <c r="G124" s="54" t="s">
+        <v>212</v>
+      </c>
+      <c r="H124" s="60" t="s">
+        <v>213</v>
+      </c>
+      <c r="I124" s="48" t="s">
+        <v>26</v>
+      </c>
+      <c r="J124" s="51" t="s">
+        <v>56</v>
+      </c>
+      <c r="K124" s="48" t="s">
+        <v>28</v>
+      </c>
       <c r="L124" s="2"/>
       <c r="M124" s="2"/>
       <c r="N124" s="2"/>
@@ -6375,17 +6523,17 @@
       <c r="AA124" s="2"/>
     </row>
     <row r="125" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A125" s="2"/>
-      <c r="B125" s="38"/>
-      <c r="C125" s="2"/>
-      <c r="D125" s="38"/>
-      <c r="E125" s="38"/>
-      <c r="F125" s="2"/>
-      <c r="G125" s="38"/>
-      <c r="H125" s="38"/>
-      <c r="I125" s="2"/>
-      <c r="J125" s="38"/>
-      <c r="K125" s="2"/>
+      <c r="A125" s="64"/>
+      <c r="B125" s="55"/>
+      <c r="C125" s="55"/>
+      <c r="D125" s="55"/>
+      <c r="E125" s="55"/>
+      <c r="F125" s="58"/>
+      <c r="G125" s="55"/>
+      <c r="H125" s="61"/>
+      <c r="I125" s="49"/>
+      <c r="J125" s="52"/>
+      <c r="K125" s="49"/>
       <c r="L125" s="2"/>
       <c r="M125" s="2"/>
       <c r="N125" s="2"/>
@@ -6404,17 +6552,17 @@
       <c r="AA125" s="2"/>
     </row>
     <row r="126" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A126" s="2"/>
-      <c r="B126" s="38"/>
-      <c r="C126" s="2"/>
-      <c r="D126" s="38"/>
-      <c r="E126" s="38"/>
-      <c r="F126" s="2"/>
-      <c r="G126" s="38"/>
-      <c r="H126" s="38"/>
-      <c r="I126" s="2"/>
-      <c r="J126" s="38"/>
-      <c r="K126" s="2"/>
+      <c r="A126" s="64"/>
+      <c r="B126" s="55"/>
+      <c r="C126" s="55"/>
+      <c r="D126" s="55"/>
+      <c r="E126" s="55"/>
+      <c r="F126" s="59"/>
+      <c r="G126" s="55"/>
+      <c r="H126" s="61"/>
+      <c r="I126" s="49"/>
+      <c r="J126" s="52"/>
+      <c r="K126" s="49"/>
       <c r="L126" s="2"/>
       <c r="M126" s="2"/>
       <c r="N126" s="2"/>
@@ -6433,17 +6581,19 @@
       <c r="AA126" s="2"/>
     </row>
     <row r="127" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A127" s="2"/>
-      <c r="B127" s="38"/>
-      <c r="C127" s="2"/>
-      <c r="D127" s="38"/>
-      <c r="E127" s="38"/>
-      <c r="F127" s="2"/>
-      <c r="G127" s="38"/>
-      <c r="H127" s="38"/>
-      <c r="I127" s="2"/>
-      <c r="J127" s="38"/>
-      <c r="K127" s="2"/>
+      <c r="A127" s="65"/>
+      <c r="B127" s="56"/>
+      <c r="C127" s="56"/>
+      <c r="D127" s="56"/>
+      <c r="E127" s="56"/>
+      <c r="F127" s="30" t="s">
+        <v>67</v>
+      </c>
+      <c r="G127" s="30"/>
+      <c r="H127" s="30"/>
+      <c r="I127" s="50"/>
+      <c r="J127" s="53"/>
+      <c r="K127" s="50"/>
       <c r="L127" s="2"/>
       <c r="M127" s="2"/>
       <c r="N127" s="2"/>
@@ -6462,17 +6612,39 @@
       <c r="AA127" s="2"/>
     </row>
     <row r="128" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A128" s="2"/>
-      <c r="B128" s="38"/>
-      <c r="C128" s="2"/>
-      <c r="D128" s="38"/>
-      <c r="E128" s="38"/>
-      <c r="F128" s="2"/>
-      <c r="G128" s="38"/>
-      <c r="H128" s="38"/>
-      <c r="I128" s="2"/>
-      <c r="J128" s="38"/>
-      <c r="K128" s="2"/>
+      <c r="A128" s="63" t="s">
+        <v>221</v>
+      </c>
+      <c r="B128" s="54" t="s">
+        <v>201</v>
+      </c>
+      <c r="C128" s="54" t="s">
+        <v>214</v>
+      </c>
+      <c r="D128" s="54" t="s">
+        <v>215</v>
+      </c>
+      <c r="E128" s="54" t="s">
+        <v>225</v>
+      </c>
+      <c r="F128" s="57" t="s">
+        <v>53</v>
+      </c>
+      <c r="G128" s="57" t="s">
+        <v>216</v>
+      </c>
+      <c r="H128" s="60" t="s">
+        <v>217</v>
+      </c>
+      <c r="I128" s="48" t="s">
+        <v>26</v>
+      </c>
+      <c r="J128" s="51" t="s">
+        <v>56</v>
+      </c>
+      <c r="K128" s="48" t="s">
+        <v>28</v>
+      </c>
       <c r="L128" s="2"/>
       <c r="M128" s="2"/>
       <c r="N128" s="2"/>
@@ -6491,17 +6663,17 @@
       <c r="AA128" s="2"/>
     </row>
     <row r="129" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A129" s="2"/>
-      <c r="B129" s="38"/>
-      <c r="C129" s="2"/>
-      <c r="D129" s="38"/>
-      <c r="E129" s="38"/>
-      <c r="F129" s="2"/>
-      <c r="G129" s="38"/>
-      <c r="H129" s="38"/>
-      <c r="I129" s="2"/>
-      <c r="J129" s="38"/>
-      <c r="K129" s="2"/>
+      <c r="A129" s="64"/>
+      <c r="B129" s="55"/>
+      <c r="C129" s="55"/>
+      <c r="D129" s="55"/>
+      <c r="E129" s="55"/>
+      <c r="F129" s="59"/>
+      <c r="G129" s="59"/>
+      <c r="H129" s="62"/>
+      <c r="I129" s="49"/>
+      <c r="J129" s="52"/>
+      <c r="K129" s="49"/>
       <c r="L129" s="2"/>
       <c r="M129" s="2"/>
       <c r="N129" s="2"/>
@@ -6520,17 +6692,19 @@
       <c r="AA129" s="2"/>
     </row>
     <row r="130" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A130" s="2"/>
-      <c r="B130" s="38"/>
-      <c r="C130" s="2"/>
-      <c r="D130" s="38"/>
-      <c r="E130" s="38"/>
-      <c r="F130" s="2"/>
-      <c r="G130" s="38"/>
-      <c r="H130" s="38"/>
-      <c r="I130" s="2"/>
-      <c r="J130" s="38"/>
-      <c r="K130" s="2"/>
+      <c r="A130" s="64"/>
+      <c r="B130" s="55"/>
+      <c r="C130" s="55"/>
+      <c r="D130" s="55"/>
+      <c r="E130" s="55"/>
+      <c r="F130" s="30" t="s">
+        <v>67</v>
+      </c>
+      <c r="G130" s="30"/>
+      <c r="H130" s="30"/>
+      <c r="I130" s="49"/>
+      <c r="J130" s="52"/>
+      <c r="K130" s="49"/>
       <c r="L130" s="2"/>
       <c r="M130" s="2"/>
       <c r="N130" s="2"/>
@@ -6549,17 +6723,19 @@
       <c r="AA130" s="2"/>
     </row>
     <row r="131" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A131" s="2"/>
-      <c r="B131" s="38"/>
-      <c r="C131" s="2"/>
-      <c r="D131" s="38"/>
-      <c r="E131" s="38"/>
-      <c r="F131" s="2"/>
-      <c r="G131" s="38"/>
-      <c r="H131" s="38"/>
-      <c r="I131" s="2"/>
-      <c r="J131" s="38"/>
-      <c r="K131" s="2"/>
+      <c r="A131" s="65"/>
+      <c r="B131" s="56"/>
+      <c r="C131" s="56"/>
+      <c r="D131" s="56"/>
+      <c r="E131" s="56"/>
+      <c r="F131" s="30" t="s">
+        <v>70</v>
+      </c>
+      <c r="G131" s="30"/>
+      <c r="H131" s="30"/>
+      <c r="I131" s="50"/>
+      <c r="J131" s="53"/>
+      <c r="K131" s="50"/>
       <c r="L131" s="2"/>
       <c r="M131" s="2"/>
       <c r="N131" s="2"/>
@@ -29778,102 +29954,175 @@
       <c r="AA931" s="6"/>
     </row>
   </sheetData>
-  <mergeCells count="245">
-    <mergeCell ref="I108:I111"/>
-    <mergeCell ref="J108:J111"/>
-    <mergeCell ref="K108:K111"/>
-    <mergeCell ref="I112:I115"/>
-    <mergeCell ref="J112:J115"/>
-    <mergeCell ref="K112:K115"/>
-    <mergeCell ref="B112:B115"/>
-    <mergeCell ref="C112:C115"/>
-    <mergeCell ref="D112:D115"/>
-    <mergeCell ref="E112:E115"/>
-    <mergeCell ref="F112:F115"/>
-    <mergeCell ref="G112:G115"/>
-    <mergeCell ref="H112:H115"/>
-    <mergeCell ref="A108:A111"/>
-    <mergeCell ref="A112:A115"/>
-    <mergeCell ref="B108:B111"/>
-    <mergeCell ref="C108:C111"/>
-    <mergeCell ref="D108:D111"/>
-    <mergeCell ref="E108:E111"/>
-    <mergeCell ref="K84:K87"/>
-    <mergeCell ref="A88:A91"/>
-    <mergeCell ref="B88:B91"/>
-    <mergeCell ref="C88:C91"/>
-    <mergeCell ref="D88:D91"/>
-    <mergeCell ref="E88:E91"/>
-    <mergeCell ref="I88:I91"/>
-    <mergeCell ref="J88:J91"/>
-    <mergeCell ref="K88:K91"/>
-    <mergeCell ref="B84:B87"/>
-    <mergeCell ref="C84:C87"/>
-    <mergeCell ref="D84:D87"/>
-    <mergeCell ref="E84:E87"/>
-    <mergeCell ref="I84:I87"/>
-    <mergeCell ref="J84:J87"/>
-    <mergeCell ref="A84:A87"/>
-    <mergeCell ref="B36:B39"/>
-    <mergeCell ref="C36:C39"/>
-    <mergeCell ref="D36:D39"/>
-    <mergeCell ref="E36:E39"/>
-    <mergeCell ref="J44:J47"/>
-    <mergeCell ref="J36:J39"/>
-    <mergeCell ref="A76:A79"/>
-    <mergeCell ref="B76:B79"/>
-    <mergeCell ref="C76:C79"/>
-    <mergeCell ref="D76:D79"/>
-    <mergeCell ref="E76:E79"/>
-    <mergeCell ref="I76:I79"/>
-    <mergeCell ref="J76:J79"/>
-    <mergeCell ref="A60:A63"/>
-    <mergeCell ref="J56:J59"/>
-    <mergeCell ref="K44:K47"/>
-    <mergeCell ref="I48:I51"/>
-    <mergeCell ref="J48:J51"/>
-    <mergeCell ref="K48:K51"/>
-    <mergeCell ref="B48:B51"/>
-    <mergeCell ref="C48:C51"/>
-    <mergeCell ref="D48:D51"/>
-    <mergeCell ref="E48:E51"/>
-    <mergeCell ref="K40:K43"/>
-    <mergeCell ref="I40:I43"/>
-    <mergeCell ref="B40:B43"/>
-    <mergeCell ref="C40:C43"/>
-    <mergeCell ref="D40:D43"/>
-    <mergeCell ref="E40:E43"/>
-    <mergeCell ref="K76:K79"/>
-    <mergeCell ref="J80:J83"/>
-    <mergeCell ref="K80:K83"/>
-    <mergeCell ref="A80:A83"/>
-    <mergeCell ref="B80:B83"/>
-    <mergeCell ref="C80:C83"/>
-    <mergeCell ref="D80:D83"/>
-    <mergeCell ref="E80:E83"/>
-    <mergeCell ref="I80:I83"/>
-    <mergeCell ref="K56:K59"/>
-    <mergeCell ref="J60:J63"/>
-    <mergeCell ref="K60:K63"/>
-    <mergeCell ref="I68:I71"/>
-    <mergeCell ref="J68:J71"/>
-    <mergeCell ref="K68:K71"/>
-    <mergeCell ref="A72:A75"/>
-    <mergeCell ref="B72:B75"/>
-    <mergeCell ref="C72:C75"/>
-    <mergeCell ref="D72:D75"/>
-    <mergeCell ref="E72:E75"/>
-    <mergeCell ref="I72:I75"/>
-    <mergeCell ref="J72:J75"/>
-    <mergeCell ref="K72:K75"/>
-    <mergeCell ref="A68:A71"/>
-    <mergeCell ref="B68:B71"/>
-    <mergeCell ref="C68:C71"/>
-    <mergeCell ref="D68:D71"/>
-    <mergeCell ref="E68:E71"/>
-    <mergeCell ref="A64:A67"/>
-    <mergeCell ref="J64:J67"/>
-    <mergeCell ref="K64:K67"/>
+  <mergeCells count="289">
+    <mergeCell ref="A116:A119"/>
+    <mergeCell ref="A120:A123"/>
+    <mergeCell ref="A124:A127"/>
+    <mergeCell ref="A128:A131"/>
+    <mergeCell ref="I116:I119"/>
+    <mergeCell ref="J116:J119"/>
+    <mergeCell ref="K116:K119"/>
+    <mergeCell ref="I120:I123"/>
+    <mergeCell ref="J120:J123"/>
+    <mergeCell ref="K120:K123"/>
+    <mergeCell ref="I124:I127"/>
+    <mergeCell ref="J124:J127"/>
+    <mergeCell ref="K124:K127"/>
+    <mergeCell ref="I128:I131"/>
+    <mergeCell ref="J128:J131"/>
+    <mergeCell ref="K128:K131"/>
+    <mergeCell ref="B124:B127"/>
+    <mergeCell ref="C124:C127"/>
+    <mergeCell ref="D124:D127"/>
+    <mergeCell ref="E124:E127"/>
+    <mergeCell ref="F124:F126"/>
+    <mergeCell ref="G124:G126"/>
+    <mergeCell ref="H124:H126"/>
+    <mergeCell ref="B128:B131"/>
+    <mergeCell ref="C128:C131"/>
+    <mergeCell ref="D128:D131"/>
+    <mergeCell ref="E128:E131"/>
+    <mergeCell ref="F128:F129"/>
+    <mergeCell ref="G128:G129"/>
+    <mergeCell ref="H128:H129"/>
+    <mergeCell ref="B116:B119"/>
+    <mergeCell ref="C116:C119"/>
+    <mergeCell ref="D116:D119"/>
+    <mergeCell ref="E116:E119"/>
+    <mergeCell ref="F116:F118"/>
+    <mergeCell ref="G116:G118"/>
+    <mergeCell ref="H116:H118"/>
+    <mergeCell ref="B120:B123"/>
+    <mergeCell ref="C120:C123"/>
+    <mergeCell ref="D120:D123"/>
+    <mergeCell ref="E120:E123"/>
+    <mergeCell ref="F120:F122"/>
+    <mergeCell ref="G120:G122"/>
+    <mergeCell ref="H120:H122"/>
+    <mergeCell ref="J92:J95"/>
+    <mergeCell ref="K92:K95"/>
+    <mergeCell ref="I96:I99"/>
+    <mergeCell ref="J96:J99"/>
+    <mergeCell ref="K96:K99"/>
+    <mergeCell ref="I100:I103"/>
+    <mergeCell ref="J100:J103"/>
+    <mergeCell ref="K100:K103"/>
+    <mergeCell ref="I104:I107"/>
+    <mergeCell ref="J104:J107"/>
+    <mergeCell ref="K104:K107"/>
+    <mergeCell ref="D104:D107"/>
+    <mergeCell ref="E104:E107"/>
+    <mergeCell ref="A92:A95"/>
+    <mergeCell ref="A96:A99"/>
+    <mergeCell ref="A100:A103"/>
+    <mergeCell ref="A104:A107"/>
+    <mergeCell ref="I92:I95"/>
+    <mergeCell ref="B92:B95"/>
+    <mergeCell ref="C92:C95"/>
+    <mergeCell ref="D92:D95"/>
+    <mergeCell ref="E92:E95"/>
+    <mergeCell ref="B96:B99"/>
+    <mergeCell ref="C96:C99"/>
+    <mergeCell ref="D96:D99"/>
+    <mergeCell ref="E96:E99"/>
+    <mergeCell ref="B100:B103"/>
+    <mergeCell ref="C100:C103"/>
+    <mergeCell ref="D100:D103"/>
+    <mergeCell ref="E100:E103"/>
+    <mergeCell ref="C32:C35"/>
+    <mergeCell ref="B32:B35"/>
+    <mergeCell ref="B28:B31"/>
+    <mergeCell ref="C4:C7"/>
+    <mergeCell ref="C8:C11"/>
+    <mergeCell ref="C12:C15"/>
+    <mergeCell ref="C16:C19"/>
+    <mergeCell ref="C20:C23"/>
+    <mergeCell ref="C24:C27"/>
+    <mergeCell ref="C28:C31"/>
+    <mergeCell ref="A4:A7"/>
+    <mergeCell ref="A8:A11"/>
+    <mergeCell ref="A12:A15"/>
+    <mergeCell ref="A16:A19"/>
+    <mergeCell ref="A20:A23"/>
+    <mergeCell ref="A24:A27"/>
+    <mergeCell ref="B24:B27"/>
+    <mergeCell ref="B20:B23"/>
+    <mergeCell ref="B16:B19"/>
+    <mergeCell ref="B12:B15"/>
+    <mergeCell ref="B8:B11"/>
+    <mergeCell ref="B4:B7"/>
+    <mergeCell ref="K2:K3"/>
+    <mergeCell ref="I4:I7"/>
+    <mergeCell ref="I8:I11"/>
+    <mergeCell ref="I12:I15"/>
+    <mergeCell ref="I16:I19"/>
+    <mergeCell ref="E28:E31"/>
+    <mergeCell ref="E2:E3"/>
+    <mergeCell ref="G12:G13"/>
+    <mergeCell ref="G8:G9"/>
+    <mergeCell ref="F12:F13"/>
+    <mergeCell ref="F4:F5"/>
+    <mergeCell ref="F8:F9"/>
+    <mergeCell ref="K28:K31"/>
+    <mergeCell ref="E16:E19"/>
+    <mergeCell ref="E20:E23"/>
+    <mergeCell ref="E24:E27"/>
+    <mergeCell ref="F2:H2"/>
+    <mergeCell ref="I2:I3"/>
+    <mergeCell ref="I20:I23"/>
+    <mergeCell ref="I24:I27"/>
+    <mergeCell ref="I28:I31"/>
+    <mergeCell ref="E4:E7"/>
+    <mergeCell ref="E8:E11"/>
+    <mergeCell ref="E12:E15"/>
+    <mergeCell ref="E32:E35"/>
+    <mergeCell ref="C2:C3"/>
+    <mergeCell ref="H4:H5"/>
+    <mergeCell ref="G4:G5"/>
+    <mergeCell ref="H8:H9"/>
+    <mergeCell ref="H12:H13"/>
+    <mergeCell ref="K32:K35"/>
+    <mergeCell ref="K36:K39"/>
+    <mergeCell ref="J4:J7"/>
+    <mergeCell ref="J8:J11"/>
+    <mergeCell ref="J12:J15"/>
+    <mergeCell ref="J16:J19"/>
+    <mergeCell ref="J20:J23"/>
+    <mergeCell ref="J24:J27"/>
+    <mergeCell ref="J28:J31"/>
+    <mergeCell ref="I32:I35"/>
+    <mergeCell ref="I36:I39"/>
+    <mergeCell ref="K4:K7"/>
+    <mergeCell ref="K8:K11"/>
+    <mergeCell ref="K12:K15"/>
+    <mergeCell ref="K16:K19"/>
+    <mergeCell ref="K20:K23"/>
+    <mergeCell ref="K24:K27"/>
+    <mergeCell ref="J2:J3"/>
+    <mergeCell ref="J32:J35"/>
+    <mergeCell ref="B2:B3"/>
+    <mergeCell ref="A2:A3"/>
+    <mergeCell ref="A52:A55"/>
+    <mergeCell ref="B52:B55"/>
+    <mergeCell ref="C56:C59"/>
+    <mergeCell ref="D56:D59"/>
+    <mergeCell ref="C52:C55"/>
+    <mergeCell ref="D52:D55"/>
+    <mergeCell ref="A44:A47"/>
+    <mergeCell ref="A48:A51"/>
+    <mergeCell ref="D24:D27"/>
+    <mergeCell ref="D20:D23"/>
+    <mergeCell ref="D16:D19"/>
+    <mergeCell ref="D12:D15"/>
+    <mergeCell ref="D8:D11"/>
+    <mergeCell ref="D4:D7"/>
+    <mergeCell ref="A28:A31"/>
+    <mergeCell ref="A32:A35"/>
+    <mergeCell ref="A36:A39"/>
+    <mergeCell ref="A40:A43"/>
+    <mergeCell ref="D32:D35"/>
+    <mergeCell ref="D28:D31"/>
+    <mergeCell ref="A56:A59"/>
     <mergeCell ref="D2:D3"/>
     <mergeCell ref="J52:J55"/>
     <mergeCell ref="K52:K55"/>
@@ -29898,132 +30147,103 @@
     <mergeCell ref="I56:I59"/>
     <mergeCell ref="I44:I47"/>
     <mergeCell ref="J40:J43"/>
-    <mergeCell ref="J32:J35"/>
-    <mergeCell ref="B2:B3"/>
-    <mergeCell ref="A2:A3"/>
-    <mergeCell ref="A52:A55"/>
-    <mergeCell ref="B52:B55"/>
-    <mergeCell ref="C56:C59"/>
-    <mergeCell ref="D56:D59"/>
-    <mergeCell ref="C52:C55"/>
-    <mergeCell ref="D52:D55"/>
-    <mergeCell ref="A44:A47"/>
-    <mergeCell ref="A48:A51"/>
-    <mergeCell ref="D24:D27"/>
-    <mergeCell ref="D20:D23"/>
-    <mergeCell ref="D16:D19"/>
-    <mergeCell ref="D12:D15"/>
-    <mergeCell ref="D8:D11"/>
-    <mergeCell ref="D4:D7"/>
-    <mergeCell ref="A28:A31"/>
-    <mergeCell ref="A32:A35"/>
-    <mergeCell ref="A36:A39"/>
-    <mergeCell ref="A40:A43"/>
-    <mergeCell ref="D32:D35"/>
-    <mergeCell ref="D28:D31"/>
-    <mergeCell ref="A56:A59"/>
-    <mergeCell ref="E32:E35"/>
-    <mergeCell ref="C2:C3"/>
-    <mergeCell ref="H4:H5"/>
-    <mergeCell ref="G4:G5"/>
-    <mergeCell ref="H8:H9"/>
-    <mergeCell ref="H12:H13"/>
-    <mergeCell ref="K32:K35"/>
-    <mergeCell ref="K36:K39"/>
-    <mergeCell ref="J4:J7"/>
-    <mergeCell ref="J8:J11"/>
-    <mergeCell ref="J12:J15"/>
-    <mergeCell ref="J16:J19"/>
-    <mergeCell ref="J20:J23"/>
-    <mergeCell ref="J24:J27"/>
-    <mergeCell ref="J28:J31"/>
-    <mergeCell ref="I32:I35"/>
-    <mergeCell ref="I36:I39"/>
-    <mergeCell ref="K4:K7"/>
-    <mergeCell ref="K8:K11"/>
-    <mergeCell ref="K12:K15"/>
-    <mergeCell ref="K16:K19"/>
-    <mergeCell ref="K20:K23"/>
-    <mergeCell ref="K24:K27"/>
-    <mergeCell ref="J2:J3"/>
-    <mergeCell ref="K2:K3"/>
-    <mergeCell ref="I4:I7"/>
-    <mergeCell ref="I8:I11"/>
-    <mergeCell ref="I12:I15"/>
-    <mergeCell ref="I16:I19"/>
-    <mergeCell ref="E28:E31"/>
-    <mergeCell ref="E2:E3"/>
-    <mergeCell ref="G12:G13"/>
-    <mergeCell ref="G8:G9"/>
-    <mergeCell ref="F12:F13"/>
-    <mergeCell ref="F4:F5"/>
-    <mergeCell ref="F8:F9"/>
-    <mergeCell ref="K28:K31"/>
-    <mergeCell ref="E16:E19"/>
-    <mergeCell ref="E20:E23"/>
-    <mergeCell ref="E24:E27"/>
-    <mergeCell ref="F2:H2"/>
-    <mergeCell ref="I2:I3"/>
-    <mergeCell ref="I20:I23"/>
-    <mergeCell ref="I24:I27"/>
-    <mergeCell ref="I28:I31"/>
-    <mergeCell ref="E4:E7"/>
-    <mergeCell ref="E8:E11"/>
-    <mergeCell ref="E12:E15"/>
-    <mergeCell ref="A4:A7"/>
-    <mergeCell ref="A8:A11"/>
-    <mergeCell ref="A12:A15"/>
-    <mergeCell ref="A16:A19"/>
-    <mergeCell ref="A20:A23"/>
-    <mergeCell ref="A24:A27"/>
-    <mergeCell ref="B24:B27"/>
-    <mergeCell ref="B20:B23"/>
-    <mergeCell ref="B16:B19"/>
-    <mergeCell ref="B12:B15"/>
-    <mergeCell ref="B8:B11"/>
-    <mergeCell ref="B4:B7"/>
-    <mergeCell ref="C32:C35"/>
-    <mergeCell ref="B32:B35"/>
-    <mergeCell ref="B28:B31"/>
-    <mergeCell ref="C4:C7"/>
-    <mergeCell ref="C8:C11"/>
-    <mergeCell ref="C12:C15"/>
-    <mergeCell ref="C16:C19"/>
-    <mergeCell ref="C20:C23"/>
-    <mergeCell ref="C24:C27"/>
-    <mergeCell ref="C28:C31"/>
+    <mergeCell ref="K56:K59"/>
+    <mergeCell ref="J60:J63"/>
+    <mergeCell ref="K60:K63"/>
+    <mergeCell ref="I68:I71"/>
+    <mergeCell ref="J68:J71"/>
+    <mergeCell ref="K68:K71"/>
+    <mergeCell ref="A72:A75"/>
+    <mergeCell ref="B72:B75"/>
+    <mergeCell ref="C72:C75"/>
+    <mergeCell ref="D72:D75"/>
+    <mergeCell ref="E72:E75"/>
+    <mergeCell ref="I72:I75"/>
+    <mergeCell ref="J72:J75"/>
+    <mergeCell ref="K72:K75"/>
+    <mergeCell ref="A68:A71"/>
+    <mergeCell ref="B68:B71"/>
+    <mergeCell ref="C68:C71"/>
+    <mergeCell ref="D68:D71"/>
+    <mergeCell ref="E68:E71"/>
+    <mergeCell ref="A64:A67"/>
+    <mergeCell ref="J64:J67"/>
+    <mergeCell ref="K64:K67"/>
+    <mergeCell ref="K76:K79"/>
+    <mergeCell ref="J80:J83"/>
+    <mergeCell ref="K80:K83"/>
+    <mergeCell ref="A80:A83"/>
+    <mergeCell ref="B80:B83"/>
+    <mergeCell ref="C80:C83"/>
+    <mergeCell ref="D80:D83"/>
+    <mergeCell ref="E80:E83"/>
+    <mergeCell ref="I80:I83"/>
+    <mergeCell ref="K44:K47"/>
+    <mergeCell ref="I48:I51"/>
+    <mergeCell ref="J48:J51"/>
+    <mergeCell ref="K48:K51"/>
+    <mergeCell ref="B48:B51"/>
+    <mergeCell ref="C48:C51"/>
+    <mergeCell ref="D48:D51"/>
+    <mergeCell ref="E48:E51"/>
+    <mergeCell ref="K40:K43"/>
+    <mergeCell ref="I40:I43"/>
+    <mergeCell ref="B40:B43"/>
+    <mergeCell ref="C40:C43"/>
+    <mergeCell ref="D40:D43"/>
+    <mergeCell ref="E40:E43"/>
+    <mergeCell ref="B36:B39"/>
+    <mergeCell ref="C36:C39"/>
+    <mergeCell ref="D36:D39"/>
+    <mergeCell ref="E36:E39"/>
+    <mergeCell ref="J44:J47"/>
+    <mergeCell ref="J36:J39"/>
+    <mergeCell ref="A76:A79"/>
+    <mergeCell ref="B76:B79"/>
+    <mergeCell ref="C76:C79"/>
+    <mergeCell ref="D76:D79"/>
+    <mergeCell ref="E76:E79"/>
+    <mergeCell ref="I76:I79"/>
+    <mergeCell ref="J76:J79"/>
+    <mergeCell ref="A60:A63"/>
+    <mergeCell ref="J56:J59"/>
+    <mergeCell ref="A108:A111"/>
+    <mergeCell ref="A112:A115"/>
+    <mergeCell ref="B108:B111"/>
+    <mergeCell ref="C108:C111"/>
+    <mergeCell ref="D108:D111"/>
+    <mergeCell ref="E108:E111"/>
+    <mergeCell ref="K84:K87"/>
+    <mergeCell ref="A88:A91"/>
+    <mergeCell ref="B88:B91"/>
+    <mergeCell ref="C88:C91"/>
+    <mergeCell ref="D88:D91"/>
+    <mergeCell ref="E88:E91"/>
+    <mergeCell ref="I88:I91"/>
+    <mergeCell ref="J88:J91"/>
+    <mergeCell ref="K88:K91"/>
+    <mergeCell ref="B84:B87"/>
+    <mergeCell ref="C84:C87"/>
+    <mergeCell ref="D84:D87"/>
+    <mergeCell ref="E84:E87"/>
+    <mergeCell ref="I84:I87"/>
+    <mergeCell ref="J84:J87"/>
+    <mergeCell ref="A84:A87"/>
     <mergeCell ref="B104:B107"/>
     <mergeCell ref="C104:C107"/>
-    <mergeCell ref="D104:D107"/>
-    <mergeCell ref="E104:E107"/>
-    <mergeCell ref="A92:A95"/>
-    <mergeCell ref="A96:A99"/>
-    <mergeCell ref="A100:A103"/>
-    <mergeCell ref="A104:A107"/>
-    <mergeCell ref="I92:I95"/>
-    <mergeCell ref="B92:B95"/>
-    <mergeCell ref="C92:C95"/>
-    <mergeCell ref="D92:D95"/>
-    <mergeCell ref="E92:E95"/>
-    <mergeCell ref="B96:B99"/>
-    <mergeCell ref="C96:C99"/>
-    <mergeCell ref="D96:D99"/>
-    <mergeCell ref="E96:E99"/>
-    <mergeCell ref="B100:B103"/>
-    <mergeCell ref="C100:C103"/>
-    <mergeCell ref="D100:D103"/>
-    <mergeCell ref="E100:E103"/>
-    <mergeCell ref="J92:J95"/>
-    <mergeCell ref="K92:K95"/>
-    <mergeCell ref="I96:I99"/>
-    <mergeCell ref="J96:J99"/>
-    <mergeCell ref="K96:K99"/>
-    <mergeCell ref="I100:I103"/>
-    <mergeCell ref="J100:J103"/>
-    <mergeCell ref="K100:K103"/>
-    <mergeCell ref="I104:I107"/>
-    <mergeCell ref="J104:J107"/>
-    <mergeCell ref="K104:K107"/>
+    <mergeCell ref="I108:I111"/>
+    <mergeCell ref="J108:J111"/>
+    <mergeCell ref="K108:K111"/>
+    <mergeCell ref="I112:I115"/>
+    <mergeCell ref="J112:J115"/>
+    <mergeCell ref="K112:K115"/>
+    <mergeCell ref="B112:B115"/>
+    <mergeCell ref="C112:C115"/>
+    <mergeCell ref="D112:D115"/>
+    <mergeCell ref="E112:E115"/>
+    <mergeCell ref="F112:F115"/>
+    <mergeCell ref="G112:G115"/>
+    <mergeCell ref="H112:H115"/>
   </mergeCells>
   <conditionalFormatting sqref="I4 I8 I12">
     <cfRule type="cellIs" dxfId="27" priority="21" operator="equal">
@@ -30125,31 +30345,31 @@
       <formula>"IN REVIEW"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I88 I92 I96 I100 I104 I108 I112">
+  <conditionalFormatting sqref="I88 I92 I96 I100 I104 I108 I112 I116 I120 I124 I128">
     <cfRule type="cellIs" dxfId="7" priority="1" operator="equal">
       <formula>"TO DO"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I88 I92 I96 I100 I104 I108 I112">
+  <conditionalFormatting sqref="I88 I92 I96 I100 I104 I108 I112 I116 I120 I124 I128">
     <cfRule type="cellIs" dxfId="6" priority="2" operator="equal">
       <formula>"IN PROGRESS"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I88 I92 I96 I100 I104 I108 I112">
+  <conditionalFormatting sqref="I88 I92 I96 I100 I104 I108 I112 I116 I120 I124 I128">
     <cfRule type="cellIs" dxfId="5" priority="3" operator="equal">
       <formula>"REVIEWED"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I88 I92 I96 I100 I104 I108 I112">
+  <conditionalFormatting sqref="I88 I92 I96 I100 I104 I108 I112 I116 I120 I124 I128">
     <cfRule type="cellIs" dxfId="4" priority="4" operator="equal">
       <formula>"IN REVIEW"</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" sqref="I52 I64 I24 I16 I20 I4 I8 I12 I68 I56 I60 I32 I36 I28 I40 I44 I48 I84 I76 I72 I80 I88 I92 I96 I100 I104 I108 I112">
+    <dataValidation type="list" allowBlank="1" sqref="I52 I64 I24 I16 I20 I4 I8 I12 I68 I56 I60 I32 I36 I28 I40 I44 I48 I84 I76 I72 I80 I88 I92 I96 I100 I104 I108 I112 I116 I120 I124 I128">
       <formula1>"TO DO,In Progress,In Review,Reviewed"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" sqref="K76 K36 K40 K32 K28 K4 K12 K8 K48 K44 K52 K60 K56 K64 K68 K72 K80 K20 K24 K16 K84 K88 K92 K96 K100 K104 K108 K112">
+    <dataValidation type="list" allowBlank="1" sqref="K76 K36 K40 K32 K28 K4 K12 K8 K48 K44 K52 K60 K56 K64 K68 K72 K80 K20 K24 K16 K84 K88 K92 K96 K100 K104 K108 K112 K116 K120 K124 K128">
       <formula1>"Smoke,Regresión"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
Se resuelven los casos de prueba correspondientes a la US42
</commit_message>
<xml_diff>
--- a/Testing 2024/template_caso_prueba-ISPC2024-sprint-1.xlsx
+++ b/Testing 2024/template_caso_prueba-ISPC2024-sprint-1.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\giuly\OneDrive\Escritorio\ISPC\Tercer Año\Practica profesional\PROYECTO\practicaProfesionalizante-ISPC\Testing 2024\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\giuly\OneDrive\Escritorio\practicaProfesionalizante-ISPC\Testing 2024\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F5AC43C-6C53-423C-B466-7CF0BD4C20FF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{82ED24DA-04B0-4069-9572-4E2AE4F04227}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1271,6 +1271,15 @@
     <xf numFmtId="0" fontId="1" fillId="7" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="14" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="14" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="14" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1312,14 +1321,23 @@
     <xf numFmtId="0" fontId="1" fillId="7" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="14" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="12" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="14" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="12" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="14" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="12" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="10" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1330,50 +1348,20 @@
     <xf numFmtId="0" fontId="1" fillId="10" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="13" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="11" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="13" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="11" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="13" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="11" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="12" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="12" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="12" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1390,14 +1378,26 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="11" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="11" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="11" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="13" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="13" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="13" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1947,8 +1947,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AA931"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B110" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="60" workbookViewId="0">
-      <selection activeCell="I116" sqref="I116:I119"/>
+    <sheetView tabSelected="1" topLeftCell="A65" zoomScale="79" zoomScaleNormal="79" zoomScalePageLayoutView="60" workbookViewId="0">
+      <selection activeCell="I84" sqref="I84:I87"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.54296875" defaultRowHeight="12.5"/>
@@ -1997,33 +1997,33 @@
       <c r="AA1" s="2"/>
     </row>
     <row r="2" spans="1:27" s="30" customFormat="1" ht="15.75" customHeight="1">
-      <c r="A2" s="83" t="s">
+      <c r="A2" s="86" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="81" t="s">
+      <c r="B2" s="79" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="83" t="s">
+      <c r="C2" s="86" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="81" t="s">
+      <c r="D2" s="79" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="81" t="s">
+      <c r="E2" s="79" t="s">
         <v>4</v>
       </c>
-      <c r="F2" s="85" t="s">
+      <c r="F2" s="81" t="s">
         <v>5</v>
       </c>
-      <c r="G2" s="86"/>
-      <c r="H2" s="87"/>
-      <c r="I2" s="88" t="s">
+      <c r="G2" s="82"/>
+      <c r="H2" s="83"/>
+      <c r="I2" s="84" t="s">
         <v>6</v>
       </c>
-      <c r="J2" s="81" t="s">
+      <c r="J2" s="79" t="s">
         <v>7</v>
       </c>
-      <c r="K2" s="81" t="s">
+      <c r="K2" s="79" t="s">
         <v>27</v>
       </c>
       <c r="L2" s="31"/>
@@ -2044,11 +2044,11 @@
       <c r="AA2" s="32"/>
     </row>
     <row r="3" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A3" s="84"/>
-      <c r="B3" s="82"/>
-      <c r="C3" s="84"/>
-      <c r="D3" s="82"/>
-      <c r="E3" s="82"/>
+      <c r="A3" s="87"/>
+      <c r="B3" s="80"/>
+      <c r="C3" s="87"/>
+      <c r="D3" s="80"/>
+      <c r="E3" s="80"/>
       <c r="F3" s="33" t="s">
         <v>8</v>
       </c>
@@ -2058,9 +2058,9 @@
       <c r="H3" s="41" t="s">
         <v>10</v>
       </c>
-      <c r="I3" s="89"/>
-      <c r="J3" s="82"/>
-      <c r="K3" s="82"/>
+      <c r="I3" s="85"/>
+      <c r="J3" s="80"/>
+      <c r="K3" s="80"/>
       <c r="L3" s="3"/>
       <c r="M3" s="2"/>
       <c r="N3" s="2"/>
@@ -2079,37 +2079,37 @@
       <c r="AA3" s="2"/>
     </row>
     <row r="4" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A4" s="67" t="s">
+      <c r="A4" s="73" t="s">
         <v>29</v>
       </c>
-      <c r="B4" s="55" t="s">
+      <c r="B4" s="58" t="s">
         <v>49</v>
       </c>
-      <c r="C4" s="55" t="s">
+      <c r="C4" s="58" t="s">
         <v>50</v>
       </c>
-      <c r="D4" s="55" t="s">
+      <c r="D4" s="58" t="s">
         <v>51</v>
       </c>
-      <c r="E4" s="55" t="s">
+      <c r="E4" s="58" t="s">
         <v>52</v>
       </c>
-      <c r="F4" s="55" t="s">
+      <c r="F4" s="58" t="s">
         <v>53</v>
       </c>
-      <c r="G4" s="55" t="s">
+      <c r="G4" s="58" t="s">
         <v>54</v>
       </c>
-      <c r="H4" s="61" t="s">
+      <c r="H4" s="64" t="s">
         <v>55</v>
       </c>
-      <c r="I4" s="49" t="s">
+      <c r="I4" s="52" t="s">
         <v>26</v>
       </c>
-      <c r="J4" s="52" t="s">
+      <c r="J4" s="55" t="s">
         <v>56</v>
       </c>
-      <c r="K4" s="49" t="s">
+      <c r="K4" s="52" t="s">
         <v>28</v>
       </c>
       <c r="L4" s="3"/>
@@ -2130,17 +2130,17 @@
       <c r="AA4" s="2"/>
     </row>
     <row r="5" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A5" s="68"/>
-      <c r="B5" s="56"/>
-      <c r="C5" s="56"/>
-      <c r="D5" s="56"/>
-      <c r="E5" s="56"/>
-      <c r="F5" s="57"/>
-      <c r="G5" s="57"/>
-      <c r="H5" s="63"/>
-      <c r="I5" s="50"/>
-      <c r="J5" s="53"/>
-      <c r="K5" s="50"/>
+      <c r="A5" s="74"/>
+      <c r="B5" s="59"/>
+      <c r="C5" s="59"/>
+      <c r="D5" s="59"/>
+      <c r="E5" s="59"/>
+      <c r="F5" s="60"/>
+      <c r="G5" s="60"/>
+      <c r="H5" s="66"/>
+      <c r="I5" s="53"/>
+      <c r="J5" s="56"/>
+      <c r="K5" s="53"/>
       <c r="L5" s="3"/>
       <c r="M5" s="2"/>
       <c r="N5" s="2"/>
@@ -2159,17 +2159,17 @@
       <c r="AA5" s="2"/>
     </row>
     <row r="6" spans="1:27" s="28" customFormat="1" ht="15.75" customHeight="1">
-      <c r="A6" s="68"/>
-      <c r="B6" s="56"/>
-      <c r="C6" s="56"/>
-      <c r="D6" s="56"/>
-      <c r="E6" s="56"/>
+      <c r="A6" s="74"/>
+      <c r="B6" s="59"/>
+      <c r="C6" s="59"/>
+      <c r="D6" s="59"/>
+      <c r="E6" s="59"/>
       <c r="F6" s="29"/>
       <c r="G6" s="34"/>
       <c r="H6" s="34"/>
-      <c r="I6" s="50"/>
-      <c r="J6" s="53"/>
-      <c r="K6" s="50"/>
+      <c r="I6" s="53"/>
+      <c r="J6" s="56"/>
+      <c r="K6" s="53"/>
       <c r="L6" s="26"/>
       <c r="M6" s="27"/>
       <c r="N6" s="27"/>
@@ -2188,17 +2188,17 @@
       <c r="AA6" s="27"/>
     </row>
     <row r="7" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A7" s="69"/>
-      <c r="B7" s="57"/>
-      <c r="C7" s="57"/>
-      <c r="D7" s="57"/>
-      <c r="E7" s="57"/>
+      <c r="A7" s="75"/>
+      <c r="B7" s="60"/>
+      <c r="C7" s="60"/>
+      <c r="D7" s="60"/>
+      <c r="E7" s="60"/>
       <c r="F7" s="29"/>
       <c r="G7" s="34"/>
       <c r="H7" s="34"/>
-      <c r="I7" s="51"/>
-      <c r="J7" s="54"/>
-      <c r="K7" s="51"/>
+      <c r="I7" s="54"/>
+      <c r="J7" s="57"/>
+      <c r="K7" s="54"/>
       <c r="L7" s="3"/>
       <c r="M7" s="2"/>
       <c r="N7" s="2"/>
@@ -2217,37 +2217,37 @@
       <c r="AA7" s="2"/>
     </row>
     <row r="8" spans="1:27">
-      <c r="A8" s="67" t="s">
+      <c r="A8" s="73" t="s">
         <v>30</v>
       </c>
-      <c r="B8" s="55" t="s">
+      <c r="B8" s="58" t="s">
         <v>49</v>
       </c>
-      <c r="C8" s="55" t="s">
+      <c r="C8" s="58" t="s">
         <v>57</v>
       </c>
-      <c r="D8" s="55" t="s">
+      <c r="D8" s="58" t="s">
         <v>58</v>
       </c>
-      <c r="E8" s="55" t="s">
+      <c r="E8" s="58" t="s">
         <v>59</v>
       </c>
-      <c r="F8" s="55" t="s">
+      <c r="F8" s="58" t="s">
         <v>53</v>
       </c>
-      <c r="G8" s="55" t="s">
+      <c r="G8" s="58" t="s">
         <v>54</v>
       </c>
-      <c r="H8" s="61" t="s">
+      <c r="H8" s="64" t="s">
         <v>55</v>
       </c>
-      <c r="I8" s="49" t="s">
+      <c r="I8" s="52" t="s">
         <v>26</v>
       </c>
-      <c r="J8" s="52" t="s">
+      <c r="J8" s="55" t="s">
         <v>56</v>
       </c>
-      <c r="K8" s="49" t="s">
+      <c r="K8" s="52" t="s">
         <v>28</v>
       </c>
       <c r="L8" s="3"/>
@@ -2268,17 +2268,17 @@
       <c r="AA8" s="2"/>
     </row>
     <row r="9" spans="1:27">
-      <c r="A9" s="68"/>
-      <c r="B9" s="56"/>
-      <c r="C9" s="56"/>
-      <c r="D9" s="56"/>
-      <c r="E9" s="56"/>
-      <c r="F9" s="57"/>
-      <c r="G9" s="57"/>
-      <c r="H9" s="63"/>
-      <c r="I9" s="50"/>
-      <c r="J9" s="53"/>
-      <c r="K9" s="50"/>
+      <c r="A9" s="74"/>
+      <c r="B9" s="59"/>
+      <c r="C9" s="59"/>
+      <c r="D9" s="59"/>
+      <c r="E9" s="59"/>
+      <c r="F9" s="60"/>
+      <c r="G9" s="60"/>
+      <c r="H9" s="66"/>
+      <c r="I9" s="53"/>
+      <c r="J9" s="56"/>
+      <c r="K9" s="53"/>
       <c r="L9" s="3"/>
       <c r="M9" s="2"/>
       <c r="N9" s="2"/>
@@ -2297,17 +2297,17 @@
       <c r="AA9" s="2"/>
     </row>
     <row r="10" spans="1:27" s="28" customFormat="1" ht="15.75" customHeight="1">
-      <c r="A10" s="68"/>
-      <c r="B10" s="56"/>
-      <c r="C10" s="56"/>
-      <c r="D10" s="56"/>
-      <c r="E10" s="56"/>
+      <c r="A10" s="74"/>
+      <c r="B10" s="59"/>
+      <c r="C10" s="59"/>
+      <c r="D10" s="59"/>
+      <c r="E10" s="59"/>
       <c r="F10" s="29"/>
       <c r="G10" s="34"/>
       <c r="H10" s="34"/>
-      <c r="I10" s="50"/>
-      <c r="J10" s="53"/>
-      <c r="K10" s="50"/>
+      <c r="I10" s="53"/>
+      <c r="J10" s="56"/>
+      <c r="K10" s="53"/>
       <c r="L10" s="26"/>
       <c r="M10" s="27"/>
       <c r="N10" s="27"/>
@@ -2326,17 +2326,17 @@
       <c r="AA10" s="27"/>
     </row>
     <row r="11" spans="1:27">
-      <c r="A11" s="69"/>
-      <c r="B11" s="57"/>
-      <c r="C11" s="57"/>
-      <c r="D11" s="57"/>
-      <c r="E11" s="57"/>
+      <c r="A11" s="75"/>
+      <c r="B11" s="60"/>
+      <c r="C11" s="60"/>
+      <c r="D11" s="60"/>
+      <c r="E11" s="60"/>
       <c r="F11" s="29"/>
       <c r="G11" s="34"/>
       <c r="H11" s="34"/>
-      <c r="I11" s="51"/>
-      <c r="J11" s="54"/>
-      <c r="K11" s="51"/>
+      <c r="I11" s="54"/>
+      <c r="J11" s="57"/>
+      <c r="K11" s="54"/>
       <c r="L11" s="3"/>
       <c r="M11" s="2"/>
       <c r="N11" s="2"/>
@@ -2355,37 +2355,37 @@
       <c r="AA11" s="2"/>
     </row>
     <row r="12" spans="1:27">
-      <c r="A12" s="67" t="s">
+      <c r="A12" s="73" t="s">
         <v>31</v>
       </c>
-      <c r="B12" s="55" t="s">
+      <c r="B12" s="58" t="s">
         <v>49</v>
       </c>
-      <c r="C12" s="55" t="s">
+      <c r="C12" s="58" t="s">
         <v>60</v>
       </c>
-      <c r="D12" s="55" t="s">
+      <c r="D12" s="58" t="s">
         <v>61</v>
       </c>
-      <c r="E12" s="55" t="s">
+      <c r="E12" s="58" t="s">
         <v>62</v>
       </c>
-      <c r="F12" s="55" t="s">
+      <c r="F12" s="58" t="s">
         <v>53</v>
       </c>
-      <c r="G12" s="55" t="s">
+      <c r="G12" s="58" t="s">
         <v>54</v>
       </c>
-      <c r="H12" s="61" t="s">
+      <c r="H12" s="64" t="s">
         <v>55</v>
       </c>
-      <c r="I12" s="49" t="s">
+      <c r="I12" s="52" t="s">
         <v>26</v>
       </c>
-      <c r="J12" s="52" t="s">
+      <c r="J12" s="55" t="s">
         <v>56</v>
       </c>
-      <c r="K12" s="49" t="s">
+      <c r="K12" s="52" t="s">
         <v>28</v>
       </c>
       <c r="L12" s="2"/>
@@ -2406,17 +2406,17 @@
       <c r="AA12" s="2"/>
     </row>
     <row r="13" spans="1:27">
-      <c r="A13" s="68"/>
-      <c r="B13" s="56"/>
-      <c r="C13" s="56"/>
-      <c r="D13" s="56"/>
-      <c r="E13" s="56"/>
-      <c r="F13" s="57"/>
-      <c r="G13" s="57"/>
-      <c r="H13" s="63"/>
-      <c r="I13" s="50"/>
-      <c r="J13" s="53"/>
-      <c r="K13" s="50"/>
+      <c r="A13" s="74"/>
+      <c r="B13" s="59"/>
+      <c r="C13" s="59"/>
+      <c r="D13" s="59"/>
+      <c r="E13" s="59"/>
+      <c r="F13" s="60"/>
+      <c r="G13" s="60"/>
+      <c r="H13" s="66"/>
+      <c r="I13" s="53"/>
+      <c r="J13" s="56"/>
+      <c r="K13" s="53"/>
       <c r="L13" s="2"/>
       <c r="M13" s="2"/>
       <c r="N13" s="2"/>
@@ -2435,17 +2435,17 @@
       <c r="AA13" s="2"/>
     </row>
     <row r="14" spans="1:27" s="28" customFormat="1">
-      <c r="A14" s="68"/>
-      <c r="B14" s="56"/>
-      <c r="C14" s="56"/>
-      <c r="D14" s="56"/>
-      <c r="E14" s="56"/>
+      <c r="A14" s="74"/>
+      <c r="B14" s="59"/>
+      <c r="C14" s="59"/>
+      <c r="D14" s="59"/>
+      <c r="E14" s="59"/>
       <c r="F14" s="29"/>
       <c r="G14" s="34"/>
       <c r="H14" s="34"/>
-      <c r="I14" s="50"/>
-      <c r="J14" s="53"/>
-      <c r="K14" s="50"/>
+      <c r="I14" s="53"/>
+      <c r="J14" s="56"/>
+      <c r="K14" s="53"/>
       <c r="L14" s="27"/>
       <c r="M14" s="27"/>
       <c r="N14" s="27"/>
@@ -2464,17 +2464,17 @@
       <c r="AA14" s="27"/>
     </row>
     <row r="15" spans="1:27">
-      <c r="A15" s="69"/>
-      <c r="B15" s="57"/>
-      <c r="C15" s="57"/>
-      <c r="D15" s="57"/>
-      <c r="E15" s="57"/>
+      <c r="A15" s="75"/>
+      <c r="B15" s="60"/>
+      <c r="C15" s="60"/>
+      <c r="D15" s="60"/>
+      <c r="E15" s="60"/>
       <c r="F15" s="29"/>
       <c r="G15" s="34"/>
       <c r="H15" s="34"/>
-      <c r="I15" s="51"/>
-      <c r="J15" s="54"/>
-      <c r="K15" s="51"/>
+      <c r="I15" s="54"/>
+      <c r="J15" s="57"/>
+      <c r="K15" s="54"/>
       <c r="L15" s="2"/>
       <c r="M15" s="2"/>
       <c r="N15" s="2"/>
@@ -2493,19 +2493,19 @@
       <c r="AA15" s="2"/>
     </row>
     <row r="16" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A16" s="90" t="s">
+      <c r="A16" s="76" t="s">
         <v>32</v>
       </c>
-      <c r="B16" s="55" t="s">
+      <c r="B16" s="58" t="s">
         <v>63</v>
       </c>
-      <c r="C16" s="55" t="s">
+      <c r="C16" s="58" t="s">
         <v>64</v>
       </c>
-      <c r="D16" s="55" t="s">
+      <c r="D16" s="58" t="s">
         <v>65</v>
       </c>
-      <c r="E16" s="55" t="s">
+      <c r="E16" s="58" t="s">
         <v>83</v>
       </c>
       <c r="F16" s="29" t="s">
@@ -2517,13 +2517,13 @@
       <c r="H16" s="34" t="s">
         <v>66</v>
       </c>
-      <c r="I16" s="49" t="s">
+      <c r="I16" s="52" t="s">
         <v>26</v>
       </c>
-      <c r="J16" s="52" t="s">
+      <c r="J16" s="55" t="s">
         <v>56</v>
       </c>
-      <c r="K16" s="49" t="s">
+      <c r="K16" s="52" t="s">
         <v>28</v>
       </c>
       <c r="L16" s="2"/>
@@ -2544,11 +2544,11 @@
       <c r="AA16" s="2"/>
     </row>
     <row r="17" spans="1:27" ht="16.5" customHeight="1">
-      <c r="A17" s="91"/>
-      <c r="B17" s="56"/>
-      <c r="C17" s="56"/>
-      <c r="D17" s="56"/>
-      <c r="E17" s="56"/>
+      <c r="A17" s="77"/>
+      <c r="B17" s="59"/>
+      <c r="C17" s="59"/>
+      <c r="D17" s="59"/>
+      <c r="E17" s="59"/>
       <c r="F17" s="29" t="s">
         <v>67</v>
       </c>
@@ -2558,9 +2558,9 @@
       <c r="H17" s="34" t="s">
         <v>69</v>
       </c>
-      <c r="I17" s="50"/>
-      <c r="J17" s="53"/>
-      <c r="K17" s="50"/>
+      <c r="I17" s="53"/>
+      <c r="J17" s="56"/>
+      <c r="K17" s="53"/>
       <c r="L17" s="2"/>
       <c r="M17" s="2"/>
       <c r="N17" s="2"/>
@@ -2579,11 +2579,11 @@
       <c r="AA17" s="2"/>
     </row>
     <row r="18" spans="1:27" s="28" customFormat="1" ht="25">
-      <c r="A18" s="91"/>
-      <c r="B18" s="56"/>
-      <c r="C18" s="56"/>
-      <c r="D18" s="56"/>
-      <c r="E18" s="56"/>
+      <c r="A18" s="77"/>
+      <c r="B18" s="59"/>
+      <c r="C18" s="59"/>
+      <c r="D18" s="59"/>
+      <c r="E18" s="59"/>
       <c r="F18" s="29" t="s">
         <v>70</v>
       </c>
@@ -2593,9 +2593,9 @@
       <c r="H18" s="34" t="s">
         <v>72</v>
       </c>
-      <c r="I18" s="50"/>
-      <c r="J18" s="53"/>
-      <c r="K18" s="50"/>
+      <c r="I18" s="53"/>
+      <c r="J18" s="56"/>
+      <c r="K18" s="53"/>
       <c r="L18" s="27"/>
       <c r="M18" s="27"/>
       <c r="N18" s="27"/>
@@ -2614,17 +2614,17 @@
       <c r="AA18" s="27"/>
     </row>
     <row r="19" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A19" s="92"/>
-      <c r="B19" s="57"/>
-      <c r="C19" s="57"/>
-      <c r="D19" s="57"/>
-      <c r="E19" s="57"/>
+      <c r="A19" s="78"/>
+      <c r="B19" s="60"/>
+      <c r="C19" s="60"/>
+      <c r="D19" s="60"/>
+      <c r="E19" s="60"/>
       <c r="F19" s="29"/>
       <c r="G19" s="34"/>
       <c r="H19" s="34"/>
-      <c r="I19" s="51"/>
-      <c r="J19" s="54"/>
-      <c r="K19" s="51"/>
+      <c r="I19" s="54"/>
+      <c r="J19" s="57"/>
+      <c r="K19" s="54"/>
       <c r="L19" s="2"/>
       <c r="M19" s="2"/>
       <c r="N19" s="2"/>
@@ -2643,19 +2643,19 @@
       <c r="AA19" s="2"/>
     </row>
     <row r="20" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A20" s="90" t="s">
+      <c r="A20" s="76" t="s">
         <v>33</v>
       </c>
-      <c r="B20" s="55" t="s">
+      <c r="B20" s="58" t="s">
         <v>63</v>
       </c>
       <c r="C20" s="70" t="s">
         <v>73</v>
       </c>
-      <c r="D20" s="55" t="s">
+      <c r="D20" s="58" t="s">
         <v>74</v>
       </c>
-      <c r="E20" s="55" t="s">
+      <c r="E20" s="58" t="s">
         <v>75</v>
       </c>
       <c r="F20" s="29" t="s">
@@ -2667,13 +2667,13 @@
       <c r="H20" s="34" t="s">
         <v>76</v>
       </c>
-      <c r="I20" s="49" t="s">
+      <c r="I20" s="52" t="s">
         <v>26</v>
       </c>
-      <c r="J20" s="52" t="s">
+      <c r="J20" s="55" t="s">
         <v>56</v>
       </c>
-      <c r="K20" s="49" t="s">
+      <c r="K20" s="52" t="s">
         <v>28</v>
       </c>
       <c r="L20" s="2"/>
@@ -2694,11 +2694,11 @@
       <c r="AA20" s="2"/>
     </row>
     <row r="21" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A21" s="91"/>
-      <c r="B21" s="56"/>
-      <c r="C21" s="79"/>
-      <c r="D21" s="56"/>
-      <c r="E21" s="56"/>
+      <c r="A21" s="77"/>
+      <c r="B21" s="59"/>
+      <c r="C21" s="71"/>
+      <c r="D21" s="59"/>
+      <c r="E21" s="59"/>
       <c r="F21" s="29" t="s">
         <v>67</v>
       </c>
@@ -2706,9 +2706,9 @@
         <v>77</v>
       </c>
       <c r="H21" s="34"/>
-      <c r="I21" s="50"/>
-      <c r="J21" s="53"/>
-      <c r="K21" s="50"/>
+      <c r="I21" s="53"/>
+      <c r="J21" s="56"/>
+      <c r="K21" s="53"/>
       <c r="L21" s="2"/>
       <c r="M21" s="2"/>
       <c r="N21" s="2"/>
@@ -2727,11 +2727,11 @@
       <c r="AA21" s="2"/>
     </row>
     <row r="22" spans="1:27" s="28" customFormat="1" ht="15.75" customHeight="1">
-      <c r="A22" s="91"/>
-      <c r="B22" s="56"/>
-      <c r="C22" s="79"/>
-      <c r="D22" s="56"/>
-      <c r="E22" s="56"/>
+      <c r="A22" s="77"/>
+      <c r="B22" s="59"/>
+      <c r="C22" s="71"/>
+      <c r="D22" s="59"/>
+      <c r="E22" s="59"/>
       <c r="F22" s="29" t="s">
         <v>70</v>
       </c>
@@ -2741,9 +2741,9 @@
       <c r="H22" s="34" t="s">
         <v>79</v>
       </c>
-      <c r="I22" s="50"/>
-      <c r="J22" s="53"/>
-      <c r="K22" s="50"/>
+      <c r="I22" s="53"/>
+      <c r="J22" s="56"/>
+      <c r="K22" s="53"/>
       <c r="L22" s="27"/>
       <c r="M22" s="27"/>
       <c r="N22" s="27"/>
@@ -2762,17 +2762,17 @@
       <c r="AA22" s="27"/>
     </row>
     <row r="23" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A23" s="92"/>
-      <c r="B23" s="57"/>
-      <c r="C23" s="80"/>
-      <c r="D23" s="57"/>
-      <c r="E23" s="57"/>
+      <c r="A23" s="78"/>
+      <c r="B23" s="60"/>
+      <c r="C23" s="72"/>
+      <c r="D23" s="60"/>
+      <c r="E23" s="60"/>
       <c r="F23" s="29"/>
       <c r="G23" s="34"/>
       <c r="H23" s="34"/>
-      <c r="I23" s="51"/>
-      <c r="J23" s="54"/>
-      <c r="K23" s="51"/>
+      <c r="I23" s="54"/>
+      <c r="J23" s="57"/>
+      <c r="K23" s="54"/>
       <c r="L23" s="2"/>
       <c r="M23" s="2"/>
       <c r="N23" s="2"/>
@@ -2791,19 +2791,19 @@
       <c r="AA23" s="2"/>
     </row>
     <row r="24" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A24" s="90" t="s">
+      <c r="A24" s="76" t="s">
         <v>34</v>
       </c>
-      <c r="B24" s="55" t="s">
+      <c r="B24" s="58" t="s">
         <v>63</v>
       </c>
       <c r="C24" s="70" t="s">
         <v>80</v>
       </c>
-      <c r="D24" s="55" t="s">
+      <c r="D24" s="58" t="s">
         <v>81</v>
       </c>
-      <c r="E24" s="55" t="s">
+      <c r="E24" s="58" t="s">
         <v>75</v>
       </c>
       <c r="F24" s="29" t="s">
@@ -2815,13 +2815,13 @@
       <c r="H24" s="34" t="s">
         <v>76</v>
       </c>
-      <c r="I24" s="49" t="s">
+      <c r="I24" s="52" t="s">
         <v>26</v>
       </c>
-      <c r="J24" s="52" t="s">
+      <c r="J24" s="55" t="s">
         <v>56</v>
       </c>
-      <c r="K24" s="49" t="s">
+      <c r="K24" s="52" t="s">
         <v>28</v>
       </c>
       <c r="L24" s="2"/>
@@ -2842,11 +2842,11 @@
       <c r="AA24" s="2"/>
     </row>
     <row r="25" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A25" s="91"/>
-      <c r="B25" s="56"/>
-      <c r="C25" s="79"/>
-      <c r="D25" s="56"/>
-      <c r="E25" s="56"/>
+      <c r="A25" s="77"/>
+      <c r="B25" s="59"/>
+      <c r="C25" s="71"/>
+      <c r="D25" s="59"/>
+      <c r="E25" s="59"/>
       <c r="F25" s="29" t="s">
         <v>67</v>
       </c>
@@ -2854,9 +2854,9 @@
         <v>77</v>
       </c>
       <c r="H25" s="34"/>
-      <c r="I25" s="50"/>
-      <c r="J25" s="53"/>
-      <c r="K25" s="50"/>
+      <c r="I25" s="53"/>
+      <c r="J25" s="56"/>
+      <c r="K25" s="53"/>
       <c r="L25" s="2"/>
       <c r="M25" s="2"/>
       <c r="N25" s="2"/>
@@ -2875,11 +2875,11 @@
       <c r="AA25" s="2"/>
     </row>
     <row r="26" spans="1:27" s="28" customFormat="1" ht="25">
-      <c r="A26" s="91"/>
-      <c r="B26" s="56"/>
-      <c r="C26" s="79"/>
-      <c r="D26" s="56"/>
-      <c r="E26" s="56"/>
+      <c r="A26" s="77"/>
+      <c r="B26" s="59"/>
+      <c r="C26" s="71"/>
+      <c r="D26" s="59"/>
+      <c r="E26" s="59"/>
       <c r="F26" s="29" t="s">
         <v>70</v>
       </c>
@@ -2889,9 +2889,9 @@
       <c r="H26" s="34" t="s">
         <v>82</v>
       </c>
-      <c r="I26" s="50"/>
-      <c r="J26" s="53"/>
-      <c r="K26" s="50"/>
+      <c r="I26" s="53"/>
+      <c r="J26" s="56"/>
+      <c r="K26" s="53"/>
       <c r="L26" s="27"/>
       <c r="M26" s="27"/>
       <c r="N26" s="27"/>
@@ -2910,17 +2910,17 @@
       <c r="AA26" s="27"/>
     </row>
     <row r="27" spans="1:27" ht="18.75" customHeight="1">
-      <c r="A27" s="92"/>
-      <c r="B27" s="57"/>
-      <c r="C27" s="80"/>
-      <c r="D27" s="57"/>
-      <c r="E27" s="57"/>
+      <c r="A27" s="78"/>
+      <c r="B27" s="60"/>
+      <c r="C27" s="72"/>
+      <c r="D27" s="60"/>
+      <c r="E27" s="60"/>
       <c r="F27" s="29"/>
       <c r="G27" s="34"/>
       <c r="H27" s="34"/>
-      <c r="I27" s="51"/>
-      <c r="J27" s="54"/>
-      <c r="K27" s="51"/>
+      <c r="I27" s="54"/>
+      <c r="J27" s="57"/>
+      <c r="K27" s="54"/>
       <c r="L27" s="2"/>
       <c r="M27" s="2"/>
       <c r="N27" s="2"/>
@@ -2939,19 +2939,19 @@
       <c r="AA27" s="2"/>
     </row>
     <row r="28" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A28" s="76" t="s">
+      <c r="A28" s="67" t="s">
         <v>35</v>
       </c>
-      <c r="B28" s="55" t="s">
+      <c r="B28" s="58" t="s">
         <v>84</v>
       </c>
-      <c r="C28" s="55" t="s">
+      <c r="C28" s="58" t="s">
         <v>85</v>
       </c>
-      <c r="D28" s="55" t="s">
+      <c r="D28" s="58" t="s">
         <v>86</v>
       </c>
-      <c r="E28" s="55" t="s">
+      <c r="E28" s="58" t="s">
         <v>83</v>
       </c>
       <c r="F28" s="29" t="s">
@@ -2963,13 +2963,13 @@
       <c r="H28" s="34" t="s">
         <v>88</v>
       </c>
-      <c r="I28" s="49" t="s">
+      <c r="I28" s="52" t="s">
         <v>26</v>
       </c>
-      <c r="J28" s="52" t="s">
+      <c r="J28" s="55" t="s">
         <v>56</v>
       </c>
-      <c r="K28" s="49" t="s">
+      <c r="K28" s="52" t="s">
         <v>28</v>
       </c>
       <c r="L28" s="2"/>
@@ -2990,19 +2990,19 @@
       <c r="AA28" s="2"/>
     </row>
     <row r="29" spans="1:27">
-      <c r="A29" s="77"/>
-      <c r="B29" s="56"/>
-      <c r="C29" s="56"/>
-      <c r="D29" s="56"/>
-      <c r="E29" s="56"/>
+      <c r="A29" s="68"/>
+      <c r="B29" s="59"/>
+      <c r="C29" s="59"/>
+      <c r="D29" s="59"/>
+      <c r="E29" s="59"/>
       <c r="F29" s="29" t="s">
         <v>67</v>
       </c>
       <c r="G29" s="34"/>
       <c r="H29" s="34"/>
-      <c r="I29" s="50"/>
-      <c r="J29" s="53"/>
-      <c r="K29" s="50"/>
+      <c r="I29" s="53"/>
+      <c r="J29" s="56"/>
+      <c r="K29" s="53"/>
       <c r="L29" s="2"/>
       <c r="M29" s="2"/>
       <c r="N29" s="2"/>
@@ -3021,17 +3021,17 @@
       <c r="AA29" s="2"/>
     </row>
     <row r="30" spans="1:27" s="28" customFormat="1" ht="15.75" customHeight="1">
-      <c r="A30" s="77"/>
-      <c r="B30" s="56"/>
-      <c r="C30" s="56"/>
-      <c r="D30" s="56"/>
-      <c r="E30" s="56"/>
+      <c r="A30" s="68"/>
+      <c r="B30" s="59"/>
+      <c r="C30" s="59"/>
+      <c r="D30" s="59"/>
+      <c r="E30" s="59"/>
       <c r="F30" s="29"/>
       <c r="G30" s="34"/>
       <c r="H30" s="34"/>
-      <c r="I30" s="50"/>
-      <c r="J30" s="53"/>
-      <c r="K30" s="50"/>
+      <c r="I30" s="53"/>
+      <c r="J30" s="56"/>
+      <c r="K30" s="53"/>
       <c r="L30" s="27"/>
       <c r="M30" s="27"/>
       <c r="N30" s="27"/>
@@ -3050,17 +3050,17 @@
       <c r="AA30" s="27"/>
     </row>
     <row r="31" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A31" s="78"/>
-      <c r="B31" s="57"/>
-      <c r="C31" s="57"/>
-      <c r="D31" s="57"/>
-      <c r="E31" s="57"/>
+      <c r="A31" s="69"/>
+      <c r="B31" s="60"/>
+      <c r="C31" s="60"/>
+      <c r="D31" s="60"/>
+      <c r="E31" s="60"/>
       <c r="F31" s="29"/>
       <c r="G31" s="34"/>
       <c r="H31" s="34"/>
-      <c r="I31" s="51"/>
-      <c r="J31" s="54"/>
-      <c r="K31" s="51"/>
+      <c r="I31" s="54"/>
+      <c r="J31" s="57"/>
+      <c r="K31" s="54"/>
       <c r="L31" s="2"/>
       <c r="M31" s="2"/>
       <c r="N31" s="2"/>
@@ -3079,19 +3079,19 @@
       <c r="AA31" s="2"/>
     </row>
     <row r="32" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A32" s="76" t="s">
+      <c r="A32" s="67" t="s">
         <v>36</v>
       </c>
-      <c r="B32" s="55" t="s">
+      <c r="B32" s="58" t="s">
         <v>84</v>
       </c>
-      <c r="C32" s="55" t="s">
+      <c r="C32" s="58" t="s">
         <v>89</v>
       </c>
-      <c r="D32" s="55" t="s">
+      <c r="D32" s="58" t="s">
         <v>90</v>
       </c>
-      <c r="E32" s="55" t="s">
+      <c r="E32" s="58" t="s">
         <v>83</v>
       </c>
       <c r="F32" s="29" t="s">
@@ -3103,13 +3103,13 @@
       <c r="H32" s="34" t="s">
         <v>92</v>
       </c>
-      <c r="I32" s="49" t="s">
+      <c r="I32" s="52" t="s">
         <v>26</v>
       </c>
-      <c r="J32" s="52" t="s">
+      <c r="J32" s="55" t="s">
         <v>56</v>
       </c>
-      <c r="K32" s="49" t="s">
+      <c r="K32" s="52" t="s">
         <v>28</v>
       </c>
       <c r="L32" s="2"/>
@@ -3130,17 +3130,17 @@
       <c r="AA32" s="2"/>
     </row>
     <row r="33" spans="1:27">
-      <c r="A33" s="77"/>
-      <c r="B33" s="56"/>
-      <c r="C33" s="56"/>
-      <c r="D33" s="56"/>
-      <c r="E33" s="56"/>
+      <c r="A33" s="68"/>
+      <c r="B33" s="59"/>
+      <c r="C33" s="59"/>
+      <c r="D33" s="59"/>
+      <c r="E33" s="59"/>
       <c r="F33" s="29"/>
       <c r="G33" s="42"/>
       <c r="H33" s="42"/>
-      <c r="I33" s="50"/>
-      <c r="J33" s="53"/>
-      <c r="K33" s="50"/>
+      <c r="I33" s="53"/>
+      <c r="J33" s="56"/>
+      <c r="K33" s="53"/>
       <c r="L33" s="2"/>
       <c r="M33" s="2"/>
       <c r="N33" s="2"/>
@@ -3159,17 +3159,17 @@
       <c r="AA33" s="2"/>
     </row>
     <row r="34" spans="1:27">
-      <c r="A34" s="77"/>
-      <c r="B34" s="56"/>
-      <c r="C34" s="56"/>
-      <c r="D34" s="56"/>
-      <c r="E34" s="56"/>
+      <c r="A34" s="68"/>
+      <c r="B34" s="59"/>
+      <c r="C34" s="59"/>
+      <c r="D34" s="59"/>
+      <c r="E34" s="59"/>
       <c r="F34" s="29"/>
       <c r="G34" s="42"/>
       <c r="H34" s="42"/>
-      <c r="I34" s="50"/>
-      <c r="J34" s="53"/>
-      <c r="K34" s="50"/>
+      <c r="I34" s="53"/>
+      <c r="J34" s="56"/>
+      <c r="K34" s="53"/>
       <c r="L34" s="2"/>
       <c r="M34" s="2"/>
       <c r="N34" s="2"/>
@@ -3188,17 +3188,17 @@
       <c r="AA34" s="2"/>
     </row>
     <row r="35" spans="1:27">
-      <c r="A35" s="78"/>
-      <c r="B35" s="57"/>
-      <c r="C35" s="57"/>
-      <c r="D35" s="57"/>
-      <c r="E35" s="57"/>
+      <c r="A35" s="69"/>
+      <c r="B35" s="60"/>
+      <c r="C35" s="60"/>
+      <c r="D35" s="60"/>
+      <c r="E35" s="60"/>
       <c r="F35" s="29"/>
       <c r="G35" s="34"/>
       <c r="H35" s="34"/>
-      <c r="I35" s="51"/>
-      <c r="J35" s="54"/>
-      <c r="K35" s="51"/>
+      <c r="I35" s="54"/>
+      <c r="J35" s="57"/>
+      <c r="K35" s="54"/>
       <c r="L35" s="2"/>
       <c r="M35" s="2"/>
       <c r="N35" s="2"/>
@@ -3217,19 +3217,19 @@
       <c r="AA35" s="2"/>
     </row>
     <row r="36" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A36" s="76" t="s">
+      <c r="A36" s="67" t="s">
         <v>37</v>
       </c>
-      <c r="B36" s="55" t="s">
+      <c r="B36" s="58" t="s">
         <v>84</v>
       </c>
-      <c r="C36" s="55" t="s">
+      <c r="C36" s="58" t="s">
         <v>93</v>
       </c>
-      <c r="D36" s="55" t="s">
+      <c r="D36" s="58" t="s">
         <v>94</v>
       </c>
-      <c r="E36" s="55" t="s">
+      <c r="E36" s="58" t="s">
         <v>95</v>
       </c>
       <c r="F36" s="29" t="s">
@@ -3241,13 +3241,13 @@
       <c r="H36" s="34" t="s">
         <v>92</v>
       </c>
-      <c r="I36" s="49" t="s">
+      <c r="I36" s="52" t="s">
         <v>26</v>
       </c>
-      <c r="J36" s="52" t="s">
+      <c r="J36" s="55" t="s">
         <v>56</v>
       </c>
-      <c r="K36" s="49" t="s">
+      <c r="K36" s="52" t="s">
         <v>28</v>
       </c>
       <c r="L36" s="2"/>
@@ -3268,11 +3268,11 @@
       <c r="AA36" s="2"/>
     </row>
     <row r="37" spans="1:27" ht="25">
-      <c r="A37" s="77"/>
-      <c r="B37" s="56"/>
-      <c r="C37" s="56"/>
-      <c r="D37" s="56"/>
-      <c r="E37" s="56"/>
+      <c r="A37" s="68"/>
+      <c r="B37" s="59"/>
+      <c r="C37" s="59"/>
+      <c r="D37" s="59"/>
+      <c r="E37" s="59"/>
       <c r="F37" s="29" t="s">
         <v>67</v>
       </c>
@@ -3280,9 +3280,9 @@
         <v>96</v>
       </c>
       <c r="H37" s="34"/>
-      <c r="I37" s="50"/>
-      <c r="J37" s="53"/>
-      <c r="K37" s="50"/>
+      <c r="I37" s="53"/>
+      <c r="J37" s="56"/>
+      <c r="K37" s="53"/>
       <c r="L37" s="2"/>
       <c r="M37" s="2"/>
       <c r="N37" s="2"/>
@@ -3301,11 +3301,11 @@
       <c r="AA37" s="2"/>
     </row>
     <row r="38" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A38" s="77"/>
-      <c r="B38" s="56"/>
-      <c r="C38" s="56"/>
-      <c r="D38" s="56"/>
-      <c r="E38" s="56"/>
+      <c r="A38" s="68"/>
+      <c r="B38" s="59"/>
+      <c r="C38" s="59"/>
+      <c r="D38" s="59"/>
+      <c r="E38" s="59"/>
       <c r="F38" s="29" t="s">
         <v>70</v>
       </c>
@@ -3315,9 +3315,9 @@
       <c r="H38" s="34" t="s">
         <v>98</v>
       </c>
-      <c r="I38" s="50"/>
-      <c r="J38" s="53"/>
-      <c r="K38" s="50"/>
+      <c r="I38" s="53"/>
+      <c r="J38" s="56"/>
+      <c r="K38" s="53"/>
       <c r="L38" s="2"/>
       <c r="M38" s="2"/>
       <c r="N38" s="2"/>
@@ -3336,19 +3336,19 @@
       <c r="AA38" s="2"/>
     </row>
     <row r="39" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A39" s="78"/>
-      <c r="B39" s="57"/>
-      <c r="C39" s="57"/>
-      <c r="D39" s="57"/>
-      <c r="E39" s="57"/>
+      <c r="A39" s="69"/>
+      <c r="B39" s="60"/>
+      <c r="C39" s="60"/>
+      <c r="D39" s="60"/>
+      <c r="E39" s="60"/>
       <c r="F39" s="29" t="s">
         <v>99</v>
       </c>
       <c r="G39" s="34"/>
       <c r="H39" s="34"/>
-      <c r="I39" s="51"/>
-      <c r="J39" s="54"/>
-      <c r="K39" s="51"/>
+      <c r="I39" s="54"/>
+      <c r="J39" s="57"/>
+      <c r="K39" s="54"/>
       <c r="L39" s="2"/>
       <c r="M39" s="2"/>
       <c r="N39" s="2"/>
@@ -3367,19 +3367,19 @@
       <c r="AA39" s="2"/>
     </row>
     <row r="40" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A40" s="76" t="s">
+      <c r="A40" s="67" t="s">
         <v>38</v>
       </c>
-      <c r="B40" s="55" t="s">
+      <c r="B40" s="58" t="s">
         <v>84</v>
       </c>
-      <c r="C40" s="55" t="s">
+      <c r="C40" s="58" t="s">
         <v>100</v>
       </c>
-      <c r="D40" s="55" t="s">
+      <c r="D40" s="58" t="s">
         <v>101</v>
       </c>
-      <c r="E40" s="55" t="s">
+      <c r="E40" s="58" t="s">
         <v>102</v>
       </c>
       <c r="F40" s="29" t="s">
@@ -3391,13 +3391,13 @@
       <c r="H40" s="34" t="s">
         <v>88</v>
       </c>
-      <c r="I40" s="49" t="s">
+      <c r="I40" s="52" t="s">
         <v>26</v>
       </c>
-      <c r="J40" s="52" t="s">
+      <c r="J40" s="55" t="s">
         <v>56</v>
       </c>
-      <c r="K40" s="49" t="s">
+      <c r="K40" s="52" t="s">
         <v>28</v>
       </c>
       <c r="L40" s="2"/>
@@ -3418,11 +3418,11 @@
       <c r="AA40" s="2"/>
     </row>
     <row r="41" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A41" s="77"/>
-      <c r="B41" s="56"/>
-      <c r="C41" s="56"/>
-      <c r="D41" s="56"/>
-      <c r="E41" s="56"/>
+      <c r="A41" s="68"/>
+      <c r="B41" s="59"/>
+      <c r="C41" s="59"/>
+      <c r="D41" s="59"/>
+      <c r="E41" s="59"/>
       <c r="F41" s="29" t="s">
         <v>67</v>
       </c>
@@ -3430,9 +3430,9 @@
         <v>103</v>
       </c>
       <c r="H41" s="34"/>
-      <c r="I41" s="50"/>
-      <c r="J41" s="53"/>
-      <c r="K41" s="50"/>
+      <c r="I41" s="53"/>
+      <c r="J41" s="56"/>
+      <c r="K41" s="53"/>
       <c r="L41" s="2"/>
       <c r="M41" s="2"/>
       <c r="N41" s="2"/>
@@ -3451,11 +3451,11 @@
       <c r="AA41" s="2"/>
     </row>
     <row r="42" spans="1:27" ht="16.5" customHeight="1">
-      <c r="A42" s="77"/>
-      <c r="B42" s="56"/>
-      <c r="C42" s="56"/>
-      <c r="D42" s="56"/>
-      <c r="E42" s="56"/>
+      <c r="A42" s="68"/>
+      <c r="B42" s="59"/>
+      <c r="C42" s="59"/>
+      <c r="D42" s="59"/>
+      <c r="E42" s="59"/>
       <c r="F42" s="29" t="s">
         <v>70</v>
       </c>
@@ -3465,9 +3465,9 @@
       <c r="H42" s="34" t="s">
         <v>105</v>
       </c>
-      <c r="I42" s="50"/>
-      <c r="J42" s="53"/>
-      <c r="K42" s="50"/>
+      <c r="I42" s="53"/>
+      <c r="J42" s="56"/>
+      <c r="K42" s="53"/>
       <c r="L42" s="2"/>
       <c r="M42" s="2"/>
       <c r="N42" s="2"/>
@@ -3486,19 +3486,19 @@
       <c r="AA42" s="2"/>
     </row>
     <row r="43" spans="1:27" ht="18.75" customHeight="1">
-      <c r="A43" s="78"/>
-      <c r="B43" s="57"/>
-      <c r="C43" s="57"/>
-      <c r="D43" s="57"/>
-      <c r="E43" s="57"/>
+      <c r="A43" s="69"/>
+      <c r="B43" s="60"/>
+      <c r="C43" s="60"/>
+      <c r="D43" s="60"/>
+      <c r="E43" s="60"/>
       <c r="F43" s="29" t="s">
         <v>99</v>
       </c>
       <c r="G43" s="34"/>
       <c r="H43" s="34"/>
-      <c r="I43" s="51"/>
-      <c r="J43" s="54"/>
-      <c r="K43" s="51"/>
+      <c r="I43" s="54"/>
+      <c r="J43" s="57"/>
+      <c r="K43" s="54"/>
       <c r="L43" s="2"/>
       <c r="M43" s="2"/>
       <c r="N43" s="2"/>
@@ -3517,19 +3517,19 @@
       <c r="AA43" s="2"/>
     </row>
     <row r="44" spans="1:27" ht="25">
-      <c r="A44" s="76" t="s">
+      <c r="A44" s="67" t="s">
         <v>39</v>
       </c>
-      <c r="B44" s="55" t="s">
+      <c r="B44" s="58" t="s">
         <v>84</v>
       </c>
-      <c r="C44" s="55" t="s">
+      <c r="C44" s="58" t="s">
         <v>106</v>
       </c>
-      <c r="D44" s="55" t="s">
+      <c r="D44" s="58" t="s">
         <v>107</v>
       </c>
-      <c r="E44" s="55" t="s">
+      <c r="E44" s="58" t="s">
         <v>108</v>
       </c>
       <c r="F44" s="29" t="s">
@@ -3541,13 +3541,13 @@
       <c r="H44" s="34" t="s">
         <v>88</v>
       </c>
-      <c r="I44" s="49" t="s">
+      <c r="I44" s="52" t="s">
         <v>26</v>
       </c>
-      <c r="J44" s="52" t="s">
+      <c r="J44" s="55" t="s">
         <v>56</v>
       </c>
-      <c r="K44" s="49" t="s">
+      <c r="K44" s="52" t="s">
         <v>28</v>
       </c>
       <c r="L44" s="2"/>
@@ -3568,11 +3568,11 @@
       <c r="AA44" s="2"/>
     </row>
     <row r="45" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A45" s="77"/>
-      <c r="B45" s="56"/>
-      <c r="C45" s="56"/>
-      <c r="D45" s="56"/>
-      <c r="E45" s="56"/>
+      <c r="A45" s="68"/>
+      <c r="B45" s="59"/>
+      <c r="C45" s="59"/>
+      <c r="D45" s="59"/>
+      <c r="E45" s="59"/>
       <c r="F45" s="29" t="s">
         <v>67</v>
       </c>
@@ -3580,9 +3580,9 @@
         <v>109</v>
       </c>
       <c r="H45" s="34"/>
-      <c r="I45" s="50"/>
-      <c r="J45" s="53"/>
-      <c r="K45" s="50"/>
+      <c r="I45" s="53"/>
+      <c r="J45" s="56"/>
+      <c r="K45" s="53"/>
       <c r="L45" s="2"/>
       <c r="M45" s="2"/>
       <c r="N45" s="2"/>
@@ -3601,11 +3601,11 @@
       <c r="AA45" s="2"/>
     </row>
     <row r="46" spans="1:27" ht="25">
-      <c r="A46" s="77"/>
-      <c r="B46" s="56"/>
-      <c r="C46" s="56"/>
-      <c r="D46" s="56"/>
-      <c r="E46" s="56"/>
+      <c r="A46" s="68"/>
+      <c r="B46" s="59"/>
+      <c r="C46" s="59"/>
+      <c r="D46" s="59"/>
+      <c r="E46" s="59"/>
       <c r="F46" s="29" t="s">
         <v>70</v>
       </c>
@@ -3615,9 +3615,9 @@
       <c r="H46" s="34" t="s">
         <v>110</v>
       </c>
-      <c r="I46" s="50"/>
-      <c r="J46" s="53"/>
-      <c r="K46" s="50"/>
+      <c r="I46" s="53"/>
+      <c r="J46" s="56"/>
+      <c r="K46" s="53"/>
       <c r="L46" s="2"/>
       <c r="M46" s="2"/>
       <c r="N46" s="2"/>
@@ -3636,19 +3636,19 @@
       <c r="AA46" s="2"/>
     </row>
     <row r="47" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A47" s="78"/>
-      <c r="B47" s="57"/>
-      <c r="C47" s="57"/>
-      <c r="D47" s="57"/>
-      <c r="E47" s="57"/>
+      <c r="A47" s="69"/>
+      <c r="B47" s="60"/>
+      <c r="C47" s="60"/>
+      <c r="D47" s="60"/>
+      <c r="E47" s="60"/>
       <c r="F47" s="29" t="s">
         <v>99</v>
       </c>
       <c r="G47" s="34"/>
       <c r="H47" s="35"/>
-      <c r="I47" s="51"/>
-      <c r="J47" s="54"/>
-      <c r="K47" s="51"/>
+      <c r="I47" s="54"/>
+      <c r="J47" s="57"/>
+      <c r="K47" s="54"/>
       <c r="L47" s="2"/>
       <c r="M47" s="2"/>
       <c r="N47" s="2"/>
@@ -3667,19 +3667,19 @@
       <c r="AA47" s="2"/>
     </row>
     <row r="48" spans="1:27" ht="25">
-      <c r="A48" s="76" t="s">
+      <c r="A48" s="67" t="s">
         <v>40</v>
       </c>
-      <c r="B48" s="55" t="s">
+      <c r="B48" s="58" t="s">
         <v>84</v>
       </c>
-      <c r="C48" s="55" t="s">
+      <c r="C48" s="58" t="s">
         <v>111</v>
       </c>
-      <c r="D48" s="55" t="s">
+      <c r="D48" s="58" t="s">
         <v>112</v>
       </c>
-      <c r="E48" s="55" t="s">
+      <c r="E48" s="58" t="s">
         <v>102</v>
       </c>
       <c r="F48" s="29" t="s">
@@ -3691,13 +3691,13 @@
       <c r="H48" s="34" t="s">
         <v>88</v>
       </c>
-      <c r="I48" s="49" t="s">
+      <c r="I48" s="52" t="s">
         <v>26</v>
       </c>
-      <c r="J48" s="52" t="s">
+      <c r="J48" s="55" t="s">
         <v>56</v>
       </c>
-      <c r="K48" s="49" t="s">
+      <c r="K48" s="52" t="s">
         <v>28</v>
       </c>
       <c r="L48" s="2"/>
@@ -3718,11 +3718,11 @@
       <c r="AA48" s="2"/>
     </row>
     <row r="49" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A49" s="77"/>
-      <c r="B49" s="56"/>
-      <c r="C49" s="56"/>
-      <c r="D49" s="56"/>
-      <c r="E49" s="56"/>
+      <c r="A49" s="68"/>
+      <c r="B49" s="59"/>
+      <c r="C49" s="59"/>
+      <c r="D49" s="59"/>
+      <c r="E49" s="59"/>
       <c r="F49" s="29" t="s">
         <v>67</v>
       </c>
@@ -3730,9 +3730,9 @@
         <v>113</v>
       </c>
       <c r="H49" s="34"/>
-      <c r="I49" s="50"/>
-      <c r="J49" s="53"/>
-      <c r="K49" s="50"/>
+      <c r="I49" s="53"/>
+      <c r="J49" s="56"/>
+      <c r="K49" s="53"/>
       <c r="L49" s="2"/>
       <c r="M49" s="2"/>
       <c r="N49" s="2"/>
@@ -3751,11 +3751,11 @@
       <c r="AA49" s="2"/>
     </row>
     <row r="50" spans="1:27" ht="27" customHeight="1">
-      <c r="A50" s="77"/>
-      <c r="B50" s="56"/>
-      <c r="C50" s="56"/>
-      <c r="D50" s="56"/>
-      <c r="E50" s="56"/>
+      <c r="A50" s="68"/>
+      <c r="B50" s="59"/>
+      <c r="C50" s="59"/>
+      <c r="D50" s="59"/>
+      <c r="E50" s="59"/>
       <c r="F50" s="29" t="s">
         <v>70</v>
       </c>
@@ -3765,9 +3765,9 @@
       <c r="H50" s="34" t="s">
         <v>110</v>
       </c>
-      <c r="I50" s="50"/>
-      <c r="J50" s="53"/>
-      <c r="K50" s="50"/>
+      <c r="I50" s="53"/>
+      <c r="J50" s="56"/>
+      <c r="K50" s="53"/>
       <c r="L50" s="2"/>
       <c r="M50" s="2"/>
       <c r="N50" s="2"/>
@@ -3786,19 +3786,19 @@
       <c r="AA50" s="2"/>
     </row>
     <row r="51" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A51" s="78"/>
-      <c r="B51" s="57"/>
-      <c r="C51" s="57"/>
-      <c r="D51" s="57"/>
-      <c r="E51" s="57"/>
+      <c r="A51" s="69"/>
+      <c r="B51" s="60"/>
+      <c r="C51" s="60"/>
+      <c r="D51" s="60"/>
+      <c r="E51" s="60"/>
       <c r="F51" s="29" t="s">
         <v>99</v>
       </c>
       <c r="G51" s="34"/>
       <c r="H51" s="35"/>
-      <c r="I51" s="51"/>
-      <c r="J51" s="54"/>
-      <c r="K51" s="51"/>
+      <c r="I51" s="54"/>
+      <c r="J51" s="57"/>
+      <c r="K51" s="54"/>
       <c r="L51" s="2"/>
       <c r="M51" s="2"/>
       <c r="N51" s="2"/>
@@ -3817,19 +3817,19 @@
       <c r="AA51" s="2"/>
     </row>
     <row r="52" spans="1:27">
-      <c r="A52" s="76" t="s">
+      <c r="A52" s="67" t="s">
         <v>41</v>
       </c>
-      <c r="B52" s="55" t="s">
+      <c r="B52" s="58" t="s">
         <v>84</v>
       </c>
-      <c r="C52" s="55" t="s">
+      <c r="C52" s="58" t="s">
         <v>114</v>
       </c>
-      <c r="D52" s="55" t="s">
+      <c r="D52" s="58" t="s">
         <v>129</v>
       </c>
-      <c r="E52" s="55" t="s">
+      <c r="E52" s="58" t="s">
         <v>95</v>
       </c>
       <c r="F52" s="29" t="s">
@@ -3841,13 +3841,13 @@
       <c r="H52" s="34" t="s">
         <v>92</v>
       </c>
-      <c r="I52" s="49" t="s">
+      <c r="I52" s="52" t="s">
         <v>26</v>
       </c>
-      <c r="J52" s="52" t="s">
+      <c r="J52" s="55" t="s">
         <v>56</v>
       </c>
-      <c r="K52" s="49" t="s">
+      <c r="K52" s="52" t="s">
         <v>28</v>
       </c>
       <c r="L52" s="2"/>
@@ -3868,11 +3868,11 @@
       <c r="AA52" s="2"/>
     </row>
     <row r="53" spans="1:27" ht="25">
-      <c r="A53" s="77"/>
-      <c r="B53" s="56"/>
-      <c r="C53" s="56"/>
-      <c r="D53" s="56"/>
-      <c r="E53" s="56"/>
+      <c r="A53" s="68"/>
+      <c r="B53" s="59"/>
+      <c r="C53" s="59"/>
+      <c r="D53" s="59"/>
+      <c r="E53" s="59"/>
       <c r="F53" s="29" t="s">
         <v>67</v>
       </c>
@@ -3882,9 +3882,9 @@
       <c r="H53" s="35" t="s">
         <v>116</v>
       </c>
-      <c r="I53" s="50"/>
-      <c r="J53" s="53"/>
-      <c r="K53" s="50"/>
+      <c r="I53" s="53"/>
+      <c r="J53" s="56"/>
+      <c r="K53" s="53"/>
       <c r="L53" s="2"/>
       <c r="M53" s="2"/>
       <c r="N53" s="2"/>
@@ -3903,17 +3903,17 @@
       <c r="AA53" s="2"/>
     </row>
     <row r="54" spans="1:27" ht="13.5" customHeight="1">
-      <c r="A54" s="77"/>
-      <c r="B54" s="56"/>
-      <c r="C54" s="56"/>
-      <c r="D54" s="56"/>
-      <c r="E54" s="56"/>
+      <c r="A54" s="68"/>
+      <c r="B54" s="59"/>
+      <c r="C54" s="59"/>
+      <c r="D54" s="59"/>
+      <c r="E54" s="59"/>
       <c r="F54" s="29"/>
       <c r="G54" s="42"/>
       <c r="H54" s="42"/>
-      <c r="I54" s="50"/>
-      <c r="J54" s="53"/>
-      <c r="K54" s="50"/>
+      <c r="I54" s="53"/>
+      <c r="J54" s="56"/>
+      <c r="K54" s="53"/>
       <c r="L54" s="2"/>
       <c r="M54" s="2"/>
       <c r="N54" s="2"/>
@@ -3932,17 +3932,17 @@
       <c r="AA54" s="2"/>
     </row>
     <row r="55" spans="1:27" ht="15" customHeight="1">
-      <c r="A55" s="78"/>
-      <c r="B55" s="57"/>
-      <c r="C55" s="57"/>
-      <c r="D55" s="57"/>
-      <c r="E55" s="57"/>
+      <c r="A55" s="69"/>
+      <c r="B55" s="60"/>
+      <c r="C55" s="60"/>
+      <c r="D55" s="60"/>
+      <c r="E55" s="60"/>
       <c r="F55" s="29"/>
       <c r="G55" s="42"/>
       <c r="H55" s="42"/>
-      <c r="I55" s="51"/>
-      <c r="J55" s="54"/>
-      <c r="K55" s="51"/>
+      <c r="I55" s="54"/>
+      <c r="J55" s="57"/>
+      <c r="K55" s="54"/>
       <c r="L55" s="2"/>
       <c r="M55" s="2"/>
       <c r="N55" s="2"/>
@@ -3961,19 +3961,19 @@
       <c r="AA55" s="2"/>
     </row>
     <row r="56" spans="1:27">
-      <c r="A56" s="76" t="s">
+      <c r="A56" s="67" t="s">
         <v>42</v>
       </c>
-      <c r="B56" s="55" t="s">
+      <c r="B56" s="58" t="s">
         <v>84</v>
       </c>
-      <c r="C56" s="55" t="s">
+      <c r="C56" s="58" t="s">
         <v>117</v>
       </c>
-      <c r="D56" s="55" t="s">
+      <c r="D56" s="58" t="s">
         <v>118</v>
       </c>
-      <c r="E56" s="55" t="s">
+      <c r="E56" s="58" t="s">
         <v>95</v>
       </c>
       <c r="F56" s="29" t="s">
@@ -3985,13 +3985,13 @@
       <c r="H56" s="34" t="s">
         <v>92</v>
       </c>
-      <c r="I56" s="49" t="s">
+      <c r="I56" s="52" t="s">
         <v>26</v>
       </c>
-      <c r="J56" s="52" t="s">
+      <c r="J56" s="55" t="s">
         <v>56</v>
       </c>
-      <c r="K56" s="49" t="s">
+      <c r="K56" s="52" t="s">
         <v>28</v>
       </c>
       <c r="L56" s="2"/>
@@ -4012,11 +4012,11 @@
       <c r="AA56" s="2"/>
     </row>
     <row r="57" spans="1:27" ht="17.25" customHeight="1">
-      <c r="A57" s="77"/>
-      <c r="B57" s="56"/>
-      <c r="C57" s="56"/>
-      <c r="D57" s="56"/>
-      <c r="E57" s="56"/>
+      <c r="A57" s="68"/>
+      <c r="B57" s="59"/>
+      <c r="C57" s="59"/>
+      <c r="D57" s="59"/>
+      <c r="E57" s="59"/>
       <c r="F57" s="29" t="s">
         <v>67</v>
       </c>
@@ -4026,9 +4026,9 @@
       <c r="H57" s="35" t="s">
         <v>120</v>
       </c>
-      <c r="I57" s="50"/>
-      <c r="J57" s="53"/>
-      <c r="K57" s="50"/>
+      <c r="I57" s="53"/>
+      <c r="J57" s="56"/>
+      <c r="K57" s="53"/>
       <c r="L57" s="2"/>
       <c r="M57" s="2"/>
       <c r="N57" s="2"/>
@@ -4047,11 +4047,11 @@
       <c r="AA57" s="2"/>
     </row>
     <row r="58" spans="1:27" ht="25">
-      <c r="A58" s="77"/>
-      <c r="B58" s="56"/>
-      <c r="C58" s="56"/>
-      <c r="D58" s="56"/>
-      <c r="E58" s="56"/>
+      <c r="A58" s="68"/>
+      <c r="B58" s="59"/>
+      <c r="C58" s="59"/>
+      <c r="D58" s="59"/>
+      <c r="E58" s="59"/>
       <c r="F58" s="29" t="s">
         <v>70</v>
       </c>
@@ -4061,9 +4061,9 @@
       <c r="H58" s="35" t="s">
         <v>122</v>
       </c>
-      <c r="I58" s="50"/>
-      <c r="J58" s="53"/>
-      <c r="K58" s="50"/>
+      <c r="I58" s="53"/>
+      <c r="J58" s="56"/>
+      <c r="K58" s="53"/>
       <c r="L58" s="2"/>
       <c r="M58" s="2"/>
       <c r="N58" s="2"/>
@@ -4082,11 +4082,11 @@
       <c r="AA58" s="2"/>
     </row>
     <row r="59" spans="1:27" ht="25">
-      <c r="A59" s="78"/>
-      <c r="B59" s="57"/>
-      <c r="C59" s="57"/>
-      <c r="D59" s="57"/>
-      <c r="E59" s="57"/>
+      <c r="A59" s="69"/>
+      <c r="B59" s="60"/>
+      <c r="C59" s="60"/>
+      <c r="D59" s="60"/>
+      <c r="E59" s="60"/>
       <c r="F59" s="29" t="s">
         <v>99</v>
       </c>
@@ -4096,9 +4096,9 @@
       <c r="H59" s="35" t="s">
         <v>123</v>
       </c>
-      <c r="I59" s="51"/>
-      <c r="J59" s="54"/>
-      <c r="K59" s="51"/>
+      <c r="I59" s="54"/>
+      <c r="J59" s="57"/>
+      <c r="K59" s="54"/>
       <c r="L59" s="2"/>
       <c r="M59" s="2"/>
       <c r="N59" s="2"/>
@@ -4117,19 +4117,19 @@
       <c r="AA59" s="2"/>
     </row>
     <row r="60" spans="1:27">
-      <c r="A60" s="76" t="s">
+      <c r="A60" s="67" t="s">
         <v>43</v>
       </c>
-      <c r="B60" s="55" t="s">
+      <c r="B60" s="58" t="s">
         <v>84</v>
       </c>
-      <c r="C60" s="55" t="s">
+      <c r="C60" s="58" t="s">
         <v>124</v>
       </c>
-      <c r="D60" s="55" t="s">
+      <c r="D60" s="58" t="s">
         <v>125</v>
       </c>
-      <c r="E60" s="55" t="s">
+      <c r="E60" s="58" t="s">
         <v>102</v>
       </c>
       <c r="F60" s="29" t="s">
@@ -4141,13 +4141,13 @@
       <c r="H60" s="34" t="s">
         <v>92</v>
       </c>
-      <c r="I60" s="49" t="s">
+      <c r="I60" s="52" t="s">
         <v>26</v>
       </c>
-      <c r="J60" s="52" t="s">
+      <c r="J60" s="55" t="s">
         <v>56</v>
       </c>
-      <c r="K60" s="49" t="s">
+      <c r="K60" s="52" t="s">
         <v>28</v>
       </c>
       <c r="L60" s="2"/>
@@ -4168,11 +4168,11 @@
       <c r="AA60" s="2"/>
     </row>
     <row r="61" spans="1:27" ht="25">
-      <c r="A61" s="77"/>
-      <c r="B61" s="56"/>
-      <c r="C61" s="56"/>
-      <c r="D61" s="56"/>
-      <c r="E61" s="56"/>
+      <c r="A61" s="68"/>
+      <c r="B61" s="59"/>
+      <c r="C61" s="59"/>
+      <c r="D61" s="59"/>
+      <c r="E61" s="59"/>
       <c r="F61" s="29" t="s">
         <v>67</v>
       </c>
@@ -4182,9 +4182,9 @@
       <c r="H61" s="35" t="s">
         <v>120</v>
       </c>
-      <c r="I61" s="50"/>
-      <c r="J61" s="53"/>
-      <c r="K61" s="50"/>
+      <c r="I61" s="53"/>
+      <c r="J61" s="56"/>
+      <c r="K61" s="53"/>
       <c r="L61" s="2"/>
       <c r="M61" s="2"/>
       <c r="N61" s="2"/>
@@ -4203,11 +4203,11 @@
       <c r="AA61" s="2"/>
     </row>
     <row r="62" spans="1:27" ht="25">
-      <c r="A62" s="77"/>
-      <c r="B62" s="56"/>
-      <c r="C62" s="56"/>
-      <c r="D62" s="56"/>
-      <c r="E62" s="56"/>
+      <c r="A62" s="68"/>
+      <c r="B62" s="59"/>
+      <c r="C62" s="59"/>
+      <c r="D62" s="59"/>
+      <c r="E62" s="59"/>
       <c r="F62" s="29" t="s">
         <v>70</v>
       </c>
@@ -4217,9 +4217,9 @@
       <c r="H62" s="35" t="s">
         <v>122</v>
       </c>
-      <c r="I62" s="50"/>
-      <c r="J62" s="53"/>
-      <c r="K62" s="50"/>
+      <c r="I62" s="53"/>
+      <c r="J62" s="56"/>
+      <c r="K62" s="53"/>
       <c r="L62" s="2"/>
       <c r="M62" s="2"/>
       <c r="N62" s="2"/>
@@ -4238,11 +4238,11 @@
       <c r="AA62" s="2"/>
     </row>
     <row r="63" spans="1:27" ht="25">
-      <c r="A63" s="78"/>
-      <c r="B63" s="57"/>
-      <c r="C63" s="57"/>
-      <c r="D63" s="57"/>
-      <c r="E63" s="57"/>
+      <c r="A63" s="69"/>
+      <c r="B63" s="60"/>
+      <c r="C63" s="60"/>
+      <c r="D63" s="60"/>
+      <c r="E63" s="60"/>
       <c r="F63" s="29" t="s">
         <v>99</v>
       </c>
@@ -4252,9 +4252,9 @@
       <c r="H63" s="34" t="s">
         <v>128</v>
       </c>
-      <c r="I63" s="51"/>
-      <c r="J63" s="54"/>
-      <c r="K63" s="51"/>
+      <c r="I63" s="54"/>
+      <c r="J63" s="57"/>
+      <c r="K63" s="54"/>
       <c r="L63" s="2"/>
       <c r="M63" s="2"/>
       <c r="N63" s="2"/>
@@ -4273,19 +4273,19 @@
       <c r="AA63" s="2"/>
     </row>
     <row r="64" spans="1:27" ht="25">
-      <c r="A64" s="67" t="s">
+      <c r="A64" s="73" t="s">
         <v>44</v>
       </c>
-      <c r="B64" s="55" t="s">
+      <c r="B64" s="58" t="s">
         <v>49</v>
       </c>
       <c r="C64" s="70" t="s">
         <v>130</v>
       </c>
-      <c r="D64" s="55" t="s">
+      <c r="D64" s="58" t="s">
         <v>131</v>
       </c>
-      <c r="E64" s="55" t="s">
+      <c r="E64" s="58" t="s">
         <v>83</v>
       </c>
       <c r="F64" s="29" t="s">
@@ -4297,13 +4297,13 @@
       <c r="H64" s="34" t="s">
         <v>133</v>
       </c>
-      <c r="I64" s="49" t="s">
+      <c r="I64" s="52" t="s">
         <v>26</v>
       </c>
-      <c r="J64" s="52" t="s">
+      <c r="J64" s="55" t="s">
         <v>56</v>
       </c>
-      <c r="K64" s="49" t="s">
+      <c r="K64" s="52" t="s">
         <v>28</v>
       </c>
       <c r="L64" s="2"/>
@@ -4324,17 +4324,17 @@
       <c r="AA64" s="2"/>
     </row>
     <row r="65" spans="1:27">
-      <c r="A65" s="68"/>
-      <c r="B65" s="56"/>
-      <c r="C65" s="79"/>
-      <c r="D65" s="56"/>
-      <c r="E65" s="56"/>
+      <c r="A65" s="74"/>
+      <c r="B65" s="59"/>
+      <c r="C65" s="71"/>
+      <c r="D65" s="59"/>
+      <c r="E65" s="59"/>
       <c r="F65" s="29"/>
       <c r="G65" s="34"/>
       <c r="H65" s="34"/>
-      <c r="I65" s="50"/>
-      <c r="J65" s="53"/>
-      <c r="K65" s="50"/>
+      <c r="I65" s="53"/>
+      <c r="J65" s="56"/>
+      <c r="K65" s="53"/>
       <c r="L65" s="2"/>
       <c r="M65" s="2"/>
       <c r="N65" s="2"/>
@@ -4353,17 +4353,17 @@
       <c r="AA65" s="2"/>
     </row>
     <row r="66" spans="1:27">
-      <c r="A66" s="68"/>
-      <c r="B66" s="56"/>
-      <c r="C66" s="79"/>
-      <c r="D66" s="56"/>
-      <c r="E66" s="56"/>
+      <c r="A66" s="74"/>
+      <c r="B66" s="59"/>
+      <c r="C66" s="71"/>
+      <c r="D66" s="59"/>
+      <c r="E66" s="59"/>
       <c r="F66" s="29"/>
       <c r="G66" s="34"/>
       <c r="H66" s="34"/>
-      <c r="I66" s="50"/>
-      <c r="J66" s="53"/>
-      <c r="K66" s="50"/>
+      <c r="I66" s="53"/>
+      <c r="J66" s="56"/>
+      <c r="K66" s="53"/>
       <c r="L66" s="2"/>
       <c r="M66" s="2"/>
       <c r="N66" s="2"/>
@@ -4382,17 +4382,17 @@
       <c r="AA66" s="2"/>
     </row>
     <row r="67" spans="1:27">
-      <c r="A67" s="69"/>
-      <c r="B67" s="57"/>
-      <c r="C67" s="80"/>
-      <c r="D67" s="57"/>
-      <c r="E67" s="57"/>
+      <c r="A67" s="75"/>
+      <c r="B67" s="60"/>
+      <c r="C67" s="72"/>
+      <c r="D67" s="60"/>
+      <c r="E67" s="60"/>
       <c r="F67" s="29"/>
       <c r="G67" s="34"/>
       <c r="H67" s="34"/>
-      <c r="I67" s="51"/>
-      <c r="J67" s="54"/>
-      <c r="K67" s="51"/>
+      <c r="I67" s="54"/>
+      <c r="J67" s="57"/>
+      <c r="K67" s="54"/>
       <c r="L67" s="2"/>
       <c r="M67" s="2"/>
       <c r="N67" s="2"/>
@@ -4411,19 +4411,19 @@
       <c r="AA67" s="2"/>
     </row>
     <row r="68" spans="1:27" ht="25">
-      <c r="A68" s="67" t="s">
+      <c r="A68" s="73" t="s">
         <v>45</v>
       </c>
-      <c r="B68" s="55" t="s">
+      <c r="B68" s="58" t="s">
         <v>49</v>
       </c>
       <c r="C68" s="70" t="s">
         <v>134</v>
       </c>
-      <c r="D68" s="55" t="s">
+      <c r="D68" s="58" t="s">
         <v>135</v>
       </c>
-      <c r="E68" s="55" t="s">
+      <c r="E68" s="58" t="s">
         <v>83</v>
       </c>
       <c r="F68" s="29" t="s">
@@ -4435,13 +4435,13 @@
       <c r="H68" s="34" t="s">
         <v>137</v>
       </c>
-      <c r="I68" s="49" t="s">
+      <c r="I68" s="52" t="s">
         <v>26</v>
       </c>
-      <c r="J68" s="52" t="s">
+      <c r="J68" s="55" t="s">
         <v>56</v>
       </c>
-      <c r="K68" s="49" t="s">
+      <c r="K68" s="52" t="s">
         <v>28</v>
       </c>
       <c r="L68" s="2"/>
@@ -4462,17 +4462,17 @@
       <c r="AA68" s="2"/>
     </row>
     <row r="69" spans="1:27">
-      <c r="A69" s="68"/>
-      <c r="B69" s="56"/>
-      <c r="C69" s="79"/>
-      <c r="D69" s="56"/>
-      <c r="E69" s="56"/>
+      <c r="A69" s="74"/>
+      <c r="B69" s="59"/>
+      <c r="C69" s="71"/>
+      <c r="D69" s="59"/>
+      <c r="E69" s="59"/>
       <c r="F69" s="29"/>
       <c r="G69" s="34"/>
       <c r="H69" s="34"/>
-      <c r="I69" s="50"/>
-      <c r="J69" s="53"/>
-      <c r="K69" s="50"/>
+      <c r="I69" s="53"/>
+      <c r="J69" s="56"/>
+      <c r="K69" s="53"/>
       <c r="L69" s="2"/>
       <c r="M69" s="2"/>
       <c r="N69" s="2"/>
@@ -4491,17 +4491,17 @@
       <c r="AA69" s="2"/>
     </row>
     <row r="70" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A70" s="68"/>
-      <c r="B70" s="56"/>
-      <c r="C70" s="79"/>
-      <c r="D70" s="56"/>
-      <c r="E70" s="56"/>
+      <c r="A70" s="74"/>
+      <c r="B70" s="59"/>
+      <c r="C70" s="71"/>
+      <c r="D70" s="59"/>
+      <c r="E70" s="59"/>
       <c r="F70" s="29"/>
       <c r="G70" s="34"/>
       <c r="H70" s="34"/>
-      <c r="I70" s="50"/>
-      <c r="J70" s="53"/>
-      <c r="K70" s="50"/>
+      <c r="I70" s="53"/>
+      <c r="J70" s="56"/>
+      <c r="K70" s="53"/>
       <c r="L70" s="2"/>
       <c r="M70" s="2"/>
       <c r="N70" s="2"/>
@@ -4520,17 +4520,17 @@
       <c r="AA70" s="2"/>
     </row>
     <row r="71" spans="1:27">
-      <c r="A71" s="69"/>
-      <c r="B71" s="57"/>
-      <c r="C71" s="80"/>
-      <c r="D71" s="57"/>
-      <c r="E71" s="57"/>
+      <c r="A71" s="75"/>
+      <c r="B71" s="60"/>
+      <c r="C71" s="72"/>
+      <c r="D71" s="60"/>
+      <c r="E71" s="60"/>
       <c r="F71" s="29"/>
       <c r="G71" s="34"/>
       <c r="H71" s="34"/>
-      <c r="I71" s="51"/>
-      <c r="J71" s="54"/>
-      <c r="K71" s="51"/>
+      <c r="I71" s="54"/>
+      <c r="J71" s="57"/>
+      <c r="K71" s="54"/>
       <c r="L71" s="2"/>
       <c r="M71" s="2"/>
       <c r="N71" s="2"/>
@@ -4549,7 +4549,7 @@
       <c r="AA71" s="2"/>
     </row>
     <row r="72" spans="1:27">
-      <c r="A72" s="73" t="s">
+      <c r="A72" s="88" t="s">
         <v>46</v>
       </c>
       <c r="B72" s="70" t="s">
@@ -4573,13 +4573,13 @@
       <c r="H72" s="44" t="s">
         <v>143</v>
       </c>
-      <c r="I72" s="49" t="s">
-        <v>26</v>
-      </c>
-      <c r="J72" s="52" t="s">
+      <c r="I72" s="52" t="s">
+        <v>226</v>
+      </c>
+      <c r="J72" s="55" t="s">
         <v>56</v>
       </c>
-      <c r="K72" s="49" t="s">
+      <c r="K72" s="52" t="s">
         <v>28</v>
       </c>
       <c r="L72" s="2"/>
@@ -4600,11 +4600,11 @@
       <c r="AA72" s="2"/>
     </row>
     <row r="73" spans="1:27">
-      <c r="A73" s="74"/>
-      <c r="B73" s="71"/>
-      <c r="C73" s="71"/>
-      <c r="D73" s="71"/>
-      <c r="E73" s="71"/>
+      <c r="A73" s="89"/>
+      <c r="B73" s="91"/>
+      <c r="C73" s="91"/>
+      <c r="D73" s="91"/>
+      <c r="E73" s="91"/>
       <c r="F73" s="43" t="s">
         <v>67</v>
       </c>
@@ -4612,9 +4612,9 @@
         <v>144</v>
       </c>
       <c r="H73" s="44"/>
-      <c r="I73" s="50"/>
-      <c r="J73" s="53"/>
-      <c r="K73" s="50"/>
+      <c r="I73" s="53"/>
+      <c r="J73" s="56"/>
+      <c r="K73" s="53"/>
       <c r="L73" s="2"/>
       <c r="M73" s="2"/>
       <c r="N73" s="2"/>
@@ -4633,11 +4633,11 @@
       <c r="AA73" s="2"/>
     </row>
     <row r="74" spans="1:27">
-      <c r="A74" s="74"/>
-      <c r="B74" s="71"/>
-      <c r="C74" s="71"/>
-      <c r="D74" s="71"/>
-      <c r="E74" s="71"/>
+      <c r="A74" s="89"/>
+      <c r="B74" s="91"/>
+      <c r="C74" s="91"/>
+      <c r="D74" s="91"/>
+      <c r="E74" s="91"/>
       <c r="F74" s="43" t="s">
         <v>70</v>
       </c>
@@ -4647,9 +4647,9 @@
       <c r="H74" s="44" t="s">
         <v>146</v>
       </c>
-      <c r="I74" s="50"/>
-      <c r="J74" s="53"/>
-      <c r="K74" s="50"/>
+      <c r="I74" s="53"/>
+      <c r="J74" s="56"/>
+      <c r="K74" s="53"/>
       <c r="L74" s="2"/>
       <c r="M74" s="2"/>
       <c r="N74" s="2"/>
@@ -4668,11 +4668,11 @@
       <c r="AA74" s="2"/>
     </row>
     <row r="75" spans="1:27">
-      <c r="A75" s="75"/>
-      <c r="B75" s="72"/>
-      <c r="C75" s="72"/>
-      <c r="D75" s="72"/>
-      <c r="E75" s="72"/>
+      <c r="A75" s="90"/>
+      <c r="B75" s="92"/>
+      <c r="C75" s="92"/>
+      <c r="D75" s="92"/>
+      <c r="E75" s="92"/>
       <c r="F75" s="43" t="s">
         <v>99</v>
       </c>
@@ -4682,9 +4682,9 @@
       <c r="H75" s="44" t="s">
         <v>163</v>
       </c>
-      <c r="I75" s="51"/>
-      <c r="J75" s="54"/>
-      <c r="K75" s="51"/>
+      <c r="I75" s="54"/>
+      <c r="J75" s="57"/>
+      <c r="K75" s="54"/>
       <c r="L75" s="2"/>
       <c r="M75" s="2"/>
       <c r="N75" s="2"/>
@@ -4703,7 +4703,7 @@
       <c r="AA75" s="2"/>
     </row>
     <row r="76" spans="1:27">
-      <c r="A76" s="73" t="s">
+      <c r="A76" s="88" t="s">
         <v>47</v>
       </c>
       <c r="B76" s="70" t="s">
@@ -4727,13 +4727,13 @@
       <c r="H76" s="44" t="s">
         <v>143</v>
       </c>
-      <c r="I76" s="49" t="s">
-        <v>26</v>
-      </c>
-      <c r="J76" s="52" t="s">
+      <c r="I76" s="52" t="s">
+        <v>226</v>
+      </c>
+      <c r="J76" s="55" t="s">
         <v>56</v>
       </c>
-      <c r="K76" s="49" t="s">
+      <c r="K76" s="52" t="s">
         <v>28</v>
       </c>
       <c r="L76" s="2"/>
@@ -4754,11 +4754,11 @@
       <c r="AA76" s="2"/>
     </row>
     <row r="77" spans="1:27">
-      <c r="A77" s="74"/>
-      <c r="B77" s="71"/>
-      <c r="C77" s="71"/>
-      <c r="D77" s="71"/>
-      <c r="E77" s="71"/>
+      <c r="A77" s="89"/>
+      <c r="B77" s="91"/>
+      <c r="C77" s="91"/>
+      <c r="D77" s="91"/>
+      <c r="E77" s="91"/>
       <c r="F77" s="43" t="s">
         <v>67</v>
       </c>
@@ -4768,9 +4768,9 @@
       <c r="H77" s="44" t="s">
         <v>146</v>
       </c>
-      <c r="I77" s="50"/>
-      <c r="J77" s="53"/>
-      <c r="K77" s="50"/>
+      <c r="I77" s="53"/>
+      <c r="J77" s="56"/>
+      <c r="K77" s="53"/>
       <c r="L77" s="2"/>
       <c r="M77" s="2"/>
       <c r="N77" s="2"/>
@@ -4789,11 +4789,11 @@
       <c r="AA77" s="2"/>
     </row>
     <row r="78" spans="1:27">
-      <c r="A78" s="74"/>
-      <c r="B78" s="71"/>
-      <c r="C78" s="71"/>
-      <c r="D78" s="71"/>
-      <c r="E78" s="71"/>
+      <c r="A78" s="89"/>
+      <c r="B78" s="91"/>
+      <c r="C78" s="91"/>
+      <c r="D78" s="91"/>
+      <c r="E78" s="91"/>
       <c r="F78" s="43" t="s">
         <v>70</v>
       </c>
@@ -4803,9 +4803,9 @@
       <c r="H78" s="44" t="s">
         <v>151</v>
       </c>
-      <c r="I78" s="50"/>
-      <c r="J78" s="53"/>
-      <c r="K78" s="50"/>
+      <c r="I78" s="53"/>
+      <c r="J78" s="56"/>
+      <c r="K78" s="53"/>
       <c r="L78" s="2"/>
       <c r="M78" s="2"/>
       <c r="N78" s="2"/>
@@ -4824,19 +4824,19 @@
       <c r="AA78" s="2"/>
     </row>
     <row r="79" spans="1:27">
-      <c r="A79" s="75"/>
-      <c r="B79" s="72"/>
-      <c r="C79" s="72"/>
-      <c r="D79" s="72"/>
-      <c r="E79" s="72"/>
+      <c r="A79" s="90"/>
+      <c r="B79" s="92"/>
+      <c r="C79" s="92"/>
+      <c r="D79" s="92"/>
+      <c r="E79" s="92"/>
       <c r="F79" s="43" t="s">
         <v>99</v>
       </c>
       <c r="G79" s="44"/>
       <c r="H79" s="44"/>
-      <c r="I79" s="51"/>
-      <c r="J79" s="54"/>
-      <c r="K79" s="51"/>
+      <c r="I79" s="54"/>
+      <c r="J79" s="57"/>
+      <c r="K79" s="54"/>
       <c r="L79" s="2"/>
       <c r="M79" s="2"/>
       <c r="N79" s="2"/>
@@ -4855,7 +4855,7 @@
       <c r="AA79" s="2"/>
     </row>
     <row r="80" spans="1:27">
-      <c r="A80" s="73" t="s">
+      <c r="A80" s="88" t="s">
         <v>48</v>
       </c>
       <c r="B80" s="70" t="s">
@@ -4879,13 +4879,13 @@
       <c r="H80" s="44" t="s">
         <v>143</v>
       </c>
-      <c r="I80" s="49" t="s">
-        <v>26</v>
-      </c>
-      <c r="J80" s="52" t="s">
+      <c r="I80" s="52" t="s">
+        <v>226</v>
+      </c>
+      <c r="J80" s="55" t="s">
         <v>56</v>
       </c>
-      <c r="K80" s="49" t="s">
+      <c r="K80" s="52" t="s">
         <v>28</v>
       </c>
       <c r="L80" s="2"/>
@@ -4906,11 +4906,11 @@
       <c r="AA80" s="2"/>
     </row>
     <row r="81" spans="1:27">
-      <c r="A81" s="74"/>
-      <c r="B81" s="71"/>
-      <c r="C81" s="71"/>
-      <c r="D81" s="71"/>
-      <c r="E81" s="71"/>
+      <c r="A81" s="89"/>
+      <c r="B81" s="91"/>
+      <c r="C81" s="91"/>
+      <c r="D81" s="91"/>
+      <c r="E81" s="91"/>
       <c r="F81" s="43" t="s">
         <v>67</v>
       </c>
@@ -4918,9 +4918,9 @@
         <v>154</v>
       </c>
       <c r="H81" s="44"/>
-      <c r="I81" s="50"/>
-      <c r="J81" s="53"/>
-      <c r="K81" s="50"/>
+      <c r="I81" s="53"/>
+      <c r="J81" s="56"/>
+      <c r="K81" s="53"/>
       <c r="L81" s="2"/>
       <c r="M81" s="2"/>
       <c r="N81" s="2"/>
@@ -4939,11 +4939,11 @@
       <c r="AA81" s="2"/>
     </row>
     <row r="82" spans="1:27">
-      <c r="A82" s="74"/>
-      <c r="B82" s="71"/>
-      <c r="C82" s="71"/>
-      <c r="D82" s="71"/>
-      <c r="E82" s="71"/>
+      <c r="A82" s="89"/>
+      <c r="B82" s="91"/>
+      <c r="C82" s="91"/>
+      <c r="D82" s="91"/>
+      <c r="E82" s="91"/>
       <c r="F82" s="43" t="s">
         <v>70</v>
       </c>
@@ -4953,9 +4953,9 @@
       <c r="H82" s="44" t="s">
         <v>146</v>
       </c>
-      <c r="I82" s="50"/>
-      <c r="J82" s="53"/>
-      <c r="K82" s="50"/>
+      <c r="I82" s="53"/>
+      <c r="J82" s="56"/>
+      <c r="K82" s="53"/>
       <c r="L82" s="2"/>
       <c r="M82" s="2"/>
       <c r="N82" s="2"/>
@@ -4974,11 +4974,11 @@
       <c r="AA82" s="2"/>
     </row>
     <row r="83" spans="1:27">
-      <c r="A83" s="75"/>
-      <c r="B83" s="72"/>
-      <c r="C83" s="72"/>
-      <c r="D83" s="72"/>
-      <c r="E83" s="72"/>
+      <c r="A83" s="90"/>
+      <c r="B83" s="92"/>
+      <c r="C83" s="92"/>
+      <c r="D83" s="92"/>
+      <c r="E83" s="92"/>
       <c r="F83" s="43" t="s">
         <v>99</v>
       </c>
@@ -4988,9 +4988,9 @@
       <c r="H83" s="44" t="s">
         <v>156</v>
       </c>
-      <c r="I83" s="51"/>
-      <c r="J83" s="54"/>
-      <c r="K83" s="51"/>
+      <c r="I83" s="54"/>
+      <c r="J83" s="57"/>
+      <c r="K83" s="54"/>
       <c r="L83" s="2"/>
       <c r="M83" s="2"/>
       <c r="N83" s="2"/>
@@ -5009,7 +5009,7 @@
       <c r="AA83" s="2"/>
     </row>
     <row r="84" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A84" s="73" t="s">
+      <c r="A84" s="88" t="s">
         <v>162</v>
       </c>
       <c r="B84" s="70" t="s">
@@ -5033,13 +5033,13 @@
       <c r="H84" s="44" t="s">
         <v>143</v>
       </c>
-      <c r="I84" s="49" t="s">
-        <v>26</v>
-      </c>
-      <c r="J84" s="52" t="s">
+      <c r="I84" s="52" t="s">
+        <v>226</v>
+      </c>
+      <c r="J84" s="55" t="s">
         <v>56</v>
       </c>
-      <c r="K84" s="49" t="s">
+      <c r="K84" s="52" t="s">
         <v>28</v>
       </c>
       <c r="L84" s="2"/>
@@ -5060,11 +5060,11 @@
       <c r="AA84" s="2"/>
     </row>
     <row r="85" spans="1:27" ht="24" customHeight="1">
-      <c r="A85" s="74"/>
-      <c r="B85" s="71"/>
-      <c r="C85" s="71"/>
-      <c r="D85" s="71"/>
-      <c r="E85" s="71"/>
+      <c r="A85" s="89"/>
+      <c r="B85" s="91"/>
+      <c r="C85" s="91"/>
+      <c r="D85" s="91"/>
+      <c r="E85" s="91"/>
       <c r="F85" s="43" t="s">
         <v>67</v>
       </c>
@@ -5074,9 +5074,9 @@
       <c r="H85" s="44" t="s">
         <v>160</v>
       </c>
-      <c r="I85" s="50"/>
-      <c r="J85" s="53"/>
-      <c r="K85" s="50"/>
+      <c r="I85" s="53"/>
+      <c r="J85" s="56"/>
+      <c r="K85" s="53"/>
       <c r="L85" s="2"/>
       <c r="M85" s="2"/>
       <c r="N85" s="2"/>
@@ -5095,11 +5095,11 @@
       <c r="AA85" s="2"/>
     </row>
     <row r="86" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A86" s="74"/>
-      <c r="B86" s="71"/>
-      <c r="C86" s="71"/>
-      <c r="D86" s="71"/>
-      <c r="E86" s="71"/>
+      <c r="A86" s="89"/>
+      <c r="B86" s="91"/>
+      <c r="C86" s="91"/>
+      <c r="D86" s="91"/>
+      <c r="E86" s="91"/>
       <c r="F86" s="43" t="s">
         <v>70</v>
       </c>
@@ -5109,9 +5109,9 @@
       <c r="H86" s="44" t="s">
         <v>161</v>
       </c>
-      <c r="I86" s="50"/>
-      <c r="J86" s="53"/>
-      <c r="K86" s="50"/>
+      <c r="I86" s="53"/>
+      <c r="J86" s="56"/>
+      <c r="K86" s="53"/>
       <c r="L86" s="2"/>
       <c r="M86" s="2"/>
       <c r="N86" s="2"/>
@@ -5130,17 +5130,17 @@
       <c r="AA86" s="2"/>
     </row>
     <row r="87" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A87" s="75"/>
-      <c r="B87" s="72"/>
-      <c r="C87" s="72"/>
-      <c r="D87" s="72"/>
-      <c r="E87" s="72"/>
+      <c r="A87" s="90"/>
+      <c r="B87" s="92"/>
+      <c r="C87" s="92"/>
+      <c r="D87" s="92"/>
+      <c r="E87" s="92"/>
       <c r="F87" s="43"/>
       <c r="G87" s="44"/>
       <c r="H87" s="44"/>
-      <c r="I87" s="51"/>
-      <c r="J87" s="54"/>
-      <c r="K87" s="51"/>
+      <c r="I87" s="54"/>
+      <c r="J87" s="57"/>
+      <c r="K87" s="54"/>
       <c r="L87" s="2"/>
       <c r="M87" s="2"/>
       <c r="N87" s="2"/>
@@ -5159,19 +5159,19 @@
       <c r="AA87" s="2"/>
     </row>
     <row r="88" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A88" s="67" t="s">
+      <c r="A88" s="73" t="s">
         <v>169</v>
       </c>
-      <c r="B88" s="58" t="s">
+      <c r="B88" s="61" t="s">
         <v>49</v>
       </c>
-      <c r="C88" s="55" t="s">
+      <c r="C88" s="58" t="s">
         <v>164</v>
       </c>
-      <c r="D88" s="55" t="s">
+      <c r="D88" s="58" t="s">
         <v>165</v>
       </c>
-      <c r="E88" s="55" t="s">
+      <c r="E88" s="58" t="s">
         <v>166</v>
       </c>
       <c r="F88" s="29" t="s">
@@ -5183,13 +5183,13 @@
       <c r="H88" s="29" t="s">
         <v>168</v>
       </c>
-      <c r="I88" s="49" t="s">
+      <c r="I88" s="52" t="s">
         <v>26</v>
       </c>
-      <c r="J88" s="52" t="s">
+      <c r="J88" s="55" t="s">
         <v>56</v>
       </c>
-      <c r="K88" s="49" t="s">
+      <c r="K88" s="52" t="s">
         <v>28</v>
       </c>
       <c r="L88" s="2"/>
@@ -5210,19 +5210,19 @@
       <c r="AA88" s="2"/>
     </row>
     <row r="89" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A89" s="68"/>
-      <c r="B89" s="59"/>
-      <c r="C89" s="56"/>
-      <c r="D89" s="56"/>
-      <c r="E89" s="56"/>
+      <c r="A89" s="74"/>
+      <c r="B89" s="62"/>
+      <c r="C89" s="59"/>
+      <c r="D89" s="59"/>
+      <c r="E89" s="59"/>
       <c r="F89" s="29" t="s">
         <v>67</v>
       </c>
       <c r="G89" s="34"/>
       <c r="H89" s="34"/>
-      <c r="I89" s="50"/>
-      <c r="J89" s="53"/>
-      <c r="K89" s="50"/>
+      <c r="I89" s="53"/>
+      <c r="J89" s="56"/>
+      <c r="K89" s="53"/>
       <c r="L89" s="2"/>
       <c r="M89" s="2"/>
       <c r="N89" s="2"/>
@@ -5241,19 +5241,19 @@
       <c r="AA89" s="2"/>
     </row>
     <row r="90" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A90" s="68"/>
-      <c r="B90" s="59"/>
-      <c r="C90" s="56"/>
-      <c r="D90" s="56"/>
-      <c r="E90" s="56"/>
+      <c r="A90" s="74"/>
+      <c r="B90" s="62"/>
+      <c r="C90" s="59"/>
+      <c r="D90" s="59"/>
+      <c r="E90" s="59"/>
       <c r="F90" s="29" t="s">
         <v>70</v>
       </c>
       <c r="G90" s="45"/>
       <c r="H90" s="45"/>
-      <c r="I90" s="50"/>
-      <c r="J90" s="53"/>
-      <c r="K90" s="50"/>
+      <c r="I90" s="53"/>
+      <c r="J90" s="56"/>
+      <c r="K90" s="53"/>
       <c r="L90" s="2"/>
       <c r="M90" s="2"/>
       <c r="N90" s="2"/>
@@ -5272,19 +5272,19 @@
       <c r="AA90" s="2"/>
     </row>
     <row r="91" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A91" s="69"/>
-      <c r="B91" s="60"/>
-      <c r="C91" s="57"/>
-      <c r="D91" s="57"/>
-      <c r="E91" s="57"/>
+      <c r="A91" s="75"/>
+      <c r="B91" s="63"/>
+      <c r="C91" s="60"/>
+      <c r="D91" s="60"/>
+      <c r="E91" s="60"/>
       <c r="F91" s="29" t="s">
         <v>99</v>
       </c>
       <c r="G91" s="29"/>
       <c r="H91" s="29"/>
-      <c r="I91" s="51"/>
-      <c r="J91" s="54"/>
-      <c r="K91" s="51"/>
+      <c r="I91" s="54"/>
+      <c r="J91" s="57"/>
+      <c r="K91" s="54"/>
       <c r="L91" s="2"/>
       <c r="M91" s="2"/>
       <c r="N91" s="2"/>
@@ -5303,19 +5303,19 @@
       <c r="AA91" s="2"/>
     </row>
     <row r="92" spans="1:27" ht="25.5" customHeight="1">
-      <c r="A92" s="76" t="s">
+      <c r="A92" s="67" t="s">
         <v>186</v>
       </c>
-      <c r="B92" s="55" t="s">
+      <c r="B92" s="58" t="s">
         <v>84</v>
       </c>
-      <c r="C92" s="55" t="s">
+      <c r="C92" s="58" t="s">
         <v>170</v>
       </c>
-      <c r="D92" s="55" t="s">
+      <c r="D92" s="58" t="s">
         <v>171</v>
       </c>
-      <c r="E92" s="55" t="s">
+      <c r="E92" s="58" t="s">
         <v>172</v>
       </c>
       <c r="F92" s="29" t="s">
@@ -5327,13 +5327,13 @@
       <c r="H92" s="29" t="s">
         <v>174</v>
       </c>
-      <c r="I92" s="49" t="s">
+      <c r="I92" s="52" t="s">
         <v>26</v>
       </c>
-      <c r="J92" s="52" t="s">
+      <c r="J92" s="55" t="s">
         <v>56</v>
       </c>
-      <c r="K92" s="49" t="s">
+      <c r="K92" s="52" t="s">
         <v>28</v>
       </c>
       <c r="L92" s="2"/>
@@ -5354,19 +5354,19 @@
       <c r="AA92" s="2"/>
     </row>
     <row r="93" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A93" s="77"/>
-      <c r="B93" s="56"/>
-      <c r="C93" s="56"/>
-      <c r="D93" s="56"/>
-      <c r="E93" s="56"/>
+      <c r="A93" s="68"/>
+      <c r="B93" s="59"/>
+      <c r="C93" s="59"/>
+      <c r="D93" s="59"/>
+      <c r="E93" s="59"/>
       <c r="F93" s="29" t="s">
         <v>67</v>
       </c>
       <c r="G93" s="34"/>
       <c r="H93" s="29"/>
-      <c r="I93" s="50"/>
-      <c r="J93" s="53"/>
-      <c r="K93" s="50"/>
+      <c r="I93" s="53"/>
+      <c r="J93" s="56"/>
+      <c r="K93" s="53"/>
       <c r="L93" s="2"/>
       <c r="M93" s="2"/>
       <c r="N93" s="2"/>
@@ -5385,19 +5385,19 @@
       <c r="AA93" s="2"/>
     </row>
     <row r="94" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A94" s="77"/>
-      <c r="B94" s="56"/>
-      <c r="C94" s="56"/>
-      <c r="D94" s="56"/>
-      <c r="E94" s="56"/>
+      <c r="A94" s="68"/>
+      <c r="B94" s="59"/>
+      <c r="C94" s="59"/>
+      <c r="D94" s="59"/>
+      <c r="E94" s="59"/>
       <c r="F94" s="29" t="s">
         <v>70</v>
       </c>
       <c r="G94" s="45"/>
       <c r="H94" s="45"/>
-      <c r="I94" s="50"/>
-      <c r="J94" s="53"/>
-      <c r="K94" s="50"/>
+      <c r="I94" s="53"/>
+      <c r="J94" s="56"/>
+      <c r="K94" s="53"/>
       <c r="L94" s="2"/>
       <c r="M94" s="2"/>
       <c r="N94" s="2"/>
@@ -5416,19 +5416,19 @@
       <c r="AA94" s="2"/>
     </row>
     <row r="95" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A95" s="78"/>
-      <c r="B95" s="57"/>
-      <c r="C95" s="57"/>
-      <c r="D95" s="57"/>
-      <c r="E95" s="57"/>
+      <c r="A95" s="69"/>
+      <c r="B95" s="60"/>
+      <c r="C95" s="60"/>
+      <c r="D95" s="60"/>
+      <c r="E95" s="60"/>
       <c r="F95" s="29" t="s">
         <v>99</v>
       </c>
       <c r="G95" s="29"/>
       <c r="H95" s="29"/>
-      <c r="I95" s="51"/>
-      <c r="J95" s="54"/>
-      <c r="K95" s="51"/>
+      <c r="I95" s="54"/>
+      <c r="J95" s="57"/>
+      <c r="K95" s="54"/>
       <c r="L95" s="2"/>
       <c r="M95" s="2"/>
       <c r="N95" s="2"/>
@@ -5447,19 +5447,19 @@
       <c r="AA95" s="2"/>
     </row>
     <row r="96" spans="1:27" ht="26.25" customHeight="1">
-      <c r="A96" s="76" t="s">
+      <c r="A96" s="67" t="s">
         <v>187</v>
       </c>
-      <c r="B96" s="55" t="s">
+      <c r="B96" s="58" t="s">
         <v>84</v>
       </c>
-      <c r="C96" s="55" t="s">
+      <c r="C96" s="58" t="s">
         <v>175</v>
       </c>
-      <c r="D96" s="55" t="s">
+      <c r="D96" s="58" t="s">
         <v>176</v>
       </c>
-      <c r="E96" s="55" t="s">
+      <c r="E96" s="58" t="s">
         <v>177</v>
       </c>
       <c r="F96" s="29" t="s">
@@ -5471,13 +5471,13 @@
       <c r="H96" s="29" t="s">
         <v>174</v>
       </c>
-      <c r="I96" s="49" t="s">
+      <c r="I96" s="52" t="s">
         <v>26</v>
       </c>
-      <c r="J96" s="52" t="s">
+      <c r="J96" s="55" t="s">
         <v>56</v>
       </c>
-      <c r="K96" s="49" t="s">
+      <c r="K96" s="52" t="s">
         <v>28</v>
       </c>
       <c r="L96" s="2"/>
@@ -5498,19 +5498,19 @@
       <c r="AA96" s="2"/>
     </row>
     <row r="97" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A97" s="77"/>
-      <c r="B97" s="56"/>
-      <c r="C97" s="56"/>
-      <c r="D97" s="56"/>
-      <c r="E97" s="56"/>
+      <c r="A97" s="68"/>
+      <c r="B97" s="59"/>
+      <c r="C97" s="59"/>
+      <c r="D97" s="59"/>
+      <c r="E97" s="59"/>
       <c r="F97" s="29" t="s">
         <v>67</v>
       </c>
       <c r="G97" s="34"/>
       <c r="H97" s="29"/>
-      <c r="I97" s="50"/>
-      <c r="J97" s="53"/>
-      <c r="K97" s="50"/>
+      <c r="I97" s="53"/>
+      <c r="J97" s="56"/>
+      <c r="K97" s="53"/>
       <c r="L97" s="2"/>
       <c r="M97" s="2"/>
       <c r="N97" s="2"/>
@@ -5529,19 +5529,19 @@
       <c r="AA97" s="2"/>
     </row>
     <row r="98" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A98" s="77"/>
-      <c r="B98" s="56"/>
-      <c r="C98" s="56"/>
-      <c r="D98" s="56"/>
-      <c r="E98" s="56"/>
+      <c r="A98" s="68"/>
+      <c r="B98" s="59"/>
+      <c r="C98" s="59"/>
+      <c r="D98" s="59"/>
+      <c r="E98" s="59"/>
       <c r="F98" s="29" t="s">
         <v>70</v>
       </c>
       <c r="G98" s="29"/>
       <c r="H98" s="29"/>
-      <c r="I98" s="50"/>
-      <c r="J98" s="53"/>
-      <c r="K98" s="50"/>
+      <c r="I98" s="53"/>
+      <c r="J98" s="56"/>
+      <c r="K98" s="53"/>
       <c r="L98" s="2"/>
       <c r="M98" s="2"/>
       <c r="N98" s="2"/>
@@ -5560,19 +5560,19 @@
       <c r="AA98" s="2"/>
     </row>
     <row r="99" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A99" s="78"/>
-      <c r="B99" s="57"/>
-      <c r="C99" s="57"/>
-      <c r="D99" s="57"/>
-      <c r="E99" s="57"/>
+      <c r="A99" s="69"/>
+      <c r="B99" s="60"/>
+      <c r="C99" s="60"/>
+      <c r="D99" s="60"/>
+      <c r="E99" s="60"/>
       <c r="F99" s="29" t="s">
         <v>99</v>
       </c>
       <c r="G99" s="29"/>
       <c r="H99" s="29"/>
-      <c r="I99" s="51"/>
-      <c r="J99" s="54"/>
-      <c r="K99" s="51"/>
+      <c r="I99" s="54"/>
+      <c r="J99" s="57"/>
+      <c r="K99" s="54"/>
       <c r="L99" s="2"/>
       <c r="M99" s="2"/>
       <c r="N99" s="2"/>
@@ -5591,19 +5591,19 @@
       <c r="AA99" s="2"/>
     </row>
     <row r="100" spans="1:27" ht="24.75" customHeight="1">
-      <c r="A100" s="76" t="s">
+      <c r="A100" s="67" t="s">
         <v>188</v>
       </c>
-      <c r="B100" s="55" t="s">
+      <c r="B100" s="58" t="s">
         <v>84</v>
       </c>
-      <c r="C100" s="55" t="s">
+      <c r="C100" s="58" t="s">
         <v>178</v>
       </c>
-      <c r="D100" s="55" t="s">
+      <c r="D100" s="58" t="s">
         <v>179</v>
       </c>
-      <c r="E100" s="55" t="s">
+      <c r="E100" s="58" t="s">
         <v>172</v>
       </c>
       <c r="F100" s="29" t="s">
@@ -5615,13 +5615,13 @@
       <c r="H100" s="29" t="s">
         <v>181</v>
       </c>
-      <c r="I100" s="49" t="s">
+      <c r="I100" s="52" t="s">
         <v>26</v>
       </c>
-      <c r="J100" s="52" t="s">
+      <c r="J100" s="55" t="s">
         <v>56</v>
       </c>
-      <c r="K100" s="49" t="s">
+      <c r="K100" s="52" t="s">
         <v>28</v>
       </c>
       <c r="L100" s="2"/>
@@ -5642,19 +5642,19 @@
       <c r="AA100" s="2"/>
     </row>
     <row r="101" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A101" s="77"/>
-      <c r="B101" s="56"/>
-      <c r="C101" s="56"/>
-      <c r="D101" s="56"/>
-      <c r="E101" s="56"/>
+      <c r="A101" s="68"/>
+      <c r="B101" s="59"/>
+      <c r="C101" s="59"/>
+      <c r="D101" s="59"/>
+      <c r="E101" s="59"/>
       <c r="F101" s="29" t="s">
         <v>67</v>
       </c>
       <c r="G101" s="34"/>
       <c r="H101" s="29"/>
-      <c r="I101" s="50"/>
-      <c r="J101" s="53"/>
-      <c r="K101" s="50"/>
+      <c r="I101" s="53"/>
+      <c r="J101" s="56"/>
+      <c r="K101" s="53"/>
       <c r="L101" s="2"/>
       <c r="M101" s="2"/>
       <c r="N101" s="2"/>
@@ -5673,19 +5673,19 @@
       <c r="AA101" s="2"/>
     </row>
     <row r="102" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A102" s="77"/>
-      <c r="B102" s="56"/>
-      <c r="C102" s="56"/>
-      <c r="D102" s="56"/>
-      <c r="E102" s="56"/>
+      <c r="A102" s="68"/>
+      <c r="B102" s="59"/>
+      <c r="C102" s="59"/>
+      <c r="D102" s="59"/>
+      <c r="E102" s="59"/>
       <c r="F102" s="29" t="s">
         <v>70</v>
       </c>
       <c r="G102" s="45"/>
       <c r="H102" s="45"/>
-      <c r="I102" s="50"/>
-      <c r="J102" s="53"/>
-      <c r="K102" s="50"/>
+      <c r="I102" s="53"/>
+      <c r="J102" s="56"/>
+      <c r="K102" s="53"/>
       <c r="L102" s="2"/>
       <c r="M102" s="2"/>
       <c r="N102" s="2"/>
@@ -5704,19 +5704,19 @@
       <c r="AA102" s="2"/>
     </row>
     <row r="103" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A103" s="78"/>
-      <c r="B103" s="57"/>
-      <c r="C103" s="57"/>
-      <c r="D103" s="57"/>
-      <c r="E103" s="57"/>
+      <c r="A103" s="69"/>
+      <c r="B103" s="60"/>
+      <c r="C103" s="60"/>
+      <c r="D103" s="60"/>
+      <c r="E103" s="60"/>
       <c r="F103" s="29" t="s">
         <v>99</v>
       </c>
       <c r="G103" s="45"/>
       <c r="H103" s="45"/>
-      <c r="I103" s="51"/>
-      <c r="J103" s="54"/>
-      <c r="K103" s="51"/>
+      <c r="I103" s="54"/>
+      <c r="J103" s="57"/>
+      <c r="K103" s="54"/>
       <c r="L103" s="2"/>
       <c r="M103" s="2"/>
       <c r="N103" s="2"/>
@@ -5735,19 +5735,19 @@
       <c r="AA103" s="2"/>
     </row>
     <row r="104" spans="1:27" ht="24.75" customHeight="1">
-      <c r="A104" s="76" t="s">
+      <c r="A104" s="67" t="s">
         <v>189</v>
       </c>
-      <c r="B104" s="55" t="s">
+      <c r="B104" s="58" t="s">
         <v>84</v>
       </c>
-      <c r="C104" s="55" t="s">
+      <c r="C104" s="58" t="s">
         <v>182</v>
       </c>
-      <c r="D104" s="55" t="s">
+      <c r="D104" s="58" t="s">
         <v>183</v>
       </c>
-      <c r="E104" s="55" t="s">
+      <c r="E104" s="58" t="s">
         <v>177</v>
       </c>
       <c r="F104" s="29" t="s">
@@ -5759,13 +5759,13 @@
       <c r="H104" s="29" t="s">
         <v>185</v>
       </c>
-      <c r="I104" s="49" t="s">
+      <c r="I104" s="52" t="s">
         <v>26</v>
       </c>
-      <c r="J104" s="52" t="s">
+      <c r="J104" s="55" t="s">
         <v>56</v>
       </c>
-      <c r="K104" s="49" t="s">
+      <c r="K104" s="52" t="s">
         <v>28</v>
       </c>
       <c r="L104" s="2"/>
@@ -5786,19 +5786,19 @@
       <c r="AA104" s="2"/>
     </row>
     <row r="105" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A105" s="77"/>
-      <c r="B105" s="56"/>
-      <c r="C105" s="56"/>
-      <c r="D105" s="56"/>
-      <c r="E105" s="56"/>
+      <c r="A105" s="68"/>
+      <c r="B105" s="59"/>
+      <c r="C105" s="59"/>
+      <c r="D105" s="59"/>
+      <c r="E105" s="59"/>
       <c r="F105" s="29" t="s">
         <v>67</v>
       </c>
       <c r="G105" s="34"/>
       <c r="H105" s="29"/>
-      <c r="I105" s="50"/>
-      <c r="J105" s="53"/>
-      <c r="K105" s="50"/>
+      <c r="I105" s="53"/>
+      <c r="J105" s="56"/>
+      <c r="K105" s="53"/>
       <c r="L105" s="2"/>
       <c r="M105" s="2"/>
       <c r="N105" s="2"/>
@@ -5817,19 +5817,19 @@
       <c r="AA105" s="2"/>
     </row>
     <row r="106" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A106" s="77"/>
-      <c r="B106" s="56"/>
-      <c r="C106" s="56"/>
-      <c r="D106" s="56"/>
-      <c r="E106" s="56"/>
+      <c r="A106" s="68"/>
+      <c r="B106" s="59"/>
+      <c r="C106" s="59"/>
+      <c r="D106" s="59"/>
+      <c r="E106" s="59"/>
       <c r="F106" s="29" t="s">
         <v>70</v>
       </c>
       <c r="G106" s="45"/>
       <c r="H106" s="45"/>
-      <c r="I106" s="50"/>
-      <c r="J106" s="53"/>
-      <c r="K106" s="50"/>
+      <c r="I106" s="53"/>
+      <c r="J106" s="56"/>
+      <c r="K106" s="53"/>
       <c r="L106" s="2"/>
       <c r="M106" s="2"/>
       <c r="N106" s="2"/>
@@ -5848,19 +5848,19 @@
       <c r="AA106" s="2"/>
     </row>
     <row r="107" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A107" s="78"/>
-      <c r="B107" s="57"/>
-      <c r="C107" s="57"/>
-      <c r="D107" s="57"/>
-      <c r="E107" s="57"/>
+      <c r="A107" s="69"/>
+      <c r="B107" s="60"/>
+      <c r="C107" s="60"/>
+      <c r="D107" s="60"/>
+      <c r="E107" s="60"/>
       <c r="F107" s="29" t="s">
         <v>99</v>
       </c>
       <c r="G107" s="45"/>
       <c r="H107" s="46"/>
-      <c r="I107" s="51"/>
-      <c r="J107" s="54"/>
-      <c r="K107" s="51"/>
+      <c r="I107" s="54"/>
+      <c r="J107" s="57"/>
+      <c r="K107" s="54"/>
       <c r="L107" s="2"/>
       <c r="M107" s="2"/>
       <c r="N107" s="2"/>
@@ -5879,19 +5879,19 @@
       <c r="AA107" s="2"/>
     </row>
     <row r="108" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A108" s="64" t="s">
+      <c r="A108" s="49" t="s">
         <v>198</v>
       </c>
-      <c r="B108" s="55" t="s">
+      <c r="B108" s="58" t="s">
         <v>190</v>
       </c>
-      <c r="C108" s="55" t="s">
+      <c r="C108" s="58" t="s">
         <v>191</v>
       </c>
-      <c r="D108" s="55" t="s">
+      <c r="D108" s="58" t="s">
         <v>200</v>
       </c>
-      <c r="E108" s="55" t="s">
+      <c r="E108" s="58" t="s">
         <v>83</v>
       </c>
       <c r="F108" s="29" t="s">
@@ -5903,13 +5903,13 @@
       <c r="H108" s="29" t="s">
         <v>193</v>
       </c>
-      <c r="I108" s="49" t="s">
+      <c r="I108" s="52" t="s">
         <v>26</v>
       </c>
-      <c r="J108" s="52" t="s">
+      <c r="J108" s="55" t="s">
         <v>56</v>
       </c>
-      <c r="K108" s="49" t="s">
+      <c r="K108" s="52" t="s">
         <v>28</v>
       </c>
       <c r="L108" s="2"/>
@@ -5930,19 +5930,19 @@
       <c r="AA108" s="2"/>
     </row>
     <row r="109" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A109" s="65"/>
-      <c r="B109" s="56"/>
-      <c r="C109" s="56"/>
-      <c r="D109" s="56"/>
-      <c r="E109" s="56"/>
+      <c r="A109" s="50"/>
+      <c r="B109" s="59"/>
+      <c r="C109" s="59"/>
+      <c r="D109" s="59"/>
+      <c r="E109" s="59"/>
       <c r="F109" s="29" t="s">
         <v>67</v>
       </c>
       <c r="G109" s="29"/>
       <c r="H109" s="29"/>
-      <c r="I109" s="50"/>
-      <c r="J109" s="53"/>
-      <c r="K109" s="50"/>
+      <c r="I109" s="53"/>
+      <c r="J109" s="56"/>
+      <c r="K109" s="53"/>
       <c r="L109" s="2"/>
       <c r="M109" s="2"/>
       <c r="N109" s="2"/>
@@ -5961,19 +5961,19 @@
       <c r="AA109" s="2"/>
     </row>
     <row r="110" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A110" s="65"/>
-      <c r="B110" s="56"/>
-      <c r="C110" s="56"/>
-      <c r="D110" s="56"/>
-      <c r="E110" s="56"/>
+      <c r="A110" s="50"/>
+      <c r="B110" s="59"/>
+      <c r="C110" s="59"/>
+      <c r="D110" s="59"/>
+      <c r="E110" s="59"/>
       <c r="F110" s="29" t="s">
         <v>70</v>
       </c>
       <c r="G110" s="29"/>
       <c r="H110" s="29"/>
-      <c r="I110" s="50"/>
-      <c r="J110" s="53"/>
-      <c r="K110" s="50"/>
+      <c r="I110" s="53"/>
+      <c r="J110" s="56"/>
+      <c r="K110" s="53"/>
       <c r="L110" s="2"/>
       <c r="M110" s="2"/>
       <c r="N110" s="2"/>
@@ -5992,19 +5992,19 @@
       <c r="AA110" s="2"/>
     </row>
     <row r="111" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A111" s="66"/>
-      <c r="B111" s="56"/>
-      <c r="C111" s="57"/>
-      <c r="D111" s="57"/>
-      <c r="E111" s="57"/>
+      <c r="A111" s="51"/>
+      <c r="B111" s="59"/>
+      <c r="C111" s="60"/>
+      <c r="D111" s="60"/>
+      <c r="E111" s="60"/>
       <c r="F111" s="29" t="s">
         <v>99</v>
       </c>
       <c r="G111" s="29"/>
       <c r="H111" s="29"/>
-      <c r="I111" s="51"/>
-      <c r="J111" s="54"/>
-      <c r="K111" s="51"/>
+      <c r="I111" s="54"/>
+      <c r="J111" s="57"/>
+      <c r="K111" s="54"/>
       <c r="L111" s="2"/>
       <c r="M111" s="2"/>
       <c r="N111" s="2"/>
@@ -6023,37 +6023,37 @@
       <c r="AA111" s="2"/>
     </row>
     <row r="112" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A112" s="64" t="s">
+      <c r="A112" s="49" t="s">
         <v>199</v>
       </c>
-      <c r="B112" s="55" t="s">
+      <c r="B112" s="58" t="s">
         <v>190</v>
       </c>
-      <c r="C112" s="55" t="s">
+      <c r="C112" s="58" t="s">
         <v>194</v>
       </c>
-      <c r="D112" s="55" t="s">
+      <c r="D112" s="58" t="s">
         <v>195</v>
       </c>
-      <c r="E112" s="55" t="s">
+      <c r="E112" s="58" t="s">
         <v>83</v>
       </c>
-      <c r="F112" s="58" t="s">
+      <c r="F112" s="61" t="s">
         <v>53</v>
       </c>
-      <c r="G112" s="58" t="s">
+      <c r="G112" s="61" t="s">
         <v>196</v>
       </c>
-      <c r="H112" s="61" t="s">
+      <c r="H112" s="64" t="s">
         <v>197</v>
       </c>
-      <c r="I112" s="49" t="s">
+      <c r="I112" s="52" t="s">
         <v>226</v>
       </c>
-      <c r="J112" s="52" t="s">
+      <c r="J112" s="55" t="s">
         <v>56</v>
       </c>
-      <c r="K112" s="49" t="s">
+      <c r="K112" s="52" t="s">
         <v>28</v>
       </c>
       <c r="L112" s="2"/>
@@ -6074,17 +6074,17 @@
       <c r="AA112" s="2"/>
     </row>
     <row r="113" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A113" s="65"/>
-      <c r="B113" s="56"/>
-      <c r="C113" s="56"/>
-      <c r="D113" s="56"/>
-      <c r="E113" s="56"/>
-      <c r="F113" s="59"/>
-      <c r="G113" s="59"/>
-      <c r="H113" s="62"/>
-      <c r="I113" s="50"/>
-      <c r="J113" s="53"/>
-      <c r="K113" s="50"/>
+      <c r="A113" s="50"/>
+      <c r="B113" s="59"/>
+      <c r="C113" s="59"/>
+      <c r="D113" s="59"/>
+      <c r="E113" s="59"/>
+      <c r="F113" s="62"/>
+      <c r="G113" s="62"/>
+      <c r="H113" s="65"/>
+      <c r="I113" s="53"/>
+      <c r="J113" s="56"/>
+      <c r="K113" s="53"/>
       <c r="L113" s="2"/>
       <c r="M113" s="2"/>
       <c r="N113" s="2"/>
@@ -6103,17 +6103,17 @@
       <c r="AA113" s="2"/>
     </row>
     <row r="114" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A114" s="65"/>
-      <c r="B114" s="56"/>
-      <c r="C114" s="56"/>
-      <c r="D114" s="56"/>
-      <c r="E114" s="56"/>
-      <c r="F114" s="59"/>
-      <c r="G114" s="59"/>
-      <c r="H114" s="62"/>
-      <c r="I114" s="50"/>
-      <c r="J114" s="53"/>
-      <c r="K114" s="50"/>
+      <c r="A114" s="50"/>
+      <c r="B114" s="59"/>
+      <c r="C114" s="59"/>
+      <c r="D114" s="59"/>
+      <c r="E114" s="59"/>
+      <c r="F114" s="62"/>
+      <c r="G114" s="62"/>
+      <c r="H114" s="65"/>
+      <c r="I114" s="53"/>
+      <c r="J114" s="56"/>
+      <c r="K114" s="53"/>
       <c r="L114" s="2"/>
       <c r="M114" s="2"/>
       <c r="N114" s="2"/>
@@ -6132,17 +6132,17 @@
       <c r="AA114" s="2"/>
     </row>
     <row r="115" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A115" s="66"/>
-      <c r="B115" s="57"/>
-      <c r="C115" s="57"/>
-      <c r="D115" s="57"/>
-      <c r="E115" s="57"/>
-      <c r="F115" s="60"/>
-      <c r="G115" s="60"/>
-      <c r="H115" s="63"/>
-      <c r="I115" s="51"/>
-      <c r="J115" s="54"/>
-      <c r="K115" s="51"/>
+      <c r="A115" s="51"/>
+      <c r="B115" s="60"/>
+      <c r="C115" s="60"/>
+      <c r="D115" s="60"/>
+      <c r="E115" s="60"/>
+      <c r="F115" s="63"/>
+      <c r="G115" s="63"/>
+      <c r="H115" s="66"/>
+      <c r="I115" s="54"/>
+      <c r="J115" s="57"/>
+      <c r="K115" s="54"/>
       <c r="L115" s="2"/>
       <c r="M115" s="2"/>
       <c r="N115" s="2"/>
@@ -6161,37 +6161,37 @@
       <c r="AA115" s="2"/>
     </row>
     <row r="116" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A116" s="64" t="s">
+      <c r="A116" s="49" t="s">
         <v>218</v>
       </c>
-      <c r="B116" s="55" t="s">
+      <c r="B116" s="58" t="s">
         <v>201</v>
       </c>
-      <c r="C116" s="55" t="s">
+      <c r="C116" s="58" t="s">
         <v>202</v>
       </c>
-      <c r="D116" s="55" t="s">
+      <c r="D116" s="58" t="s">
         <v>203</v>
       </c>
-      <c r="E116" s="55" t="s">
+      <c r="E116" s="58" t="s">
         <v>222</v>
       </c>
-      <c r="F116" s="58" t="s">
+      <c r="F116" s="61" t="s">
         <v>53</v>
       </c>
-      <c r="G116" s="55" t="s">
+      <c r="G116" s="58" t="s">
         <v>204</v>
       </c>
-      <c r="H116" s="61" t="s">
+      <c r="H116" s="64" t="s">
         <v>205</v>
       </c>
-      <c r="I116" s="49" t="s">
+      <c r="I116" s="52" t="s">
         <v>226</v>
       </c>
-      <c r="J116" s="52" t="s">
+      <c r="J116" s="55" t="s">
         <v>56</v>
       </c>
-      <c r="K116" s="49" t="s">
+      <c r="K116" s="52" t="s">
         <v>28</v>
       </c>
       <c r="L116" s="2"/>
@@ -6212,17 +6212,17 @@
       <c r="AA116" s="2"/>
     </row>
     <row r="117" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A117" s="65"/>
-      <c r="B117" s="56"/>
-      <c r="C117" s="56"/>
-      <c r="D117" s="56"/>
-      <c r="E117" s="56"/>
-      <c r="F117" s="59"/>
-      <c r="G117" s="56"/>
-      <c r="H117" s="62"/>
-      <c r="I117" s="50"/>
-      <c r="J117" s="53"/>
-      <c r="K117" s="50"/>
+      <c r="A117" s="50"/>
+      <c r="B117" s="59"/>
+      <c r="C117" s="59"/>
+      <c r="D117" s="59"/>
+      <c r="E117" s="59"/>
+      <c r="F117" s="62"/>
+      <c r="G117" s="59"/>
+      <c r="H117" s="65"/>
+      <c r="I117" s="53"/>
+      <c r="J117" s="56"/>
+      <c r="K117" s="53"/>
       <c r="L117" s="2"/>
       <c r="M117" s="2"/>
       <c r="N117" s="2"/>
@@ -6241,17 +6241,17 @@
       <c r="AA117" s="2"/>
     </row>
     <row r="118" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A118" s="65"/>
-      <c r="B118" s="56"/>
-      <c r="C118" s="56"/>
-      <c r="D118" s="56"/>
-      <c r="E118" s="56"/>
-      <c r="F118" s="60"/>
-      <c r="G118" s="56"/>
-      <c r="H118" s="62"/>
-      <c r="I118" s="50"/>
-      <c r="J118" s="53"/>
-      <c r="K118" s="50"/>
+      <c r="A118" s="50"/>
+      <c r="B118" s="59"/>
+      <c r="C118" s="59"/>
+      <c r="D118" s="59"/>
+      <c r="E118" s="59"/>
+      <c r="F118" s="63"/>
+      <c r="G118" s="59"/>
+      <c r="H118" s="65"/>
+      <c r="I118" s="53"/>
+      <c r="J118" s="56"/>
+      <c r="K118" s="53"/>
       <c r="L118" s="2"/>
       <c r="M118" s="2"/>
       <c r="N118" s="2"/>
@@ -6270,19 +6270,19 @@
       <c r="AA118" s="2"/>
     </row>
     <row r="119" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A119" s="66"/>
-      <c r="B119" s="57"/>
-      <c r="C119" s="57"/>
-      <c r="D119" s="57"/>
-      <c r="E119" s="57"/>
+      <c r="A119" s="51"/>
+      <c r="B119" s="60"/>
+      <c r="C119" s="60"/>
+      <c r="D119" s="60"/>
+      <c r="E119" s="60"/>
       <c r="F119" s="29" t="s">
         <v>67</v>
       </c>
       <c r="G119" s="47"/>
       <c r="H119" s="48"/>
-      <c r="I119" s="51"/>
-      <c r="J119" s="54"/>
-      <c r="K119" s="51"/>
+      <c r="I119" s="54"/>
+      <c r="J119" s="57"/>
+      <c r="K119" s="54"/>
       <c r="L119" s="2"/>
       <c r="M119" s="2"/>
       <c r="N119" s="2"/>
@@ -6301,37 +6301,37 @@
       <c r="AA119" s="2"/>
     </row>
     <row r="120" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A120" s="64" t="s">
+      <c r="A120" s="49" t="s">
         <v>219</v>
       </c>
-      <c r="B120" s="55" t="s">
+      <c r="B120" s="58" t="s">
         <v>201</v>
       </c>
-      <c r="C120" s="55" t="s">
+      <c r="C120" s="58" t="s">
         <v>206</v>
       </c>
-      <c r="D120" s="55" t="s">
+      <c r="D120" s="58" t="s">
         <v>207</v>
       </c>
-      <c r="E120" s="55" t="s">
+      <c r="E120" s="58" t="s">
         <v>223</v>
       </c>
-      <c r="F120" s="58" t="s">
+      <c r="F120" s="61" t="s">
         <v>53</v>
       </c>
-      <c r="G120" s="55" t="s">
+      <c r="G120" s="58" t="s">
         <v>208</v>
       </c>
-      <c r="H120" s="61" t="s">
+      <c r="H120" s="64" t="s">
         <v>209</v>
       </c>
-      <c r="I120" s="49" t="s">
+      <c r="I120" s="52" t="s">
         <v>26</v>
       </c>
-      <c r="J120" s="52" t="s">
+      <c r="J120" s="55" t="s">
         <v>56</v>
       </c>
-      <c r="K120" s="49" t="s">
+      <c r="K120" s="52" t="s">
         <v>28</v>
       </c>
       <c r="L120" s="2"/>
@@ -6352,17 +6352,17 @@
       <c r="AA120" s="2"/>
     </row>
     <row r="121" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A121" s="65"/>
-      <c r="B121" s="56"/>
-      <c r="C121" s="56"/>
-      <c r="D121" s="56"/>
-      <c r="E121" s="56"/>
-      <c r="F121" s="59"/>
-      <c r="G121" s="56"/>
-      <c r="H121" s="62"/>
-      <c r="I121" s="50"/>
-      <c r="J121" s="53"/>
-      <c r="K121" s="50"/>
+      <c r="A121" s="50"/>
+      <c r="B121" s="59"/>
+      <c r="C121" s="59"/>
+      <c r="D121" s="59"/>
+      <c r="E121" s="59"/>
+      <c r="F121" s="62"/>
+      <c r="G121" s="59"/>
+      <c r="H121" s="65"/>
+      <c r="I121" s="53"/>
+      <c r="J121" s="56"/>
+      <c r="K121" s="53"/>
       <c r="L121" s="2"/>
       <c r="M121" s="2"/>
       <c r="N121" s="2"/>
@@ -6381,17 +6381,17 @@
       <c r="AA121" s="2"/>
     </row>
     <row r="122" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A122" s="65"/>
-      <c r="B122" s="56"/>
-      <c r="C122" s="56"/>
-      <c r="D122" s="56"/>
-      <c r="E122" s="56"/>
-      <c r="F122" s="60"/>
-      <c r="G122" s="56"/>
-      <c r="H122" s="62"/>
-      <c r="I122" s="50"/>
-      <c r="J122" s="53"/>
-      <c r="K122" s="50"/>
+      <c r="A122" s="50"/>
+      <c r="B122" s="59"/>
+      <c r="C122" s="59"/>
+      <c r="D122" s="59"/>
+      <c r="E122" s="59"/>
+      <c r="F122" s="63"/>
+      <c r="G122" s="59"/>
+      <c r="H122" s="65"/>
+      <c r="I122" s="53"/>
+      <c r="J122" s="56"/>
+      <c r="K122" s="53"/>
       <c r="L122" s="2"/>
       <c r="M122" s="2"/>
       <c r="N122" s="2"/>
@@ -6410,19 +6410,19 @@
       <c r="AA122" s="2"/>
     </row>
     <row r="123" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A123" s="66"/>
-      <c r="B123" s="57"/>
-      <c r="C123" s="57"/>
-      <c r="D123" s="57"/>
-      <c r="E123" s="57"/>
+      <c r="A123" s="51"/>
+      <c r="B123" s="60"/>
+      <c r="C123" s="60"/>
+      <c r="D123" s="60"/>
+      <c r="E123" s="60"/>
       <c r="F123" s="29" t="s">
         <v>67</v>
       </c>
       <c r="G123" s="29"/>
       <c r="H123" s="29"/>
-      <c r="I123" s="51"/>
-      <c r="J123" s="54"/>
-      <c r="K123" s="51"/>
+      <c r="I123" s="54"/>
+      <c r="J123" s="57"/>
+      <c r="K123" s="54"/>
       <c r="L123" s="2"/>
       <c r="M123" s="2"/>
       <c r="N123" s="2"/>
@@ -6441,37 +6441,37 @@
       <c r="AA123" s="2"/>
     </row>
     <row r="124" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A124" s="64" t="s">
+      <c r="A124" s="49" t="s">
         <v>220</v>
       </c>
-      <c r="B124" s="55" t="s">
+      <c r="B124" s="58" t="s">
         <v>201</v>
       </c>
-      <c r="C124" s="55" t="s">
+      <c r="C124" s="58" t="s">
         <v>210</v>
       </c>
-      <c r="D124" s="55" t="s">
+      <c r="D124" s="58" t="s">
         <v>211</v>
       </c>
-      <c r="E124" s="55" t="s">
+      <c r="E124" s="58" t="s">
         <v>224</v>
       </c>
-      <c r="F124" s="58" t="s">
+      <c r="F124" s="61" t="s">
         <v>53</v>
       </c>
-      <c r="G124" s="55" t="s">
+      <c r="G124" s="58" t="s">
         <v>212</v>
       </c>
-      <c r="H124" s="61" t="s">
+      <c r="H124" s="64" t="s">
         <v>213</v>
       </c>
-      <c r="I124" s="49" t="s">
+      <c r="I124" s="52" t="s">
         <v>26</v>
       </c>
-      <c r="J124" s="52" t="s">
+      <c r="J124" s="55" t="s">
         <v>56</v>
       </c>
-      <c r="K124" s="49" t="s">
+      <c r="K124" s="52" t="s">
         <v>28</v>
       </c>
       <c r="L124" s="2"/>
@@ -6492,17 +6492,17 @@
       <c r="AA124" s="2"/>
     </row>
     <row r="125" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A125" s="65"/>
-      <c r="B125" s="56"/>
-      <c r="C125" s="56"/>
-      <c r="D125" s="56"/>
-      <c r="E125" s="56"/>
-      <c r="F125" s="59"/>
-      <c r="G125" s="56"/>
-      <c r="H125" s="62"/>
-      <c r="I125" s="50"/>
-      <c r="J125" s="53"/>
-      <c r="K125" s="50"/>
+      <c r="A125" s="50"/>
+      <c r="B125" s="59"/>
+      <c r="C125" s="59"/>
+      <c r="D125" s="59"/>
+      <c r="E125" s="59"/>
+      <c r="F125" s="62"/>
+      <c r="G125" s="59"/>
+      <c r="H125" s="65"/>
+      <c r="I125" s="53"/>
+      <c r="J125" s="56"/>
+      <c r="K125" s="53"/>
       <c r="L125" s="2"/>
       <c r="M125" s="2"/>
       <c r="N125" s="2"/>
@@ -6521,17 +6521,17 @@
       <c r="AA125" s="2"/>
     </row>
     <row r="126" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A126" s="65"/>
-      <c r="B126" s="56"/>
-      <c r="C126" s="56"/>
-      <c r="D126" s="56"/>
-      <c r="E126" s="56"/>
-      <c r="F126" s="60"/>
-      <c r="G126" s="56"/>
-      <c r="H126" s="62"/>
-      <c r="I126" s="50"/>
-      <c r="J126" s="53"/>
-      <c r="K126" s="50"/>
+      <c r="A126" s="50"/>
+      <c r="B126" s="59"/>
+      <c r="C126" s="59"/>
+      <c r="D126" s="59"/>
+      <c r="E126" s="59"/>
+      <c r="F126" s="63"/>
+      <c r="G126" s="59"/>
+      <c r="H126" s="65"/>
+      <c r="I126" s="53"/>
+      <c r="J126" s="56"/>
+      <c r="K126" s="53"/>
       <c r="L126" s="2"/>
       <c r="M126" s="2"/>
       <c r="N126" s="2"/>
@@ -6550,19 +6550,19 @@
       <c r="AA126" s="2"/>
     </row>
     <row r="127" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A127" s="66"/>
-      <c r="B127" s="57"/>
-      <c r="C127" s="57"/>
-      <c r="D127" s="57"/>
-      <c r="E127" s="57"/>
+      <c r="A127" s="51"/>
+      <c r="B127" s="60"/>
+      <c r="C127" s="60"/>
+      <c r="D127" s="60"/>
+      <c r="E127" s="60"/>
       <c r="F127" s="29" t="s">
         <v>67</v>
       </c>
       <c r="G127" s="29"/>
       <c r="H127" s="29"/>
-      <c r="I127" s="51"/>
-      <c r="J127" s="54"/>
-      <c r="K127" s="51"/>
+      <c r="I127" s="54"/>
+      <c r="J127" s="57"/>
+      <c r="K127" s="54"/>
       <c r="L127" s="2"/>
       <c r="M127" s="2"/>
       <c r="N127" s="2"/>
@@ -6581,37 +6581,37 @@
       <c r="AA127" s="2"/>
     </row>
     <row r="128" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A128" s="64" t="s">
+      <c r="A128" s="49" t="s">
         <v>221</v>
       </c>
-      <c r="B128" s="55" t="s">
+      <c r="B128" s="58" t="s">
         <v>201</v>
       </c>
-      <c r="C128" s="55" t="s">
+      <c r="C128" s="58" t="s">
         <v>214</v>
       </c>
-      <c r="D128" s="55" t="s">
+      <c r="D128" s="58" t="s">
         <v>215</v>
       </c>
-      <c r="E128" s="55" t="s">
+      <c r="E128" s="58" t="s">
         <v>225</v>
       </c>
-      <c r="F128" s="58" t="s">
+      <c r="F128" s="61" t="s">
         <v>53</v>
       </c>
-      <c r="G128" s="58" t="s">
+      <c r="G128" s="61" t="s">
         <v>216</v>
       </c>
-      <c r="H128" s="61" t="s">
+      <c r="H128" s="64" t="s">
         <v>217</v>
       </c>
-      <c r="I128" s="49" t="s">
+      <c r="I128" s="52" t="s">
         <v>26</v>
       </c>
-      <c r="J128" s="52" t="s">
+      <c r="J128" s="55" t="s">
         <v>56</v>
       </c>
-      <c r="K128" s="49" t="s">
+      <c r="K128" s="52" t="s">
         <v>28</v>
       </c>
       <c r="L128" s="2"/>
@@ -6632,17 +6632,17 @@
       <c r="AA128" s="2"/>
     </row>
     <row r="129" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A129" s="65"/>
-      <c r="B129" s="56"/>
-      <c r="C129" s="56"/>
-      <c r="D129" s="56"/>
-      <c r="E129" s="56"/>
-      <c r="F129" s="60"/>
-      <c r="G129" s="60"/>
-      <c r="H129" s="63"/>
-      <c r="I129" s="50"/>
-      <c r="J129" s="53"/>
-      <c r="K129" s="50"/>
+      <c r="A129" s="50"/>
+      <c r="B129" s="59"/>
+      <c r="C129" s="59"/>
+      <c r="D129" s="59"/>
+      <c r="E129" s="59"/>
+      <c r="F129" s="63"/>
+      <c r="G129" s="63"/>
+      <c r="H129" s="66"/>
+      <c r="I129" s="53"/>
+      <c r="J129" s="56"/>
+      <c r="K129" s="53"/>
       <c r="L129" s="2"/>
       <c r="M129" s="2"/>
       <c r="N129" s="2"/>
@@ -6661,19 +6661,19 @@
       <c r="AA129" s="2"/>
     </row>
     <row r="130" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A130" s="65"/>
-      <c r="B130" s="56"/>
-      <c r="C130" s="56"/>
-      <c r="D130" s="56"/>
-      <c r="E130" s="56"/>
+      <c r="A130" s="50"/>
+      <c r="B130" s="59"/>
+      <c r="C130" s="59"/>
+      <c r="D130" s="59"/>
+      <c r="E130" s="59"/>
       <c r="F130" s="29" t="s">
         <v>67</v>
       </c>
       <c r="G130" s="29"/>
       <c r="H130" s="29"/>
-      <c r="I130" s="50"/>
-      <c r="J130" s="53"/>
-      <c r="K130" s="50"/>
+      <c r="I130" s="53"/>
+      <c r="J130" s="56"/>
+      <c r="K130" s="53"/>
       <c r="L130" s="2"/>
       <c r="M130" s="2"/>
       <c r="N130" s="2"/>
@@ -6692,19 +6692,19 @@
       <c r="AA130" s="2"/>
     </row>
     <row r="131" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A131" s="66"/>
-      <c r="B131" s="57"/>
-      <c r="C131" s="57"/>
-      <c r="D131" s="57"/>
-      <c r="E131" s="57"/>
+      <c r="A131" s="51"/>
+      <c r="B131" s="60"/>
+      <c r="C131" s="60"/>
+      <c r="D131" s="60"/>
+      <c r="E131" s="60"/>
       <c r="F131" s="29" t="s">
         <v>70</v>
       </c>
       <c r="G131" s="29"/>
       <c r="H131" s="29"/>
-      <c r="I131" s="51"/>
-      <c r="J131" s="54"/>
-      <c r="K131" s="51"/>
+      <c r="I131" s="54"/>
+      <c r="J131" s="57"/>
+      <c r="K131" s="54"/>
       <c r="L131" s="2"/>
       <c r="M131" s="2"/>
       <c r="N131" s="2"/>
@@ -29924,6 +29924,271 @@
     </row>
   </sheetData>
   <mergeCells count="289">
+    <mergeCell ref="I108:I111"/>
+    <mergeCell ref="J108:J111"/>
+    <mergeCell ref="K108:K111"/>
+    <mergeCell ref="I112:I115"/>
+    <mergeCell ref="J112:J115"/>
+    <mergeCell ref="K112:K115"/>
+    <mergeCell ref="B112:B115"/>
+    <mergeCell ref="C112:C115"/>
+    <mergeCell ref="D112:D115"/>
+    <mergeCell ref="E112:E115"/>
+    <mergeCell ref="F112:F115"/>
+    <mergeCell ref="G112:G115"/>
+    <mergeCell ref="H112:H115"/>
+    <mergeCell ref="A108:A111"/>
+    <mergeCell ref="A112:A115"/>
+    <mergeCell ref="B108:B111"/>
+    <mergeCell ref="C108:C111"/>
+    <mergeCell ref="D108:D111"/>
+    <mergeCell ref="E108:E111"/>
+    <mergeCell ref="K84:K87"/>
+    <mergeCell ref="A88:A91"/>
+    <mergeCell ref="B88:B91"/>
+    <mergeCell ref="C88:C91"/>
+    <mergeCell ref="D88:D91"/>
+    <mergeCell ref="E88:E91"/>
+    <mergeCell ref="I88:I91"/>
+    <mergeCell ref="J88:J91"/>
+    <mergeCell ref="K88:K91"/>
+    <mergeCell ref="B84:B87"/>
+    <mergeCell ref="C84:C87"/>
+    <mergeCell ref="D84:D87"/>
+    <mergeCell ref="E84:E87"/>
+    <mergeCell ref="I84:I87"/>
+    <mergeCell ref="J84:J87"/>
+    <mergeCell ref="A84:A87"/>
+    <mergeCell ref="B104:B107"/>
+    <mergeCell ref="C104:C107"/>
+    <mergeCell ref="B36:B39"/>
+    <mergeCell ref="C36:C39"/>
+    <mergeCell ref="D36:D39"/>
+    <mergeCell ref="E36:E39"/>
+    <mergeCell ref="J44:J47"/>
+    <mergeCell ref="J36:J39"/>
+    <mergeCell ref="A76:A79"/>
+    <mergeCell ref="B76:B79"/>
+    <mergeCell ref="C76:C79"/>
+    <mergeCell ref="D76:D79"/>
+    <mergeCell ref="E76:E79"/>
+    <mergeCell ref="I76:I79"/>
+    <mergeCell ref="J76:J79"/>
+    <mergeCell ref="A60:A63"/>
+    <mergeCell ref="J56:J59"/>
+    <mergeCell ref="K44:K47"/>
+    <mergeCell ref="I48:I51"/>
+    <mergeCell ref="J48:J51"/>
+    <mergeCell ref="K48:K51"/>
+    <mergeCell ref="B48:B51"/>
+    <mergeCell ref="C48:C51"/>
+    <mergeCell ref="D48:D51"/>
+    <mergeCell ref="E48:E51"/>
+    <mergeCell ref="K40:K43"/>
+    <mergeCell ref="I40:I43"/>
+    <mergeCell ref="B40:B43"/>
+    <mergeCell ref="C40:C43"/>
+    <mergeCell ref="D40:D43"/>
+    <mergeCell ref="E40:E43"/>
+    <mergeCell ref="K76:K79"/>
+    <mergeCell ref="J80:J83"/>
+    <mergeCell ref="K80:K83"/>
+    <mergeCell ref="A80:A83"/>
+    <mergeCell ref="B80:B83"/>
+    <mergeCell ref="C80:C83"/>
+    <mergeCell ref="D80:D83"/>
+    <mergeCell ref="E80:E83"/>
+    <mergeCell ref="I80:I83"/>
+    <mergeCell ref="K56:K59"/>
+    <mergeCell ref="J60:J63"/>
+    <mergeCell ref="K60:K63"/>
+    <mergeCell ref="I68:I71"/>
+    <mergeCell ref="J68:J71"/>
+    <mergeCell ref="K68:K71"/>
+    <mergeCell ref="A72:A75"/>
+    <mergeCell ref="B72:B75"/>
+    <mergeCell ref="C72:C75"/>
+    <mergeCell ref="D72:D75"/>
+    <mergeCell ref="E72:E75"/>
+    <mergeCell ref="I72:I75"/>
+    <mergeCell ref="J72:J75"/>
+    <mergeCell ref="K72:K75"/>
+    <mergeCell ref="A68:A71"/>
+    <mergeCell ref="B68:B71"/>
+    <mergeCell ref="C68:C71"/>
+    <mergeCell ref="D68:D71"/>
+    <mergeCell ref="E68:E71"/>
+    <mergeCell ref="A64:A67"/>
+    <mergeCell ref="J64:J67"/>
+    <mergeCell ref="K64:K67"/>
+    <mergeCell ref="D2:D3"/>
+    <mergeCell ref="J52:J55"/>
+    <mergeCell ref="K52:K55"/>
+    <mergeCell ref="E52:E55"/>
+    <mergeCell ref="B44:B47"/>
+    <mergeCell ref="C44:C47"/>
+    <mergeCell ref="D44:D47"/>
+    <mergeCell ref="E44:E47"/>
+    <mergeCell ref="B64:B67"/>
+    <mergeCell ref="C64:C67"/>
+    <mergeCell ref="D64:D67"/>
+    <mergeCell ref="E64:E67"/>
+    <mergeCell ref="I64:I67"/>
+    <mergeCell ref="B60:B63"/>
+    <mergeCell ref="C60:C63"/>
+    <mergeCell ref="D60:D63"/>
+    <mergeCell ref="E60:E63"/>
+    <mergeCell ref="I60:I63"/>
+    <mergeCell ref="E56:E59"/>
+    <mergeCell ref="I52:I55"/>
+    <mergeCell ref="B56:B59"/>
+    <mergeCell ref="I56:I59"/>
+    <mergeCell ref="I44:I47"/>
+    <mergeCell ref="J40:J43"/>
+    <mergeCell ref="J32:J35"/>
+    <mergeCell ref="B2:B3"/>
+    <mergeCell ref="A2:A3"/>
+    <mergeCell ref="A52:A55"/>
+    <mergeCell ref="B52:B55"/>
+    <mergeCell ref="C56:C59"/>
+    <mergeCell ref="D56:D59"/>
+    <mergeCell ref="C52:C55"/>
+    <mergeCell ref="D52:D55"/>
+    <mergeCell ref="A44:A47"/>
+    <mergeCell ref="A48:A51"/>
+    <mergeCell ref="D24:D27"/>
+    <mergeCell ref="D20:D23"/>
+    <mergeCell ref="D16:D19"/>
+    <mergeCell ref="D12:D15"/>
+    <mergeCell ref="D8:D11"/>
+    <mergeCell ref="D4:D7"/>
+    <mergeCell ref="A28:A31"/>
+    <mergeCell ref="A32:A35"/>
+    <mergeCell ref="A36:A39"/>
+    <mergeCell ref="A40:A43"/>
+    <mergeCell ref="D32:D35"/>
+    <mergeCell ref="D28:D31"/>
+    <mergeCell ref="A56:A59"/>
+    <mergeCell ref="E32:E35"/>
+    <mergeCell ref="C2:C3"/>
+    <mergeCell ref="H4:H5"/>
+    <mergeCell ref="G4:G5"/>
+    <mergeCell ref="H8:H9"/>
+    <mergeCell ref="H12:H13"/>
+    <mergeCell ref="K32:K35"/>
+    <mergeCell ref="K36:K39"/>
+    <mergeCell ref="J4:J7"/>
+    <mergeCell ref="J8:J11"/>
+    <mergeCell ref="J12:J15"/>
+    <mergeCell ref="J16:J19"/>
+    <mergeCell ref="J20:J23"/>
+    <mergeCell ref="J24:J27"/>
+    <mergeCell ref="J28:J31"/>
+    <mergeCell ref="I32:I35"/>
+    <mergeCell ref="I36:I39"/>
+    <mergeCell ref="K4:K7"/>
+    <mergeCell ref="K8:K11"/>
+    <mergeCell ref="K12:K15"/>
+    <mergeCell ref="K16:K19"/>
+    <mergeCell ref="K20:K23"/>
+    <mergeCell ref="K24:K27"/>
+    <mergeCell ref="J2:J3"/>
+    <mergeCell ref="K2:K3"/>
+    <mergeCell ref="I4:I7"/>
+    <mergeCell ref="I8:I11"/>
+    <mergeCell ref="I12:I15"/>
+    <mergeCell ref="I16:I19"/>
+    <mergeCell ref="E28:E31"/>
+    <mergeCell ref="E2:E3"/>
+    <mergeCell ref="G12:G13"/>
+    <mergeCell ref="G8:G9"/>
+    <mergeCell ref="F12:F13"/>
+    <mergeCell ref="F4:F5"/>
+    <mergeCell ref="F8:F9"/>
+    <mergeCell ref="K28:K31"/>
+    <mergeCell ref="E16:E19"/>
+    <mergeCell ref="E20:E23"/>
+    <mergeCell ref="E24:E27"/>
+    <mergeCell ref="F2:H2"/>
+    <mergeCell ref="I2:I3"/>
+    <mergeCell ref="I20:I23"/>
+    <mergeCell ref="I24:I27"/>
+    <mergeCell ref="I28:I31"/>
+    <mergeCell ref="E4:E7"/>
+    <mergeCell ref="E8:E11"/>
+    <mergeCell ref="E12:E15"/>
+    <mergeCell ref="A4:A7"/>
+    <mergeCell ref="A8:A11"/>
+    <mergeCell ref="A12:A15"/>
+    <mergeCell ref="A16:A19"/>
+    <mergeCell ref="A20:A23"/>
+    <mergeCell ref="A24:A27"/>
+    <mergeCell ref="B24:B27"/>
+    <mergeCell ref="B20:B23"/>
+    <mergeCell ref="B16:B19"/>
+    <mergeCell ref="B12:B15"/>
+    <mergeCell ref="B8:B11"/>
+    <mergeCell ref="B4:B7"/>
+    <mergeCell ref="C32:C35"/>
+    <mergeCell ref="B32:B35"/>
+    <mergeCell ref="B28:B31"/>
+    <mergeCell ref="C4:C7"/>
+    <mergeCell ref="C8:C11"/>
+    <mergeCell ref="C12:C15"/>
+    <mergeCell ref="C16:C19"/>
+    <mergeCell ref="C20:C23"/>
+    <mergeCell ref="C24:C27"/>
+    <mergeCell ref="C28:C31"/>
+    <mergeCell ref="D104:D107"/>
+    <mergeCell ref="E104:E107"/>
+    <mergeCell ref="A92:A95"/>
+    <mergeCell ref="A96:A99"/>
+    <mergeCell ref="A100:A103"/>
+    <mergeCell ref="A104:A107"/>
+    <mergeCell ref="I92:I95"/>
+    <mergeCell ref="B92:B95"/>
+    <mergeCell ref="C92:C95"/>
+    <mergeCell ref="D92:D95"/>
+    <mergeCell ref="E92:E95"/>
+    <mergeCell ref="B96:B99"/>
+    <mergeCell ref="C96:C99"/>
+    <mergeCell ref="D96:D99"/>
+    <mergeCell ref="E96:E99"/>
+    <mergeCell ref="B100:B103"/>
+    <mergeCell ref="C100:C103"/>
+    <mergeCell ref="D100:D103"/>
+    <mergeCell ref="E100:E103"/>
+    <mergeCell ref="J92:J95"/>
+    <mergeCell ref="K92:K95"/>
+    <mergeCell ref="I96:I99"/>
+    <mergeCell ref="J96:J99"/>
+    <mergeCell ref="K96:K99"/>
+    <mergeCell ref="I100:I103"/>
+    <mergeCell ref="J100:J103"/>
+    <mergeCell ref="K100:K103"/>
+    <mergeCell ref="I104:I107"/>
+    <mergeCell ref="J104:J107"/>
+    <mergeCell ref="K104:K107"/>
+    <mergeCell ref="C128:C131"/>
+    <mergeCell ref="D128:D131"/>
+    <mergeCell ref="E128:E131"/>
+    <mergeCell ref="F128:F129"/>
+    <mergeCell ref="G128:G129"/>
+    <mergeCell ref="H128:H129"/>
+    <mergeCell ref="B116:B119"/>
+    <mergeCell ref="C116:C119"/>
+    <mergeCell ref="D116:D119"/>
+    <mergeCell ref="E116:E119"/>
+    <mergeCell ref="F116:F118"/>
+    <mergeCell ref="G116:G118"/>
+    <mergeCell ref="H116:H118"/>
+    <mergeCell ref="B120:B123"/>
+    <mergeCell ref="C120:C123"/>
+    <mergeCell ref="D120:D123"/>
+    <mergeCell ref="E120:E123"/>
+    <mergeCell ref="F120:F122"/>
+    <mergeCell ref="G120:G122"/>
+    <mergeCell ref="H120:H122"/>
     <mergeCell ref="A116:A119"/>
     <mergeCell ref="A120:A123"/>
     <mergeCell ref="A124:A127"/>
@@ -29948,271 +30213,6 @@
     <mergeCell ref="G124:G126"/>
     <mergeCell ref="H124:H126"/>
     <mergeCell ref="B128:B131"/>
-    <mergeCell ref="C128:C131"/>
-    <mergeCell ref="D128:D131"/>
-    <mergeCell ref="E128:E131"/>
-    <mergeCell ref="F128:F129"/>
-    <mergeCell ref="G128:G129"/>
-    <mergeCell ref="H128:H129"/>
-    <mergeCell ref="B116:B119"/>
-    <mergeCell ref="C116:C119"/>
-    <mergeCell ref="D116:D119"/>
-    <mergeCell ref="E116:E119"/>
-    <mergeCell ref="F116:F118"/>
-    <mergeCell ref="G116:G118"/>
-    <mergeCell ref="H116:H118"/>
-    <mergeCell ref="B120:B123"/>
-    <mergeCell ref="C120:C123"/>
-    <mergeCell ref="D120:D123"/>
-    <mergeCell ref="E120:E123"/>
-    <mergeCell ref="F120:F122"/>
-    <mergeCell ref="G120:G122"/>
-    <mergeCell ref="H120:H122"/>
-    <mergeCell ref="J92:J95"/>
-    <mergeCell ref="K92:K95"/>
-    <mergeCell ref="I96:I99"/>
-    <mergeCell ref="J96:J99"/>
-    <mergeCell ref="K96:K99"/>
-    <mergeCell ref="I100:I103"/>
-    <mergeCell ref="J100:J103"/>
-    <mergeCell ref="K100:K103"/>
-    <mergeCell ref="I104:I107"/>
-    <mergeCell ref="J104:J107"/>
-    <mergeCell ref="K104:K107"/>
-    <mergeCell ref="D104:D107"/>
-    <mergeCell ref="E104:E107"/>
-    <mergeCell ref="A92:A95"/>
-    <mergeCell ref="A96:A99"/>
-    <mergeCell ref="A100:A103"/>
-    <mergeCell ref="A104:A107"/>
-    <mergeCell ref="I92:I95"/>
-    <mergeCell ref="B92:B95"/>
-    <mergeCell ref="C92:C95"/>
-    <mergeCell ref="D92:D95"/>
-    <mergeCell ref="E92:E95"/>
-    <mergeCell ref="B96:B99"/>
-    <mergeCell ref="C96:C99"/>
-    <mergeCell ref="D96:D99"/>
-    <mergeCell ref="E96:E99"/>
-    <mergeCell ref="B100:B103"/>
-    <mergeCell ref="C100:C103"/>
-    <mergeCell ref="D100:D103"/>
-    <mergeCell ref="E100:E103"/>
-    <mergeCell ref="C32:C35"/>
-    <mergeCell ref="B32:B35"/>
-    <mergeCell ref="B28:B31"/>
-    <mergeCell ref="C4:C7"/>
-    <mergeCell ref="C8:C11"/>
-    <mergeCell ref="C12:C15"/>
-    <mergeCell ref="C16:C19"/>
-    <mergeCell ref="C20:C23"/>
-    <mergeCell ref="C24:C27"/>
-    <mergeCell ref="C28:C31"/>
-    <mergeCell ref="A4:A7"/>
-    <mergeCell ref="A8:A11"/>
-    <mergeCell ref="A12:A15"/>
-    <mergeCell ref="A16:A19"/>
-    <mergeCell ref="A20:A23"/>
-    <mergeCell ref="A24:A27"/>
-    <mergeCell ref="B24:B27"/>
-    <mergeCell ref="B20:B23"/>
-    <mergeCell ref="B16:B19"/>
-    <mergeCell ref="B12:B15"/>
-    <mergeCell ref="B8:B11"/>
-    <mergeCell ref="B4:B7"/>
-    <mergeCell ref="K2:K3"/>
-    <mergeCell ref="I4:I7"/>
-    <mergeCell ref="I8:I11"/>
-    <mergeCell ref="I12:I15"/>
-    <mergeCell ref="I16:I19"/>
-    <mergeCell ref="E28:E31"/>
-    <mergeCell ref="E2:E3"/>
-    <mergeCell ref="G12:G13"/>
-    <mergeCell ref="G8:G9"/>
-    <mergeCell ref="F12:F13"/>
-    <mergeCell ref="F4:F5"/>
-    <mergeCell ref="F8:F9"/>
-    <mergeCell ref="K28:K31"/>
-    <mergeCell ref="E16:E19"/>
-    <mergeCell ref="E20:E23"/>
-    <mergeCell ref="E24:E27"/>
-    <mergeCell ref="F2:H2"/>
-    <mergeCell ref="I2:I3"/>
-    <mergeCell ref="I20:I23"/>
-    <mergeCell ref="I24:I27"/>
-    <mergeCell ref="I28:I31"/>
-    <mergeCell ref="E4:E7"/>
-    <mergeCell ref="E8:E11"/>
-    <mergeCell ref="E12:E15"/>
-    <mergeCell ref="E32:E35"/>
-    <mergeCell ref="C2:C3"/>
-    <mergeCell ref="H4:H5"/>
-    <mergeCell ref="G4:G5"/>
-    <mergeCell ref="H8:H9"/>
-    <mergeCell ref="H12:H13"/>
-    <mergeCell ref="K32:K35"/>
-    <mergeCell ref="K36:K39"/>
-    <mergeCell ref="J4:J7"/>
-    <mergeCell ref="J8:J11"/>
-    <mergeCell ref="J12:J15"/>
-    <mergeCell ref="J16:J19"/>
-    <mergeCell ref="J20:J23"/>
-    <mergeCell ref="J24:J27"/>
-    <mergeCell ref="J28:J31"/>
-    <mergeCell ref="I32:I35"/>
-    <mergeCell ref="I36:I39"/>
-    <mergeCell ref="K4:K7"/>
-    <mergeCell ref="K8:K11"/>
-    <mergeCell ref="K12:K15"/>
-    <mergeCell ref="K16:K19"/>
-    <mergeCell ref="K20:K23"/>
-    <mergeCell ref="K24:K27"/>
-    <mergeCell ref="J2:J3"/>
-    <mergeCell ref="J32:J35"/>
-    <mergeCell ref="B2:B3"/>
-    <mergeCell ref="A2:A3"/>
-    <mergeCell ref="A52:A55"/>
-    <mergeCell ref="B52:B55"/>
-    <mergeCell ref="C56:C59"/>
-    <mergeCell ref="D56:D59"/>
-    <mergeCell ref="C52:C55"/>
-    <mergeCell ref="D52:D55"/>
-    <mergeCell ref="A44:A47"/>
-    <mergeCell ref="A48:A51"/>
-    <mergeCell ref="D24:D27"/>
-    <mergeCell ref="D20:D23"/>
-    <mergeCell ref="D16:D19"/>
-    <mergeCell ref="D12:D15"/>
-    <mergeCell ref="D8:D11"/>
-    <mergeCell ref="D4:D7"/>
-    <mergeCell ref="A28:A31"/>
-    <mergeCell ref="A32:A35"/>
-    <mergeCell ref="A36:A39"/>
-    <mergeCell ref="A40:A43"/>
-    <mergeCell ref="D32:D35"/>
-    <mergeCell ref="D28:D31"/>
-    <mergeCell ref="A56:A59"/>
-    <mergeCell ref="D2:D3"/>
-    <mergeCell ref="J52:J55"/>
-    <mergeCell ref="K52:K55"/>
-    <mergeCell ref="E52:E55"/>
-    <mergeCell ref="B44:B47"/>
-    <mergeCell ref="C44:C47"/>
-    <mergeCell ref="D44:D47"/>
-    <mergeCell ref="E44:E47"/>
-    <mergeCell ref="B64:B67"/>
-    <mergeCell ref="C64:C67"/>
-    <mergeCell ref="D64:D67"/>
-    <mergeCell ref="E64:E67"/>
-    <mergeCell ref="I64:I67"/>
-    <mergeCell ref="B60:B63"/>
-    <mergeCell ref="C60:C63"/>
-    <mergeCell ref="D60:D63"/>
-    <mergeCell ref="E60:E63"/>
-    <mergeCell ref="I60:I63"/>
-    <mergeCell ref="E56:E59"/>
-    <mergeCell ref="I52:I55"/>
-    <mergeCell ref="B56:B59"/>
-    <mergeCell ref="I56:I59"/>
-    <mergeCell ref="I44:I47"/>
-    <mergeCell ref="J40:J43"/>
-    <mergeCell ref="K56:K59"/>
-    <mergeCell ref="J60:J63"/>
-    <mergeCell ref="K60:K63"/>
-    <mergeCell ref="I68:I71"/>
-    <mergeCell ref="J68:J71"/>
-    <mergeCell ref="K68:K71"/>
-    <mergeCell ref="A72:A75"/>
-    <mergeCell ref="B72:B75"/>
-    <mergeCell ref="C72:C75"/>
-    <mergeCell ref="D72:D75"/>
-    <mergeCell ref="E72:E75"/>
-    <mergeCell ref="I72:I75"/>
-    <mergeCell ref="J72:J75"/>
-    <mergeCell ref="K72:K75"/>
-    <mergeCell ref="A68:A71"/>
-    <mergeCell ref="B68:B71"/>
-    <mergeCell ref="C68:C71"/>
-    <mergeCell ref="D68:D71"/>
-    <mergeCell ref="E68:E71"/>
-    <mergeCell ref="A64:A67"/>
-    <mergeCell ref="J64:J67"/>
-    <mergeCell ref="K64:K67"/>
-    <mergeCell ref="K76:K79"/>
-    <mergeCell ref="J80:J83"/>
-    <mergeCell ref="K80:K83"/>
-    <mergeCell ref="A80:A83"/>
-    <mergeCell ref="B80:B83"/>
-    <mergeCell ref="C80:C83"/>
-    <mergeCell ref="D80:D83"/>
-    <mergeCell ref="E80:E83"/>
-    <mergeCell ref="I80:I83"/>
-    <mergeCell ref="K44:K47"/>
-    <mergeCell ref="I48:I51"/>
-    <mergeCell ref="J48:J51"/>
-    <mergeCell ref="K48:K51"/>
-    <mergeCell ref="B48:B51"/>
-    <mergeCell ref="C48:C51"/>
-    <mergeCell ref="D48:D51"/>
-    <mergeCell ref="E48:E51"/>
-    <mergeCell ref="K40:K43"/>
-    <mergeCell ref="I40:I43"/>
-    <mergeCell ref="B40:B43"/>
-    <mergeCell ref="C40:C43"/>
-    <mergeCell ref="D40:D43"/>
-    <mergeCell ref="E40:E43"/>
-    <mergeCell ref="B36:B39"/>
-    <mergeCell ref="C36:C39"/>
-    <mergeCell ref="D36:D39"/>
-    <mergeCell ref="E36:E39"/>
-    <mergeCell ref="J44:J47"/>
-    <mergeCell ref="J36:J39"/>
-    <mergeCell ref="A76:A79"/>
-    <mergeCell ref="B76:B79"/>
-    <mergeCell ref="C76:C79"/>
-    <mergeCell ref="D76:D79"/>
-    <mergeCell ref="E76:E79"/>
-    <mergeCell ref="I76:I79"/>
-    <mergeCell ref="J76:J79"/>
-    <mergeCell ref="A60:A63"/>
-    <mergeCell ref="J56:J59"/>
-    <mergeCell ref="A108:A111"/>
-    <mergeCell ref="A112:A115"/>
-    <mergeCell ref="B108:B111"/>
-    <mergeCell ref="C108:C111"/>
-    <mergeCell ref="D108:D111"/>
-    <mergeCell ref="E108:E111"/>
-    <mergeCell ref="K84:K87"/>
-    <mergeCell ref="A88:A91"/>
-    <mergeCell ref="B88:B91"/>
-    <mergeCell ref="C88:C91"/>
-    <mergeCell ref="D88:D91"/>
-    <mergeCell ref="E88:E91"/>
-    <mergeCell ref="I88:I91"/>
-    <mergeCell ref="J88:J91"/>
-    <mergeCell ref="K88:K91"/>
-    <mergeCell ref="B84:B87"/>
-    <mergeCell ref="C84:C87"/>
-    <mergeCell ref="D84:D87"/>
-    <mergeCell ref="E84:E87"/>
-    <mergeCell ref="I84:I87"/>
-    <mergeCell ref="J84:J87"/>
-    <mergeCell ref="A84:A87"/>
-    <mergeCell ref="B104:B107"/>
-    <mergeCell ref="C104:C107"/>
-    <mergeCell ref="I108:I111"/>
-    <mergeCell ref="J108:J111"/>
-    <mergeCell ref="K108:K111"/>
-    <mergeCell ref="I112:I115"/>
-    <mergeCell ref="J112:J115"/>
-    <mergeCell ref="K112:K115"/>
-    <mergeCell ref="B112:B115"/>
-    <mergeCell ref="C112:C115"/>
-    <mergeCell ref="D112:D115"/>
-    <mergeCell ref="E112:E115"/>
-    <mergeCell ref="F112:F115"/>
-    <mergeCell ref="G112:G115"/>
-    <mergeCell ref="H112:H115"/>
   </mergeCells>
   <conditionalFormatting sqref="I4 I8 I12">
     <cfRule type="cellIs" dxfId="23" priority="21" operator="equal">

</xml_diff>